<commit_message>
stock updated by raj time 11:33
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 12-Dec-2024</t>
+    <t>1-Jul-2024 to 14-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -293,7 +293,7 @@
     <t>1920 PATRIKA-B</t>
   </si>
   <si>
-    <t>1920 PATRIKA (RED) 14.12</t>
+    <t>1920 PATRIKA (RED)</t>
   </si>
   <si>
     <t>1921 PATRIKA (GOLDEN)</t>
@@ -1196,7 +1196,7 @@
     <t>6549 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6550 PATRIKA {M}</t>
+    <t>6550 PATRIKA {M} (DC)</t>
   </si>
   <si>
     <t>7250 PATRIKA</t>
@@ -2460,13 +2460,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>-126</v>
+        <v>-146</v>
       </c>
       <c r="C11" s="19">
         <v>0.98</v>
       </c>
       <c r="D11" s="20">
-        <v>-123.48</v>
+        <v>-143.08000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2572,13 +2572,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="18">
-        <v>126.5</v>
+        <v>124</v>
       </c>
       <c r="C19" s="19">
         <v>2</v>
       </c>
       <c r="D19" s="20">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2650,13 +2650,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="18">
-        <v>123.5</v>
+        <v>121.5</v>
       </c>
       <c r="C25" s="19">
         <v>2.1</v>
       </c>
       <c r="D25" s="20">
-        <v>259.35000000000002</v>
+        <v>255.15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,13 +2816,13 @@
         <v>41</v>
       </c>
       <c r="B39" s="18">
-        <v>112.5</v>
+        <v>111</v>
       </c>
       <c r="C39" s="19">
         <v>2.7</v>
       </c>
       <c r="D39" s="20">
-        <v>303.75</v>
+        <v>299.7</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,13 +2970,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>173.5</v>
+        <v>153.5</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>190.85</v>
+        <v>168.85</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,13 +2998,13 @@
         <v>54</v>
       </c>
       <c r="B52" s="18">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="C52" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D52" s="20">
-        <v>212.3</v>
+        <v>199.1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,13 +3012,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="18">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C53" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D53" s="20">
-        <v>118.8</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,13 +3026,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>75.900000000000006</v>
+        <v>64.900000000000006</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,13 +3054,13 @@
         <v>58</v>
       </c>
       <c r="B56" s="18">
-        <v>-10</v>
+        <v>-30</v>
       </c>
       <c r="C56" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D56" s="20">
-        <v>-11</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3068,13 +3068,13 @@
         <v>59</v>
       </c>
       <c r="B57" s="18">
-        <v>607</v>
+        <v>604.5</v>
       </c>
       <c r="C57" s="19">
         <v>1.9</v>
       </c>
       <c r="D57" s="20">
-        <v>1153.3</v>
+        <v>1148.55</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,13 +3124,13 @@
         <v>63</v>
       </c>
       <c r="B61" s="18">
-        <v>40.5</v>
+        <v>35.5</v>
       </c>
       <c r="C61" s="19">
         <v>2.1</v>
       </c>
       <c r="D61" s="20">
-        <v>85.05</v>
+        <v>74.55</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,13 +3152,13 @@
         <v>65</v>
       </c>
       <c r="B63" s="18">
-        <v>55.5</v>
+        <v>49.5</v>
       </c>
       <c r="C63" s="19">
         <v>2.1</v>
       </c>
       <c r="D63" s="20">
-        <v>116.55</v>
+        <v>103.95</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,13 +3166,13 @@
         <v>66</v>
       </c>
       <c r="B64" s="18">
-        <v>414.5</v>
+        <v>411.5</v>
       </c>
       <c r="C64" s="19">
         <v>2.1</v>
       </c>
       <c r="D64" s="20">
-        <v>870.45</v>
+        <v>864.15</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,13 +3194,13 @@
         <v>68</v>
       </c>
       <c r="B66" s="18">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="C66" s="19">
         <v>0.52</v>
       </c>
       <c r="D66" s="20">
-        <v>153.4</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3208,13 +3208,13 @@
         <v>69</v>
       </c>
       <c r="B67" s="18">
-        <v>273</v>
+        <v>253</v>
       </c>
       <c r="C67" s="19">
         <v>0.52</v>
       </c>
       <c r="D67" s="20">
-        <v>141.96</v>
+        <v>131.56</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3222,13 +3222,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="18">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="C68" s="19">
         <v>0.7</v>
       </c>
       <c r="D68" s="20">
-        <v>158.9</v>
+        <v>144.9</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,13 +3236,13 @@
         <v>71</v>
       </c>
       <c r="B69" s="18">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="C69" s="19">
         <v>0.7</v>
       </c>
       <c r="D69" s="20">
-        <v>135.80000000000001</v>
+        <v>121.8</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,13 +3250,13 @@
         <v>72</v>
       </c>
       <c r="B70" s="18">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C70" s="19">
         <v>0.9</v>
       </c>
       <c r="D70" s="20">
-        <v>105.3</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,13 +3264,13 @@
         <v>73</v>
       </c>
       <c r="B71" s="18">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C71" s="19">
         <v>0.9</v>
       </c>
       <c r="D71" s="20">
-        <v>126.9</v>
+        <v>117.9</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,13 +3278,13 @@
         <v>74</v>
       </c>
       <c r="B72" s="18">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C72" s="19">
         <v>1.55</v>
       </c>
       <c r="D72" s="20">
-        <v>826.15</v>
+        <v>810.65</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3292,13 +3292,13 @@
         <v>75</v>
       </c>
       <c r="B73" s="18">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="C73" s="19">
         <v>1.55</v>
       </c>
       <c r="D73" s="20">
-        <v>888.15</v>
+        <v>872.65</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,13 +3306,13 @@
         <v>76</v>
       </c>
       <c r="B74" s="18">
-        <v>715.5</v>
+        <v>705.5</v>
       </c>
       <c r="C74" s="19">
         <v>1.55</v>
       </c>
       <c r="D74" s="20">
-        <v>1109.03</v>
+        <v>1093.53</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="18">
-        <v>108.5</v>
+        <v>177.5</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="21"/>
@@ -3330,7 +3330,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="18">
-        <v>-22.5</v>
+        <v>27.5</v>
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="21"/>
@@ -3370,7 +3370,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="18">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
@@ -3408,13 +3408,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>-2</v>
+        <v>152</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>-2.8</v>
+        <v>212.8</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,13 +3422,13 @@
         <v>86</v>
       </c>
       <c r="B84" s="18">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C84" s="19">
         <v>1.4</v>
       </c>
       <c r="D84" s="20">
-        <v>191.8</v>
+        <v>184.8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3458,13 +3458,13 @@
         <v>89</v>
       </c>
       <c r="B87" s="18">
-        <v>-14.5</v>
+        <v>85.5</v>
       </c>
       <c r="C87" s="19">
         <v>2</v>
       </c>
       <c r="D87" s="20">
-        <v>-29</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3472,13 +3472,13 @@
         <v>90</v>
       </c>
       <c r="B88" s="18">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C88" s="19">
         <v>2</v>
       </c>
       <c r="D88" s="20">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3486,13 +3486,13 @@
         <v>91</v>
       </c>
       <c r="B89" s="18">
-        <v>244</v>
+        <v>520</v>
       </c>
       <c r="C89" s="19">
-        <v>1.26</v>
+        <v>1.21</v>
       </c>
       <c r="D89" s="20">
-        <v>307.44</v>
+        <v>629.05999999999995</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3500,13 +3500,13 @@
         <v>92</v>
       </c>
       <c r="B90" s="18">
-        <v>225.5</v>
+        <v>513.5</v>
       </c>
       <c r="C90" s="19">
-        <v>1.26</v>
+        <v>1.21</v>
       </c>
       <c r="D90" s="20">
-        <v>284.13</v>
+        <v>621.1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3636,13 +3636,13 @@
         <v>103</v>
       </c>
       <c r="B101" s="18">
-        <v>4.5</v>
+        <v>1</v>
       </c>
       <c r="C101" s="19">
         <v>12.5</v>
       </c>
       <c r="D101" s="20">
-        <v>56.25</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,13 +3650,13 @@
         <v>104</v>
       </c>
       <c r="B102" s="18">
-        <v>9.5</v>
+        <v>5.5</v>
       </c>
       <c r="C102" s="19">
         <v>12.5</v>
       </c>
       <c r="D102" s="20">
-        <v>118.75</v>
+        <v>68.75</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3720,13 +3720,13 @@
         <v>109</v>
       </c>
       <c r="B107" s="18">
-        <v>9.86</v>
+        <v>7.36</v>
       </c>
       <c r="C107" s="19">
         <v>12.5</v>
       </c>
       <c r="D107" s="20">
-        <v>123.25</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,13 +3734,13 @@
         <v>110</v>
       </c>
       <c r="B108" s="18">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="C108" s="19">
         <v>12.5</v>
       </c>
       <c r="D108" s="20">
-        <v>106.25</v>
+        <v>81.25</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3748,13 +3748,13 @@
         <v>111</v>
       </c>
       <c r="B109" s="18">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C109" s="19">
         <v>12.5</v>
       </c>
       <c r="D109" s="20">
-        <v>400</v>
+        <v>337.5</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,22 +4056,28 @@
         <v>133</v>
       </c>
       <c r="B131" s="18">
-        <v>1.5</v>
+        <v>-2.5</v>
       </c>
       <c r="C131" s="19">
         <v>18.27</v>
       </c>
       <c r="D131" s="20">
-        <v>27.4</v>
+        <v>-45.67</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B132" s="21"/>
-      <c r="C132" s="22"/>
-      <c r="D132" s="21"/>
+      <c r="B132" s="18">
+        <v>-2.5</v>
+      </c>
+      <c r="C132" s="19">
+        <v>18.27</v>
+      </c>
+      <c r="D132" s="20">
+        <v>-45.67</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
@@ -4246,13 +4252,13 @@
         <v>147</v>
       </c>
       <c r="B145" s="18">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C145" s="19">
         <v>3.4</v>
       </c>
       <c r="D145" s="20">
-        <v>295.8</v>
+        <v>285.60000000000002</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4288,13 +4294,13 @@
         <v>150</v>
       </c>
       <c r="B148" s="18">
-        <v>105.5</v>
+        <v>101</v>
       </c>
       <c r="C148" s="19">
         <v>2.8</v>
       </c>
       <c r="D148" s="20">
-        <v>295.39999999999998</v>
+        <v>282.8</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,13 +4308,13 @@
         <v>151</v>
       </c>
       <c r="B149" s="18">
-        <v>108</v>
+        <v>103.5</v>
       </c>
       <c r="C149" s="19">
         <v>2.8</v>
       </c>
       <c r="D149" s="20">
-        <v>302.39999999999998</v>
+        <v>289.8</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4386,13 +4392,13 @@
         <v>157</v>
       </c>
       <c r="B155" s="18">
-        <v>84</v>
+        <v>81.5</v>
       </c>
       <c r="C155" s="19">
         <v>2.95</v>
       </c>
       <c r="D155" s="20">
-        <v>247.8</v>
+        <v>240.43</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4534,13 +4540,13 @@
         <v>168</v>
       </c>
       <c r="B166" s="18">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C166" s="19">
         <v>3.33</v>
       </c>
       <c r="D166" s="20">
-        <v>329.67</v>
+        <v>326.33999999999997</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4626,13 +4632,13 @@
         <v>175</v>
       </c>
       <c r="B173" s="18">
-        <v>37.5</v>
+        <v>150.5</v>
       </c>
       <c r="C173" s="19">
         <v>4.5</v>
       </c>
       <c r="D173" s="20">
-        <v>168.75</v>
+        <v>677.25</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4696,13 +4702,13 @@
         <v>180</v>
       </c>
       <c r="B178" s="18">
-        <v>15</v>
+        <v>15.5</v>
       </c>
       <c r="C178" s="19">
         <v>4.5</v>
       </c>
       <c r="D178" s="20">
-        <v>67.5</v>
+        <v>69.75</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4838,13 +4844,13 @@
         <v>191</v>
       </c>
       <c r="B189" s="18">
-        <v>52.24</v>
+        <v>50.24</v>
       </c>
       <c r="C189" s="19">
         <v>3.05</v>
       </c>
       <c r="D189" s="20">
-        <v>159.33000000000001</v>
+        <v>153.22999999999999</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4912,13 +4918,13 @@
         <v>198</v>
       </c>
       <c r="B196" s="18">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C196" s="19">
         <v>3.8</v>
       </c>
       <c r="D196" s="20">
-        <v>98.8</v>
+        <v>79.8</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4976,13 +4982,13 @@
         <v>203</v>
       </c>
       <c r="B201" s="18">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C201" s="19">
         <v>4.0999999999999996</v>
       </c>
       <c r="D201" s="20">
-        <v>176.3</v>
+        <v>159.9</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4990,13 +4996,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>86.5</v>
+        <v>86</v>
       </c>
       <c r="C202" s="19">
         <v>4.1100000000000003</v>
       </c>
       <c r="D202" s="20">
-        <v>355.34</v>
+        <v>353.29</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5046,13 +5052,13 @@
         <v>208</v>
       </c>
       <c r="B206" s="18">
-        <v>92</v>
+        <v>73.5</v>
       </c>
       <c r="C206" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D206" s="20">
-        <v>404.8</v>
+        <v>323.39999999999998</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5096,13 +5102,13 @@
         <v>212</v>
       </c>
       <c r="B210" s="18">
-        <v>-14.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C210" s="19">
         <v>4.5</v>
       </c>
       <c r="D210" s="20">
-        <v>-65.25</v>
+        <v>-78.75</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5110,13 +5116,13 @@
         <v>213</v>
       </c>
       <c r="B211" s="18">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C211" s="19">
         <v>4.5</v>
       </c>
       <c r="D211" s="20">
-        <v>508.5</v>
+        <v>504</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5124,13 +5130,13 @@
         <v>214</v>
       </c>
       <c r="B212" s="18">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C212" s="19">
         <v>5.25</v>
       </c>
       <c r="D212" s="20">
-        <v>220.5</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5166,13 +5172,13 @@
         <v>217</v>
       </c>
       <c r="B215" s="18">
-        <v>71.5</v>
+        <v>69.5</v>
       </c>
       <c r="C215" s="19">
         <v>4.5</v>
       </c>
       <c r="D215" s="20">
-        <v>321.75</v>
+        <v>312.75</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5222,13 +5228,13 @@
         <v>221</v>
       </c>
       <c r="B219" s="18">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C219" s="19">
         <v>5.25</v>
       </c>
       <c r="D219" s="20">
-        <v>304.5</v>
+        <v>283.5</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5250,13 +5256,13 @@
         <v>223</v>
       </c>
       <c r="B221" s="18">
-        <v>86.5</v>
+        <v>72.5</v>
       </c>
       <c r="C221" s="19">
         <v>4.75</v>
       </c>
       <c r="D221" s="20">
-        <v>410.88</v>
+        <v>344.38</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5299,15 +5305,9 @@
       <c r="A225" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B225" s="18">
-        <v>-8</v>
-      </c>
-      <c r="C225" s="19">
-        <v>6</v>
-      </c>
-      <c r="D225" s="20">
-        <v>-48</v>
-      </c>
+      <c r="B225" s="21"/>
+      <c r="C225" s="22"/>
+      <c r="D225" s="21"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="17" t="s">
@@ -5322,13 +5322,13 @@
         <v>229</v>
       </c>
       <c r="B227" s="18">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C227" s="19">
         <v>5.7</v>
       </c>
       <c r="D227" s="20">
-        <v>96.9</v>
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5378,13 +5378,13 @@
         <v>233</v>
       </c>
       <c r="B231" s="18">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C231" s="19">
         <v>5.96</v>
       </c>
       <c r="D231" s="20">
-        <v>423.45</v>
+        <v>387.67</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5504,13 +5504,13 @@
         <v>242</v>
       </c>
       <c r="B240" s="18">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C240" s="19">
         <v>3.5</v>
       </c>
       <c r="D240" s="20">
-        <v>224</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5518,13 +5518,13 @@
         <v>243</v>
       </c>
       <c r="B241" s="18">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C241" s="19">
         <v>4.25</v>
       </c>
       <c r="D241" s="20">
-        <v>837.25</v>
+        <v>811.75</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5554,13 +5554,13 @@
         <v>246</v>
       </c>
       <c r="B244" s="18">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C244" s="19">
         <v>4.18</v>
       </c>
       <c r="D244" s="20">
-        <v>271.7</v>
+        <v>259.16000000000003</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -5582,13 +5582,13 @@
         <v>248</v>
       </c>
       <c r="B246" s="18">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C246" s="19">
         <v>4.28</v>
       </c>
       <c r="D246" s="20">
-        <v>535</v>
+        <v>530.72</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5596,13 +5596,13 @@
         <v>249</v>
       </c>
       <c r="B247" s="18">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C247" s="19">
         <v>4.28</v>
       </c>
       <c r="D247" s="20">
-        <v>342.4</v>
+        <v>333.84</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5696,13 +5696,13 @@
         <v>257</v>
       </c>
       <c r="B255" s="18">
-        <v>21.5</v>
+        <v>15</v>
       </c>
       <c r="C255" s="19">
         <v>5.0999999999999996</v>
       </c>
       <c r="D255" s="20">
-        <v>109.65</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -5724,13 +5724,13 @@
         <v>259</v>
       </c>
       <c r="B257" s="18">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C257" s="19">
         <v>5.4</v>
       </c>
       <c r="D257" s="20">
-        <v>243</v>
+        <v>237.6</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -5886,13 +5886,13 @@
         <v>271</v>
       </c>
       <c r="B269" s="18">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C269" s="19">
         <v>5.94</v>
       </c>
       <c r="D269" s="20">
-        <v>249.48</v>
+        <v>457.38</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,13 +5942,13 @@
         <v>275</v>
       </c>
       <c r="B273" s="18">
-        <v>28.5</v>
+        <v>25.5</v>
       </c>
       <c r="C273" s="19">
-        <v>6.6</v>
+        <v>6.59</v>
       </c>
       <c r="D273" s="20">
-        <v>187.96</v>
+        <v>168.17</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -5964,13 +5964,13 @@
         <v>277</v>
       </c>
       <c r="B275" s="18">
-        <v>48</v>
+        <v>45.5</v>
       </c>
       <c r="C275" s="19">
         <v>6.18</v>
       </c>
       <c r="D275" s="20">
-        <v>296.64</v>
+        <v>281.19</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -6070,13 +6070,13 @@
         <v>285</v>
       </c>
       <c r="B283" s="18">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C283" s="19">
         <v>6.4</v>
       </c>
       <c r="D283" s="20">
-        <v>198.4</v>
+        <v>179.2</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,13 +6092,13 @@
         <v>287</v>
       </c>
       <c r="B285" s="18">
-        <v>48</v>
+        <v>44.5</v>
       </c>
       <c r="C285" s="19">
         <v>6.65</v>
       </c>
       <c r="D285" s="20">
-        <v>319.2</v>
+        <v>295.93</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -6106,13 +6106,13 @@
         <v>288</v>
       </c>
       <c r="B286" s="18">
-        <v>31.5</v>
+        <v>31</v>
       </c>
       <c r="C286" s="19">
         <v>6.18</v>
       </c>
       <c r="D286" s="20">
-        <v>194.67</v>
+        <v>191.58</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -6128,13 +6128,13 @@
         <v>290</v>
       </c>
       <c r="B288" s="18">
-        <v>33.5</v>
+        <v>32.5</v>
       </c>
       <c r="C288" s="19">
         <v>7.18</v>
       </c>
       <c r="D288" s="20">
-        <v>240.46</v>
+        <v>233.28</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6156,13 +6156,13 @@
         <v>292</v>
       </c>
       <c r="B290" s="18">
-        <v>88</v>
+        <v>85.5</v>
       </c>
       <c r="C290" s="19">
         <v>7.13</v>
       </c>
       <c r="D290" s="20">
-        <v>627.44000000000005</v>
+        <v>609.62</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6184,13 +6184,13 @@
         <v>294</v>
       </c>
       <c r="B292" s="18">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C292" s="19">
         <v>6.65</v>
       </c>
       <c r="D292" s="20">
-        <v>66.5</v>
+        <v>219.45</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6206,13 +6206,13 @@
         <v>296</v>
       </c>
       <c r="B294" s="18">
-        <v>37.5</v>
+        <v>36</v>
       </c>
       <c r="C294" s="19">
         <v>7.6</v>
       </c>
       <c r="D294" s="20">
-        <v>285</v>
+        <v>273.60000000000002</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6270,13 +6270,13 @@
         <v>301</v>
       </c>
       <c r="B299" s="18">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C299" s="19">
         <v>8.08</v>
       </c>
       <c r="D299" s="20">
-        <v>96.96</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6376,13 +6376,13 @@
         <v>309</v>
       </c>
       <c r="B307" s="18">
-        <v>14.5</v>
+        <v>10.5</v>
       </c>
       <c r="C307" s="19">
         <v>9.25</v>
       </c>
       <c r="D307" s="20">
-        <v>134.13</v>
+        <v>97.13</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6404,13 +6404,13 @@
         <v>311</v>
       </c>
       <c r="B309" s="18">
-        <v>34</v>
+        <v>33.5</v>
       </c>
       <c r="C309" s="19">
         <v>9.31</v>
       </c>
       <c r="D309" s="20">
-        <v>316.63</v>
+        <v>311.97000000000003</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.25">
@@ -6432,13 +6432,13 @@
         <v>313</v>
       </c>
       <c r="B311" s="18">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C311" s="19">
         <v>9.5</v>
       </c>
       <c r="D311" s="20">
-        <v>180.5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6446,13 +6446,13 @@
         <v>314</v>
       </c>
       <c r="B312" s="18">
-        <v>17.5</v>
+        <v>15.5</v>
       </c>
       <c r="C312" s="19">
         <v>10</v>
       </c>
       <c r="D312" s="20">
-        <v>175</v>
+        <v>155</v>
       </c>
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.25">
@@ -6474,13 +6474,13 @@
         <v>316</v>
       </c>
       <c r="B314" s="18">
-        <v>11</v>
+        <v>-1</v>
       </c>
       <c r="C314" s="19">
         <v>9.25</v>
       </c>
       <c r="D314" s="20">
-        <v>101.75</v>
+        <v>-9.25</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -6572,13 +6572,13 @@
         <v>323</v>
       </c>
       <c r="B321" s="18">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C321" s="19">
         <v>7.13</v>
       </c>
       <c r="D321" s="20">
-        <v>171.12</v>
+        <v>163.99</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -6600,13 +6600,13 @@
         <v>325</v>
       </c>
       <c r="B323" s="18">
-        <v>30</v>
+        <v>28.5</v>
       </c>
       <c r="C323" s="19">
         <v>8.5</v>
       </c>
       <c r="D323" s="20">
-        <v>255</v>
+        <v>242.25</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -6656,13 +6656,13 @@
         <v>329</v>
       </c>
       <c r="B327" s="18">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C327" s="19">
         <v>6.9</v>
       </c>
       <c r="D327" s="20">
-        <v>89.7</v>
+        <v>82.8</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6714,13 +6714,13 @@
         <v>334</v>
       </c>
       <c r="B332" s="18">
-        <v>20</v>
+        <v>14.5</v>
       </c>
       <c r="C332" s="19">
         <v>4.9000000000000004</v>
       </c>
       <c r="D332" s="20">
-        <v>98</v>
+        <v>71.05</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -6742,13 +6742,13 @@
         <v>336</v>
       </c>
       <c r="B334" s="18">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C334" s="19">
         <v>7.36</v>
       </c>
       <c r="D334" s="20">
-        <v>117.76</v>
+        <v>103.04</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -6882,13 +6882,13 @@
         <v>346</v>
       </c>
       <c r="B344" s="18">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="C344" s="19">
         <v>18</v>
       </c>
       <c r="D344" s="20">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -6938,13 +6938,13 @@
         <v>350</v>
       </c>
       <c r="B348" s="18">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C348" s="19">
         <v>39</v>
       </c>
       <c r="D348" s="20">
-        <v>390</v>
+        <v>273</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -6952,13 +6952,13 @@
         <v>351</v>
       </c>
       <c r="B349" s="18">
-        <v>13.99</v>
+        <v>12.99</v>
       </c>
       <c r="C349" s="19">
         <v>12</v>
       </c>
       <c r="D349" s="20">
-        <v>167.88</v>
+        <v>155.88</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -7064,13 +7064,13 @@
         <v>359</v>
       </c>
       <c r="B357" s="18">
-        <v>5.73</v>
+        <v>0.23</v>
       </c>
       <c r="C357" s="19">
         <v>10</v>
       </c>
       <c r="D357" s="20">
-        <v>57.3</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -7148,13 +7148,13 @@
         <v>365</v>
       </c>
       <c r="B363" s="18">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C363" s="19">
         <v>9.5</v>
       </c>
       <c r="D363" s="20">
-        <v>256.5</v>
+        <v>237.5</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -7162,13 +7162,13 @@
         <v>366</v>
       </c>
       <c r="B364" s="18">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="C364" s="19">
         <v>15</v>
       </c>
       <c r="D364" s="20">
-        <v>82.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7176,13 +7176,13 @@
         <v>367</v>
       </c>
       <c r="B365" s="18">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="C365" s="19">
         <v>10</v>
       </c>
       <c r="D365" s="20">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7204,13 +7204,13 @@
         <v>369</v>
       </c>
       <c r="B367" s="18">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="C367" s="19">
         <v>17</v>
       </c>
       <c r="D367" s="20">
-        <v>170</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -7232,13 +7232,13 @@
         <v>371</v>
       </c>
       <c r="B369" s="18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C369" s="19">
         <v>25</v>
       </c>
       <c r="D369" s="20">
-        <v>150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7260,13 +7260,13 @@
         <v>373</v>
       </c>
       <c r="B371" s="18">
-        <v>34.5</v>
+        <v>35.5</v>
       </c>
       <c r="C371" s="19">
         <v>10.93</v>
       </c>
       <c r="D371" s="20">
-        <v>377.09</v>
+        <v>388.02</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7302,13 +7302,13 @@
         <v>376</v>
       </c>
       <c r="B374" s="18">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="C374" s="19">
         <v>21.5</v>
       </c>
       <c r="D374" s="20">
-        <v>64.5</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,13 +7330,13 @@
         <v>378</v>
       </c>
       <c r="B376" s="18">
-        <v>38.25</v>
+        <v>34.75</v>
       </c>
       <c r="C376" s="19">
         <v>11.5</v>
       </c>
       <c r="D376" s="20">
-        <v>439.88</v>
+        <v>399.63</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7358,13 +7358,13 @@
         <v>380</v>
       </c>
       <c r="B378" s="18">
-        <v>12.5</v>
+        <v>4.5</v>
       </c>
       <c r="C378" s="19">
         <v>11.4</v>
       </c>
       <c r="D378" s="20">
-        <v>142.5</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
@@ -7428,13 +7428,13 @@
         <v>385</v>
       </c>
       <c r="B383" s="18">
-        <v>40.5</v>
+        <v>38.5</v>
       </c>
       <c r="C383" s="19">
         <v>10.93</v>
       </c>
       <c r="D383" s="20">
-        <v>442.67</v>
+        <v>420.81</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -7484,13 +7484,13 @@
         <v>389</v>
       </c>
       <c r="B387" s="18">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
       <c r="C387" s="19">
         <v>10.45</v>
       </c>
       <c r="D387" s="20">
-        <v>130.63</v>
+        <v>15.68</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -7498,13 +7498,13 @@
         <v>390</v>
       </c>
       <c r="B388" s="18">
-        <v>0.5</v>
+        <v>-5</v>
       </c>
       <c r="C388" s="19">
-        <v>10.46</v>
+        <v>10.45</v>
       </c>
       <c r="D388" s="20">
-        <v>5.23</v>
+        <v>-52.25</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -7732,13 +7732,13 @@
         <v>408</v>
       </c>
       <c r="B406" s="18">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C406" s="19">
         <v>2.75</v>
       </c>
       <c r="D406" s="20">
-        <v>115.5</v>
+        <v>112.75</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -7796,13 +7796,13 @@
         <v>413</v>
       </c>
       <c r="B411" s="18">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C411" s="19">
         <v>2.8</v>
       </c>
       <c r="D411" s="20">
-        <v>187.6</v>
+        <v>184.8</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
@@ -7908,13 +7908,13 @@
         <v>421</v>
       </c>
       <c r="B419" s="18">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="C419" s="19">
         <v>3.25</v>
       </c>
       <c r="D419" s="20">
-        <v>60.13</v>
+        <v>53.63</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
@@ -7958,13 +7958,13 @@
         <v>425</v>
       </c>
       <c r="B423" s="18">
-        <v>34.5</v>
+        <v>30.5</v>
       </c>
       <c r="C423" s="19">
         <v>3.4</v>
       </c>
       <c r="D423" s="20">
-        <v>117.3</v>
+        <v>103.7</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -8014,13 +8014,13 @@
         <v>429</v>
       </c>
       <c r="B427" s="18">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C427" s="19">
         <v>3.33</v>
       </c>
       <c r="D427" s="20">
-        <v>133.19999999999999</v>
+        <v>126.54</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
@@ -8072,13 +8072,13 @@
         <v>434</v>
       </c>
       <c r="B432" s="18">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C432" s="19">
         <v>4.25</v>
       </c>
       <c r="D432" s="20">
-        <v>174.25</v>
+        <v>170</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
@@ -8114,13 +8114,13 @@
         <v>437</v>
       </c>
       <c r="B435" s="18">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="C435" s="19">
         <v>4.25</v>
       </c>
       <c r="D435" s="20">
-        <v>70.13</v>
+        <v>63.75</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -8418,13 +8418,13 @@
         <v>460</v>
       </c>
       <c r="B458" s="18">
-        <v>54.5</v>
+        <v>52</v>
       </c>
       <c r="C458" s="19">
         <v>7.13</v>
       </c>
       <c r="D458" s="20">
-        <v>388.59</v>
+        <v>370.76</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -8446,13 +8446,13 @@
         <v>462</v>
       </c>
       <c r="B460" s="18">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C460" s="19">
         <v>7</v>
       </c>
       <c r="D460" s="20">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -8460,13 +8460,13 @@
         <v>463</v>
       </c>
       <c r="B461" s="18">
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="C461" s="19">
         <v>7.6</v>
       </c>
       <c r="D461" s="20">
-        <v>304</v>
+        <v>285</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -8566,13 +8566,13 @@
         <v>471</v>
       </c>
       <c r="B469" s="18">
-        <v>20.5</v>
+        <v>18.5</v>
       </c>
       <c r="C469" s="19">
         <v>9.5</v>
       </c>
       <c r="D469" s="20">
-        <v>194.75</v>
+        <v>175.75</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -8650,13 +8650,13 @@
         <v>477</v>
       </c>
       <c r="B475" s="18">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C475" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D475" s="20">
-        <v>88</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
@@ -8664,13 +8664,13 @@
         <v>478</v>
       </c>
       <c r="B476" s="18">
-        <v>51.5</v>
+        <v>49.5</v>
       </c>
       <c r="C476" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D476" s="20">
-        <v>56.65</v>
+        <v>54.45</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -8700,13 +8700,13 @@
         <v>481</v>
       </c>
       <c r="B479" s="18">
-        <v>150.5</v>
+        <v>149.5</v>
       </c>
       <c r="C479" s="19">
         <v>1.4</v>
       </c>
       <c r="D479" s="20">
-        <v>210.7</v>
+        <v>209.3</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -8728,13 +8728,13 @@
         <v>483</v>
       </c>
       <c r="B481" s="18">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="C481" s="19">
         <v>3</v>
       </c>
       <c r="D481" s="20">
-        <v>67.5</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
@@ -8784,13 +8784,13 @@
         <v>487</v>
       </c>
       <c r="B485" s="18">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C485" s="19">
         <v>1.5</v>
       </c>
       <c r="D485" s="20">
-        <v>325.5</v>
+        <v>324</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
@@ -8798,13 +8798,13 @@
         <v>488</v>
       </c>
       <c r="B486" s="18">
-        <v>220.5</v>
+        <v>217.5</v>
       </c>
       <c r="C486" s="19">
         <v>1.5</v>
       </c>
       <c r="D486" s="20">
-        <v>330.75</v>
+        <v>326.25</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
@@ -8868,13 +8868,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>69.5</v>
+        <v>60</v>
       </c>
       <c r="C491" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D491" s="20">
-        <v>158.46</v>
+        <v>136.80000000000001</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -9052,13 +9052,13 @@
         <v>507</v>
       </c>
       <c r="B505" s="18">
-        <v>20.5</v>
+        <v>60.5</v>
       </c>
       <c r="C505" s="19">
         <v>3.25</v>
       </c>
       <c r="D505" s="20">
-        <v>66.63</v>
+        <v>196.63</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
@@ -9124,13 +9124,13 @@
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>66.5</v>
+        <v>61.5</v>
       </c>
       <c r="C511" s="19">
         <v>3.33</v>
       </c>
       <c r="D511" s="20">
-        <v>221.45</v>
+        <v>204.8</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9196,13 +9196,13 @@
         <v>519</v>
       </c>
       <c r="B517" s="18">
-        <v>19.5</v>
+        <v>14.5</v>
       </c>
       <c r="C517" s="19">
         <v>3.6</v>
       </c>
       <c r="D517" s="20">
-        <v>70.2</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
@@ -9260,13 +9260,13 @@
         <v>524</v>
       </c>
       <c r="B522" s="18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C522" s="19">
         <v>4</v>
       </c>
       <c r="D522" s="20">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
@@ -9330,13 +9330,13 @@
         <v>529</v>
       </c>
       <c r="B527" s="18">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C527" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D527" s="20">
-        <v>79.2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
@@ -9358,13 +9358,13 @@
         <v>531</v>
       </c>
       <c r="B529" s="18">
-        <v>27</v>
+        <v>24.5</v>
       </c>
       <c r="C529" s="19">
         <v>4.75</v>
       </c>
       <c r="D529" s="20">
-        <v>128.25</v>
+        <v>116.38</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
@@ -9428,13 +9428,13 @@
         <v>536</v>
       </c>
       <c r="B534" s="18">
-        <v>16.5</v>
+        <v>26.5</v>
       </c>
       <c r="C534" s="19">
         <v>5</v>
       </c>
       <c r="D534" s="20">
-        <v>82.5</v>
+        <v>132.5</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
@@ -9470,13 +9470,13 @@
         <v>539</v>
       </c>
       <c r="B537" s="18">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C537" s="19">
         <v>5</v>
       </c>
       <c r="D537" s="20">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
@@ -9716,13 +9716,13 @@
         <v>557</v>
       </c>
       <c r="B555" s="18">
-        <v>7.5</v>
+        <v>19.5</v>
       </c>
       <c r="C555" s="19">
         <v>8.75</v>
       </c>
       <c r="D555" s="20">
-        <v>65.63</v>
+        <v>170.63</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
@@ -9752,13 +9752,13 @@
         <v>560</v>
       </c>
       <c r="B558" s="18">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C558" s="19">
         <v>2.76</v>
       </c>
       <c r="D558" s="20">
-        <v>228.79</v>
+        <v>220.52</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
@@ -9766,13 +9766,13 @@
         <v>561</v>
       </c>
       <c r="B559" s="18">
-        <v>81.5</v>
+        <v>74</v>
       </c>
       <c r="C559" s="19">
         <v>2.76</v>
       </c>
       <c r="D559" s="20">
-        <v>224.55</v>
+        <v>203.89</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
@@ -9780,13 +9780,13 @@
         <v>562</v>
       </c>
       <c r="B560" s="18">
-        <v>112.5</v>
+        <v>109.5</v>
       </c>
       <c r="C560" s="19">
         <v>2.76</v>
       </c>
       <c r="D560" s="20">
-        <v>310.5</v>
+        <v>302.22000000000003</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
@@ -9836,13 +9836,13 @@
         <v>566</v>
       </c>
       <c r="B564" s="18">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C564" s="19">
         <v>2.76</v>
       </c>
       <c r="D564" s="20">
-        <v>182.16</v>
+        <v>126.96</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.25">
@@ -9850,13 +9850,13 @@
         <v>567</v>
       </c>
       <c r="B565" s="18">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="C565" s="19">
         <v>2.76</v>
       </c>
       <c r="D565" s="20">
-        <v>122.82</v>
+        <v>120.06</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
@@ -9892,13 +9892,13 @@
         <v>570</v>
       </c>
       <c r="B568" s="18">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C568" s="19">
         <v>3</v>
       </c>
       <c r="D568" s="20">
-        <v>222</v>
+        <v>216</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
@@ -9906,13 +9906,13 @@
         <v>571</v>
       </c>
       <c r="B569" s="18">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C569" s="19">
         <v>3.1</v>
       </c>
       <c r="D569" s="20">
-        <v>158.1</v>
+        <v>124</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
@@ -10004,13 +10004,13 @@
         <v>578</v>
       </c>
       <c r="B576" s="18">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C576" s="19">
         <v>5.01</v>
       </c>
       <c r="D576" s="20">
-        <v>165.48</v>
+        <v>145.43</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.25">
@@ -10032,13 +10032,13 @@
         <v>580</v>
       </c>
       <c r="B578" s="18">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C578" s="19">
         <v>1.96</v>
       </c>
       <c r="D578" s="20">
-        <v>27.46</v>
+        <v>17.649999999999999</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.25">
@@ -10046,13 +10046,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>250.5</v>
+        <v>249</v>
       </c>
       <c r="C579" s="19">
         <v>1.93</v>
       </c>
       <c r="D579" s="20">
-        <v>483.47</v>
+        <v>480.57</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10060,13 +10060,13 @@
         <v>582</v>
       </c>
       <c r="B580" s="18">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C580" s="19">
         <v>2.79</v>
       </c>
       <c r="D580" s="20">
-        <v>382.42</v>
+        <v>362.88</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
@@ -10102,13 +10102,13 @@
         <v>585</v>
       </c>
       <c r="B583" s="18">
-        <v>68.5</v>
+        <v>62.5</v>
       </c>
       <c r="C583" s="19">
         <v>4.05</v>
       </c>
       <c r="D583" s="20">
-        <v>277.43</v>
+        <v>253.13</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
@@ -10116,13 +10116,13 @@
         <v>586</v>
       </c>
       <c r="B584" s="18">
-        <v>105.5</v>
+        <v>104.5</v>
       </c>
       <c r="C584" s="19">
         <v>4.05</v>
       </c>
       <c r="D584" s="20">
-        <v>427.28</v>
+        <v>423.23</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
@@ -10130,13 +10130,13 @@
         <v>587</v>
       </c>
       <c r="B585" s="18">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C585" s="19">
         <v>1.36</v>
       </c>
       <c r="D585" s="20">
-        <v>211.71</v>
+        <v>207.64</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
@@ -10158,13 +10158,13 @@
         <v>589</v>
       </c>
       <c r="B587" s="18">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C587" s="19">
         <v>1.37</v>
       </c>
       <c r="D587" s="20">
-        <v>143.99</v>
+        <v>128.9</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
@@ -10182,7 +10182,7 @@
         <v>591</v>
       </c>
       <c r="B589" s="18">
-        <v>40</v>
+        <v>37.5</v>
       </c>
       <c r="C589" s="22"/>
       <c r="D589" s="21"/>
@@ -10192,7 +10192,7 @@
         <v>592</v>
       </c>
       <c r="B590" s="18">
-        <v>51.5</v>
+        <v>49.5</v>
       </c>
       <c r="C590" s="22"/>
       <c r="D590" s="21"/>
@@ -10202,7 +10202,7 @@
         <v>593</v>
       </c>
       <c r="B591" s="18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C591" s="22"/>
       <c r="D591" s="21"/>
@@ -10212,13 +10212,13 @@
         <v>594</v>
       </c>
       <c r="B592" s="18">
-        <v>547.5</v>
+        <v>546.5</v>
       </c>
       <c r="C592" s="19">
         <v>0.8</v>
       </c>
       <c r="D592" s="20">
-        <v>438</v>
+        <v>437.2</v>
       </c>
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.25">
@@ -10254,13 +10254,13 @@
         <v>597</v>
       </c>
       <c r="B595" s="18">
-        <v>521.5</v>
+        <v>511.5</v>
       </c>
       <c r="C595" s="19">
         <v>0.8</v>
       </c>
       <c r="D595" s="20">
-        <v>417.2</v>
+        <v>409.2</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
@@ -10268,13 +10268,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="C596" s="19">
         <v>0.52</v>
       </c>
       <c r="D596" s="20">
-        <v>173.68</v>
+        <v>164.84</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10282,13 +10282,13 @@
         <v>599</v>
       </c>
       <c r="B597" s="18">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C597" s="19">
         <v>0.52</v>
       </c>
       <c r="D597" s="20">
-        <v>268.32</v>
+        <v>265.2</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.25">
@@ -10296,13 +10296,13 @@
         <v>600</v>
       </c>
       <c r="B598" s="18">
-        <v>859.5</v>
+        <v>853.5</v>
       </c>
       <c r="C598" s="19">
         <v>0.52</v>
       </c>
       <c r="D598" s="20">
-        <v>446.94</v>
+        <v>443.82</v>
       </c>
     </row>
     <row r="599" spans="1:4" x14ac:dyDescent="0.25">
@@ -10310,13 +10310,13 @@
         <v>601</v>
       </c>
       <c r="B599" s="18">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C599" s="19">
         <v>0.7</v>
       </c>
       <c r="D599" s="20">
-        <v>38.5</v>
+        <v>34.299999999999997</v>
       </c>
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.25">
@@ -10332,13 +10332,13 @@
         <v>603</v>
       </c>
       <c r="B601" s="18">
-        <v>549.5</v>
+        <v>536.5</v>
       </c>
       <c r="C601" s="19">
         <v>0.7</v>
       </c>
       <c r="D601" s="20">
-        <v>384.65</v>
+        <v>375.55</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.25">
@@ -10374,11 +10374,11 @@
         <v>606</v>
       </c>
       <c r="B604" s="24">
-        <v>33900.97</v>
+        <v>34405.97</v>
       </c>
       <c r="C604" s="25"/>
       <c r="D604" s="26">
-        <v>100769.98</v>
+        <v>100264.81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 1:17
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -2346,7 +2346,7 @@
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,13 +2432,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="18">
-        <v>742.5</v>
+        <v>722.5</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
       <c r="D9" s="20">
-        <v>742.5</v>
+        <v>722.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,13 +2446,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="18">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="C10" s="19">
         <v>1</v>
       </c>
       <c r="D10" s="20">
-        <v>324</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2886,13 +2886,13 @@
         <v>46</v>
       </c>
       <c r="B44" s="18">
-        <v>154.5</v>
+        <v>150.5</v>
       </c>
       <c r="C44" s="19">
         <v>2.25</v>
       </c>
       <c r="D44" s="20">
-        <v>347.63</v>
+        <v>338.63</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,13 +2970,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>153.5</v>
+        <v>133.5</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>168.85</v>
+        <v>146.85</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,13 +2998,13 @@
         <v>54</v>
       </c>
       <c r="B52" s="18">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="C52" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D52" s="20">
-        <v>199.1</v>
+        <v>177.1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,13 +3012,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="18">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="C53" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D53" s="20">
-        <v>96.8</v>
+        <v>52.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,13 +3026,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>64.900000000000006</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,7 +3350,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>74.5</v>
+        <v>72.5</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="21"/>
@@ -4378,13 +4378,13 @@
         <v>156</v>
       </c>
       <c r="B154" s="18">
-        <v>99.5</v>
+        <v>98</v>
       </c>
       <c r="C154" s="19">
         <v>2.95</v>
       </c>
       <c r="D154" s="20">
-        <v>293.52999999999997</v>
+        <v>289.10000000000002</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4392,13 +4392,13 @@
         <v>157</v>
       </c>
       <c r="B155" s="18">
-        <v>81.5</v>
+        <v>80</v>
       </c>
       <c r="C155" s="19">
         <v>2.95</v>
       </c>
       <c r="D155" s="20">
-        <v>240.43</v>
+        <v>236</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,13 +4996,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C202" s="19">
         <v>4.1100000000000003</v>
       </c>
       <c r="D202" s="20">
-        <v>353.29</v>
+        <v>349.18</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5130,13 +5130,13 @@
         <v>214</v>
       </c>
       <c r="B212" s="18">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C212" s="19">
         <v>5.25</v>
       </c>
       <c r="D212" s="20">
-        <v>199.5</v>
+        <v>189</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5322,13 +5322,13 @@
         <v>229</v>
       </c>
       <c r="B227" s="18">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C227" s="19">
         <v>5.7</v>
       </c>
       <c r="D227" s="20">
-        <v>68.400000000000006</v>
+        <v>57</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5406,13 +5406,13 @@
         <v>235</v>
       </c>
       <c r="B233" s="18">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="C233" s="19">
         <v>4</v>
       </c>
       <c r="D233" s="20">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5518,13 +5518,13 @@
         <v>243</v>
       </c>
       <c r="B241" s="18">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C241" s="19">
         <v>4.25</v>
       </c>
       <c r="D241" s="20">
-        <v>811.75</v>
+        <v>803.25</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -6390,13 +6390,13 @@
         <v>310</v>
       </c>
       <c r="B308" s="18">
-        <v>28.7</v>
+        <v>27.7</v>
       </c>
       <c r="C308" s="19">
         <v>8.8000000000000007</v>
       </c>
       <c r="D308" s="20">
-        <v>252.56</v>
+        <v>243.76</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -7880,13 +7880,13 @@
         <v>419</v>
       </c>
       <c r="B417" s="18">
-        <v>22.95</v>
+        <v>21.95</v>
       </c>
       <c r="C417" s="19">
         <v>3.15</v>
       </c>
       <c r="D417" s="20">
-        <v>72.290000000000006</v>
+        <v>69.14</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -9016,13 +9016,13 @@
         <v>504</v>
       </c>
       <c r="B502" s="18">
-        <v>45.5</v>
+        <v>44</v>
       </c>
       <c r="C502" s="19">
         <v>3.2</v>
       </c>
       <c r="D502" s="20">
-        <v>145.6</v>
+        <v>140.80000000000001</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
@@ -9124,13 +9124,13 @@
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>61.5</v>
+        <v>59.5</v>
       </c>
       <c r="C511" s="19">
         <v>3.33</v>
       </c>
       <c r="D511" s="20">
-        <v>204.8</v>
+        <v>198.14</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9892,13 +9892,13 @@
         <v>570</v>
       </c>
       <c r="B568" s="18">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C568" s="19">
         <v>3</v>
       </c>
       <c r="D568" s="20">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
@@ -10060,13 +10060,13 @@
         <v>582</v>
       </c>
       <c r="B580" s="18">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C580" s="19">
         <v>2.79</v>
       </c>
       <c r="D580" s="20">
-        <v>362.88</v>
+        <v>348.92</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
@@ -10130,13 +10130,13 @@
         <v>587</v>
       </c>
       <c r="B585" s="18">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C585" s="19">
         <v>1.36</v>
       </c>
       <c r="D585" s="20">
-        <v>207.64</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
@@ -10268,13 +10268,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>317</v>
+        <v>217</v>
       </c>
       <c r="C596" s="19">
         <v>0.52</v>
       </c>
       <c r="D596" s="20">
-        <v>164.84</v>
+        <v>112.84</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10282,13 +10282,13 @@
         <v>599</v>
       </c>
       <c r="B597" s="18">
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="C597" s="19">
         <v>0.52</v>
       </c>
       <c r="D597" s="20">
-        <v>265.2</v>
+        <v>213.2</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.25">
@@ -10374,11 +10374,11 @@
         <v>606</v>
       </c>
       <c r="B604" s="24">
-        <v>34405.97</v>
+        <v>34029.47</v>
       </c>
       <c r="C604" s="25"/>
       <c r="D604" s="26">
-        <v>100264.81</v>
+        <v>99898.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:39
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 14-Dec-2024</t>
+    <t>1-Jul-2024 to 16-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -2346,7 +2346,7 @@
     <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,13 +2432,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="18">
-        <v>722.5</v>
+        <v>712.5</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
       </c>
       <c r="D9" s="20">
-        <v>722.5</v>
+        <v>712.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2460,13 +2460,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>-146</v>
+        <v>252</v>
       </c>
       <c r="C11" s="19">
-        <v>0.98</v>
+        <v>0.92</v>
       </c>
       <c r="D11" s="20">
-        <v>-143.08000000000001</v>
+        <v>231.91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,13 +2474,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="18">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C12" s="19">
         <v>1.65</v>
       </c>
       <c r="D12" s="20">
-        <v>39.6</v>
+        <v>105.6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2516,13 +2516,13 @@
         <v>17</v>
       </c>
       <c r="B15" s="18">
-        <v>91.5</v>
+        <v>83.5</v>
       </c>
       <c r="C15" s="19">
         <v>1.8</v>
       </c>
       <c r="D15" s="20">
-        <v>164.7</v>
+        <v>150.30000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2572,22 +2572,28 @@
         <v>21</v>
       </c>
       <c r="B19" s="18">
-        <v>124</v>
+        <v>122.5</v>
       </c>
       <c r="C19" s="19">
         <v>2</v>
       </c>
       <c r="D19" s="20">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="18">
+        <v>140</v>
+      </c>
+      <c r="C20" s="19">
+        <v>2</v>
+      </c>
+      <c r="D20" s="20">
+        <v>280</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
@@ -2636,13 +2642,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24" s="19">
         <v>2.1</v>
       </c>
       <c r="D24" s="20">
-        <v>165.9</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2672,13 +2678,13 @@
         <v>29</v>
       </c>
       <c r="B27" s="18">
-        <v>88.72</v>
+        <v>84.72</v>
       </c>
       <c r="C27" s="19">
         <v>2.35</v>
       </c>
       <c r="D27" s="20">
-        <v>208.49</v>
+        <v>199.09</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2686,13 +2692,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="18">
-        <v>78.17</v>
+        <v>72.17</v>
       </c>
       <c r="C28" s="19">
         <v>2.35</v>
       </c>
       <c r="D28" s="20">
-        <v>183.7</v>
+        <v>169.6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2700,13 +2706,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="18">
-        <v>179.8</v>
+        <v>189.8</v>
       </c>
       <c r="C29" s="19">
-        <v>2.5099999999999998</v>
+        <v>2.59</v>
       </c>
       <c r="D29" s="20">
-        <v>452.18</v>
+        <v>490.77</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,13 +2822,13 @@
         <v>41</v>
       </c>
       <c r="B39" s="18">
-        <v>111</v>
+        <v>109.5</v>
       </c>
       <c r="C39" s="19">
         <v>2.7</v>
       </c>
       <c r="D39" s="20">
-        <v>299.7</v>
+        <v>295.64999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,13 +2976,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>133.5</v>
+        <v>153.5</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>146.85</v>
+        <v>168.85</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,13 +3004,13 @@
         <v>54</v>
       </c>
       <c r="B52" s="18">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C52" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D52" s="20">
-        <v>177.1</v>
+        <v>199.1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,13 +3018,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="18">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="C53" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D53" s="20">
-        <v>52.8</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,13 +3032,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>42.9</v>
+        <v>58.3</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3068,13 +3074,13 @@
         <v>59</v>
       </c>
       <c r="B57" s="18">
-        <v>604.5</v>
+        <v>599.5</v>
       </c>
       <c r="C57" s="19">
         <v>1.9</v>
       </c>
       <c r="D57" s="20">
-        <v>1148.55</v>
+        <v>1139.05</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,13 +3172,13 @@
         <v>66</v>
       </c>
       <c r="B64" s="18">
-        <v>411.5</v>
+        <v>407.5</v>
       </c>
       <c r="C64" s="19">
         <v>2.1</v>
       </c>
       <c r="D64" s="20">
-        <v>864.15</v>
+        <v>855.75</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,13 +3186,13 @@
         <v>67</v>
       </c>
       <c r="B65" s="18">
-        <v>457.5</v>
+        <v>456.5</v>
       </c>
       <c r="C65" s="19">
         <v>2.1</v>
       </c>
       <c r="D65" s="20">
-        <v>960.75</v>
+        <v>958.65</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,13 +3270,13 @@
         <v>73</v>
       </c>
       <c r="B71" s="18">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C71" s="19">
         <v>0.9</v>
       </c>
       <c r="D71" s="20">
-        <v>117.9</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,13 +3284,13 @@
         <v>74</v>
       </c>
       <c r="B72" s="18">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C72" s="19">
         <v>1.55</v>
       </c>
       <c r="D72" s="20">
-        <v>810.65</v>
+        <v>802.9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,13 +3312,13 @@
         <v>76</v>
       </c>
       <c r="B74" s="18">
-        <v>705.5</v>
+        <v>702.5</v>
       </c>
       <c r="C74" s="19">
         <v>1.55</v>
       </c>
       <c r="D74" s="20">
-        <v>1093.53</v>
+        <v>1088.8800000000001</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,7 +3326,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="18">
-        <v>177.5</v>
+        <v>175.5</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="21"/>
@@ -3330,7 +3336,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="18">
-        <v>27.5</v>
+        <v>7.5</v>
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="21"/>
@@ -3340,7 +3346,7 @@
         <v>79</v>
       </c>
       <c r="B77" s="18">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="21"/>
@@ -3350,7 +3356,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>72.5</v>
+        <v>69.5</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="21"/>
@@ -3360,7 +3366,7 @@
         <v>81</v>
       </c>
       <c r="B79" s="18">
-        <v>205.5</v>
+        <v>185.5</v>
       </c>
       <c r="C79" s="22"/>
       <c r="D79" s="21"/>
@@ -3370,7 +3376,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="18">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
@@ -3394,13 +3400,13 @@
         <v>84</v>
       </c>
       <c r="B82" s="18">
-        <v>544</v>
+        <v>532.5</v>
       </c>
       <c r="C82" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D82" s="20">
-        <v>625.6</v>
+        <v>612.38</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3408,13 +3414,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>212.8</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,13 +3428,13 @@
         <v>86</v>
       </c>
       <c r="B84" s="18">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C84" s="19">
         <v>1.4</v>
       </c>
       <c r="D84" s="20">
-        <v>184.8</v>
+        <v>170.8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3458,13 +3464,13 @@
         <v>89</v>
       </c>
       <c r="B87" s="18">
-        <v>85.5</v>
+        <v>58.5</v>
       </c>
       <c r="C87" s="19">
         <v>2</v>
       </c>
       <c r="D87" s="20">
-        <v>171</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3486,13 +3492,13 @@
         <v>91</v>
       </c>
       <c r="B89" s="18">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C89" s="19">
-        <v>1.21</v>
+        <v>1.26</v>
       </c>
       <c r="D89" s="20">
-        <v>629.05999999999995</v>
+        <v>647.64</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3503,10 +3509,10 @@
         <v>513.5</v>
       </c>
       <c r="C90" s="19">
-        <v>1.21</v>
+        <v>1.26</v>
       </c>
       <c r="D90" s="20">
-        <v>621.1</v>
+        <v>647.01</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3611,10 +3617,10 @@
         <v>12</v>
       </c>
       <c r="C99" s="19">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D99" s="20">
-        <v>13.2</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,10 +3631,10 @@
         <v>14</v>
       </c>
       <c r="C100" s="19">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D100" s="20">
-        <v>15.4</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,13 +3656,13 @@
         <v>104</v>
       </c>
       <c r="B102" s="18">
-        <v>5.5</v>
+        <v>24.5</v>
       </c>
       <c r="C102" s="19">
         <v>12.5</v>
       </c>
       <c r="D102" s="20">
-        <v>68.75</v>
+        <v>306.25</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3734,13 +3740,13 @@
         <v>110</v>
       </c>
       <c r="B108" s="18">
-        <v>6.5</v>
+        <v>21.5</v>
       </c>
       <c r="C108" s="19">
         <v>12.5</v>
       </c>
       <c r="D108" s="20">
-        <v>81.25</v>
+        <v>268.75</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3888,13 +3894,13 @@
         <v>121</v>
       </c>
       <c r="B119" s="18">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C119" s="19">
         <v>15.5</v>
       </c>
       <c r="D119" s="20">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4014,13 +4020,13 @@
         <v>130</v>
       </c>
       <c r="B128" s="18">
-        <v>1.5</v>
+        <v>11.5</v>
       </c>
       <c r="C128" s="19">
-        <v>18.41</v>
+        <v>18.43</v>
       </c>
       <c r="D128" s="20">
-        <v>27.61</v>
+        <v>211.95</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4070,13 +4076,13 @@
         <v>134</v>
       </c>
       <c r="B132" s="18">
-        <v>-2.5</v>
+        <v>3</v>
       </c>
       <c r="C132" s="19">
-        <v>18.27</v>
+        <v>18.37</v>
       </c>
       <c r="D132" s="20">
-        <v>-45.67</v>
+        <v>55.11</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4111,15 +4117,9 @@
       <c r="A135" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B135" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="C135" s="19">
-        <v>18.41</v>
-      </c>
-      <c r="D135" s="20">
-        <v>27.61</v>
-      </c>
+      <c r="B135" s="21"/>
+      <c r="C135" s="22"/>
+      <c r="D135" s="21"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="17" t="s">
@@ -4196,13 +4196,13 @@
         <v>143</v>
       </c>
       <c r="B141" s="18">
-        <v>61.5</v>
+        <v>56.5</v>
       </c>
       <c r="C141" s="19">
         <v>2.8</v>
       </c>
       <c r="D141" s="20">
-        <v>172.2</v>
+        <v>158.19999999999999</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4224,13 +4224,13 @@
         <v>145</v>
       </c>
       <c r="B143" s="18">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C143" s="19">
         <v>2.75</v>
       </c>
       <c r="D143" s="20">
-        <v>275</v>
+        <v>269.5</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4252,13 +4252,13 @@
         <v>147</v>
       </c>
       <c r="B145" s="18">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C145" s="19">
         <v>3.4</v>
       </c>
       <c r="D145" s="20">
-        <v>285.60000000000002</v>
+        <v>268.60000000000002</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4294,13 +4294,13 @@
         <v>150</v>
       </c>
       <c r="B148" s="18">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C148" s="19">
         <v>2.8</v>
       </c>
       <c r="D148" s="20">
-        <v>282.8</v>
+        <v>274.39999999999998</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4308,13 +4308,13 @@
         <v>151</v>
       </c>
       <c r="B149" s="18">
-        <v>103.5</v>
+        <v>103</v>
       </c>
       <c r="C149" s="19">
         <v>2.8</v>
       </c>
       <c r="D149" s="20">
-        <v>289.8</v>
+        <v>288.39999999999998</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4350,13 +4350,13 @@
         <v>154</v>
       </c>
       <c r="B152" s="18">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C152" s="19">
         <v>2.8</v>
       </c>
       <c r="D152" s="20">
-        <v>361.2</v>
+        <v>358.4</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4484,13 +4484,13 @@
         <v>164</v>
       </c>
       <c r="B162" s="18">
-        <v>127.5</v>
+        <v>67.5</v>
       </c>
       <c r="C162" s="19">
         <v>3.9</v>
       </c>
       <c r="D162" s="20">
-        <v>497.25</v>
+        <v>263.25</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4554,13 +4554,13 @@
         <v>169</v>
       </c>
       <c r="B167" s="18">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C167" s="19">
         <v>3.33</v>
       </c>
       <c r="D167" s="20">
-        <v>196.47</v>
+        <v>189.81</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,13 +4632,13 @@
         <v>175</v>
       </c>
       <c r="B173" s="18">
-        <v>150.5</v>
+        <v>153.5</v>
       </c>
       <c r="C173" s="19">
         <v>4.5</v>
       </c>
       <c r="D173" s="20">
-        <v>677.25</v>
+        <v>690.75</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,10 +4719,10 @@
         <v>140.5</v>
       </c>
       <c r="C179" s="19">
-        <v>3.73</v>
+        <v>3.93</v>
       </c>
       <c r="D179" s="20">
-        <v>523.47</v>
+        <v>552.17999999999995</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4730,13 +4730,13 @@
         <v>182</v>
       </c>
       <c r="B180" s="18">
-        <v>93.5</v>
+        <v>98.5</v>
       </c>
       <c r="C180" s="19">
-        <v>3.69</v>
+        <v>3.94</v>
       </c>
       <c r="D180" s="20">
-        <v>345.02</v>
+        <v>388.33</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4758,13 +4758,13 @@
         <v>184</v>
       </c>
       <c r="B182" s="18">
-        <v>98.5</v>
+        <v>95.5</v>
       </c>
       <c r="C182" s="19">
         <v>3</v>
       </c>
       <c r="D182" s="20">
-        <v>295.5</v>
+        <v>286.5</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4844,13 +4844,13 @@
         <v>191</v>
       </c>
       <c r="B189" s="18">
-        <v>50.24</v>
+        <v>44.74</v>
       </c>
       <c r="C189" s="19">
-        <v>3.05</v>
+        <v>3.14</v>
       </c>
       <c r="D189" s="20">
-        <v>153.22999999999999</v>
+        <v>140.47999999999999</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4918,13 +4918,13 @@
         <v>198</v>
       </c>
       <c r="B196" s="18">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C196" s="19">
         <v>3.8</v>
       </c>
       <c r="D196" s="20">
-        <v>79.8</v>
+        <v>72.2</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,13 +4982,13 @@
         <v>203</v>
       </c>
       <c r="B201" s="18">
-        <v>39</v>
+        <v>26.5</v>
       </c>
       <c r="C201" s="19">
-        <v>4.0999999999999996</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="D201" s="20">
-        <v>159.9</v>
+        <v>108.91</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,13 +4996,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C202" s="19">
-        <v>4.1100000000000003</v>
+        <v>4.12</v>
       </c>
       <c r="D202" s="20">
-        <v>349.18</v>
+        <v>321.05</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5052,13 +5052,13 @@
         <v>208</v>
       </c>
       <c r="B206" s="18">
-        <v>73.5</v>
+        <v>70.5</v>
       </c>
       <c r="C206" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D206" s="20">
-        <v>323.39999999999998</v>
+        <v>310.2</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5088,13 +5088,13 @@
         <v>211</v>
       </c>
       <c r="B209" s="18">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C209" s="19">
         <v>4.5</v>
       </c>
       <c r="D209" s="20">
-        <v>234</v>
+        <v>229.5</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,13 +5102,13 @@
         <v>212</v>
       </c>
       <c r="B210" s="18">
-        <v>-17.5</v>
+        <v>-3</v>
       </c>
       <c r="C210" s="19">
         <v>4.5</v>
       </c>
       <c r="D210" s="20">
-        <v>-78.75</v>
+        <v>-13.5</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5186,13 +5186,13 @@
         <v>218</v>
       </c>
       <c r="B216" s="18">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="C216" s="19">
         <v>4.75</v>
       </c>
       <c r="D216" s="20">
-        <v>116.38</v>
+        <v>121.13</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5256,13 +5256,13 @@
         <v>223</v>
       </c>
       <c r="B221" s="18">
-        <v>72.5</v>
+        <v>79.5</v>
       </c>
       <c r="C221" s="19">
         <v>4.75</v>
       </c>
       <c r="D221" s="20">
-        <v>344.38</v>
+        <v>377.63</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5322,13 +5322,13 @@
         <v>229</v>
       </c>
       <c r="B227" s="18">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="C227" s="19">
         <v>5.7</v>
       </c>
       <c r="D227" s="20">
-        <v>57</v>
+        <v>42.75</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5378,13 +5378,13 @@
         <v>233</v>
       </c>
       <c r="B231" s="18">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C231" s="19">
         <v>5.96</v>
       </c>
       <c r="D231" s="20">
-        <v>387.67</v>
+        <v>351.88</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5395,10 +5395,10 @@
         <v>23.5</v>
       </c>
       <c r="C232" s="19">
-        <v>4.25</v>
+        <v>4.26</v>
       </c>
       <c r="D232" s="20">
-        <v>99.99</v>
+        <v>100.11</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -5462,13 +5462,13 @@
         <v>239</v>
       </c>
       <c r="B237" s="18">
-        <v>23.5</v>
+        <v>21.5</v>
       </c>
       <c r="C237" s="19">
         <v>5</v>
       </c>
       <c r="D237" s="20">
-        <v>117.5</v>
+        <v>107.5</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -5504,13 +5504,13 @@
         <v>242</v>
       </c>
       <c r="B240" s="18">
-        <v>57</v>
+        <v>48.5</v>
       </c>
       <c r="C240" s="19">
         <v>3.5</v>
       </c>
       <c r="D240" s="20">
-        <v>199.5</v>
+        <v>169.75</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5518,13 +5518,13 @@
         <v>243</v>
       </c>
       <c r="B241" s="18">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C241" s="19">
         <v>4.25</v>
       </c>
       <c r="D241" s="20">
-        <v>803.25</v>
+        <v>811.75</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5582,13 +5582,13 @@
         <v>248</v>
       </c>
       <c r="B246" s="18">
-        <v>124</v>
+        <v>106.5</v>
       </c>
       <c r="C246" s="19">
         <v>4.28</v>
       </c>
       <c r="D246" s="20">
-        <v>530.72</v>
+        <v>455.82</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -5638,13 +5638,13 @@
         <v>252</v>
       </c>
       <c r="B250" s="18">
-        <v>17</v>
+        <v>13.5</v>
       </c>
       <c r="C250" s="19">
         <v>4.95</v>
       </c>
       <c r="D250" s="20">
-        <v>84.15</v>
+        <v>66.83</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -5652,13 +5652,13 @@
         <v>253</v>
       </c>
       <c r="B251" s="18">
-        <v>25</v>
+        <v>24.5</v>
       </c>
       <c r="C251" s="19">
         <v>4.75</v>
       </c>
       <c r="D251" s="20">
-        <v>118.75</v>
+        <v>116.38</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -5858,13 +5858,13 @@
         <v>269</v>
       </c>
       <c r="B267" s="18">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C267" s="19">
         <v>6</v>
       </c>
       <c r="D267" s="20">
-        <v>264</v>
+        <v>246</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -5886,13 +5886,13 @@
         <v>271</v>
       </c>
       <c r="B269" s="18">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C269" s="19">
         <v>5.94</v>
       </c>
       <c r="D269" s="20">
-        <v>457.38</v>
+        <v>427.68</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,13 +5942,13 @@
         <v>275</v>
       </c>
       <c r="B273" s="18">
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="C273" s="19">
-        <v>6.59</v>
+        <v>6.6</v>
       </c>
       <c r="D273" s="20">
-        <v>168.17</v>
+        <v>158.28</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,13 +6092,13 @@
         <v>287</v>
       </c>
       <c r="B285" s="18">
-        <v>44.5</v>
+        <v>43.5</v>
       </c>
       <c r="C285" s="19">
         <v>6.65</v>
       </c>
       <c r="D285" s="20">
-        <v>295.93</v>
+        <v>289.27999999999997</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -6128,13 +6128,13 @@
         <v>290</v>
       </c>
       <c r="B288" s="18">
-        <v>32.5</v>
+        <v>31</v>
       </c>
       <c r="C288" s="19">
         <v>7.18</v>
       </c>
       <c r="D288" s="20">
-        <v>233.28</v>
+        <v>222.51</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6142,13 +6142,13 @@
         <v>291</v>
       </c>
       <c r="B289" s="18">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C289" s="19">
         <v>7.13</v>
       </c>
       <c r="D289" s="20">
-        <v>78.430000000000007</v>
+        <v>163.99</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6184,13 +6184,13 @@
         <v>294</v>
       </c>
       <c r="B292" s="18">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C292" s="19">
         <v>6.65</v>
       </c>
       <c r="D292" s="20">
-        <v>219.45</v>
+        <v>212.8</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.25">
@@ -6256,13 +6256,13 @@
         <v>300</v>
       </c>
       <c r="B298" s="18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C298" s="19">
         <v>7.6</v>
       </c>
       <c r="D298" s="20">
-        <v>129.19999999999999</v>
+        <v>121.6</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.25">
@@ -6270,13 +6270,13 @@
         <v>301</v>
       </c>
       <c r="B299" s="18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C299" s="19">
         <v>8.08</v>
       </c>
       <c r="D299" s="20">
-        <v>8.08</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.25">
@@ -6474,13 +6474,13 @@
         <v>316</v>
       </c>
       <c r="B314" s="18">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C314" s="19">
         <v>9.25</v>
       </c>
       <c r="D314" s="20">
-        <v>-9.25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -6547,10 +6547,10 @@
         <v>60.5</v>
       </c>
       <c r="C319" s="19">
-        <v>6.79</v>
+        <v>6.86</v>
       </c>
       <c r="D319" s="20">
-        <v>410.7</v>
+        <v>415.06</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6561,10 +6561,10 @@
         <v>60.5</v>
       </c>
       <c r="C320" s="19">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
       <c r="D320" s="20">
-        <v>393.25</v>
+        <v>417.45</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -6714,13 +6714,13 @@
         <v>334</v>
       </c>
       <c r="B332" s="18">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="C332" s="19">
         <v>4.9000000000000004</v>
       </c>
       <c r="D332" s="20">
-        <v>71.05</v>
+        <v>61.25</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -6759,10 +6759,10 @@
         <v>31.5</v>
       </c>
       <c r="C335" s="19">
-        <v>7.66</v>
+        <v>7.6</v>
       </c>
       <c r="D335" s="20">
-        <v>241.39</v>
+        <v>239.4</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -6882,13 +6882,13 @@
         <v>346</v>
       </c>
       <c r="B344" s="18">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="C344" s="19">
         <v>18</v>
       </c>
       <c r="D344" s="20">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -6980,13 +6980,13 @@
         <v>353</v>
       </c>
       <c r="B351" s="18">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="C351" s="19">
         <v>7.84</v>
       </c>
       <c r="D351" s="20">
-        <v>27.44</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7176,13 +7176,13 @@
         <v>367</v>
       </c>
       <c r="B365" s="18">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="C365" s="19">
         <v>10</v>
       </c>
       <c r="D365" s="20">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7232,13 +7232,13 @@
         <v>371</v>
       </c>
       <c r="B369" s="18">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C369" s="19">
         <v>25</v>
       </c>
       <c r="D369" s="20">
-        <v>100</v>
+        <v>400</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7301,15 +7301,9 @@
       <c r="A374" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="B374" s="18">
-        <v>1.5</v>
-      </c>
-      <c r="C374" s="19">
-        <v>21.5</v>
-      </c>
-      <c r="D374" s="20">
-        <v>32.25</v>
-      </c>
+      <c r="B374" s="21"/>
+      <c r="C374" s="22"/>
+      <c r="D374" s="21"/>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" s="17" t="s">
@@ -7428,13 +7422,13 @@
         <v>385</v>
       </c>
       <c r="B383" s="18">
-        <v>38.5</v>
+        <v>23</v>
       </c>
       <c r="C383" s="19">
         <v>10.93</v>
       </c>
       <c r="D383" s="20">
-        <v>420.81</v>
+        <v>251.39</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -7512,13 +7506,13 @@
         <v>391</v>
       </c>
       <c r="B389" s="18">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="C389" s="19">
         <v>2</v>
       </c>
       <c r="D389" s="20">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
@@ -7526,13 +7520,13 @@
         <v>392</v>
       </c>
       <c r="B390" s="18">
-        <v>37.5</v>
+        <v>30.5</v>
       </c>
       <c r="C390" s="19">
         <v>2</v>
       </c>
       <c r="D390" s="20">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -7662,13 +7656,13 @@
         <v>403</v>
       </c>
       <c r="B401" s="18">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C401" s="19">
         <v>2.5</v>
       </c>
       <c r="D401" s="20">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -7690,13 +7684,13 @@
         <v>405</v>
       </c>
       <c r="B403" s="18">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C403" s="19">
         <v>2.7</v>
       </c>
       <c r="D403" s="20">
-        <v>234.9</v>
+        <v>218.7</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -7732,13 +7726,13 @@
         <v>408</v>
       </c>
       <c r="B406" s="18">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C406" s="19">
         <v>2.75</v>
       </c>
       <c r="D406" s="20">
-        <v>112.75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -7880,13 +7874,13 @@
         <v>419</v>
       </c>
       <c r="B417" s="18">
-        <v>21.95</v>
+        <v>20.95</v>
       </c>
       <c r="C417" s="19">
         <v>3.15</v>
       </c>
       <c r="D417" s="20">
-        <v>69.14</v>
+        <v>65.989999999999995</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -7972,13 +7966,13 @@
         <v>426</v>
       </c>
       <c r="B424" s="18">
-        <v>46.56</v>
+        <v>46.06</v>
       </c>
       <c r="C424" s="19">
         <v>3.5</v>
       </c>
       <c r="D424" s="20">
-        <v>162.96</v>
+        <v>161.21</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
@@ -7986,13 +7980,13 @@
         <v>427</v>
       </c>
       <c r="B425" s="18">
-        <v>59.5</v>
+        <v>60.5</v>
       </c>
       <c r="C425" s="19">
         <v>3.8</v>
       </c>
       <c r="D425" s="20">
-        <v>226.1</v>
+        <v>229.9</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
@@ -8100,13 +8094,13 @@
         <v>436</v>
       </c>
       <c r="B434" s="18">
-        <v>11.5</v>
+        <v>10</v>
       </c>
       <c r="C434" s="19">
         <v>4.0999999999999996</v>
       </c>
       <c r="D434" s="20">
-        <v>47.13</v>
+        <v>40.98</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
@@ -8114,13 +8108,13 @@
         <v>437</v>
       </c>
       <c r="B435" s="18">
-        <v>15</v>
+        <v>12.5</v>
       </c>
       <c r="C435" s="19">
         <v>4.25</v>
       </c>
       <c r="D435" s="20">
-        <v>63.75</v>
+        <v>53.13</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -8198,13 +8192,13 @@
         <v>443</v>
       </c>
       <c r="B441" s="18">
-        <v>50.5</v>
+        <v>50</v>
       </c>
       <c r="C441" s="19">
         <v>4.75</v>
       </c>
       <c r="D441" s="20">
-        <v>239.88</v>
+        <v>237.5</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -8290,13 +8284,13 @@
         <v>450</v>
       </c>
       <c r="B448" s="18">
-        <v>14.5</v>
+        <v>11.5</v>
       </c>
       <c r="C448" s="19">
         <v>5.5</v>
       </c>
       <c r="D448" s="20">
-        <v>79.75</v>
+        <v>63.25</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -8460,13 +8454,13 @@
         <v>463</v>
       </c>
       <c r="B461" s="18">
-        <v>37.5</v>
+        <v>35</v>
       </c>
       <c r="C461" s="19">
         <v>7.6</v>
       </c>
       <c r="D461" s="20">
-        <v>285</v>
+        <v>266</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -8566,13 +8560,13 @@
         <v>471</v>
       </c>
       <c r="B469" s="18">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="C469" s="19">
         <v>9.5</v>
       </c>
       <c r="D469" s="20">
-        <v>175.75</v>
+        <v>156.75</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -8608,13 +8602,13 @@
         <v>474</v>
       </c>
       <c r="B472" s="18">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C472" s="19">
         <v>5.7</v>
       </c>
       <c r="D472" s="20">
-        <v>330.6</v>
+        <v>307.8</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
@@ -8868,13 +8862,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C491" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D491" s="20">
-        <v>136.80000000000001</v>
+        <v>129.96</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -8904,13 +8898,13 @@
         <v>496</v>
       </c>
       <c r="B494" s="18">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="C494" s="19">
         <v>2.75</v>
       </c>
       <c r="D494" s="20">
-        <v>56.38</v>
+        <v>53.63</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
@@ -9002,13 +8996,13 @@
         <v>503</v>
       </c>
       <c r="B501" s="18">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C501" s="19">
         <v>3.2</v>
       </c>
       <c r="D501" s="20">
-        <v>192</v>
+        <v>188.8</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.25">
@@ -9016,13 +9010,13 @@
         <v>504</v>
       </c>
       <c r="B502" s="18">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C502" s="19">
         <v>3.2</v>
       </c>
       <c r="D502" s="20">
-        <v>140.80000000000001</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
@@ -9052,13 +9046,13 @@
         <v>507</v>
       </c>
       <c r="B505" s="18">
-        <v>60.5</v>
+        <v>58.5</v>
       </c>
       <c r="C505" s="19">
         <v>3.25</v>
       </c>
       <c r="D505" s="20">
-        <v>196.63</v>
+        <v>190.13</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
@@ -9124,13 +9118,13 @@
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>59.5</v>
+        <v>58</v>
       </c>
       <c r="C511" s="19">
         <v>3.33</v>
       </c>
       <c r="D511" s="20">
-        <v>198.14</v>
+        <v>193.14</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9288,13 +9282,13 @@
         <v>526</v>
       </c>
       <c r="B524" s="18">
-        <v>38.5</v>
+        <v>33.5</v>
       </c>
       <c r="C524" s="19">
         <v>3.8</v>
       </c>
       <c r="D524" s="20">
-        <v>146.30000000000001</v>
+        <v>127.3</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
@@ -9358,13 +9352,13 @@
         <v>531</v>
       </c>
       <c r="B529" s="18">
-        <v>24.5</v>
+        <v>14.5</v>
       </c>
       <c r="C529" s="19">
         <v>4.75</v>
       </c>
       <c r="D529" s="20">
-        <v>116.38</v>
+        <v>68.88</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
@@ -9428,13 +9422,13 @@
         <v>536</v>
       </c>
       <c r="B534" s="18">
-        <v>26.5</v>
+        <v>-1</v>
       </c>
       <c r="C534" s="19">
         <v>5</v>
       </c>
       <c r="D534" s="20">
-        <v>132.5</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
@@ -9442,13 +9436,13 @@
         <v>537</v>
       </c>
       <c r="B535" s="18">
-        <v>14.5</v>
+        <v>34.5</v>
       </c>
       <c r="C535" s="19">
         <v>5</v>
       </c>
       <c r="D535" s="20">
-        <v>72.5</v>
+        <v>172.5</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
@@ -9487,10 +9481,10 @@
         <v>24</v>
       </c>
       <c r="C538" s="19">
-        <v>5.2</v>
+        <v>5.41</v>
       </c>
       <c r="D538" s="20">
-        <v>124.8</v>
+        <v>129.78</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
@@ -9526,13 +9520,13 @@
         <v>543</v>
       </c>
       <c r="B541" s="18">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="C541" s="19">
         <v>5.75</v>
       </c>
       <c r="D541" s="20">
-        <v>169.63</v>
+        <v>158.13</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
@@ -9568,13 +9562,13 @@
         <v>546</v>
       </c>
       <c r="B544" s="18">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
       <c r="C544" s="19">
         <v>5.75</v>
       </c>
       <c r="D544" s="20">
-        <v>204.13</v>
+        <v>186.88</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
@@ -9752,13 +9746,13 @@
         <v>560</v>
       </c>
       <c r="B558" s="18">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="C558" s="19">
         <v>2.76</v>
       </c>
       <c r="D558" s="20">
-        <v>220.52</v>
+        <v>245.64</v>
       </c>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
@@ -9772,7 +9766,7 @@
         <v>2.76</v>
       </c>
       <c r="D559" s="20">
-        <v>203.89</v>
+        <v>204.24</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
@@ -9780,13 +9774,13 @@
         <v>562</v>
       </c>
       <c r="B560" s="18">
-        <v>109.5</v>
+        <v>107.5</v>
       </c>
       <c r="C560" s="19">
         <v>2.76</v>
       </c>
       <c r="D560" s="20">
-        <v>302.22000000000003</v>
+        <v>296.7</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
@@ -9811,10 +9805,10 @@
         <v>53</v>
       </c>
       <c r="C562" s="19">
-        <v>2.83</v>
+        <v>2.87</v>
       </c>
       <c r="D562" s="20">
-        <v>150.1</v>
+        <v>152.22</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
@@ -9892,13 +9886,13 @@
         <v>570</v>
       </c>
       <c r="B568" s="18">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C568" s="19">
         <v>3</v>
       </c>
       <c r="D568" s="20">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
@@ -9920,13 +9914,13 @@
         <v>572</v>
       </c>
       <c r="B570" s="18">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C570" s="19">
         <v>6</v>
       </c>
       <c r="D570" s="20">
-        <v>162</v>
+        <v>42</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.25">
@@ -10018,13 +10012,13 @@
         <v>579</v>
       </c>
       <c r="B577" s="18">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="C577" s="19">
         <v>1.92</v>
       </c>
       <c r="D577" s="20">
-        <v>565.9</v>
+        <v>491.64</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.25">
@@ -10046,13 +10040,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C579" s="19">
         <v>1.93</v>
       </c>
       <c r="D579" s="20">
-        <v>480.57</v>
+        <v>488.19</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10060,13 +10054,13 @@
         <v>582</v>
       </c>
       <c r="B580" s="18">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C580" s="19">
-        <v>2.79</v>
+        <v>2.84</v>
       </c>
       <c r="D580" s="20">
-        <v>348.92</v>
+        <v>349.06</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
@@ -10088,13 +10082,13 @@
         <v>584</v>
       </c>
       <c r="B582" s="18">
-        <v>36.5</v>
+        <v>34.5</v>
       </c>
       <c r="C582" s="19">
         <v>4.28</v>
       </c>
       <c r="D582" s="20">
-        <v>156.22</v>
+        <v>147.66</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.25">
@@ -10102,13 +10096,13 @@
         <v>585</v>
       </c>
       <c r="B583" s="18">
-        <v>62.5</v>
+        <v>56.5</v>
       </c>
       <c r="C583" s="19">
         <v>4.05</v>
       </c>
       <c r="D583" s="20">
-        <v>253.13</v>
+        <v>228.83</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
@@ -10116,13 +10110,13 @@
         <v>586</v>
       </c>
       <c r="B584" s="18">
-        <v>104.5</v>
+        <v>80.5</v>
       </c>
       <c r="C584" s="19">
         <v>4.05</v>
       </c>
       <c r="D584" s="20">
-        <v>423.23</v>
+        <v>326.02999999999997</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
@@ -10133,10 +10127,10 @@
         <v>147</v>
       </c>
       <c r="C585" s="19">
-        <v>1.36</v>
+        <v>1.39</v>
       </c>
       <c r="D585" s="20">
-        <v>199.5</v>
+        <v>204.64</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
@@ -10147,10 +10141,10 @@
         <v>378</v>
       </c>
       <c r="C586" s="19">
-        <v>1.36</v>
+        <v>1.4</v>
       </c>
       <c r="D586" s="20">
-        <v>512.54</v>
+        <v>529.20000000000005</v>
       </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.25">
@@ -10158,13 +10152,13 @@
         <v>589</v>
       </c>
       <c r="B587" s="18">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="C587" s="19">
-        <v>1.37</v>
+        <v>1.4</v>
       </c>
       <c r="D587" s="20">
-        <v>128.9</v>
+        <v>166.6</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
@@ -10182,7 +10176,7 @@
         <v>591</v>
       </c>
       <c r="B589" s="18">
-        <v>37.5</v>
+        <v>35.5</v>
       </c>
       <c r="C589" s="22"/>
       <c r="D589" s="21"/>
@@ -10212,13 +10206,13 @@
         <v>594</v>
       </c>
       <c r="B592" s="18">
-        <v>546.5</v>
+        <v>526.5</v>
       </c>
       <c r="C592" s="19">
         <v>0.8</v>
       </c>
       <c r="D592" s="20">
-        <v>437.2</v>
+        <v>421.2</v>
       </c>
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.25">
@@ -10254,13 +10248,13 @@
         <v>597</v>
       </c>
       <c r="B595" s="18">
-        <v>511.5</v>
+        <v>509.5</v>
       </c>
       <c r="C595" s="19">
         <v>0.8</v>
       </c>
       <c r="D595" s="20">
-        <v>409.2</v>
+        <v>407.6</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
@@ -10268,13 +10262,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="C596" s="19">
         <v>0.52</v>
       </c>
       <c r="D596" s="20">
-        <v>112.84</v>
+        <v>102.44</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10282,13 +10276,13 @@
         <v>599</v>
       </c>
       <c r="B597" s="18">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C597" s="19">
         <v>0.52</v>
       </c>
       <c r="D597" s="20">
-        <v>213.2</v>
+        <v>211.12</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.25">
@@ -10310,13 +10304,13 @@
         <v>601</v>
       </c>
       <c r="B599" s="18">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C599" s="19">
         <v>0.7</v>
       </c>
       <c r="D599" s="20">
-        <v>34.299999999999997</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.25">
@@ -10332,13 +10326,13 @@
         <v>603</v>
       </c>
       <c r="B601" s="18">
-        <v>536.5</v>
+        <v>465.5</v>
       </c>
       <c r="C601" s="19">
         <v>0.7</v>
       </c>
       <c r="D601" s="20">
-        <v>375.55</v>
+        <v>325.85000000000002</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.25">
@@ -10374,11 +10368,11 @@
         <v>606</v>
       </c>
       <c r="B604" s="24">
-        <v>34029.47</v>
+        <v>34166.47</v>
       </c>
       <c r="C604" s="25"/>
       <c r="D604" s="26">
-        <v>99898.93</v>
+        <v>100320.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -2477,13 +2477,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="18">
-        <v>64</v>
+        <v>60.5</v>
       </c>
       <c r="C12" s="19">
         <v>1.65</v>
       </c>
       <c r="D12" s="20">
-        <v>105.6</v>
+        <v>99.83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3359,7 +3359,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>69.5</v>
+        <v>67</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="21"/>
@@ -3445,13 +3445,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="18">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C85" s="19">
         <v>1.4</v>
       </c>
       <c r="D85" s="20">
-        <v>239.4</v>
+        <v>233.8</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,13 +4065,13 @@
         <v>133</v>
       </c>
       <c r="B131" s="18">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="C131" s="19">
         <v>18.37</v>
       </c>
       <c r="D131" s="20">
-        <v>146.96</v>
+        <v>119.4</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4767,13 +4767,13 @@
         <v>184</v>
       </c>
       <c r="B182" s="18">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C182" s="19">
         <v>3</v>
       </c>
       <c r="D182" s="20">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,13 +5153,13 @@
         <v>215</v>
       </c>
       <c r="B213" s="18">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C213" s="19">
         <v>4.8</v>
       </c>
       <c r="D213" s="20">
-        <v>206.4</v>
+        <v>196.8</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5569,13 +5569,13 @@
         <v>246</v>
       </c>
       <c r="B244" s="18">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C244" s="19">
         <v>4.18</v>
       </c>
       <c r="D244" s="20">
-        <v>259.16000000000003</v>
+        <v>250.8</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -6143,13 +6143,13 @@
         <v>290</v>
       </c>
       <c r="B288" s="18">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C288" s="19">
         <v>7.18</v>
       </c>
       <c r="D288" s="20">
-        <v>222.51</v>
+        <v>200.98</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -7233,13 +7233,13 @@
         <v>370</v>
       </c>
       <c r="B368" s="18">
-        <v>25.5</v>
+        <v>23.5</v>
       </c>
       <c r="C368" s="19">
         <v>7.84</v>
       </c>
       <c r="D368" s="20">
-        <v>199.92</v>
+        <v>184.24</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -8413,13 +8413,13 @@
         <v>459</v>
       </c>
       <c r="B457" s="18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C457" s="19">
         <v>7.5</v>
       </c>
       <c r="D457" s="20">
-        <v>150</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
@@ -10055,13 +10055,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="C579" s="19">
         <v>1.96</v>
       </c>
       <c r="D579" s="20">
-        <v>17.649999999999999</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10083,13 +10083,13 @@
         <v>583</v>
       </c>
       <c r="B581" s="18">
-        <v>119.5</v>
+        <v>117.5</v>
       </c>
       <c r="C581" s="19">
         <v>2.84</v>
       </c>
       <c r="D581" s="20">
-        <v>339.12</v>
+        <v>333.45</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.25">
@@ -10397,11 +10397,11 @@
         <v>607</v>
       </c>
       <c r="B605" s="24">
-        <v>36478.97</v>
+        <v>36447.97</v>
       </c>
       <c r="C605" s="25"/>
       <c r="D605" s="26">
-        <v>104367.95</v>
+        <v>104231.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:31
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 18-Dec-2024</t>
+    <t>1-Jul-2024 to 19-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -512,7 +512,7 @@
     <t>4220 PATRIKA</t>
   </si>
   <si>
-    <t>4221 PATRIKA (20.12 6K)</t>
+    <t>4221 PATRIKA (AA GYA)</t>
   </si>
   <si>
     <t>4222 PATRIKA (DC)</t>
@@ -929,7 +929,7 @@
     <t>5908 PATRIKA</t>
   </si>
   <si>
-    <t>5909 PATRIKA {M}</t>
+    <t>5909 PATRIKA {M} (AA GYA)</t>
   </si>
   <si>
     <t>5910 PATRIKA {M}</t>
@@ -974,7 +974,7 @@
     <t>5923 PATRIKA (DC) {{10}}</t>
   </si>
   <si>
-    <t>5924 PATRIKA {M}</t>
+    <t>5924 PATRIKA {M} (400)</t>
   </si>
   <si>
     <t>5925 PATRIKA {M}</t>
@@ -1139,7 +1139,7 @@
     <t>6530 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6531 PATRIKA {M}</t>
+    <t>6531 PATRIKA {M} (1500)</t>
   </si>
   <si>
     <t>6532 PATRIKA (Dc) REMOVE</t>
@@ -1376,7 +1376,7 @@
     <t>7309 PATRIKA</t>
   </si>
   <si>
-    <t>7310 PATRIKA (D)</t>
+    <t>7310 PATRIKA (D) (AA GYA)</t>
   </si>
   <si>
     <t>7311 PATRIKA (DC) {{10}}</t>
@@ -2449,13 +2449,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="18">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="C10" s="19">
         <v>1</v>
       </c>
       <c r="D10" s="20">
-        <v>304</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2463,13 +2463,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="19">
         <v>0.92</v>
       </c>
       <c r="D11" s="20">
-        <v>210.74</v>
+        <v>209.82</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2589,13 +2589,13 @@
         <v>22</v>
       </c>
       <c r="B20" s="18">
-        <v>131.5</v>
+        <v>129.5</v>
       </c>
       <c r="C20" s="19">
         <v>2</v>
       </c>
       <c r="D20" s="20">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2631,13 +2631,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="18">
-        <v>124</v>
+        <v>119.5</v>
       </c>
       <c r="C23" s="19">
         <v>2</v>
       </c>
       <c r="D23" s="20">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2645,13 +2645,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18">
-        <v>66.5</v>
+        <v>60.5</v>
       </c>
       <c r="C24" s="19">
         <v>2.1</v>
       </c>
       <c r="D24" s="20">
-        <v>139.65</v>
+        <v>127.05</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,13 +2979,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>149.6</v>
+        <v>141.9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,13 +3035,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>35.200000000000003</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,13 +3287,13 @@
         <v>74</v>
       </c>
       <c r="B72" s="18">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C72" s="19">
         <v>1.55</v>
       </c>
       <c r="D72" s="20">
-        <v>753.3</v>
+        <v>757.95</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,13 +3315,13 @@
         <v>76</v>
       </c>
       <c r="B74" s="18">
-        <v>702.5</v>
+        <v>700.5</v>
       </c>
       <c r="C74" s="19">
         <v>1.55</v>
       </c>
       <c r="D74" s="20">
-        <v>1088.8800000000001</v>
+        <v>1085.78</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,7 +3329,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="18">
-        <v>165.5</v>
+        <v>160.5</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="21"/>
@@ -3359,7 +3359,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>67</v>
+        <v>64.5</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="21"/>
@@ -3379,7 +3379,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="18">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
@@ -3417,13 +3417,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>989.8</v>
+        <v>992.6</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,13 +3509,13 @@
         <v>92</v>
       </c>
       <c r="B90" s="18">
-        <v>513.5</v>
+        <v>511.5</v>
       </c>
       <c r="C90" s="19">
         <v>1.26</v>
       </c>
       <c r="D90" s="20">
-        <v>647.01</v>
+        <v>644.49</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3594,23 +3594,23 @@
       <c r="A97" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B97" s="18">
-        <v>-10</v>
-      </c>
-      <c r="C97" s="19">
-        <v>1.55</v>
-      </c>
-      <c r="D97" s="20">
-        <v>-15.5</v>
-      </c>
+      <c r="B97" s="21"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="21"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B98" s="21"/>
-      <c r="C98" s="22"/>
-      <c r="D98" s="21"/>
+      <c r="B98" s="18">
+        <v>8</v>
+      </c>
+      <c r="C98" s="19">
+        <v>1.55</v>
+      </c>
+      <c r="D98" s="20">
+        <v>12.4</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
@@ -3771,13 +3771,13 @@
         <v>112</v>
       </c>
       <c r="B110" s="18">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="C110" s="19">
         <v>12.5</v>
       </c>
       <c r="D110" s="20">
-        <v>243.75</v>
+        <v>231.25</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,13 +4065,13 @@
         <v>133</v>
       </c>
       <c r="B131" s="18">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="C131" s="19">
         <v>18.37</v>
       </c>
       <c r="D131" s="20">
-        <v>119.4</v>
+        <v>146.96</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4205,13 +4205,13 @@
         <v>143</v>
       </c>
       <c r="B141" s="18">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C141" s="19">
         <v>2.8</v>
       </c>
       <c r="D141" s="20">
-        <v>154</v>
+        <v>137.19999999999999</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4219,13 +4219,13 @@
         <v>144</v>
       </c>
       <c r="B142" s="18">
-        <v>110.5</v>
+        <v>107</v>
       </c>
       <c r="C142" s="19">
         <v>2.75</v>
       </c>
       <c r="D142" s="20">
-        <v>303.88</v>
+        <v>294.25</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4247,13 +4247,13 @@
         <v>146</v>
       </c>
       <c r="B144" s="18">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C144" s="19">
         <v>4.7</v>
       </c>
       <c r="D144" s="20">
-        <v>155.1</v>
+        <v>150.4</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4261,13 +4261,13 @@
         <v>147</v>
       </c>
       <c r="B145" s="18">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C145" s="19">
         <v>3.4</v>
       </c>
       <c r="D145" s="20">
-        <v>261.8</v>
+        <v>258.39999999999998</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,13 +4317,13 @@
         <v>151</v>
       </c>
       <c r="B149" s="18">
-        <v>103</v>
+        <v>99.5</v>
       </c>
       <c r="C149" s="19">
         <v>2.8</v>
       </c>
       <c r="D149" s="20">
-        <v>288.39999999999998</v>
+        <v>278.60000000000002</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4535,13 +4535,13 @@
         <v>167</v>
       </c>
       <c r="B165" s="18">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C165" s="19">
         <v>3.33</v>
       </c>
       <c r="D165" s="20">
-        <v>136.53</v>
+        <v>103.23</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -4697,13 +4697,13 @@
         <v>179</v>
       </c>
       <c r="B177" s="18">
-        <v>33.5</v>
+        <v>30.5</v>
       </c>
       <c r="C177" s="19">
         <v>4.5</v>
       </c>
       <c r="D177" s="20">
-        <v>150.75</v>
+        <v>137.25</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4725,13 +4725,13 @@
         <v>181</v>
       </c>
       <c r="B179" s="18">
-        <v>138.5</v>
+        <v>123.5</v>
       </c>
       <c r="C179" s="19">
         <v>3.93</v>
       </c>
       <c r="D179" s="20">
-        <v>544.32000000000005</v>
+        <v>485.37</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4739,13 +4739,13 @@
         <v>182</v>
       </c>
       <c r="B180" s="18">
-        <v>98.5</v>
+        <v>95.5</v>
       </c>
       <c r="C180" s="19">
         <v>3.94</v>
       </c>
       <c r="D180" s="20">
-        <v>388.33</v>
+        <v>376.51</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,13 +4941,13 @@
         <v>199</v>
       </c>
       <c r="B197" s="18">
-        <v>20.5</v>
+        <v>14.5</v>
       </c>
       <c r="C197" s="19">
         <v>3.8</v>
       </c>
       <c r="D197" s="20">
-        <v>77.900000000000006</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4991,13 +4991,13 @@
         <v>203</v>
       </c>
       <c r="B201" s="18">
-        <v>29.5</v>
+        <v>26.5</v>
       </c>
       <c r="C201" s="19">
         <v>4.1100000000000003</v>
       </c>
       <c r="D201" s="20">
-        <v>121.24</v>
+        <v>108.91</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5005,13 +5005,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C202" s="19">
         <v>4.12</v>
       </c>
       <c r="D202" s="20">
-        <v>156.41</v>
+        <v>148.18</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5111,13 +5111,13 @@
         <v>212</v>
       </c>
       <c r="B210" s="18">
-        <v>297</v>
+        <v>290.5</v>
       </c>
       <c r="C210" s="19">
         <v>4.5</v>
       </c>
       <c r="D210" s="20">
-        <v>1336.5</v>
+        <v>1307.25</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5139,13 +5139,13 @@
         <v>214</v>
       </c>
       <c r="B212" s="18">
-        <v>19</v>
+        <v>25.5</v>
       </c>
       <c r="C212" s="19">
         <v>5.25</v>
       </c>
       <c r="D212" s="20">
-        <v>99.75</v>
+        <v>133.88</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5315,13 +5315,13 @@
         <v>227</v>
       </c>
       <c r="B225" s="18">
-        <v>3.5</v>
+        <v>8.5</v>
       </c>
       <c r="C225" s="19">
         <v>6</v>
       </c>
       <c r="D225" s="20">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5504,28 +5504,22 @@
       <c r="A239" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="B239" s="18">
-        <v>6.5</v>
-      </c>
-      <c r="C239" s="19">
-        <v>5.25</v>
-      </c>
-      <c r="D239" s="20">
-        <v>34.130000000000003</v>
-      </c>
+      <c r="B239" s="21"/>
+      <c r="C239" s="22"/>
+      <c r="D239" s="21"/>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="17" t="s">
         <v>242</v>
       </c>
       <c r="B240" s="18">
-        <v>46.5</v>
+        <v>45.5</v>
       </c>
       <c r="C240" s="19">
         <v>3.5</v>
       </c>
       <c r="D240" s="20">
-        <v>162.75</v>
+        <v>159.25</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5681,13 +5675,13 @@
         <v>254</v>
       </c>
       <c r="B252" s="18">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C252" s="19">
         <v>5</v>
       </c>
       <c r="D252" s="20">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -5831,13 +5825,13 @@
         <v>266</v>
       </c>
       <c r="B264" s="18">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="C264" s="19">
         <v>6.25</v>
       </c>
       <c r="D264" s="20">
-        <v>184.38</v>
+        <v>171.88</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -5873,13 +5867,13 @@
         <v>269</v>
       </c>
       <c r="B267" s="18">
-        <v>38</v>
+        <v>36.5</v>
       </c>
       <c r="C267" s="19">
         <v>6</v>
       </c>
       <c r="D267" s="20">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -5901,13 +5895,13 @@
         <v>271</v>
       </c>
       <c r="B269" s="18">
-        <v>75.5</v>
+        <v>72.5</v>
       </c>
       <c r="C269" s="19">
         <v>5.94</v>
       </c>
       <c r="D269" s="20">
-        <v>448.47</v>
+        <v>430.65</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6143,13 +6137,13 @@
         <v>290</v>
       </c>
       <c r="B288" s="18">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C288" s="19">
         <v>7.18</v>
       </c>
       <c r="D288" s="20">
-        <v>200.98</v>
+        <v>179.44</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -6157,13 +6151,13 @@
         <v>291</v>
       </c>
       <c r="B289" s="18">
-        <v>19.5</v>
+        <v>15.5</v>
       </c>
       <c r="C289" s="19">
         <v>7.13</v>
       </c>
       <c r="D289" s="20">
-        <v>139.04</v>
+        <v>110.52</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6475,13 +6469,13 @@
         <v>315</v>
       </c>
       <c r="B313" s="18">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="C313" s="19">
         <v>11</v>
       </c>
       <c r="D313" s="20">
-        <v>104.5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.25">
@@ -6545,13 +6539,13 @@
         <v>320</v>
       </c>
       <c r="B318" s="18">
-        <v>88.5</v>
+        <v>91.5</v>
       </c>
       <c r="C318" s="19">
         <v>5.5</v>
       </c>
       <c r="D318" s="20">
-        <v>486.75</v>
+        <v>503.25</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.25">
@@ -6671,13 +6665,13 @@
         <v>329</v>
       </c>
       <c r="B327" s="18">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="C327" s="19">
         <v>6.9</v>
       </c>
       <c r="D327" s="20">
-        <v>69</v>
+        <v>58.65</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -6729,13 +6723,13 @@
         <v>334</v>
       </c>
       <c r="B332" s="18">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C332" s="19">
         <v>4.9000000000000004</v>
       </c>
       <c r="D332" s="20">
-        <v>78.400000000000006</v>
+        <v>68.599999999999994</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -6799,13 +6793,13 @@
         <v>339</v>
       </c>
       <c r="B337" s="18">
-        <v>65.5</v>
+        <v>64</v>
       </c>
       <c r="C337" s="19">
         <v>6.5</v>
       </c>
       <c r="D337" s="20">
-        <v>425.75</v>
+        <v>416</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -6995,13 +6989,13 @@
         <v>353</v>
       </c>
       <c r="B351" s="18">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="C351" s="19">
         <v>7.84</v>
       </c>
       <c r="D351" s="20">
-        <v>35.28</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7233,13 +7227,13 @@
         <v>370</v>
       </c>
       <c r="B368" s="18">
-        <v>23.5</v>
+        <v>20.5</v>
       </c>
       <c r="C368" s="19">
         <v>7.84</v>
       </c>
       <c r="D368" s="20">
-        <v>184.24</v>
+        <v>160.72</v>
       </c>
     </row>
     <row r="369" spans="1:4" x14ac:dyDescent="0.25">
@@ -7247,13 +7241,13 @@
         <v>371</v>
       </c>
       <c r="B369" s="18">
-        <v>15</v>
+        <v>8.5</v>
       </c>
       <c r="C369" s="19">
         <v>25</v>
       </c>
       <c r="D369" s="20">
-        <v>375</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7275,13 +7269,13 @@
         <v>373</v>
       </c>
       <c r="B371" s="18">
-        <v>35.5</v>
+        <v>34.5</v>
       </c>
       <c r="C371" s="19">
         <v>10.93</v>
       </c>
       <c r="D371" s="20">
-        <v>388.02</v>
+        <v>377.09</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
@@ -7437,13 +7431,13 @@
         <v>385</v>
       </c>
       <c r="B383" s="18">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C383" s="19">
         <v>10.93</v>
       </c>
       <c r="D383" s="20">
-        <v>284.18</v>
+        <v>240.46</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -7535,13 +7529,13 @@
         <v>392</v>
       </c>
       <c r="B390" s="18">
-        <v>29.5</v>
+        <v>28</v>
       </c>
       <c r="C390" s="19">
         <v>2</v>
       </c>
       <c r="D390" s="20">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
@@ -7699,13 +7693,13 @@
         <v>405</v>
       </c>
       <c r="B403" s="18">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C403" s="19">
         <v>2.7</v>
       </c>
       <c r="D403" s="20">
-        <v>218.7</v>
+        <v>216</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -7967,13 +7961,13 @@
         <v>425</v>
       </c>
       <c r="B423" s="18">
-        <v>30.5</v>
+        <v>25</v>
       </c>
       <c r="C423" s="19">
         <v>3.4</v>
       </c>
       <c r="D423" s="20">
-        <v>103.7</v>
+        <v>85</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -8299,13 +8293,13 @@
         <v>450</v>
       </c>
       <c r="B448" s="18">
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
       <c r="C448" s="19">
         <v>5.5</v>
       </c>
       <c r="D448" s="20">
-        <v>46.75</v>
+        <v>35.75</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -8427,13 +8421,13 @@
         <v>460</v>
       </c>
       <c r="B458" s="18">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C458" s="19">
         <v>7.13</v>
       </c>
       <c r="D458" s="20">
-        <v>349.37</v>
+        <v>342.24</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -8561,13 +8555,13 @@
         <v>470</v>
       </c>
       <c r="B468" s="18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C468" s="19">
         <v>4.28</v>
       </c>
       <c r="D468" s="20">
-        <v>107</v>
+        <v>102.72</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -8729,13 +8723,13 @@
         <v>482</v>
       </c>
       <c r="B480" s="18">
-        <v>106.5</v>
+        <v>86.5</v>
       </c>
       <c r="C480" s="19">
         <v>1.4</v>
       </c>
       <c r="D480" s="20">
-        <v>149.1</v>
+        <v>121.1</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -8827,13 +8821,13 @@
         <v>489</v>
       </c>
       <c r="B487" s="18">
-        <v>217.5</v>
+        <v>209.5</v>
       </c>
       <c r="C487" s="19">
         <v>1.5</v>
       </c>
       <c r="D487" s="20">
-        <v>326.25</v>
+        <v>314.25</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -8841,13 +8835,13 @@
         <v>490</v>
       </c>
       <c r="B488" s="18">
-        <v>352.5</v>
+        <v>350.5</v>
       </c>
       <c r="C488" s="19">
         <v>1.5</v>
       </c>
       <c r="D488" s="20">
-        <v>528.75</v>
+        <v>525.75</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -8869,13 +8863,13 @@
         <v>492</v>
       </c>
       <c r="B490" s="18">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C490" s="19">
         <v>0.39</v>
       </c>
       <c r="D490" s="20">
-        <v>57.59</v>
+        <v>53.67</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -8883,13 +8877,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C491" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D491" s="20">
-        <v>223.44</v>
+        <v>218.88</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -8961,13 +8955,13 @@
         <v>499</v>
       </c>
       <c r="B497" s="18">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C497" s="19">
         <v>2.8</v>
       </c>
       <c r="D497" s="20">
-        <v>39.200000000000003</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
@@ -9153,13 +9147,13 @@
         <v>514</v>
       </c>
       <c r="B512" s="18">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C512" s="19">
         <v>3.33</v>
       </c>
       <c r="D512" s="20">
-        <v>203.13</v>
+        <v>193.14</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
@@ -9203,13 +9197,13 @@
         <v>518</v>
       </c>
       <c r="B516" s="18">
-        <v>54.5</v>
+        <v>53.5</v>
       </c>
       <c r="C516" s="19">
         <v>3.6</v>
       </c>
       <c r="D516" s="20">
-        <v>196.2</v>
+        <v>192.6</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
@@ -9317,13 +9311,13 @@
         <v>527</v>
       </c>
       <c r="B525" s="18">
-        <v>33.5</v>
+        <v>31.5</v>
       </c>
       <c r="C525" s="19">
         <v>3.8</v>
       </c>
       <c r="D525" s="20">
-        <v>127.3</v>
+        <v>119.7</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
@@ -9465,13 +9459,13 @@
         <v>538</v>
       </c>
       <c r="B536" s="18">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="C536" s="19">
         <v>5</v>
       </c>
       <c r="D536" s="20">
-        <v>172.5</v>
+        <v>162.5</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
@@ -9605,13 +9599,13 @@
         <v>548</v>
       </c>
       <c r="B546" s="18">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C546" s="19">
         <v>6</v>
       </c>
       <c r="D546" s="20">
-        <v>174</v>
+        <v>138</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
@@ -9619,13 +9613,13 @@
         <v>549</v>
       </c>
       <c r="B547" s="18">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C547" s="19">
         <v>6</v>
       </c>
       <c r="D547" s="20">
-        <v>78</v>
+        <v>18</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
@@ -10041,13 +10035,13 @@
         <v>580</v>
       </c>
       <c r="B578" s="18">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C578" s="19">
         <v>1.92</v>
       </c>
       <c r="D578" s="20">
-        <v>487.8</v>
+        <v>482.04</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.25">
@@ -10055,13 +10049,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>6.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C579" s="19">
         <v>1.96</v>
       </c>
       <c r="D579" s="20">
-        <v>12.75</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10069,13 +10063,13 @@
         <v>582</v>
       </c>
       <c r="B580" s="18">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C580" s="19">
         <v>1.93</v>
       </c>
       <c r="D580" s="20">
-        <v>486.26</v>
+        <v>480.48</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
@@ -10083,13 +10077,13 @@
         <v>583</v>
       </c>
       <c r="B581" s="18">
-        <v>117.5</v>
+        <v>115.5</v>
       </c>
       <c r="C581" s="19">
         <v>2.84</v>
       </c>
       <c r="D581" s="20">
-        <v>333.45</v>
+        <v>327.77</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.25">
@@ -10205,7 +10199,7 @@
         <v>592</v>
       </c>
       <c r="B590" s="18">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="C590" s="22"/>
       <c r="D590" s="21"/>
@@ -10215,7 +10209,7 @@
         <v>593</v>
       </c>
       <c r="B591" s="18">
-        <v>51.5</v>
+        <v>49.5</v>
       </c>
       <c r="C591" s="22"/>
       <c r="D591" s="21"/>
@@ -10249,13 +10243,13 @@
         <v>596</v>
       </c>
       <c r="B594" s="18">
-        <v>630.5</v>
+        <v>628.5</v>
       </c>
       <c r="C594" s="19">
         <v>0.8</v>
       </c>
       <c r="D594" s="20">
-        <v>504.4</v>
+        <v>502.8</v>
       </c>
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.25">
@@ -10277,13 +10271,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>483.5</v>
+        <v>479.5</v>
       </c>
       <c r="C596" s="19">
         <v>0.8</v>
       </c>
       <c r="D596" s="20">
-        <v>386.8</v>
+        <v>383.6</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10355,13 +10349,13 @@
         <v>604</v>
       </c>
       <c r="B602" s="18">
-        <v>469.5</v>
+        <v>467.5</v>
       </c>
       <c r="C602" s="19">
         <v>0.68</v>
       </c>
       <c r="D602" s="20">
-        <v>320.2</v>
+        <v>318.83999999999997</v>
       </c>
     </row>
     <row r="603" spans="1:4" x14ac:dyDescent="0.25">
@@ -10397,11 +10391,11 @@
         <v>607</v>
       </c>
       <c r="B605" s="24">
-        <v>36447.97</v>
+        <v>36240.47</v>
       </c>
       <c r="C605" s="25"/>
       <c r="D605" s="26">
-        <v>104231.78</v>
+        <v>103376.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:26
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="611">
   <si>
     <t>StkSummary</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 19-Dec-2024</t>
+    <t>1-Jul-2024 to 20-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -425,7 +425,7 @@
     <t>2050 PATRIKA {L}</t>
   </si>
   <si>
-    <t>2051 PATRIKA {L}</t>
+    <t>2051 PATRIKA {L} (DC)</t>
   </si>
   <si>
     <t>2052 PATRIKA {L}</t>
@@ -437,7 +437,7 @@
     <t>2054 PATRIKA {L}</t>
   </si>
   <si>
-    <t>2055 PATRIKA (Saturday 21.12 1000)</t>
+    <t>2055 PATRIKA</t>
   </si>
   <si>
     <t>2056 PATRIKA {L}</t>
@@ -680,7 +680,7 @@
     <t>5025 PATRIKA (DORI) {M}</t>
   </si>
   <si>
-    <t>5026 PATRIKA</t>
+    <t>5026 PATRIKA (3000)</t>
   </si>
   <si>
     <t>5027 PATRIKA (DC)</t>
@@ -713,7 +713,7 @@
     <t>5036 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5037 PATRIKA</t>
+    <t>5037 PATRIKA (8000)</t>
   </si>
   <si>
     <t>5038 PATRIKA</t>
@@ -728,7 +728,7 @@
     <t>5040 PATRIKA</t>
   </si>
   <si>
-    <t>5041 PATRIKA</t>
+    <t>5041 PATRIKA (2400)</t>
   </si>
   <si>
     <t>5042 PATRIKA (AA GYA)</t>
@@ -1010,7 +1010,7 @@
     <t>5935 PATRIKA {M}</t>
   </si>
   <si>
-    <t>5936 PATRIKA {M}</t>
+    <t>5936 PATRIKA {M} (26.12 4K)</t>
   </si>
   <si>
     <t>5937 PATRIKA (Dc) {{10}}</t>
@@ -1103,10 +1103,10 @@
     <t>6518 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6519 PATRIKA {M}</t>
-  </si>
-  <si>
-    <t>6520 PATRIKA {M}</t>
+    <t>6519 PATRIKA {M} (2000)</t>
+  </si>
+  <si>
+    <t>6520 PATRIKA {M} (1400 Total)</t>
   </si>
   <si>
     <t>6521 PATRIKA (GGN) {M}</t>
@@ -1130,7 +1130,7 @@
     <t>6527 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6528 PATRIKA {M}</t>
+    <t>6528 PATRIKA {M} (2200)</t>
   </si>
   <si>
     <t>6529 PATRIKA</t>
@@ -1166,7 +1166,7 @@
     <t>6539 PATRIKA</t>
   </si>
   <si>
-    <t>6540 PATRIKA {M}</t>
+    <t>6540 PATRIKA {M} (2700)</t>
   </si>
   <si>
     <t>6541 PATRIKA</t>
@@ -1208,6 +1208,9 @@
     <t>7252 PATRIKA</t>
   </si>
   <si>
+    <t>7253 PATRIKA</t>
+  </si>
+  <si>
     <t>7253 PATRIKA - B (Dc)</t>
   </si>
   <si>
@@ -1250,7 +1253,7 @@
     <t>7266 PATRIKA</t>
   </si>
   <si>
-    <t>7267 PATRIKA</t>
+    <t>7267 PATRIKA (5000)</t>
   </si>
   <si>
     <t>7268 PATRIKA</t>
@@ -1334,7 +1337,7 @@
     <t>7295 PATRIKA</t>
   </si>
   <si>
-    <t>7296 PATRIKA {F}</t>
+    <t>7296 PATRIKA {F} (5200)</t>
   </si>
   <si>
     <t>7297 PATRIKA {F/G}</t>
@@ -1364,7 +1367,7 @@
     <t>7305 PATRIKA</t>
   </si>
   <si>
-    <t>7306 PATRIKA</t>
+    <t>7306 PATRIKA (1800)</t>
   </si>
   <si>
     <t>7307 PATRIKA</t>
@@ -1439,7 +1442,7 @@
     <t>7330 PATRIKA</t>
   </si>
   <si>
-    <t>7331 PATRIKA {F/G}</t>
+    <t>7331 PATRIKA {F/G} (2400)</t>
   </si>
   <si>
     <t>7332 PATRIKA</t>
@@ -1634,7 +1637,7 @@
     <t>9048 CARD</t>
   </si>
   <si>
-    <t>9049 CARD</t>
+    <t>9049 CARD (1200)</t>
   </si>
   <si>
     <t>9050 CARD</t>
@@ -1845,6 +1848,12 @@
   </si>
   <si>
     <t>9955 CARDS ♠</t>
+  </si>
+  <si>
+    <t>GIFT ENVELOPE -116</t>
+  </si>
+  <si>
+    <t>GIFT ENVELOPE 143</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2340,13 +2349,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D605"/>
+  <dimension ref="A1:D608"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -2463,13 +2472,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="C11" s="19">
         <v>0.92</v>
       </c>
       <c r="D11" s="20">
-        <v>208.9</v>
+        <v>192.33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2533,13 +2542,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="18">
-        <v>44</v>
+        <v>41.5</v>
       </c>
       <c r="C16" s="19">
         <v>1.8</v>
       </c>
       <c r="D16" s="20">
-        <v>79.2</v>
+        <v>74.7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2547,13 +2556,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="18">
-        <v>123.5</v>
+        <v>121.5</v>
       </c>
       <c r="C17" s="19">
         <v>2</v>
       </c>
       <c r="D17" s="20">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2867,13 +2876,13 @@
         <v>44</v>
       </c>
       <c r="B42" s="18">
-        <v>137.5</v>
+        <v>136.5</v>
       </c>
       <c r="C42" s="19">
         <v>2.85</v>
       </c>
       <c r="D42" s="20">
-        <v>391.88</v>
+        <v>389.03</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2937,13 +2946,13 @@
         <v>49</v>
       </c>
       <c r="B47" s="18">
-        <v>6</v>
+        <v>298</v>
       </c>
       <c r="C47" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D47" s="20">
-        <v>6.6</v>
+        <v>327.8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2951,13 +2960,13 @@
         <v>50</v>
       </c>
       <c r="B48" s="18">
-        <v>18</v>
+        <v>308</v>
       </c>
       <c r="C48" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D48" s="20">
-        <v>19.8</v>
+        <v>338.8</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2965,13 +2974,13 @@
         <v>51</v>
       </c>
       <c r="B49" s="18">
-        <v>14.5</v>
+        <v>304.5</v>
       </c>
       <c r="C49" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D49" s="20">
-        <v>15.95</v>
+        <v>334.95</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,13 +2988,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>123</v>
+        <v>413</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>135.30000000000001</v>
+        <v>454.3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,13 +3002,13 @@
         <v>53</v>
       </c>
       <c r="B51" s="18">
-        <v>8</v>
+        <v>294</v>
       </c>
       <c r="C51" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D51" s="20">
-        <v>8.8000000000000007</v>
+        <v>323.39999999999998</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,13 +3016,13 @@
         <v>54</v>
       </c>
       <c r="B52" s="18">
-        <v>178</v>
+        <v>458</v>
       </c>
       <c r="C52" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D52" s="20">
-        <v>195.8</v>
+        <v>503.8</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3021,13 +3030,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="18">
-        <v>88</v>
+        <v>368</v>
       </c>
       <c r="C53" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D53" s="20">
-        <v>96.8</v>
+        <v>404.8</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,13 +3044,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>24.5</v>
+        <v>304.5</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>26.95</v>
+        <v>334.95</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3049,13 +3058,13 @@
         <v>57</v>
       </c>
       <c r="B55" s="18">
-        <v>16</v>
+        <v>306</v>
       </c>
       <c r="C55" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D55" s="20">
-        <v>17.600000000000001</v>
+        <v>336.6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3063,13 +3072,13 @@
         <v>58</v>
       </c>
       <c r="B56" s="18">
-        <v>-22</v>
+        <v>262</v>
       </c>
       <c r="C56" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D56" s="20">
-        <v>-24.2</v>
+        <v>288.2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3287,13 +3296,13 @@
         <v>74</v>
       </c>
       <c r="B72" s="18">
-        <v>489</v>
+        <v>474</v>
       </c>
       <c r="C72" s="19">
         <v>1.55</v>
       </c>
       <c r="D72" s="20">
-        <v>757.95</v>
+        <v>734.7</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3301,13 +3310,13 @@
         <v>75</v>
       </c>
       <c r="B73" s="18">
-        <v>543</v>
+        <v>521</v>
       </c>
       <c r="C73" s="19">
         <v>1.55</v>
       </c>
       <c r="D73" s="20">
-        <v>841.65</v>
+        <v>807.55</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3315,13 +3324,13 @@
         <v>76</v>
       </c>
       <c r="B74" s="18">
-        <v>700.5</v>
+        <v>696.5</v>
       </c>
       <c r="C74" s="19">
         <v>1.55</v>
       </c>
       <c r="D74" s="20">
-        <v>1085.78</v>
+        <v>1079.58</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3329,7 +3338,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="18">
-        <v>160.5</v>
+        <v>156.5</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="21"/>
@@ -3339,7 +3348,7 @@
         <v>78</v>
       </c>
       <c r="B76" s="18">
-        <v>102.5</v>
+        <v>145.5</v>
       </c>
       <c r="C76" s="22"/>
       <c r="D76" s="21"/>
@@ -3359,7 +3368,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>58.5</v>
+        <v>54.5</v>
       </c>
       <c r="C78" s="22"/>
       <c r="D78" s="21"/>
@@ -3379,7 +3388,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="18">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
@@ -3389,13 +3398,13 @@
         <v>83</v>
       </c>
       <c r="B81" s="18">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="C81" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D81" s="20">
-        <v>657.8</v>
+        <v>647.45000000000005</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3417,13 +3426,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>709</v>
+        <v>686.5</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>992.6</v>
+        <v>961.1</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3445,13 +3454,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="18">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C85" s="19">
         <v>1.4</v>
       </c>
       <c r="D85" s="20">
-        <v>225.4</v>
+        <v>211.4</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,13 +3518,13 @@
         <v>92</v>
       </c>
       <c r="B90" s="18">
-        <v>511.5</v>
+        <v>506.5</v>
       </c>
       <c r="C90" s="19">
         <v>1.26</v>
       </c>
       <c r="D90" s="20">
-        <v>644.49</v>
+        <v>638.19000000000005</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3617,13 +3626,13 @@
         <v>101</v>
       </c>
       <c r="B99" s="18">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C99" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D99" s="20">
-        <v>13.8</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3631,13 +3640,13 @@
         <v>102</v>
       </c>
       <c r="B100" s="18">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C100" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D100" s="20">
-        <v>16.100000000000001</v>
+        <v>14.95</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3645,13 +3654,13 @@
         <v>103</v>
       </c>
       <c r="B101" s="18">
-        <v>22.5</v>
+        <v>18.5</v>
       </c>
       <c r="C101" s="19">
         <v>12.5</v>
       </c>
       <c r="D101" s="20">
-        <v>281.25</v>
+        <v>231.25</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,13 +3682,13 @@
         <v>105</v>
       </c>
       <c r="B103" s="18">
-        <v>51.5</v>
+        <v>51</v>
       </c>
       <c r="C103" s="19">
         <v>12.5</v>
       </c>
       <c r="D103" s="20">
-        <v>643.75</v>
+        <v>637.5</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3687,13 +3696,13 @@
         <v>106</v>
       </c>
       <c r="B104" s="18">
-        <v>52.5</v>
+        <v>44.5</v>
       </c>
       <c r="C104" s="19">
         <v>12.5</v>
       </c>
       <c r="D104" s="20">
-        <v>656.25</v>
+        <v>556.25</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3757,13 +3766,13 @@
         <v>111</v>
       </c>
       <c r="B109" s="18">
-        <v>29.5</v>
+        <v>24</v>
       </c>
       <c r="C109" s="19">
         <v>12.5</v>
       </c>
       <c r="D109" s="20">
-        <v>368.75</v>
+        <v>300</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3771,13 +3780,13 @@
         <v>112</v>
       </c>
       <c r="B110" s="18">
-        <v>13</v>
+        <v>9.5</v>
       </c>
       <c r="C110" s="19">
         <v>12.5</v>
       </c>
       <c r="D110" s="20">
-        <v>162.5</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,13 +3808,13 @@
         <v>114</v>
       </c>
       <c r="B112" s="18">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C112" s="19">
         <v>15.5</v>
       </c>
       <c r="D112" s="20">
-        <v>232.5</v>
+        <v>170.5</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,13 +4102,13 @@
         <v>135</v>
       </c>
       <c r="B133" s="18">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="C133" s="19">
         <v>18.27</v>
       </c>
       <c r="D133" s="20">
-        <v>191.83</v>
+        <v>155.29</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4121,13 +4130,13 @@
         <v>137</v>
       </c>
       <c r="B135" s="18">
-        <v>-1.5</v>
+        <v>3.5</v>
       </c>
       <c r="C135" s="19">
-        <v>18.41</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="D135" s="20">
-        <v>-27.61</v>
+        <v>64.47</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4205,13 +4214,13 @@
         <v>143</v>
       </c>
       <c r="B141" s="18">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C141" s="19">
         <v>2.8</v>
       </c>
       <c r="D141" s="20">
-        <v>137.19999999999999</v>
+        <v>134.4</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4317,13 +4326,13 @@
         <v>151</v>
       </c>
       <c r="B149" s="18">
-        <v>99.5</v>
+        <v>95.5</v>
       </c>
       <c r="C149" s="19">
         <v>2.8</v>
       </c>
       <c r="D149" s="20">
-        <v>278.60000000000002</v>
+        <v>267.39999999999998</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4471,13 +4480,13 @@
         <v>162</v>
       </c>
       <c r="B160" s="18">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C160" s="19">
         <v>3.5</v>
       </c>
       <c r="D160" s="20">
-        <v>206.5</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4549,13 +4558,13 @@
         <v>168</v>
       </c>
       <c r="B166" s="18">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C166" s="19">
         <v>3.33</v>
       </c>
       <c r="D166" s="20">
-        <v>326.33999999999997</v>
+        <v>299.7</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -4577,13 +4586,13 @@
         <v>170</v>
       </c>
       <c r="B168" s="18">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C168" s="19">
         <v>3.6</v>
       </c>
       <c r="D168" s="20">
-        <v>500.4</v>
+        <v>496.8</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,13 +4650,13 @@
         <v>175</v>
       </c>
       <c r="B173" s="18">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C173" s="19">
         <v>4.5</v>
       </c>
       <c r="D173" s="20">
-        <v>675</v>
+        <v>648</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4753,13 +4762,13 @@
         <v>183</v>
       </c>
       <c r="B181" s="18">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C181" s="19">
         <v>4.1500000000000004</v>
       </c>
       <c r="D181" s="20">
-        <v>302.95</v>
+        <v>282.2</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4767,13 +4776,13 @@
         <v>184</v>
       </c>
       <c r="B182" s="18">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C182" s="19">
         <v>3</v>
       </c>
       <c r="D182" s="20">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4853,13 +4862,13 @@
         <v>191</v>
       </c>
       <c r="B189" s="18">
-        <v>38.24</v>
+        <v>31.24</v>
       </c>
       <c r="C189" s="19">
         <v>3.14</v>
       </c>
       <c r="D189" s="20">
-        <v>120.07</v>
+        <v>98.09</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -4941,13 +4950,13 @@
         <v>199</v>
       </c>
       <c r="B197" s="18">
-        <v>12.5</v>
+        <v>4.5</v>
       </c>
       <c r="C197" s="19">
         <v>3.8</v>
       </c>
       <c r="D197" s="20">
-        <v>47.5</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4969,13 +4978,13 @@
         <v>201</v>
       </c>
       <c r="B199" s="18">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C199" s="19">
         <v>3.6</v>
       </c>
       <c r="D199" s="20">
-        <v>61.2</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5005,13 +5014,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>33</v>
+        <v>28.5</v>
       </c>
       <c r="C202" s="19">
         <v>4.12</v>
       </c>
       <c r="D202" s="20">
-        <v>135.83000000000001</v>
+        <v>117.31</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5111,13 +5120,13 @@
         <v>212</v>
       </c>
       <c r="B210" s="18">
-        <v>279.5</v>
+        <v>277.5</v>
       </c>
       <c r="C210" s="19">
         <v>4.5</v>
       </c>
       <c r="D210" s="20">
-        <v>1257.75</v>
+        <v>1248.75</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5125,13 +5134,13 @@
         <v>213</v>
       </c>
       <c r="B211" s="18">
-        <v>136</v>
+        <v>133.5</v>
       </c>
       <c r="C211" s="19">
         <v>4.5</v>
       </c>
       <c r="D211" s="20">
-        <v>612</v>
+        <v>600.75</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5195,13 +5204,13 @@
         <v>218</v>
       </c>
       <c r="B216" s="18">
-        <v>18.5</v>
+        <v>18</v>
       </c>
       <c r="C216" s="19">
         <v>4.75</v>
       </c>
       <c r="D216" s="20">
-        <v>87.88</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5301,13 +5310,13 @@
         <v>226</v>
       </c>
       <c r="B224" s="18">
-        <v>39.5</v>
+        <v>36.5</v>
       </c>
       <c r="C224" s="19">
         <v>6</v>
       </c>
       <c r="D224" s="20">
-        <v>237</v>
+        <v>219</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5337,13 +5346,13 @@
         <v>229</v>
       </c>
       <c r="B227" s="18">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="C227" s="19">
         <v>5.7</v>
       </c>
       <c r="D227" s="20">
-        <v>-11.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5421,13 +5430,13 @@
         <v>235</v>
       </c>
       <c r="B233" s="18">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="C233" s="19">
         <v>4</v>
       </c>
       <c r="D233" s="20">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5435,13 +5444,13 @@
         <v>236</v>
       </c>
       <c r="B234" s="18">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="C234" s="19">
         <v>4</v>
       </c>
       <c r="D234" s="20">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5513,13 +5522,13 @@
         <v>242</v>
       </c>
       <c r="B240" s="18">
-        <v>45.5</v>
+        <v>40.5</v>
       </c>
       <c r="C240" s="19">
         <v>3.5</v>
       </c>
       <c r="D240" s="20">
-        <v>159.25</v>
+        <v>141.75</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,13 +5572,13 @@
         <v>246</v>
       </c>
       <c r="B244" s="18">
-        <v>57.5</v>
+        <v>54.5</v>
       </c>
       <c r="C244" s="19">
         <v>4.18</v>
       </c>
       <c r="D244" s="20">
-        <v>240.35</v>
+        <v>227.81</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -5605,13 +5614,13 @@
         <v>249</v>
       </c>
       <c r="B247" s="18">
-        <v>75</v>
+        <v>72.5</v>
       </c>
       <c r="C247" s="19">
         <v>4.28</v>
       </c>
       <c r="D247" s="20">
-        <v>321</v>
+        <v>310.3</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5733,13 +5742,13 @@
         <v>259</v>
       </c>
       <c r="B257" s="18">
-        <v>46</v>
+        <v>44.5</v>
       </c>
       <c r="C257" s="19">
         <v>5.4</v>
       </c>
       <c r="D257" s="20">
-        <v>248.4</v>
+        <v>240.3</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -5761,13 +5770,13 @@
         <v>261</v>
       </c>
       <c r="B259" s="18">
-        <v>49.5</v>
+        <v>44.5</v>
       </c>
       <c r="C259" s="19">
         <v>5.55</v>
       </c>
       <c r="D259" s="20">
-        <v>274.73</v>
+        <v>246.98</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -5909,13 +5918,13 @@
         <v>272</v>
       </c>
       <c r="B270" s="18">
-        <v>23.5</v>
+        <v>19.5</v>
       </c>
       <c r="C270" s="19">
         <v>5.7</v>
       </c>
       <c r="D270" s="20">
-        <v>133.94999999999999</v>
+        <v>111.15</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6343,13 +6352,13 @@
         <v>306</v>
       </c>
       <c r="B304" s="18">
-        <v>11.5</v>
+        <v>8.5</v>
       </c>
       <c r="C304" s="19">
         <v>8.85</v>
       </c>
       <c r="D304" s="20">
-        <v>101.78</v>
+        <v>75.23</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.25">
@@ -6385,13 +6394,13 @@
         <v>309</v>
       </c>
       <c r="B307" s="18">
-        <v>14.5</v>
+        <v>23.5</v>
       </c>
       <c r="C307" s="19">
         <v>9.25</v>
       </c>
       <c r="D307" s="20">
-        <v>134.13</v>
+        <v>217.38</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -6399,13 +6408,13 @@
         <v>310</v>
       </c>
       <c r="B308" s="18">
-        <v>27.7</v>
+        <v>23.2</v>
       </c>
       <c r="C308" s="19">
         <v>8.8000000000000007</v>
       </c>
       <c r="D308" s="20">
-        <v>243.76</v>
+        <v>204.16</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6441,13 +6450,13 @@
         <v>313</v>
       </c>
       <c r="B311" s="18">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C311" s="19">
         <v>9.5</v>
       </c>
       <c r="D311" s="20">
-        <v>104.5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.25">
@@ -6483,13 +6492,13 @@
         <v>316</v>
       </c>
       <c r="B314" s="18">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="C314" s="19">
         <v>9.25</v>
       </c>
       <c r="D314" s="20">
-        <v>50.88</v>
+        <v>46.25</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -6637,28 +6646,22 @@
         <v>327</v>
       </c>
       <c r="B325" s="18">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="C325" s="19">
         <v>10.61</v>
       </c>
       <c r="D325" s="20">
-        <v>169.83</v>
+        <v>164.52</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="B326" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="C326" s="19">
-        <v>7.84</v>
-      </c>
-      <c r="D326" s="20">
-        <v>3.92</v>
-      </c>
+      <c r="B326" s="21"/>
+      <c r="C326" s="22"/>
+      <c r="D326" s="21"/>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="17" t="s">
@@ -6723,13 +6726,13 @@
         <v>334</v>
       </c>
       <c r="B332" s="18">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C332" s="19">
         <v>4.9000000000000004</v>
       </c>
       <c r="D332" s="20">
-        <v>78.400000000000006</v>
+        <v>58.8</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -7087,13 +7090,13 @@
         <v>360</v>
       </c>
       <c r="B358" s="18">
-        <v>-1.5</v>
+        <v>-6</v>
       </c>
       <c r="C358" s="19">
         <v>10</v>
       </c>
       <c r="D358" s="20">
-        <v>-15</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7101,13 +7104,13 @@
         <v>361</v>
       </c>
       <c r="B359" s="18">
-        <v>18.5</v>
+        <v>16</v>
       </c>
       <c r="C359" s="19">
         <v>10.5</v>
       </c>
       <c r="D359" s="20">
-        <v>194.25</v>
+        <v>168</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -7297,22 +7300,28 @@
         <v>375</v>
       </c>
       <c r="B373" s="18">
-        <v>18.5</v>
+        <v>15.5</v>
       </c>
       <c r="C373" s="19">
         <v>12.5</v>
       </c>
       <c r="D373" s="20">
-        <v>231.25</v>
+        <v>193.75</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A374" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="B374" s="21"/>
-      <c r="C374" s="22"/>
-      <c r="D374" s="21"/>
+      <c r="B374" s="18">
+        <v>6</v>
+      </c>
+      <c r="C374" s="19">
+        <v>21.5</v>
+      </c>
+      <c r="D374" s="20">
+        <v>129</v>
+      </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A375" s="17" t="s">
@@ -7445,13 +7454,13 @@
         <v>386</v>
       </c>
       <c r="B384" s="18">
-        <v>23</v>
+        <v>21.5</v>
       </c>
       <c r="C384" s="19">
         <v>10.93</v>
       </c>
       <c r="D384" s="20">
-        <v>251.39</v>
+        <v>235</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
@@ -7556,31 +7565,37 @@
       <c r="A392" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="B392" s="21"/>
-      <c r="C392" s="22"/>
-      <c r="D392" s="21"/>
+      <c r="B392" s="18">
+        <v>81</v>
+      </c>
+      <c r="C392" s="19">
+        <v>2</v>
+      </c>
+      <c r="D392" s="20">
+        <v>162</v>
+      </c>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="B393" s="18">
-        <v>54.5</v>
-      </c>
-      <c r="C393" s="19">
-        <v>2</v>
-      </c>
-      <c r="D393" s="20">
-        <v>109</v>
-      </c>
+      <c r="B393" s="21"/>
+      <c r="C393" s="22"/>
+      <c r="D393" s="21"/>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="B394" s="21"/>
-      <c r="C394" s="22"/>
-      <c r="D394" s="21"/>
+      <c r="B394" s="18">
+        <v>54.5</v>
+      </c>
+      <c r="C394" s="19">
+        <v>2</v>
+      </c>
+      <c r="D394" s="20">
+        <v>109</v>
+      </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395" s="17" t="s">
@@ -7594,28 +7609,22 @@
       <c r="A396" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="B396" s="18">
-        <v>14</v>
-      </c>
-      <c r="C396" s="19">
-        <v>2.5</v>
-      </c>
-      <c r="D396" s="20">
-        <v>35</v>
-      </c>
+      <c r="B396" s="21"/>
+      <c r="C396" s="22"/>
+      <c r="D396" s="21"/>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397" s="17" t="s">
         <v>399</v>
       </c>
       <c r="B397" s="18">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C397" s="19">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="D397" s="20">
-        <v>155.25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.25">
@@ -7623,13 +7632,13 @@
         <v>400</v>
       </c>
       <c r="B398" s="18">
-        <v>62.5</v>
+        <v>67</v>
       </c>
       <c r="C398" s="19">
         <v>2.25</v>
       </c>
       <c r="D398" s="20">
-        <v>140.63</v>
+        <v>150.75</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -7637,13 +7646,13 @@
         <v>401</v>
       </c>
       <c r="B399" s="18">
-        <v>24</v>
+        <v>62.5</v>
       </c>
       <c r="C399" s="19">
         <v>2.25</v>
       </c>
       <c r="D399" s="20">
-        <v>54</v>
+        <v>140.63</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -7651,13 +7660,13 @@
         <v>402</v>
       </c>
       <c r="B400" s="18">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C400" s="19">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="D400" s="20">
-        <v>37.5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
@@ -7665,13 +7674,13 @@
         <v>403</v>
       </c>
       <c r="B401" s="18">
-        <v>22.5</v>
+        <v>15</v>
       </c>
       <c r="C401" s="19">
         <v>2.5</v>
       </c>
       <c r="D401" s="20">
-        <v>56.25</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -7679,13 +7688,13 @@
         <v>404</v>
       </c>
       <c r="B402" s="18">
-        <v>8.5</v>
+        <v>22.5</v>
       </c>
       <c r="C402" s="19">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="D402" s="20">
-        <v>22.95</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
@@ -7693,13 +7702,13 @@
         <v>405</v>
       </c>
       <c r="B403" s="18">
-        <v>80</v>
+        <v>8.5</v>
       </c>
       <c r="C403" s="19">
         <v>2.7</v>
       </c>
       <c r="D403" s="20">
-        <v>216</v>
+        <v>22.95</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.25">
@@ -7707,13 +7716,13 @@
         <v>406</v>
       </c>
       <c r="B404" s="18">
-        <v>57.5</v>
+        <v>80</v>
       </c>
       <c r="C404" s="19">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="D404" s="20">
-        <v>149.5</v>
+        <v>216</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
@@ -7721,13 +7730,13 @@
         <v>407</v>
       </c>
       <c r="B405" s="18">
-        <v>73</v>
+        <v>57.5</v>
       </c>
       <c r="C405" s="19">
-        <v>2.75</v>
+        <v>2.6</v>
       </c>
       <c r="D405" s="20">
-        <v>200.75</v>
+        <v>149.5</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -7735,13 +7744,13 @@
         <v>408</v>
       </c>
       <c r="B406" s="18">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C406" s="19">
         <v>2.75</v>
       </c>
       <c r="D406" s="20">
-        <v>99</v>
+        <v>200.75</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -7749,13 +7758,13 @@
         <v>409</v>
       </c>
       <c r="B407" s="18">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C407" s="19">
-        <v>3.8</v>
+        <v>2.75</v>
       </c>
       <c r="D407" s="20">
-        <v>171</v>
+        <v>90.75</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
@@ -7763,13 +7772,13 @@
         <v>410</v>
       </c>
       <c r="B408" s="18">
-        <v>24.5</v>
+        <v>45</v>
       </c>
       <c r="C408" s="19">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
       <c r="D408" s="20">
-        <v>68.599999999999994</v>
+        <v>171</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.25">
@@ -7777,49 +7786,49 @@
         <v>411</v>
       </c>
       <c r="B409" s="18">
-        <v>32</v>
+        <v>24.5</v>
       </c>
       <c r="C409" s="19">
         <v>2.8</v>
       </c>
       <c r="D409" s="20">
-        <v>89.6</v>
+        <v>68.599999999999994</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A410" s="17" t="s">
         <v>412</v>
       </c>
-      <c r="B410" s="21"/>
-      <c r="C410" s="22"/>
-      <c r="D410" s="21"/>
+      <c r="B410" s="18">
+        <v>32</v>
+      </c>
+      <c r="C410" s="19">
+        <v>2.8</v>
+      </c>
+      <c r="D410" s="20">
+        <v>89.6</v>
+      </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A411" s="17" t="s">
         <v>413</v>
       </c>
-      <c r="B411" s="18">
-        <v>63.5</v>
-      </c>
-      <c r="C411" s="19">
-        <v>2.8</v>
-      </c>
-      <c r="D411" s="20">
-        <v>177.8</v>
-      </c>
+      <c r="B411" s="21"/>
+      <c r="C411" s="22"/>
+      <c r="D411" s="21"/>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A412" s="17" t="s">
         <v>414</v>
       </c>
       <c r="B412" s="18">
-        <v>44</v>
+        <v>63.5</v>
       </c>
       <c r="C412" s="19">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="D412" s="20">
-        <v>129.80000000000001</v>
+        <v>177.8</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
@@ -7827,13 +7836,13 @@
         <v>415</v>
       </c>
       <c r="B413" s="18">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C413" s="19">
-        <v>3.1</v>
+        <v>2.95</v>
       </c>
       <c r="D413" s="20">
-        <v>80.599999999999994</v>
+        <v>129.80000000000001</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
@@ -7841,13 +7850,13 @@
         <v>416</v>
       </c>
       <c r="B414" s="18">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C414" s="19">
-        <v>2.85</v>
+        <v>3.1</v>
       </c>
       <c r="D414" s="20">
-        <v>59.85</v>
+        <v>80.599999999999994</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
@@ -7855,13 +7864,13 @@
         <v>417</v>
       </c>
       <c r="B415" s="18">
-        <v>29.5</v>
+        <v>21</v>
       </c>
       <c r="C415" s="19">
-        <v>3.26</v>
+        <v>2.85</v>
       </c>
       <c r="D415" s="20">
-        <v>96.17</v>
+        <v>59.85</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
@@ -7869,13 +7878,13 @@
         <v>418</v>
       </c>
       <c r="B416" s="18">
-        <v>43.5</v>
+        <v>29.5</v>
       </c>
       <c r="C416" s="19">
-        <v>3.3</v>
+        <v>3.26</v>
       </c>
       <c r="D416" s="20">
-        <v>143.55000000000001</v>
+        <v>96.17</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
@@ -7883,85 +7892,85 @@
         <v>419</v>
       </c>
       <c r="B417" s="18">
-        <v>19.95</v>
+        <v>43.5</v>
       </c>
       <c r="C417" s="19">
-        <v>3.15</v>
+        <v>3.3</v>
       </c>
       <c r="D417" s="20">
-        <v>62.84</v>
+        <v>143.55000000000001</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A418" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="B418" s="21"/>
-      <c r="C418" s="22"/>
-      <c r="D418" s="21"/>
+      <c r="B418" s="18">
+        <v>17.95</v>
+      </c>
+      <c r="C418" s="19">
+        <v>3.15</v>
+      </c>
+      <c r="D418" s="20">
+        <v>56.54</v>
+      </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A419" s="17" t="s">
         <v>421</v>
       </c>
-      <c r="B419" s="18">
-        <v>16.5</v>
-      </c>
-      <c r="C419" s="19">
-        <v>3.25</v>
-      </c>
-      <c r="D419" s="20">
-        <v>53.63</v>
-      </c>
+      <c r="B419" s="21"/>
+      <c r="C419" s="22"/>
+      <c r="D419" s="21"/>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A420" s="17" t="s">
         <v>422</v>
       </c>
       <c r="B420" s="18">
-        <v>36</v>
+        <v>16.5</v>
       </c>
       <c r="C420" s="19">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D420" s="20">
-        <v>126</v>
+        <v>53.63</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A421" s="17" t="s">
         <v>423</v>
       </c>
-      <c r="B421" s="21"/>
-      <c r="C421" s="22"/>
-      <c r="D421" s="21"/>
+      <c r="B421" s="18">
+        <v>35</v>
+      </c>
+      <c r="C421" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="D421" s="20">
+        <v>122.5</v>
+      </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A422" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="B422" s="18">
-        <v>44</v>
-      </c>
-      <c r="C422" s="19">
-        <v>3.25</v>
-      </c>
-      <c r="D422" s="20">
-        <v>143</v>
-      </c>
+      <c r="B422" s="21"/>
+      <c r="C422" s="22"/>
+      <c r="D422" s="21"/>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" s="17" t="s">
         <v>425</v>
       </c>
       <c r="B423" s="18">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C423" s="19">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="D423" s="20">
-        <v>78.2</v>
+        <v>143</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -7969,13 +7978,13 @@
         <v>426</v>
       </c>
       <c r="B424" s="18">
-        <v>45.56</v>
+        <v>23</v>
       </c>
       <c r="C424" s="19">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="D424" s="20">
-        <v>159.46</v>
+        <v>78.2</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
@@ -7983,13 +7992,13 @@
         <v>427</v>
       </c>
       <c r="B425" s="18">
-        <v>60.5</v>
+        <v>45.56</v>
       </c>
       <c r="C425" s="19">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="D425" s="20">
-        <v>229.9</v>
+        <v>159.46</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
@@ -7997,13 +8006,13 @@
         <v>428</v>
       </c>
       <c r="B426" s="18">
-        <v>28</v>
+        <v>60.5</v>
       </c>
       <c r="C426" s="19">
-        <v>3.9</v>
+        <v>3.8</v>
       </c>
       <c r="D426" s="20">
-        <v>109.2</v>
+        <v>229.9</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
@@ -8011,13 +8020,13 @@
         <v>429</v>
       </c>
       <c r="B427" s="18">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C427" s="19">
-        <v>3.33</v>
+        <v>3.9</v>
       </c>
       <c r="D427" s="20">
-        <v>119.88</v>
+        <v>109.2</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
@@ -8025,22 +8034,28 @@
         <v>430</v>
       </c>
       <c r="B428" s="18">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C428" s="19">
         <v>3.33</v>
       </c>
       <c r="D428" s="20">
-        <v>189.81</v>
+        <v>119.88</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A429" s="17" t="s">
         <v>431</v>
       </c>
-      <c r="B429" s="21"/>
-      <c r="C429" s="22"/>
-      <c r="D429" s="21"/>
+      <c r="B429" s="18">
+        <v>57</v>
+      </c>
+      <c r="C429" s="19">
+        <v>3.33</v>
+      </c>
+      <c r="D429" s="20">
+        <v>189.81</v>
+      </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A430" s="17" t="s">
@@ -8054,28 +8069,22 @@
       <c r="A431" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="B431" s="18">
-        <v>50.5</v>
-      </c>
-      <c r="C431" s="19">
-        <v>3.8</v>
-      </c>
-      <c r="D431" s="20">
-        <v>191.9</v>
-      </c>
+      <c r="B431" s="21"/>
+      <c r="C431" s="22"/>
+      <c r="D431" s="21"/>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A432" s="17" t="s">
         <v>434</v>
       </c>
       <c r="B432" s="18">
-        <v>35.5</v>
+        <v>50.5</v>
       </c>
       <c r="C432" s="19">
-        <v>4.25</v>
+        <v>3.8</v>
       </c>
       <c r="D432" s="20">
-        <v>150.88</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
@@ -8083,13 +8092,13 @@
         <v>435</v>
       </c>
       <c r="B433" s="18">
-        <v>28.5</v>
+        <v>35.5</v>
       </c>
       <c r="C433" s="19">
-        <v>3.8</v>
+        <v>4.25</v>
       </c>
       <c r="D433" s="20">
-        <v>108.3</v>
+        <v>150.88</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -8097,13 +8106,13 @@
         <v>436</v>
       </c>
       <c r="B434" s="18">
-        <v>10</v>
+        <v>28.5</v>
       </c>
       <c r="C434" s="19">
-        <v>4.0999999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="D434" s="20">
-        <v>40.98</v>
+        <v>108.3</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
@@ -8111,13 +8120,13 @@
         <v>437</v>
       </c>
       <c r="B435" s="18">
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="C435" s="19">
-        <v>4.25</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D435" s="20">
-        <v>53.13</v>
+        <v>40.98</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -8125,13 +8134,13 @@
         <v>438</v>
       </c>
       <c r="B436" s="18">
-        <v>13</v>
+        <v>12.5</v>
       </c>
       <c r="C436" s="19">
-        <v>4.75</v>
+        <v>4.25</v>
       </c>
       <c r="D436" s="20">
-        <v>61.75</v>
+        <v>53.13</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
@@ -8139,13 +8148,13 @@
         <v>439</v>
       </c>
       <c r="B437" s="18">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C437" s="19">
-        <v>4.9000000000000004</v>
+        <v>4.75</v>
       </c>
       <c r="D437" s="20">
-        <v>102.9</v>
+        <v>61.75</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
@@ -8153,13 +8162,13 @@
         <v>440</v>
       </c>
       <c r="B438" s="18">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C438" s="19">
-        <v>4.28</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D438" s="20">
-        <v>128.4</v>
+        <v>102.9</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
@@ -8170,10 +8179,10 @@
         <v>30</v>
       </c>
       <c r="C439" s="19">
-        <v>4.18</v>
+        <v>4.28</v>
       </c>
       <c r="D439" s="20">
-        <v>125.4</v>
+        <v>128.4</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
@@ -8181,13 +8190,13 @@
         <v>442</v>
       </c>
       <c r="B440" s="18">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C440" s="19">
-        <v>4.28</v>
+        <v>4.18</v>
       </c>
       <c r="D440" s="20">
-        <v>77.040000000000006</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
@@ -8195,49 +8204,49 @@
         <v>443</v>
       </c>
       <c r="B441" s="18">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C441" s="19">
-        <v>4.75</v>
+        <v>4.28</v>
       </c>
       <c r="D441" s="20">
-        <v>237.5</v>
+        <v>77.040000000000006</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A442" s="17" t="s">
         <v>444</v>
       </c>
-      <c r="B442" s="21"/>
-      <c r="C442" s="22"/>
-      <c r="D442" s="21"/>
+      <c r="B442" s="18">
+        <v>50</v>
+      </c>
+      <c r="C442" s="19">
+        <v>4.75</v>
+      </c>
+      <c r="D442" s="20">
+        <v>237.5</v>
+      </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A443" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="B443" s="18">
-        <v>34</v>
-      </c>
-      <c r="C443" s="19">
-        <v>4.75</v>
-      </c>
-      <c r="D443" s="20">
-        <v>161.5</v>
-      </c>
+      <c r="B443" s="21"/>
+      <c r="C443" s="22"/>
+      <c r="D443" s="21"/>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A444" s="17" t="s">
         <v>446</v>
       </c>
       <c r="B444" s="18">
-        <v>2.5</v>
+        <v>34</v>
       </c>
       <c r="C444" s="19">
-        <v>5.25</v>
+        <v>4.75</v>
       </c>
       <c r="D444" s="20">
-        <v>13.13</v>
+        <v>161.5</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8245,13 +8254,13 @@
         <v>447</v>
       </c>
       <c r="B445" s="18">
-        <v>13</v>
+        <v>2.5</v>
       </c>
       <c r="C445" s="19">
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="D445" s="20">
-        <v>58.5</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8259,13 +8268,13 @@
         <v>448</v>
       </c>
       <c r="B446" s="18">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C446" s="19">
-        <v>5.25</v>
+        <v>4.5</v>
       </c>
       <c r="D446" s="20">
-        <v>57.75</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -8273,13 +8282,13 @@
         <v>449</v>
       </c>
       <c r="B447" s="18">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C447" s="19">
-        <v>4.5999999999999996</v>
+        <v>5.25</v>
       </c>
       <c r="D447" s="20">
-        <v>133.4</v>
+        <v>57.75</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -8287,13 +8296,13 @@
         <v>450</v>
       </c>
       <c r="B448" s="18">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C448" s="19">
-        <v>5.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D448" s="20">
-        <v>363</v>
+        <v>133.4</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -8301,13 +8310,13 @@
         <v>451</v>
       </c>
       <c r="B449" s="18">
-        <v>5.5</v>
+        <v>60.5</v>
       </c>
       <c r="C449" s="19">
         <v>5.5</v>
       </c>
       <c r="D449" s="20">
-        <v>30.25</v>
+        <v>332.75</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
@@ -8315,13 +8324,13 @@
         <v>452</v>
       </c>
       <c r="B450" s="18">
-        <v>29.5</v>
+        <v>5.5</v>
       </c>
       <c r="C450" s="19">
-        <v>5.23</v>
+        <v>5.5</v>
       </c>
       <c r="D450" s="20">
-        <v>154.29</v>
+        <v>30.25</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
@@ -8329,71 +8338,71 @@
         <v>453</v>
       </c>
       <c r="B451" s="18">
-        <v>10.5</v>
+        <v>29.5</v>
       </c>
       <c r="C451" s="19">
-        <v>6.25</v>
+        <v>5.23</v>
       </c>
       <c r="D451" s="20">
-        <v>65.63</v>
+        <v>154.29</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A452" s="17" t="s">
         <v>454</v>
       </c>
-      <c r="B452" s="21"/>
-      <c r="C452" s="22"/>
-      <c r="D452" s="21"/>
+      <c r="B452" s="18">
+        <v>10.5</v>
+      </c>
+      <c r="C452" s="19">
+        <v>6.25</v>
+      </c>
+      <c r="D452" s="20">
+        <v>65.63</v>
+      </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A453" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="B453" s="18">
-        <v>46</v>
-      </c>
-      <c r="C453" s="19">
-        <v>6</v>
-      </c>
-      <c r="D453" s="20">
-        <v>276</v>
-      </c>
+      <c r="B453" s="21"/>
+      <c r="C453" s="22"/>
+      <c r="D453" s="21"/>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A454" s="17" t="s">
         <v>456</v>
       </c>
-      <c r="B454" s="21"/>
-      <c r="C454" s="22"/>
-      <c r="D454" s="21"/>
+      <c r="B454" s="18">
+        <v>46</v>
+      </c>
+      <c r="C454" s="19">
+        <v>6</v>
+      </c>
+      <c r="D454" s="20">
+        <v>276</v>
+      </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A455" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="B455" s="18">
-        <v>23.5</v>
-      </c>
-      <c r="C455" s="19">
-        <v>5.94</v>
-      </c>
-      <c r="D455" s="20">
-        <v>139.59</v>
-      </c>
+      <c r="B455" s="21"/>
+      <c r="C455" s="22"/>
+      <c r="D455" s="21"/>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A456" s="17" t="s">
         <v>458</v>
       </c>
       <c r="B456" s="18">
-        <v>21</v>
+        <v>23.5</v>
       </c>
       <c r="C456" s="19">
-        <v>6.75</v>
+        <v>5.94</v>
       </c>
       <c r="D456" s="20">
-        <v>141.75</v>
+        <v>139.59</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -8401,13 +8410,13 @@
         <v>459</v>
       </c>
       <c r="B457" s="18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C457" s="19">
-        <v>7.5</v>
+        <v>6.75</v>
       </c>
       <c r="D457" s="20">
-        <v>127.5</v>
+        <v>141.75</v>
       </c>
     </row>
     <row r="458" spans="1:4" x14ac:dyDescent="0.25">
@@ -8415,13 +8424,13 @@
         <v>460</v>
       </c>
       <c r="B458" s="18">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C458" s="19">
-        <v>7.13</v>
+        <v>7.5</v>
       </c>
       <c r="D458" s="20">
-        <v>342.24</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -8429,13 +8438,13 @@
         <v>461</v>
       </c>
       <c r="B459" s="18">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C459" s="19">
-        <v>8</v>
+        <v>7.13</v>
       </c>
       <c r="D459" s="20">
-        <v>192</v>
+        <v>335.11</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
@@ -8443,13 +8452,13 @@
         <v>462</v>
       </c>
       <c r="B460" s="18">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C460" s="19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D460" s="20">
-        <v>175</v>
+        <v>192</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -8457,13 +8466,13 @@
         <v>463</v>
       </c>
       <c r="B461" s="18">
-        <v>30.5</v>
+        <v>25</v>
       </c>
       <c r="C461" s="19">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="D461" s="20">
-        <v>231.8</v>
+        <v>175</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -8471,13 +8480,13 @@
         <v>464</v>
       </c>
       <c r="B462" s="18">
-        <v>43</v>
+        <v>30.5</v>
       </c>
       <c r="C462" s="19">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
       <c r="D462" s="20">
-        <v>365.5</v>
+        <v>231.8</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -8485,13 +8494,13 @@
         <v>465</v>
       </c>
       <c r="B463" s="18">
-        <v>24.5</v>
+        <v>43</v>
       </c>
       <c r="C463" s="19">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D463" s="20">
-        <v>183.75</v>
+        <v>365.5</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.25">
@@ -8499,49 +8508,49 @@
         <v>466</v>
       </c>
       <c r="B464" s="18">
-        <v>6.5</v>
+        <v>24.5</v>
       </c>
       <c r="C464" s="19">
-        <v>8.25</v>
+        <v>7.5</v>
       </c>
       <c r="D464" s="20">
-        <v>53.63</v>
+        <v>183.75</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A465" s="17" t="s">
         <v>467</v>
       </c>
-      <c r="B465" s="21"/>
-      <c r="C465" s="22"/>
-      <c r="D465" s="21"/>
+      <c r="B465" s="18">
+        <v>6.5</v>
+      </c>
+      <c r="C465" s="19">
+        <v>8.25</v>
+      </c>
+      <c r="D465" s="20">
+        <v>53.63</v>
+      </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A466" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="B466" s="18">
-        <v>11.5</v>
-      </c>
-      <c r="C466" s="19">
-        <v>9</v>
-      </c>
-      <c r="D466" s="20">
-        <v>103.5</v>
-      </c>
+      <c r="B466" s="21"/>
+      <c r="C466" s="22"/>
+      <c r="D466" s="21"/>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A467" s="17" t="s">
         <v>469</v>
       </c>
       <c r="B467" s="18">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="C467" s="19">
-        <v>3.75</v>
+        <v>9</v>
       </c>
       <c r="D467" s="20">
-        <v>50.63</v>
+        <v>103.5</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
@@ -8549,13 +8558,13 @@
         <v>470</v>
       </c>
       <c r="B468" s="18">
-        <v>24</v>
+        <v>13.5</v>
       </c>
       <c r="C468" s="19">
-        <v>4.28</v>
+        <v>3.75</v>
       </c>
       <c r="D468" s="20">
-        <v>102.72</v>
+        <v>50.63</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -8563,13 +8572,13 @@
         <v>471</v>
       </c>
       <c r="B469" s="18">
-        <v>15.5</v>
+        <v>24</v>
       </c>
       <c r="C469" s="19">
-        <v>9.5</v>
+        <v>4.28</v>
       </c>
       <c r="D469" s="20">
-        <v>147.25</v>
+        <v>102.72</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -8577,13 +8586,13 @@
         <v>472</v>
       </c>
       <c r="B470" s="18">
-        <v>35.5</v>
+        <v>15.5</v>
       </c>
       <c r="C470" s="19">
-        <v>4.5</v>
+        <v>9.5</v>
       </c>
       <c r="D470" s="20">
-        <v>159.75</v>
+        <v>147.25</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -8591,13 +8600,13 @@
         <v>473</v>
       </c>
       <c r="B471" s="18">
-        <v>50</v>
+        <v>35.5</v>
       </c>
       <c r="C471" s="19">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="D471" s="20">
-        <v>140</v>
+        <v>159.75</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
@@ -8605,13 +8614,13 @@
         <v>474</v>
       </c>
       <c r="B472" s="18">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C472" s="19">
-        <v>5.7</v>
+        <v>2.8</v>
       </c>
       <c r="D472" s="20">
-        <v>228</v>
+        <v>140</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
@@ -8619,13 +8628,13 @@
         <v>475</v>
       </c>
       <c r="B473" s="18">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C473" s="19">
-        <v>1.92</v>
+        <v>5.7</v>
       </c>
       <c r="D473" s="20">
-        <v>65.23</v>
+        <v>228</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
@@ -8633,13 +8642,13 @@
         <v>476</v>
       </c>
       <c r="B474" s="18">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C474" s="19">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="D474" s="20">
-        <v>172.9</v>
+        <v>65.23</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
@@ -8647,13 +8656,13 @@
         <v>477</v>
       </c>
       <c r="B475" s="18">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="C475" s="19">
-        <v>1.1000000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="D475" s="20">
-        <v>15.4</v>
+        <v>172.9</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
@@ -8661,13 +8670,13 @@
         <v>478</v>
       </c>
       <c r="B476" s="18">
-        <v>-3.5</v>
+        <v>29</v>
       </c>
       <c r="C476" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D476" s="20">
-        <v>-3.85</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -8675,13 +8684,13 @@
         <v>479</v>
       </c>
       <c r="B477" s="18">
-        <v>56</v>
+        <v>5.5</v>
       </c>
       <c r="C477" s="19">
-        <v>4.1500000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D477" s="20">
-        <v>232.4</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
@@ -8689,13 +8698,13 @@
         <v>480</v>
       </c>
       <c r="B478" s="18">
-        <v>135</v>
+        <v>56</v>
       </c>
       <c r="C478" s="19">
-        <v>1.4</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="D478" s="20">
-        <v>189</v>
+        <v>232.4</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
@@ -8703,13 +8712,13 @@
         <v>481</v>
       </c>
       <c r="B479" s="18">
-        <v>149.5</v>
+        <v>135</v>
       </c>
       <c r="C479" s="19">
         <v>1.4</v>
       </c>
       <c r="D479" s="20">
-        <v>209.3</v>
+        <v>189</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -8717,13 +8726,13 @@
         <v>482</v>
       </c>
       <c r="B480" s="18">
-        <v>86.5</v>
+        <v>149.5</v>
       </c>
       <c r="C480" s="19">
         <v>1.4</v>
       </c>
       <c r="D480" s="20">
-        <v>121.1</v>
+        <v>209.3</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -8731,13 +8740,13 @@
         <v>483</v>
       </c>
       <c r="B481" s="18">
-        <v>21.5</v>
+        <v>86.5</v>
       </c>
       <c r="C481" s="19">
-        <v>3</v>
+        <v>1.4</v>
       </c>
       <c r="D481" s="20">
-        <v>64.5</v>
+        <v>121.1</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
@@ -8745,13 +8754,13 @@
         <v>484</v>
       </c>
       <c r="B482" s="18">
-        <v>30.5</v>
+        <v>21.5</v>
       </c>
       <c r="C482" s="19">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="D482" s="20">
-        <v>93.03</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
@@ -8759,13 +8768,13 @@
         <v>485</v>
       </c>
       <c r="B483" s="18">
-        <v>28</v>
+        <v>30.5</v>
       </c>
       <c r="C483" s="19">
-        <v>1.55</v>
+        <v>3.05</v>
       </c>
       <c r="D483" s="20">
-        <v>43.4</v>
+        <v>93.03</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
@@ -8773,13 +8782,13 @@
         <v>486</v>
       </c>
       <c r="B484" s="18">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C484" s="19">
         <v>1.55</v>
       </c>
       <c r="D484" s="20">
-        <v>15.5</v>
+        <v>43.4</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
@@ -8787,13 +8796,13 @@
         <v>487</v>
       </c>
       <c r="B485" s="18">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="C485" s="19">
-        <v>1.38</v>
+        <v>1.55</v>
       </c>
       <c r="D485" s="20">
-        <v>227.41</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
@@ -8801,13 +8810,13 @@
         <v>488</v>
       </c>
       <c r="B486" s="18">
-        <v>96</v>
+        <v>165</v>
       </c>
       <c r="C486" s="19">
-        <v>1.5</v>
+        <v>1.38</v>
       </c>
       <c r="D486" s="20">
-        <v>144</v>
+        <v>227.41</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
@@ -8815,13 +8824,13 @@
         <v>489</v>
       </c>
       <c r="B487" s="18">
-        <v>204</v>
+        <v>96</v>
       </c>
       <c r="C487" s="19">
         <v>1.5</v>
       </c>
       <c r="D487" s="20">
-        <v>306</v>
+        <v>144</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -8829,13 +8838,13 @@
         <v>490</v>
       </c>
       <c r="B488" s="18">
-        <v>350.5</v>
+        <v>204</v>
       </c>
       <c r="C488" s="19">
         <v>1.5</v>
       </c>
       <c r="D488" s="20">
-        <v>525.75</v>
+        <v>306</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -8843,13 +8852,13 @@
         <v>491</v>
       </c>
       <c r="B489" s="18">
-        <v>48.5</v>
+        <v>350.5</v>
       </c>
       <c r="C489" s="19">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="D489" s="20">
-        <v>82.94</v>
+        <v>525.75</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -8857,13 +8866,13 @@
         <v>492</v>
       </c>
       <c r="B490" s="18">
-        <v>131.5</v>
+        <v>48.5</v>
       </c>
       <c r="C490" s="19">
-        <v>0.39</v>
+        <v>1.71</v>
       </c>
       <c r="D490" s="20">
-        <v>51.52</v>
+        <v>82.94</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -8871,13 +8880,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>96</v>
+        <v>131.5</v>
       </c>
       <c r="C491" s="19">
-        <v>2.2799999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="D491" s="20">
-        <v>218.88</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -8885,13 +8894,13 @@
         <v>494</v>
       </c>
       <c r="B492" s="18">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C492" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D492" s="20">
-        <v>104.88</v>
+        <v>202.92</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -8899,49 +8908,49 @@
         <v>495</v>
       </c>
       <c r="B493" s="18">
-        <v>27.5</v>
+        <v>46</v>
       </c>
       <c r="C493" s="19">
-        <v>2.4700000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D493" s="20">
-        <v>67.930000000000007</v>
+        <v>104.88</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A494" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="B494" s="21"/>
-      <c r="C494" s="22"/>
-      <c r="D494" s="21"/>
+      <c r="B494" s="18">
+        <v>27.5</v>
+      </c>
+      <c r="C494" s="19">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D494" s="20">
+        <v>67.930000000000007</v>
+      </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A495" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="B495" s="18">
-        <v>19.5</v>
-      </c>
-      <c r="C495" s="19">
-        <v>2.75</v>
-      </c>
-      <c r="D495" s="20">
-        <v>53.63</v>
-      </c>
+      <c r="B495" s="21"/>
+      <c r="C495" s="22"/>
+      <c r="D495" s="21"/>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A496" s="17" t="s">
         <v>498</v>
       </c>
       <c r="B496" s="18">
-        <v>86.5</v>
+        <v>19.5</v>
       </c>
       <c r="C496" s="19">
-        <v>2.73</v>
+        <v>2.75</v>
       </c>
       <c r="D496" s="20">
-        <v>236.5</v>
+        <v>53.63</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
@@ -8949,13 +8958,13 @@
         <v>499</v>
       </c>
       <c r="B497" s="18">
-        <v>12</v>
+        <v>71.5</v>
       </c>
       <c r="C497" s="19">
-        <v>2.8</v>
+        <v>2.73</v>
       </c>
       <c r="D497" s="20">
-        <v>33.6</v>
+        <v>195.49</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
@@ -8963,13 +8972,13 @@
         <v>500</v>
       </c>
       <c r="B498" s="18">
-        <v>48.5</v>
+        <v>12</v>
       </c>
       <c r="C498" s="19">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="D498" s="20">
-        <v>143.08000000000001</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
@@ -8977,13 +8986,13 @@
         <v>501</v>
       </c>
       <c r="B499" s="18">
-        <v>40</v>
+        <v>48.5</v>
       </c>
       <c r="C499" s="19">
         <v>2.95</v>
       </c>
       <c r="D499" s="20">
-        <v>118</v>
+        <v>143.08000000000001</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
@@ -8991,13 +9000,13 @@
         <v>502</v>
       </c>
       <c r="B500" s="18">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C500" s="19">
-        <v>3.5</v>
+        <v>2.95</v>
       </c>
       <c r="D500" s="20">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
@@ -9019,13 +9028,13 @@
         <v>504</v>
       </c>
       <c r="B502" s="18">
-        <v>57.5</v>
+        <v>30</v>
       </c>
       <c r="C502" s="19">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="D502" s="20">
-        <v>184</v>
+        <v>105</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
@@ -9033,49 +9042,49 @@
         <v>505</v>
       </c>
       <c r="B503" s="18">
-        <v>47</v>
+        <v>57.5</v>
       </c>
       <c r="C503" s="19">
         <v>3.2</v>
       </c>
       <c r="D503" s="20">
-        <v>150.4</v>
+        <v>184</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A504" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="B504" s="21"/>
-      <c r="C504" s="22"/>
-      <c r="D504" s="21"/>
+      <c r="B504" s="18">
+        <v>47</v>
+      </c>
+      <c r="C504" s="19">
+        <v>3.2</v>
+      </c>
+      <c r="D504" s="20">
+        <v>150.4</v>
+      </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A505" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="B505" s="18">
-        <v>46</v>
-      </c>
-      <c r="C505" s="19">
-        <v>2.85</v>
-      </c>
-      <c r="D505" s="20">
-        <v>131.1</v>
-      </c>
+      <c r="B505" s="21"/>
+      <c r="C505" s="22"/>
+      <c r="D505" s="21"/>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A506" s="17" t="s">
         <v>508</v>
       </c>
       <c r="B506" s="18">
-        <v>57.5</v>
+        <v>46</v>
       </c>
       <c r="C506" s="19">
-        <v>3.25</v>
+        <v>2.85</v>
       </c>
       <c r="D506" s="20">
-        <v>186.88</v>
+        <v>131.1</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
@@ -9083,22 +9092,28 @@
         <v>509</v>
       </c>
       <c r="B507" s="18">
-        <v>46.5</v>
+        <v>57.5</v>
       </c>
       <c r="C507" s="19">
         <v>3.25</v>
       </c>
       <c r="D507" s="20">
-        <v>151.13</v>
+        <v>186.88</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A508" s="17" t="s">
         <v>510</v>
       </c>
-      <c r="B508" s="21"/>
-      <c r="C508" s="22"/>
-      <c r="D508" s="21"/>
+      <c r="B508" s="18">
+        <v>46.5</v>
+      </c>
+      <c r="C508" s="19">
+        <v>3.25</v>
+      </c>
+      <c r="D508" s="20">
+        <v>151.13</v>
+      </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A509" s="17" t="s">
@@ -9112,28 +9127,22 @@
       <c r="A510" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="B510" s="18">
-        <v>34</v>
-      </c>
-      <c r="C510" s="19">
-        <v>3.5</v>
-      </c>
-      <c r="D510" s="20">
-        <v>119</v>
-      </c>
+      <c r="B510" s="21"/>
+      <c r="C510" s="22"/>
+      <c r="D510" s="21"/>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A511" s="17" t="s">
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C511" s="19">
         <v>3.5</v>
       </c>
       <c r="D511" s="20">
-        <v>77</v>
+        <v>108.5</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9141,49 +9150,49 @@
         <v>514</v>
       </c>
       <c r="B512" s="18">
-        <v>54.5</v>
+        <v>22</v>
       </c>
       <c r="C512" s="19">
-        <v>3.33</v>
+        <v>3.5</v>
       </c>
       <c r="D512" s="20">
-        <v>181.49</v>
+        <v>77</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A513" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="B513" s="21"/>
-      <c r="C513" s="22"/>
-      <c r="D513" s="21"/>
+      <c r="B513" s="18">
+        <v>53.5</v>
+      </c>
+      <c r="C513" s="19">
+        <v>3.33</v>
+      </c>
+      <c r="D513" s="20">
+        <v>178.16</v>
+      </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A514" s="17" t="s">
         <v>516</v>
       </c>
-      <c r="B514" s="18">
-        <v>52.5</v>
-      </c>
-      <c r="C514" s="19">
-        <v>3.8</v>
-      </c>
-      <c r="D514" s="20">
-        <v>199.5</v>
-      </c>
+      <c r="B514" s="21"/>
+      <c r="C514" s="22"/>
+      <c r="D514" s="21"/>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A515" s="17" t="s">
         <v>517</v>
       </c>
       <c r="B515" s="18">
-        <v>71.5</v>
+        <v>52.5</v>
       </c>
       <c r="C515" s="19">
-        <v>3.71</v>
+        <v>3.8</v>
       </c>
       <c r="D515" s="20">
-        <v>265.52</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
@@ -9191,71 +9200,71 @@
         <v>518</v>
       </c>
       <c r="B516" s="18">
-        <v>50.5</v>
+        <v>71.5</v>
       </c>
       <c r="C516" s="19">
-        <v>3.6</v>
+        <v>3.71</v>
       </c>
       <c r="D516" s="20">
-        <v>181.8</v>
+        <v>265.52</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A517" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="B517" s="21"/>
-      <c r="C517" s="22"/>
-      <c r="D517" s="21"/>
+      <c r="B517" s="18">
+        <v>48</v>
+      </c>
+      <c r="C517" s="19">
+        <v>3.6</v>
+      </c>
+      <c r="D517" s="20">
+        <v>172.8</v>
+      </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A518" s="17" t="s">
         <v>520</v>
       </c>
-      <c r="B518" s="18">
-        <v>76.5</v>
-      </c>
-      <c r="C518" s="19">
-        <v>3.6</v>
-      </c>
-      <c r="D518" s="20">
-        <v>275.39999999999998</v>
-      </c>
+      <c r="B518" s="21"/>
+      <c r="C518" s="22"/>
+      <c r="D518" s="21"/>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A519" s="17" t="s">
         <v>521</v>
       </c>
-      <c r="B519" s="21"/>
-      <c r="C519" s="22"/>
-      <c r="D519" s="21"/>
+      <c r="B519" s="18">
+        <v>76.5</v>
+      </c>
+      <c r="C519" s="19">
+        <v>3.6</v>
+      </c>
+      <c r="D519" s="20">
+        <v>275.39999999999998</v>
+      </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A520" s="17" t="s">
         <v>522</v>
       </c>
-      <c r="B520" s="18">
-        <v>22.5</v>
-      </c>
-      <c r="C520" s="19">
-        <v>4</v>
-      </c>
-      <c r="D520" s="20">
-        <v>90</v>
-      </c>
+      <c r="B520" s="21"/>
+      <c r="C520" s="22"/>
+      <c r="D520" s="21"/>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A521" s="17" t="s">
         <v>523</v>
       </c>
       <c r="B521" s="18">
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="C521" s="19">
         <v>4</v>
       </c>
       <c r="D521" s="20">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
@@ -9263,13 +9272,13 @@
         <v>524</v>
       </c>
       <c r="B522" s="18">
-        <v>44.5</v>
+        <v>22</v>
       </c>
       <c r="C522" s="19">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="D522" s="20">
-        <v>171.33</v>
+        <v>88</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
@@ -9277,13 +9286,13 @@
         <v>525</v>
       </c>
       <c r="B523" s="18">
-        <v>29</v>
+        <v>41.5</v>
       </c>
       <c r="C523" s="19">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="D523" s="20">
-        <v>116</v>
+        <v>159.78</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
@@ -9291,13 +9300,13 @@
         <v>526</v>
       </c>
       <c r="B524" s="18">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C524" s="19">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="D524" s="20">
-        <v>152</v>
+        <v>72</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
@@ -9305,13 +9314,13 @@
         <v>527</v>
       </c>
       <c r="B525" s="18">
-        <v>36.5</v>
+        <v>40</v>
       </c>
       <c r="C525" s="19">
         <v>3.8</v>
       </c>
       <c r="D525" s="20">
-        <v>138.69999999999999</v>
+        <v>152</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
@@ -9319,13 +9328,13 @@
         <v>528</v>
       </c>
       <c r="B526" s="18">
-        <v>43</v>
+        <v>36.5</v>
       </c>
       <c r="C526" s="19">
-        <v>4.3099999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="D526" s="20">
-        <v>185.33</v>
+        <v>138.69999999999999</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
@@ -9333,13 +9342,13 @@
         <v>529</v>
       </c>
       <c r="B527" s="18">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C527" s="19">
-        <v>4.4000000000000004</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="D527" s="20">
-        <v>114.4</v>
+        <v>185.33</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
@@ -9347,13 +9356,13 @@
         <v>530</v>
       </c>
       <c r="B528" s="18">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C528" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D528" s="20">
-        <v>66</v>
+        <v>114.4</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
@@ -9361,13 +9370,13 @@
         <v>531</v>
       </c>
       <c r="B529" s="18">
-        <v>16</v>
+        <v>13.5</v>
       </c>
       <c r="C529" s="19">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D529" s="20">
-        <v>80</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
@@ -9375,13 +9384,13 @@
         <v>532</v>
       </c>
       <c r="B530" s="18">
-        <v>10.5</v>
+        <v>16</v>
       </c>
       <c r="C530" s="19">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="D530" s="20">
-        <v>49.88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
@@ -9389,13 +9398,13 @@
         <v>533</v>
       </c>
       <c r="B531" s="18">
-        <v>28</v>
+        <v>10.5</v>
       </c>
       <c r="C531" s="19">
         <v>4.75</v>
       </c>
       <c r="D531" s="20">
-        <v>133</v>
+        <v>49.88</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
@@ -9403,13 +9412,13 @@
         <v>534</v>
       </c>
       <c r="B532" s="18">
-        <v>35.5</v>
+        <v>28</v>
       </c>
       <c r="C532" s="19">
         <v>4.75</v>
       </c>
       <c r="D532" s="20">
-        <v>168.63</v>
+        <v>133</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
@@ -9417,13 +9426,13 @@
         <v>535</v>
       </c>
       <c r="B533" s="18">
-        <v>25.5</v>
+        <v>35.5</v>
       </c>
       <c r="C533" s="19">
         <v>4.75</v>
       </c>
       <c r="D533" s="20">
-        <v>121.13</v>
+        <v>168.63</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
@@ -9431,13 +9440,13 @@
         <v>536</v>
       </c>
       <c r="B534" s="18">
-        <v>3.5</v>
+        <v>25</v>
       </c>
       <c r="C534" s="19">
         <v>4.75</v>
       </c>
       <c r="D534" s="20">
-        <v>16.63</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
@@ -9445,13 +9454,13 @@
         <v>537</v>
       </c>
       <c r="B535" s="18">
-        <v>25</v>
+        <v>3.5</v>
       </c>
       <c r="C535" s="19">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="D535" s="20">
-        <v>125</v>
+        <v>16.63</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
@@ -9459,13 +9468,13 @@
         <v>538</v>
       </c>
       <c r="B536" s="18">
-        <v>32.5</v>
+        <v>19</v>
       </c>
       <c r="C536" s="19">
         <v>5</v>
       </c>
       <c r="D536" s="20">
-        <v>162.5</v>
+        <v>95</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
@@ -9473,13 +9482,13 @@
         <v>539</v>
       </c>
       <c r="B537" s="18">
-        <v>18</v>
+        <v>29.5</v>
       </c>
       <c r="C537" s="19">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="D537" s="20">
-        <v>94.5</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
@@ -9487,13 +9496,13 @@
         <v>540</v>
       </c>
       <c r="B538" s="18">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C538" s="19">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="D538" s="20">
-        <v>175</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
@@ -9501,13 +9510,13 @@
         <v>541</v>
       </c>
       <c r="B539" s="18">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C539" s="19">
-        <v>5.41</v>
+        <v>5</v>
       </c>
       <c r="D539" s="20">
-        <v>129.78</v>
+        <v>175</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
@@ -9515,13 +9524,13 @@
         <v>542</v>
       </c>
       <c r="B540" s="18">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C540" s="19">
-        <v>5.5</v>
+        <v>5.41</v>
       </c>
       <c r="D540" s="20">
-        <v>71.5</v>
+        <v>129.78</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
@@ -9529,13 +9538,13 @@
         <v>543</v>
       </c>
       <c r="B541" s="18">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C541" s="19">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c r="D541" s="20">
-        <v>161</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
@@ -9543,13 +9552,13 @@
         <v>544</v>
       </c>
       <c r="B542" s="18">
-        <v>20.5</v>
+        <v>28</v>
       </c>
       <c r="C542" s="19">
         <v>5.75</v>
       </c>
       <c r="D542" s="20">
-        <v>117.88</v>
+        <v>161</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
@@ -9557,13 +9566,13 @@
         <v>545</v>
       </c>
       <c r="B543" s="18">
-        <v>53</v>
+        <v>20.5</v>
       </c>
       <c r="C543" s="19">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="D543" s="20">
-        <v>291.5</v>
+        <v>117.88</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
@@ -9571,13 +9580,13 @@
         <v>546</v>
       </c>
       <c r="B544" s="18">
-        <v>27.5</v>
+        <v>53</v>
       </c>
       <c r="C544" s="19">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c r="D544" s="20">
-        <v>158.13</v>
+        <v>291.5</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
@@ -9585,13 +9594,13 @@
         <v>547</v>
       </c>
       <c r="B545" s="18">
-        <v>32.5</v>
+        <v>27.5</v>
       </c>
       <c r="C545" s="19">
         <v>5.75</v>
       </c>
       <c r="D545" s="20">
-        <v>186.88</v>
+        <v>158.13</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
@@ -9599,13 +9608,13 @@
         <v>548</v>
       </c>
       <c r="B546" s="18">
-        <v>23</v>
+        <v>32.5</v>
       </c>
       <c r="C546" s="19">
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="D546" s="20">
-        <v>138</v>
+        <v>186.88</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
@@ -9613,13 +9622,13 @@
         <v>549</v>
       </c>
       <c r="B547" s="18">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C547" s="19">
         <v>6</v>
       </c>
       <c r="D547" s="20">
-        <v>18</v>
+        <v>138</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
@@ -9627,13 +9636,13 @@
         <v>550</v>
       </c>
       <c r="B548" s="18">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C548" s="19">
         <v>6</v>
       </c>
       <c r="D548" s="20">
-        <v>204</v>
+        <v>78</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
@@ -9641,49 +9650,49 @@
         <v>551</v>
       </c>
       <c r="B549" s="18">
-        <v>13.5</v>
+        <v>34</v>
       </c>
       <c r="C549" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D549" s="20">
-        <v>94.5</v>
+        <v>204</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A550" s="17" t="s">
         <v>552</v>
       </c>
-      <c r="B550" s="21"/>
-      <c r="C550" s="22"/>
-      <c r="D550" s="21"/>
+      <c r="B550" s="18">
+        <v>13.5</v>
+      </c>
+      <c r="C550" s="19">
+        <v>7</v>
+      </c>
+      <c r="D550" s="20">
+        <v>94.5</v>
+      </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A551" s="17" t="s">
         <v>553</v>
       </c>
-      <c r="B551" s="18">
-        <v>34</v>
-      </c>
-      <c r="C551" s="19">
-        <v>7</v>
-      </c>
-      <c r="D551" s="20">
-        <v>238</v>
-      </c>
+      <c r="B551" s="21"/>
+      <c r="C551" s="22"/>
+      <c r="D551" s="21"/>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A552" s="17" t="s">
         <v>554</v>
       </c>
       <c r="B552" s="18">
-        <v>17.5</v>
+        <v>34</v>
       </c>
       <c r="C552" s="19">
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="D552" s="20">
-        <v>126.88</v>
+        <v>238</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
@@ -9691,13 +9700,13 @@
         <v>555</v>
       </c>
       <c r="B553" s="18">
-        <v>24.5</v>
+        <v>17.5</v>
       </c>
       <c r="C553" s="19">
-        <v>7.75</v>
+        <v>7.25</v>
       </c>
       <c r="D553" s="20">
-        <v>189.88</v>
+        <v>126.88</v>
       </c>
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.25">
@@ -9705,13 +9714,13 @@
         <v>556</v>
       </c>
       <c r="B554" s="18">
-        <v>11.5</v>
+        <v>24.5</v>
       </c>
       <c r="C554" s="19">
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="D554" s="20">
-        <v>92</v>
+        <v>189.88</v>
       </c>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.25">
@@ -9719,13 +9728,13 @@
         <v>557</v>
       </c>
       <c r="B555" s="18">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="C555" s="19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D555" s="20">
-        <v>130</v>
+        <v>92</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
@@ -9733,49 +9742,49 @@
         <v>558</v>
       </c>
       <c r="B556" s="18">
-        <v>16.5</v>
+        <v>12</v>
       </c>
       <c r="C556" s="19">
-        <v>8.75</v>
+        <v>10</v>
       </c>
       <c r="D556" s="20">
-        <v>144.38</v>
+        <v>120</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A557" s="17" t="s">
         <v>559</v>
       </c>
-      <c r="B557" s="21"/>
-      <c r="C557" s="22"/>
-      <c r="D557" s="21"/>
+      <c r="B557" s="18">
+        <v>16.5</v>
+      </c>
+      <c r="C557" s="19">
+        <v>8.75</v>
+      </c>
+      <c r="D557" s="20">
+        <v>144.38</v>
+      </c>
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A558" s="17" t="s">
         <v>560</v>
       </c>
-      <c r="B558" s="18">
-        <v>16.5</v>
-      </c>
-      <c r="C558" s="19">
-        <v>11</v>
-      </c>
-      <c r="D558" s="20">
-        <v>181.5</v>
-      </c>
+      <c r="B558" s="21"/>
+      <c r="C558" s="22"/>
+      <c r="D558" s="21"/>
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A559" s="17" t="s">
         <v>561</v>
       </c>
       <c r="B559" s="18">
-        <v>71</v>
+        <v>16.5</v>
       </c>
       <c r="C559" s="19">
-        <v>2.76</v>
+        <v>11</v>
       </c>
       <c r="D559" s="20">
-        <v>195.96</v>
+        <v>181.5</v>
       </c>
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
@@ -9783,13 +9792,13 @@
         <v>562</v>
       </c>
       <c r="B560" s="18">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C560" s="19">
         <v>2.76</v>
       </c>
       <c r="D560" s="20">
-        <v>204.24</v>
+        <v>195.96</v>
       </c>
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
@@ -9797,13 +9806,13 @@
         <v>563</v>
       </c>
       <c r="B561" s="18">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C561" s="19">
         <v>2.76</v>
       </c>
       <c r="D561" s="20">
-        <v>287.04000000000002</v>
+        <v>204.24</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
@@ -9811,13 +9820,13 @@
         <v>564</v>
       </c>
       <c r="B562" s="18">
-        <v>34</v>
+        <v>104</v>
       </c>
       <c r="C562" s="19">
-        <v>2.8</v>
+        <v>2.76</v>
       </c>
       <c r="D562" s="20">
-        <v>95.2</v>
+        <v>287.04000000000002</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
@@ -9825,13 +9834,13 @@
         <v>565</v>
       </c>
       <c r="B563" s="18">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C563" s="19">
-        <v>2.87</v>
+        <v>2.8</v>
       </c>
       <c r="D563" s="20">
-        <v>152.22</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
@@ -9839,13 +9848,13 @@
         <v>566</v>
       </c>
       <c r="B564" s="18">
-        <v>40.5</v>
+        <v>53</v>
       </c>
       <c r="C564" s="19">
-        <v>2.76</v>
+        <v>2.87</v>
       </c>
       <c r="D564" s="20">
-        <v>111.78</v>
+        <v>152.22</v>
       </c>
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.25">
@@ -9853,13 +9862,13 @@
         <v>567</v>
       </c>
       <c r="B565" s="18">
-        <v>21</v>
+        <v>40.5</v>
       </c>
       <c r="C565" s="19">
         <v>2.76</v>
       </c>
       <c r="D565" s="20">
-        <v>57.96</v>
+        <v>111.78</v>
       </c>
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
@@ -9867,13 +9876,13 @@
         <v>568</v>
       </c>
       <c r="B566" s="18">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C566" s="19">
         <v>2.76</v>
       </c>
       <c r="D566" s="20">
-        <v>121.44</v>
+        <v>57.96</v>
       </c>
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.25">
@@ -9881,13 +9890,13 @@
         <v>569</v>
       </c>
       <c r="B567" s="18">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C567" s="19">
-        <v>3.5</v>
+        <v>2.76</v>
       </c>
       <c r="D567" s="20">
-        <v>105</v>
+        <v>121.44</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.25">
@@ -9895,13 +9904,13 @@
         <v>570</v>
       </c>
       <c r="B568" s="18">
-        <v>42.5</v>
+        <v>30</v>
       </c>
       <c r="C568" s="19">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D568" s="20">
-        <v>127.5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="569" spans="1:4" x14ac:dyDescent="0.25">
@@ -9909,13 +9918,13 @@
         <v>571</v>
       </c>
       <c r="B569" s="18">
-        <v>70</v>
+        <v>41.5</v>
       </c>
       <c r="C569" s="19">
         <v>3</v>
       </c>
       <c r="D569" s="20">
-        <v>210</v>
+        <v>124.5</v>
       </c>
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
@@ -9923,13 +9932,13 @@
         <v>572</v>
       </c>
       <c r="B570" s="18">
-        <v>38.5</v>
+        <v>70</v>
       </c>
       <c r="C570" s="19">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D570" s="20">
-        <v>119.35</v>
+        <v>210</v>
       </c>
     </row>
     <row r="571" spans="1:4" x14ac:dyDescent="0.25">
@@ -9937,13 +9946,13 @@
         <v>573</v>
       </c>
       <c r="B571" s="18">
-        <v>7</v>
+        <v>38.5</v>
       </c>
       <c r="C571" s="19">
-        <v>6</v>
+        <v>3.1</v>
       </c>
       <c r="D571" s="20">
-        <v>42</v>
+        <v>119.35</v>
       </c>
     </row>
     <row r="572" spans="1:4" x14ac:dyDescent="0.25">
@@ -9951,13 +9960,13 @@
         <v>574</v>
       </c>
       <c r="B572" s="18">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C572" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D572" s="20">
-        <v>148</v>
+        <v>42</v>
       </c>
     </row>
     <row r="573" spans="1:4" x14ac:dyDescent="0.25">
@@ -9965,13 +9974,13 @@
         <v>575</v>
       </c>
       <c r="B573" s="18">
-        <v>25.5</v>
+        <v>37</v>
       </c>
       <c r="C573" s="19">
         <v>4</v>
       </c>
       <c r="D573" s="20">
-        <v>102</v>
+        <v>148</v>
       </c>
     </row>
     <row r="574" spans="1:4" x14ac:dyDescent="0.25">
@@ -9979,13 +9988,13 @@
         <v>576</v>
       </c>
       <c r="B574" s="18">
-        <v>24</v>
+        <v>25.5</v>
       </c>
       <c r="C574" s="19">
         <v>4</v>
       </c>
       <c r="D574" s="20">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.25">
@@ -9993,13 +10002,13 @@
         <v>577</v>
       </c>
       <c r="B575" s="18">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C575" s="19">
         <v>4</v>
       </c>
       <c r="D575" s="20">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.25">
@@ -10007,13 +10016,13 @@
         <v>578</v>
       </c>
       <c r="B576" s="18">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C576" s="19">
-        <v>5.25</v>
+        <v>4</v>
       </c>
       <c r="D576" s="20">
-        <v>246.75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.25">
@@ -10021,13 +10030,13 @@
         <v>579</v>
       </c>
       <c r="B577" s="18">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C577" s="19">
-        <v>5.01</v>
+        <v>5.25</v>
       </c>
       <c r="D577" s="20">
-        <v>125.37</v>
+        <v>246.75</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.25">
@@ -10035,13 +10044,13 @@
         <v>580</v>
       </c>
       <c r="B578" s="18">
-        <v>251</v>
+        <v>25</v>
       </c>
       <c r="C578" s="19">
-        <v>1.92</v>
+        <v>5.01</v>
       </c>
       <c r="D578" s="20">
-        <v>482.04</v>
+        <v>125.37</v>
       </c>
     </row>
     <row r="579" spans="1:4" x14ac:dyDescent="0.25">
@@ -10049,13 +10058,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>-1.5</v>
+        <v>247.5</v>
       </c>
       <c r="C579" s="19">
-        <v>1.96</v>
+        <v>1.92</v>
       </c>
       <c r="D579" s="20">
-        <v>-2.94</v>
+        <v>475.32</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10063,13 +10072,13 @@
         <v>582</v>
       </c>
       <c r="B580" s="18">
-        <v>249</v>
+        <v>-1.5</v>
       </c>
       <c r="C580" s="19">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="D580" s="20">
-        <v>480.48</v>
+        <v>-2.94</v>
       </c>
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
@@ -10077,13 +10086,13 @@
         <v>583</v>
       </c>
       <c r="B581" s="18">
-        <v>108.5</v>
+        <v>249</v>
       </c>
       <c r="C581" s="19">
-        <v>2.84</v>
+        <v>1.93</v>
       </c>
       <c r="D581" s="20">
-        <v>307.91000000000003</v>
+        <v>480.48</v>
       </c>
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.25">
@@ -10091,13 +10100,13 @@
         <v>584</v>
       </c>
       <c r="B582" s="18">
-        <v>5</v>
+        <v>108.5</v>
       </c>
       <c r="C582" s="19">
-        <v>4.28</v>
+        <v>2.84</v>
       </c>
       <c r="D582" s="20">
-        <v>21.4</v>
+        <v>307.91000000000003</v>
       </c>
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.25">
@@ -10105,13 +10114,13 @@
         <v>585</v>
       </c>
       <c r="B583" s="18">
-        <v>34.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C583" s="19">
         <v>4.28</v>
       </c>
       <c r="D583" s="20">
-        <v>147.66</v>
+        <v>-6.42</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
@@ -10119,13 +10128,13 @@
         <v>586</v>
       </c>
       <c r="B584" s="18">
-        <v>56.5</v>
+        <v>34.5</v>
       </c>
       <c r="C584" s="19">
-        <v>4.05</v>
+        <v>4.28</v>
       </c>
       <c r="D584" s="20">
-        <v>228.83</v>
+        <v>147.66</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
@@ -10133,13 +10142,13 @@
         <v>587</v>
       </c>
       <c r="B585" s="18">
-        <v>71</v>
+        <v>56.5</v>
       </c>
       <c r="C585" s="19">
         <v>4.05</v>
       </c>
       <c r="D585" s="20">
-        <v>287.55</v>
+        <v>228.83</v>
       </c>
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
@@ -10147,13 +10156,13 @@
         <v>588</v>
       </c>
       <c r="B586" s="18">
-        <v>136</v>
+        <v>69</v>
       </c>
       <c r="C586" s="19">
-        <v>1.39</v>
+        <v>4.05</v>
       </c>
       <c r="D586" s="20">
-        <v>189.32</v>
+        <v>279.45</v>
       </c>
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.25">
@@ -10161,13 +10170,13 @@
         <v>589</v>
       </c>
       <c r="B587" s="18">
-        <v>373.5</v>
+        <v>133</v>
       </c>
       <c r="C587" s="19">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="D587" s="20">
-        <v>522.9</v>
+        <v>185.15</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
@@ -10175,13 +10184,13 @@
         <v>590</v>
       </c>
       <c r="B588" s="18">
-        <v>98.5</v>
+        <v>367.5</v>
       </c>
       <c r="C588" s="19">
         <v>1.4</v>
       </c>
       <c r="D588" s="20">
-        <v>137.9</v>
+        <v>514.5</v>
       </c>
     </row>
     <row r="589" spans="1:4" x14ac:dyDescent="0.25">
@@ -10189,17 +10198,21 @@
         <v>591</v>
       </c>
       <c r="B589" s="18">
-        <v>90</v>
-      </c>
-      <c r="C589" s="22"/>
-      <c r="D589" s="21"/>
+        <v>98.5</v>
+      </c>
+      <c r="C589" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="D589" s="20">
+        <v>137.9</v>
+      </c>
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A590" s="17" t="s">
         <v>592</v>
       </c>
       <c r="B590" s="18">
-        <v>29.5</v>
+        <v>90</v>
       </c>
       <c r="C590" s="22"/>
       <c r="D590" s="21"/>
@@ -10209,7 +10222,7 @@
         <v>593</v>
       </c>
       <c r="B591" s="18">
-        <v>47.5</v>
+        <v>29.5</v>
       </c>
       <c r="C591" s="22"/>
       <c r="D591" s="21"/>
@@ -10219,7 +10232,7 @@
         <v>594</v>
       </c>
       <c r="B592" s="18">
-        <v>10</v>
+        <v>45.5</v>
       </c>
       <c r="C592" s="22"/>
       <c r="D592" s="21"/>
@@ -10229,27 +10242,23 @@
         <v>595</v>
       </c>
       <c r="B593" s="18">
-        <v>516.5</v>
-      </c>
-      <c r="C593" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="D593" s="20">
-        <v>413.2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C593" s="22"/>
+      <c r="D593" s="21"/>
     </row>
     <row r="594" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A594" s="17" t="s">
         <v>596</v>
       </c>
       <c r="B594" s="18">
-        <v>628.5</v>
+        <v>2016.5</v>
       </c>
       <c r="C594" s="19">
         <v>0.8</v>
       </c>
       <c r="D594" s="20">
-        <v>502.8</v>
+        <v>1613.2</v>
       </c>
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.25">
@@ -10257,13 +10266,13 @@
         <v>597</v>
       </c>
       <c r="B595" s="18">
-        <v>731</v>
+        <v>628.5</v>
       </c>
       <c r="C595" s="19">
         <v>0.8</v>
       </c>
       <c r="D595" s="20">
-        <v>584.79999999999995</v>
+        <v>502.8</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
@@ -10271,13 +10280,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>479.5</v>
+        <v>731</v>
       </c>
       <c r="C596" s="19">
         <v>0.8</v>
       </c>
       <c r="D596" s="20">
-        <v>383.6</v>
+        <v>584.79999999999995</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10285,13 +10294,13 @@
         <v>599</v>
       </c>
       <c r="B597" s="18">
-        <v>179.5</v>
+        <v>479.5</v>
       </c>
       <c r="C597" s="19">
-        <v>0.52</v>
+        <v>0.8</v>
       </c>
       <c r="D597" s="20">
-        <v>93.34</v>
+        <v>383.6</v>
       </c>
     </row>
     <row r="598" spans="1:4" x14ac:dyDescent="0.25">
@@ -10299,13 +10308,13 @@
         <v>600</v>
       </c>
       <c r="B598" s="18">
-        <v>331</v>
+        <v>179.5</v>
       </c>
       <c r="C598" s="19">
         <v>0.52</v>
       </c>
       <c r="D598" s="20">
-        <v>172.12</v>
+        <v>93.34</v>
       </c>
     </row>
     <row r="599" spans="1:4" x14ac:dyDescent="0.25">
@@ -10313,13 +10322,13 @@
         <v>601</v>
       </c>
       <c r="B599" s="18">
-        <v>853.5</v>
+        <v>311</v>
       </c>
       <c r="C599" s="19">
         <v>0.52</v>
       </c>
       <c r="D599" s="20">
-        <v>443.82</v>
+        <v>161.72</v>
       </c>
     </row>
     <row r="600" spans="1:4" x14ac:dyDescent="0.25">
@@ -10327,13 +10336,13 @@
         <v>602</v>
       </c>
       <c r="B600" s="18">
-        <v>663</v>
+        <v>840</v>
       </c>
       <c r="C600" s="19">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="D600" s="20">
-        <v>464.1</v>
+        <v>436.8</v>
       </c>
     </row>
     <row r="601" spans="1:4" x14ac:dyDescent="0.25">
@@ -10341,13 +10350,13 @@
         <v>603</v>
       </c>
       <c r="B601" s="18">
-        <v>-2</v>
+        <v>658.5</v>
       </c>
       <c r="C601" s="19">
         <v>0.7</v>
       </c>
       <c r="D601" s="20">
-        <v>-1.4</v>
+        <v>460.95</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.25">
@@ -10355,13 +10364,13 @@
         <v>604</v>
       </c>
       <c r="B602" s="18">
-        <v>465.5</v>
+        <v>-2</v>
       </c>
       <c r="C602" s="19">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="D602" s="20">
-        <v>317.48</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="603" spans="1:4" x14ac:dyDescent="0.25">
@@ -10369,13 +10378,13 @@
         <v>605</v>
       </c>
       <c r="B603" s="18">
-        <v>11</v>
+        <v>445.5</v>
       </c>
       <c r="C603" s="19">
-        <v>4.5</v>
+        <v>0.68</v>
       </c>
       <c r="D603" s="20">
-        <v>49.5</v>
+        <v>303.83999999999997</v>
       </c>
     </row>
     <row r="604" spans="1:4" x14ac:dyDescent="0.25">
@@ -10383,25 +10392,67 @@
         <v>606</v>
       </c>
       <c r="B604" s="18">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C604" s="19">
         <v>4.5</v>
       </c>
       <c r="D604" s="20">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="605" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A605" s="17" t="s">
+        <v>607</v>
+      </c>
+      <c r="B605" s="18">
+        <v>41</v>
+      </c>
+      <c r="C605" s="19">
+        <v>4.5</v>
+      </c>
+      <c r="D605" s="20">
         <v>184.5</v>
       </c>
     </row>
-    <row r="605" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A605" s="23" t="s">
-        <v>607</v>
-      </c>
-      <c r="B605" s="24">
-        <v>36510.67</v>
-      </c>
-      <c r="C605" s="25"/>
-      <c r="D605" s="26">
-        <v>106182.08</v>
+    <row r="606" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A606" s="17" t="s">
+        <v>608</v>
+      </c>
+      <c r="B606" s="18">
+        <v>7</v>
+      </c>
+      <c r="C606" s="19">
+        <v>3</v>
+      </c>
+      <c r="D606" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="607" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A607" s="17" t="s">
+        <v>609</v>
+      </c>
+      <c r="B607" s="18">
+        <v>3</v>
+      </c>
+      <c r="C607" s="19">
+        <v>3</v>
+      </c>
+      <c r="D607" s="20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A608" s="23" t="s">
+        <v>610</v>
+      </c>
+      <c r="B608" s="24">
+        <v>40644.17</v>
+      </c>
+      <c r="C608" s="25"/>
+      <c r="D608" s="26">
+        <v>109634.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 2:27
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 20-Dec-2024</t>
+    <t>1-Jul-2024 to 21-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -2472,13 +2472,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C11" s="19">
         <v>0.92</v>
       </c>
       <c r="D11" s="20">
-        <v>192.33</v>
+        <v>186.81</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2556,13 +2556,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="18">
-        <v>121.5</v>
+        <v>106.5</v>
       </c>
       <c r="C17" s="19">
         <v>2</v>
       </c>
       <c r="D17" s="20">
-        <v>243</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2640,13 +2640,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="18">
-        <v>119.5</v>
+        <v>118.5</v>
       </c>
       <c r="C23" s="19">
         <v>2</v>
       </c>
       <c r="D23" s="20">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2654,13 +2654,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18">
-        <v>60.5</v>
+        <v>56.5</v>
       </c>
       <c r="C24" s="19">
         <v>2.1</v>
       </c>
       <c r="D24" s="20">
-        <v>127.05</v>
+        <v>118.65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,13 +2704,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="18">
-        <v>64.37</v>
+        <v>60.37</v>
       </c>
       <c r="C28" s="19">
         <v>2.35</v>
       </c>
       <c r="D28" s="20">
-        <v>151.27000000000001</v>
+        <v>141.87</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2834,13 +2834,13 @@
         <v>41</v>
       </c>
       <c r="B39" s="18">
-        <v>108.5</v>
+        <v>105.5</v>
       </c>
       <c r="C39" s="19">
         <v>2.7</v>
       </c>
       <c r="D39" s="20">
-        <v>292.95</v>
+        <v>284.85000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2946,13 +2946,13 @@
         <v>49</v>
       </c>
       <c r="B47" s="18">
-        <v>298</v>
+        <v>218</v>
       </c>
       <c r="C47" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D47" s="20">
-        <v>327.8</v>
+        <v>239.8</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3002,13 +3002,13 @@
         <v>53</v>
       </c>
       <c r="B51" s="18">
-        <v>294</v>
+        <v>174</v>
       </c>
       <c r="C51" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D51" s="20">
-        <v>323.39999999999998</v>
+        <v>191.4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3016,13 +3016,13 @@
         <v>54</v>
       </c>
       <c r="B52" s="18">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C52" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D52" s="20">
-        <v>503.8</v>
+        <v>498.3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3058,13 +3058,13 @@
         <v>57</v>
       </c>
       <c r="B55" s="18">
-        <v>306</v>
+        <v>226</v>
       </c>
       <c r="C55" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D55" s="20">
-        <v>336.6</v>
+        <v>248.6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,13 +3142,13 @@
         <v>63</v>
       </c>
       <c r="B61" s="18">
-        <v>35.5</v>
+        <v>33.5</v>
       </c>
       <c r="C61" s="19">
         <v>2.1</v>
       </c>
       <c r="D61" s="20">
-        <v>74.55</v>
+        <v>70.349999999999994</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3268,13 +3268,13 @@
         <v>72</v>
       </c>
       <c r="B70" s="18">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C70" s="19">
         <v>0.9</v>
       </c>
       <c r="D70" s="20">
-        <v>87.3</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3388,7 +3388,7 @@
         <v>82</v>
       </c>
       <c r="B80" s="18">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
@@ -3398,13 +3398,13 @@
         <v>83</v>
       </c>
       <c r="B81" s="18">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C81" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D81" s="20">
-        <v>647.45000000000005</v>
+        <v>644</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3426,13 +3426,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>686.5</v>
+        <v>675.5</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>961.1</v>
+        <v>945.7</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3518,13 +3518,13 @@
         <v>92</v>
       </c>
       <c r="B90" s="18">
-        <v>506.5</v>
+        <v>505.5</v>
       </c>
       <c r="C90" s="19">
         <v>1.26</v>
       </c>
       <c r="D90" s="20">
-        <v>638.19000000000005</v>
+        <v>636.92999999999995</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,13 +3752,13 @@
         <v>110</v>
       </c>
       <c r="B108" s="18">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="C108" s="19">
         <v>12.5</v>
       </c>
       <c r="D108" s="20">
-        <v>281.25</v>
+        <v>268.75</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4214,13 +4214,13 @@
         <v>143</v>
       </c>
       <c r="B141" s="18">
-        <v>48</v>
+        <v>45.5</v>
       </c>
       <c r="C141" s="19">
         <v>2.8</v>
       </c>
       <c r="D141" s="20">
-        <v>134.4</v>
+        <v>127.4</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5014,13 +5014,13 @@
         <v>204</v>
       </c>
       <c r="B202" s="18">
-        <v>28.5</v>
+        <v>27</v>
       </c>
       <c r="C202" s="19">
         <v>4.12</v>
       </c>
       <c r="D202" s="20">
-        <v>117.31</v>
+        <v>111.13</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5120,13 +5120,13 @@
         <v>212</v>
       </c>
       <c r="B210" s="18">
-        <v>277.5</v>
+        <v>275.5</v>
       </c>
       <c r="C210" s="19">
         <v>4.5</v>
       </c>
       <c r="D210" s="20">
-        <v>1248.75</v>
+        <v>1239.75</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5134,13 +5134,13 @@
         <v>213</v>
       </c>
       <c r="B211" s="18">
-        <v>133.5</v>
+        <v>128.5</v>
       </c>
       <c r="C211" s="19">
         <v>4.5</v>
       </c>
       <c r="D211" s="20">
-        <v>600.75</v>
+        <v>578.25</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5904,13 +5904,13 @@
         <v>271</v>
       </c>
       <c r="B269" s="18">
-        <v>72.5</v>
+        <v>70.5</v>
       </c>
       <c r="C269" s="19">
         <v>5.94</v>
       </c>
       <c r="D269" s="20">
-        <v>430.65</v>
+        <v>418.77</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -6408,13 +6408,13 @@
         <v>310</v>
       </c>
       <c r="B308" s="18">
-        <v>23.2</v>
+        <v>16.2</v>
       </c>
       <c r="C308" s="19">
         <v>8.8000000000000007</v>
       </c>
       <c r="D308" s="20">
-        <v>204.16</v>
+        <v>142.56</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -7090,13 +7090,13 @@
         <v>360</v>
       </c>
       <c r="B358" s="18">
-        <v>-6</v>
+        <v>-10</v>
       </c>
       <c r="C358" s="19">
         <v>10</v>
       </c>
       <c r="D358" s="20">
-        <v>-60</v>
+        <v>-100</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -7342,13 +7342,13 @@
         <v>378</v>
       </c>
       <c r="B376" s="18">
-        <v>31.75</v>
+        <v>25.75</v>
       </c>
       <c r="C376" s="19">
         <v>11.5</v>
       </c>
       <c r="D376" s="20">
-        <v>365.13</v>
+        <v>296.13</v>
       </c>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
@@ -7496,13 +7496,13 @@
         <v>389</v>
       </c>
       <c r="B387" s="18">
-        <v>12.5</v>
+        <v>1.5</v>
       </c>
       <c r="C387" s="19">
         <v>10.45</v>
       </c>
       <c r="D387" s="20">
-        <v>130.63</v>
+        <v>15.68</v>
       </c>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
@@ -7800,13 +7800,13 @@
         <v>412</v>
       </c>
       <c r="B410" s="18">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C410" s="19">
         <v>2.8</v>
       </c>
       <c r="D410" s="20">
-        <v>89.6</v>
+        <v>86.8</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
@@ -7836,13 +7836,13 @@
         <v>415</v>
       </c>
       <c r="B413" s="18">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C413" s="19">
         <v>2.95</v>
       </c>
       <c r="D413" s="20">
-        <v>129.80000000000001</v>
+        <v>115.05</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
@@ -8480,13 +8480,13 @@
         <v>464</v>
       </c>
       <c r="B462" s="18">
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="C462" s="19">
         <v>7.6</v>
       </c>
       <c r="D462" s="20">
-        <v>231.8</v>
+        <v>216.6</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -8558,13 +8558,13 @@
         <v>470</v>
       </c>
       <c r="B468" s="18">
-        <v>13.5</v>
+        <v>18.5</v>
       </c>
       <c r="C468" s="19">
         <v>3.75</v>
       </c>
       <c r="D468" s="20">
-        <v>50.63</v>
+        <v>69.38</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -8684,13 +8684,13 @@
         <v>479</v>
       </c>
       <c r="B477" s="18">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="C477" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D477" s="20">
-        <v>6.05</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
@@ -8894,13 +8894,13 @@
         <v>494</v>
       </c>
       <c r="B492" s="18">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C492" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D492" s="20">
-        <v>202.92</v>
+        <v>198.36</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -9300,13 +9300,13 @@
         <v>526</v>
       </c>
       <c r="B524" s="18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C524" s="19">
         <v>4</v>
       </c>
       <c r="D524" s="20">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
@@ -9468,13 +9468,13 @@
         <v>538</v>
       </c>
       <c r="B536" s="18">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C536" s="19">
         <v>5</v>
       </c>
       <c r="D536" s="20">
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
@@ -9482,13 +9482,13 @@
         <v>539</v>
       </c>
       <c r="B537" s="18">
-        <v>29.5</v>
+        <v>25.5</v>
       </c>
       <c r="C537" s="19">
         <v>5</v>
       </c>
       <c r="D537" s="20">
-        <v>147.5</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
@@ -9608,13 +9608,13 @@
         <v>548</v>
       </c>
       <c r="B546" s="18">
-        <v>32.5</v>
+        <v>28.5</v>
       </c>
       <c r="C546" s="19">
         <v>5.75</v>
       </c>
       <c r="D546" s="20">
-        <v>186.88</v>
+        <v>163.88</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
@@ -9806,13 +9806,13 @@
         <v>563</v>
       </c>
       <c r="B561" s="18">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C561" s="19">
         <v>2.76</v>
       </c>
       <c r="D561" s="20">
-        <v>204.24</v>
+        <v>190.44</v>
       </c>
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
@@ -10058,13 +10058,13 @@
         <v>581</v>
       </c>
       <c r="B579" s="18">
-        <v>247.5</v>
+        <v>246.5</v>
       </c>
       <c r="C579" s="19">
         <v>1.92</v>
       </c>
       <c r="D579" s="20">
-        <v>475.32</v>
+        <v>473.4</v>
       </c>
     </row>
     <row r="580" spans="1:4" x14ac:dyDescent="0.25">
@@ -10128,13 +10128,13 @@
         <v>586</v>
       </c>
       <c r="B584" s="18">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="C584" s="19">
         <v>4.28</v>
       </c>
       <c r="D584" s="20">
-        <v>147.66</v>
+        <v>139.1</v>
       </c>
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
@@ -10448,11 +10448,11 @@
         <v>610</v>
       </c>
       <c r="B608" s="24">
-        <v>40644.17</v>
+        <v>40225.17</v>
       </c>
       <c r="C608" s="25"/>
       <c r="D608" s="26">
-        <v>109634.31</v>
+        <v>108750.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 1:25
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 23-Dec-2024</t>
+    <t>1-Jul-2024 to 24-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -2587,13 +2587,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="18">
-        <v>118</v>
+        <v>120.5</v>
       </c>
       <c r="C19" s="19">
         <v>2</v>
       </c>
       <c r="D19" s="20">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -5053,13 +5053,13 @@
         <v>207</v>
       </c>
       <c r="B205" s="18">
-        <v>29.5</v>
+        <v>29</v>
       </c>
       <c r="C205" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D205" s="20">
-        <v>129.80000000000001</v>
+        <v>127.6</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -6659,13 +6659,13 @@
         <v>329</v>
       </c>
       <c r="B327" s="18">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="C327" s="19">
         <v>6.9</v>
       </c>
       <c r="D327" s="20">
-        <v>69</v>
+        <v>58.65</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -7707,13 +7707,13 @@
         <v>406</v>
       </c>
       <c r="B404" s="18">
-        <v>77.5</v>
+        <v>72.5</v>
       </c>
       <c r="C404" s="19">
         <v>2.7</v>
       </c>
       <c r="D404" s="20">
-        <v>209.25</v>
+        <v>195.75</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.25">
@@ -7897,13 +7897,13 @@
         <v>420</v>
       </c>
       <c r="B418" s="18">
-        <v>17.95</v>
+        <v>16.45</v>
       </c>
       <c r="C418" s="19">
         <v>3.15</v>
       </c>
       <c r="D418" s="20">
-        <v>56.54</v>
+        <v>51.82</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
@@ -10449,11 +10449,11 @@
         <v>611</v>
       </c>
       <c r="B609" s="24">
-        <v>39580.269999999997</v>
+        <v>39574.269999999997</v>
       </c>
       <c r="C609" s="25"/>
       <c r="D609" s="26">
-        <v>110126</v>
+        <v>110100.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:25
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -1793,13 +1793,13 @@
     <t>9100 CARD</t>
   </si>
   <si>
-    <t>9101 CARD (MIL JAYEGA)</t>
-  </si>
-  <si>
-    <t>9102 CARD</t>
-  </si>
-  <si>
-    <t>9103 CARD (MIL JAYEGA)</t>
+    <t>9101 CARD (YELLOW)</t>
+  </si>
+  <si>
+    <t>9102 CARD (RED)</t>
+  </si>
+  <si>
+    <t>9103 CARD (GOLDEN)</t>
   </si>
   <si>
     <t>9104 CARD</t>
@@ -2475,13 +2475,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="18">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C11" s="19">
         <v>0.92</v>
       </c>
       <c r="D11" s="20">
-        <v>182.21</v>
+        <v>174.85</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2489,13 +2489,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="18">
-        <v>58.5</v>
+        <v>218.5</v>
       </c>
       <c r="C12" s="19">
         <v>1.65</v>
       </c>
       <c r="D12" s="20">
-        <v>96.53</v>
+        <v>360.53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2629,13 +2629,13 @@
         <v>24</v>
       </c>
       <c r="B22" s="18">
-        <v>94.5</v>
+        <v>92.5</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
       </c>
       <c r="D22" s="20">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2657,13 +2657,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18">
-        <v>60.5</v>
+        <v>59</v>
       </c>
       <c r="C24" s="19">
         <v>2.1</v>
       </c>
       <c r="D24" s="20">
-        <v>127.05</v>
+        <v>123.9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2671,13 +2671,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="18">
-        <v>119.5</v>
+        <v>116</v>
       </c>
       <c r="C25" s="19">
         <v>2.1</v>
       </c>
       <c r="D25" s="20">
-        <v>250.95</v>
+        <v>243.6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2778,9 +2778,15 @@
       <c r="A34" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21"/>
+      <c r="B34" s="18">
+        <v>66</v>
+      </c>
+      <c r="C34" s="19">
+        <v>2.5</v>
+      </c>
+      <c r="D34" s="20">
+        <v>165</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
@@ -2991,13 +2997,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>441.1</v>
+        <v>434.5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3047,13 +3053,13 @@
         <v>56</v>
       </c>
       <c r="B54" s="18">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C54" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D54" s="20">
-        <v>286</v>
+        <v>281.60000000000002</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,13 +3081,13 @@
         <v>58</v>
       </c>
       <c r="B56" s="18">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="C56" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D56" s="20">
-        <v>257.39999999999998</v>
+        <v>266.2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3243,13 +3249,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="18">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C68" s="19">
         <v>0.7</v>
       </c>
       <c r="D68" s="20">
-        <v>130.9</v>
+        <v>126.7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,13 +3277,13 @@
         <v>72</v>
       </c>
       <c r="B70" s="18">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="C70" s="19">
         <v>0.9</v>
       </c>
       <c r="D70" s="20">
-        <v>76.5</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,13 +3291,13 @@
         <v>73</v>
       </c>
       <c r="B71" s="18">
-        <v>124</v>
+        <v>121.5</v>
       </c>
       <c r="C71" s="19">
         <v>0.9</v>
       </c>
       <c r="D71" s="20">
-        <v>111.6</v>
+        <v>109.35</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,13 +3305,13 @@
         <v>74</v>
       </c>
       <c r="B72" s="18">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C72" s="19">
         <v>1.55</v>
       </c>
       <c r="D72" s="20">
-        <v>595.20000000000005</v>
+        <v>579.70000000000005</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,7 +3347,7 @@
         <v>77</v>
       </c>
       <c r="B75" s="18">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C75" s="22"/>
       <c r="D75" s="21"/>
@@ -3457,13 +3463,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="18">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="C85" s="19">
         <v>1.4</v>
       </c>
       <c r="D85" s="20">
-        <v>169.4</v>
+        <v>127.4</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,13 +3671,13 @@
         <v>104</v>
       </c>
       <c r="B102" s="18">
-        <v>24.5</v>
+        <v>20</v>
       </c>
       <c r="C102" s="19">
         <v>12.5</v>
       </c>
       <c r="D102" s="20">
-        <v>306.25</v>
+        <v>250</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3679,13 +3685,13 @@
         <v>105</v>
       </c>
       <c r="B103" s="18">
-        <v>51.5</v>
+        <v>43.5</v>
       </c>
       <c r="C103" s="19">
         <v>12.5</v>
       </c>
       <c r="D103" s="20">
-        <v>643.75</v>
+        <v>543.75</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3693,13 +3699,13 @@
         <v>106</v>
       </c>
       <c r="B104" s="18">
-        <v>44.5</v>
+        <v>39.5</v>
       </c>
       <c r="C104" s="19">
         <v>12.5</v>
       </c>
       <c r="D104" s="20">
-        <v>556.25</v>
+        <v>493.75</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,13 +3783,13 @@
         <v>112</v>
       </c>
       <c r="B110" s="18">
-        <v>9.5</v>
+        <v>8</v>
       </c>
       <c r="C110" s="19">
         <v>12.5</v>
       </c>
       <c r="D110" s="20">
-        <v>118.75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3833,13 +3839,13 @@
         <v>116</v>
       </c>
       <c r="B114" s="18">
-        <v>12.5</v>
+        <v>9.5</v>
       </c>
       <c r="C114" s="19">
         <v>15.5</v>
       </c>
       <c r="D114" s="20">
-        <v>193.75</v>
+        <v>147.25</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,13 +4007,13 @@
         <v>128</v>
       </c>
       <c r="B126" s="18">
-        <v>13.5</v>
+        <v>8.5</v>
       </c>
       <c r="C126" s="19">
         <v>15.5</v>
       </c>
       <c r="D126" s="20">
-        <v>209.25</v>
+        <v>131.75</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4127,13 +4133,13 @@
         <v>137</v>
       </c>
       <c r="B135" s="18">
-        <v>3.5</v>
+        <v>13.5</v>
       </c>
       <c r="C135" s="19">
-        <v>18.420000000000002</v>
+        <v>18.440000000000001</v>
       </c>
       <c r="D135" s="20">
-        <v>64.47</v>
+        <v>248.89</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,13 +4217,13 @@
         <v>143</v>
       </c>
       <c r="B141" s="18">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C141" s="19">
         <v>2.8</v>
       </c>
       <c r="D141" s="20">
-        <v>114.8</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,13 +4245,13 @@
         <v>145</v>
       </c>
       <c r="B143" s="18">
-        <v>96.5</v>
+        <v>93.5</v>
       </c>
       <c r="C143" s="19">
         <v>2.75</v>
       </c>
       <c r="D143" s="20">
-        <v>265.38</v>
+        <v>257.13</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,13 +4301,13 @@
         <v>149</v>
       </c>
       <c r="B147" s="18">
-        <v>41.5</v>
+        <v>40.5</v>
       </c>
       <c r="C147" s="19">
         <v>2.7</v>
       </c>
       <c r="D147" s="20">
-        <v>112.05</v>
+        <v>109.35</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,13 +4315,13 @@
         <v>150</v>
       </c>
       <c r="B148" s="18">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C148" s="19">
         <v>2.8</v>
       </c>
       <c r="D148" s="20">
-        <v>268.8</v>
+        <v>249.2</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4323,13 +4329,13 @@
         <v>151</v>
       </c>
       <c r="B149" s="18">
-        <v>94.5</v>
+        <v>92.5</v>
       </c>
       <c r="C149" s="19">
         <v>2.8</v>
       </c>
       <c r="D149" s="20">
-        <v>264.60000000000002</v>
+        <v>259</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4407,13 +4413,13 @@
         <v>157</v>
       </c>
       <c r="B155" s="18">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C155" s="19">
         <v>2.95</v>
       </c>
       <c r="D155" s="20">
-        <v>233.05</v>
+        <v>227.15</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4477,13 +4483,13 @@
         <v>162</v>
       </c>
       <c r="B160" s="18">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C160" s="19">
         <v>3.5</v>
       </c>
       <c r="D160" s="20">
-        <v>189</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4583,13 +4589,13 @@
         <v>170</v>
       </c>
       <c r="B168" s="18">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C168" s="19">
         <v>3.6</v>
       </c>
       <c r="D168" s="20">
-        <v>496.8</v>
+        <v>486</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4859,13 +4865,13 @@
         <v>191</v>
       </c>
       <c r="B189" s="18">
-        <v>21.74</v>
+        <v>18.739999999999998</v>
       </c>
       <c r="C189" s="19">
         <v>3.14</v>
       </c>
       <c r="D189" s="20">
-        <v>68.260000000000005</v>
+        <v>58.84</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5131,13 +5137,13 @@
         <v>213</v>
       </c>
       <c r="B211" s="18">
-        <v>117.5</v>
+        <v>189.5</v>
       </c>
       <c r="C211" s="19">
         <v>4.5</v>
       </c>
       <c r="D211" s="20">
-        <v>528.75</v>
+        <v>852.75</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5145,13 +5151,13 @@
         <v>214</v>
       </c>
       <c r="B212" s="18">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="C212" s="19">
         <v>5.25</v>
       </c>
       <c r="D212" s="20">
-        <v>73.5</v>
+        <v>65.63</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5271,13 +5277,13 @@
         <v>223</v>
       </c>
       <c r="B221" s="18">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C221" s="19">
         <v>4.75</v>
       </c>
       <c r="D221" s="20">
-        <v>375.25</v>
+        <v>351.5</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5379,13 +5385,13 @@
         <v>232</v>
       </c>
       <c r="B230" s="18">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C230" s="19">
         <v>6.75</v>
       </c>
       <c r="D230" s="20">
-        <v>513</v>
+        <v>519.75</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5393,13 +5399,13 @@
         <v>233</v>
       </c>
       <c r="B231" s="18">
-        <v>162.5</v>
+        <v>160.5</v>
       </c>
       <c r="C231" s="19">
         <v>5.97</v>
       </c>
       <c r="D231" s="20">
-        <v>970.92</v>
+        <v>958.97</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5407,13 +5413,13 @@
         <v>234</v>
       </c>
       <c r="B232" s="18">
-        <v>47.5</v>
+        <v>44.5</v>
       </c>
       <c r="C232" s="19">
         <v>4.26</v>
       </c>
       <c r="D232" s="20">
-        <v>202.35</v>
+        <v>189.57</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -5513,13 +5519,13 @@
         <v>242</v>
       </c>
       <c r="B240" s="18">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C240" s="19">
         <v>3.5</v>
       </c>
       <c r="D240" s="20">
-        <v>129.5</v>
+        <v>213.5</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5541,13 +5547,13 @@
         <v>244</v>
       </c>
       <c r="B242" s="18">
-        <v>14.5</v>
+        <v>94.5</v>
       </c>
       <c r="C242" s="19">
         <v>4.25</v>
       </c>
       <c r="D242" s="20">
-        <v>61.63</v>
+        <v>401.63</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -5647,13 +5653,13 @@
         <v>252</v>
       </c>
       <c r="B250" s="18">
-        <v>33.5</v>
+        <v>29</v>
       </c>
       <c r="C250" s="19">
         <v>4.95</v>
       </c>
       <c r="D250" s="20">
-        <v>165.83</v>
+        <v>143.55000000000001</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -5895,13 +5901,13 @@
         <v>271</v>
       </c>
       <c r="B269" s="18">
-        <v>64.5</v>
+        <v>62.5</v>
       </c>
       <c r="C269" s="19">
         <v>5.94</v>
       </c>
       <c r="D269" s="20">
-        <v>383.13</v>
+        <v>371.25</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
@@ -5987,13 +5993,13 @@
         <v>278</v>
       </c>
       <c r="B276" s="18">
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
       <c r="C276" s="19">
         <v>6.18</v>
       </c>
       <c r="D276" s="20">
-        <v>64.89</v>
+        <v>126.69</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
@@ -6101,13 +6107,13 @@
         <v>287</v>
       </c>
       <c r="B285" s="18">
-        <v>46</v>
+        <v>44.5</v>
       </c>
       <c r="C285" s="19">
         <v>6.65</v>
       </c>
       <c r="D285" s="20">
-        <v>305.89999999999998</v>
+        <v>295.93</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -6151,13 +6157,13 @@
         <v>291</v>
       </c>
       <c r="B289" s="18">
-        <v>15.5</v>
+        <v>91</v>
       </c>
       <c r="C289" s="19">
         <v>7.13</v>
       </c>
       <c r="D289" s="20">
-        <v>110.52</v>
+        <v>648.83000000000004</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6215,13 +6221,13 @@
         <v>296</v>
       </c>
       <c r="B294" s="18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C294" s="19">
         <v>7.6</v>
       </c>
       <c r="D294" s="20">
-        <v>228</v>
+        <v>220.4</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
@@ -6371,13 +6377,13 @@
         <v>308</v>
       </c>
       <c r="B306" s="18">
-        <v>5.5</v>
+        <v>-12.5</v>
       </c>
       <c r="C306" s="19">
         <v>9.4600000000000009</v>
       </c>
       <c r="D306" s="20">
-        <v>52.02</v>
+        <v>-118.23</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.25">
@@ -6399,13 +6405,13 @@
         <v>310</v>
       </c>
       <c r="B308" s="18">
-        <v>20.7</v>
+        <v>56.7</v>
       </c>
       <c r="C308" s="19">
         <v>8.8000000000000007</v>
       </c>
       <c r="D308" s="20">
-        <v>182.16</v>
+        <v>498.96</v>
       </c>
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.25">
@@ -6483,13 +6489,13 @@
         <v>316</v>
       </c>
       <c r="B314" s="18">
-        <v>2.5</v>
+        <v>50.5</v>
       </c>
       <c r="C314" s="19">
         <v>9.25</v>
       </c>
       <c r="D314" s="20">
-        <v>23.13</v>
+        <v>467.13</v>
       </c>
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.25">
@@ -6650,9 +6656,15 @@
       <c r="A326" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="B326" s="21"/>
-      <c r="C326" s="22"/>
-      <c r="D326" s="21"/>
+      <c r="B326" s="18">
+        <v>39</v>
+      </c>
+      <c r="C326" s="19">
+        <v>7.84</v>
+      </c>
+      <c r="D326" s="20">
+        <v>305.76</v>
+      </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="17" t="s">
@@ -6695,13 +6707,13 @@
         <v>332</v>
       </c>
       <c r="B330" s="18">
-        <v>29.5</v>
+        <v>28</v>
       </c>
       <c r="C330" s="19">
         <v>6.51</v>
       </c>
       <c r="D330" s="20">
-        <v>192.06</v>
+        <v>182.29</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -6955,13 +6967,13 @@
         <v>351</v>
       </c>
       <c r="B349" s="18">
-        <v>13.99</v>
+        <v>11.49</v>
       </c>
       <c r="C349" s="19">
         <v>12</v>
       </c>
       <c r="D349" s="20">
-        <v>167.88</v>
+        <v>137.88</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -6983,13 +6995,13 @@
         <v>353</v>
       </c>
       <c r="B351" s="18">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="C351" s="19">
         <v>7.84</v>
       </c>
       <c r="D351" s="20">
-        <v>-7.84</v>
+        <v>274.39999999999998</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7053,13 +7065,13 @@
         <v>358</v>
       </c>
       <c r="B356" s="18">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="C356" s="19">
         <v>10.5</v>
       </c>
       <c r="D356" s="20">
-        <v>68.25</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -7179,13 +7191,13 @@
         <v>367</v>
       </c>
       <c r="B365" s="18">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="C365" s="19">
         <v>10</v>
       </c>
       <c r="D365" s="20">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="366" spans="1:4" x14ac:dyDescent="0.25">
@@ -7235,13 +7247,13 @@
         <v>371</v>
       </c>
       <c r="B369" s="18">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="C369" s="19">
         <v>25</v>
       </c>
       <c r="D369" s="20">
-        <v>512.5</v>
+        <v>487.5</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7501,13 +7513,13 @@
         <v>390</v>
       </c>
       <c r="B388" s="18">
-        <v>-5.5</v>
+        <v>0.25</v>
       </c>
       <c r="C388" s="19">
-        <v>10.45</v>
+        <v>10.84</v>
       </c>
       <c r="D388" s="20">
-        <v>-57.48</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
@@ -7579,13 +7591,13 @@
         <v>396</v>
       </c>
       <c r="B394" s="18">
-        <v>54.5</v>
+        <v>53.5</v>
       </c>
       <c r="C394" s="19">
         <v>2</v>
       </c>
       <c r="D394" s="20">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
@@ -7637,13 +7649,13 @@
         <v>401</v>
       </c>
       <c r="B399" s="18">
-        <v>62.5</v>
+        <v>61.5</v>
       </c>
       <c r="C399" s="19">
         <v>2.25</v>
       </c>
       <c r="D399" s="20">
-        <v>140.63</v>
+        <v>138.38</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -7679,13 +7691,13 @@
         <v>404</v>
       </c>
       <c r="B402" s="18">
-        <v>22.5</v>
+        <v>55.5</v>
       </c>
       <c r="C402" s="19">
         <v>2.5</v>
       </c>
       <c r="D402" s="20">
-        <v>56.25</v>
+        <v>138.75</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
@@ -7749,13 +7761,13 @@
         <v>409</v>
       </c>
       <c r="B407" s="18">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C407" s="19">
         <v>2.75</v>
       </c>
       <c r="D407" s="20">
-        <v>225.5</v>
+        <v>220</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.25">
@@ -7777,13 +7789,13 @@
         <v>411</v>
       </c>
       <c r="B409" s="18">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="C409" s="19">
         <v>2.8</v>
       </c>
       <c r="D409" s="20">
-        <v>77</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.25">
@@ -7791,13 +7803,13 @@
         <v>412</v>
       </c>
       <c r="B410" s="18">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C410" s="19">
         <v>2.8</v>
       </c>
       <c r="D410" s="20">
-        <v>86.8</v>
+        <v>81.2</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
@@ -7883,13 +7895,13 @@
         <v>419</v>
       </c>
       <c r="B417" s="18">
-        <v>42.5</v>
+        <v>41</v>
       </c>
       <c r="C417" s="19">
         <v>3.3</v>
       </c>
       <c r="D417" s="20">
-        <v>140.25</v>
+        <v>135.30000000000001</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -7919,13 +7931,13 @@
         <v>422</v>
       </c>
       <c r="B420" s="18">
-        <v>14.5</v>
+        <v>11.5</v>
       </c>
       <c r="C420" s="19">
         <v>3.25</v>
       </c>
       <c r="D420" s="20">
-        <v>47.13</v>
+        <v>37.380000000000003</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
@@ -8083,13 +8095,13 @@
         <v>435</v>
       </c>
       <c r="B433" s="18">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C433" s="19">
         <v>4.25</v>
       </c>
       <c r="D433" s="20">
-        <v>131.75</v>
+        <v>123.25</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -8195,13 +8207,13 @@
         <v>443</v>
       </c>
       <c r="B441" s="18">
-        <v>16.5</v>
+        <v>56.5</v>
       </c>
       <c r="C441" s="19">
         <v>4.28</v>
       </c>
       <c r="D441" s="20">
-        <v>70.62</v>
+        <v>241.82</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -8365,13 +8377,13 @@
         <v>456</v>
       </c>
       <c r="B454" s="18">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C454" s="19">
         <v>6</v>
       </c>
       <c r="D454" s="20">
-        <v>276</v>
+        <v>258</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
@@ -8387,13 +8399,13 @@
         <v>458</v>
       </c>
       <c r="B456" s="18">
-        <v>23.5</v>
+        <v>20.5</v>
       </c>
       <c r="C456" s="19">
         <v>5.94</v>
       </c>
       <c r="D456" s="20">
-        <v>139.59</v>
+        <v>121.77</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -8457,13 +8469,13 @@
         <v>463</v>
       </c>
       <c r="B461" s="18">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C461" s="19">
         <v>7</v>
       </c>
       <c r="D461" s="20">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -8471,13 +8483,13 @@
         <v>464</v>
       </c>
       <c r="B462" s="18">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="C462" s="19">
         <v>7.6</v>
       </c>
       <c r="D462" s="20">
-        <v>209</v>
+        <v>201.4</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -8577,13 +8589,13 @@
         <v>472</v>
       </c>
       <c r="B470" s="18">
-        <v>39.5</v>
+        <v>38.5</v>
       </c>
       <c r="C470" s="19">
         <v>9.5</v>
       </c>
       <c r="D470" s="20">
-        <v>375.25</v>
+        <v>365.75</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -8661,13 +8673,13 @@
         <v>478</v>
       </c>
       <c r="B476" s="18">
-        <v>15</v>
+        <v>13.5</v>
       </c>
       <c r="C476" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D476" s="20">
-        <v>16.5</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -8703,13 +8715,13 @@
         <v>481</v>
       </c>
       <c r="B479" s="18">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C479" s="19">
         <v>1.4</v>
       </c>
       <c r="D479" s="20">
-        <v>183.4</v>
+        <v>162.4</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -8829,13 +8841,13 @@
         <v>490</v>
       </c>
       <c r="B488" s="18">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C488" s="19">
         <v>1.5</v>
       </c>
       <c r="D488" s="20">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -8843,13 +8855,13 @@
         <v>491</v>
       </c>
       <c r="B489" s="18">
-        <v>350.5</v>
+        <v>347.5</v>
       </c>
       <c r="C489" s="19">
         <v>1.5</v>
       </c>
       <c r="D489" s="20">
-        <v>525.75</v>
+        <v>521.25</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -8871,13 +8883,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>130.5</v>
+        <v>128.5</v>
       </c>
       <c r="C491" s="19">
         <v>0.39</v>
       </c>
       <c r="D491" s="20">
-        <v>51.12</v>
+        <v>50.34</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -8885,13 +8897,13 @@
         <v>494</v>
       </c>
       <c r="B492" s="18">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C492" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D492" s="20">
-        <v>266.76</v>
+        <v>264.48</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -9127,13 +9139,13 @@
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="C511" s="19">
         <v>3.5</v>
       </c>
       <c r="D511" s="20">
-        <v>75.25</v>
+        <v>71.75</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9205,13 +9217,13 @@
         <v>519</v>
       </c>
       <c r="B517" s="18">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C517" s="19">
         <v>3.6</v>
       </c>
       <c r="D517" s="20">
-        <v>183.6</v>
+        <v>172.8</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
@@ -9305,13 +9317,13 @@
         <v>527</v>
       </c>
       <c r="B525" s="18">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C525" s="19">
         <v>3.8</v>
       </c>
       <c r="D525" s="20">
-        <v>152</v>
+        <v>133</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
@@ -9347,13 +9359,13 @@
         <v>530</v>
       </c>
       <c r="B528" s="18">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C528" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D528" s="20">
-        <v>114.4</v>
+        <v>110</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
@@ -9529,13 +9541,13 @@
         <v>543</v>
       </c>
       <c r="B541" s="18">
-        <v>13</v>
+        <v>6.5</v>
       </c>
       <c r="C541" s="19">
         <v>5.5</v>
       </c>
       <c r="D541" s="20">
-        <v>71.5</v>
+        <v>35.75</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
@@ -9613,13 +9625,13 @@
         <v>549</v>
       </c>
       <c r="B547" s="18">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C547" s="19">
         <v>6</v>
       </c>
       <c r="D547" s="20">
-        <v>138</v>
+        <v>282</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
@@ -9811,13 +9823,13 @@
         <v>564</v>
       </c>
       <c r="B562" s="18">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C562" s="19">
         <v>2.76</v>
       </c>
       <c r="D562" s="20">
-        <v>264.95999999999998</v>
+        <v>256.68</v>
       </c>
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
@@ -9881,13 +9893,13 @@
         <v>569</v>
       </c>
       <c r="B567" s="18">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C567" s="19">
         <v>2.76</v>
       </c>
       <c r="D567" s="20">
-        <v>121.44</v>
+        <v>118.68</v>
       </c>
     </row>
     <row r="568" spans="1:4" x14ac:dyDescent="0.25">
@@ -10021,13 +10033,13 @@
         <v>579</v>
       </c>
       <c r="B577" s="18">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C577" s="19">
         <v>5.25</v>
       </c>
       <c r="D577" s="20">
-        <v>220.5</v>
+        <v>215.25</v>
       </c>
     </row>
     <row r="578" spans="1:4" x14ac:dyDescent="0.25">
@@ -10105,13 +10117,13 @@
         <v>585</v>
       </c>
       <c r="B583" s="18">
-        <v>-1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C583" s="19">
         <v>4.28</v>
       </c>
       <c r="D583" s="20">
-        <v>-6.42</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
@@ -10161,13 +10173,13 @@
         <v>589</v>
       </c>
       <c r="B587" s="18">
-        <v>122</v>
+        <v>119.5</v>
       </c>
       <c r="C587" s="19">
         <v>1.39</v>
       </c>
       <c r="D587" s="20">
-        <v>169.83</v>
+        <v>166.35</v>
       </c>
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
@@ -10175,13 +10187,13 @@
         <v>590</v>
       </c>
       <c r="B588" s="18">
-        <v>344.5</v>
+        <v>354.5</v>
       </c>
       <c r="C588" s="19">
         <v>1.4</v>
       </c>
       <c r="D588" s="20">
-        <v>482.3</v>
+        <v>496.3</v>
       </c>
     </row>
     <row r="589" spans="1:4" x14ac:dyDescent="0.25">
@@ -10189,13 +10201,13 @@
         <v>591</v>
       </c>
       <c r="B589" s="18">
-        <v>80.5</v>
+        <v>78.5</v>
       </c>
       <c r="C589" s="19">
         <v>1.4</v>
       </c>
       <c r="D589" s="20">
-        <v>112.7</v>
+        <v>109.9</v>
       </c>
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.25">
@@ -10213,7 +10225,7 @@
         <v>593</v>
       </c>
       <c r="B591" s="18">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="C591" s="22"/>
       <c r="D591" s="21"/>
@@ -10233,7 +10245,7 @@
         <v>595</v>
       </c>
       <c r="B593" s="18">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="C593" s="22"/>
       <c r="D593" s="21"/>
@@ -10243,7 +10255,7 @@
         <v>596</v>
       </c>
       <c r="B594" s="18">
-        <v>-10</v>
+        <v>470</v>
       </c>
       <c r="C594" s="22"/>
       <c r="D594" s="21"/>
@@ -10253,13 +10265,13 @@
         <v>597</v>
       </c>
       <c r="B595" s="18">
-        <v>1756.5</v>
+        <v>1753.5</v>
       </c>
       <c r="C595" s="19">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="D595" s="20">
-        <v>1405.2</v>
+        <v>1446.64</v>
       </c>
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
@@ -10267,13 +10279,13 @@
         <v>598</v>
       </c>
       <c r="B596" s="18">
-        <v>617.5</v>
+        <v>614.5</v>
       </c>
       <c r="C596" s="19">
         <v>0.8</v>
       </c>
       <c r="D596" s="20">
-        <v>494</v>
+        <v>491.6</v>
       </c>
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
@@ -10323,13 +10335,13 @@
         <v>602</v>
       </c>
       <c r="B600" s="18">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C600" s="19">
         <v>0.52</v>
       </c>
       <c r="D600" s="20">
-        <v>139.88</v>
+        <v>138.32</v>
       </c>
     </row>
     <row r="601" spans="1:4" x14ac:dyDescent="0.25">
@@ -10337,13 +10349,13 @@
         <v>603</v>
       </c>
       <c r="B601" s="18">
-        <v>830</v>
+        <v>816</v>
       </c>
       <c r="C601" s="19">
         <v>0.52</v>
       </c>
       <c r="D601" s="20">
-        <v>431.6</v>
+        <v>424.32</v>
       </c>
     </row>
     <row r="602" spans="1:4" x14ac:dyDescent="0.25">
@@ -10449,11 +10461,11 @@
         <v>611</v>
       </c>
       <c r="B609" s="24">
-        <v>39574.269999999997</v>
+        <v>40521.019999999997</v>
       </c>
       <c r="C609" s="25"/>
       <c r="D609" s="26">
-        <v>110100.23</v>
+        <v>112722.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:59
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 27-Dec-2024</t>
+    <t>1-Jul-2024 to 28-Dec-2024</t>
   </si>
   <si>
     <t/>
@@ -2489,13 +2489,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="18">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" s="19">
         <v>2.1</v>
       </c>
       <c r="D24" s="20">
-        <v>123.9</v>
+        <v>119.7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,13 +2503,13 @@
         <v>27</v>
       </c>
       <c r="B25" s="18">
-        <v>114.5</v>
+        <v>111.5</v>
       </c>
       <c r="C25" s="19">
         <v>2.1</v>
       </c>
       <c r="D25" s="20">
-        <v>240.45</v>
+        <v>234.15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2783,13 +2783,13 @@
         <v>47</v>
       </c>
       <c r="B45" s="18">
-        <v>246.5</v>
+        <v>242.5</v>
       </c>
       <c r="C45" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D45" s="20">
-        <v>271.14999999999998</v>
+        <v>266.75</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2797,13 +2797,13 @@
         <v>48</v>
       </c>
       <c r="B46" s="18">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C46" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D46" s="20">
-        <v>411.4</v>
+        <v>407</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2853,13 +2853,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>279.39999999999998</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,13 +3091,13 @@
         <v>69</v>
       </c>
       <c r="B67" s="18">
-        <v>107.5</v>
+        <v>105.5</v>
       </c>
       <c r="C67" s="19">
         <v>0.9</v>
       </c>
       <c r="D67" s="20">
-        <v>96.75</v>
+        <v>94.95</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3105,13 +3105,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="18">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C68" s="19">
         <v>1.55</v>
       </c>
       <c r="D68" s="20">
-        <v>564.20000000000005</v>
+        <v>556.45000000000005</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3207,13 +3207,13 @@
         <v>79</v>
       </c>
       <c r="B77" s="18">
-        <v>487.5</v>
+        <v>484.5</v>
       </c>
       <c r="C77" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D77" s="20">
-        <v>560.63</v>
+        <v>557.17999999999995</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3221,13 +3221,13 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>466.5</v>
+        <v>463.5</v>
       </c>
       <c r="C78" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D78" s="20">
-        <v>536.48</v>
+        <v>533.03</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4383,13 +4383,13 @@
         <v>163</v>
       </c>
       <c r="B161" s="18">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C161" s="19">
         <v>3.8</v>
       </c>
       <c r="D161" s="20">
-        <v>349.6</v>
+        <v>334.4</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4677,13 +4677,13 @@
         <v>184</v>
       </c>
       <c r="B182" s="18">
-        <v>84.5</v>
+        <v>80.5</v>
       </c>
       <c r="C182" s="19">
         <v>3.8</v>
       </c>
       <c r="D182" s="20">
-        <v>321.10000000000002</v>
+        <v>305.89999999999998</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,13 +4719,13 @@
         <v>187</v>
       </c>
       <c r="B185" s="18">
-        <v>16.5</v>
+        <v>15</v>
       </c>
       <c r="C185" s="19">
         <v>4.1100000000000003</v>
       </c>
       <c r="D185" s="20">
-        <v>67.84</v>
+        <v>61.68</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -5027,13 +5027,13 @@
         <v>209</v>
       </c>
       <c r="B207" s="18">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C207" s="19">
         <v>5.7</v>
       </c>
       <c r="D207" s="20">
-        <v>461.7</v>
+        <v>404.7</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5755,13 +5755,13 @@
         <v>261</v>
       </c>
       <c r="B259" s="18">
-        <v>22.5</v>
+        <v>20.5</v>
       </c>
       <c r="C259" s="19">
         <v>7.18</v>
       </c>
       <c r="D259" s="20">
-        <v>161.5</v>
+        <v>147.13999999999999</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -7225,13 +7225,13 @@
         <v>366</v>
       </c>
       <c r="B364" s="18">
-        <v>69.5</v>
+        <v>66</v>
       </c>
       <c r="C364" s="19">
         <v>2.7</v>
       </c>
       <c r="D364" s="20">
-        <v>187.65</v>
+        <v>178.2</v>
       </c>
     </row>
     <row r="365" spans="1:4" x14ac:dyDescent="0.25">
@@ -7491,13 +7491,13 @@
         <v>385</v>
       </c>
       <c r="B383" s="18">
-        <v>38.06</v>
+        <v>37.06</v>
       </c>
       <c r="C383" s="19">
         <v>3.5</v>
       </c>
       <c r="D383" s="20">
-        <v>133.21</v>
+        <v>129.71</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -7897,13 +7897,13 @@
         <v>414</v>
       </c>
       <c r="B412" s="18">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C412" s="19">
         <v>7.13</v>
       </c>
       <c r="D412" s="20">
-        <v>313.72000000000003</v>
+        <v>306.58999999999997</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
@@ -8191,13 +8191,13 @@
         <v>435</v>
       </c>
       <c r="B433" s="18">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="C433" s="19">
         <v>3</v>
       </c>
       <c r="D433" s="20">
-        <v>64.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -8303,13 +8303,13 @@
         <v>443</v>
       </c>
       <c r="B441" s="18">
-        <v>80.5</v>
+        <v>80</v>
       </c>
       <c r="C441" s="19">
         <v>1.71</v>
       </c>
       <c r="D441" s="20">
-        <v>137.66</v>
+        <v>136.80000000000001</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -8849,13 +8849,13 @@
         <v>482</v>
       </c>
       <c r="B480" s="18">
-        <v>46.5</v>
+        <v>34.5</v>
       </c>
       <c r="C480" s="19">
         <v>5</v>
       </c>
       <c r="D480" s="20">
-        <v>232.5</v>
+        <v>172.5</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -9507,13 +9507,13 @@
         <v>529</v>
       </c>
       <c r="B527" s="18">
-        <v>58.5</v>
+        <v>48.5</v>
       </c>
       <c r="C527" s="19">
         <v>4.05</v>
       </c>
       <c r="D527" s="20">
-        <v>236.93</v>
+        <v>196.43</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
@@ -9563,13 +9563,13 @@
         <v>533</v>
       </c>
       <c r="B531" s="18">
-        <v>59.5</v>
+        <v>57.5</v>
       </c>
       <c r="C531" s="19">
         <v>1.4</v>
       </c>
       <c r="D531" s="20">
-        <v>83.3</v>
+        <v>80.5</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
@@ -9641,13 +9641,13 @@
         <v>540</v>
       </c>
       <c r="B538" s="18">
-        <v>551.5</v>
+        <v>550</v>
       </c>
       <c r="C538" s="19">
         <v>0.8</v>
       </c>
       <c r="D538" s="20">
-        <v>441.2</v>
+        <v>440</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
@@ -9669,13 +9669,13 @@
         <v>542</v>
       </c>
       <c r="B540" s="18">
-        <v>401.5</v>
+        <v>400</v>
       </c>
       <c r="C540" s="19">
         <v>0.8</v>
       </c>
       <c r="D540" s="20">
-        <v>321.2</v>
+        <v>320</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
@@ -9843,11 +9843,11 @@
         <v>555</v>
       </c>
       <c r="B553" s="24">
-        <v>40226.720000000001</v>
+        <v>40140.720000000001</v>
       </c>
       <c r="C553" s="25"/>
       <c r="D553" s="26">
-        <v>111869.13</v>
+        <v>111589.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:28
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="562">
   <si>
     <t>StkSummary</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 1-Jan-2025</t>
+    <t>1-Jul-2024 to 2-Jan-2025</t>
   </si>
   <si>
     <t/>
@@ -1272,6 +1272,9 @@
   </si>
   <si>
     <t>7314 PATRIKA (DC) {{10}}</t>
+  </si>
+  <si>
+    <t>7315 PATRIKA (DC) {{10}}</t>
   </si>
   <si>
     <t>7316 PATRIKA</t>
@@ -2199,7 +2202,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D558"/>
+  <dimension ref="A1:D559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2336,13 +2339,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="18">
-        <v>192.5</v>
+        <v>188.5</v>
       </c>
       <c r="C12" s="19">
         <v>1.65</v>
       </c>
       <c r="D12" s="20">
-        <v>317.63</v>
+        <v>311.02999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2406,13 +2409,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="18">
-        <v>98.5</v>
+        <v>96.5</v>
       </c>
       <c r="C17" s="19">
         <v>2</v>
       </c>
       <c r="D17" s="20">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,13 +2479,13 @@
         <v>24</v>
       </c>
       <c r="B22" s="18">
-        <v>82.5</v>
+        <v>80</v>
       </c>
       <c r="C22" s="19">
         <v>2</v>
       </c>
       <c r="D22" s="20">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2490,13 +2493,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="18">
-        <v>116.5</v>
+        <v>114.5</v>
       </c>
       <c r="C23" s="19">
         <v>2</v>
       </c>
       <c r="D23" s="20">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2532,13 +2535,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="18">
-        <v>54.82</v>
+        <v>51.32</v>
       </c>
       <c r="C26" s="19">
         <v>2.35</v>
       </c>
       <c r="D26" s="20">
-        <v>128.83000000000001</v>
+        <v>120.6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2546,13 +2549,13 @@
         <v>29</v>
       </c>
       <c r="B27" s="18">
-        <v>43.37</v>
+        <v>38.369999999999997</v>
       </c>
       <c r="C27" s="19">
         <v>2.35</v>
       </c>
       <c r="D27" s="20">
-        <v>101.92</v>
+        <v>90.17</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2560,13 +2563,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="18">
-        <v>176.8</v>
+        <v>164.8</v>
       </c>
       <c r="C28" s="19">
         <v>2.59</v>
       </c>
       <c r="D28" s="20">
-        <v>457.15</v>
+        <v>426.13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2602,13 +2605,13 @@
         <v>33</v>
       </c>
       <c r="B31" s="18">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C31" s="19">
         <v>2.5</v>
       </c>
       <c r="D31" s="20">
-        <v>117.5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2728,13 +2731,13 @@
         <v>42</v>
       </c>
       <c r="B40" s="18">
-        <v>137.5</v>
+        <v>128.5</v>
       </c>
       <c r="C40" s="19">
         <v>2.25</v>
       </c>
       <c r="D40" s="20">
-        <v>309.38</v>
+        <v>289.13</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2798,13 +2801,13 @@
         <v>47</v>
       </c>
       <c r="B45" s="18">
-        <v>104.5</v>
+        <v>95.5</v>
       </c>
       <c r="C45" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D45" s="20">
-        <v>114.95</v>
+        <v>105.05</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2812,13 +2815,13 @@
         <v>48</v>
       </c>
       <c r="B46" s="18">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C46" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D46" s="20">
-        <v>264</v>
+        <v>261.8</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2826,13 +2829,13 @@
         <v>49</v>
       </c>
       <c r="B47" s="18">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C47" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D47" s="20">
-        <v>180.4</v>
+        <v>169.4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2840,13 +2843,13 @@
         <v>50</v>
       </c>
       <c r="B48" s="18">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="C48" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D48" s="20">
-        <v>338.8</v>
+        <v>325.60000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2868,13 +2871,13 @@
         <v>52</v>
       </c>
       <c r="B50" s="18">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C50" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D50" s="20">
-        <v>146.30000000000001</v>
+        <v>119.9</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2882,13 +2885,13 @@
         <v>53</v>
       </c>
       <c r="B51" s="18">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C51" s="19">
         <v>1.1000000000000001</v>
       </c>
       <c r="D51" s="20">
-        <v>226.6</v>
+        <v>215.6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2910,13 +2913,13 @@
         <v>55</v>
       </c>
       <c r="B53" s="18">
-        <v>563.5</v>
+        <v>559.5</v>
       </c>
       <c r="C53" s="19">
         <v>1.9</v>
       </c>
       <c r="D53" s="20">
-        <v>1070.6500000000001</v>
+        <v>1063.05</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2938,13 +2941,13 @@
         <v>57</v>
       </c>
       <c r="B55" s="18">
-        <v>245</v>
+        <v>243.5</v>
       </c>
       <c r="C55" s="19">
         <v>1.9</v>
       </c>
       <c r="D55" s="20">
-        <v>465.5</v>
+        <v>462.65</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3078,13 +3081,13 @@
         <v>67</v>
       </c>
       <c r="B65" s="18">
-        <v>153.5</v>
+        <v>152.5</v>
       </c>
       <c r="C65" s="19">
         <v>0.7</v>
       </c>
       <c r="D65" s="20">
-        <v>107.45</v>
+        <v>106.75</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3120,13 +3123,13 @@
         <v>70</v>
       </c>
       <c r="B68" s="18">
-        <v>340</v>
+        <v>330.5</v>
       </c>
       <c r="C68" s="19">
         <v>1.55</v>
       </c>
       <c r="D68" s="20">
-        <v>527</v>
+        <v>512.28</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3192,7 +3195,7 @@
         <v>76</v>
       </c>
       <c r="B74" s="18">
-        <v>37.5</v>
+        <v>24.5</v>
       </c>
       <c r="C74" s="21"/>
       <c r="D74" s="22"/>
@@ -3232,7 +3235,7 @@
         <v>80</v>
       </c>
       <c r="B78" s="18">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C78" s="21"/>
       <c r="D78" s="22"/>
@@ -3242,13 +3245,13 @@
         <v>81</v>
       </c>
       <c r="B79" s="18">
-        <v>441.5</v>
+        <v>434.5</v>
       </c>
       <c r="C79" s="19">
         <v>1.1499999999999999</v>
       </c>
       <c r="D79" s="20">
-        <v>507.73</v>
+        <v>499.68</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3270,13 +3273,13 @@
         <v>83</v>
       </c>
       <c r="B81" s="18">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="C81" s="19">
         <v>1.4</v>
       </c>
       <c r="D81" s="20">
-        <v>708.4</v>
+        <v>694.4</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3298,13 +3301,13 @@
         <v>85</v>
       </c>
       <c r="B83" s="18">
-        <v>16.5</v>
+        <v>14.5</v>
       </c>
       <c r="C83" s="19">
         <v>1.4</v>
       </c>
       <c r="D83" s="20">
-        <v>23.1</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,13 +3329,13 @@
         <v>87</v>
       </c>
       <c r="B85" s="18">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C85" s="19">
         <v>2</v>
       </c>
       <c r="D85" s="20">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,13 +3343,13 @@
         <v>88</v>
       </c>
       <c r="B86" s="18">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C86" s="19">
         <v>1.26</v>
       </c>
       <c r="D86" s="20">
-        <v>574.55999999999995</v>
+        <v>570.78</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,13 +3357,13 @@
         <v>89</v>
       </c>
       <c r="B87" s="18">
-        <v>450.5</v>
+        <v>444.5</v>
       </c>
       <c r="C87" s="19">
         <v>1.26</v>
       </c>
       <c r="D87" s="20">
-        <v>567.63</v>
+        <v>560.07000000000005</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3466,7 +3469,7 @@
         <v>97</v>
       </c>
       <c r="B95" s="18">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C95" s="21"/>
       <c r="D95" s="22"/>
@@ -3524,13 +3527,13 @@
         <v>102</v>
       </c>
       <c r="B100" s="18">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C100" s="19">
         <v>12.5</v>
       </c>
       <c r="D100" s="20">
-        <v>250</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3552,13 +3555,13 @@
         <v>104</v>
       </c>
       <c r="B102" s="18">
-        <v>18.5</v>
+        <v>14.5</v>
       </c>
       <c r="C102" s="19">
         <v>12.5</v>
       </c>
       <c r="D102" s="20">
-        <v>231.25</v>
+        <v>181.25</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3566,13 +3569,13 @@
         <v>105</v>
       </c>
       <c r="B103" s="18">
-        <v>33</v>
+        <v>30.5</v>
       </c>
       <c r="C103" s="19">
         <v>12.5</v>
       </c>
       <c r="D103" s="20">
-        <v>412.5</v>
+        <v>381.25</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3580,13 +3583,13 @@
         <v>106</v>
       </c>
       <c r="B104" s="18">
-        <v>42.86</v>
+        <v>37.86</v>
       </c>
       <c r="C104" s="19">
         <v>12.5</v>
       </c>
       <c r="D104" s="20">
-        <v>535.75</v>
+        <v>473.25</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3986,13 +3989,13 @@
         <v>135</v>
       </c>
       <c r="B133" s="18">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="C133" s="19">
         <v>18.37</v>
       </c>
       <c r="D133" s="20">
-        <v>82.66</v>
+        <v>55.11</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4000,13 +4003,13 @@
         <v>136</v>
       </c>
       <c r="B134" s="18">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C134" s="19">
         <v>18.34</v>
       </c>
       <c r="D134" s="20">
-        <v>27.51</v>
+        <v>9.17</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -4042,13 +4045,13 @@
         <v>139</v>
       </c>
       <c r="B137" s="18">
-        <v>54.5</v>
+        <v>51.5</v>
       </c>
       <c r="C137" s="19">
         <v>3.3</v>
       </c>
       <c r="D137" s="20">
-        <v>179.85</v>
+        <v>169.95</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4056,13 +4059,13 @@
         <v>140</v>
       </c>
       <c r="B138" s="18">
-        <v>25</v>
+        <v>19.5</v>
       </c>
       <c r="C138" s="19">
         <v>2.8</v>
       </c>
       <c r="D138" s="20">
-        <v>70</v>
+        <v>54.6</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4070,13 +4073,13 @@
         <v>141</v>
       </c>
       <c r="B139" s="18">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C139" s="19">
         <v>2.75</v>
       </c>
       <c r="D139" s="20">
-        <v>280.5</v>
+        <v>272.25</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4084,13 +4087,13 @@
         <v>142</v>
       </c>
       <c r="B140" s="18">
-        <v>75</v>
+        <v>72.5</v>
       </c>
       <c r="C140" s="19">
         <v>2.75</v>
       </c>
       <c r="D140" s="20">
-        <v>206.25</v>
+        <v>199.38</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,13 +4115,13 @@
         <v>144</v>
       </c>
       <c r="B142" s="18">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C142" s="19">
         <v>3.4</v>
       </c>
       <c r="D142" s="20">
-        <v>176.8</v>
+        <v>173.4</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4140,13 +4143,13 @@
         <v>146</v>
       </c>
       <c r="B144" s="18">
-        <v>31.5</v>
+        <v>23</v>
       </c>
       <c r="C144" s="19">
         <v>2.7</v>
       </c>
       <c r="D144" s="20">
-        <v>85.05</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4154,13 +4157,13 @@
         <v>147</v>
       </c>
       <c r="B145" s="18">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C145" s="19">
         <v>2.8</v>
       </c>
       <c r="D145" s="20">
-        <v>196</v>
+        <v>190.4</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4168,13 +4171,13 @@
         <v>148</v>
       </c>
       <c r="B146" s="18">
-        <v>87.5</v>
+        <v>80.5</v>
       </c>
       <c r="C146" s="19">
         <v>2.8</v>
       </c>
       <c r="D146" s="20">
-        <v>245</v>
+        <v>225.4</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4238,13 +4241,13 @@
         <v>153</v>
       </c>
       <c r="B151" s="18">
-        <v>78.5</v>
+        <v>72.5</v>
       </c>
       <c r="C151" s="19">
         <v>2.95</v>
       </c>
       <c r="D151" s="20">
-        <v>231.58</v>
+        <v>213.88</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4252,13 +4255,13 @@
         <v>154</v>
       </c>
       <c r="B152" s="18">
-        <v>46.5</v>
+        <v>44</v>
       </c>
       <c r="C152" s="19">
         <v>2.95</v>
       </c>
       <c r="D152" s="20">
-        <v>137.18</v>
+        <v>129.80000000000001</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,13 +4269,13 @@
         <v>155</v>
       </c>
       <c r="B153" s="18">
-        <v>89.5</v>
+        <v>77.5</v>
       </c>
       <c r="C153" s="19">
         <v>3</v>
       </c>
       <c r="D153" s="20">
-        <v>268.5</v>
+        <v>232.5</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4392,13 +4395,13 @@
         <v>164</v>
       </c>
       <c r="B162" s="18">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C162" s="19">
         <v>3.33</v>
       </c>
       <c r="D162" s="20">
-        <v>299.7</v>
+        <v>293.04000000000002</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4420,13 +4423,13 @@
         <v>166</v>
       </c>
       <c r="B164" s="18">
-        <v>133.5</v>
+        <v>128.5</v>
       </c>
       <c r="C164" s="19">
         <v>3.6</v>
       </c>
       <c r="D164" s="20">
-        <v>480.6</v>
+        <v>462.6</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4476,13 +4479,13 @@
         <v>170</v>
       </c>
       <c r="B168" s="18">
-        <v>124.5</v>
+        <v>120</v>
       </c>
       <c r="C168" s="19">
         <v>4.5</v>
       </c>
       <c r="D168" s="20">
-        <v>560.25</v>
+        <v>540</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4574,13 +4577,13 @@
         <v>177</v>
       </c>
       <c r="B175" s="18">
-        <v>130.5</v>
+        <v>128</v>
       </c>
       <c r="C175" s="19">
         <v>3.96</v>
       </c>
       <c r="D175" s="20">
-        <v>516.41999999999996</v>
+        <v>506.53</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -4672,13 +4675,13 @@
         <v>184</v>
       </c>
       <c r="B182" s="18">
-        <v>86.24</v>
+        <v>79.239999999999995</v>
       </c>
       <c r="C182" s="19">
         <v>3.11</v>
       </c>
       <c r="D182" s="20">
-        <v>267.88</v>
+        <v>246.14</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4812,13 +4815,13 @@
         <v>194</v>
       </c>
       <c r="B192" s="18">
-        <v>50.5</v>
+        <v>45.5</v>
       </c>
       <c r="C192" s="19">
         <v>4.75</v>
       </c>
       <c r="D192" s="20">
-        <v>239.88</v>
+        <v>216.13</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -4840,13 +4843,13 @@
         <v>196</v>
       </c>
       <c r="B194" s="18">
-        <v>73</v>
+        <v>65.5</v>
       </c>
       <c r="C194" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D194" s="20">
-        <v>321.2</v>
+        <v>288.2</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -4882,13 +4885,13 @@
         <v>199</v>
       </c>
       <c r="B197" s="18">
-        <v>224.5</v>
+        <v>223.5</v>
       </c>
       <c r="C197" s="19">
         <v>4.5</v>
       </c>
       <c r="D197" s="20">
-        <v>1010.25</v>
+        <v>1005.75</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -4896,13 +4899,13 @@
         <v>200</v>
       </c>
       <c r="B198" s="18">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C198" s="19">
         <v>4.5</v>
       </c>
       <c r="D198" s="20">
-        <v>796.5</v>
+        <v>765</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -4994,13 +4997,13 @@
         <v>207</v>
       </c>
       <c r="B205" s="18">
-        <v>32.5</v>
+        <v>31</v>
       </c>
       <c r="C205" s="19">
         <v>5.25</v>
       </c>
       <c r="D205" s="20">
-        <v>170.63</v>
+        <v>162.75</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5008,13 +5011,13 @@
         <v>208</v>
       </c>
       <c r="B206" s="18">
-        <v>48.5</v>
+        <v>33.5</v>
       </c>
       <c r="C206" s="19">
         <v>5.25</v>
       </c>
       <c r="D206" s="20">
-        <v>254.63</v>
+        <v>175.88</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5022,13 +5025,13 @@
         <v>209</v>
       </c>
       <c r="B207" s="18">
-        <v>34.5</v>
+        <v>39.5</v>
       </c>
       <c r="C207" s="19">
         <v>4.75</v>
       </c>
       <c r="D207" s="20">
-        <v>163.88</v>
+        <v>187.63</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5092,13 +5095,13 @@
         <v>214</v>
       </c>
       <c r="B212" s="18">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C212" s="19">
         <v>5.7</v>
       </c>
       <c r="D212" s="20">
-        <v>313.5</v>
+        <v>296.39999999999998</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5260,13 +5263,13 @@
         <v>226</v>
       </c>
       <c r="B224" s="18">
-        <v>32.5</v>
+        <v>28</v>
       </c>
       <c r="C224" s="19">
         <v>3.5</v>
       </c>
       <c r="D224" s="20">
-        <v>113.75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5302,13 +5305,13 @@
         <v>229</v>
       </c>
       <c r="B227" s="18">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C227" s="19">
         <v>4.18</v>
       </c>
       <c r="D227" s="20">
-        <v>217.36</v>
+        <v>213.18</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5344,13 +5347,13 @@
         <v>232</v>
       </c>
       <c r="B230" s="18">
-        <v>68.5</v>
+        <v>67</v>
       </c>
       <c r="C230" s="19">
         <v>4.28</v>
       </c>
       <c r="D230" s="20">
-        <v>293.18</v>
+        <v>286.76</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5386,13 +5389,13 @@
         <v>235</v>
       </c>
       <c r="B233" s="18">
-        <v>20</v>
+        <v>22.5</v>
       </c>
       <c r="C233" s="19">
         <v>4.95</v>
       </c>
       <c r="D233" s="20">
-        <v>99</v>
+        <v>111.38</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5414,13 +5417,13 @@
         <v>237</v>
       </c>
       <c r="B235" s="18">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="C235" s="19">
         <v>5</v>
       </c>
       <c r="D235" s="20">
-        <v>152.5</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5428,13 +5431,13 @@
         <v>238</v>
       </c>
       <c r="B236" s="18">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C236" s="19">
         <v>5.0999999999999996</v>
       </c>
       <c r="D236" s="20">
-        <v>117.3</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -5526,13 +5529,13 @@
         <v>245</v>
       </c>
       <c r="B243" s="18">
-        <v>34.5</v>
+        <v>33.5</v>
       </c>
       <c r="C243" s="19">
         <v>5.46</v>
       </c>
       <c r="D243" s="20">
-        <v>188.37</v>
+        <v>182.91</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -5582,13 +5585,13 @@
         <v>249</v>
       </c>
       <c r="B247" s="18">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C247" s="19">
         <v>6</v>
       </c>
       <c r="D247" s="20">
-        <v>138</v>
+        <v>108</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5610,13 +5613,13 @@
         <v>251</v>
       </c>
       <c r="B249" s="18">
-        <v>48.38</v>
+        <v>46.88</v>
       </c>
       <c r="C249" s="19">
         <v>5.94</v>
       </c>
       <c r="D249" s="20">
-        <v>287.38</v>
+        <v>278.47000000000003</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -5652,13 +5655,13 @@
         <v>254</v>
       </c>
       <c r="B252" s="18">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C252" s="19">
         <v>5.94</v>
       </c>
       <c r="D252" s="20">
-        <v>297</v>
+        <v>279.18</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -5666,13 +5669,13 @@
         <v>255</v>
       </c>
       <c r="B253" s="18">
-        <v>27</v>
+        <v>22.5</v>
       </c>
       <c r="C253" s="19">
         <v>6.67</v>
       </c>
       <c r="D253" s="20">
-        <v>180.09</v>
+        <v>150.08000000000001</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -5834,13 +5837,13 @@
         <v>267</v>
       </c>
       <c r="B265" s="18">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C265" s="19">
         <v>7.13</v>
       </c>
       <c r="D265" s="20">
-        <v>634.57000000000005</v>
+        <v>627.44000000000005</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -5848,13 +5851,13 @@
         <v>268</v>
       </c>
       <c r="B266" s="18">
-        <v>81</v>
+        <v>78.5</v>
       </c>
       <c r="C266" s="19">
         <v>7.13</v>
       </c>
       <c r="D266" s="20">
-        <v>577.53</v>
+        <v>559.71</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -5946,13 +5949,13 @@
         <v>275</v>
       </c>
       <c r="B273" s="18">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C273" s="19">
         <v>8.75</v>
       </c>
       <c r="D273" s="20">
-        <v>245</v>
+        <v>201.25</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6072,13 +6075,13 @@
         <v>284</v>
       </c>
       <c r="B282" s="18">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="C282" s="19">
         <v>9.5</v>
       </c>
       <c r="D282" s="20">
-        <v>52.25</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -6114,13 +6117,13 @@
         <v>287</v>
       </c>
       <c r="B285" s="18">
-        <v>46.5</v>
+        <v>37</v>
       </c>
       <c r="C285" s="19">
         <v>9.25</v>
       </c>
       <c r="D285" s="20">
-        <v>430.13</v>
+        <v>342.25</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -6170,13 +6173,13 @@
         <v>291</v>
       </c>
       <c r="B289" s="18">
-        <v>74</v>
+        <v>71.5</v>
       </c>
       <c r="C289" s="19">
         <v>5.5</v>
       </c>
       <c r="D289" s="20">
-        <v>407</v>
+        <v>393.25</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.25">
@@ -6184,13 +6187,13 @@
         <v>292</v>
       </c>
       <c r="B290" s="18">
-        <v>55.5</v>
+        <v>54.5</v>
       </c>
       <c r="C290" s="19">
         <v>6.86</v>
       </c>
       <c r="D290" s="20">
-        <v>380.76</v>
+        <v>373.9</v>
       </c>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.25">
@@ -6324,13 +6327,13 @@
         <v>302</v>
       </c>
       <c r="B300" s="18">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C300" s="19">
         <v>4.9000000000000004</v>
       </c>
       <c r="D300" s="20">
-        <v>548.79999999999995</v>
+        <v>529.20000000000005</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.25">
@@ -6366,13 +6369,13 @@
         <v>305</v>
       </c>
       <c r="B303" s="18">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="C303" s="19">
         <v>7.6</v>
       </c>
       <c r="D303" s="20">
-        <v>231.8</v>
+        <v>224.2</v>
       </c>
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.25">
@@ -6394,13 +6397,13 @@
         <v>307</v>
       </c>
       <c r="B305" s="18">
-        <v>59</v>
+        <v>57.5</v>
       </c>
       <c r="C305" s="19">
         <v>6.5</v>
       </c>
       <c r="D305" s="20">
-        <v>383.5</v>
+        <v>373.75</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6562,13 +6565,13 @@
         <v>319</v>
       </c>
       <c r="B317" s="18">
-        <v>3.99</v>
+        <v>1.99</v>
       </c>
       <c r="C317" s="19">
         <v>12</v>
       </c>
       <c r="D317" s="20">
-        <v>47.88</v>
+        <v>23.88</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.25">
@@ -6590,13 +6593,13 @@
         <v>321</v>
       </c>
       <c r="B319" s="18">
-        <v>18.5</v>
+        <v>13.5</v>
       </c>
       <c r="C319" s="19">
         <v>7.84</v>
       </c>
       <c r="D319" s="20">
-        <v>145.04</v>
+        <v>105.84</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.25">
@@ -6758,13 +6761,13 @@
         <v>333</v>
       </c>
       <c r="B331" s="18">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C331" s="19">
         <v>9.5</v>
       </c>
       <c r="D331" s="20">
-        <v>627</v>
+        <v>560.5</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">
@@ -6898,13 +6901,13 @@
         <v>343</v>
       </c>
       <c r="B341" s="18">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="C341" s="19">
         <v>12.5</v>
       </c>
       <c r="D341" s="20">
-        <v>43.75</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -6968,13 +6971,13 @@
         <v>348</v>
       </c>
       <c r="B346" s="18">
-        <v>24.5</v>
+        <v>13.5</v>
       </c>
       <c r="C346" s="19">
         <v>11.4</v>
       </c>
       <c r="D346" s="20">
-        <v>279.3</v>
+        <v>153.9</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.25">
@@ -6996,13 +6999,13 @@
         <v>350</v>
       </c>
       <c r="B348" s="18">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
       <c r="C348" s="19">
         <v>22.5</v>
       </c>
       <c r="D348" s="20">
-        <v>303.75</v>
+        <v>236.25</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -7038,13 +7041,13 @@
         <v>353</v>
       </c>
       <c r="B351" s="18">
-        <v>15.5</v>
+        <v>13</v>
       </c>
       <c r="C351" s="19">
         <v>10.93</v>
       </c>
       <c r="D351" s="20">
-        <v>169.42</v>
+        <v>142.09</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -7094,13 +7097,13 @@
         <v>357</v>
       </c>
       <c r="B355" s="18">
-        <v>9.5</v>
+        <v>4</v>
       </c>
       <c r="C355" s="19">
         <v>10.45</v>
       </c>
       <c r="D355" s="20">
-        <v>99.28</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -7290,13 +7293,13 @@
         <v>371</v>
       </c>
       <c r="B369" s="18">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C369" s="19">
         <v>2.7</v>
       </c>
       <c r="D369" s="20">
-        <v>170.1</v>
+        <v>164.7</v>
       </c>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
@@ -7332,13 +7335,13 @@
         <v>374</v>
       </c>
       <c r="B372" s="18">
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="C372" s="19">
         <v>2.75</v>
       </c>
       <c r="D372" s="20">
-        <v>204.88</v>
+        <v>202.13</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
@@ -7472,13 +7475,13 @@
         <v>384</v>
       </c>
       <c r="B382" s="18">
-        <v>10.4</v>
+        <v>9.4</v>
       </c>
       <c r="C382" s="19">
         <v>3.15</v>
       </c>
       <c r="D382" s="20">
-        <v>32.76</v>
+        <v>29.61</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -7920,13 +7923,13 @@
         <v>416</v>
       </c>
       <c r="B414" s="18">
-        <v>43</v>
+        <v>-6</v>
       </c>
       <c r="C414" s="19">
-        <v>6</v>
+        <v>5.46</v>
       </c>
       <c r="D414" s="20">
-        <v>258</v>
+        <v>-32.76</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
@@ -7934,13 +7937,13 @@
         <v>417</v>
       </c>
       <c r="B415" s="18">
-        <v>18.5</v>
+        <v>43</v>
       </c>
       <c r="C415" s="19">
-        <v>5.94</v>
+        <v>6</v>
       </c>
       <c r="D415" s="20">
-        <v>109.89</v>
+        <v>258</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
@@ -7948,13 +7951,13 @@
         <v>418</v>
       </c>
       <c r="B416" s="18">
-        <v>21</v>
+        <v>18.5</v>
       </c>
       <c r="C416" s="19">
-        <v>6.75</v>
+        <v>5.94</v>
       </c>
       <c r="D416" s="20">
-        <v>141.75</v>
+        <v>109.89</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
@@ -7962,13 +7965,13 @@
         <v>419</v>
       </c>
       <c r="B417" s="18">
-        <v>13.5</v>
+        <v>21</v>
       </c>
       <c r="C417" s="19">
-        <v>7.5</v>
+        <v>6.75</v>
       </c>
       <c r="D417" s="20">
-        <v>101.25</v>
+        <v>141.75</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
@@ -7976,13 +7979,13 @@
         <v>420</v>
       </c>
       <c r="B418" s="18">
-        <v>37.5</v>
+        <v>13.5</v>
       </c>
       <c r="C418" s="19">
-        <v>7.13</v>
+        <v>7.5</v>
       </c>
       <c r="D418" s="20">
-        <v>267.38</v>
+        <v>101.25</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
@@ -7990,13 +7993,13 @@
         <v>421</v>
       </c>
       <c r="B419" s="18">
-        <v>24</v>
+        <v>37.5</v>
       </c>
       <c r="C419" s="19">
-        <v>8</v>
+        <v>7.13</v>
       </c>
       <c r="D419" s="20">
-        <v>192</v>
+        <v>267.38</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
@@ -8004,13 +8007,13 @@
         <v>422</v>
       </c>
       <c r="B420" s="18">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C420" s="19">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D420" s="20">
-        <v>140</v>
+        <v>192</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.25">
@@ -8018,13 +8021,13 @@
         <v>423</v>
       </c>
       <c r="B421" s="18">
-        <v>18.5</v>
+        <v>20</v>
       </c>
       <c r="C421" s="19">
-        <v>7.6</v>
+        <v>7</v>
       </c>
       <c r="D421" s="20">
-        <v>140.6</v>
+        <v>140</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.25">
@@ -8032,13 +8035,13 @@
         <v>424</v>
       </c>
       <c r="B422" s="18">
-        <v>43</v>
+        <v>18.5</v>
       </c>
       <c r="C422" s="19">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
       <c r="D422" s="20">
-        <v>365.5</v>
+        <v>140.6</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
@@ -8046,13 +8049,13 @@
         <v>425</v>
       </c>
       <c r="B423" s="18">
-        <v>24.5</v>
+        <v>43</v>
       </c>
       <c r="C423" s="19">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="D423" s="20">
-        <v>183.75</v>
+        <v>365.5</v>
       </c>
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.25">
@@ -8060,13 +8063,13 @@
         <v>426</v>
       </c>
       <c r="B424" s="18">
-        <v>11.5</v>
+        <v>24.5</v>
       </c>
       <c r="C424" s="19">
-        <v>9</v>
+        <v>7.5</v>
       </c>
       <c r="D424" s="20">
-        <v>103.5</v>
+        <v>183.75</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.25">
@@ -8074,13 +8077,13 @@
         <v>427</v>
       </c>
       <c r="B425" s="18">
-        <v>18.5</v>
+        <v>11.5</v>
       </c>
       <c r="C425" s="19">
-        <v>3.75</v>
+        <v>9</v>
       </c>
       <c r="D425" s="20">
-        <v>69.38</v>
+        <v>103.5</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.25">
@@ -8088,13 +8091,13 @@
         <v>428</v>
       </c>
       <c r="B426" s="18">
-        <v>21.5</v>
+        <v>18.5</v>
       </c>
       <c r="C426" s="19">
-        <v>4.28</v>
+        <v>3.75</v>
       </c>
       <c r="D426" s="20">
-        <v>92.02</v>
+        <v>69.38</v>
       </c>
     </row>
     <row r="427" spans="1:4" x14ac:dyDescent="0.25">
@@ -8102,13 +8105,13 @@
         <v>429</v>
       </c>
       <c r="B427" s="18">
-        <v>37</v>
+        <v>21.5</v>
       </c>
       <c r="C427" s="19">
-        <v>9.5</v>
+        <v>4.28</v>
       </c>
       <c r="D427" s="20">
-        <v>351.5</v>
+        <v>92.02</v>
       </c>
     </row>
     <row r="428" spans="1:4" x14ac:dyDescent="0.25">
@@ -8116,13 +8119,13 @@
         <v>430</v>
       </c>
       <c r="B428" s="18">
-        <v>35.5</v>
+        <v>37</v>
       </c>
       <c r="C428" s="19">
-        <v>4.5</v>
+        <v>9.5</v>
       </c>
       <c r="D428" s="20">
-        <v>159.75</v>
+        <v>351.5</v>
       </c>
     </row>
     <row r="429" spans="1:4" x14ac:dyDescent="0.25">
@@ -8130,13 +8133,13 @@
         <v>431</v>
       </c>
       <c r="B429" s="18">
-        <v>50</v>
+        <v>35.5</v>
       </c>
       <c r="C429" s="19">
-        <v>2.8</v>
+        <v>4.5</v>
       </c>
       <c r="D429" s="20">
-        <v>140</v>
+        <v>159.75</v>
       </c>
     </row>
     <row r="430" spans="1:4" x14ac:dyDescent="0.25">
@@ -8144,13 +8147,13 @@
         <v>432</v>
       </c>
       <c r="B430" s="18">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C430" s="19">
-        <v>5.7</v>
+        <v>2.8</v>
       </c>
       <c r="D430" s="20">
-        <v>205.2</v>
+        <v>140</v>
       </c>
     </row>
     <row r="431" spans="1:4" x14ac:dyDescent="0.25">
@@ -8158,13 +8161,13 @@
         <v>433</v>
       </c>
       <c r="B431" s="18">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C431" s="19">
-        <v>1.92</v>
+        <v>5.7</v>
       </c>
       <c r="D431" s="20">
-        <v>65.23</v>
+        <v>205.2</v>
       </c>
     </row>
     <row r="432" spans="1:4" x14ac:dyDescent="0.25">
@@ -8172,13 +8175,13 @@
         <v>434</v>
       </c>
       <c r="B432" s="18">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C432" s="19">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="D432" s="20">
-        <v>172.9</v>
+        <v>65.23</v>
       </c>
     </row>
     <row r="433" spans="1:4" x14ac:dyDescent="0.25">
@@ -8186,13 +8189,13 @@
         <v>435</v>
       </c>
       <c r="B433" s="18">
-        <v>-3</v>
+        <v>91</v>
       </c>
       <c r="C433" s="19">
-        <v>1.1000000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="D433" s="20">
-        <v>-3.3</v>
+        <v>172.9</v>
       </c>
     </row>
     <row r="434" spans="1:4" x14ac:dyDescent="0.25">
@@ -8200,13 +8203,13 @@
         <v>436</v>
       </c>
       <c r="B434" s="18">
-        <v>56</v>
+        <v>-3</v>
       </c>
       <c r="C434" s="19">
-        <v>4.1500000000000004</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D434" s="20">
-        <v>232.4</v>
+        <v>-3.3</v>
       </c>
     </row>
     <row r="435" spans="1:4" x14ac:dyDescent="0.25">
@@ -8214,13 +8217,13 @@
         <v>437</v>
       </c>
       <c r="B435" s="18">
-        <v>113</v>
+        <v>56</v>
       </c>
       <c r="C435" s="19">
-        <v>1.4</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="D435" s="20">
-        <v>158.19999999999999</v>
+        <v>232.4</v>
       </c>
     </row>
     <row r="436" spans="1:4" x14ac:dyDescent="0.25">
@@ -8228,13 +8231,13 @@
         <v>438</v>
       </c>
       <c r="B436" s="18">
-        <v>149.5</v>
+        <v>113</v>
       </c>
       <c r="C436" s="19">
         <v>1.4</v>
       </c>
       <c r="D436" s="20">
-        <v>209.3</v>
+        <v>158.19999999999999</v>
       </c>
     </row>
     <row r="437" spans="1:4" x14ac:dyDescent="0.25">
@@ -8242,13 +8245,13 @@
         <v>439</v>
       </c>
       <c r="B437" s="18">
-        <v>80.5</v>
+        <v>149.5</v>
       </c>
       <c r="C437" s="19">
         <v>1.4</v>
       </c>
       <c r="D437" s="20">
-        <v>112.7</v>
+        <v>209.3</v>
       </c>
     </row>
     <row r="438" spans="1:4" x14ac:dyDescent="0.25">
@@ -8256,13 +8259,13 @@
         <v>440</v>
       </c>
       <c r="B438" s="18">
-        <v>20</v>
+        <v>80.5</v>
       </c>
       <c r="C438" s="19">
-        <v>3</v>
+        <v>1.4</v>
       </c>
       <c r="D438" s="20">
-        <v>60</v>
+        <v>112.7</v>
       </c>
     </row>
     <row r="439" spans="1:4" x14ac:dyDescent="0.25">
@@ -8270,13 +8273,13 @@
         <v>441</v>
       </c>
       <c r="B439" s="18">
-        <v>30.5</v>
+        <v>20</v>
       </c>
       <c r="C439" s="19">
-        <v>3.05</v>
+        <v>3</v>
       </c>
       <c r="D439" s="20">
-        <v>93.03</v>
+        <v>60</v>
       </c>
     </row>
     <row r="440" spans="1:4" x14ac:dyDescent="0.25">
@@ -8284,13 +8287,13 @@
         <v>442</v>
       </c>
       <c r="B440" s="18">
-        <v>28</v>
+        <v>30.5</v>
       </c>
       <c r="C440" s="19">
-        <v>1.55</v>
+        <v>3.05</v>
       </c>
       <c r="D440" s="20">
-        <v>43.4</v>
+        <v>93.03</v>
       </c>
     </row>
     <row r="441" spans="1:4" x14ac:dyDescent="0.25">
@@ -8298,13 +8301,13 @@
         <v>443</v>
       </c>
       <c r="B441" s="18">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C441" s="19">
         <v>1.55</v>
       </c>
       <c r="D441" s="20">
-        <v>1.55</v>
+        <v>43.4</v>
       </c>
     </row>
     <row r="442" spans="1:4" x14ac:dyDescent="0.25">
@@ -8312,13 +8315,13 @@
         <v>444</v>
       </c>
       <c r="B442" s="18">
-        <v>149</v>
+        <v>1</v>
       </c>
       <c r="C442" s="19">
-        <v>1.38</v>
+        <v>1.55</v>
       </c>
       <c r="D442" s="20">
-        <v>205.36</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="443" spans="1:4" x14ac:dyDescent="0.25">
@@ -8326,13 +8329,13 @@
         <v>445</v>
       </c>
       <c r="B443" s="18">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C443" s="19">
-        <v>1.5</v>
+        <v>1.38</v>
       </c>
       <c r="D443" s="20">
-        <v>135</v>
+        <v>198.47</v>
       </c>
     </row>
     <row r="444" spans="1:4" x14ac:dyDescent="0.25">
@@ -8340,13 +8343,13 @@
         <v>446</v>
       </c>
       <c r="B444" s="18">
-        <v>166</v>
+        <v>90</v>
       </c>
       <c r="C444" s="19">
         <v>1.5</v>
       </c>
       <c r="D444" s="20">
-        <v>249</v>
+        <v>135</v>
       </c>
     </row>
     <row r="445" spans="1:4" x14ac:dyDescent="0.25">
@@ -8354,13 +8357,13 @@
         <v>447</v>
       </c>
       <c r="B445" s="18">
-        <v>344</v>
+        <v>160</v>
       </c>
       <c r="C445" s="19">
         <v>1.5</v>
       </c>
       <c r="D445" s="20">
-        <v>516</v>
+        <v>240</v>
       </c>
     </row>
     <row r="446" spans="1:4" x14ac:dyDescent="0.25">
@@ -8368,13 +8371,13 @@
         <v>448</v>
       </c>
       <c r="B446" s="18">
-        <v>53</v>
+        <v>342.5</v>
       </c>
       <c r="C446" s="19">
-        <v>1.71</v>
+        <v>1.5</v>
       </c>
       <c r="D446" s="20">
-        <v>90.63</v>
+        <v>513.75</v>
       </c>
     </row>
     <row r="447" spans="1:4" x14ac:dyDescent="0.25">
@@ -8382,13 +8385,13 @@
         <v>449</v>
       </c>
       <c r="B447" s="18">
-        <v>128.5</v>
+        <v>53</v>
       </c>
       <c r="C447" s="19">
-        <v>0.39</v>
+        <v>1.71</v>
       </c>
       <c r="D447" s="20">
-        <v>50.34</v>
+        <v>90.63</v>
       </c>
     </row>
     <row r="448" spans="1:4" x14ac:dyDescent="0.25">
@@ -8396,13 +8399,13 @@
         <v>450</v>
       </c>
       <c r="B448" s="18">
-        <v>84.7</v>
+        <v>128.5</v>
       </c>
       <c r="C448" s="19">
-        <v>2.2799999999999998</v>
+        <v>0.39</v>
       </c>
       <c r="D448" s="20">
-        <v>193.12</v>
+        <v>50.34</v>
       </c>
     </row>
     <row r="449" spans="1:4" x14ac:dyDescent="0.25">
@@ -8410,13 +8413,13 @@
         <v>451</v>
       </c>
       <c r="B449" s="18">
-        <v>167.5</v>
+        <v>68.7</v>
       </c>
       <c r="C449" s="19">
         <v>2.2799999999999998</v>
       </c>
       <c r="D449" s="20">
-        <v>381.9</v>
+        <v>156.63999999999999</v>
       </c>
     </row>
     <row r="450" spans="1:4" x14ac:dyDescent="0.25">
@@ -8424,13 +8427,13 @@
         <v>452</v>
       </c>
       <c r="B450" s="18">
-        <v>22</v>
+        <v>160.5</v>
       </c>
       <c r="C450" s="19">
-        <v>2.4700000000000002</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D450" s="20">
-        <v>54.34</v>
+        <v>365.94</v>
       </c>
     </row>
     <row r="451" spans="1:4" x14ac:dyDescent="0.25">
@@ -8438,13 +8441,13 @@
         <v>453</v>
       </c>
       <c r="B451" s="18">
-        <v>18.5</v>
+        <v>22</v>
       </c>
       <c r="C451" s="19">
-        <v>2.75</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D451" s="20">
-        <v>50.88</v>
+        <v>54.34</v>
       </c>
     </row>
     <row r="452" spans="1:4" x14ac:dyDescent="0.25">
@@ -8452,13 +8455,13 @@
         <v>454</v>
       </c>
       <c r="B452" s="18">
-        <v>71.5</v>
+        <v>18.5</v>
       </c>
       <c r="C452" s="19">
-        <v>2.73</v>
+        <v>2.75</v>
       </c>
       <c r="D452" s="20">
-        <v>195.49</v>
+        <v>50.88</v>
       </c>
     </row>
     <row r="453" spans="1:4" x14ac:dyDescent="0.25">
@@ -8466,13 +8469,13 @@
         <v>455</v>
       </c>
       <c r="B453" s="18">
-        <v>110.5</v>
+        <v>71.5</v>
       </c>
       <c r="C453" s="19">
-        <v>2.8</v>
+        <v>2.73</v>
       </c>
       <c r="D453" s="20">
-        <v>309.39999999999998</v>
+        <v>195.49</v>
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
@@ -8480,13 +8483,13 @@
         <v>456</v>
       </c>
       <c r="B454" s="18">
-        <v>48.5</v>
+        <v>110.5</v>
       </c>
       <c r="C454" s="19">
-        <v>2.95</v>
+        <v>2.8</v>
       </c>
       <c r="D454" s="20">
-        <v>143.08000000000001</v>
+        <v>309.39999999999998</v>
       </c>
     </row>
     <row r="455" spans="1:4" x14ac:dyDescent="0.25">
@@ -8494,13 +8497,13 @@
         <v>457</v>
       </c>
       <c r="B455" s="18">
-        <v>40</v>
+        <v>48.5</v>
       </c>
       <c r="C455" s="19">
         <v>2.95</v>
       </c>
       <c r="D455" s="20">
-        <v>118</v>
+        <v>143.08000000000001</v>
       </c>
     </row>
     <row r="456" spans="1:4" x14ac:dyDescent="0.25">
@@ -8508,13 +8511,13 @@
         <v>458</v>
       </c>
       <c r="B456" s="18">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C456" s="19">
-        <v>3.5</v>
+        <v>2.95</v>
       </c>
       <c r="D456" s="20">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
     <row r="457" spans="1:4" x14ac:dyDescent="0.25">
@@ -8536,13 +8539,13 @@
         <v>460</v>
       </c>
       <c r="B458" s="18">
-        <v>57.5</v>
+        <v>30</v>
       </c>
       <c r="C458" s="19">
-        <v>3.2</v>
+        <v>3.5</v>
       </c>
       <c r="D458" s="20">
-        <v>184</v>
+        <v>105</v>
       </c>
     </row>
     <row r="459" spans="1:4" x14ac:dyDescent="0.25">
@@ -8550,13 +8553,13 @@
         <v>461</v>
       </c>
       <c r="B459" s="18">
-        <v>46</v>
+        <v>57.5</v>
       </c>
       <c r="C459" s="19">
         <v>3.2</v>
       </c>
       <c r="D459" s="20">
-        <v>147.19999999999999</v>
+        <v>184</v>
       </c>
     </row>
     <row r="460" spans="1:4" x14ac:dyDescent="0.25">
@@ -8567,10 +8570,10 @@
         <v>46</v>
       </c>
       <c r="C460" s="19">
-        <v>2.85</v>
+        <v>3.2</v>
       </c>
       <c r="D460" s="20">
-        <v>131.1</v>
+        <v>147.19999999999999</v>
       </c>
     </row>
     <row r="461" spans="1:4" x14ac:dyDescent="0.25">
@@ -8578,13 +8581,13 @@
         <v>463</v>
       </c>
       <c r="B461" s="18">
-        <v>56.5</v>
+        <v>46</v>
       </c>
       <c r="C461" s="19">
-        <v>3.25</v>
+        <v>2.85</v>
       </c>
       <c r="D461" s="20">
-        <v>183.63</v>
+        <v>131.1</v>
       </c>
     </row>
     <row r="462" spans="1:4" x14ac:dyDescent="0.25">
@@ -8592,13 +8595,13 @@
         <v>464</v>
       </c>
       <c r="B462" s="18">
-        <v>46.5</v>
+        <v>56.5</v>
       </c>
       <c r="C462" s="19">
         <v>3.25</v>
       </c>
       <c r="D462" s="20">
-        <v>151.13</v>
+        <v>183.63</v>
       </c>
     </row>
     <row r="463" spans="1:4" x14ac:dyDescent="0.25">
@@ -8606,13 +8609,13 @@
         <v>465</v>
       </c>
       <c r="B463" s="18">
-        <v>9.5</v>
+        <v>46.5</v>
       </c>
       <c r="C463" s="19">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="D463" s="20">
-        <v>33.25</v>
+        <v>151.13</v>
       </c>
     </row>
     <row r="464" spans="1:4" x14ac:dyDescent="0.25">
@@ -8620,13 +8623,13 @@
         <v>466</v>
       </c>
       <c r="B464" s="18">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C464" s="19">
         <v>3.5</v>
       </c>
       <c r="D464" s="20">
-        <v>73.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="465" spans="1:4" x14ac:dyDescent="0.25">
@@ -8634,13 +8637,13 @@
         <v>467</v>
       </c>
       <c r="B465" s="18">
-        <v>40.5</v>
+        <v>21</v>
       </c>
       <c r="C465" s="19">
-        <v>3.33</v>
+        <v>3.5</v>
       </c>
       <c r="D465" s="20">
-        <v>134.87</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="466" spans="1:4" x14ac:dyDescent="0.25">
@@ -8648,13 +8651,13 @@
         <v>468</v>
       </c>
       <c r="B466" s="18">
-        <v>50.5</v>
+        <v>38.5</v>
       </c>
       <c r="C466" s="19">
-        <v>3.8</v>
+        <v>3.33</v>
       </c>
       <c r="D466" s="20">
-        <v>191.9</v>
+        <v>128.21</v>
       </c>
     </row>
     <row r="467" spans="1:4" x14ac:dyDescent="0.25">
@@ -8662,13 +8665,13 @@
         <v>469</v>
       </c>
       <c r="B467" s="18">
-        <v>71.5</v>
+        <v>50.5</v>
       </c>
       <c r="C467" s="19">
-        <v>3.71</v>
+        <v>3.8</v>
       </c>
       <c r="D467" s="20">
-        <v>265.52</v>
+        <v>191.9</v>
       </c>
     </row>
     <row r="468" spans="1:4" x14ac:dyDescent="0.25">
@@ -8676,13 +8679,13 @@
         <v>470</v>
       </c>
       <c r="B468" s="18">
-        <v>42</v>
+        <v>71.5</v>
       </c>
       <c r="C468" s="19">
-        <v>3.6</v>
+        <v>3.71</v>
       </c>
       <c r="D468" s="20">
-        <v>151.19999999999999</v>
+        <v>265.52</v>
       </c>
     </row>
     <row r="469" spans="1:4" x14ac:dyDescent="0.25">
@@ -8690,13 +8693,13 @@
         <v>471</v>
       </c>
       <c r="B469" s="18">
-        <v>64.5</v>
+        <v>41</v>
       </c>
       <c r="C469" s="19">
         <v>3.6</v>
       </c>
       <c r="D469" s="20">
-        <v>232.2</v>
+        <v>147.6</v>
       </c>
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
@@ -8704,13 +8707,13 @@
         <v>472</v>
       </c>
       <c r="B470" s="18">
-        <v>22.5</v>
+        <v>64.5</v>
       </c>
       <c r="C470" s="19">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="D470" s="20">
-        <v>90</v>
+        <v>232.2</v>
       </c>
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
@@ -8718,13 +8721,13 @@
         <v>473</v>
       </c>
       <c r="B471" s="18">
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="C471" s="19">
         <v>4</v>
       </c>
       <c r="D471" s="20">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
@@ -8732,13 +8735,13 @@
         <v>474</v>
       </c>
       <c r="B472" s="18">
-        <v>31.5</v>
+        <v>19</v>
       </c>
       <c r="C472" s="19">
-        <v>3.85</v>
+        <v>4</v>
       </c>
       <c r="D472" s="20">
-        <v>121.28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="473" spans="1:4" x14ac:dyDescent="0.25">
@@ -8746,13 +8749,13 @@
         <v>475</v>
       </c>
       <c r="B473" s="18">
-        <v>12</v>
+        <v>31.5</v>
       </c>
       <c r="C473" s="19">
-        <v>4</v>
+        <v>3.85</v>
       </c>
       <c r="D473" s="20">
-        <v>48</v>
+        <v>121.28</v>
       </c>
     </row>
     <row r="474" spans="1:4" x14ac:dyDescent="0.25">
@@ -8760,13 +8763,13 @@
         <v>476</v>
       </c>
       <c r="B474" s="18">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C474" s="19">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="D474" s="20">
-        <v>125.4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="475" spans="1:4" x14ac:dyDescent="0.25">
@@ -8774,13 +8777,13 @@
         <v>477</v>
       </c>
       <c r="B475" s="18">
-        <v>23.5</v>
+        <v>33</v>
       </c>
       <c r="C475" s="19">
         <v>3.8</v>
       </c>
       <c r="D475" s="20">
-        <v>89.3</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="476" spans="1:4" x14ac:dyDescent="0.25">
@@ -8788,13 +8791,13 @@
         <v>478</v>
       </c>
       <c r="B476" s="18">
-        <v>42</v>
+        <v>23.5</v>
       </c>
       <c r="C476" s="19">
-        <v>4.3099999999999996</v>
+        <v>3.8</v>
       </c>
       <c r="D476" s="20">
-        <v>181.02</v>
+        <v>89.3</v>
       </c>
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
@@ -8802,13 +8805,13 @@
         <v>479</v>
       </c>
       <c r="B477" s="18">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C477" s="19">
-        <v>4.4000000000000004</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="D477" s="20">
-        <v>101.2</v>
+        <v>181.02</v>
       </c>
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
@@ -8816,13 +8819,13 @@
         <v>480</v>
       </c>
       <c r="B478" s="18">
-        <v>13.5</v>
+        <v>22</v>
       </c>
       <c r="C478" s="19">
         <v>4.4000000000000004</v>
       </c>
       <c r="D478" s="20">
-        <v>59.4</v>
+        <v>96.8</v>
       </c>
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
@@ -8830,13 +8833,13 @@
         <v>481</v>
       </c>
       <c r="B479" s="18">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="C479" s="19">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D479" s="20">
-        <v>70</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
@@ -8844,13 +8847,13 @@
         <v>482</v>
       </c>
       <c r="B480" s="18">
-        <v>5.5</v>
+        <v>14</v>
       </c>
       <c r="C480" s="19">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="D480" s="20">
-        <v>26.13</v>
+        <v>70</v>
       </c>
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
@@ -8858,13 +8861,13 @@
         <v>483</v>
       </c>
       <c r="B481" s="18">
-        <v>28</v>
+        <v>5.5</v>
       </c>
       <c r="C481" s="19">
         <v>4.75</v>
       </c>
       <c r="D481" s="20">
-        <v>133</v>
+        <v>26.13</v>
       </c>
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
@@ -8872,13 +8875,13 @@
         <v>484</v>
       </c>
       <c r="B482" s="18">
-        <v>35.5</v>
+        <v>28</v>
       </c>
       <c r="C482" s="19">
         <v>4.75</v>
       </c>
       <c r="D482" s="20">
-        <v>168.63</v>
+        <v>133</v>
       </c>
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
@@ -8886,13 +8889,13 @@
         <v>485</v>
       </c>
       <c r="B483" s="18">
-        <v>20</v>
+        <v>35.5</v>
       </c>
       <c r="C483" s="19">
         <v>4.75</v>
       </c>
       <c r="D483" s="20">
-        <v>95</v>
+        <v>168.63</v>
       </c>
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
@@ -8900,13 +8903,13 @@
         <v>486</v>
       </c>
       <c r="B484" s="18">
-        <v>10.5</v>
+        <v>20</v>
       </c>
       <c r="C484" s="19">
         <v>4.75</v>
       </c>
       <c r="D484" s="20">
-        <v>49.88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
@@ -8914,13 +8917,13 @@
         <v>487</v>
       </c>
       <c r="B485" s="18">
-        <v>45.5</v>
+        <v>10.5</v>
       </c>
       <c r="C485" s="19">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="D485" s="20">
-        <v>227.5</v>
+        <v>49.88</v>
       </c>
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
@@ -8928,13 +8931,13 @@
         <v>488</v>
       </c>
       <c r="B486" s="18">
-        <v>28.5</v>
+        <v>45.5</v>
       </c>
       <c r="C486" s="19">
         <v>5</v>
       </c>
       <c r="D486" s="20">
-        <v>142.5</v>
+        <v>227.5</v>
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
@@ -8942,13 +8945,13 @@
         <v>489</v>
       </c>
       <c r="B487" s="18">
-        <v>18</v>
+        <v>18.5</v>
       </c>
       <c r="C487" s="19">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="D487" s="20">
-        <v>94.5</v>
+        <v>92.5</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
@@ -8956,13 +8959,13 @@
         <v>490</v>
       </c>
       <c r="B488" s="18">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C488" s="19">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="D488" s="20">
-        <v>175</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
@@ -8970,13 +8973,13 @@
         <v>491</v>
       </c>
       <c r="B489" s="18">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C489" s="19">
-        <v>5.41</v>
+        <v>5</v>
       </c>
       <c r="D489" s="20">
-        <v>113.56</v>
+        <v>175</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
@@ -8984,13 +8987,13 @@
         <v>492</v>
       </c>
       <c r="B490" s="18">
-        <v>75.5</v>
+        <v>21</v>
       </c>
       <c r="C490" s="19">
-        <v>5.5</v>
+        <v>5.41</v>
       </c>
       <c r="D490" s="20">
-        <v>415.25</v>
+        <v>113.56</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
@@ -8998,13 +9001,13 @@
         <v>493</v>
       </c>
       <c r="B491" s="18">
-        <v>23.5</v>
+        <v>57.5</v>
       </c>
       <c r="C491" s="19">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c r="D491" s="20">
-        <v>135.13</v>
+        <v>316.25</v>
       </c>
     </row>
     <row r="492" spans="1:4" x14ac:dyDescent="0.25">
@@ -9012,13 +9015,13 @@
         <v>494</v>
       </c>
       <c r="B492" s="18">
-        <v>14.5</v>
+        <v>23.5</v>
       </c>
       <c r="C492" s="19">
         <v>5.75</v>
       </c>
       <c r="D492" s="20">
-        <v>83.38</v>
+        <v>135.13</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -9026,13 +9029,13 @@
         <v>495</v>
       </c>
       <c r="B493" s="18">
-        <v>53</v>
+        <v>14.5</v>
       </c>
       <c r="C493" s="19">
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="D493" s="20">
-        <v>291.5</v>
+        <v>83.38</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
@@ -9040,13 +9043,13 @@
         <v>496</v>
       </c>
       <c r="B494" s="18">
-        <v>27.5</v>
+        <v>53</v>
       </c>
       <c r="C494" s="19">
-        <v>5.75</v>
+        <v>5.5</v>
       </c>
       <c r="D494" s="20">
-        <v>158.13</v>
+        <v>291.5</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
@@ -9068,13 +9071,13 @@
         <v>498</v>
       </c>
       <c r="B496" s="18">
-        <v>47</v>
+        <v>27.5</v>
       </c>
       <c r="C496" s="19">
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="D496" s="20">
-        <v>282</v>
+        <v>158.13</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
@@ -9082,13 +9085,13 @@
         <v>499</v>
       </c>
       <c r="B497" s="18">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C497" s="19">
         <v>6</v>
       </c>
       <c r="D497" s="20">
-        <v>42</v>
+        <v>222</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
@@ -9096,13 +9099,13 @@
         <v>500</v>
       </c>
       <c r="B498" s="18">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C498" s="19">
         <v>6</v>
       </c>
       <c r="D498" s="20">
-        <v>156</v>
+        <v>42</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
@@ -9110,13 +9113,13 @@
         <v>501</v>
       </c>
       <c r="B499" s="18">
-        <v>8.5</v>
+        <v>26</v>
       </c>
       <c r="C499" s="19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D499" s="20">
-        <v>59.5</v>
+        <v>156</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
@@ -9124,13 +9127,13 @@
         <v>502</v>
       </c>
       <c r="B500" s="18">
-        <v>34</v>
+        <v>8.5</v>
       </c>
       <c r="C500" s="19">
         <v>7</v>
       </c>
       <c r="D500" s="20">
-        <v>238</v>
+        <v>59.5</v>
       </c>
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
@@ -9138,13 +9141,13 @@
         <v>503</v>
       </c>
       <c r="B501" s="18">
-        <v>17.5</v>
+        <v>34</v>
       </c>
       <c r="C501" s="19">
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="D501" s="20">
-        <v>126.88</v>
+        <v>238</v>
       </c>
     </row>
     <row r="502" spans="1:4" x14ac:dyDescent="0.25">
@@ -9152,13 +9155,13 @@
         <v>504</v>
       </c>
       <c r="B502" s="18">
-        <v>23</v>
+        <v>17.5</v>
       </c>
       <c r="C502" s="19">
-        <v>7.75</v>
+        <v>7.25</v>
       </c>
       <c r="D502" s="20">
-        <v>178.25</v>
+        <v>126.88</v>
       </c>
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
@@ -9166,13 +9169,13 @@
         <v>505</v>
       </c>
       <c r="B503" s="18">
-        <v>11.5</v>
+        <v>23</v>
       </c>
       <c r="C503" s="19">
-        <v>8</v>
+        <v>7.75</v>
       </c>
       <c r="D503" s="20">
-        <v>92</v>
+        <v>178.25</v>
       </c>
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
@@ -9180,13 +9183,13 @@
         <v>506</v>
       </c>
       <c r="B504" s="18">
-        <v>4.5</v>
+        <v>11.5</v>
       </c>
       <c r="C504" s="19">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D504" s="20">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="505" spans="1:4" x14ac:dyDescent="0.25">
@@ -9194,13 +9197,13 @@
         <v>507</v>
       </c>
       <c r="B505" s="18">
-        <v>18.5</v>
+        <v>4.5</v>
       </c>
       <c r="C505" s="19">
-        <v>8.75</v>
+        <v>10</v>
       </c>
       <c r="D505" s="20">
-        <v>161.88</v>
+        <v>45</v>
       </c>
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
@@ -9208,13 +9211,13 @@
         <v>508</v>
       </c>
       <c r="B506" s="18">
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="C506" s="19">
-        <v>11</v>
+        <v>8.75</v>
       </c>
       <c r="D506" s="20">
-        <v>181.5</v>
+        <v>161.88</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
@@ -9222,13 +9225,13 @@
         <v>509</v>
       </c>
       <c r="B507" s="18">
-        <v>64.5</v>
+        <v>16.5</v>
       </c>
       <c r="C507" s="19">
-        <v>2.76</v>
+        <v>11</v>
       </c>
       <c r="D507" s="20">
-        <v>178.02</v>
+        <v>181.5</v>
       </c>
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
@@ -9236,13 +9239,13 @@
         <v>510</v>
       </c>
       <c r="B508" s="18">
-        <v>56</v>
+        <v>69.5</v>
       </c>
       <c r="C508" s="19">
         <v>2.76</v>
       </c>
       <c r="D508" s="20">
-        <v>154.56</v>
+        <v>191.82</v>
       </c>
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
@@ -9250,13 +9253,13 @@
         <v>511</v>
       </c>
       <c r="B509" s="18">
-        <v>81.5</v>
+        <v>56</v>
       </c>
       <c r="C509" s="19">
         <v>2.76</v>
       </c>
       <c r="D509" s="20">
-        <v>224.94</v>
+        <v>154.56</v>
       </c>
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.25">
@@ -9264,13 +9267,13 @@
         <v>512</v>
       </c>
       <c r="B510" s="18">
-        <v>34</v>
+        <v>83.5</v>
       </c>
       <c r="C510" s="19">
-        <v>2.8</v>
+        <v>2.76</v>
       </c>
       <c r="D510" s="20">
-        <v>95.2</v>
+        <v>230.46</v>
       </c>
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
@@ -9278,13 +9281,13 @@
         <v>513</v>
       </c>
       <c r="B511" s="18">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C511" s="19">
-        <v>2.87</v>
+        <v>2.8</v>
       </c>
       <c r="D511" s="20">
-        <v>134.97999999999999</v>
+        <v>95.2</v>
       </c>
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
@@ -9292,13 +9295,13 @@
         <v>514</v>
       </c>
       <c r="B512" s="18">
-        <v>40.5</v>
+        <v>47</v>
       </c>
       <c r="C512" s="19">
-        <v>2.76</v>
+        <v>2.87</v>
       </c>
       <c r="D512" s="20">
-        <v>111.78</v>
+        <v>134.97999999999999</v>
       </c>
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
@@ -9306,13 +9309,13 @@
         <v>515</v>
       </c>
       <c r="B513" s="18">
-        <v>21</v>
+        <v>40.5</v>
       </c>
       <c r="C513" s="19">
         <v>2.76</v>
       </c>
       <c r="D513" s="20">
-        <v>57.96</v>
+        <v>111.78</v>
       </c>
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
@@ -9320,13 +9323,13 @@
         <v>516</v>
       </c>
       <c r="B514" s="18">
-        <v>35.5</v>
+        <v>21</v>
       </c>
       <c r="C514" s="19">
         <v>2.76</v>
       </c>
       <c r="D514" s="20">
-        <v>97.98</v>
+        <v>57.96</v>
       </c>
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
@@ -9334,13 +9337,13 @@
         <v>517</v>
       </c>
       <c r="B515" s="18">
-        <v>30</v>
+        <v>35.5</v>
       </c>
       <c r="C515" s="19">
-        <v>3.5</v>
+        <v>2.76</v>
       </c>
       <c r="D515" s="20">
-        <v>105</v>
+        <v>97.98</v>
       </c>
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
@@ -9348,13 +9351,13 @@
         <v>518</v>
       </c>
       <c r="B516" s="18">
-        <v>41.5</v>
+        <v>30</v>
       </c>
       <c r="C516" s="19">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D516" s="20">
-        <v>124.5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
@@ -9362,13 +9365,13 @@
         <v>519</v>
       </c>
       <c r="B517" s="18">
-        <v>62.5</v>
+        <v>41.5</v>
       </c>
       <c r="C517" s="19">
         <v>3</v>
       </c>
       <c r="D517" s="20">
-        <v>187.5</v>
+        <v>124.5</v>
       </c>
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.25">
@@ -9376,13 +9379,13 @@
         <v>520</v>
       </c>
       <c r="B518" s="18">
-        <v>23.5</v>
+        <v>62.5</v>
       </c>
       <c r="C518" s="19">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="D518" s="20">
-        <v>72.849999999999994</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
@@ -9390,13 +9393,13 @@
         <v>521</v>
       </c>
       <c r="B519" s="18">
-        <v>7</v>
+        <v>23.5</v>
       </c>
       <c r="C519" s="19">
-        <v>6</v>
+        <v>3.1</v>
       </c>
       <c r="D519" s="20">
-        <v>42</v>
+        <v>72.849999999999994</v>
       </c>
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
@@ -9404,13 +9407,13 @@
         <v>522</v>
       </c>
       <c r="B520" s="18">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C520" s="19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D520" s="20">
-        <v>148</v>
+        <v>42</v>
       </c>
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
@@ -9418,13 +9421,13 @@
         <v>523</v>
       </c>
       <c r="B521" s="18">
-        <v>23.5</v>
+        <v>37</v>
       </c>
       <c r="C521" s="19">
         <v>4</v>
       </c>
       <c r="D521" s="20">
-        <v>94</v>
+        <v>148</v>
       </c>
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
@@ -9432,13 +9435,13 @@
         <v>524</v>
       </c>
       <c r="B522" s="18">
-        <v>24</v>
+        <v>23.5</v>
       </c>
       <c r="C522" s="19">
         <v>4</v>
       </c>
       <c r="D522" s="20">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
@@ -9446,13 +9449,13 @@
         <v>525</v>
       </c>
       <c r="B523" s="18">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C523" s="19">
         <v>4</v>
       </c>
       <c r="D523" s="20">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
@@ -9460,13 +9463,13 @@
         <v>526</v>
       </c>
       <c r="B524" s="18">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C524" s="19">
-        <v>5.25</v>
+        <v>4</v>
       </c>
       <c r="D524" s="20">
-        <v>215.25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
@@ -9474,13 +9477,13 @@
         <v>527</v>
       </c>
       <c r="B525" s="18">
-        <v>18.5</v>
+        <v>41</v>
       </c>
       <c r="C525" s="19">
-        <v>5.01</v>
+        <v>5.25</v>
       </c>
       <c r="D525" s="20">
-        <v>92.77</v>
+        <v>215.25</v>
       </c>
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
@@ -9488,13 +9491,13 @@
         <v>528</v>
       </c>
       <c r="B526" s="18">
-        <v>238</v>
+        <v>18.5</v>
       </c>
       <c r="C526" s="19">
-        <v>1.92</v>
+        <v>5.01</v>
       </c>
       <c r="D526" s="20">
-        <v>457.07</v>
+        <v>92.77</v>
       </c>
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
@@ -9502,13 +9505,13 @@
         <v>529</v>
       </c>
       <c r="B527" s="18">
-        <v>-4.5</v>
+        <v>238</v>
       </c>
       <c r="C527" s="19">
-        <v>1.96</v>
+        <v>1.92</v>
       </c>
       <c r="D527" s="20">
-        <v>-8.83</v>
+        <v>457.07</v>
       </c>
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
@@ -9516,13 +9519,13 @@
         <v>530</v>
       </c>
       <c r="B528" s="18">
-        <v>231.5</v>
+        <v>-8.5</v>
       </c>
       <c r="C528" s="19">
-        <v>1.93</v>
+        <v>1.96</v>
       </c>
       <c r="D528" s="20">
-        <v>446.71</v>
+        <v>-16.670000000000002</v>
       </c>
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
@@ -9530,13 +9533,13 @@
         <v>531</v>
       </c>
       <c r="B529" s="18">
-        <v>91.5</v>
+        <v>231.5</v>
       </c>
       <c r="C529" s="19">
-        <v>2.84</v>
+        <v>1.93</v>
       </c>
       <c r="D529" s="20">
-        <v>259.66000000000003</v>
+        <v>446.71</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
@@ -9544,13 +9547,13 @@
         <v>532</v>
       </c>
       <c r="B530" s="18">
-        <v>0.5</v>
+        <v>87</v>
       </c>
       <c r="C530" s="19">
-        <v>4.28</v>
+        <v>2.84</v>
       </c>
       <c r="D530" s="20">
-        <v>2.14</v>
+        <v>246.89</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
@@ -9558,13 +9561,13 @@
         <v>533</v>
       </c>
       <c r="B531" s="18">
-        <v>27.5</v>
+        <v>0.5</v>
       </c>
       <c r="C531" s="19">
         <v>4.28</v>
       </c>
       <c r="D531" s="20">
-        <v>117.7</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
@@ -9572,13 +9575,13 @@
         <v>534</v>
       </c>
       <c r="B532" s="18">
-        <v>43.5</v>
+        <v>27.5</v>
       </c>
       <c r="C532" s="19">
-        <v>4.05</v>
+        <v>4.28</v>
       </c>
       <c r="D532" s="20">
-        <v>176.18</v>
+        <v>117.7</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
@@ -9586,13 +9589,13 @@
         <v>535</v>
       </c>
       <c r="B533" s="18">
-        <v>59.5</v>
+        <v>43.5</v>
       </c>
       <c r="C533" s="19">
         <v>4.05</v>
       </c>
       <c r="D533" s="20">
-        <v>240.98</v>
+        <v>176.18</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
@@ -9600,13 +9603,13 @@
         <v>536</v>
       </c>
       <c r="B534" s="18">
-        <v>113</v>
+        <v>59.5</v>
       </c>
       <c r="C534" s="19">
-        <v>1.39</v>
+        <v>4.05</v>
       </c>
       <c r="D534" s="20">
-        <v>157.31</v>
+        <v>240.98</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
@@ -9614,13 +9617,13 @@
         <v>537</v>
       </c>
       <c r="B535" s="18">
-        <v>348</v>
+        <v>113</v>
       </c>
       <c r="C535" s="19">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="D535" s="20">
-        <v>487.2</v>
+        <v>157.31</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
@@ -9628,13 +9631,13 @@
         <v>538</v>
       </c>
       <c r="B536" s="18">
-        <v>58</v>
+        <v>346</v>
       </c>
       <c r="C536" s="19">
         <v>1.4</v>
       </c>
       <c r="D536" s="20">
-        <v>81.2</v>
+        <v>484.4</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
@@ -9642,17 +9645,21 @@
         <v>539</v>
       </c>
       <c r="B537" s="18">
-        <v>48.5</v>
-      </c>
-      <c r="C537" s="21"/>
-      <c r="D537" s="22"/>
+        <v>58</v>
+      </c>
+      <c r="C537" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="D537" s="20">
+        <v>81.2</v>
+      </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" s="17" t="s">
         <v>540</v>
       </c>
       <c r="B538" s="18">
-        <v>18</v>
+        <v>47.5</v>
       </c>
       <c r="C538" s="21"/>
       <c r="D538" s="22"/>
@@ -9662,7 +9669,7 @@
         <v>541</v>
       </c>
       <c r="B539" s="18">
-        <v>47.5</v>
+        <v>18</v>
       </c>
       <c r="C539" s="21"/>
       <c r="D539" s="22"/>
@@ -9672,7 +9679,7 @@
         <v>542</v>
       </c>
       <c r="B540" s="18">
-        <v>34.299999999999997</v>
+        <v>47.5</v>
       </c>
       <c r="C540" s="21"/>
       <c r="D540" s="22"/>
@@ -9682,7 +9689,7 @@
         <v>543</v>
       </c>
       <c r="B541" s="18">
-        <v>470</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="C541" s="21"/>
       <c r="D541" s="22"/>
@@ -9692,27 +9699,23 @@
         <v>544</v>
       </c>
       <c r="B542" s="18">
-        <v>1705.5</v>
-      </c>
-      <c r="C542" s="19">
-        <v>0.83</v>
-      </c>
-      <c r="D542" s="20">
-        <v>1407.04</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="C542" s="21"/>
+      <c r="D542" s="22"/>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A543" s="17" t="s">
         <v>545</v>
       </c>
       <c r="B543" s="18">
-        <v>546</v>
+        <v>1705.5</v>
       </c>
       <c r="C543" s="19">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="D543" s="20">
-        <v>436.8</v>
+        <v>1407.04</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
@@ -9720,13 +9723,13 @@
         <v>546</v>
       </c>
       <c r="B544" s="18">
-        <v>661</v>
+        <v>543</v>
       </c>
       <c r="C544" s="19">
         <v>0.8</v>
       </c>
       <c r="D544" s="20">
-        <v>528.79999999999995</v>
+        <v>434.4</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
@@ -9734,13 +9737,13 @@
         <v>547</v>
       </c>
       <c r="B545" s="18">
-        <v>372.5</v>
+        <v>655</v>
       </c>
       <c r="C545" s="19">
         <v>0.8</v>
       </c>
       <c r="D545" s="20">
-        <v>298</v>
+        <v>524</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
@@ -9748,13 +9751,13 @@
         <v>548</v>
       </c>
       <c r="B546" s="18">
-        <v>32</v>
+        <v>366.5</v>
       </c>
       <c r="C546" s="19">
-        <v>0.52</v>
+        <v>0.8</v>
       </c>
       <c r="D546" s="20">
-        <v>16.64</v>
+        <v>293.2</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
@@ -9762,13 +9765,13 @@
         <v>549</v>
       </c>
       <c r="B547" s="18">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C547" s="19">
         <v>0.52</v>
       </c>
       <c r="D547" s="20">
-        <v>7.8</v>
+        <v>8.32</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
@@ -9776,13 +9779,13 @@
         <v>550</v>
       </c>
       <c r="B548" s="18">
-        <v>667</v>
+        <v>-1</v>
       </c>
       <c r="C548" s="19">
         <v>0.52</v>
       </c>
       <c r="D548" s="20">
-        <v>346.84</v>
+        <v>-0.52</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
@@ -9790,13 +9793,13 @@
         <v>551</v>
       </c>
       <c r="B549" s="18">
-        <v>858</v>
+        <v>632.5</v>
       </c>
       <c r="C549" s="19">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="D549" s="20">
-        <v>600.6</v>
+        <v>328.9</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
@@ -9804,13 +9807,13 @@
         <v>552</v>
       </c>
       <c r="B550" s="18">
-        <v>209</v>
+        <v>845</v>
       </c>
       <c r="C550" s="19">
         <v>0.7</v>
       </c>
       <c r="D550" s="20">
-        <v>146.30000000000001</v>
+        <v>591.5</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
@@ -9818,13 +9821,13 @@
         <v>553</v>
       </c>
       <c r="B551" s="18">
-        <v>306.5</v>
+        <v>192</v>
       </c>
       <c r="C551" s="19">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
       <c r="D551" s="20">
-        <v>209.04</v>
+        <v>134.4</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
@@ -9832,17 +9835,21 @@
         <v>554</v>
       </c>
       <c r="B552" s="18">
-        <v>227</v>
-      </c>
-      <c r="C552" s="21"/>
-      <c r="D552" s="22"/>
+        <v>305.5</v>
+      </c>
+      <c r="C552" s="19">
+        <v>0.68</v>
+      </c>
+      <c r="D552" s="20">
+        <v>208.35</v>
+      </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A553" s="17" t="s">
         <v>555</v>
       </c>
       <c r="B553" s="18">
-        <v>147</v>
+        <v>227</v>
       </c>
       <c r="C553" s="21"/>
       <c r="D553" s="22"/>
@@ -9852,27 +9859,23 @@
         <v>556</v>
       </c>
       <c r="B554" s="18">
-        <v>1</v>
-      </c>
-      <c r="C554" s="19">
-        <v>4.5</v>
-      </c>
-      <c r="D554" s="20">
-        <v>4.5</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C554" s="21"/>
+      <c r="D554" s="22"/>
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A555" s="17" t="s">
         <v>557</v>
       </c>
       <c r="B555" s="18">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C555" s="19">
         <v>4.5</v>
       </c>
       <c r="D555" s="20">
-        <v>184.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="556" spans="1:4" x14ac:dyDescent="0.25">
@@ -9880,13 +9883,13 @@
         <v>558</v>
       </c>
       <c r="B556" s="18">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C556" s="19">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="D556" s="20">
-        <v>21</v>
+        <v>184.5</v>
       </c>
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.25">
@@ -9894,25 +9897,39 @@
         <v>559</v>
       </c>
       <c r="B557" s="18">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C557" s="19">
         <v>3</v>
       </c>
       <c r="D557" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A558" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="B558" s="18">
+        <v>3</v>
+      </c>
+      <c r="C558" s="19">
+        <v>3</v>
+      </c>
+      <c r="D558" s="20">
         <v>9</v>
       </c>
     </row>
-    <row r="558" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A558" s="23" t="s">
-        <v>560</v>
-      </c>
-      <c r="B558" s="24">
-        <v>38484.25</v>
-      </c>
-      <c r="C558" s="25"/>
-      <c r="D558" s="26">
-        <v>107936.78</v>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A559" s="23" t="s">
+        <v>561</v>
+      </c>
+      <c r="B559" s="24">
+        <v>37845.75</v>
+      </c>
+      <c r="C559" s="25"/>
+      <c r="D559" s="26">
+        <v>105638.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:58
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 6-Jan-2025</t>
+    <t>1-Jul-2024 to 8-Jan-2025</t>
   </si>
   <si>
     <t/>
@@ -1877,7 +1877,7 @@
     <t>9205 CARD (RED)</t>
   </si>
   <si>
-    <t>9206 CARD (YELLOW) (07.01)</t>
+    <t>9206 CARD (YELLOW)</t>
   </si>
   <si>
     <t>9207 CARD (GOLDEN)</t>
@@ -2539,16 +2539,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="23">
-        <v>672.5</v>
+        <v>669.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>672.5</v>
+        <v>669.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2556,16 +2556,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="23">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
       </c>
       <c r="E10" s="25">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,16 +2590,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="23">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>287.10000000000002</v>
+        <v>273.89999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,16 +2607,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C13" s="23">
-        <v>158.5</v>
+        <v>155</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>261.52999999999997</v>
+        <v>255.75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2624,16 +2624,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="23">
-        <v>36.5</v>
+        <v>34.5</v>
       </c>
       <c r="D14" s="24">
         <v>1.8</v>
       </c>
       <c r="E14" s="25">
-        <v>65.7</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,16 +2675,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="23">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2692,16 +2692,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C18" s="23">
-        <v>55.5</v>
+        <v>48.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,16 +2726,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C20" s="23">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2743,16 +2743,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="23">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
       </c>
       <c r="E21" s="25">
-        <v>206</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2777,16 +2777,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C23" s="23">
-        <v>108.5</v>
+        <v>96.5</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>217</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,16 +2837,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C27" s="23">
-        <v>40.82</v>
+        <v>36.82</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>95.93</v>
+        <v>86.53</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2854,16 +2854,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C28" s="23">
-        <v>35.369999999999997</v>
+        <v>33.369999999999997</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>83.12</v>
+        <v>78.42</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2914,16 +2914,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="23">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>302.5</v>
+        <v>277.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2942,16 +2942,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" s="23">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2985,16 +2985,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C37" s="23">
-        <v>35.5</v>
+        <v>34</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>92.3</v>
+        <v>88.4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3019,16 +3019,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C39" s="23">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>216</v>
+        <v>194.4</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3085,16 +3085,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C43" s="23">
-        <v>39.5</v>
+        <v>37.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>88.88</v>
+        <v>84.38</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3102,16 +3102,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C44" s="23">
-        <v>122.5</v>
+        <v>117.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>275.63</v>
+        <v>264.38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3136,16 +3136,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C46" s="23">
-        <v>143.5</v>
+        <v>141.5</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>337.23</v>
+        <v>332.53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3153,16 +3153,16 @@
         <v>51</v>
       </c>
       <c r="B47" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C47" s="23">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D47" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E47" s="25">
-        <v>96.8</v>
+        <v>94.6</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3187,16 +3187,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C49" s="23">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D49" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>67.099999999999994</v>
+        <v>58.3</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3204,16 +3204,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C50" s="23">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D50" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>169.4</v>
+        <v>160.6</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3238,16 +3238,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C52" s="23">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="D52" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>162.80000000000001</v>
+        <v>144.1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3255,16 +3255,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" s="23">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D53" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E53" s="25">
-        <v>239.8</v>
+        <v>235.4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,16 +3272,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C54" s="23">
-        <v>71.5</v>
+        <v>63.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>78.650000000000006</v>
+        <v>69.849999999999994</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3306,16 +3306,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C56" s="23">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>185.9</v>
+        <v>181.5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3323,16 +3323,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C57" s="23">
-        <v>531.5</v>
+        <v>524</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>1009.85</v>
+        <v>995.6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3372,16 +3372,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C60" s="23">
-        <v>427.5</v>
+        <v>420.5</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>812.25</v>
+        <v>798.95</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3389,16 +3389,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C61" s="23">
-        <v>26.5</v>
+        <v>22.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>55.65</v>
+        <v>47.25</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3438,16 +3438,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C64" s="23">
-        <v>314.5</v>
+        <v>310.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>660.45</v>
+        <v>652.04999999999995</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3455,16 +3455,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C65" s="23">
-        <v>426.5</v>
+        <v>424.5</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>895.65</v>
+        <v>891.45</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3472,16 +3472,16 @@
         <v>70</v>
       </c>
       <c r="B66" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C66" s="23">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D66" s="24">
         <v>0.52</v>
       </c>
       <c r="E66" s="25">
-        <v>123.76</v>
+        <v>122.2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3489,16 +3489,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C67" s="23">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>105.04</v>
+        <v>101.4</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3506,16 +3506,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C68" s="23">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>124.6</v>
+        <v>121.8</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3523,16 +3523,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C69" s="23">
-        <v>152.5</v>
+        <v>136.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>106.75</v>
+        <v>95.55</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3540,16 +3540,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C70" s="23">
-        <v>285.5</v>
+        <v>278.5</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>256.95</v>
+        <v>250.65</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3557,16 +3557,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C71" s="23">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>280.8</v>
+        <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3574,16 +3574,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C72" s="23">
-        <v>196.5</v>
+        <v>192.5</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>304.58</v>
+        <v>298.38</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3591,16 +3591,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C73" s="23">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>480.5</v>
+        <v>474.3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3608,16 +3608,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C74" s="23">
-        <v>544</v>
+        <v>525</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>843.2</v>
+        <v>813.75</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,10 +3636,10 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C76" s="23">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D76" s="27"/>
       <c r="E76" s="26"/>
@@ -3662,10 +3662,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C78" s="23">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3688,10 +3688,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C80" s="23">
-        <v>284.5</v>
+        <v>224.5</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3701,10 +3701,10 @@
         <v>85</v>
       </c>
       <c r="B81" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C81" s="23">
-        <v>135.5</v>
+        <v>125.5</v>
       </c>
       <c r="D81" s="27"/>
       <c r="E81" s="26"/>
@@ -3727,16 +3727,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C83" s="23">
-        <v>403</v>
+        <v>378.5</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>463.45</v>
+        <v>435.28</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3744,16 +3744,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C84" s="23">
-        <v>350.5</v>
+        <v>332.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>403.08</v>
+        <v>382.38</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3761,16 +3761,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C85" s="23">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>578.20000000000005</v>
+        <v>565.6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3778,16 +3778,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C86" s="23">
-        <v>68.5</v>
+        <v>253.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>95.9</v>
+        <v>354.9</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3821,16 +3821,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C89" s="23">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>102</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3838,16 +3838,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C90" s="23">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>330</v>
+        <v>302</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3855,16 +3855,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C91" s="23">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>507.78</v>
+        <v>497.7</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3872,16 +3872,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C92" s="23">
-        <v>373.5</v>
+        <v>370.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>470.61</v>
+        <v>466.83</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4029,10 +4029,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C103" s="23">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4060,10 +4060,10 @@
         <v>110</v>
       </c>
       <c r="B106" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C106" s="23">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D106" s="27"/>
       <c r="E106" s="26"/>
@@ -4081,9 +4081,11 @@
       <c r="A108" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="22"/>
+      <c r="B108" s="22">
+        <v>1</v>
+      </c>
       <c r="C108" s="23">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D108" s="27"/>
       <c r="E108" s="26"/>
@@ -4125,16 +4127,16 @@
         <v>115</v>
       </c>
       <c r="B111" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C111" s="23">
-        <v>14.5</v>
+        <v>14</v>
       </c>
       <c r="D111" s="24">
         <v>12.5</v>
       </c>
       <c r="E111" s="25">
-        <v>181.25</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4142,16 +4144,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C112" s="23">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>225</v>
+        <v>675</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4159,16 +4161,16 @@
         <v>117</v>
       </c>
       <c r="B113" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C113" s="23">
-        <v>36.5</v>
+        <v>35</v>
       </c>
       <c r="D113" s="24">
         <v>12.5</v>
       </c>
       <c r="E113" s="25">
-        <v>456.25</v>
+        <v>437.5</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4176,16 +4178,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C114" s="23">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>137.5</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4311,15 +4313,17 @@
       <c r="A122" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B122" s="22"/>
+      <c r="B122" s="22">
+        <v>1</v>
+      </c>
       <c r="C122" s="23">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D122" s="24">
         <v>15.5</v>
       </c>
       <c r="E122" s="25">
-        <v>325.5</v>
+        <v>279</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4378,16 +4382,16 @@
         <v>130</v>
       </c>
       <c r="B126" s="22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C126" s="23">
-        <v>15.5</v>
+        <v>18.5</v>
       </c>
       <c r="D126" s="24">
         <v>15.5</v>
       </c>
       <c r="E126" s="25">
-        <v>240.25</v>
+        <v>286.75</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4559,16 +4563,16 @@
         <v>141</v>
       </c>
       <c r="B137" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C137" s="23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D137" s="24">
         <v>18.45</v>
       </c>
       <c r="E137" s="25">
-        <v>313.62</v>
+        <v>295.17</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4678,16 +4682,16 @@
         <v>148</v>
       </c>
       <c r="B144" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C144" s="23">
-        <v>13.5</v>
+        <v>12.5</v>
       </c>
       <c r="D144" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E144" s="25">
-        <v>248.89</v>
+        <v>230.45</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4695,17 +4699,11 @@
         <v>149</v>
       </c>
       <c r="B145" s="22">
-        <v>9</v>
-      </c>
-      <c r="C145" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="D145" s="24">
-        <v>18.36</v>
-      </c>
-      <c r="E145" s="25">
-        <v>9.18</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C145" s="26"/>
+      <c r="D145" s="27"/>
+      <c r="E145" s="26"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="21" t="s">
@@ -4763,16 +4761,16 @@
         <v>153</v>
       </c>
       <c r="B149" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C149" s="23">
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="D149" s="24">
         <v>3.3</v>
       </c>
       <c r="E149" s="25">
-        <v>136.94999999999999</v>
+        <v>130.35</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4780,16 +4778,16 @@
         <v>154</v>
       </c>
       <c r="B150" s="22">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C150" s="23">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D150" s="24">
         <v>2.8</v>
       </c>
       <c r="E150" s="25">
-        <v>291.2</v>
+        <v>277.2</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4797,16 +4795,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C151" s="23">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D151" s="24">
         <v>2.75</v>
       </c>
       <c r="E151" s="25">
-        <v>264</v>
+        <v>239.25</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4814,16 +4812,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C152" s="23">
-        <v>72.5</v>
+        <v>62.5</v>
       </c>
       <c r="D152" s="24">
         <v>2.75</v>
       </c>
       <c r="E152" s="25">
-        <v>199.38</v>
+        <v>171.88</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4831,16 +4829,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C153" s="23">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D153" s="24">
         <v>4.7</v>
       </c>
       <c r="E153" s="25">
-        <v>122.2</v>
+        <v>112.8</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4848,16 +4846,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C154" s="23">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D154" s="24">
         <v>3.4</v>
       </c>
       <c r="E154" s="25">
-        <v>153</v>
+        <v>241.4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4882,16 +4880,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C156" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D156" s="24">
         <v>2.7</v>
       </c>
       <c r="E156" s="25">
-        <v>13.5</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4933,16 +4931,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C159" s="23">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D159" s="24">
         <v>2.5</v>
       </c>
       <c r="E159" s="25">
-        <v>242.5</v>
+        <v>217.5</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -5001,16 +4999,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C163" s="23">
-        <v>70.5</v>
+        <v>63.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.95</v>
       </c>
       <c r="E163" s="25">
-        <v>207.98</v>
+        <v>187.33</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5018,16 +5016,16 @@
         <v>168</v>
       </c>
       <c r="B164" s="22">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C164" s="23">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D164" s="24">
         <v>2.95</v>
       </c>
       <c r="E164" s="25">
-        <v>97.35</v>
+        <v>85.55</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5035,16 +5033,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C165" s="23">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D165" s="24">
         <v>3</v>
       </c>
       <c r="E165" s="25">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5052,16 +5050,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C166" s="23">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D166" s="24">
         <v>3</v>
       </c>
       <c r="E166" s="25">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5069,16 +5067,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C167" s="23">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D167" s="24">
         <v>3.3</v>
       </c>
       <c r="E167" s="25">
-        <v>363</v>
+        <v>359.7</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5103,16 +5101,16 @@
         <v>173</v>
       </c>
       <c r="B169" s="22">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C169" s="23">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D169" s="24">
         <v>3.5</v>
       </c>
       <c r="E169" s="25">
-        <v>245</v>
+        <v>213.5</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5129,16 +5127,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C171" s="23">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D171" s="24">
         <v>3.9</v>
       </c>
       <c r="E171" s="25">
-        <v>249.6</v>
+        <v>241.8</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5229,16 +5227,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C177" s="23">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D177" s="24">
         <v>3.6</v>
       </c>
       <c r="E177" s="25">
-        <v>446.4</v>
+        <v>439.2</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5306,16 +5304,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C182" s="23">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D182" s="24">
         <v>4.5</v>
       </c>
       <c r="E182" s="25">
-        <v>450</v>
+        <v>432</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5372,16 +5370,16 @@
         <v>190</v>
       </c>
       <c r="B186" s="22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C186" s="23">
-        <v>20.5</v>
+        <v>8</v>
       </c>
       <c r="D186" s="24">
         <v>4.5</v>
       </c>
       <c r="E186" s="25">
-        <v>92.25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5389,16 +5387,16 @@
         <v>191</v>
       </c>
       <c r="B187" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C187" s="23">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D187" s="24">
         <v>4.5</v>
       </c>
       <c r="E187" s="25">
-        <v>576</v>
+        <v>553.5</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5406,16 +5404,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C188" s="23">
-        <v>115</v>
+        <v>114.5</v>
       </c>
       <c r="D188" s="24">
         <v>3.93</v>
       </c>
       <c r="E188" s="25">
-        <v>451.96</v>
+        <v>450</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5423,16 +5421,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C189" s="23">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D189" s="24">
         <v>3.96</v>
       </c>
       <c r="E189" s="25">
-        <v>466.95</v>
+        <v>459.04</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5556,16 +5554,16 @@
         <v>202</v>
       </c>
       <c r="B198" s="22">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C198" s="23">
-        <v>62.74</v>
+        <v>34.24</v>
       </c>
       <c r="D198" s="24">
         <v>3.11</v>
       </c>
       <c r="E198" s="25">
-        <v>194.89</v>
+        <v>106.36</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5582,16 +5580,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C200" s="23">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D200" s="24">
         <v>3.26</v>
       </c>
       <c r="E200" s="25">
-        <v>4.8899999999999997</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5675,16 +5673,16 @@
         <v>211</v>
       </c>
       <c r="B207" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C207" s="23">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D207" s="24">
         <v>3.8</v>
       </c>
       <c r="E207" s="25">
-        <v>300.2</v>
+        <v>296.39999999999998</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5748,16 +5746,16 @@
         <v>216</v>
       </c>
       <c r="B212" s="22">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C212" s="23">
-        <v>34.5</v>
+        <v>15</v>
       </c>
       <c r="D212" s="24">
         <v>4.12</v>
       </c>
       <c r="E212" s="25">
-        <v>142.03</v>
+        <v>61.75</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -5799,16 +5797,16 @@
         <v>219</v>
       </c>
       <c r="B215" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C215" s="23">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D215" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E215" s="25">
-        <v>127.6</v>
+        <v>105.6</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5878,16 +5876,16 @@
         <v>224</v>
       </c>
       <c r="B220" s="22">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C220" s="23">
-        <v>199.5</v>
+        <v>196</v>
       </c>
       <c r="D220" s="24">
         <v>4.5</v>
       </c>
       <c r="E220" s="25">
-        <v>897.75</v>
+        <v>882</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -5895,16 +5893,16 @@
         <v>225</v>
       </c>
       <c r="B221" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C221" s="23">
-        <v>161.5</v>
+        <v>153.5</v>
       </c>
       <c r="D221" s="24">
         <v>4.5</v>
       </c>
       <c r="E221" s="25">
-        <v>726.75</v>
+        <v>690.75</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -5912,16 +5910,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C222" s="23">
-        <v>53.5</v>
+        <v>35</v>
       </c>
       <c r="D222" s="24">
         <v>5.25</v>
       </c>
       <c r="E222" s="25">
-        <v>280.88</v>
+        <v>183.75</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6046,16 +6044,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C230" s="23">
-        <v>39.5</v>
+        <v>38.5</v>
       </c>
       <c r="D230" s="24">
         <v>4.75</v>
       </c>
       <c r="E230" s="25">
-        <v>187.63</v>
+        <v>182.88</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6160,16 +6158,16 @@
         <v>242</v>
       </c>
       <c r="B238" s="22">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C238" s="23">
-        <v>41</v>
+        <v>39.5</v>
       </c>
       <c r="D238" s="24">
         <v>5.7</v>
       </c>
       <c r="E238" s="25">
-        <v>233.7</v>
+        <v>225.15</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -6209,16 +6207,16 @@
         <v>245</v>
       </c>
       <c r="B241" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C241" s="23">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D241" s="24">
         <v>6.75</v>
       </c>
       <c r="E241" s="25">
-        <v>499.5</v>
+        <v>479.25</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6226,16 +6224,16 @@
         <v>246</v>
       </c>
       <c r="B242" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C242" s="23">
-        <v>136</v>
+        <v>219</v>
       </c>
       <c r="D242" s="24">
-        <v>5.97</v>
+        <v>5.98</v>
       </c>
       <c r="E242" s="25">
-        <v>812.59</v>
+        <v>1309.6500000000001</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6243,16 +6241,16 @@
         <v>247</v>
       </c>
       <c r="B243" s="22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C243" s="23">
-        <v>37.5</v>
+        <v>40</v>
       </c>
       <c r="D243" s="24">
         <v>4.26</v>
       </c>
       <c r="E243" s="25">
-        <v>159.75</v>
+        <v>170.4</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6260,16 +6258,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C244" s="23">
-        <v>112.5</v>
+        <v>103</v>
       </c>
       <c r="D244" s="24">
         <v>4</v>
       </c>
       <c r="E244" s="25">
-        <v>450</v>
+        <v>412</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6294,16 +6292,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C246" s="23">
-        <v>78</v>
+        <v>76.5</v>
       </c>
       <c r="D246" s="24">
         <v>4.5</v>
       </c>
       <c r="E246" s="25">
-        <v>351</v>
+        <v>344.25</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6326,16 +6324,16 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C248" s="23">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D248" s="24">
         <v>5</v>
       </c>
       <c r="E248" s="25">
-        <v>72.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6343,16 +6341,16 @@
         <v>253</v>
       </c>
       <c r="B249" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C249" s="23">
-        <v>18.5</v>
+        <v>8.5</v>
       </c>
       <c r="D249" s="24">
         <v>3.8</v>
       </c>
       <c r="E249" s="25">
-        <v>70.3</v>
+        <v>32.299999999999997</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6382,16 +6380,16 @@
         <v>256</v>
       </c>
       <c r="B252" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C252" s="23">
-        <v>155.5</v>
+        <v>152.5</v>
       </c>
       <c r="D252" s="24">
         <v>4.25</v>
       </c>
       <c r="E252" s="25">
-        <v>660.88</v>
+        <v>648.13</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6459,16 +6457,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C257" s="23">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D257" s="24">
         <v>4.28</v>
       </c>
       <c r="E257" s="25">
-        <v>312.44</v>
+        <v>299.60000000000002</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6544,16 +6542,16 @@
         <v>266</v>
       </c>
       <c r="B262" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C262" s="23">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="D262" s="24">
         <v>4.75</v>
       </c>
       <c r="E262" s="25">
-        <v>92.63</v>
+        <v>87.88</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6630,16 +6628,16 @@
         <v>272</v>
       </c>
       <c r="B268" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C268" s="23">
-        <v>115.5</v>
+        <v>114.5</v>
       </c>
       <c r="D268" s="24">
         <v>5.4</v>
       </c>
       <c r="E268" s="25">
-        <v>623.70000000000005</v>
+        <v>618.29999999999995</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6698,16 +6696,16 @@
         <v>276</v>
       </c>
       <c r="B272" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C272" s="23">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D272" s="24">
         <v>5.23</v>
       </c>
       <c r="E272" s="25">
-        <v>88.91</v>
+        <v>78.45</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6741,16 +6739,16 @@
         <v>279</v>
       </c>
       <c r="B275" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C275" s="23">
-        <v>15.5</v>
+        <v>14</v>
       </c>
       <c r="D275" s="24">
         <v>6.25</v>
       </c>
       <c r="E275" s="25">
-        <v>96.88</v>
+        <v>87.5</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -6843,16 +6841,16 @@
         <v>285</v>
       </c>
       <c r="B281" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C281" s="23">
-        <v>20.5</v>
+        <v>19.5</v>
       </c>
       <c r="D281" s="24">
         <v>5.7</v>
       </c>
       <c r="E281" s="25">
-        <v>116.85</v>
+        <v>111.15</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6860,16 +6858,16 @@
         <v>286</v>
       </c>
       <c r="B282" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C282" s="23">
-        <v>80.5</v>
+        <v>78</v>
       </c>
       <c r="D282" s="24">
         <v>5.94</v>
       </c>
       <c r="E282" s="25">
-        <v>478.17</v>
+        <v>463.32</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6877,16 +6875,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C283" s="23">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D283" s="24">
         <v>5.94</v>
       </c>
       <c r="E283" s="25">
-        <v>279.18</v>
+        <v>273.24</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6937,16 +6935,16 @@
         <v>291</v>
       </c>
       <c r="B287" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C287" s="23">
-        <v>54.5</v>
+        <v>52.5</v>
       </c>
       <c r="D287" s="24">
         <v>6.18</v>
       </c>
       <c r="E287" s="25">
-        <v>336.81</v>
+        <v>324.45</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -6963,16 +6961,16 @@
         <v>293</v>
       </c>
       <c r="B289" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C289" s="23">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D289" s="24">
         <v>6.18</v>
       </c>
       <c r="E289" s="25">
-        <v>278.10000000000002</v>
+        <v>265.74</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7048,16 +7046,16 @@
         <v>298</v>
       </c>
       <c r="B294" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C294" s="23">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D294" s="24">
         <v>6.4</v>
       </c>
       <c r="E294" s="25">
-        <v>134.4</v>
+        <v>115.2</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -7117,16 +7115,16 @@
         <v>303</v>
       </c>
       <c r="B299" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C299" s="23">
-        <v>19.5</v>
+        <v>19</v>
       </c>
       <c r="D299" s="24">
         <v>7.18</v>
       </c>
       <c r="E299" s="25">
-        <v>139.97</v>
+        <v>136.38</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7134,16 +7132,16 @@
         <v>304</v>
       </c>
       <c r="B300" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C300" s="23">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D300" s="24">
         <v>7.13</v>
       </c>
       <c r="E300" s="25">
-        <v>584.66</v>
+        <v>499.1</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7151,16 +7149,16 @@
         <v>305</v>
       </c>
       <c r="B301" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C301" s="23">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D301" s="24">
         <v>7.13</v>
       </c>
       <c r="E301" s="25">
-        <v>556.14</v>
+        <v>527.62</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7185,16 +7183,16 @@
         <v>307</v>
       </c>
       <c r="B303" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C303" s="23">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="D303" s="24">
         <v>6.65</v>
       </c>
       <c r="E303" s="25">
-        <v>182.88</v>
+        <v>176.23</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7211,16 +7209,16 @@
         <v>309</v>
       </c>
       <c r="B305" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C305" s="23">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D305" s="24">
         <v>7.6</v>
       </c>
       <c r="E305" s="25">
-        <v>205.2</v>
+        <v>174.8</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -7280,16 +7278,16 @@
         <v>314</v>
       </c>
       <c r="B310" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C310" s="23">
-        <v>36.5</v>
+        <v>24.5</v>
       </c>
       <c r="D310" s="24">
         <v>8.08</v>
       </c>
       <c r="E310" s="25">
-        <v>294.92</v>
+        <v>197.96</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -7417,16 +7415,16 @@
         <v>323</v>
       </c>
       <c r="B319" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C319" s="23">
-        <v>31.2</v>
+        <v>29.7</v>
       </c>
       <c r="D319" s="24">
         <v>8.8000000000000007</v>
       </c>
       <c r="E319" s="25">
-        <v>274.56</v>
+        <v>261.36</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -7519,16 +7517,16 @@
         <v>329</v>
       </c>
       <c r="B325" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C325" s="23">
-        <v>27.5</v>
+        <v>19.5</v>
       </c>
       <c r="D325" s="24">
         <v>9.25</v>
       </c>
       <c r="E325" s="25">
-        <v>254.38</v>
+        <v>180.38</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7587,16 +7585,16 @@
         <v>333</v>
       </c>
       <c r="B329" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C329" s="23">
-        <v>64.5</v>
+        <v>61</v>
       </c>
       <c r="D329" s="24">
         <v>5.5</v>
       </c>
       <c r="E329" s="25">
-        <v>354.75</v>
+        <v>335.5</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
@@ -7604,16 +7602,16 @@
         <v>334</v>
       </c>
       <c r="B330" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C330" s="23">
-        <v>45.5</v>
+        <v>44.5</v>
       </c>
       <c r="D330" s="24">
         <v>6.86</v>
       </c>
       <c r="E330" s="25">
-        <v>312.16000000000003</v>
+        <v>305.3</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -7672,16 +7670,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C334" s="23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D334" s="24">
         <v>8.5</v>
       </c>
       <c r="E334" s="25">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7751,16 +7749,16 @@
         <v>343</v>
       </c>
       <c r="B339" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C339" s="23">
-        <v>12.5</v>
+        <v>7.5</v>
       </c>
       <c r="D339" s="24">
-        <v>7.82</v>
+        <v>7.83</v>
       </c>
       <c r="E339" s="25">
-        <v>97.81</v>
+        <v>58.69</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -7890,16 +7888,16 @@
         <v>352</v>
       </c>
       <c r="B348" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C348" s="23">
-        <v>54.5</v>
+        <v>51.5</v>
       </c>
       <c r="D348" s="24">
         <v>6.5</v>
       </c>
       <c r="E348" s="25">
-        <v>354.25</v>
+        <v>334.75</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -7924,16 +7922,16 @@
         <v>354</v>
       </c>
       <c r="B350" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C350" s="23">
-        <v>17.5</v>
+        <v>15.5</v>
       </c>
       <c r="D350" s="24">
         <v>16</v>
       </c>
       <c r="E350" s="25">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -8094,16 +8092,16 @@
         <v>364</v>
       </c>
       <c r="B360" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C360" s="23">
-        <v>1.99</v>
+        <v>0.49</v>
       </c>
       <c r="D360" s="24">
         <v>12</v>
       </c>
       <c r="E360" s="25">
-        <v>23.88</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -8111,16 +8109,16 @@
         <v>365</v>
       </c>
       <c r="B361" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C361" s="23">
-        <v>16.5</v>
+        <v>13.75</v>
       </c>
       <c r="D361" s="24">
         <v>12</v>
       </c>
       <c r="E361" s="25">
-        <v>198</v>
+        <v>165</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8145,16 +8143,16 @@
         <v>367</v>
       </c>
       <c r="B363" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C363" s="23">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D363" s="24">
         <v>11</v>
       </c>
       <c r="E363" s="25">
-        <v>82.5</v>
+        <v>49.5</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8230,16 +8228,16 @@
         <v>372</v>
       </c>
       <c r="B368" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C368" s="23">
-        <v>40.729999999999997</v>
+        <v>36.729999999999997</v>
       </c>
       <c r="D368" s="24">
         <v>10</v>
       </c>
       <c r="E368" s="25">
-        <v>407.3</v>
+        <v>367.3</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -8383,16 +8381,16 @@
         <v>381</v>
       </c>
       <c r="B377" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C377" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D377" s="24">
         <v>10</v>
       </c>
       <c r="E377" s="25">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -8400,16 +8398,16 @@
         <v>382</v>
       </c>
       <c r="B378" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C378" s="23">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="D378" s="24">
         <v>17</v>
       </c>
       <c r="E378" s="25">
-        <v>170</v>
+        <v>161.5</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
@@ -8554,13 +8552,13 @@
         <v>32</v>
       </c>
       <c r="C387" s="23">
-        <v>14.75</v>
+        <v>17.25</v>
       </c>
       <c r="D387" s="24">
         <v>11.5</v>
       </c>
       <c r="E387" s="25">
-        <v>169.63</v>
+        <v>198.38</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
@@ -8649,16 +8647,16 @@
         <v>397</v>
       </c>
       <c r="B393" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C393" s="23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D393" s="24">
         <v>9.5</v>
       </c>
       <c r="E393" s="25">
-        <v>114</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
@@ -8666,16 +8664,16 @@
         <v>398</v>
       </c>
       <c r="B394" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C394" s="23">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D394" s="24">
         <v>10.93</v>
       </c>
       <c r="E394" s="25">
-        <v>568.36</v>
+        <v>524.64</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -8683,16 +8681,16 @@
         <v>399</v>
       </c>
       <c r="B395" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C395" s="23">
-        <v>16</v>
+        <v>13.5</v>
       </c>
       <c r="D395" s="24">
         <v>10.93</v>
       </c>
       <c r="E395" s="25">
-        <v>174.88</v>
+        <v>147.56</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
@@ -9050,16 +9048,16 @@
         <v>422</v>
       </c>
       <c r="B418" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C418" s="23">
-        <v>71.5</v>
+        <v>70.5</v>
       </c>
       <c r="D418" s="24">
         <v>2.75</v>
       </c>
       <c r="E418" s="25">
-        <v>196.63</v>
+        <v>193.88</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
@@ -9127,16 +9125,16 @@
         <v>427</v>
       </c>
       <c r="B423" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C423" s="23">
-        <v>43</v>
+        <v>39.5</v>
       </c>
       <c r="D423" s="24">
         <v>2.8</v>
       </c>
       <c r="E423" s="25">
-        <v>120.4</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -9144,16 +9142,16 @@
         <v>428</v>
       </c>
       <c r="B424" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C424" s="23">
-        <v>40.5</v>
+        <v>40</v>
       </c>
       <c r="D424" s="24">
         <v>2.95</v>
       </c>
       <c r="E424" s="25">
-        <v>119.48</v>
+        <v>118</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -9507,16 +9505,16 @@
         <v>451</v>
       </c>
       <c r="B447" s="22">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C447" s="23">
-        <v>53</v>
+        <v>53.5</v>
       </c>
       <c r="D447" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E447" s="25">
-        <v>219.98</v>
+        <v>222.05</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9626,16 +9624,16 @@
         <v>458</v>
       </c>
       <c r="B454" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C454" s="23">
-        <v>46.5</v>
+        <v>44.5</v>
       </c>
       <c r="D454" s="24">
         <v>4.75</v>
       </c>
       <c r="E454" s="25">
-        <v>220.88</v>
+        <v>211.38</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
@@ -9808,13 +9806,13 @@
         <v>8</v>
       </c>
       <c r="C465" s="23">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="D465" s="24">
         <v>5.46</v>
       </c>
       <c r="E465" s="25">
-        <v>-32.76</v>
+        <v>21.84</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
@@ -9880,16 +9878,16 @@
         <v>474</v>
       </c>
       <c r="B470" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C470" s="23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D470" s="24">
         <v>7.5</v>
       </c>
       <c r="E470" s="25">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
@@ -9897,16 +9895,16 @@
         <v>475</v>
       </c>
       <c r="B471" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C471" s="23">
-        <v>32.5</v>
+        <v>32</v>
       </c>
       <c r="D471" s="24">
         <v>7.13</v>
       </c>
       <c r="E471" s="25">
-        <v>231.73</v>
+        <v>228.16</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
@@ -10053,16 +10051,16 @@
         <v>485</v>
       </c>
       <c r="B481" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C481" s="23">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="D481" s="24">
         <v>4.28</v>
       </c>
       <c r="E481" s="25">
-        <v>92.02</v>
+        <v>87.74</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
@@ -10070,16 +10068,16 @@
         <v>486</v>
       </c>
       <c r="B482" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C482" s="23">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D482" s="24">
         <v>9.5</v>
       </c>
       <c r="E482" s="25">
-        <v>313.5</v>
+        <v>256.5</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
@@ -10119,16 +10117,16 @@
         <v>489</v>
       </c>
       <c r="B485" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C485" s="23">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D485" s="24">
         <v>5.7</v>
       </c>
       <c r="E485" s="25">
-        <v>205.2</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
@@ -10351,16 +10349,16 @@
         <v>503</v>
       </c>
       <c r="B499" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C499" s="23">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D499" s="24">
         <v>1.38</v>
       </c>
       <c r="E499" s="25">
-        <v>194.33</v>
+        <v>188.82</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10419,16 +10417,16 @@
         <v>507</v>
       </c>
       <c r="B503" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C503" s="23">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D503" s="24">
         <v>1.71</v>
       </c>
       <c r="E503" s="25">
-        <v>68.400000000000006</v>
+        <v>66.69</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10436,16 +10434,16 @@
         <v>508</v>
       </c>
       <c r="B504" s="22">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C504" s="23">
-        <v>127.5</v>
+        <v>122.5</v>
       </c>
       <c r="D504" s="24">
         <v>0.39</v>
       </c>
       <c r="E504" s="25">
-        <v>49.95</v>
+        <v>47.99</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
@@ -10456,13 +10454,13 @@
         <v>75</v>
       </c>
       <c r="C505" s="23">
-        <v>65.7</v>
+        <v>235.7</v>
       </c>
       <c r="D505" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E505" s="25">
-        <v>149.80000000000001</v>
+        <v>537.4</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -10547,16 +10545,16 @@
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C511" s="23">
-        <v>107.5</v>
+        <v>104.5</v>
       </c>
       <c r="D511" s="24">
         <v>2.8</v>
       </c>
       <c r="E511" s="25">
-        <v>301</v>
+        <v>292.60000000000002</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10564,16 +10562,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C512" s="23">
-        <v>48.5</v>
+        <v>46.5</v>
       </c>
       <c r="D512" s="24">
         <v>2.95</v>
       </c>
       <c r="E512" s="25">
-        <v>143.08000000000001</v>
+        <v>137.18</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10757,16 +10755,16 @@
         <v>529</v>
       </c>
       <c r="B525" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C525" s="23">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D525" s="24">
         <v>3.5</v>
       </c>
       <c r="E525" s="25">
-        <v>73.5</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
@@ -10774,16 +10772,16 @@
         <v>530</v>
       </c>
       <c r="B526" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C526" s="23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D526" s="24">
         <v>3.33</v>
       </c>
       <c r="E526" s="25">
-        <v>116.55</v>
+        <v>113.22</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10937,16 +10935,16 @@
         <v>541</v>
       </c>
       <c r="B537" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C537" s="23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D537" s="24">
         <v>4</v>
       </c>
       <c r="E537" s="25">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -11005,16 +11003,16 @@
         <v>545</v>
       </c>
       <c r="B541" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C541" s="23">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D541" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E541" s="25">
-        <v>96.8</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -11107,27 +11105,33 @@
         <v>551</v>
       </c>
       <c r="B547" s="22">
-        <v>11</v>
-      </c>
-      <c r="C547" s="26"/>
-      <c r="D547" s="27"/>
-      <c r="E547" s="26"/>
+        <v>13</v>
+      </c>
+      <c r="C547" s="23">
+        <v>-16</v>
+      </c>
+      <c r="D547" s="24">
+        <v>4.75</v>
+      </c>
+      <c r="E547" s="25">
+        <v>-76</v>
+      </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A548" s="21" t="s">
         <v>552</v>
       </c>
       <c r="B548" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C548" s="23">
-        <v>17.5</v>
+        <v>7.5</v>
       </c>
       <c r="D548" s="24">
         <v>4.75</v>
       </c>
       <c r="E548" s="25">
-        <v>83.13</v>
+        <v>35.630000000000003</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.25">
@@ -11135,16 +11139,16 @@
         <v>553</v>
       </c>
       <c r="B549" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C549" s="23">
-        <v>44.5</v>
+        <v>44</v>
       </c>
       <c r="D549" s="24">
         <v>5</v>
       </c>
       <c r="E549" s="25">
-        <v>222.5</v>
+        <v>220</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -11220,16 +11224,16 @@
         <v>558</v>
       </c>
       <c r="B554" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C554" s="23">
-        <v>54.5</v>
+        <v>52.5</v>
       </c>
       <c r="D554" s="24">
         <v>5.5</v>
       </c>
       <c r="E554" s="25">
-        <v>299.75</v>
+        <v>288.75</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
@@ -11254,16 +11258,16 @@
         <v>560</v>
       </c>
       <c r="B556" s="22">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C556" s="23">
-        <v>26.5</v>
+        <v>23</v>
       </c>
       <c r="D556" s="24">
         <v>5.75</v>
       </c>
       <c r="E556" s="25">
-        <v>152.38</v>
+        <v>132.25</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
@@ -11337,16 +11341,16 @@
         <v>565</v>
       </c>
       <c r="B561" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C561" s="23">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D561" s="24">
         <v>6</v>
       </c>
       <c r="E561" s="25">
-        <v>186</v>
+        <v>156</v>
       </c>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
@@ -11693,16 +11697,16 @@
         <v>587</v>
       </c>
       <c r="B583" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C583" s="23">
-        <v>57.5</v>
+        <v>55.5</v>
       </c>
       <c r="D583" s="24">
         <v>3</v>
       </c>
       <c r="E583" s="25">
-        <v>172.5</v>
+        <v>166.5</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
@@ -11842,16 +11846,16 @@
         <v>596</v>
       </c>
       <c r="B592" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C592" s="23">
-        <v>233.5</v>
+        <v>232.5</v>
       </c>
       <c r="D592" s="24">
         <v>1.92</v>
       </c>
       <c r="E592" s="25">
-        <v>448.43</v>
+        <v>446.51</v>
       </c>
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
@@ -11859,16 +11863,16 @@
         <v>597</v>
       </c>
       <c r="B593" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C593" s="23">
-        <v>-12.5</v>
+        <v>-17.5</v>
       </c>
       <c r="D593" s="24">
         <v>1.96</v>
       </c>
       <c r="E593" s="25">
-        <v>-24.52</v>
+        <v>-34.32</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
@@ -11876,16 +11880,16 @@
         <v>598</v>
       </c>
       <c r="B594" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C594" s="23">
-        <v>216.5</v>
+        <v>213.5</v>
       </c>
       <c r="D594" s="24">
         <v>1.93</v>
       </c>
       <c r="E594" s="25">
-        <v>417.76</v>
+        <v>411.97</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
@@ -11893,16 +11897,16 @@
         <v>599</v>
       </c>
       <c r="B595" s="22">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C595" s="23">
-        <v>193.5</v>
+        <v>173.5</v>
       </c>
       <c r="D595" s="24">
         <v>2.84</v>
       </c>
       <c r="E595" s="25">
-        <v>549.24</v>
+        <v>492.47</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -11944,16 +11948,16 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C598" s="23">
-        <v>43.5</v>
+        <v>42.5</v>
       </c>
       <c r="D598" s="24">
         <v>4.05</v>
       </c>
       <c r="E598" s="25">
-        <v>176.18</v>
+        <v>172.13</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11995,16 +11999,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C601" s="23">
-        <v>338.5</v>
+        <v>332.5</v>
       </c>
       <c r="D601" s="24">
         <v>1.4</v>
       </c>
       <c r="E601" s="25">
-        <v>473.9</v>
+        <v>465.5</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12012,16 +12016,16 @@
         <v>606</v>
       </c>
       <c r="B602" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C602" s="23">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D602" s="24">
         <v>1.4</v>
       </c>
       <c r="E602" s="25">
-        <v>70</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12029,10 +12033,10 @@
         <v>607</v>
       </c>
       <c r="B603" s="22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C603" s="23">
-        <v>40.5</v>
+        <v>28</v>
       </c>
       <c r="D603" s="27"/>
       <c r="E603" s="26"/>
@@ -12042,10 +12046,10 @@
         <v>608</v>
       </c>
       <c r="B604" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C604" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D604" s="27"/>
       <c r="E604" s="26"/>
@@ -12068,10 +12072,10 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C606" s="23">
-        <v>30.3</v>
+        <v>28.3</v>
       </c>
       <c r="D606" s="27"/>
       <c r="E606" s="26"/>
@@ -12094,16 +12098,16 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C608" s="23">
-        <v>1629.5</v>
+        <v>1609.5</v>
       </c>
       <c r="D608" s="24">
         <v>0.83</v>
       </c>
       <c r="E608" s="25">
-        <v>1344.34</v>
+        <v>1327.84</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12111,16 +12115,16 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C609" s="23">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="D609" s="24">
         <v>0.8</v>
       </c>
       <c r="E609" s="25">
-        <v>421.6</v>
+        <v>413.6</v>
       </c>
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
@@ -12128,16 +12132,16 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C610" s="23">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="D610" s="24">
         <v>0.8</v>
       </c>
       <c r="E610" s="25">
-        <v>524</v>
+        <v>515.20000000000005</v>
       </c>
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.25">
@@ -12145,16 +12149,16 @@
         <v>615</v>
       </c>
       <c r="B611" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C611" s="23">
-        <v>353.5</v>
+        <v>343.5</v>
       </c>
       <c r="D611" s="24">
         <v>0.8</v>
       </c>
       <c r="E611" s="25">
-        <v>282.8</v>
+        <v>274.8</v>
       </c>
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.25">
@@ -12162,27 +12166,33 @@
         <v>616</v>
       </c>
       <c r="B612" s="22">
-        <v>121</v>
-      </c>
-      <c r="C612" s="26"/>
-      <c r="D612" s="27"/>
-      <c r="E612" s="26"/>
+        <v>124</v>
+      </c>
+      <c r="C612" s="23">
+        <v>765</v>
+      </c>
+      <c r="D612" s="24">
+        <v>0.52</v>
+      </c>
+      <c r="E612" s="25">
+        <v>397.8</v>
+      </c>
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A613" s="21" t="s">
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C613" s="23">
-        <v>-7</v>
+        <v>699</v>
       </c>
       <c r="D613" s="24">
         <v>0.52</v>
       </c>
       <c r="E613" s="25">
-        <v>-3.64</v>
+        <v>363.48</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12190,16 +12200,16 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C614" s="23">
-        <v>559.5</v>
+        <v>524.5</v>
       </c>
       <c r="D614" s="24">
         <v>0.52</v>
       </c>
       <c r="E614" s="25">
-        <v>290.94</v>
+        <v>272.74</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12207,16 +12217,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C615" s="23">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D615" s="24">
         <v>0.7</v>
       </c>
       <c r="E615" s="25">
-        <v>588.70000000000005</v>
+        <v>588</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12224,16 +12234,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C616" s="23">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="D616" s="24">
         <v>0.7</v>
       </c>
       <c r="E616" s="25">
-        <v>89.6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12241,16 +12251,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C617" s="23">
-        <v>272.5</v>
+        <v>250.5</v>
       </c>
       <c r="D617" s="24">
         <v>0.68</v>
       </c>
       <c r="E617" s="25">
-        <v>185.85</v>
+        <v>170.84</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12366,11 +12376,11 @@
       </c>
       <c r="B625" s="29"/>
       <c r="C625" s="30">
-        <v>35874.550000000003</v>
+        <v>36855.300000000003</v>
       </c>
       <c r="D625" s="31"/>
       <c r="E625" s="32">
-        <v>101967.27</v>
+        <v>101594.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:19
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -104,7 +104,7 @@
     <t>1860 PATRIKA</t>
   </si>
   <si>
-    <t>1861 PATRIKA (15000)</t>
+    <t>1861 PATRIKA</t>
   </si>
   <si>
     <t>1862 PATRIKA</t>
@@ -137,7 +137,7 @@
     <t>1871 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>1872 PATRIKA (9900)</t>
+    <t>1872 PATRIKA</t>
   </si>
   <si>
     <t>1873 PATRIKA (DC)</t>
@@ -383,7 +383,7 @@
     <t>2024 PATRIKA {L}</t>
   </si>
   <si>
-    <t>2025 PATRIKA (1500)</t>
+    <t>2025 PATRIKA</t>
   </si>
   <si>
     <t>2026 PATRIKA {L}</t>
@@ -398,7 +398,7 @@
     <t>2029 PATRIKA {M}</t>
   </si>
   <si>
-    <t>2030 PATRIKA {M} (2000)</t>
+    <t>2030 PATRIKA {M}</t>
   </si>
   <si>
     <t>2031 PATRIKA (DC)</t>
@@ -470,13 +470,13 @@
     <t>2053 PATRIKA {L} DC</t>
   </si>
   <si>
-    <t>2054 PATRIKA {L} (1000)</t>
+    <t>2054 PATRIKA {L}</t>
   </si>
   <si>
     <t>2055 PATRIKA</t>
   </si>
   <si>
-    <t>2056 PATRIKA {L} (1000)</t>
+    <t>2056 PATRIKA {L}</t>
   </si>
   <si>
     <t>2057 PATRIKA {L}</t>
@@ -677,7 +677,7 @@
     <t>5012 PATRIKA</t>
   </si>
   <si>
-    <t>5013 PATRIKA (11400)</t>
+    <t>5013 PATRIKA</t>
   </si>
   <si>
     <t>5014 PATRIKA</t>
@@ -770,10 +770,10 @@
     <t>5040 PATRIKA (GRAPH AAYEGA)</t>
   </si>
   <si>
-    <t>5041 PATRIKA (AA GYA)</t>
-  </si>
-  <si>
-    <t>5042 PATRIKA 2400</t>
+    <t>5041 PATRIKA</t>
+  </si>
+  <si>
+    <t>5042 PATRIKA</t>
   </si>
   <si>
     <t>5042 PATRIKA - B (DC)</t>
@@ -794,7 +794,7 @@
     <t>5047 PATRIKA (5022-B)</t>
   </si>
   <si>
-    <t>5850 PATRIKA (HALKA D/F) 6600</t>
+    <t>5850 PATRIKA (HALKA D/F)</t>
   </si>
   <si>
     <t>5851 PATRIKA</t>
@@ -902,13 +902,13 @@
     <t>5885 PATRIKA</t>
   </si>
   <si>
-    <t>5886 PATRIKA (2500)</t>
+    <t>5886 PATRIKA</t>
   </si>
   <si>
     <t>5887 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5888 PATRIKA {M}</t>
+    <t>5888 PATRIKA {M} Monday Ayga</t>
   </si>
   <si>
     <t>5889 PATRIKA (DC) {{10}}</t>
@@ -1115,7 +1115,7 @@
     <t>6508 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6509 PATRIKA (1000)</t>
+    <t>6509 PATRIKA</t>
   </si>
   <si>
     <t>6510 PATRIKA {L}</t>
@@ -1124,7 +1124,7 @@
     <t>6511 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6512 PATRIKA {M} (1000)</t>
+    <t>6512 PATRIKA {M}</t>
   </si>
   <si>
     <t>6513 PATRIKA {M}</t>
@@ -1148,7 +1148,7 @@
     <t>6519 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6520 PATRIKA {M} (1800)</t>
+    <t>6520 PATRIKA {M}</t>
   </si>
   <si>
     <t>6521 PATRIKA (GGN) {M}</t>
@@ -1220,7 +1220,7 @@
     <t>6543 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6544 PATRIKA (GGN) {M} (3000)</t>
+    <t>6544 PATRIKA (GGN) {M}</t>
   </si>
   <si>
     <t>6545 PATRIKA {M}</t>
@@ -1820,7 +1820,7 @@
     <t>9091 CARD</t>
   </si>
   <si>
-    <t>9092 CARD (3600)</t>
+    <t>9092 CARD</t>
   </si>
   <si>
     <t>9093 CARD</t>
@@ -2594,16 +2594,16 @@
         <v>14</v>
       </c>
       <c r="B11" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="23">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="D11" s="24">
         <v>0.83</v>
       </c>
       <c r="E11" s="25">
-        <v>689.48</v>
+        <v>686.97</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2611,16 +2611,16 @@
         <v>15</v>
       </c>
       <c r="B12" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="23">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>130.35</v>
+        <v>122.1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2628,16 +2628,16 @@
         <v>16</v>
       </c>
       <c r="B13" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" s="23">
-        <v>120.5</v>
+        <v>116.5</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>198.83</v>
+        <v>192.23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2679,16 +2679,16 @@
         <v>19</v>
       </c>
       <c r="B16" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="23">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>82.8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,16 +2696,16 @@
         <v>20</v>
       </c>
       <c r="B17" s="22">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C17" s="23">
-        <v>149.5</v>
+        <v>147.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,13 +2801,13 @@
         <v>42</v>
       </c>
       <c r="C23" s="23">
-        <v>1.75</v>
+        <v>151.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>3.5</v>
+        <v>303.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2815,16 +2815,16 @@
         <v>27</v>
       </c>
       <c r="B24" s="22">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="23">
-        <v>122.5</v>
+        <v>127.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>257.25</v>
+        <v>267.75</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,16 +2935,16 @@
         <v>35</v>
       </c>
       <c r="B32" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C32" s="23">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>145</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,13 +2966,13 @@
         <v>43</v>
       </c>
       <c r="C34" s="23">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>15</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3174,16 +3174,16 @@
         <v>50</v>
       </c>
       <c r="B47" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C47" s="23">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D47" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E47" s="25">
-        <v>13.2</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3208,16 +3208,16 @@
         <v>52</v>
       </c>
       <c r="B49" s="22">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C49" s="23">
-        <v>742</v>
+        <v>732</v>
       </c>
       <c r="D49" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>816.2</v>
+        <v>805.2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3242,16 +3242,16 @@
         <v>54</v>
       </c>
       <c r="B51" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C51" s="23">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D51" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E51" s="25">
-        <v>19.8</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3259,16 +3259,16 @@
         <v>55</v>
       </c>
       <c r="B52" s="22">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C52" s="23">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D52" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>148.5</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3327,16 +3327,16 @@
         <v>59</v>
       </c>
       <c r="B56" s="22">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C56" s="23">
-        <v>510.5</v>
+        <v>507.5</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>561.54999999999995</v>
+        <v>558.25</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3476,16 +3476,16 @@
         <v>68</v>
       </c>
       <c r="B65" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C65" s="23">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>791.7</v>
+        <v>787.5</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,16 +3561,16 @@
         <v>73</v>
       </c>
       <c r="B70" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C70" s="23">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>82.8</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,16 +3578,16 @@
         <v>74</v>
       </c>
       <c r="B71" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C71" s="23">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>105.3</v>
+        <v>101.7</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3645,9 +3645,11 @@
       <c r="A75" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="22"/>
+      <c r="B75" s="22">
+        <v>1</v>
+      </c>
       <c r="C75" s="23">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D75" s="27"/>
       <c r="E75" s="26"/>
@@ -3660,7 +3662,7 @@
         <v>63</v>
       </c>
       <c r="C76" s="23">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="D76" s="27"/>
       <c r="E76" s="26"/>
@@ -3683,10 +3685,10 @@
         <v>81</v>
       </c>
       <c r="B78" s="22">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C78" s="23">
-        <v>364.5</v>
+        <v>363.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3735,10 +3737,10 @@
         <v>85</v>
       </c>
       <c r="B82" s="22">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C82" s="23">
-        <v>98.5</v>
+        <v>99.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3748,16 +3750,16 @@
         <v>86</v>
       </c>
       <c r="B83" s="22">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C83" s="23">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>741.75</v>
+        <v>730.25</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3765,16 +3767,16 @@
         <v>87</v>
       </c>
       <c r="B84" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C84" s="23">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>830.3</v>
+        <v>825.7</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3782,16 +3784,16 @@
         <v>88</v>
       </c>
       <c r="B85" s="22">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C85" s="23">
-        <v>1468.5</v>
+        <v>1448.5</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>2055.9</v>
+        <v>2027.9</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,13 +3847,13 @@
         <v>65</v>
       </c>
       <c r="C89" s="23">
-        <v>867.5</v>
+        <v>874.5</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1735</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,16 +3861,16 @@
         <v>93</v>
       </c>
       <c r="B90" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C90" s="23">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1160</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3876,16 +3878,16 @@
         <v>94</v>
       </c>
       <c r="B91" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C91" s="23">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>583.38</v>
+        <v>577.08000000000004</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3893,16 +3895,16 @@
         <v>95</v>
       </c>
       <c r="B92" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C92" s="23">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>816.48</v>
+        <v>807.66</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4175,16 +4177,16 @@
         <v>115</v>
       </c>
       <c r="B112" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C112" s="23">
-        <v>21.5</v>
+        <v>10.5</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>268.75</v>
+        <v>131.25</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4246,13 +4248,13 @@
         <v>23</v>
       </c>
       <c r="C116" s="23">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D116" s="24">
         <v>12.5</v>
       </c>
       <c r="E116" s="25">
-        <v>112.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4331,13 +4333,13 @@
         <v>43</v>
       </c>
       <c r="C121" s="23">
-        <v>17</v>
+        <v>34.5</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>212.5</v>
+        <v>431.25</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4507,16 +4509,16 @@
         <v>135</v>
       </c>
       <c r="B132" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C132" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D132" s="24">
         <v>15.5</v>
       </c>
       <c r="E132" s="25">
-        <v>62</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4575,16 +4577,16 @@
         <v>139</v>
       </c>
       <c r="B136" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136" s="23">
-        <v>17</v>
+        <v>13.5</v>
       </c>
       <c r="D136" s="24">
         <v>15.5</v>
       </c>
       <c r="E136" s="25">
-        <v>263.5</v>
+        <v>209.25</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4663,13 +4665,13 @@
         <v>8</v>
       </c>
       <c r="C141" s="23">
-        <v>3.9</v>
+        <v>4</v>
       </c>
       <c r="D141" s="24">
         <v>17.940000000000001</v>
       </c>
       <c r="E141" s="25">
-        <v>69.98</v>
+        <v>71.77</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4730,9 +4732,15 @@
       <c r="B145" s="22">
         <v>11</v>
       </c>
-      <c r="C145" s="26"/>
-      <c r="D145" s="27"/>
-      <c r="E145" s="26"/>
+      <c r="C145" s="23">
+        <v>10</v>
+      </c>
+      <c r="D145" s="24">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E145" s="25">
+        <v>183.97</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="21" t="s">
@@ -4759,13 +4767,13 @@
         <v>20</v>
       </c>
       <c r="C147" s="23">
-        <v>-0.5</v>
+        <v>9.5</v>
       </c>
       <c r="D147" s="24">
-        <v>18.399999999999999</v>
+        <v>18.43</v>
       </c>
       <c r="E147" s="25">
-        <v>-9.1999999999999993</v>
+        <v>175.09</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4773,16 +4781,16 @@
         <v>151</v>
       </c>
       <c r="B148" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C148" s="23">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D148" s="24">
         <v>18.420000000000002</v>
       </c>
       <c r="E148" s="25">
-        <v>239.5</v>
+        <v>147.38</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4824,16 +4832,16 @@
         <v>154</v>
       </c>
       <c r="B151" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C151" s="23">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>84.15</v>
+        <v>80.849999999999994</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4841,16 +4849,16 @@
         <v>155</v>
       </c>
       <c r="B152" s="22">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C152" s="23">
-        <v>79.5</v>
+        <v>74.5</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>222.6</v>
+        <v>208.6</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4892,16 +4900,16 @@
         <v>158</v>
       </c>
       <c r="B155" s="22">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C155" s="23">
-        <v>12</v>
+        <v>14.5</v>
       </c>
       <c r="D155" s="24">
         <v>4.7</v>
       </c>
       <c r="E155" s="25">
-        <v>56.4</v>
+        <v>68.150000000000006</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4943,16 +4951,16 @@
         <v>161</v>
       </c>
       <c r="B158" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C158" s="23">
-        <v>120</v>
+        <v>118.5</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>324</v>
+        <v>319.95</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4977,16 +4985,16 @@
         <v>163</v>
       </c>
       <c r="B160" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C160" s="23">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>386.4</v>
+        <v>383.6</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4994,16 +5002,16 @@
         <v>164</v>
       </c>
       <c r="B161" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C161" s="23">
-        <v>33.5</v>
+        <v>32</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>83.75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5045,16 +5053,16 @@
         <v>167</v>
       </c>
       <c r="B164" s="22">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C164" s="23">
-        <v>89.5</v>
+        <v>92.5</v>
       </c>
       <c r="D164" s="24">
         <v>2.8</v>
       </c>
       <c r="E164" s="25">
-        <v>250.6</v>
+        <v>259</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5079,16 +5087,16 @@
         <v>169</v>
       </c>
       <c r="B166" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C166" s="23">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>265.5</v>
+        <v>259.60000000000002</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5113,16 +5121,16 @@
         <v>171</v>
       </c>
       <c r="B168" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C168" s="23">
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
       <c r="D168" s="24">
         <v>3</v>
       </c>
       <c r="E168" s="25">
-        <v>73.5</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5147,16 +5155,16 @@
         <v>173</v>
       </c>
       <c r="B170" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C170" s="23">
-        <v>91.5</v>
+        <v>89.5</v>
       </c>
       <c r="D170" s="24">
         <v>3.3</v>
       </c>
       <c r="E170" s="25">
-        <v>301.95</v>
+        <v>295.35000000000002</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5256,16 +5264,16 @@
         <v>180</v>
       </c>
       <c r="B177" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C177" s="23">
-        <v>73.5</v>
+        <v>93</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>244.76</v>
+        <v>309.69</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5273,17 +5281,11 @@
         <v>181</v>
       </c>
       <c r="B178" s="22">
-        <v>30</v>
-      </c>
-      <c r="C178" s="23">
-        <v>30.5</v>
-      </c>
-      <c r="D178" s="24">
-        <v>3.33</v>
-      </c>
-      <c r="E178" s="25">
-        <v>101.57</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C178" s="26"/>
+      <c r="D178" s="27"/>
+      <c r="E178" s="26"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="21" t="s">
@@ -5621,16 +5623,16 @@
         <v>203</v>
       </c>
       <c r="B200" s="22">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C200" s="23">
-        <v>66.239999999999995</v>
+        <v>62.24</v>
       </c>
       <c r="D200" s="24">
         <v>3.09</v>
       </c>
       <c r="E200" s="25">
-        <v>204.37</v>
+        <v>192.03</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5810,13 +5812,13 @@
         <v>101</v>
       </c>
       <c r="C214" s="23">
-        <v>96.5</v>
+        <v>210.5</v>
       </c>
       <c r="D214" s="24">
-        <v>4.12</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="E214" s="25">
-        <v>397.17</v>
+        <v>865.71</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5875,16 +5877,16 @@
         <v>221</v>
       </c>
       <c r="B218" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C218" s="23">
-        <v>100.5</v>
+        <v>90.5</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>436.26</v>
+        <v>392.85</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5931,16 +5933,16 @@
         <v>225</v>
       </c>
       <c r="B222" s="22">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C222" s="23">
-        <v>233.5</v>
+        <v>228</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>1050.75</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6065,16 +6067,16 @@
         <v>233</v>
       </c>
       <c r="B230" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C230" s="23">
-        <v>34.5</v>
+        <v>29.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>181.13</v>
+        <v>154.88</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6213,16 +6215,16 @@
         <v>243</v>
       </c>
       <c r="B240" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C240" s="23">
-        <v>120.3</v>
+        <v>118.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>685.71</v>
+        <v>677.16</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6279,16 +6281,16 @@
         <v>247</v>
       </c>
       <c r="B244" s="22">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C244" s="23">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>586.04999999999995</v>
+        <v>562.13</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6299,13 +6301,13 @@
         <v>31</v>
       </c>
       <c r="C245" s="23">
-        <v>11.5</v>
+        <v>52.5</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>48.99</v>
+        <v>223.5</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6313,16 +6315,16 @@
         <v>249</v>
       </c>
       <c r="B246" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C246" s="23">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6379,16 +6381,16 @@
         <v>253</v>
       </c>
       <c r="B250" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C250" s="23">
-        <v>30</v>
+        <v>29.5</v>
       </c>
       <c r="D250" s="24">
         <v>5</v>
       </c>
       <c r="E250" s="25">
-        <v>150</v>
+        <v>147.5</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6424,16 +6426,16 @@
         <v>256</v>
       </c>
       <c r="B253" s="22">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C253" s="23">
-        <v>30.5</v>
+        <v>99</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>106.75</v>
+        <v>346.5</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6586,16 +6588,16 @@
         <v>266</v>
       </c>
       <c r="B263" s="22">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C263" s="23">
-        <v>79.8</v>
+        <v>80.8</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>395.01</v>
+        <v>399.96</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6757,16 +6759,16 @@
         <v>277</v>
       </c>
       <c r="B274" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C274" s="23">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="D274" s="24">
         <v>5.23</v>
       </c>
       <c r="E274" s="25">
-        <v>60.15</v>
+        <v>57.53</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -6800,16 +6802,16 @@
         <v>280</v>
       </c>
       <c r="B277" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C277" s="23">
-        <v>87.5</v>
+        <v>83.5</v>
       </c>
       <c r="D277" s="24">
         <v>6.25</v>
       </c>
       <c r="E277" s="25">
-        <v>546.88</v>
+        <v>521.88</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6885,16 +6887,16 @@
         <v>285</v>
       </c>
       <c r="B282" s="22">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C282" s="23">
-        <v>73.88</v>
+        <v>70.88</v>
       </c>
       <c r="D282" s="24">
         <v>5.94</v>
       </c>
       <c r="E282" s="25">
-        <v>438.85</v>
+        <v>421.03</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6999,13 +7001,13 @@
         <v>37</v>
       </c>
       <c r="C289" s="23">
-        <v>16.5</v>
+        <v>41.5</v>
       </c>
       <c r="D289" s="24">
         <v>6.18</v>
       </c>
       <c r="E289" s="25">
-        <v>101.97</v>
+        <v>256.47000000000003</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7025,13 +7027,13 @@
         <v>66</v>
       </c>
       <c r="C291" s="23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>43.26</v>
+        <v>30.9</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7084,16 +7086,16 @@
         <v>298</v>
       </c>
       <c r="B295" s="22">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C295" s="23">
-        <v>26</v>
+        <v>16.5</v>
       </c>
       <c r="D295" s="24">
         <v>6.46</v>
       </c>
       <c r="E295" s="25">
-        <v>167.96</v>
+        <v>106.59</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -7127,16 +7129,16 @@
         <v>301</v>
       </c>
       <c r="B298" s="22">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C298" s="23">
-        <v>19</v>
+        <v>19.5</v>
       </c>
       <c r="D298" s="24">
         <v>6.65</v>
       </c>
       <c r="E298" s="25">
-        <v>126.35</v>
+        <v>129.68</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -7187,16 +7189,16 @@
         <v>305</v>
       </c>
       <c r="B302" s="22">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C302" s="23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D302" s="24">
         <v>7.13</v>
       </c>
       <c r="E302" s="25">
-        <v>99.82</v>
+        <v>85.56</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7350,16 +7352,16 @@
         <v>316</v>
       </c>
       <c r="B313" s="22">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C313" s="23">
-        <v>4.5</v>
+        <v>9.5</v>
       </c>
       <c r="D313" s="24">
         <v>8.75</v>
       </c>
       <c r="E313" s="25">
-        <v>39.380000000000003</v>
+        <v>83.13</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -7538,16 +7540,16 @@
         <v>328</v>
       </c>
       <c r="B325" s="22">
+        <v>12</v>
+      </c>
+      <c r="C325" s="23">
         <v>11</v>
-      </c>
-      <c r="C325" s="23">
-        <v>14</v>
       </c>
       <c r="D325" s="24">
         <v>10</v>
       </c>
       <c r="E325" s="25">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7572,16 +7574,16 @@
         <v>330</v>
       </c>
       <c r="B327" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C327" s="23">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D327" s="24">
         <v>9.25</v>
       </c>
       <c r="E327" s="25">
-        <v>333</v>
+        <v>305.25</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -7674,16 +7676,16 @@
         <v>336</v>
       </c>
       <c r="B333" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C333" s="23">
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="D333" s="24">
         <v>6.9</v>
       </c>
       <c r="E333" s="25">
-        <v>286.35000000000002</v>
+        <v>272.55</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7759,17 +7761,11 @@
         <v>341</v>
       </c>
       <c r="B338" s="22">
-        <v>11</v>
-      </c>
-      <c r="C338" s="23">
-        <v>3.5</v>
-      </c>
-      <c r="D338" s="24">
-        <v>10.61</v>
-      </c>
-      <c r="E338" s="25">
-        <v>37.15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C338" s="26"/>
+      <c r="D338" s="27"/>
+      <c r="E338" s="26"/>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" s="21" t="s">
@@ -7830,16 +7826,16 @@
         <v>346</v>
       </c>
       <c r="B343" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C343" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D343" s="24">
         <v>6.51</v>
       </c>
       <c r="E343" s="25">
-        <v>156.25</v>
+        <v>143.22999999999999</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -8045,33 +8041,27 @@
         <v>359</v>
       </c>
       <c r="B356" s="22">
-        <v>7</v>
-      </c>
-      <c r="C356" s="23">
-        <v>2.5</v>
-      </c>
-      <c r="D356" s="24">
-        <v>11</v>
-      </c>
-      <c r="E356" s="25">
-        <v>27.5</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C356" s="26"/>
+      <c r="D356" s="27"/>
+      <c r="E356" s="26"/>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="21" t="s">
         <v>360</v>
       </c>
       <c r="B357" s="22">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C357" s="23">
-        <v>4.5</v>
+        <v>8</v>
       </c>
       <c r="D357" s="24">
         <v>18</v>
       </c>
       <c r="E357" s="25">
-        <v>81</v>
+        <v>144</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8116,13 +8106,13 @@
         <v>20</v>
       </c>
       <c r="C360" s="23">
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
       <c r="D360" s="24">
         <v>11</v>
       </c>
       <c r="E360" s="25">
-        <v>115.5</v>
+        <v>225.5</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -8147,16 +8137,16 @@
         <v>365</v>
       </c>
       <c r="B362" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C362" s="23">
-        <v>15.99</v>
+        <v>14.99</v>
       </c>
       <c r="D362" s="24">
         <v>12</v>
       </c>
       <c r="E362" s="25">
-        <v>191.88</v>
+        <v>179.88</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -8167,13 +8157,13 @@
         <v>10</v>
       </c>
       <c r="C363" s="23">
-        <v>0.5</v>
+        <v>10.5</v>
       </c>
       <c r="D363" s="24">
         <v>12</v>
       </c>
       <c r="E363" s="25">
-        <v>6</v>
+        <v>126</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8303,13 +8293,13 @@
         <v>19</v>
       </c>
       <c r="C371" s="23">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>60</v>
+        <v>240</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8351,16 +8341,16 @@
         <v>377</v>
       </c>
       <c r="B374" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C374" s="23">
-        <v>18.5</v>
+        <v>15.5</v>
       </c>
       <c r="D374" s="24">
         <v>18</v>
       </c>
       <c r="E374" s="25">
-        <v>333</v>
+        <v>279</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
@@ -8385,16 +8375,16 @@
         <v>379</v>
       </c>
       <c r="B376" s="22">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C376" s="23">
-        <v>27.01</v>
+        <v>47.26</v>
       </c>
       <c r="D376" s="24">
         <v>9.5</v>
       </c>
       <c r="E376" s="25">
-        <v>256.60000000000002</v>
+        <v>448.97</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
@@ -8402,16 +8392,16 @@
         <v>380</v>
       </c>
       <c r="B377" s="22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C377" s="23">
-        <v>7.3</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D377" s="24">
         <v>15</v>
       </c>
       <c r="E377" s="25">
-        <v>109.5</v>
+        <v>132</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -8532,16 +8522,16 @@
         <v>388</v>
       </c>
       <c r="B385" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C385" s="23">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D385" s="24">
         <v>11.4</v>
       </c>
       <c r="E385" s="25">
-        <v>142.5</v>
+        <v>119.7</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
@@ -8700,16 +8690,16 @@
         <v>398</v>
       </c>
       <c r="B395" s="22">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C395" s="23">
-        <v>1.5</v>
+        <v>32.5</v>
       </c>
       <c r="D395" s="24">
         <v>9.5</v>
       </c>
       <c r="E395" s="25">
-        <v>14.25</v>
+        <v>308.75</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
@@ -8734,16 +8724,16 @@
         <v>400</v>
       </c>
       <c r="B397" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C397" s="23">
-        <v>11.5</v>
+        <v>5.5</v>
       </c>
       <c r="D397" s="24">
         <v>10.93</v>
       </c>
       <c r="E397" s="25">
-        <v>125.7</v>
+        <v>60.12</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8768,16 +8758,16 @@
         <v>402</v>
       </c>
       <c r="B399" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C399" s="23">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D399" s="24">
         <v>10</v>
       </c>
       <c r="E399" s="25">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -8819,16 +8809,16 @@
         <v>405</v>
       </c>
       <c r="B402" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C402" s="23">
-        <v>27</v>
+        <v>26.5</v>
       </c>
       <c r="D402" s="24">
         <v>2</v>
       </c>
       <c r="E402" s="25">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
@@ -9178,16 +9168,16 @@
         <v>428</v>
       </c>
       <c r="B425" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C425" s="23">
-        <v>30.5</v>
+        <v>30</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>85.4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9195,16 +9185,16 @@
         <v>429</v>
       </c>
       <c r="B426" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C426" s="23">
-        <v>39.5</v>
+        <v>37.5</v>
       </c>
       <c r="D426" s="24">
         <v>2.95</v>
       </c>
       <c r="E426" s="25">
-        <v>116.53</v>
+        <v>110.63</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
@@ -9215,13 +9205,13 @@
         <v>8</v>
       </c>
       <c r="C427" s="23">
-        <v>25.5</v>
+        <v>25</v>
       </c>
       <c r="D427" s="24">
         <v>3.1</v>
       </c>
       <c r="E427" s="25">
-        <v>79.05</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -9246,16 +9236,16 @@
         <v>432</v>
       </c>
       <c r="B429" s="22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C429" s="23">
-        <v>23.5</v>
+        <v>26</v>
       </c>
       <c r="D429" s="24">
         <v>3.26</v>
       </c>
       <c r="E429" s="25">
-        <v>76.61</v>
+        <v>84.76</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9297,16 +9287,16 @@
         <v>435</v>
       </c>
       <c r="B432" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C432" s="23">
-        <v>47.5</v>
+        <v>46.5</v>
       </c>
       <c r="D432" s="24">
         <v>3.05</v>
       </c>
       <c r="E432" s="25">
-        <v>144.88</v>
+        <v>141.83000000000001</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
@@ -9790,16 +9780,16 @@
         <v>466</v>
       </c>
       <c r="B463" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C463" s="23">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="D463" s="24">
         <v>5.5</v>
       </c>
       <c r="E463" s="25">
-        <v>77</v>
+        <v>74.25</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -9983,16 +9973,16 @@
         <v>479</v>
       </c>
       <c r="B476" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C476" s="23">
-        <v>45.5</v>
+        <v>43.5</v>
       </c>
       <c r="D476" s="24">
         <v>7.6</v>
       </c>
       <c r="E476" s="25">
-        <v>345.8</v>
+        <v>330.6</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10105,16 +10095,16 @@
         <v>487</v>
       </c>
       <c r="B484" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C484" s="23">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="D484" s="24">
         <v>9.5</v>
       </c>
       <c r="E484" s="25">
-        <v>251.75</v>
+        <v>247</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
@@ -10154,16 +10144,16 @@
         <v>490</v>
       </c>
       <c r="B487" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C487" s="23">
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="D487" s="24">
         <v>5.7</v>
       </c>
       <c r="E487" s="25">
-        <v>116.85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
@@ -10205,16 +10195,16 @@
         <v>493</v>
       </c>
       <c r="B490" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C490" s="23">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>650.1</v>
+        <v>647.9</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10222,16 +10212,16 @@
         <v>494</v>
       </c>
       <c r="B491" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C491" s="23">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D491" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E491" s="25">
-        <v>536.79999999999995</v>
+        <v>534.6</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -10426,16 +10416,16 @@
         <v>506</v>
       </c>
       <c r="B503" s="22">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C503" s="23">
-        <v>474.5</v>
+        <v>629.5</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>711.75</v>
+        <v>944.25</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10460,16 +10450,16 @@
         <v>508</v>
       </c>
       <c r="B505" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C505" s="23">
-        <v>326.5</v>
+        <v>325.5</v>
       </c>
       <c r="D505" s="24">
         <v>1.5</v>
       </c>
       <c r="E505" s="25">
-        <v>489.75</v>
+        <v>488.25</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -10494,16 +10484,16 @@
         <v>510</v>
       </c>
       <c r="B507" s="22">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C507" s="23">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="D507" s="24">
         <v>1.71</v>
       </c>
       <c r="E507" s="25">
-        <v>112.86</v>
+        <v>61.56</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10528,16 +10518,16 @@
         <v>512</v>
       </c>
       <c r="B509" s="22">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C509" s="23">
-        <v>129.19999999999999</v>
+        <v>125.2</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>294.58</v>
+        <v>285.45999999999998</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10605,16 +10595,16 @@
         <v>517</v>
       </c>
       <c r="B514" s="22">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C514" s="23">
-        <v>52.5</v>
+        <v>53.5</v>
       </c>
       <c r="D514" s="24">
         <v>2.73</v>
       </c>
       <c r="E514" s="25">
-        <v>143.54</v>
+        <v>146.27000000000001</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
@@ -10622,16 +10612,16 @@
         <v>518</v>
       </c>
       <c r="B515" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C515" s="23">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D515" s="24">
         <v>2.8</v>
       </c>
       <c r="E515" s="25">
-        <v>400.4</v>
+        <v>394.8</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -10817,16 +10807,16 @@
         <v>531</v>
       </c>
       <c r="B528" s="22">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C528" s="23">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D528" s="24">
         <v>3.5</v>
       </c>
       <c r="E528" s="25">
-        <v>52.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -11218,16 +11208,16 @@
         <v>556</v>
       </c>
       <c r="B553" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C553" s="23">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D553" s="24">
         <v>5</v>
       </c>
       <c r="E553" s="25">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11286,16 +11276,16 @@
         <v>560</v>
       </c>
       <c r="B557" s="22">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C557" s="23">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D557" s="24">
         <v>5.41</v>
       </c>
       <c r="E557" s="25">
-        <v>37.85</v>
+        <v>43.26</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11320,16 +11310,16 @@
         <v>562</v>
       </c>
       <c r="B559" s="22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C559" s="23">
-        <v>8.5</v>
+        <v>13</v>
       </c>
       <c r="D559" s="24">
         <v>5.75</v>
       </c>
       <c r="E559" s="25">
-        <v>48.88</v>
+        <v>74.75</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
@@ -11456,16 +11446,16 @@
         <v>570</v>
       </c>
       <c r="B567" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C567" s="23">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="D567" s="24">
         <v>7</v>
       </c>
       <c r="E567" s="25">
-        <v>24.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
@@ -11613,13 +11603,13 @@
         <v>48</v>
       </c>
       <c r="C577" s="23">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D577" s="24">
         <v>2.76</v>
       </c>
       <c r="E577" s="25">
-        <v>4.1399999999999997</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
@@ -11627,16 +11617,16 @@
         <v>581</v>
       </c>
       <c r="B578" s="22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C578" s="23">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D578" s="24">
         <v>2.76</v>
       </c>
       <c r="E578" s="25">
-        <v>179.13</v>
+        <v>146.06</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
@@ -11678,16 +11668,16 @@
         <v>584</v>
       </c>
       <c r="B581" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C581" s="23">
-        <v>77.5</v>
+        <v>67.5</v>
       </c>
       <c r="D581" s="24">
         <v>2.88</v>
       </c>
       <c r="E581" s="25">
-        <v>223.43</v>
+        <v>194.6</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
@@ -11912,16 +11902,16 @@
         <v>598</v>
       </c>
       <c r="B595" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C595" s="23">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D595" s="24">
-        <v>5.01</v>
+        <v>4.95</v>
       </c>
       <c r="E595" s="25">
-        <v>5.01</v>
+        <v>173.1</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -11929,16 +11919,16 @@
         <v>599</v>
       </c>
       <c r="B596" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C596" s="23">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D596" s="24">
         <v>1.92</v>
       </c>
       <c r="E596" s="25">
-        <v>341.85</v>
+        <v>332.24</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
@@ -11946,16 +11936,16 @@
         <v>600</v>
       </c>
       <c r="B597" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C597" s="23">
-        <v>406.5</v>
+        <v>396.5</v>
       </c>
       <c r="D597" s="24">
         <v>1.91</v>
       </c>
       <c r="E597" s="25">
-        <v>777.44</v>
+        <v>758.31</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -11966,13 +11956,13 @@
         <v>63</v>
       </c>
       <c r="C598" s="23">
-        <v>163.5</v>
+        <v>223.5</v>
       </c>
       <c r="D598" s="24">
         <v>1.93</v>
       </c>
       <c r="E598" s="25">
-        <v>315.49</v>
+        <v>430.24</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11980,16 +11970,16 @@
         <v>602</v>
       </c>
       <c r="B599" s="22">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C599" s="23">
-        <v>77</v>
+        <v>71.5</v>
       </c>
       <c r="D599" s="24">
         <v>2.84</v>
       </c>
       <c r="E599" s="25">
-        <v>218.58</v>
+        <v>202.97</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12048,33 +12038,27 @@
         <v>606</v>
       </c>
       <c r="B603" s="22">
-        <v>33</v>
-      </c>
-      <c r="C603" s="23">
-        <v>-10</v>
-      </c>
-      <c r="D603" s="24">
-        <v>4.05</v>
-      </c>
-      <c r="E603" s="25">
-        <v>-40.5</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C603" s="26"/>
+      <c r="D603" s="27"/>
+      <c r="E603" s="26"/>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A604" s="21" t="s">
         <v>607</v>
       </c>
       <c r="B604" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C604" s="23">
-        <v>355.5</v>
+        <v>354.5</v>
       </c>
       <c r="D604" s="24">
         <v>1.4</v>
       </c>
       <c r="E604" s="25">
-        <v>496.62</v>
+        <v>495.22</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12099,16 +12083,16 @@
         <v>609</v>
       </c>
       <c r="B606" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C606" s="23">
-        <v>-3.5</v>
+        <v>-6</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>-4.9000000000000004</v>
+        <v>-8.4</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12129,10 +12113,10 @@
         <v>611</v>
       </c>
       <c r="B608" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C608" s="23">
-        <v>106.5</v>
+        <v>96.5</v>
       </c>
       <c r="D608" s="27"/>
       <c r="E608" s="26"/>
@@ -12155,10 +12139,10 @@
         <v>613</v>
       </c>
       <c r="B610" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C610" s="23">
-        <v>56.8</v>
+        <v>56.3</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12181,10 +12165,10 @@
         <v>615</v>
       </c>
       <c r="B612" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C612" s="23">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D612" s="27"/>
       <c r="E612" s="26"/>
@@ -12194,16 +12178,16 @@
         <v>616</v>
       </c>
       <c r="B613" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C613" s="23">
-        <v>1477</v>
+        <v>1465</v>
       </c>
       <c r="D613" s="24">
         <v>0.83</v>
       </c>
       <c r="E613" s="25">
-        <v>1218.53</v>
+        <v>1208.6300000000001</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12211,16 +12195,16 @@
         <v>617</v>
       </c>
       <c r="B614" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C614" s="23">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D614" s="24">
         <v>0.8</v>
       </c>
       <c r="E614" s="25">
-        <v>360</v>
+        <v>355.2</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12279,16 +12263,16 @@
         <v>621</v>
       </c>
       <c r="B618" s="22">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C618" s="23">
-        <v>1476.5</v>
+        <v>1479.5</v>
       </c>
       <c r="D618" s="24">
         <v>0.52</v>
       </c>
       <c r="E618" s="25">
-        <v>767.78</v>
+        <v>769.34</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12313,16 +12297,16 @@
         <v>623</v>
       </c>
       <c r="B620" s="22">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C620" s="23">
-        <v>1133.5</v>
+        <v>1123.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.52</v>
       </c>
       <c r="E620" s="25">
-        <v>589.41999999999996</v>
+        <v>584.22</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12381,16 +12365,16 @@
         <v>627</v>
       </c>
       <c r="B624" s="22">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C624" s="23">
-        <v>268</v>
+        <v>216</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>187.6</v>
+        <v>151.19999999999999</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12441,16 +12425,16 @@
         <v>631</v>
       </c>
       <c r="B628" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C628" s="23">
-        <v>1847.5</v>
+        <v>1841.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E628" s="25">
-        <v>1016.64</v>
+        <v>1013.34</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12523,11 +12507,11 @@
       </c>
       <c r="B633" s="29"/>
       <c r="C633" s="30">
-        <v>53249.46</v>
+        <v>53729.81</v>
       </c>
       <c r="D633" s="31"/>
       <c r="E633" s="32">
-        <v>115771.24</v>
+        <v>118420.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:32
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -1112,7 +1112,7 @@
     <t>6506 PATRIKA {L}</t>
   </si>
   <si>
-    <t>6507 PATRIKA (GGN)</t>
+    <t>6507 PATRIKA (GGN) (12.02)</t>
   </si>
   <si>
     <t>6508 PATRIKA {M}</t>
@@ -2603,10 +2603,10 @@
         <v>816</v>
       </c>
       <c r="D11" s="24">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>681.13</v>
+        <v>740.85</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2631,16 +2631,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="23">
-        <v>116.5</v>
+        <v>114.5</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>192.23</v>
+        <v>188.93</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,16 +2699,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="23">
-        <v>147.5</v>
+        <v>142.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,16 +2750,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="23">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2784,16 +2784,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C22" s="23">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D22" s="24">
         <v>2</v>
       </c>
       <c r="E22" s="25">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,16 +2801,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23" s="23">
-        <v>151.75</v>
+        <v>121.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>303.5</v>
+        <v>243.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2818,16 +2818,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C24" s="23">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>260.39999999999998</v>
+        <v>249.9</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2861,16 +2861,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C27" s="23">
-        <v>131.5</v>
+        <v>126.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>309.02999999999997</v>
+        <v>297.27999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2895,16 +2895,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="23">
-        <v>86.8</v>
+        <v>80.8</v>
       </c>
       <c r="D29" s="24">
         <v>2.59</v>
       </c>
       <c r="E29" s="25">
-        <v>224.44</v>
+        <v>208.93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,16 +2966,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" s="23">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>320</v>
+        <v>307.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3009,16 +3009,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C37" s="23">
-        <v>157.5</v>
+        <v>152.5</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>409.5</v>
+        <v>396.5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,13 +3112,13 @@
         <v>23</v>
       </c>
       <c r="C43" s="23">
-        <v>51.5</v>
+        <v>81.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>115.88</v>
+        <v>183.38</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3126,16 +3126,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" s="23">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>207</v>
+        <v>204.75</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3211,16 +3211,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C49" s="23">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="D49" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>798.6</v>
+        <v>792</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3228,16 +3228,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C50" s="23">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="D50" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>409.2</v>
+        <v>398.2</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,16 +3296,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C54" s="23">
-        <v>775.5</v>
+        <v>751.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>853.05</v>
+        <v>826.65</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3313,16 +3313,16 @@
         <v>59</v>
       </c>
       <c r="B55" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C55" s="23">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D55" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E55" s="25">
-        <v>83.6</v>
+        <v>72.599999999999994</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,16 +3462,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C64" s="23">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>573.29999999999995</v>
+        <v>569.1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3513,16 +3513,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C67" s="23">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>81.64</v>
+        <v>81.12</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,16 +3547,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C69" s="23">
-        <v>324.5</v>
+        <v>322.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>227.15</v>
+        <v>225.75</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3564,16 +3564,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C70" s="23">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>64.8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,16 +3581,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C71" s="23">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>99</v>
+        <v>79.2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3598,16 +3598,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C72" s="23">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>172.05</v>
+        <v>156.55000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3615,16 +3615,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C73" s="23">
-        <v>130</v>
+        <v>118.5</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>201.5</v>
+        <v>183.68</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3632,16 +3632,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C74" s="23">
-        <v>285.5</v>
+        <v>278.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>442.53</v>
+        <v>431.68</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3740,10 +3740,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C82" s="23">
-        <v>98.5</v>
+        <v>95.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3753,16 +3753,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C83" s="23">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>724.5</v>
+        <v>718.75</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3804,16 +3804,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C86" s="23">
-        <v>959.5</v>
+        <v>954.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>1343.3</v>
+        <v>1336.3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3821,16 +3821,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C87" s="23">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>197.4</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3864,16 +3864,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C90" s="23">
-        <v>578</v>
+        <v>728.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1156</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,16 +3898,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C92" s="23">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>807.66</v>
+        <v>795.06</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,16 +4027,16 @@
         <v>105</v>
       </c>
       <c r="B101" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C101" s="23">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="D101" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E101" s="25">
-        <v>523.25</v>
+        <v>511.75</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,16 +4180,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C112" s="23">
-        <v>1.5</v>
+        <v>14.5</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>18.75</v>
+        <v>181.25</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,16 +4214,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C114" s="23">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>337.5</v>
+        <v>312.5</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,16 +4231,16 @@
         <v>119</v>
       </c>
       <c r="B115" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C115" s="23">
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
       <c r="D115" s="24">
         <v>12.5</v>
       </c>
       <c r="E115" s="25">
-        <v>306.25</v>
+        <v>293.75</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,16 +4316,16 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C120" s="23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D120" s="24">
         <v>12.5</v>
       </c>
       <c r="E120" s="25">
-        <v>87.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,16 +4333,16 @@
         <v>125</v>
       </c>
       <c r="B121" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C121" s="23">
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>431.25</v>
+        <v>425</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4699,16 +4699,16 @@
         <v>147</v>
       </c>
       <c r="B143" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C143" s="23">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D143" s="24">
         <v>18.420000000000002</v>
       </c>
       <c r="E143" s="25">
-        <v>193.42</v>
+        <v>175</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4835,16 +4835,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C151" s="23">
-        <v>24.5</v>
+        <v>21.5</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>80.849999999999994</v>
+        <v>70.95</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4920,16 +4920,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C156" s="23">
-        <v>161.75</v>
+        <v>230.75</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>549.95000000000005</v>
+        <v>784.55</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4974,13 +4974,13 @@
         <v>66</v>
       </c>
       <c r="C159" s="23">
-        <v>40.5</v>
+        <v>139.5</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>113.4</v>
+        <v>390.6</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -5076,13 +5076,13 @@
         <v>29</v>
       </c>
       <c r="C165" s="23">
-        <v>36.5</v>
+        <v>48.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>107.68</v>
+        <v>143.08000000000001</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5090,16 +5090,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C166" s="23">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>259.60000000000002</v>
+        <v>253.7</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5440,16 +5440,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C188" s="23">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D188" s="24">
         <v>4.5</v>
       </c>
       <c r="E188" s="25">
-        <v>450</v>
+        <v>427.5</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5457,16 +5457,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C189" s="23">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>337.5</v>
+        <v>310.5</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5474,16 +5474,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C190" s="23">
-        <v>79.5</v>
+        <v>76.5</v>
       </c>
       <c r="D190" s="24">
         <v>3.93</v>
       </c>
       <c r="E190" s="25">
-        <v>312.44</v>
+        <v>300.64999999999998</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5497,10 +5497,10 @@
         <v>236.5</v>
       </c>
       <c r="D191" s="24">
-        <v>3.79</v>
+        <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>895.67</v>
+        <v>939.65</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5626,16 +5626,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C200" s="23">
-        <v>58.74</v>
+        <v>56.74</v>
       </c>
       <c r="D200" s="24">
         <v>3.09</v>
       </c>
       <c r="E200" s="25">
-        <v>181.23</v>
+        <v>175.06</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5651,15 +5651,17 @@
       <c r="A202" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="B202" s="22"/>
+      <c r="B202" s="22">
+        <v>1</v>
+      </c>
       <c r="C202" s="23">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D202" s="24">
-        <v>3.42</v>
+        <v>3.5</v>
       </c>
       <c r="E202" s="25">
-        <v>85.47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5745,16 +5747,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C209" s="23">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>345.8</v>
+        <v>326.8</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5762,16 +5764,16 @@
         <v>214</v>
       </c>
       <c r="B210" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C210" s="23">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D210" s="24">
         <v>3.6</v>
       </c>
       <c r="E210" s="25">
-        <v>100.8</v>
+        <v>93.6</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5801,16 +5803,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C213" s="23">
-        <v>93.5</v>
+        <v>88.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>384.87</v>
+        <v>364.29</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5824,10 +5826,10 @@
         <v>210.5</v>
       </c>
       <c r="D214" s="24">
-        <v>4.1100000000000003</v>
+        <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>865.71</v>
+        <v>866.97</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5886,16 +5888,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C218" s="23">
-        <v>90.5</v>
+        <v>89</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>392.85</v>
+        <v>386.34</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5942,16 +5944,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C222" s="23">
-        <v>220</v>
+        <v>214.5</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>990</v>
+        <v>965.25</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5959,16 +5961,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C223" s="23">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>468</v>
+        <v>454.5</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5976,16 +5978,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C224" s="23">
-        <v>123.5</v>
+        <v>120.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>648.38</v>
+        <v>632.63</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6079,13 +6081,13 @@
         <v>34</v>
       </c>
       <c r="C230" s="23">
-        <v>29.5</v>
+        <v>25.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>154.88</v>
+        <v>133.88</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6096,13 +6098,13 @@
         <v>14</v>
       </c>
       <c r="C231" s="23">
-        <v>63.5</v>
+        <v>103.5</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>333.38</v>
+        <v>543.38</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6224,16 +6226,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C240" s="23">
-        <v>118.8</v>
+        <v>114.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>677.16</v>
+        <v>654.36</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6307,16 +6309,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C245" s="23">
-        <v>52.5</v>
+        <v>46.5</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>223.5</v>
+        <v>198.09</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6324,16 +6326,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C246" s="23">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>432</v>
+        <v>392</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6396,10 +6398,10 @@
         <v>29.5</v>
       </c>
       <c r="D250" s="24">
-        <v>5</v>
+        <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>147.5</v>
+        <v>152.08000000000001</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6563,16 +6565,16 @@
         <v>265</v>
       </c>
       <c r="B261" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C261" s="23">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D261" s="24">
         <v>4.5999999999999996</v>
       </c>
       <c r="E261" s="25">
-        <v>138</v>
+        <v>124.2</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6700,16 +6702,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C270" s="23">
-        <v>55.5</v>
+        <v>54.5</v>
       </c>
       <c r="D270" s="24">
         <v>5.4</v>
       </c>
       <c r="E270" s="25">
-        <v>299.7</v>
+        <v>294.3</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6828,16 +6830,16 @@
         <v>282</v>
       </c>
       <c r="B278" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C278" s="23">
-        <v>34.700000000000003</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="D278" s="24">
         <v>6.38</v>
       </c>
       <c r="E278" s="25">
-        <v>221.42</v>
+        <v>215.04</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6970,10 +6972,10 @@
         <v>68</v>
       </c>
       <c r="D286" s="24">
-        <v>6.6</v>
+        <v>6.8</v>
       </c>
       <c r="E286" s="25">
-        <v>449.06</v>
+        <v>462.31</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -7007,16 +7009,16 @@
         <v>293</v>
       </c>
       <c r="B289" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C289" s="23">
-        <v>41.5</v>
+        <v>21.5</v>
       </c>
       <c r="D289" s="24">
         <v>6.18</v>
       </c>
       <c r="E289" s="25">
-        <v>256.47000000000003</v>
+        <v>132.87</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7036,13 +7038,13 @@
         <v>66</v>
       </c>
       <c r="C291" s="23">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>30.9</v>
+        <v>40.17</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7095,16 +7097,16 @@
         <v>299</v>
       </c>
       <c r="B295" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C295" s="23">
-        <v>16.5</v>
+        <v>13.5</v>
       </c>
       <c r="D295" s="24">
         <v>6.46</v>
       </c>
       <c r="E295" s="25">
-        <v>106.59</v>
+        <v>87.21</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -7155,16 +7157,16 @@
         <v>303</v>
       </c>
       <c r="B299" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C299" s="23">
-        <v>16.5</v>
+        <v>11.5</v>
       </c>
       <c r="D299" s="24">
         <v>6.18</v>
       </c>
       <c r="E299" s="25">
-        <v>101.97</v>
+        <v>71.069999999999993</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7201,13 +7203,13 @@
         <v>62</v>
       </c>
       <c r="C302" s="23">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D302" s="24">
         <v>7.13</v>
       </c>
       <c r="E302" s="25">
-        <v>513.36</v>
+        <v>598.91999999999996</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7464,16 +7466,16 @@
         <v>324</v>
       </c>
       <c r="B320" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C320" s="23">
-        <v>29</v>
+        <v>26.5</v>
       </c>
       <c r="D320" s="24">
         <v>9.25</v>
       </c>
       <c r="E320" s="25">
-        <v>268.25</v>
+        <v>245.13</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -7671,13 +7673,13 @@
         <v>38</v>
       </c>
       <c r="C332" s="23">
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="D332" s="24">
-        <v>6.79</v>
+        <v>6.89</v>
       </c>
       <c r="E332" s="25">
-        <v>196.77</v>
+        <v>203.26</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7776,10 +7778,10 @@
         <v>1</v>
       </c>
       <c r="D338" s="24">
-        <v>10.6</v>
+        <v>10.66</v>
       </c>
       <c r="E338" s="25">
-        <v>10.6</v>
+        <v>10.66</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -7841,16 +7843,16 @@
         <v>347</v>
       </c>
       <c r="B343" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C343" s="23">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D343" s="24">
         <v>6.51</v>
       </c>
       <c r="E343" s="25">
-        <v>143.22999999999999</v>
+        <v>123.7</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -8058,9 +8060,15 @@
       <c r="B356" s="22">
         <v>8</v>
       </c>
-      <c r="C356" s="26"/>
-      <c r="D356" s="27"/>
-      <c r="E356" s="26"/>
+      <c r="C356" s="23">
+        <v>10</v>
+      </c>
+      <c r="D356" s="24">
+        <v>11</v>
+      </c>
+      <c r="E356" s="25">
+        <v>110</v>
+      </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" s="21" t="s">
@@ -8495,13 +8503,13 @@
         <v>40</v>
       </c>
       <c r="C382" s="23">
-        <v>3.49</v>
+        <v>11.99</v>
       </c>
       <c r="D382" s="24">
         <v>25</v>
       </c>
       <c r="E382" s="25">
-        <v>87.25</v>
+        <v>299.75</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -8773,16 +8781,16 @@
         <v>403</v>
       </c>
       <c r="B399" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C399" s="23">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D399" s="24">
         <v>10</v>
       </c>
       <c r="E399" s="25">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -8901,16 +8909,16 @@
         <v>411</v>
       </c>
       <c r="B407" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C407" s="23">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D407" s="24">
         <v>2</v>
       </c>
       <c r="E407" s="25">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -9183,16 +9191,16 @@
         <v>429</v>
       </c>
       <c r="B425" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C425" s="23">
-        <v>30</v>
+        <v>29.84</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>84</v>
+        <v>83.55</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9268,16 +9276,16 @@
         <v>434</v>
       </c>
       <c r="B430" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C430" s="23">
-        <v>37.5</v>
+        <v>36.5</v>
       </c>
       <c r="D430" s="24">
         <v>3.3</v>
       </c>
       <c r="E430" s="25">
-        <v>123.75</v>
+        <v>120.45</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -9285,16 +9293,16 @@
         <v>435</v>
       </c>
       <c r="B431" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C431" s="23">
-        <v>73.5</v>
+        <v>71.5</v>
       </c>
       <c r="D431" s="24">
         <v>3.15</v>
       </c>
       <c r="E431" s="25">
-        <v>231.53</v>
+        <v>225.23</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -9798,13 +9806,13 @@
         <v>84</v>
       </c>
       <c r="C463" s="23">
-        <v>13.5</v>
+        <v>83.5</v>
       </c>
       <c r="D463" s="24">
         <v>5.5</v>
       </c>
       <c r="E463" s="25">
-        <v>74.25</v>
+        <v>459.25</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -9937,16 +9945,16 @@
         <v>477</v>
       </c>
       <c r="B473" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C473" s="23">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D473" s="24">
         <v>7.13</v>
       </c>
       <c r="E473" s="25">
-        <v>249.55</v>
+        <v>213.9</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
@@ -10210,16 +10218,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C490" s="23">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>647.9</v>
+        <v>636.9</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10227,16 +10235,16 @@
         <v>495</v>
       </c>
       <c r="B491" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C491" s="23">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="D491" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E491" s="25">
-        <v>534.6</v>
+        <v>523.6</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -10434,13 +10442,13 @@
         <v>120</v>
       </c>
       <c r="C503" s="23">
-        <v>629.5</v>
+        <v>697.5</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>944.25</v>
+        <v>1046.25</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10522,10 +10530,10 @@
         <v>143</v>
       </c>
       <c r="D508" s="24">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="E508" s="25">
-        <v>127.42</v>
+        <v>132.15</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10536,13 +10544,13 @@
         <v>134</v>
       </c>
       <c r="C509" s="23">
-        <v>119.2</v>
+        <v>247.2</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>271.77999999999997</v>
+        <v>563.62</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -11002,16 +11010,16 @@
         <v>544</v>
       </c>
       <c r="B540" s="22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C540" s="23">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D540" s="24">
         <v>3.85</v>
       </c>
       <c r="E540" s="25">
-        <v>207.9</v>
+        <v>200.2</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
@@ -11019,16 +11027,16 @@
         <v>545</v>
       </c>
       <c r="B541" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C541" s="23">
-        <v>67.5</v>
+        <v>66.5</v>
       </c>
       <c r="D541" s="24">
         <v>4</v>
       </c>
       <c r="E541" s="25">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -11104,16 +11112,16 @@
         <v>550</v>
       </c>
       <c r="B546" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C546" s="23">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="D546" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E546" s="25">
-        <v>85.8</v>
+        <v>81.400000000000006</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -11376,16 +11384,16 @@
         <v>566</v>
       </c>
       <c r="B562" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C562" s="23">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="D562" s="24">
         <v>5.75</v>
       </c>
       <c r="E562" s="25">
-        <v>129.38</v>
+        <v>123.63</v>
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
@@ -11632,16 +11640,16 @@
         <v>582</v>
       </c>
       <c r="B578" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C578" s="23">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="D578" s="24">
         <v>2.76</v>
       </c>
       <c r="E578" s="25">
-        <v>146.06</v>
+        <v>278.76</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
@@ -11649,16 +11657,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C579" s="23">
-        <v>2.5</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>6.89</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11743,7 +11751,7 @@
         <v>2.76</v>
       </c>
       <c r="E584" s="25">
-        <v>216.31</v>
+        <v>216.66</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11786,13 +11794,13 @@
         <v>40</v>
       </c>
       <c r="C587" s="23">
-        <v>38.5</v>
+        <v>46.5</v>
       </c>
       <c r="D587" s="24">
         <v>3</v>
       </c>
       <c r="E587" s="25">
-        <v>115.5</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -11934,16 +11942,16 @@
         <v>600</v>
       </c>
       <c r="B596" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C596" s="23">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D596" s="24">
         <v>1.92</v>
       </c>
       <c r="E596" s="25">
-        <v>324.56</v>
+        <v>314.95999999999998</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
@@ -11951,16 +11959,16 @@
         <v>601</v>
       </c>
       <c r="B597" s="22">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C597" s="23">
-        <v>396.5</v>
+        <v>389.5</v>
       </c>
       <c r="D597" s="24">
         <v>1.91</v>
       </c>
       <c r="E597" s="25">
-        <v>758.31</v>
+        <v>744.92</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -11971,13 +11979,13 @@
         <v>63</v>
       </c>
       <c r="C598" s="23">
-        <v>223.5</v>
+        <v>163.5</v>
       </c>
       <c r="D598" s="24">
         <v>1.93</v>
       </c>
       <c r="E598" s="25">
-        <v>430.24</v>
+        <v>315.49</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -12067,13 +12075,13 @@
         <v>46</v>
       </c>
       <c r="C604" s="23">
-        <v>352.5</v>
+        <v>404.5</v>
       </c>
       <c r="D604" s="24">
         <v>1.4</v>
       </c>
       <c r="E604" s="25">
-        <v>492.43</v>
+        <v>565.17999999999995</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12081,16 +12089,16 @@
         <v>609</v>
       </c>
       <c r="B605" s="22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C605" s="23">
-        <v>851</v>
+        <v>979.5</v>
       </c>
       <c r="D605" s="24">
         <v>1.4</v>
       </c>
       <c r="E605" s="25">
-        <v>1191.4000000000001</v>
+        <v>1371.3</v>
       </c>
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
@@ -12098,16 +12106,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C606" s="23">
-        <v>-6</v>
+        <v>-11</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>-8.4</v>
+        <v>-15.4</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12193,16 +12201,16 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C613" s="23">
-        <v>1465</v>
+        <v>1155</v>
       </c>
       <c r="D613" s="24">
         <v>0.83</v>
       </c>
       <c r="E613" s="25">
-        <v>1208.6300000000001</v>
+        <v>952.88</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12227,16 +12235,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C615" s="23">
-        <v>541.5</v>
+        <v>341.5</v>
       </c>
       <c r="D615" s="24">
         <v>0.8</v>
       </c>
       <c r="E615" s="25">
-        <v>433.2</v>
+        <v>273.2</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12244,16 +12252,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C616" s="23">
-        <v>208.5</v>
+        <v>206.5</v>
       </c>
       <c r="D616" s="24">
         <v>0.8</v>
       </c>
       <c r="E616" s="25">
-        <v>166.8</v>
+        <v>165.2</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12278,16 +12286,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C618" s="23">
-        <v>1474.5</v>
+        <v>1472.5</v>
       </c>
       <c r="D618" s="24">
         <v>0.52</v>
       </c>
       <c r="E618" s="25">
-        <v>766.74</v>
+        <v>765.7</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12312,16 +12320,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C620" s="23">
-        <v>1086.5</v>
+        <v>1079.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.52</v>
       </c>
       <c r="E620" s="25">
-        <v>564.98</v>
+        <v>561.34</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12346,16 +12354,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C622" s="23">
-        <v>248.5</v>
+        <v>246.5</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>129.22</v>
+        <v>128.18</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12363,16 +12371,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C623" s="23">
-        <v>682.5</v>
+        <v>982.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.7</v>
       </c>
       <c r="E623" s="25">
-        <v>477.75</v>
+        <v>687.75</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12397,16 +12405,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C625" s="23">
-        <v>82.5</v>
+        <v>287.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.68</v>
       </c>
       <c r="E625" s="25">
-        <v>56.27</v>
+        <v>196.93</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12440,16 +12448,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C628" s="23">
-        <v>1840.5</v>
+        <v>1830.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E628" s="25">
-        <v>1012.79</v>
+        <v>1007.29</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12522,11 +12530,11 @@
       </c>
       <c r="B633" s="29"/>
       <c r="C633" s="30">
-        <v>53765.22</v>
+        <v>54204.800000000003</v>
       </c>
       <c r="D633" s="31"/>
       <c r="E633" s="32">
-        <v>119014.78</v>
+        <v>120660.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:53
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 13-Feb-2025</t>
+    <t>1-Jul-2024 to 14-Feb-2025</t>
   </si>
   <si>
     <t/>
@@ -422,7 +422,7 @@
     <t>2036 PATRIKA {L}</t>
   </si>
   <si>
-    <t>2037 PATRIKA {L}</t>
+    <t>2037 PATRIKA {L} (Dc)</t>
   </si>
   <si>
     <t>2038 PATRIKA {M}</t>
@@ -1913,7 +1913,7 @@
     <t>9209 CARD (YELLOW)</t>
   </si>
   <si>
-    <t>9210 CARD (GOLDEN BOLNA)</t>
+    <t>9210 CARD (GOLDEN BOLNA) STCK NO</t>
   </si>
   <si>
     <t>9211 CARD (NEW)</t>
@@ -2461,7 +2461,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -2597,16 +2597,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C11" s="23">
-        <v>800</v>
+        <v>779.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>726.32</v>
+        <v>707.71</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,16 +2699,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C17" s="23">
-        <v>141.5</v>
+        <v>117.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>283</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,16 +2750,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="23">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>176</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2784,16 +2784,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C22" s="23">
-        <v>47</v>
+        <v>43.5</v>
       </c>
       <c r="D22" s="24">
         <v>2</v>
       </c>
       <c r="E22" s="25">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2861,16 +2861,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" s="23">
-        <v>122.5</v>
+        <v>121.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>287.88</v>
+        <v>285.52999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2992,16 +2992,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" s="23">
-        <v>71</v>
+        <v>69.5</v>
       </c>
       <c r="D36" s="24">
         <v>2.6</v>
       </c>
       <c r="E36" s="25">
-        <v>184.6</v>
+        <v>180.7</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,16 +3043,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="23">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>83.7</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3211,16 +3211,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C49" s="23">
-        <v>643.5</v>
+        <v>612.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>707.85</v>
+        <v>673.75</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3228,16 +3228,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C50" s="23">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D50" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>353.1</v>
+        <v>349.8</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,16 +3296,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C54" s="23">
-        <v>657.5</v>
+        <v>648.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>723.25</v>
+        <v>713.35</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3413,16 +3413,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C61" s="23">
-        <v>75.5</v>
+        <v>40.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>158.55000000000001</v>
+        <v>85.05</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3462,16 +3462,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C64" s="23">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>560.70000000000005</v>
+        <v>558.6</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,16 +3581,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C71" s="23">
-        <v>251.5</v>
+        <v>241.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>226.35</v>
+        <v>217.35</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3598,16 +3598,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C72" s="23">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>142.6</v>
+        <v>139.5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3662,10 +3662,10 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C76" s="23">
-        <v>2.5</v>
+        <v>-2.5</v>
       </c>
       <c r="D76" s="27"/>
       <c r="E76" s="26"/>
@@ -3691,7 +3691,7 @@
         <v>65</v>
       </c>
       <c r="C78" s="23">
-        <v>332.5</v>
+        <v>442.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3717,7 +3717,7 @@
         <v>105</v>
       </c>
       <c r="C80" s="23">
-        <v>151.5</v>
+        <v>201.5</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3753,16 +3753,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C83" s="23">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>660.1</v>
+        <v>647.45000000000005</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3770,16 +3770,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C84" s="23">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>798.1</v>
+        <v>790.05</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3787,16 +3787,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C85" s="23">
-        <v>1335</v>
+        <v>1976</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>1869</v>
+        <v>2766.4</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3804,16 +3804,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C86" s="23">
-        <v>883.5</v>
+        <v>1199.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>1236.9000000000001</v>
+        <v>1679.3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3821,16 +3821,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C87" s="23">
-        <v>1184</v>
+        <v>1179</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1657.6</v>
+        <v>1650.6</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3847,16 +3847,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C89" s="23">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1744</v>
+        <v>1740</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3867,13 +3867,13 @@
         <v>60</v>
       </c>
       <c r="C90" s="23">
-        <v>718.5</v>
+        <v>1118.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1437</v>
+        <v>2237</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,16 +4027,16 @@
         <v>105</v>
       </c>
       <c r="B101" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C101" s="23">
-        <v>445</v>
+        <v>425</v>
       </c>
       <c r="D101" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E101" s="25">
-        <v>511.75</v>
+        <v>488.75</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4044,16 +4044,16 @@
         <v>106</v>
       </c>
       <c r="B102" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C102" s="23">
-        <v>418</v>
+        <v>378</v>
       </c>
       <c r="D102" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E102" s="25">
-        <v>480.7</v>
+        <v>434.7</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,10 +4061,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C103" s="23">
-        <v>-140</v>
+        <v>29</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4087,10 +4087,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C105" s="23">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4103,7 +4103,7 @@
         <v>6</v>
       </c>
       <c r="C106" s="23">
-        <v>297</v>
+        <v>346</v>
       </c>
       <c r="D106" s="27"/>
       <c r="E106" s="26"/>
@@ -4112,8 +4112,12 @@
       <c r="A107" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B107" s="22"/>
-      <c r="C107" s="26"/>
+      <c r="B107" s="22">
+        <v>1</v>
+      </c>
+      <c r="C107" s="23">
+        <v>28.5</v>
+      </c>
       <c r="D107" s="27"/>
       <c r="E107" s="26"/>
     </row>
@@ -4267,16 +4271,16 @@
         <v>121</v>
       </c>
       <c r="B117" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C117" s="23">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D117" s="24">
         <v>12.5</v>
       </c>
       <c r="E117" s="25">
-        <v>250</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4318,16 +4322,16 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C120" s="23">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D120" s="24">
         <v>12.5</v>
       </c>
       <c r="E120" s="25">
-        <v>50</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4854,16 +4858,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C152" s="23">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>159.6</v>
+        <v>137.19999999999999</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4871,16 +4875,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C153" s="23">
-        <v>72.5</v>
+        <v>73.5</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>199.38</v>
+        <v>202.13</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4905,16 +4909,16 @@
         <v>159</v>
       </c>
       <c r="B155" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C155" s="23">
-        <v>14.5</v>
+        <v>10.5</v>
       </c>
       <c r="D155" s="24">
         <v>4.7</v>
       </c>
       <c r="E155" s="25">
-        <v>68.150000000000006</v>
+        <v>49.35</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4922,16 +4926,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C156" s="23">
-        <v>214.25</v>
+        <v>213.25</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>728.45</v>
+        <v>725.05</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4956,16 +4960,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C158" s="23">
-        <v>109</v>
+        <v>108.5</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>294.3</v>
+        <v>292.95</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4973,16 +4977,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C159" s="23">
-        <v>139.5</v>
+        <v>138.5</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>390.6</v>
+        <v>387.8</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -5078,13 +5082,13 @@
         <v>29</v>
       </c>
       <c r="C165" s="23">
-        <v>48.5</v>
+        <v>236.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>143.08000000000001</v>
+        <v>697.68</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5095,13 +5099,13 @@
         <v>67</v>
       </c>
       <c r="C166" s="23">
-        <v>83</v>
+        <v>262</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>244.85</v>
+        <v>772.9</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5442,16 +5446,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C188" s="23">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D188" s="24">
         <v>4.5</v>
       </c>
       <c r="E188" s="25">
-        <v>427.5</v>
+        <v>423</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5493,16 +5497,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C191" s="23">
-        <v>231.5</v>
+        <v>230.5</v>
       </c>
       <c r="D191" s="24">
         <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>919.78</v>
+        <v>915.81</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5527,16 +5531,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C193" s="23">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5631,13 +5635,13 @@
         <v>121</v>
       </c>
       <c r="C200" s="23">
-        <v>48.24</v>
+        <v>249.24</v>
       </c>
       <c r="D200" s="24">
-        <v>3.09</v>
+        <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>148.84</v>
+        <v>766.01</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5822,16 +5826,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C214" s="23">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>815.48</v>
+        <v>811.36</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5890,16 +5894,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C218" s="23">
-        <v>85.5</v>
+        <v>82.5</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>371.15</v>
+        <v>358.13</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5946,16 +5950,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C222" s="23">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>891</v>
+        <v>855</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5980,16 +5984,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C224" s="23">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>551.25</v>
+        <v>540.75</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6083,13 +6087,13 @@
         <v>34</v>
       </c>
       <c r="C230" s="23">
-        <v>60.5</v>
+        <v>61.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>317.63</v>
+        <v>322.88</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6187,16 +6191,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C237" s="23">
-        <v>65</v>
+        <v>64.5</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6245,16 +6249,16 @@
         <v>245</v>
       </c>
       <c r="B241" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C241" s="23">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="D241" s="24">
         <v>6.75</v>
       </c>
       <c r="E241" s="25">
-        <v>43.88</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6362,16 +6366,16 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C248" s="23">
-        <v>55.5</v>
+        <v>53</v>
       </c>
       <c r="D248" s="24">
         <v>4.5</v>
       </c>
       <c r="E248" s="25">
-        <v>249.75</v>
+        <v>238.5</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6439,16 +6443,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C253" s="23">
-        <v>74.5</v>
+        <v>73.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>260.75</v>
+        <v>257.25</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6704,16 +6708,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C270" s="23">
-        <v>51.5</v>
+        <v>47.5</v>
       </c>
       <c r="D270" s="24">
         <v>5.4</v>
       </c>
       <c r="E270" s="25">
-        <v>278.10000000000002</v>
+        <v>256.5</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6815,16 +6819,16 @@
         <v>281</v>
       </c>
       <c r="B277" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C277" s="23">
-        <v>83.5</v>
+        <v>81.5</v>
       </c>
       <c r="D277" s="24">
         <v>6.25</v>
       </c>
       <c r="E277" s="25">
-        <v>521.88</v>
+        <v>509.38</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -7014,13 +7018,13 @@
         <v>41</v>
       </c>
       <c r="C289" s="23">
-        <v>16.5</v>
+        <v>42.5</v>
       </c>
       <c r="D289" s="24">
         <v>6.18</v>
       </c>
       <c r="E289" s="25">
-        <v>101.97</v>
+        <v>262.64999999999998</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7040,13 +7044,13 @@
         <v>69</v>
       </c>
       <c r="C291" s="23">
-        <v>15.5</v>
+        <v>16.5</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>95.79</v>
+        <v>101.97</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7162,13 +7166,13 @@
         <v>43</v>
       </c>
       <c r="C299" s="23">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D299" s="24">
         <v>6.18</v>
       </c>
       <c r="E299" s="25">
-        <v>395.52</v>
+        <v>401.7</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7502,16 +7506,16 @@
         <v>326</v>
       </c>
       <c r="B322" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C322" s="23">
-        <v>26.5</v>
+        <v>25.5</v>
       </c>
       <c r="D322" s="24">
         <v>9.31</v>
       </c>
       <c r="E322" s="25">
-        <v>246.78</v>
+        <v>237.47</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -8128,16 +8132,16 @@
         <v>364</v>
       </c>
       <c r="B360" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C360" s="23">
-        <v>20.5</v>
+        <v>5.5</v>
       </c>
       <c r="D360" s="24">
         <v>11</v>
       </c>
       <c r="E360" s="25">
-        <v>225.5</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -8403,13 +8407,13 @@
         <v>62</v>
       </c>
       <c r="C376" s="23">
-        <v>39.26</v>
+        <v>57.26</v>
       </c>
       <c r="D376" s="24">
         <v>9.5</v>
       </c>
       <c r="E376" s="25">
-        <v>372.97</v>
+        <v>543.97</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
@@ -8547,16 +8551,16 @@
         <v>389</v>
       </c>
       <c r="B385" s="22">
+        <v>6</v>
+      </c>
+      <c r="C385" s="23">
         <v>4</v>
-      </c>
-      <c r="C385" s="23">
-        <v>8.5</v>
       </c>
       <c r="D385" s="24">
         <v>11.4</v>
       </c>
       <c r="E385" s="25">
-        <v>96.9</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
@@ -8615,16 +8619,16 @@
         <v>393</v>
       </c>
       <c r="B389" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C389" s="23">
-        <v>29.25</v>
+        <v>27.75</v>
       </c>
       <c r="D389" s="24">
         <v>11.5</v>
       </c>
       <c r="E389" s="25">
-        <v>336.38</v>
+        <v>319.13</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
@@ -8749,16 +8753,16 @@
         <v>401</v>
       </c>
       <c r="B397" s="22">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C397" s="23">
-        <v>1.5</v>
+        <v>28</v>
       </c>
       <c r="D397" s="24">
         <v>10.93</v>
       </c>
       <c r="E397" s="25">
-        <v>16.399999999999999</v>
+        <v>306.04000000000002</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -9295,16 +9299,16 @@
         <v>435</v>
       </c>
       <c r="B431" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C431" s="23">
-        <v>71.5</v>
+        <v>70.5</v>
       </c>
       <c r="D431" s="24">
         <v>3.15</v>
       </c>
       <c r="E431" s="25">
-        <v>225.23</v>
+        <v>222.08</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -9312,16 +9316,16 @@
         <v>436</v>
       </c>
       <c r="B432" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C432" s="23">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D432" s="24">
         <v>3.05</v>
       </c>
       <c r="E432" s="25">
-        <v>122</v>
+        <v>112.85</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
@@ -9329,16 +9333,16 @@
         <v>437</v>
       </c>
       <c r="B433" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C433" s="23">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="D433" s="24">
         <v>3.25</v>
       </c>
       <c r="E433" s="25">
-        <v>84.5</v>
+        <v>79.63</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
@@ -9389,16 +9393,16 @@
         <v>441</v>
       </c>
       <c r="B437" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C437" s="23">
-        <v>16.5</v>
+        <v>13</v>
       </c>
       <c r="D437" s="24">
         <v>3.4</v>
       </c>
       <c r="E437" s="25">
-        <v>56.1</v>
+        <v>44.2</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -9558,16 +9562,16 @@
         <v>452</v>
       </c>
       <c r="B448" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C448" s="23">
-        <v>28.5</v>
+        <v>27.5</v>
       </c>
       <c r="D448" s="24">
         <v>3.8</v>
       </c>
       <c r="E448" s="25">
-        <v>108.3</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -9575,16 +9579,16 @@
         <v>453</v>
       </c>
       <c r="B449" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C449" s="23">
-        <v>31.5</v>
+        <v>27.5</v>
       </c>
       <c r="D449" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E449" s="25">
-        <v>130.74</v>
+        <v>114.14</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -9805,16 +9809,16 @@
         <v>467</v>
       </c>
       <c r="B463" s="22">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C463" s="23">
-        <v>78.5</v>
+        <v>76.5</v>
       </c>
       <c r="D463" s="24">
         <v>5.5</v>
       </c>
       <c r="E463" s="25">
-        <v>431.75</v>
+        <v>420.75</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -10120,16 +10124,16 @@
         <v>488</v>
       </c>
       <c r="B484" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C484" s="23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D484" s="24">
         <v>9.5</v>
       </c>
       <c r="E484" s="25">
-        <v>218.5</v>
+        <v>209</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
@@ -10401,16 +10405,16 @@
         <v>505</v>
       </c>
       <c r="B501" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C501" s="23">
-        <v>110.5</v>
+        <v>108</v>
       </c>
       <c r="D501" s="24">
         <v>1.38</v>
       </c>
       <c r="E501" s="25">
-        <v>152.30000000000001</v>
+        <v>148.85</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
@@ -10554,16 +10558,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C510" s="23">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D510" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E510" s="25">
-        <v>200.64</v>
+        <v>191.52</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10826,16 +10830,16 @@
         <v>532</v>
       </c>
       <c r="B528" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C528" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D528" s="24">
         <v>3.5</v>
       </c>
       <c r="E528" s="25">
-        <v>14</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -10843,16 +10847,16 @@
         <v>533</v>
       </c>
       <c r="B529" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C529" s="23">
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="D529" s="24">
         <v>3.5</v>
       </c>
       <c r="E529" s="25">
-        <v>106.75</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -10860,16 +10864,16 @@
         <v>534</v>
       </c>
       <c r="B530" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C530" s="23">
-        <v>64.5</v>
+        <v>62.5</v>
       </c>
       <c r="D530" s="24">
         <v>3.33</v>
       </c>
       <c r="E530" s="25">
-        <v>214.79</v>
+        <v>208.13</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -10920,16 +10924,16 @@
         <v>538</v>
       </c>
       <c r="B534" s="22">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C534" s="23">
-        <v>43</v>
+        <v>43.5</v>
       </c>
       <c r="D534" s="24">
         <v>3.6</v>
       </c>
       <c r="E534" s="25">
-        <v>154.80000000000001</v>
+        <v>156.6</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -11227,16 +11231,16 @@
         <v>557</v>
       </c>
       <c r="B553" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C553" s="23">
-        <v>29.62</v>
+        <v>27.62</v>
       </c>
       <c r="D553" s="24">
         <v>5</v>
       </c>
       <c r="E553" s="25">
-        <v>148.1</v>
+        <v>138.1</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11559,16 +11563,16 @@
         <v>577</v>
       </c>
       <c r="B573" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C573" s="23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D573" s="24">
         <v>10</v>
       </c>
       <c r="E573" s="25">
-        <v>70</v>
+        <v>20</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
@@ -11738,16 +11742,16 @@
         <v>588</v>
       </c>
       <c r="B584" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C584" s="23">
-        <v>78.5</v>
+        <v>76.5</v>
       </c>
       <c r="D584" s="24">
         <v>2.76</v>
       </c>
       <c r="E584" s="25">
-        <v>216.66</v>
+        <v>211.14</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11958,13 +11962,13 @@
         <v>56</v>
       </c>
       <c r="C597" s="23">
-        <v>392.5</v>
+        <v>536.5</v>
       </c>
       <c r="D597" s="24">
         <v>1.91</v>
       </c>
       <c r="E597" s="25">
-        <v>750.63</v>
+        <v>1024.75</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -11989,16 +11993,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C599" s="23">
-        <v>43.5</v>
+        <v>238.5</v>
       </c>
       <c r="D599" s="24">
-        <v>2.84</v>
+        <v>2.8</v>
       </c>
       <c r="E599" s="25">
-        <v>123.48</v>
+        <v>666.97</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12077,13 +12081,13 @@
         <v>48</v>
       </c>
       <c r="C604" s="23">
-        <v>508.5</v>
+        <v>518.5</v>
       </c>
       <c r="D604" s="24">
         <v>1.39</v>
       </c>
       <c r="E604" s="25">
-        <v>706.1</v>
+        <v>719.7</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12203,16 +12207,16 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C613" s="23">
-        <v>1105</v>
+        <v>1065</v>
       </c>
       <c r="D613" s="24">
         <v>0.83</v>
       </c>
       <c r="E613" s="25">
-        <v>911.63</v>
+        <v>878.63</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12237,16 +12241,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C615" s="23">
-        <v>285.5</v>
+        <v>275.5</v>
       </c>
       <c r="D615" s="24">
         <v>0.8</v>
       </c>
       <c r="E615" s="25">
-        <v>228.4</v>
+        <v>220.4</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12288,16 +12292,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C618" s="23">
-        <v>1873.5</v>
+        <v>1833.5</v>
       </c>
       <c r="D618" s="24">
         <v>0.52</v>
       </c>
       <c r="E618" s="25">
-        <v>974.22</v>
+        <v>953.42</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12305,16 +12309,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C619" s="23">
-        <v>1617</v>
+        <v>1607</v>
       </c>
       <c r="D619" s="24">
         <v>0.51</v>
       </c>
       <c r="E619" s="25">
-        <v>823.68</v>
+        <v>818.59</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12322,16 +12326,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C620" s="23">
-        <v>1434.5</v>
+        <v>1390.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.52</v>
       </c>
       <c r="E620" s="25">
-        <v>745.94</v>
+        <v>723.06</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12339,16 +12343,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C621" s="23">
-        <v>638</v>
+        <v>618</v>
       </c>
       <c r="D621" s="24">
         <v>0.5</v>
       </c>
       <c r="E621" s="25">
-        <v>319</v>
+        <v>309</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12373,16 +12377,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C623" s="23">
-        <v>972.5</v>
+        <v>952.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.7</v>
       </c>
       <c r="E623" s="25">
-        <v>680.75</v>
+        <v>666.75</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12390,16 +12394,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C624" s="23">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>171.5</v>
+        <v>170.1</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12407,16 +12411,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C625" s="23">
-        <v>247.5</v>
+        <v>225.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.68</v>
       </c>
       <c r="E625" s="25">
-        <v>169.53</v>
+        <v>154.46</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12450,16 +12454,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C628" s="23">
-        <v>1610.5</v>
+        <v>1590.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E628" s="25">
-        <v>886.23</v>
+        <v>875.22</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12484,16 +12488,16 @@
         <v>634</v>
       </c>
       <c r="B630" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C630" s="23">
-        <v>32.5</v>
+        <v>17.5</v>
       </c>
       <c r="D630" s="24">
         <v>4.5</v>
       </c>
       <c r="E630" s="25">
-        <v>146.25</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
@@ -12532,11 +12536,11 @@
       </c>
       <c r="B633" s="29"/>
       <c r="C633" s="30">
-        <v>54320.42</v>
+        <v>56524.42</v>
       </c>
       <c r="D633" s="31"/>
       <c r="E633" s="32">
-        <v>119341.45</v>
+        <v>123474.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:40
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 26-Feb-2025</t>
+    <t>1-Jul-2024 to 12-Mar-2025</t>
   </si>
   <si>
     <t/>
@@ -1055,7 +1055,7 @@
     <t>5935 PATRIKA {M}</t>
   </si>
   <si>
-    <t>5936 PATRIKA {M} (26.12 4K)</t>
+    <t>5936 PATRIKA {M}</t>
   </si>
   <si>
     <t>5937 PATRIKA (Dc) {{10}}</t>
@@ -1112,7 +1112,7 @@
     <t>6506 PATRIKA {L}</t>
   </si>
   <si>
-    <t>6507 PATRIKA (GGN) AGYA 3K</t>
+    <t>6507 PATRIKA (GGN)</t>
   </si>
   <si>
     <t>6508 PATRIKA {M}</t>
@@ -1142,7 +1142,7 @@
     <t>6516 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6517 PATRIKA {M}</t>
+    <t>6517 PATRIKA {M} (Dc)</t>
   </si>
   <si>
     <t>6518 PATRIKA {M}</t>
@@ -2597,16 +2597,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="23">
-        <v>738.5</v>
+        <v>733.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>670.48</v>
+        <v>665.94</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2614,16 +2614,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="23">
-        <v>68.5</v>
+        <v>66</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>113.03</v>
+        <v>108.9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2631,16 +2631,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="23">
-        <v>104.5</v>
+        <v>101.5</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>172.43</v>
+        <v>167.48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2648,16 +2648,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="23">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="24">
         <v>1.8</v>
       </c>
       <c r="E14" s="25">
-        <v>48.6</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,16 +2682,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="23">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>54</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,16 +2699,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C17" s="23">
-        <v>96.5</v>
+        <v>85</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>193</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2716,16 +2716,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C18" s="23">
-        <v>78.5</v>
+        <v>71.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2767,16 +2767,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="22">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="23">
-        <v>59.5</v>
+        <v>63.5</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
       </c>
       <c r="E21" s="25">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2784,33 +2784,27 @@
         <v>26</v>
       </c>
       <c r="B22" s="22">
-        <v>28</v>
-      </c>
-      <c r="C22" s="23">
-        <v>8</v>
-      </c>
-      <c r="D22" s="24">
-        <v>2</v>
-      </c>
-      <c r="E22" s="25">
-        <v>16</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="23">
-        <v>20.75</v>
+        <v>23.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>41.5</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2818,16 +2812,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24" s="23">
-        <v>102.5</v>
+        <v>99.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>215.25</v>
+        <v>208.95</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2861,16 +2855,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C27" s="23">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>253.8</v>
+        <v>209.15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2878,16 +2872,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="23">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>321.95</v>
+        <v>310.2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2895,16 +2889,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" s="23">
-        <v>45.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="D29" s="24">
         <v>2.59</v>
       </c>
       <c r="E29" s="25">
-        <v>118.43</v>
+        <v>100.33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2912,16 +2906,16 @@
         <v>34</v>
       </c>
       <c r="B30" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C30" s="23">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D30" s="24">
         <v>2.5499999999999998</v>
       </c>
       <c r="E30" s="25">
-        <v>66.3</v>
+        <v>56.1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,16 +2960,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34" s="23">
-        <v>145</v>
+        <v>141.5</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>362.5</v>
+        <v>353.75</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3026,16 +3020,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C38" s="23">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>386.1</v>
+        <v>361.8</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,16 +3037,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" s="23">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>413.1</v>
+        <v>407.7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3094,16 +3088,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42" s="23">
-        <v>45.5</v>
+        <v>27.5</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>129.68</v>
+        <v>78.38</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3128,16 +3122,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="23">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>153</v>
+        <v>148.5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3162,16 +3156,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C46" s="23">
-        <v>112.5</v>
+        <v>109.5</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>264.38</v>
+        <v>257.33</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,13 +3176,13 @@
         <v>38</v>
       </c>
       <c r="C47" s="23">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D47" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E47" s="25">
-        <v>57.2</v>
+        <v>63.8</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,13 +3193,13 @@
         <v>27</v>
       </c>
       <c r="C48" s="23">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D48" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E48" s="25">
-        <v>217.8</v>
+        <v>224.4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3213,16 +3207,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C49" s="23">
-        <v>681.5</v>
+        <v>656.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>749.65</v>
+        <v>722.15</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3230,16 +3224,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C50" s="23">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D50" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>498.3</v>
+        <v>493.9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3250,13 +3244,13 @@
         <v>34</v>
       </c>
       <c r="C51" s="23">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D51" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E51" s="25">
-        <v>140.80000000000001</v>
+        <v>147.4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3264,16 +3258,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C52" s="23">
-        <v>151.5</v>
+        <v>146.5</v>
       </c>
       <c r="D52" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>166.65</v>
+        <v>161.15</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3298,16 +3292,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C54" s="23">
-        <v>717</v>
+        <v>705</v>
       </c>
       <c r="D54" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>788.7</v>
+        <v>775.5</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3332,16 +3326,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C56" s="23">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>370.7</v>
+        <v>357.5</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3349,16 +3343,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C57" s="23">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>860.7</v>
+        <v>856.9</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3381,16 +3375,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C59" s="23">
-        <v>147.5</v>
+        <v>141.5</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>280.25</v>
+        <v>268.85000000000002</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3447,16 +3441,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C63" s="23">
-        <v>84.5</v>
+        <v>82.5</v>
       </c>
       <c r="D63" s="24">
         <v>2.1</v>
       </c>
       <c r="E63" s="25">
-        <v>177.45</v>
+        <v>173.25</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,16 +3458,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C64" s="23">
-        <v>259.5</v>
+        <v>256.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>544.95000000000005</v>
+        <v>538.65</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3532,16 +3526,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C68" s="23">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>198.1</v>
+        <v>194.6</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3566,16 +3560,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C70" s="23">
-        <v>215</v>
+        <v>180</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>193.5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,16 +3577,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C71" s="23">
-        <v>221.5</v>
+        <v>218.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>199.35</v>
+        <v>196.65</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3600,16 +3594,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C72" s="23">
-        <v>2475</v>
+        <v>2442</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3836.25</v>
+        <v>3785.1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3617,16 +3611,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C73" s="23">
-        <v>1856.5</v>
+        <v>1779</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2877.58</v>
+        <v>2757.45</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3634,16 +3628,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C74" s="23">
-        <v>1449.5</v>
+        <v>1389.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>2246.73</v>
+        <v>2153.73</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3665,13 +3659,13 @@
         <v>67</v>
       </c>
       <c r="C76" s="23">
-        <v>51.5</v>
+        <v>261.5</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>16.57</v>
+        <v>84.01</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,10 +3686,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C78" s="23">
-        <v>502.5</v>
+        <v>648.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3718,10 +3712,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C80" s="23">
-        <v>179</v>
+        <v>242</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3757,16 +3751,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C83" s="23">
-        <v>532</v>
+        <v>334</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>611.79999999999995</v>
+        <v>384.1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3774,16 +3768,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C84" s="23">
-        <v>669</v>
+        <v>649</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>769.35</v>
+        <v>746.35</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3791,16 +3785,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C85" s="23">
-        <v>4601</v>
+        <v>4550</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>6441.4</v>
+        <v>6370</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,16 +3802,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C86" s="23">
-        <v>2885.5</v>
+        <v>2880.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>4039.7</v>
+        <v>4032.7</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3825,16 +3819,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C87" s="23">
-        <v>1175</v>
+        <v>1138</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1645</v>
+        <v>1593.2</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3851,16 +3845,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C89" s="23">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1730</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,16 +3862,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C90" s="23">
-        <v>1117</v>
+        <v>1115.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2234</v>
+        <v>2231</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3885,16 +3879,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C91" s="23">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>530.46</v>
+        <v>507.78</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3902,16 +3896,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C92" s="23">
-        <v>608.5</v>
+        <v>598.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>766.71</v>
+        <v>754.11</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4065,10 +4059,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C103" s="23">
-        <v>9</v>
+        <v>715</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4081,7 +4075,7 @@
         <v>4</v>
       </c>
       <c r="C104" s="23">
-        <v>-10</v>
+        <v>58</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4094,7 +4088,7 @@
         <v>7</v>
       </c>
       <c r="C105" s="23">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4190,16 +4184,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C112" s="23">
-        <v>19</v>
+        <v>12.5</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>237.5</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4224,16 +4218,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C114" s="23">
-        <v>17.5</v>
+        <v>12.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>218.75</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4241,16 +4235,16 @@
         <v>119</v>
       </c>
       <c r="B115" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C115" s="23">
-        <v>23</v>
+        <v>21.5</v>
       </c>
       <c r="D115" s="24">
         <v>12.5</v>
       </c>
       <c r="E115" s="25">
-        <v>287.5</v>
+        <v>268.75</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4343,16 +4337,16 @@
         <v>125</v>
       </c>
       <c r="B121" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C121" s="23">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>68.75</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4371,17 +4365,11 @@
         <v>127</v>
       </c>
       <c r="B123" s="22">
-        <v>11</v>
-      </c>
-      <c r="C123" s="23">
-        <v>1</v>
-      </c>
-      <c r="D123" s="24">
-        <v>15.5</v>
-      </c>
-      <c r="E123" s="25">
-        <v>15.5</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C123" s="26"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="26"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
@@ -4422,16 +4410,16 @@
         <v>130</v>
       </c>
       <c r="B126" s="22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C126" s="23">
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="D126" s="24">
         <v>15.5</v>
       </c>
       <c r="E126" s="25">
-        <v>224.75</v>
+        <v>240.25</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4709,16 +4697,16 @@
         <v>147</v>
       </c>
       <c r="B143" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C143" s="23">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="D143" s="24">
         <v>18.420000000000002</v>
       </c>
       <c r="E143" s="25">
-        <v>165.79</v>
+        <v>101.32</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4828,16 +4816,16 @@
         <v>154</v>
       </c>
       <c r="B150" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C150" s="23">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D150" s="24">
         <v>14.5</v>
       </c>
       <c r="E150" s="25">
-        <v>65.25</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4862,16 +4850,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C152" s="23">
-        <v>119.5</v>
+        <v>110</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>334.6</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4879,16 +4867,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C153" s="23">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>143</v>
+        <v>123.75</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4896,16 +4884,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C154" s="23">
-        <v>2.85</v>
+        <v>1.85</v>
       </c>
       <c r="D154" s="24">
         <v>2.75</v>
       </c>
       <c r="E154" s="25">
-        <v>7.84</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4913,16 +4901,16 @@
         <v>159</v>
       </c>
       <c r="B155" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C155" s="23">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D155" s="24">
         <v>4.7</v>
       </c>
       <c r="E155" s="25">
-        <v>28.2</v>
+        <v>25.85</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4930,16 +4918,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C156" s="23">
-        <v>200.25</v>
+        <v>194.75</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>680.85</v>
+        <v>662.15</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4992,16 +4980,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C160" s="23">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>327.60000000000002</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5009,16 +4997,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C161" s="23">
-        <v>58.5</v>
+        <v>56.5</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>146.25</v>
+        <v>141.25</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5179,16 +5167,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C171" s="23">
-        <v>243</v>
+        <v>240.5</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>850.5</v>
+        <v>841.75</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5205,16 +5193,16 @@
         <v>177</v>
       </c>
       <c r="B173" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C173" s="23">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D173" s="24">
         <v>3.9</v>
       </c>
       <c r="E173" s="25">
-        <v>222.3</v>
+        <v>210.6</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5254,16 +5242,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C176" s="23">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>246.42</v>
+        <v>216.45</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5299,16 +5287,16 @@
         <v>183</v>
       </c>
       <c r="B179" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C179" s="23">
-        <v>107.5</v>
+        <v>103</v>
       </c>
       <c r="D179" s="24">
         <v>3.6</v>
       </c>
       <c r="E179" s="25">
-        <v>387</v>
+        <v>370.8</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5342,16 +5330,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C182" s="23">
-        <v>60.5</v>
+        <v>58</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>229.9</v>
+        <v>220.4</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5376,16 +5364,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C184" s="23">
-        <v>117</v>
+        <v>108.5</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>526.5</v>
+        <v>488.25</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5444,16 +5432,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C188" s="23">
-        <v>101.5</v>
+        <v>98.5</v>
       </c>
       <c r="D188" s="24">
         <v>4.5</v>
       </c>
       <c r="E188" s="25">
-        <v>456.75</v>
+        <v>443.25</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5478,16 +5466,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C190" s="23">
-        <v>57</v>
+        <v>53.5</v>
       </c>
       <c r="D190" s="24">
         <v>3.93</v>
       </c>
       <c r="E190" s="25">
-        <v>224.02</v>
+        <v>210.26</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5495,16 +5483,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C191" s="23">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D191" s="24">
         <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>858.2</v>
+        <v>838.33</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5630,16 +5618,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C200" s="23">
-        <v>248.24</v>
+        <v>246.24</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>762.94</v>
+        <v>756.79</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5734,16 +5722,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C208" s="23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>22.8</v>
+        <v>30.4</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5807,16 +5795,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C213" s="23">
-        <v>61</v>
+        <v>48.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>251.09</v>
+        <v>199.64</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5824,16 +5812,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C214" s="23">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>675.45</v>
+        <v>663.09</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5948,16 +5936,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C222" s="23">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>774</v>
+        <v>769.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5965,16 +5953,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C223" s="23">
-        <v>90</v>
+        <v>91.5</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>405</v>
+        <v>411.75</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5982,16 +5970,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C224" s="23">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>514.5</v>
+        <v>488.25</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6016,16 +6004,16 @@
         <v>230</v>
       </c>
       <c r="B226" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C226" s="23">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D226" s="24">
         <v>4.8</v>
       </c>
       <c r="E226" s="25">
-        <v>196.8</v>
+        <v>177.6</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6033,16 +6021,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C227" s="23">
-        <v>44.5</v>
+        <v>43</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>200.25</v>
+        <v>193.5</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6099,16 +6087,16 @@
         <v>235</v>
       </c>
       <c r="B231" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C231" s="23">
-        <v>101.5</v>
+        <v>100.5</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>532.88</v>
+        <v>527.63</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6230,16 +6218,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C240" s="23">
-        <v>101.3</v>
+        <v>100.3</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>577.41</v>
+        <v>571.71</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6296,16 +6284,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C244" s="23">
-        <v>72.91</v>
+        <v>77.91</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>436.01</v>
+        <v>465.91</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6313,16 +6301,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C245" s="23">
-        <v>41.5</v>
+        <v>38</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>176.79</v>
+        <v>161.88</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6396,16 +6384,16 @@
         <v>254</v>
       </c>
       <c r="B250" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C250" s="23">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D250" s="24">
         <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>139.19</v>
+        <v>123.72</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6441,16 +6429,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C253" s="23">
-        <v>104.5</v>
+        <v>97</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>365.75</v>
+        <v>339.5</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6535,16 +6523,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C259" s="23">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>937.32</v>
+        <v>911.64</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6552,16 +6540,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C260" s="23">
-        <v>56.5</v>
+        <v>53</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>241.82</v>
+        <v>226.84</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6672,16 +6660,16 @@
         <v>272</v>
       </c>
       <c r="B268" s="22">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C268" s="23">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D268" s="24">
         <v>5.0999999999999996</v>
       </c>
       <c r="E268" s="25">
-        <v>275.39999999999998</v>
+        <v>280.5</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6706,16 +6694,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C270" s="23">
-        <v>47.5</v>
+        <v>45.5</v>
       </c>
       <c r="D270" s="24">
         <v>5.4</v>
       </c>
       <c r="E270" s="25">
-        <v>256.5</v>
+        <v>245.7</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6740,16 +6728,16 @@
         <v>276</v>
       </c>
       <c r="B272" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C272" s="23">
-        <v>74.5</v>
+        <v>68.5</v>
       </c>
       <c r="D272" s="24">
         <v>5.55</v>
       </c>
       <c r="E272" s="25">
-        <v>413.48</v>
+        <v>380.18</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6905,13 +6893,13 @@
         <v>99</v>
       </c>
       <c r="C282" s="23">
-        <v>54.88</v>
+        <v>52.88</v>
       </c>
       <c r="D282" s="24">
         <v>5.94</v>
       </c>
       <c r="E282" s="25">
-        <v>325.99</v>
+        <v>314.11</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6936,16 +6924,16 @@
         <v>288</v>
       </c>
       <c r="B284" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C284" s="23">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D284" s="24">
         <v>5.94</v>
       </c>
       <c r="E284" s="25">
-        <v>302.94</v>
+        <v>291.06</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -7101,16 +7089,16 @@
         <v>299</v>
       </c>
       <c r="B295" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C295" s="23">
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="D295" s="24">
         <v>6.46</v>
       </c>
       <c r="E295" s="25">
-        <v>113.05</v>
+        <v>106.59</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -7187,16 +7175,16 @@
         <v>305</v>
       </c>
       <c r="B301" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C301" s="23">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D301" s="24">
         <v>7.12</v>
       </c>
       <c r="E301" s="25">
-        <v>213.74</v>
+        <v>163.87</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7224,13 +7212,13 @@
         <v>23</v>
       </c>
       <c r="C303" s="23">
-        <v>70</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="D303" s="24">
         <v>7.13</v>
       </c>
       <c r="E303" s="25">
-        <v>499.1</v>
+        <v>487.69</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7238,16 +7226,16 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C304" s="23">
-        <v>17.5</v>
+        <v>14.5</v>
       </c>
       <c r="D304" s="24">
         <v>7.13</v>
       </c>
       <c r="E304" s="25">
-        <v>124.78</v>
+        <v>103.39</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7346,16 +7334,16 @@
         <v>316</v>
       </c>
       <c r="B312" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C312" s="23">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D312" s="24">
         <v>8.08</v>
       </c>
       <c r="E312" s="25">
-        <v>185.84</v>
+        <v>169.68</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -7389,16 +7377,16 @@
         <v>319</v>
       </c>
       <c r="B315" s="22">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C315" s="23">
-        <v>17.5</v>
+        <v>19.5</v>
       </c>
       <c r="D315" s="24">
         <v>8.08</v>
       </c>
       <c r="E315" s="25">
-        <v>141.4</v>
+        <v>157.56</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -7466,16 +7454,16 @@
         <v>324</v>
       </c>
       <c r="B320" s="22">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C320" s="23">
-        <v>19.5</v>
+        <v>22.5</v>
       </c>
       <c r="D320" s="24">
         <v>9.25</v>
       </c>
       <c r="E320" s="25">
-        <v>180.38</v>
+        <v>208.13</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -7517,16 +7505,16 @@
         <v>327</v>
       </c>
       <c r="B323" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C323" s="23">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D323" s="24">
         <v>9</v>
       </c>
       <c r="E323" s="25">
-        <v>117</v>
+        <v>81</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7571,13 +7559,13 @@
         <v>2</v>
       </c>
       <c r="C326" s="23">
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="D326" s="24">
         <v>11</v>
       </c>
       <c r="E326" s="25">
-        <v>99</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -7636,16 +7624,16 @@
         <v>334</v>
       </c>
       <c r="B330" s="22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C330" s="23">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D330" s="24">
         <v>8.33</v>
       </c>
       <c r="E330" s="25">
-        <v>125</v>
+        <v>141.66999999999999</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -7653,16 +7641,16 @@
         <v>335</v>
       </c>
       <c r="B331" s="22">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C331" s="23">
-        <v>102.5</v>
+        <v>105</v>
       </c>
       <c r="D331" s="24">
         <v>5.5</v>
       </c>
       <c r="E331" s="25">
-        <v>563.75</v>
+        <v>577.5</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7687,16 +7675,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C333" s="23">
-        <v>33.5</v>
+        <v>31.5</v>
       </c>
       <c r="D333" s="24">
         <v>6.9</v>
       </c>
       <c r="E333" s="25">
-        <v>231.15</v>
+        <v>217.35</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7704,16 +7692,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C334" s="23">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D334" s="24">
         <v>7.13</v>
       </c>
       <c r="E334" s="25">
-        <v>235.29</v>
+        <v>242.42</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7789,16 +7777,16 @@
         <v>343</v>
       </c>
       <c r="B339" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C339" s="23">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D339" s="24">
         <v>7.84</v>
       </c>
       <c r="E339" s="25">
-        <v>227.36</v>
+        <v>219.52</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -7846,13 +7834,13 @@
         <v>18</v>
       </c>
       <c r="C343" s="23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D343" s="24">
         <v>6.51</v>
       </c>
       <c r="E343" s="25">
-        <v>97.66</v>
+        <v>91.15</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -7871,16 +7859,16 @@
         <v>349</v>
       </c>
       <c r="B345" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C345" s="23">
-        <v>78.5</v>
+        <v>77</v>
       </c>
       <c r="D345" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E345" s="25">
-        <v>384.65</v>
+        <v>377.3</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -7939,16 +7927,16 @@
         <v>353</v>
       </c>
       <c r="B349" s="22">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C349" s="23">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D349" s="24">
         <v>8.67</v>
       </c>
       <c r="E349" s="25">
-        <v>320.93</v>
+        <v>268.88</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -8109,16 +8097,16 @@
         <v>363</v>
       </c>
       <c r="B359" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C359" s="23">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="D359" s="24">
         <v>11</v>
       </c>
       <c r="E359" s="25">
-        <v>176</v>
+        <v>170.5</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -8143,16 +8131,16 @@
         <v>365</v>
       </c>
       <c r="B361" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C361" s="23">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="D361" s="24">
         <v>39</v>
       </c>
       <c r="E361" s="25">
-        <v>253.5</v>
+        <v>234</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8194,16 +8182,16 @@
         <v>368</v>
       </c>
       <c r="B364" s="22">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C364" s="23">
-        <v>15.5</v>
+        <v>17.5</v>
       </c>
       <c r="D364" s="24">
         <v>7.84</v>
       </c>
       <c r="E364" s="25">
-        <v>121.52</v>
+        <v>137.19999999999999</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -8262,16 +8250,16 @@
         <v>372</v>
       </c>
       <c r="B368" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C368" s="23">
-        <v>1.5</v>
+        <v>-1</v>
       </c>
       <c r="D368" s="24">
         <v>13.5</v>
       </c>
       <c r="E368" s="25">
-        <v>20.25</v>
+        <v>-13.5</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -8313,16 +8301,16 @@
         <v>375</v>
       </c>
       <c r="B371" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C371" s="23">
-        <v>17</v>
+        <v>15.5</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8330,16 +8318,16 @@
         <v>376</v>
       </c>
       <c r="B372" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C372" s="23">
-        <v>9.5</v>
+        <v>6</v>
       </c>
       <c r="D372" s="24">
         <v>10.5</v>
       </c>
       <c r="E372" s="25">
-        <v>99.75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -8347,16 +8335,16 @@
         <v>377</v>
       </c>
       <c r="B373" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C373" s="23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D373" s="24">
         <v>13.5</v>
       </c>
       <c r="E373" s="25">
-        <v>108</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
@@ -8381,16 +8369,16 @@
         <v>379</v>
       </c>
       <c r="B375" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C375" s="23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D375" s="24">
         <v>10.5</v>
       </c>
       <c r="E375" s="25">
-        <v>84</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
@@ -8500,16 +8488,16 @@
         <v>386</v>
       </c>
       <c r="B382" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C382" s="23">
-        <v>14.49</v>
+        <v>9.99</v>
       </c>
       <c r="D382" s="24">
         <v>25</v>
       </c>
       <c r="E382" s="25">
-        <v>362.25</v>
+        <v>249.75</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -8562,16 +8550,16 @@
         <v>390</v>
       </c>
       <c r="B386" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C386" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D386" s="24">
         <v>12.5</v>
       </c>
       <c r="E386" s="25">
-        <v>50</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8747,16 +8735,16 @@
         <v>401</v>
       </c>
       <c r="B397" s="22">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C397" s="23">
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="D397" s="24">
         <v>10.93</v>
       </c>
       <c r="E397" s="25">
-        <v>256.86</v>
+        <v>267.79000000000002</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8866,16 +8854,16 @@
         <v>408</v>
       </c>
       <c r="B404" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C404" s="23">
-        <v>45.5</v>
+        <v>42</v>
       </c>
       <c r="D404" s="24">
         <v>2.1</v>
       </c>
       <c r="E404" s="25">
-        <v>95.55</v>
+        <v>88.2</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
@@ -8883,16 +8871,16 @@
         <v>409</v>
       </c>
       <c r="B405" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C405" s="23">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D405" s="24">
         <v>2</v>
       </c>
       <c r="E405" s="25">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
@@ -8909,16 +8897,16 @@
         <v>411</v>
       </c>
       <c r="B407" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C407" s="23">
-        <v>33</v>
+        <v>31.5</v>
       </c>
       <c r="D407" s="24">
         <v>2</v>
       </c>
       <c r="E407" s="25">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -8978,16 +8966,16 @@
         <v>416</v>
       </c>
       <c r="B412" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C412" s="23">
-        <v>54.5</v>
+        <v>51.5</v>
       </c>
       <c r="D412" s="24">
         <v>2.25</v>
       </c>
       <c r="E412" s="25">
-        <v>122.63</v>
+        <v>115.88</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -9029,16 +9017,16 @@
         <v>419</v>
       </c>
       <c r="B415" s="22">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C415" s="23">
-        <v>40.5</v>
+        <v>41.5</v>
       </c>
       <c r="D415" s="24">
         <v>2.5</v>
       </c>
       <c r="E415" s="25">
-        <v>101.25</v>
+        <v>103.75</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
@@ -9063,16 +9051,16 @@
         <v>421</v>
       </c>
       <c r="B417" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C417" s="23">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D417" s="24">
         <v>2.7</v>
       </c>
       <c r="E417" s="25">
-        <v>121.5</v>
+        <v>137.69999999999999</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
@@ -9114,16 +9102,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C420" s="23">
-        <v>34</v>
+        <v>32.5</v>
       </c>
       <c r="D420" s="24">
         <v>2.75</v>
       </c>
       <c r="E420" s="25">
-        <v>93.5</v>
+        <v>89.38</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9131,16 +9119,16 @@
         <v>425</v>
       </c>
       <c r="B421" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C421" s="23">
-        <v>34</v>
+        <v>30.5</v>
       </c>
       <c r="D421" s="24">
         <v>3.8</v>
       </c>
       <c r="E421" s="25">
-        <v>129.19999999999999</v>
+        <v>115.9</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
@@ -9191,16 +9179,16 @@
         <v>429</v>
       </c>
       <c r="B425" s="22">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C425" s="23">
-        <v>164.34</v>
+        <v>159.84</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>460.15</v>
+        <v>447.55</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9370,16 +9358,16 @@
         <v>440</v>
       </c>
       <c r="B436" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C436" s="23">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D436" s="24">
         <v>3.25</v>
       </c>
       <c r="E436" s="25">
-        <v>139.75</v>
+        <v>136.5</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
@@ -9387,16 +9375,16 @@
         <v>441</v>
       </c>
       <c r="B437" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C437" s="23">
-        <v>12</v>
+        <v>9.5</v>
       </c>
       <c r="D437" s="24">
         <v>3.4</v>
       </c>
       <c r="E437" s="25">
-        <v>40.799999999999997</v>
+        <v>32.299999999999997</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -9419,16 +9407,16 @@
         <v>443</v>
       </c>
       <c r="B439" s="22">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C439" s="23">
-        <v>58.46</v>
+        <v>55.46</v>
       </c>
       <c r="D439" s="24">
         <v>3.5</v>
       </c>
       <c r="E439" s="25">
-        <v>204.61</v>
+        <v>194.11</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
@@ -9539,16 +9527,16 @@
         <v>451</v>
       </c>
       <c r="B447" s="22">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C447" s="23">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D447" s="24">
         <v>4.25</v>
       </c>
       <c r="E447" s="25">
-        <v>174.25</v>
+        <v>191.25</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9803,16 +9791,16 @@
         <v>467</v>
       </c>
       <c r="B463" s="22">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C463" s="23">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D463" s="24">
         <v>5.5</v>
       </c>
       <c r="E463" s="25">
-        <v>401.5</v>
+        <v>390.5</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -9945,16 +9933,16 @@
         <v>477</v>
       </c>
       <c r="B473" s="22">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C473" s="23">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D473" s="24">
         <v>7.13</v>
       </c>
       <c r="E473" s="25">
-        <v>163.99</v>
+        <v>121.21</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
@@ -9996,16 +9984,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C476" s="23">
-        <v>36.5</v>
+        <v>34</v>
       </c>
       <c r="D476" s="24">
         <v>7.6</v>
       </c>
       <c r="E476" s="25">
-        <v>277.39999999999998</v>
+        <v>258.39999999999998</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10030,16 +10018,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C478" s="23">
-        <v>22.5</v>
+        <v>19.5</v>
       </c>
       <c r="D478" s="24">
         <v>7.5</v>
       </c>
       <c r="E478" s="25">
-        <v>168.75</v>
+        <v>146.25</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -10218,16 +10206,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C490" s="23">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>543.4</v>
+        <v>546.70000000000005</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10235,16 +10223,16 @@
         <v>495</v>
       </c>
       <c r="B491" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C491" s="23">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D491" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E491" s="25">
-        <v>426.8</v>
+        <v>425.7</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -10269,16 +10257,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C493" s="23">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D493" s="24">
         <v>1.4</v>
       </c>
       <c r="E493" s="25">
-        <v>373.8</v>
+        <v>372.4</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10303,16 +10291,16 @@
         <v>499</v>
       </c>
       <c r="B495" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C495" s="23">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D495" s="24">
         <v>1.4</v>
       </c>
       <c r="E495" s="25">
-        <v>515.20000000000005</v>
+        <v>506.8</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10365,16 +10353,16 @@
         <v>503</v>
       </c>
       <c r="B499" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C499" s="23">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="D499" s="24">
         <v>1.55</v>
       </c>
       <c r="E499" s="25">
-        <v>494.45</v>
+        <v>432.45</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10399,16 +10387,16 @@
         <v>505</v>
       </c>
       <c r="B501" s="22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C501" s="23">
-        <v>108</v>
+        <v>104.5</v>
       </c>
       <c r="D501" s="24">
         <v>1.38</v>
       </c>
       <c r="E501" s="25">
-        <v>148.85</v>
+        <v>144.03</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
@@ -10433,16 +10421,16 @@
         <v>507</v>
       </c>
       <c r="B503" s="22">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C503" s="23">
-        <v>660</v>
+        <v>655.5</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>990</v>
+        <v>983.25</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10501,16 +10489,16 @@
         <v>511</v>
       </c>
       <c r="B507" s="22">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C507" s="23">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="D507" s="24">
         <v>1.71</v>
       </c>
       <c r="E507" s="25">
-        <v>38.479999999999997</v>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10535,16 +10523,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C509" s="23">
-        <v>177.2</v>
+        <v>180.2</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>404.02</v>
+        <v>410.86</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10552,16 +10540,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C510" s="23">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D510" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E510" s="25">
-        <v>483.36</v>
+        <v>462.84</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10612,16 +10600,16 @@
         <v>518</v>
       </c>
       <c r="B514" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C514" s="23">
-        <v>51.5</v>
+        <v>48.5</v>
       </c>
       <c r="D514" s="24">
         <v>2.73</v>
       </c>
       <c r="E514" s="25">
-        <v>140.81</v>
+        <v>132.6</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
@@ -10629,16 +10617,16 @@
         <v>519</v>
       </c>
       <c r="B515" s="22">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C515" s="23">
-        <v>129.5</v>
+        <v>127.5</v>
       </c>
       <c r="D515" s="24">
         <v>2.8</v>
       </c>
       <c r="E515" s="25">
-        <v>362.6</v>
+        <v>357</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -10824,16 +10812,16 @@
         <v>532</v>
       </c>
       <c r="B528" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C528" s="23">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="D528" s="24">
         <v>3.5</v>
       </c>
       <c r="E528" s="25">
-        <v>68.25</v>
+        <v>64.75</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -10841,16 +10829,16 @@
         <v>533</v>
       </c>
       <c r="B529" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C529" s="23">
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="D529" s="24">
         <v>3.5</v>
       </c>
       <c r="E529" s="25">
-        <v>89.25</v>
+        <v>84</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -10884,16 +10872,16 @@
         <v>536</v>
       </c>
       <c r="B532" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C532" s="23">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D532" s="24">
         <v>3.8</v>
       </c>
       <c r="E532" s="25">
-        <v>155.80000000000001</v>
+        <v>148.19999999999999</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -10918,16 +10906,16 @@
         <v>538</v>
       </c>
       <c r="B534" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C534" s="23">
-        <v>41.5</v>
+        <v>41</v>
       </c>
       <c r="D534" s="24">
         <v>3.6</v>
       </c>
       <c r="E534" s="25">
-        <v>149.4</v>
+        <v>147.6</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -11021,16 +11009,16 @@
         <v>545</v>
       </c>
       <c r="B541" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C541" s="23">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D541" s="24">
         <v>4</v>
       </c>
       <c r="E541" s="25">
-        <v>252</v>
+        <v>216</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -11191,16 +11179,16 @@
         <v>555</v>
       </c>
       <c r="B551" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C551" s="23">
-        <v>24.5</v>
+        <v>21</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>116.38</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11208,16 +11196,16 @@
         <v>556</v>
       </c>
       <c r="B552" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C552" s="23">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="D552" s="24">
         <v>4.75</v>
       </c>
       <c r="E552" s="25">
-        <v>40.380000000000003</v>
+        <v>26.13</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11225,16 +11213,16 @@
         <v>557</v>
       </c>
       <c r="B553" s="22">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C553" s="23">
-        <v>20.62</v>
+        <v>22.12</v>
       </c>
       <c r="D553" s="24">
         <v>5</v>
       </c>
       <c r="E553" s="25">
-        <v>103.1</v>
+        <v>110.6</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11276,16 +11264,16 @@
         <v>560</v>
       </c>
       <c r="B556" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C556" s="23">
-        <v>31.5</v>
+        <v>30</v>
       </c>
       <c r="D556" s="24">
         <v>5</v>
       </c>
       <c r="E556" s="25">
-        <v>157.5</v>
+        <v>150</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
@@ -11310,16 +11298,16 @@
         <v>562</v>
       </c>
       <c r="B558" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C558" s="23">
-        <v>61.5</v>
+        <v>31.5</v>
       </c>
       <c r="D558" s="24">
         <v>5.5</v>
       </c>
       <c r="E558" s="25">
-        <v>338.25</v>
+        <v>173.25</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11560,13 +11548,13 @@
         <v>22</v>
       </c>
       <c r="C573" s="23">
-        <v>-10</v>
+        <v>-1.5</v>
       </c>
       <c r="D573" s="24">
         <v>10</v>
       </c>
       <c r="E573" s="25">
-        <v>-100</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
@@ -11651,16 +11639,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C579" s="23">
-        <v>75.739999999999995</v>
+        <v>71.739999999999995</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>208.79</v>
+        <v>197.76</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11802,16 +11790,16 @@
         <v>592</v>
       </c>
       <c r="B588" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C588" s="23">
-        <v>32.5</v>
+        <v>30.5</v>
       </c>
       <c r="D588" s="24">
         <v>3.1</v>
       </c>
       <c r="E588" s="25">
-        <v>100.75</v>
+        <v>94.55</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -11856,13 +11844,13 @@
         <v>9</v>
       </c>
       <c r="C591" s="23">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="D591" s="24">
         <v>4</v>
       </c>
       <c r="E591" s="25">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -11919,16 +11907,16 @@
         <v>599</v>
       </c>
       <c r="B595" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C595" s="23">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D595" s="24">
         <v>4.95</v>
       </c>
       <c r="E595" s="25">
-        <v>138.47999999999999</v>
+        <v>113.75</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -11953,16 +11941,16 @@
         <v>601</v>
       </c>
       <c r="B597" s="22">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C597" s="23">
-        <v>463.5</v>
+        <v>466.5</v>
       </c>
       <c r="D597" s="24">
         <v>1.91</v>
       </c>
       <c r="E597" s="25">
-        <v>885.31</v>
+        <v>891.04</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -11970,7 +11958,7 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C598" s="23">
         <v>148.5</v>
@@ -11987,16 +11975,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C599" s="23">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D599" s="24">
         <v>2.8</v>
       </c>
       <c r="E599" s="25">
-        <v>659.98</v>
+        <v>640.41</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12106,16 +12094,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C606" s="23">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>-30.8</v>
+        <v>-32.200000000000003</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12123,10 +12111,10 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C607" s="23">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D607" s="27"/>
       <c r="E607" s="26"/>
@@ -12149,10 +12137,10 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C609" s="23">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D609" s="27"/>
       <c r="E609" s="26"/>
@@ -12178,7 +12166,7 @@
         <v>5</v>
       </c>
       <c r="C611" s="23">
-        <v>425</v>
+        <v>735</v>
       </c>
       <c r="D611" s="27"/>
       <c r="E611" s="26"/>
@@ -12218,16 +12206,16 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C614" s="23">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="D614" s="24">
         <v>0.8</v>
       </c>
       <c r="E614" s="25">
-        <v>336.8</v>
+        <v>328.8</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12286,16 +12274,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C618" s="23">
-        <v>1787</v>
+        <v>1777</v>
       </c>
       <c r="D618" s="24">
         <v>0.52</v>
       </c>
       <c r="E618" s="25">
-        <v>929.24</v>
+        <v>924.04</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12320,16 +12308,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="C620" s="23">
-        <v>1257.5</v>
+        <v>1234.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.52</v>
       </c>
       <c r="E620" s="25">
-        <v>653.9</v>
+        <v>641.94000000000005</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12354,16 +12342,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C622" s="23">
-        <v>188</v>
+        <v>178.5</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>97.76</v>
+        <v>92.82</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12371,16 +12359,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C623" s="23">
-        <v>940.5</v>
+        <v>628.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.7</v>
       </c>
       <c r="E623" s="25">
-        <v>658.35</v>
+        <v>439.95</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12388,16 +12376,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C624" s="23">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>127.4</v>
+        <v>118.3</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12405,16 +12393,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C625" s="23">
-        <v>195.5</v>
+        <v>-56.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.68</v>
       </c>
       <c r="E625" s="25">
-        <v>133.91</v>
+        <v>-38.53</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12435,10 +12423,10 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C627" s="23">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="D627" s="27"/>
       <c r="E627" s="26"/>
@@ -12448,16 +12436,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C628" s="23">
-        <v>1499</v>
+        <v>1472</v>
       </c>
       <c r="D628" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E628" s="25">
-        <v>824.87</v>
+        <v>810.01</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12530,11 +12518,11 @@
       </c>
       <c r="B633" s="29"/>
       <c r="C633" s="30">
-        <v>67032.87</v>
+        <v>66814.27</v>
       </c>
       <c r="D633" s="31"/>
       <c r="E633" s="32">
-        <v>139182.29999999999</v>
+        <v>136033.14000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock update by raj time 3:48
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -515,7 +515,7 @@
     <t>4208 PATRIKA</t>
   </si>
   <si>
-    <t>4209 PATRIKA (STCOK LOT NO)</t>
+    <t>4209 PATRIKA (STK LT N.)</t>
   </si>
   <si>
     <t>4210 PATRIKA</t>
@@ -911,7 +911,7 @@
     <t>5887 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5888 PATRIKA {M} Monday Ayga</t>
+    <t>5888 PATRIKA {M}</t>
   </si>
   <si>
     <t>5889 PATRIKA (DC) {{10}}</t>
@@ -935,7 +935,7 @@
     <t>5895 PATRIKA</t>
   </si>
   <si>
-    <t>5896 PATRIKA (AGYA)</t>
+    <t>5896 PATRIKA</t>
   </si>
   <si>
     <t>5897 PATRIKA (DC)</t>
@@ -974,7 +974,7 @@
     <t>5908 PATRIKA</t>
   </si>
   <si>
-    <t>5909 PATRIKA {M} (AA GYA)</t>
+    <t>5909 PATRIKA {M}</t>
   </si>
   <si>
     <t>5910 PATRIKA {M}</t>
@@ -1136,7 +1136,7 @@
     <t>6514 PATRIKA</t>
   </si>
   <si>
-    <t>6515 PATRIKA {M}</t>
+    <t>6515 PATRIKA {M} (DC)</t>
   </si>
   <si>
     <t>6516 PATRIKA {M}</t>
@@ -1559,7 +1559,7 @@
     <t>9002 CARD -B</t>
   </si>
   <si>
-    <t>9003 CARD</t>
+    <t>9003 CARD (4 MILEGA)</t>
   </si>
   <si>
     <t>9004 CARD (9869)</t>
@@ -1757,7 +1757,7 @@
     <t>9069 CARD</t>
   </si>
   <si>
-    <t>9070 CARD (AGYA)</t>
+    <t>9070 CARD</t>
   </si>
   <si>
     <t>9071 CARD</t>
@@ -1829,7 +1829,7 @@
     <t>9093 CARD</t>
   </si>
   <si>
-    <t>9094 CARD ( MIL JAYGA)</t>
+    <t>9094 CARD</t>
   </si>
   <si>
     <t>9095 CARD</t>
@@ -1913,7 +1913,7 @@
     <t>9209 CARD (YELLOW)</t>
   </si>
   <si>
-    <t>9210 CARD (GOLDEN BOLNA) STCK NO</t>
+    <t>9210 CARD (GOLDEN BOLNA) STK LT N.</t>
   </si>
   <si>
     <t>9211 CARD (NEW)</t>
@@ -2461,7 +2461,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
@@ -2597,16 +2597,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C11" s="23">
-        <v>733.5</v>
+        <v>705.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>665.94</v>
+        <v>640.52</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2614,16 +2614,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="23">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>108.9</v>
+        <v>105.6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2631,16 +2631,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="23">
-        <v>101.5</v>
+        <v>97.5</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>167.48</v>
+        <v>160.88</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2665,16 +2665,16 @@
         <v>19</v>
       </c>
       <c r="B15" s="22">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="23">
-        <v>43.5</v>
+        <v>40.5</v>
       </c>
       <c r="D15" s="24">
         <v>1.8</v>
       </c>
       <c r="E15" s="25">
-        <v>78.3</v>
+        <v>72.900000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,16 +2682,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" s="23">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>43.2</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,16 +2699,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C17" s="23">
-        <v>85</v>
+        <v>77.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2716,16 +2716,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" s="23">
-        <v>71.5</v>
+        <v>68.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2733,16 +2733,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="23">
-        <v>95.5</v>
+        <v>94.5</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,16 +2750,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="C20" s="23">
-        <v>66.5</v>
+        <v>42</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>133</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2786,25 +2786,31 @@
       <c r="B22" s="22">
         <v>29</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="26"/>
+      <c r="C22" s="23">
+        <v>40</v>
+      </c>
+      <c r="D22" s="24">
+        <v>2</v>
+      </c>
+      <c r="E22" s="25">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C23" s="23">
-        <v>23.75</v>
+        <v>126.25</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>47.5</v>
+        <v>252.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2812,16 +2818,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C24" s="23">
-        <v>99.5</v>
+        <v>95</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>208.95</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2829,16 +2835,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C25" s="23">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D25" s="24">
         <v>2.1</v>
       </c>
       <c r="E25" s="25">
-        <v>102.9</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,16 +2878,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28" s="23">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>310.2</v>
+        <v>305.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2889,16 +2895,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C29" s="23">
-        <v>38.799999999999997</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="D29" s="24">
         <v>2.59</v>
       </c>
       <c r="E29" s="25">
-        <v>100.33</v>
+        <v>89.98</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2906,16 +2912,16 @@
         <v>34</v>
       </c>
       <c r="B30" s="22">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C30" s="23">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D30" s="24">
         <v>2.5499999999999998</v>
       </c>
       <c r="E30" s="25">
-        <v>56.1</v>
+        <v>33.15</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2932,16 +2938,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="22">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C32" s="23">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>107.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2960,16 +2966,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C34" s="23">
-        <v>141.5</v>
+        <v>138.5</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>353.75</v>
+        <v>346.25</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,16 +2992,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="22">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C36" s="23">
-        <v>68.5</v>
+        <v>64</v>
       </c>
       <c r="D36" s="24">
         <v>2.6</v>
       </c>
       <c r="E36" s="25">
-        <v>178.1</v>
+        <v>166.4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3003,16 +3009,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C37" s="23">
-        <v>142.5</v>
+        <v>140</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>370.5</v>
+        <v>364</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3020,16 +3026,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C38" s="23">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>361.8</v>
+        <v>329.4</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3088,16 +3094,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C42" s="23">
-        <v>27.5</v>
+        <v>23</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>78.38</v>
+        <v>65.55</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,16 +3213,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C49" s="23">
-        <v>656.5</v>
+        <v>1412.5</v>
       </c>
       <c r="D49" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>722.15</v>
+        <v>1573.78</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,16 +3230,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C50" s="23">
-        <v>449</v>
+        <v>1205.5</v>
       </c>
       <c r="D50" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>493.9</v>
+        <v>1347.15</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,16 +3264,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C52" s="23">
-        <v>146.5</v>
+        <v>920</v>
       </c>
       <c r="D52" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>161.15</v>
+        <v>1027.93</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,16 +3281,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C53" s="23">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D53" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E53" s="25">
-        <v>289.3</v>
+        <v>289.66000000000003</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3292,16 +3298,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C54" s="23">
-        <v>705</v>
+        <v>1463</v>
       </c>
       <c r="D54" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>775.5</v>
+        <v>1635.33</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3315,10 +3321,10 @@
         <v>226</v>
       </c>
       <c r="D55" s="24">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E55" s="25">
-        <v>248.6</v>
+        <v>250.84</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3326,16 +3332,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C56" s="23">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>357.5</v>
+        <v>341</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3343,16 +3349,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C57" s="23">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>856.9</v>
+        <v>834.1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,16 +3381,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C59" s="23">
-        <v>141.5</v>
+        <v>131.5</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>268.85000000000002</v>
+        <v>249.85</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,16 +3398,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C60" s="23">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>767.6</v>
+        <v>758.1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3441,16 +3447,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C63" s="23">
-        <v>82.5</v>
+        <v>78</v>
       </c>
       <c r="D63" s="24">
         <v>2.1</v>
       </c>
       <c r="E63" s="25">
-        <v>173.25</v>
+        <v>163.80000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3458,16 +3464,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C64" s="23">
-        <v>256.5</v>
+        <v>250.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>538.65</v>
+        <v>526.04999999999995</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3475,16 +3481,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C65" s="23">
-        <v>366.5</v>
+        <v>361.5</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>769.65</v>
+        <v>759.15</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3543,16 +3549,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C69" s="23">
-        <v>290.5</v>
+        <v>268.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>203.35</v>
+        <v>187.95</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3560,16 +3566,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C70" s="23">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3577,16 +3583,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C71" s="23">
-        <v>218.5</v>
+        <v>199.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>196.65</v>
+        <v>179.55</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3594,16 +3600,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C72" s="23">
-        <v>2442</v>
+        <v>2401</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3785.1</v>
+        <v>3721.55</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,16 +3617,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C73" s="23">
-        <v>1779</v>
+        <v>1772</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2757.45</v>
+        <v>2746.6</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3628,16 +3634,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C74" s="23">
-        <v>1389.5</v>
+        <v>1386.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>2153.73</v>
+        <v>2149.08</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3686,10 +3692,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C78" s="23">
-        <v>648.5</v>
+        <v>599.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3712,10 +3718,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C80" s="23">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3738,10 +3744,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C82" s="23">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3751,16 +3757,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C83" s="23">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>384.1</v>
+        <v>364.55</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3768,16 +3774,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C84" s="23">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>746.35</v>
+        <v>739.45</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3785,16 +3791,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C85" s="23">
-        <v>4550</v>
+        <v>4496</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>6370</v>
+        <v>6294.4</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3802,16 +3808,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C86" s="23">
-        <v>2880.5</v>
+        <v>2848.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>4032.7</v>
+        <v>3987.9</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3819,16 +3825,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C87" s="23">
-        <v>1138</v>
+        <v>1109.5</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1593.2</v>
+        <v>1553.3</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3845,16 +3851,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C89" s="23">
-        <v>861</v>
+        <v>841</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1722</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,16 +3868,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C90" s="23">
-        <v>1115.5</v>
+        <v>1103</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2231</v>
+        <v>2206</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3879,16 +3885,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C91" s="23">
-        <v>403</v>
+        <v>389.5</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>507.78</v>
+        <v>490.77</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,16 +3902,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C92" s="23">
-        <v>598.5</v>
+        <v>586.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>754.11</v>
+        <v>738.99</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4025,16 +4031,16 @@
         <v>105</v>
       </c>
       <c r="B101" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C101" s="23">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="D101" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E101" s="25">
-        <v>477.25</v>
+        <v>465.75</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4059,10 +4065,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C103" s="23">
-        <v>715</v>
+        <v>615</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4072,10 +4078,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="22">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C104" s="23">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4085,10 +4091,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C105" s="23">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4098,10 +4104,10 @@
         <v>110</v>
       </c>
       <c r="B106" s="22">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C106" s="23">
-        <v>336</v>
+        <v>306</v>
       </c>
       <c r="D106" s="27"/>
       <c r="E106" s="26"/>
@@ -4111,10 +4117,10 @@
         <v>111</v>
       </c>
       <c r="B107" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" s="23">
-        <v>23.5</v>
+        <v>13.5</v>
       </c>
       <c r="D107" s="27"/>
       <c r="E107" s="26"/>
@@ -4218,16 +4224,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C114" s="23">
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>156.25</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4235,16 +4241,16 @@
         <v>119</v>
       </c>
       <c r="B115" s="22">
+        <v>22</v>
+      </c>
+      <c r="C115" s="23">
         <v>21</v>
-      </c>
-      <c r="C115" s="23">
-        <v>21.5</v>
       </c>
       <c r="D115" s="24">
         <v>12.5</v>
       </c>
       <c r="E115" s="25">
-        <v>268.75</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4269,16 +4275,16 @@
         <v>121</v>
       </c>
       <c r="B117" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C117" s="23">
-        <v>17</v>
+        <v>14.5</v>
       </c>
       <c r="D117" s="24">
         <v>12.5</v>
       </c>
       <c r="E117" s="25">
-        <v>212.5</v>
+        <v>181.25</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4286,16 +4292,16 @@
         <v>122</v>
       </c>
       <c r="B118" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C118" s="23">
-        <v>30.86</v>
+        <v>28.86</v>
       </c>
       <c r="D118" s="24">
         <v>12.5</v>
       </c>
       <c r="E118" s="25">
-        <v>385.75</v>
+        <v>360.75</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4303,16 +4309,16 @@
         <v>123</v>
       </c>
       <c r="B119" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C119" s="23">
-        <v>24.5</v>
+        <v>13.5</v>
       </c>
       <c r="D119" s="24">
         <v>12.5</v>
       </c>
       <c r="E119" s="25">
-        <v>306.25</v>
+        <v>168.75</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4320,16 +4326,16 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C120" s="23">
-        <v>16.5</v>
+        <v>12.5</v>
       </c>
       <c r="D120" s="24">
         <v>12.5</v>
       </c>
       <c r="E120" s="25">
-        <v>206.25</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4337,16 +4343,16 @@
         <v>125</v>
       </c>
       <c r="B121" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C121" s="23">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>18.75</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4510,17 +4516,11 @@
         <v>136</v>
       </c>
       <c r="B132" s="22">
-        <v>11</v>
-      </c>
-      <c r="C132" s="23">
-        <v>2</v>
-      </c>
-      <c r="D132" s="24">
-        <v>15.5</v>
-      </c>
-      <c r="E132" s="25">
-        <v>31</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C132" s="26"/>
+      <c r="D132" s="27"/>
+      <c r="E132" s="26"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="21" t="s">
@@ -4544,16 +4544,16 @@
         <v>138</v>
       </c>
       <c r="B134" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134" s="23">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="D134" s="24">
         <v>15.5</v>
       </c>
       <c r="E134" s="25">
-        <v>193.75</v>
+        <v>178.25</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4561,16 +4561,16 @@
         <v>139</v>
       </c>
       <c r="B135" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C135" s="23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D135" s="24">
         <v>15.5</v>
       </c>
       <c r="E135" s="25">
-        <v>263.5</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4629,16 +4629,16 @@
         <v>143</v>
       </c>
       <c r="B139" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C139" s="23">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="D139" s="24">
         <v>18.45</v>
       </c>
       <c r="E139" s="25">
-        <v>202.93</v>
+        <v>193.71</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4782,16 +4782,16 @@
         <v>152</v>
       </c>
       <c r="B148" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C148" s="23">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D148" s="24">
         <v>18.420000000000002</v>
       </c>
       <c r="E148" s="25">
-        <v>147.38</v>
+        <v>55.27</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4833,16 +4833,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C151" s="23">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>31.35</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4850,16 +4850,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C152" s="23">
-        <v>110</v>
+        <v>78.5</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>308</v>
+        <v>219.8</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4867,16 +4867,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C153" s="23">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>123.75</v>
+        <v>107.25</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4884,16 +4884,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C154" s="23">
-        <v>1.85</v>
+        <v>0.85</v>
       </c>
       <c r="D154" s="24">
         <v>2.75</v>
       </c>
       <c r="E154" s="25">
-        <v>5.09</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4901,16 +4901,16 @@
         <v>159</v>
       </c>
       <c r="B155" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C155" s="23">
-        <v>5.5</v>
+        <v>34.5</v>
       </c>
       <c r="D155" s="24">
         <v>4.7</v>
       </c>
       <c r="E155" s="25">
-        <v>25.85</v>
+        <v>162.15</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4918,16 +4918,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="C156" s="23">
-        <v>194.75</v>
+        <v>182.75</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>662.15</v>
+        <v>621.35</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4946,16 +4946,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C158" s="23">
-        <v>108.5</v>
+        <v>107.5</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>292.95</v>
+        <v>290.25</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4980,16 +4980,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C160" s="23">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>322</v>
+        <v>308</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4997,16 +4997,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C161" s="23">
-        <v>56.5</v>
+        <v>32.5</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>141.25</v>
+        <v>81.25</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5031,16 +5031,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C163" s="23">
-        <v>121.5</v>
+        <v>120.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.8</v>
       </c>
       <c r="E163" s="25">
-        <v>340.2</v>
+        <v>337.4</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5065,16 +5065,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C165" s="23">
-        <v>236.5</v>
+        <v>232.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>697.68</v>
+        <v>685.88</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5082,16 +5082,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C166" s="23">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>769.95</v>
+        <v>758.15</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5099,16 +5099,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C167" s="23">
-        <v>60.5</v>
+        <v>57.5</v>
       </c>
       <c r="D167" s="24">
         <v>3</v>
       </c>
       <c r="E167" s="25">
-        <v>181.5</v>
+        <v>172.5</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5116,16 +5116,16 @@
         <v>172</v>
       </c>
       <c r="B168" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C168" s="23">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="D168" s="24">
         <v>3</v>
       </c>
       <c r="E168" s="25">
-        <v>40.5</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5133,16 +5133,16 @@
         <v>173</v>
       </c>
       <c r="B169" s="22">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C169" s="23">
-        <v>76.5</v>
+        <v>71.5</v>
       </c>
       <c r="D169" s="24">
         <v>3.3</v>
       </c>
       <c r="E169" s="25">
-        <v>252.45</v>
+        <v>235.95</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5167,16 +5167,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C171" s="23">
-        <v>240.5</v>
+        <v>236</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>841.75</v>
+        <v>826</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5193,16 +5193,16 @@
         <v>177</v>
       </c>
       <c r="B173" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C173" s="23">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D173" s="24">
         <v>3.9</v>
       </c>
       <c r="E173" s="25">
-        <v>210.6</v>
+        <v>198.9</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5242,16 +5242,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C176" s="23">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>216.45</v>
+        <v>213.12</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5259,16 +5259,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C177" s="23">
-        <v>72.5</v>
+        <v>68.5</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>241.43</v>
+        <v>228.11</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5330,16 +5330,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C182" s="23">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>220.4</v>
+        <v>209</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5364,16 +5364,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C184" s="23">
-        <v>108.5</v>
+        <v>90</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>488.25</v>
+        <v>405</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5466,16 +5466,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C190" s="23">
-        <v>53.5</v>
+        <v>40.5</v>
       </c>
       <c r="D190" s="24">
         <v>3.93</v>
       </c>
       <c r="E190" s="25">
-        <v>210.26</v>
+        <v>159.16999999999999</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5517,16 +5517,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C193" s="23">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5549,31 +5549,33 @@
         <v>199</v>
       </c>
       <c r="B195" s="22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C195" s="23">
-        <v>38</v>
+        <v>28.5</v>
       </c>
       <c r="D195" s="24">
         <v>2.8</v>
       </c>
       <c r="E195" s="25">
-        <v>106.4</v>
+        <v>79.8</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="B196" s="22"/>
+      <c r="B196" s="22">
+        <v>3</v>
+      </c>
       <c r="C196" s="23">
-        <v>21</v>
+        <v>-1.5</v>
       </c>
       <c r="D196" s="24">
         <v>3.4</v>
       </c>
       <c r="E196" s="25">
-        <v>71.400000000000006</v>
+        <v>-5.0999999999999996</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5618,16 +5620,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C200" s="23">
-        <v>246.24</v>
+        <v>231.74</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>756.79</v>
+        <v>712.23</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5667,10 +5669,10 @@
         <v>3.5</v>
       </c>
       <c r="D203" s="24">
-        <v>3.25</v>
+        <v>3.31</v>
       </c>
       <c r="E203" s="25">
-        <v>11.38</v>
+        <v>11.6</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5722,16 +5724,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C208" s="23">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>30.4</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,16 +5741,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C209" s="23">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>342</v>
+        <v>323</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5795,16 +5797,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C213" s="23">
-        <v>48.5</v>
+        <v>46.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>199.64</v>
+        <v>191.41</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5812,16 +5814,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C214" s="23">
-        <v>161</v>
+        <v>126.5</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>663.09</v>
+        <v>521</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5880,16 +5882,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C218" s="23">
-        <v>82</v>
+        <v>80.5</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>355.96</v>
+        <v>349.44</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5936,16 +5938,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="C222" s="23">
-        <v>171</v>
+        <v>158.5</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>769.5</v>
+        <v>713.25</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5953,16 +5955,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C223" s="23">
-        <v>91.5</v>
+        <v>72</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>411.75</v>
+        <v>324</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5970,16 +5972,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C224" s="23">
-        <v>93</v>
+        <v>91.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>488.25</v>
+        <v>480.38</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6004,16 +6006,16 @@
         <v>230</v>
       </c>
       <c r="B226" s="22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C226" s="23">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D226" s="24">
         <v>4.8</v>
       </c>
       <c r="E226" s="25">
-        <v>177.6</v>
+        <v>187.2</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6021,16 +6023,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C227" s="23">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>193.5</v>
+        <v>166.5</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6087,16 +6089,16 @@
         <v>235</v>
       </c>
       <c r="B231" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C231" s="23">
-        <v>100.5</v>
+        <v>99.5</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>527.63</v>
+        <v>522.38</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6177,16 +6179,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C237" s="23">
-        <v>69.5</v>
+        <v>67.5</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>417</v>
+        <v>405</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6218,16 +6220,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C240" s="23">
-        <v>100.3</v>
+        <v>92.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>571.71</v>
+        <v>528.96</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6267,16 +6269,16 @@
         <v>247</v>
       </c>
       <c r="B243" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C243" s="23">
-        <v>39.5</v>
+        <v>38.5</v>
       </c>
       <c r="D243" s="24">
         <v>6.75</v>
       </c>
       <c r="E243" s="25">
-        <v>266.63</v>
+        <v>259.88</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6284,16 +6286,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C244" s="23">
-        <v>77.91</v>
+        <v>70.91</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>465.91</v>
+        <v>424.05</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6301,16 +6303,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C245" s="23">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>161.88</v>
+        <v>157.62</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6318,16 +6320,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C246" s="23">
-        <v>91.5</v>
+        <v>110.5</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>366</v>
+        <v>442</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6352,31 +6354,33 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C248" s="23">
-        <v>50</v>
+        <v>48.5</v>
       </c>
       <c r="D248" s="24">
         <v>4.5</v>
       </c>
       <c r="E248" s="25">
-        <v>225</v>
+        <v>218.25</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="B249" s="22"/>
+      <c r="B249" s="22">
+        <v>2</v>
+      </c>
       <c r="C249" s="23">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D249" s="24">
         <v>6.5</v>
       </c>
       <c r="E249" s="25">
-        <v>130</v>
+        <v>52</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6384,16 +6388,16 @@
         <v>254</v>
       </c>
       <c r="B250" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C250" s="23">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D250" s="24">
         <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>123.72</v>
+        <v>97.95</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6429,16 +6433,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C253" s="23">
-        <v>97</v>
+        <v>66.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>339.5</v>
+        <v>232.75</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6463,16 +6467,16 @@
         <v>259</v>
       </c>
       <c r="B255" s="22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C255" s="23">
-        <v>78.5</v>
+        <v>76</v>
       </c>
       <c r="D255" s="24">
         <v>4.25</v>
       </c>
       <c r="E255" s="25">
-        <v>333.63</v>
+        <v>323</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6523,16 +6527,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C259" s="23">
-        <v>213</v>
+        <v>190.5</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>911.64</v>
+        <v>815.34</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6540,16 +6544,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C260" s="23">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>226.84</v>
+        <v>209.72</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6591,16 +6595,16 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C263" s="23">
-        <v>73.8</v>
+        <v>67.8</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>365.31</v>
+        <v>335.61</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6608,16 +6612,16 @@
         <v>268</v>
       </c>
       <c r="B264" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C264" s="23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D264" s="24">
         <v>4.75</v>
       </c>
       <c r="E264" s="25">
-        <v>38</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6677,16 +6681,16 @@
         <v>273</v>
       </c>
       <c r="B269" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C269" s="23">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D269" s="24">
         <v>5.3</v>
       </c>
       <c r="E269" s="25">
-        <v>233.2</v>
+        <v>222.6</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6694,16 +6698,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C270" s="23">
-        <v>45.5</v>
+        <v>38</v>
       </c>
       <c r="D270" s="24">
         <v>5.4</v>
       </c>
       <c r="E270" s="25">
-        <v>245.7</v>
+        <v>205.2</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6728,16 +6732,16 @@
         <v>276</v>
       </c>
       <c r="B272" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C272" s="23">
-        <v>68.5</v>
+        <v>65.5</v>
       </c>
       <c r="D272" s="24">
         <v>5.55</v>
       </c>
       <c r="E272" s="25">
-        <v>380.18</v>
+        <v>363.53</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6762,16 +6766,16 @@
         <v>278</v>
       </c>
       <c r="B274" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C274" s="23">
-        <v>9.5</v>
+        <v>5.5</v>
       </c>
       <c r="D274" s="24">
         <v>5.23</v>
       </c>
       <c r="E274" s="25">
-        <v>49.69</v>
+        <v>28.77</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -6805,16 +6809,16 @@
         <v>281</v>
       </c>
       <c r="B277" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C277" s="23">
-        <v>75.5</v>
+        <v>70.5</v>
       </c>
       <c r="D277" s="24">
         <v>6.25</v>
       </c>
       <c r="E277" s="25">
-        <v>471.88</v>
+        <v>440.63</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6856,16 +6860,16 @@
         <v>284</v>
       </c>
       <c r="B280" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C280" s="23">
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="D280" s="24">
         <v>6</v>
       </c>
       <c r="E280" s="25">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -6890,16 +6894,16 @@
         <v>286</v>
       </c>
       <c r="B282" s="22">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C282" s="23">
-        <v>52.88</v>
+        <v>46.88</v>
       </c>
       <c r="D282" s="24">
         <v>5.94</v>
       </c>
       <c r="E282" s="25">
-        <v>314.11</v>
+        <v>278.47000000000003</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -6907,16 +6911,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C283" s="23">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D283" s="24">
         <v>5.7</v>
       </c>
       <c r="E283" s="25">
-        <v>279.3</v>
+        <v>267.89999999999998</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6958,16 +6962,16 @@
         <v>290</v>
       </c>
       <c r="B286" s="22">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C286" s="23">
-        <v>63</v>
+        <v>49.5</v>
       </c>
       <c r="D286" s="24">
         <v>6.8</v>
       </c>
       <c r="E286" s="25">
-        <v>428.32</v>
+        <v>336.54</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -7027,16 +7031,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C291" s="23">
-        <v>104.5</v>
+        <v>102</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>645.80999999999995</v>
+        <v>630.36</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7072,16 +7076,16 @@
         <v>298</v>
       </c>
       <c r="B294" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C294" s="23">
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="D294" s="24">
         <v>6.4</v>
       </c>
       <c r="E294" s="25">
-        <v>112</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -7106,16 +7110,16 @@
         <v>300</v>
       </c>
       <c r="B296" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C296" s="23">
-        <v>15.5</v>
+        <v>12.5</v>
       </c>
       <c r="D296" s="24">
         <v>6.4</v>
       </c>
       <c r="E296" s="25">
-        <v>99.2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -7135,13 +7139,13 @@
         <v>37</v>
       </c>
       <c r="C298" s="23">
-        <v>76</v>
+        <v>76.5</v>
       </c>
       <c r="D298" s="24">
         <v>6.65</v>
       </c>
       <c r="E298" s="25">
-        <v>505.4</v>
+        <v>508.73</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -7149,16 +7153,16 @@
         <v>303</v>
       </c>
       <c r="B299" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C299" s="23">
-        <v>64.5</v>
+        <v>63</v>
       </c>
       <c r="D299" s="24">
         <v>6.18</v>
       </c>
       <c r="E299" s="25">
-        <v>398.61</v>
+        <v>389.34</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7175,16 +7179,16 @@
         <v>305</v>
       </c>
       <c r="B301" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C301" s="23">
-        <v>23</v>
+        <v>21.5</v>
       </c>
       <c r="D301" s="24">
         <v>7.12</v>
       </c>
       <c r="E301" s="25">
-        <v>163.87</v>
+        <v>153.18</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7226,16 +7230,16 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C304" s="23">
-        <v>14.5</v>
+        <v>11.5</v>
       </c>
       <c r="D304" s="24">
         <v>7.13</v>
       </c>
       <c r="E304" s="25">
-        <v>103.39</v>
+        <v>82</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7272,13 +7276,13 @@
         <v>24</v>
       </c>
       <c r="C307" s="23">
-        <v>5.5</v>
+        <v>25.5</v>
       </c>
       <c r="D307" s="24">
         <v>7.6</v>
       </c>
       <c r="E307" s="25">
-        <v>41.8</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7505,16 +7509,16 @@
         <v>327</v>
       </c>
       <c r="B323" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C323" s="23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D323" s="24">
         <v>9</v>
       </c>
       <c r="E323" s="25">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7522,16 +7526,16 @@
         <v>328</v>
       </c>
       <c r="B324" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C324" s="23">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D324" s="24">
         <v>9.5</v>
       </c>
       <c r="E324" s="25">
-        <v>237.5</v>
+        <v>190</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -7590,16 +7594,16 @@
         <v>332</v>
       </c>
       <c r="B328" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C328" s="23">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="D328" s="24">
         <v>11.75</v>
       </c>
       <c r="E328" s="25">
-        <v>252.63</v>
+        <v>240.88</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -7658,16 +7662,16 @@
         <v>336</v>
       </c>
       <c r="B332" s="22">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C332" s="23">
-        <v>31</v>
+        <v>19.5</v>
       </c>
       <c r="D332" s="24">
         <v>6.89</v>
       </c>
       <c r="E332" s="25">
-        <v>213.59</v>
+        <v>134.36000000000001</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7675,16 +7679,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C333" s="23">
-        <v>31.5</v>
+        <v>28.5</v>
       </c>
       <c r="D333" s="24">
         <v>6.9</v>
       </c>
       <c r="E333" s="25">
-        <v>217.35</v>
+        <v>196.65</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7692,16 +7696,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C334" s="23">
-        <v>34</v>
+        <v>31.5</v>
       </c>
       <c r="D334" s="24">
         <v>7.13</v>
       </c>
       <c r="E334" s="25">
-        <v>242.42</v>
+        <v>224.6</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7726,16 +7730,16 @@
         <v>340</v>
       </c>
       <c r="B336" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C336" s="23">
-        <v>13.5</v>
+        <v>7.5</v>
       </c>
       <c r="D336" s="24">
         <v>8.5</v>
       </c>
       <c r="E336" s="25">
-        <v>114.75</v>
+        <v>63.75</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -7760,16 +7764,16 @@
         <v>342</v>
       </c>
       <c r="B338" s="22">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C338" s="23">
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="D338" s="24">
-        <v>10.61</v>
+        <v>10.77</v>
       </c>
       <c r="E338" s="25">
-        <v>217.55</v>
+        <v>188.43</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -7859,16 +7863,16 @@
         <v>349</v>
       </c>
       <c r="B345" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C345" s="23">
-        <v>77</v>
+        <v>73.5</v>
       </c>
       <c r="D345" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E345" s="25">
-        <v>377.3</v>
+        <v>360.15</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -7910,16 +7914,16 @@
         <v>352</v>
       </c>
       <c r="B348" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C348" s="23">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D348" s="24">
         <v>7.6</v>
       </c>
       <c r="E348" s="25">
-        <v>167.2</v>
+        <v>121.6</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -7927,16 +7931,16 @@
         <v>353</v>
       </c>
       <c r="B349" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C349" s="23">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D349" s="24">
         <v>8.67</v>
       </c>
       <c r="E349" s="25">
-        <v>268.88</v>
+        <v>234.19</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -8148,16 +8152,16 @@
         <v>366</v>
       </c>
       <c r="B362" s="22">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C362" s="23">
-        <v>14.99</v>
+        <v>6.99</v>
       </c>
       <c r="D362" s="24">
         <v>12</v>
       </c>
       <c r="E362" s="25">
-        <v>179.88</v>
+        <v>83.88</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -8165,16 +8169,16 @@
         <v>367</v>
       </c>
       <c r="B363" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C363" s="23">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D363" s="24">
         <v>12</v>
       </c>
       <c r="E363" s="25">
-        <v>126</v>
+        <v>102</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8301,16 +8305,16 @@
         <v>375</v>
       </c>
       <c r="B371" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C371" s="23">
-        <v>15.5</v>
+        <v>11</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>155</v>
+        <v>110</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8318,16 +8322,16 @@
         <v>376</v>
       </c>
       <c r="B372" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C372" s="23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D372" s="24">
         <v>10.5</v>
       </c>
       <c r="E372" s="25">
-        <v>63</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -8335,16 +8339,16 @@
         <v>377</v>
       </c>
       <c r="B373" s="22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C373" s="23">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="D373" s="24">
         <v>13.5</v>
       </c>
       <c r="E373" s="25">
-        <v>67.5</v>
+        <v>87.75</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
@@ -8386,16 +8390,16 @@
         <v>380</v>
       </c>
       <c r="B376" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C376" s="23">
-        <v>49.26</v>
+        <v>43.26</v>
       </c>
       <c r="D376" s="24">
         <v>9.5</v>
       </c>
       <c r="E376" s="25">
-        <v>467.97</v>
+        <v>410.97</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
@@ -8403,16 +8407,16 @@
         <v>381</v>
       </c>
       <c r="B377" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C377" s="23">
-        <v>28.3</v>
+        <v>24.3</v>
       </c>
       <c r="D377" s="24">
         <v>15</v>
       </c>
       <c r="E377" s="25">
-        <v>424.5</v>
+        <v>364.5</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -8437,16 +8441,16 @@
         <v>383</v>
       </c>
       <c r="B379" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C379" s="23">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
       <c r="D379" s="24">
         <v>10</v>
       </c>
       <c r="E379" s="25">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
@@ -8471,16 +8475,16 @@
         <v>385</v>
       </c>
       <c r="B381" s="22">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C381" s="23">
-        <v>40</v>
+        <v>34.5</v>
       </c>
       <c r="D381" s="24">
         <v>7.84</v>
       </c>
       <c r="E381" s="25">
-        <v>313.60000000000002</v>
+        <v>270.48</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -8488,16 +8492,16 @@
         <v>386</v>
       </c>
       <c r="B382" s="22">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C382" s="23">
-        <v>9.99</v>
+        <v>3.99</v>
       </c>
       <c r="D382" s="24">
         <v>25</v>
       </c>
       <c r="E382" s="25">
-        <v>249.75</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -8553,13 +8557,13 @@
         <v>8</v>
       </c>
       <c r="C386" s="23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D386" s="24">
         <v>12.5</v>
       </c>
       <c r="E386" s="25">
-        <v>12.5</v>
+        <v>50</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8601,16 +8605,16 @@
         <v>393</v>
       </c>
       <c r="B389" s="22">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C389" s="23">
-        <v>23.25</v>
+        <v>20.75</v>
       </c>
       <c r="D389" s="24">
         <v>11.5</v>
       </c>
       <c r="E389" s="25">
-        <v>267.38</v>
+        <v>238.63</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
@@ -8701,16 +8705,16 @@
         <v>399</v>
       </c>
       <c r="B395" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C395" s="23">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D395" s="24">
         <v>9.5</v>
       </c>
       <c r="E395" s="25">
-        <v>285</v>
+        <v>237.5</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
@@ -8769,16 +8773,16 @@
         <v>403</v>
       </c>
       <c r="B399" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C399" s="23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D399" s="24">
         <v>10</v>
       </c>
       <c r="E399" s="25">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -8871,16 +8875,16 @@
         <v>409</v>
       </c>
       <c r="B405" s="22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C405" s="23">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D405" s="24">
         <v>2</v>
       </c>
       <c r="E405" s="25">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
@@ -8949,16 +8953,16 @@
         <v>415</v>
       </c>
       <c r="B411" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C411" s="23">
-        <v>56.5</v>
+        <v>55.5</v>
       </c>
       <c r="D411" s="24">
         <v>2.25</v>
       </c>
       <c r="E411" s="25">
-        <v>127.13</v>
+        <v>124.88</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -8966,16 +8970,16 @@
         <v>416</v>
       </c>
       <c r="B412" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C412" s="23">
-        <v>51.5</v>
+        <v>49</v>
       </c>
       <c r="D412" s="24">
         <v>2.25</v>
       </c>
       <c r="E412" s="25">
-        <v>115.88</v>
+        <v>110.25</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -9017,16 +9021,16 @@
         <v>419</v>
       </c>
       <c r="B415" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C415" s="23">
-        <v>41.5</v>
+        <v>39.5</v>
       </c>
       <c r="D415" s="24">
         <v>2.5</v>
       </c>
       <c r="E415" s="25">
-        <v>103.75</v>
+        <v>98.75</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
@@ -9051,16 +9055,16 @@
         <v>421</v>
       </c>
       <c r="B417" s="22">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C417" s="23">
-        <v>51</v>
+        <v>36.5</v>
       </c>
       <c r="D417" s="24">
         <v>2.7</v>
       </c>
       <c r="E417" s="25">
-        <v>137.69999999999999</v>
+        <v>98.55</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
@@ -9102,16 +9106,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C420" s="23">
-        <v>32.5</v>
+        <v>26</v>
       </c>
       <c r="D420" s="24">
         <v>2.75</v>
       </c>
       <c r="E420" s="25">
-        <v>89.38</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9136,16 +9140,16 @@
         <v>426</v>
       </c>
       <c r="B422" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C422" s="23">
-        <v>31.5</v>
+        <v>26.5</v>
       </c>
       <c r="D422" s="24">
         <v>2.8</v>
       </c>
       <c r="E422" s="25">
-        <v>88.2</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9153,16 +9157,16 @@
         <v>427</v>
       </c>
       <c r="B423" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C423" s="23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D423" s="24">
         <v>2.8</v>
       </c>
       <c r="E423" s="25">
-        <v>39.200000000000003</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -9179,16 +9183,16 @@
         <v>429</v>
       </c>
       <c r="B425" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C425" s="23">
-        <v>159.84</v>
+        <v>156.34</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>447.55</v>
+        <v>437.75</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9196,16 +9200,16 @@
         <v>430</v>
       </c>
       <c r="B426" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C426" s="23">
-        <v>37.5</v>
+        <v>29.5</v>
       </c>
       <c r="D426" s="24">
         <v>2.95</v>
       </c>
       <c r="E426" s="25">
-        <v>110.63</v>
+        <v>87.03</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
@@ -9247,16 +9251,16 @@
         <v>433</v>
       </c>
       <c r="B429" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C429" s="23">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D429" s="24">
         <v>3.26</v>
       </c>
       <c r="E429" s="25">
-        <v>84.76</v>
+        <v>68.459999999999994</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9281,16 +9285,16 @@
         <v>435</v>
       </c>
       <c r="B431" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C431" s="23">
-        <v>61</v>
+        <v>58.5</v>
       </c>
       <c r="D431" s="24">
         <v>3.15</v>
       </c>
       <c r="E431" s="25">
-        <v>192.15</v>
+        <v>184.28</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -9315,16 +9319,16 @@
         <v>437</v>
       </c>
       <c r="B433" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C433" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D433" s="24">
         <v>3.25</v>
       </c>
       <c r="E433" s="25">
-        <v>78</v>
+        <v>71.5</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
@@ -9407,16 +9411,16 @@
         <v>443</v>
       </c>
       <c r="B439" s="22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C439" s="23">
-        <v>55.46</v>
+        <v>51.46</v>
       </c>
       <c r="D439" s="24">
         <v>3.5</v>
       </c>
       <c r="E439" s="25">
-        <v>194.11</v>
+        <v>180.11</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
@@ -9527,16 +9531,16 @@
         <v>451</v>
       </c>
       <c r="B447" s="22">
+        <v>38</v>
+      </c>
+      <c r="C447" s="23">
         <v>36</v>
-      </c>
-      <c r="C447" s="23">
-        <v>45</v>
       </c>
       <c r="D447" s="24">
         <v>4.25</v>
       </c>
       <c r="E447" s="25">
-        <v>191.25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9544,16 +9548,16 @@
         <v>452</v>
       </c>
       <c r="B448" s="22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C448" s="23">
-        <v>27.5</v>
+        <v>22</v>
       </c>
       <c r="D448" s="24">
         <v>3.8</v>
       </c>
       <c r="E448" s="25">
-        <v>104.5</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -9561,16 +9565,16 @@
         <v>453</v>
       </c>
       <c r="B449" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C449" s="23">
-        <v>27.5</v>
+        <v>22.5</v>
       </c>
       <c r="D449" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E449" s="25">
-        <v>114.14</v>
+        <v>93.39</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -9663,16 +9667,16 @@
         <v>459</v>
       </c>
       <c r="B455" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C455" s="23">
-        <v>102.5</v>
+        <v>100.5</v>
       </c>
       <c r="D455" s="24">
         <v>4.28</v>
       </c>
       <c r="E455" s="25">
-        <v>438.7</v>
+        <v>430.14</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">
@@ -9742,16 +9746,16 @@
         <v>464</v>
       </c>
       <c r="B460" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C460" s="23">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D460" s="24">
         <v>4.5</v>
       </c>
       <c r="E460" s="25">
-        <v>33.75</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
@@ -9858,16 +9862,16 @@
         <v>472</v>
       </c>
       <c r="B468" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C468" s="23">
-        <v>30.5</v>
+        <v>16</v>
       </c>
       <c r="D468" s="24">
         <v>6</v>
       </c>
       <c r="E468" s="25">
-        <v>183</v>
+        <v>96</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
@@ -9984,16 +9988,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C476" s="23">
-        <v>34</v>
+        <v>22.5</v>
       </c>
       <c r="D476" s="24">
         <v>7.6</v>
       </c>
       <c r="E476" s="25">
-        <v>258.39999999999998</v>
+        <v>171</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10001,16 +10005,16 @@
         <v>481</v>
       </c>
       <c r="B477" s="22">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C477" s="23">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D477" s="24">
         <v>8.5</v>
       </c>
       <c r="E477" s="25">
-        <v>365.5</v>
+        <v>93.5</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
@@ -10018,16 +10022,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C478" s="23">
-        <v>19.5</v>
+        <v>21</v>
       </c>
       <c r="D478" s="24">
         <v>7.5</v>
       </c>
       <c r="E478" s="25">
-        <v>146.25</v>
+        <v>157.5</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -10089,16 +10093,16 @@
         <v>487</v>
       </c>
       <c r="B483" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C483" s="23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D483" s="24">
         <v>4.28</v>
       </c>
       <c r="E483" s="25">
-        <v>72.760000000000005</v>
+        <v>59.92</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
@@ -10106,16 +10110,16 @@
         <v>488</v>
       </c>
       <c r="B484" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C484" s="23">
-        <v>15.5</v>
+        <v>12.5</v>
       </c>
       <c r="D484" s="24">
         <v>9.5</v>
       </c>
       <c r="E484" s="25">
-        <v>147.25</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
@@ -10206,16 +10210,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C490" s="23">
-        <v>497</v>
+        <v>467</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>546.70000000000005</v>
+        <v>513.70000000000005</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10223,16 +10227,16 @@
         <v>495</v>
       </c>
       <c r="B491" s="22">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C491" s="23">
-        <v>387</v>
+        <v>314</v>
       </c>
       <c r="D491" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E491" s="25">
-        <v>425.7</v>
+        <v>345.4</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -10257,16 +10261,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C493" s="23">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="D493" s="24">
         <v>1.4</v>
       </c>
       <c r="E493" s="25">
-        <v>372.4</v>
+        <v>351.4</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10274,16 +10278,16 @@
         <v>498</v>
       </c>
       <c r="B494" s="22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C494" s="23">
-        <v>414</v>
+        <v>370.5</v>
       </c>
       <c r="D494" s="24">
         <v>1.4</v>
       </c>
       <c r="E494" s="25">
-        <v>579.6</v>
+        <v>518.70000000000005</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
@@ -10325,16 +10329,16 @@
         <v>501</v>
       </c>
       <c r="B497" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C497" s="23">
-        <v>30.5</v>
+        <v>20.5</v>
       </c>
       <c r="D497" s="24">
         <v>3.05</v>
       </c>
       <c r="E497" s="25">
-        <v>93.03</v>
+        <v>62.53</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
@@ -10489,16 +10493,16 @@
         <v>511</v>
       </c>
       <c r="B507" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C507" s="23">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D507" s="24">
         <v>1.71</v>
       </c>
       <c r="E507" s="25">
-        <v>34.200000000000003</v>
+        <v>29.07</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10506,16 +10510,16 @@
         <v>512</v>
       </c>
       <c r="B508" s="22">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C508" s="23">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D508" s="24">
         <v>0.92</v>
       </c>
       <c r="E508" s="25">
-        <v>132.15</v>
+        <v>126.61</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10523,16 +10527,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C509" s="23">
-        <v>180.2</v>
+        <v>179.2</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>410.86</v>
+        <v>408.58</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10540,16 +10544,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C510" s="23">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D510" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E510" s="25">
-        <v>462.84</v>
+        <v>453.72</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10583,16 +10587,16 @@
         <v>517</v>
       </c>
       <c r="B513" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C513" s="23">
-        <v>17</v>
+        <v>16.5</v>
       </c>
       <c r="D513" s="24">
         <v>2.75</v>
       </c>
       <c r="E513" s="25">
-        <v>46.75</v>
+        <v>45.38</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10600,16 +10604,16 @@
         <v>518</v>
       </c>
       <c r="B514" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C514" s="23">
-        <v>48.5</v>
+        <v>38.5</v>
       </c>
       <c r="D514" s="24">
         <v>2.73</v>
       </c>
       <c r="E514" s="25">
-        <v>132.6</v>
+        <v>105.26</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
@@ -10617,16 +10621,16 @@
         <v>519</v>
       </c>
       <c r="B515" s="22">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C515" s="23">
-        <v>127.5</v>
+        <v>125.5</v>
       </c>
       <c r="D515" s="24">
         <v>2.8</v>
       </c>
       <c r="E515" s="25">
-        <v>357</v>
+        <v>351.4</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -10700,16 +10704,16 @@
         <v>524</v>
       </c>
       <c r="B520" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C520" s="23">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D520" s="24">
         <v>3.2</v>
       </c>
       <c r="E520" s="25">
-        <v>92.8</v>
+        <v>86.4</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
@@ -10743,16 +10747,16 @@
         <v>527</v>
       </c>
       <c r="B523" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C523" s="23">
-        <v>41.5</v>
+        <v>38.5</v>
       </c>
       <c r="D523" s="24">
         <v>2.85</v>
       </c>
       <c r="E523" s="25">
-        <v>118.28</v>
+        <v>109.73</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
@@ -10812,16 +10816,16 @@
         <v>532</v>
       </c>
       <c r="B528" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C528" s="23">
-        <v>18.5</v>
+        <v>14.5</v>
       </c>
       <c r="D528" s="24">
         <v>3.5</v>
       </c>
       <c r="E528" s="25">
-        <v>64.75</v>
+        <v>50.75</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -10829,16 +10833,16 @@
         <v>533</v>
       </c>
       <c r="B529" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C529" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D529" s="24">
         <v>3.5</v>
       </c>
       <c r="E529" s="25">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -10846,16 +10850,16 @@
         <v>534</v>
       </c>
       <c r="B530" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C530" s="23">
-        <v>63.5</v>
+        <v>58.5</v>
       </c>
       <c r="D530" s="24">
         <v>3.33</v>
       </c>
       <c r="E530" s="25">
-        <v>211.46</v>
+        <v>194.81</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -10889,16 +10893,16 @@
         <v>537</v>
       </c>
       <c r="B533" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C533" s="23">
-        <v>68.5</v>
+        <v>66</v>
       </c>
       <c r="D533" s="24">
         <v>3.71</v>
       </c>
       <c r="E533" s="25">
-        <v>254.38</v>
+        <v>245.1</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -10906,16 +10910,16 @@
         <v>538</v>
       </c>
       <c r="B534" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C534" s="23">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D534" s="24">
         <v>3.6</v>
       </c>
       <c r="E534" s="25">
-        <v>147.6</v>
+        <v>140.4</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -10932,16 +10936,16 @@
         <v>540</v>
       </c>
       <c r="B536" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C536" s="23">
-        <v>45.5</v>
+        <v>44.5</v>
       </c>
       <c r="D536" s="24">
         <v>3.6</v>
       </c>
       <c r="E536" s="25">
-        <v>163.80000000000001</v>
+        <v>160.19999999999999</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
@@ -10992,16 +10996,16 @@
         <v>544</v>
       </c>
       <c r="B540" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C540" s="23">
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="D540" s="24">
         <v>3.85</v>
       </c>
       <c r="E540" s="25">
-        <v>202.13</v>
+        <v>194.43</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
@@ -11009,16 +11013,16 @@
         <v>545</v>
       </c>
       <c r="B541" s="22">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C541" s="23">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D541" s="24">
         <v>4</v>
       </c>
       <c r="E541" s="25">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -11026,16 +11030,16 @@
         <v>546</v>
       </c>
       <c r="B542" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C542" s="23">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D542" s="24">
         <v>3.8</v>
       </c>
       <c r="E542" s="25">
-        <v>110.2</v>
+        <v>72.2</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
@@ -11179,16 +11183,16 @@
         <v>555</v>
       </c>
       <c r="B551" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C551" s="23">
-        <v>21</v>
+        <v>17.5</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>99.75</v>
+        <v>83.13</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11213,16 +11217,16 @@
         <v>557</v>
       </c>
       <c r="B553" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C553" s="23">
-        <v>22.12</v>
+        <v>14.62</v>
       </c>
       <c r="D553" s="24">
         <v>5</v>
       </c>
       <c r="E553" s="25">
-        <v>110.6</v>
+        <v>73.099999999999994</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11298,16 +11302,16 @@
         <v>562</v>
       </c>
       <c r="B558" s="22">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C558" s="23">
-        <v>31.5</v>
+        <v>46.5</v>
       </c>
       <c r="D558" s="24">
         <v>5.5</v>
       </c>
       <c r="E558" s="25">
-        <v>173.25</v>
+        <v>255.75</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11315,16 +11319,16 @@
         <v>563</v>
       </c>
       <c r="B559" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C559" s="23">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
       <c r="D559" s="24">
         <v>5.75</v>
       </c>
       <c r="E559" s="25">
-        <v>43.13</v>
+        <v>31.63</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
@@ -11332,16 +11336,16 @@
         <v>564</v>
       </c>
       <c r="B560" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C560" s="23">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D560" s="24">
         <v>5.75</v>
       </c>
       <c r="E560" s="25">
-        <v>132.25</v>
+        <v>120.75</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11494,16 +11498,16 @@
         <v>574</v>
       </c>
       <c r="B570" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C570" s="23">
-        <v>14</v>
+        <v>12.5</v>
       </c>
       <c r="D570" s="24">
         <v>7.25</v>
       </c>
       <c r="E570" s="25">
-        <v>101.5</v>
+        <v>90.63</v>
       </c>
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
@@ -11545,16 +11549,16 @@
         <v>577</v>
       </c>
       <c r="B573" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C573" s="23">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="D573" s="24">
         <v>10</v>
       </c>
       <c r="E573" s="25">
-        <v>-15</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
@@ -11562,16 +11566,16 @@
         <v>578</v>
       </c>
       <c r="B574" s="22">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C574" s="23">
-        <v>16.5</v>
+        <v>11.5</v>
       </c>
       <c r="D574" s="24">
         <v>8.75</v>
       </c>
       <c r="E574" s="25">
-        <v>144.38</v>
+        <v>100.63</v>
       </c>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
@@ -11614,7 +11618,7 @@
         <v>2.76</v>
       </c>
       <c r="E577" s="25">
-        <v>245.25</v>
+        <v>245.55</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
@@ -11639,16 +11643,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C579" s="23">
-        <v>71.739999999999995</v>
+        <v>61.24</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>197.76</v>
+        <v>169.02</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11656,16 +11660,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C580" s="23">
-        <v>33</v>
+        <v>30.5</v>
       </c>
       <c r="D580" s="24">
         <v>2.8</v>
       </c>
       <c r="E580" s="25">
-        <v>92.4</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11790,16 +11794,16 @@
         <v>592</v>
       </c>
       <c r="B588" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C588" s="23">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="D588" s="24">
         <v>3.1</v>
       </c>
       <c r="E588" s="25">
-        <v>94.55</v>
+        <v>91.45</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -11958,16 +11962,16 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C598" s="23">
-        <v>148.5</v>
+        <v>147</v>
       </c>
       <c r="D598" s="24">
         <v>1.93</v>
       </c>
       <c r="E598" s="25">
-        <v>286.55</v>
+        <v>283.64999999999998</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11975,16 +11979,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C599" s="23">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D599" s="24">
-        <v>2.8</v>
+        <v>2.84</v>
       </c>
       <c r="E599" s="25">
-        <v>640.41</v>
+        <v>618.91999999999996</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12029,13 +12033,13 @@
         <v>27</v>
       </c>
       <c r="C602" s="23">
-        <v>45.5</v>
+        <v>49.5</v>
       </c>
       <c r="D602" s="24">
         <v>4.05</v>
       </c>
       <c r="E602" s="25">
-        <v>184.28</v>
+        <v>200.48</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12066,10 +12070,10 @@
         <v>513.5</v>
       </c>
       <c r="D604" s="24">
-        <v>1.39</v>
+        <v>1.4</v>
       </c>
       <c r="E604" s="25">
-        <v>712.76</v>
+        <v>717.76</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12077,16 +12081,16 @@
         <v>609</v>
       </c>
       <c r="B605" s="22">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C605" s="23">
-        <v>974.5</v>
+        <v>971</v>
       </c>
       <c r="D605" s="24">
         <v>1.4</v>
       </c>
       <c r="E605" s="25">
-        <v>1363.19</v>
+        <v>1359.4</v>
       </c>
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
@@ -12111,10 +12115,10 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C607" s="23">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D607" s="27"/>
       <c r="E607" s="26"/>
@@ -12124,10 +12128,10 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C608" s="23">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D608" s="27"/>
       <c r="E608" s="26"/>
@@ -12137,10 +12141,10 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C609" s="23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D609" s="27"/>
       <c r="E609" s="26"/>
@@ -12150,10 +12154,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C610" s="23">
-        <v>49.3</v>
+        <v>47.8</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12189,16 +12193,16 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C613" s="23">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="D613" s="24">
         <v>0.83</v>
       </c>
       <c r="E613" s="25">
-        <v>848.93</v>
+        <v>843.15</v>
       </c>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
@@ -12206,16 +12210,16 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C614" s="23">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D614" s="24">
         <v>0.8</v>
       </c>
       <c r="E614" s="25">
-        <v>328.8</v>
+        <v>324</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12223,16 +12227,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C615" s="23">
-        <v>774.5</v>
+        <v>764.5</v>
       </c>
       <c r="D615" s="24">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="E615" s="25">
-        <v>619.6</v>
+        <v>622.84</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12240,16 +12244,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C616" s="23">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D616" s="24">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="E616" s="25">
-        <v>251.2</v>
+        <v>249.41</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12274,16 +12278,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C618" s="23">
-        <v>1777</v>
+        <v>1748</v>
       </c>
       <c r="D618" s="24">
         <v>0.52</v>
       </c>
       <c r="E618" s="25">
-        <v>924.04</v>
+        <v>908.96</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12308,16 +12312,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C620" s="23">
-        <v>1234.5</v>
+        <v>1210.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.52</v>
       </c>
       <c r="E620" s="25">
-        <v>641.94000000000005</v>
+        <v>629.46</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12325,16 +12329,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C621" s="23">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="D621" s="24">
         <v>0.5</v>
       </c>
       <c r="E621" s="25">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12342,16 +12346,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C622" s="23">
-        <v>178.5</v>
+        <v>160.5</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>92.82</v>
+        <v>83.46</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12359,16 +12363,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C623" s="23">
-        <v>628.5</v>
+        <v>622.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.7</v>
       </c>
       <c r="E623" s="25">
-        <v>439.95</v>
+        <v>435.75</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12376,16 +12380,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C624" s="23">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>118.3</v>
+        <v>106.4</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12393,16 +12397,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C625" s="23">
-        <v>-56.5</v>
+        <v>-61.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.68</v>
       </c>
       <c r="E625" s="25">
-        <v>-38.53</v>
+        <v>-41.94</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12423,10 +12427,10 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C627" s="23">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D627" s="27"/>
       <c r="E627" s="26"/>
@@ -12436,16 +12440,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C628" s="23">
-        <v>1472</v>
+        <v>1339</v>
       </c>
       <c r="D628" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E628" s="25">
-        <v>810.01</v>
+        <v>736.82</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12518,11 +12522,11 @@
       </c>
       <c r="B633" s="29"/>
       <c r="C633" s="30">
-        <v>66814.27</v>
+        <v>67982.77</v>
       </c>
       <c r="D633" s="31"/>
       <c r="E633" s="32">
-        <v>136033.14000000001</v>
+        <v>134598.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
STOCK UPDATED BY RAJ TIME 2:41
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="639">
   <si>
     <t>StkSummary</t>
   </si>
@@ -662,7 +662,7 @@
     <t>5007 PATRIKA (Dc) {{10}}</t>
   </si>
   <si>
-    <t>5008 PATRIKA 14.03</t>
+    <t>5008 PATRIKA Aa Gya</t>
   </si>
   <si>
     <t>5009 PATRIKA</t>
@@ -1184,7 +1184,7 @@
     <t>6530 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6531 PATRIKA {M}</t>
+    <t>6531 PATRIKA {M} (600 16.03)</t>
   </si>
   <si>
     <t>6532 PATRIKA (Dc) REMOVE</t>
@@ -1595,7 +1595,7 @@
     <t>9015 CARD</t>
   </si>
   <si>
-    <t>9016 CARD</t>
+    <t>9016 CARD (DC)</t>
   </si>
   <si>
     <t>9017 CARD</t>
@@ -1769,13 +1769,13 @@
     <t>9073 CARD</t>
   </si>
   <si>
-    <t>9074 CARD</t>
-  </si>
-  <si>
-    <t>9075 CARD</t>
-  </si>
-  <si>
-    <t>9076 CARD</t>
+    <t>9074 CARD (GOLDEN)</t>
+  </si>
+  <si>
+    <t>9075 CARD (YELLOW)</t>
+  </si>
+  <si>
+    <t>9076 CARD (CREAM)</t>
   </si>
   <si>
     <t>9077 CARD</t>
@@ -1793,7 +1793,7 @@
     <t>9081 CARD</t>
   </si>
   <si>
-    <t>9082 CARD</t>
+    <t>9082 CARD (DC)</t>
   </si>
   <si>
     <t>9083 CARD</t>
@@ -1875,6 +1875,9 @@
   </si>
   <si>
     <t>9109 Card</t>
+  </si>
+  <si>
+    <t>9110 CARD</t>
   </si>
   <si>
     <t>9200 CARD (YLW)</t>
@@ -2455,7 +2458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E633"/>
+  <dimension ref="A1:E634"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2563,16 +2566,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="23">
-        <v>624.5</v>
+        <v>634.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>624.5</v>
+        <v>634.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2699,16 +2702,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="23">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2716,16 +2719,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="23">
-        <v>66.5</v>
+        <v>65.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2750,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="23">
-        <v>44.5</v>
+        <v>42</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2818,16 +2821,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C24" s="23">
-        <v>89.5</v>
+        <v>86.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>187.95</v>
+        <v>181.65</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2861,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C27" s="23">
-        <v>97</v>
+        <v>93.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>227.95</v>
+        <v>219.73</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2878,16 +2881,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C28" s="23">
-        <v>119.5</v>
+        <v>115.5</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>280.83</v>
+        <v>271.43</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2895,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="23">
-        <v>17.3</v>
+        <v>10.8</v>
       </c>
       <c r="D29" s="24">
         <v>2.59</v>
       </c>
       <c r="E29" s="25">
-        <v>44.73</v>
+        <v>27.93</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2912,16 +2915,16 @@
         <v>34</v>
       </c>
       <c r="B30" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" s="23">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="D30" s="24">
         <v>2.5499999999999998</v>
       </c>
       <c r="E30" s="25">
-        <v>25.5</v>
+        <v>21.68</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,16 +2941,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C32" s="23">
-        <v>32</v>
+        <v>31.5</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>80</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3043,16 +3046,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39" s="23">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>394.2</v>
+        <v>378</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3145,16 +3148,16 @@
         <v>49</v>
       </c>
       <c r="B45" s="22">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C45" s="23">
-        <v>64.5</v>
+        <v>56</v>
       </c>
       <c r="D45" s="24">
         <v>2.35</v>
       </c>
       <c r="E45" s="25">
-        <v>151.58000000000001</v>
+        <v>131.6</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3196,16 +3199,16 @@
         <v>52</v>
       </c>
       <c r="B48" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C48" s="23">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D48" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E48" s="25">
-        <v>213.4</v>
+        <v>211.2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3213,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C49" s="23">
-        <v>1355.5</v>
+        <v>1336.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>1510.27</v>
+        <v>1489.1</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3264,16 +3267,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C52" s="23">
-        <v>869</v>
+        <v>852</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>970.95</v>
+        <v>951.96</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3281,16 +3284,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C53" s="23">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D53" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E53" s="25">
-        <v>278.56</v>
+        <v>276.33999999999997</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3298,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="C54" s="23">
-        <v>1402</v>
+        <v>1377</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>1567.14</v>
+        <v>1539.2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3332,16 +3335,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C56" s="23">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>313.5</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,16 +3467,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C64" s="23">
-        <v>231.5</v>
+        <v>211.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>486.15</v>
+        <v>444.15</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3481,16 +3484,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C65" s="23">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>732.9</v>
+        <v>688.8</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3532,16 +3535,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C68" s="23">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>173.6</v>
+        <v>170.8</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3566,16 +3569,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C70" s="23">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>81.900000000000006</v>
+        <v>73.8</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,16 +3586,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C71" s="23">
-        <v>155.5</v>
+        <v>153.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>139.94999999999999</v>
+        <v>138.15</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3600,16 +3603,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C72" s="23">
-        <v>2348</v>
+        <v>2328</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3639.4</v>
+        <v>3608.4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3617,16 +3620,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C73" s="23">
-        <v>1744</v>
+        <v>1712.5</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2703.2</v>
+        <v>2654.38</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3634,16 +3637,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C74" s="23">
-        <v>1359.5</v>
+        <v>1339.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>2107.23</v>
+        <v>2076.23</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,10 +3695,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C78" s="23">
-        <v>691.5</v>
+        <v>686.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3718,10 +3721,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C80" s="23">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3744,10 +3747,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C82" s="23">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3757,16 +3760,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C83" s="23">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>277.14999999999998</v>
+        <v>246.1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3774,16 +3777,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C84" s="23">
-        <v>611</v>
+        <v>593</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>702.65</v>
+        <v>681.95</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3825,16 +3828,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C87" s="23">
-        <v>1067</v>
+        <v>1064.5</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1493.8</v>
+        <v>1490.3</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3868,16 +3871,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C90" s="23">
-        <v>1086.5</v>
+        <v>1080</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2173</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3885,16 +3888,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C91" s="23">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>424.62</v>
+        <v>419.58</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3997,16 +4000,16 @@
         <v>103</v>
       </c>
       <c r="B99" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C99" s="23">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D99" s="24">
         <v>1.55</v>
       </c>
       <c r="E99" s="25">
-        <v>421.6</v>
+        <v>406.1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4014,16 +4017,16 @@
         <v>104</v>
       </c>
       <c r="B100" s="22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C100" s="23">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="D100" s="24">
         <v>1.55</v>
       </c>
       <c r="E100" s="25">
-        <v>434</v>
+        <v>384.4</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4065,10 +4068,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C103" s="23">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4078,10 +4081,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C104" s="23">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4091,10 +4094,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C105" s="23">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4117,10 +4120,10 @@
         <v>111</v>
       </c>
       <c r="B107" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C107" s="23">
-        <v>13.5</v>
+        <v>8.5</v>
       </c>
       <c r="D107" s="27"/>
       <c r="E107" s="26"/>
@@ -4207,16 +4210,16 @@
         <v>117</v>
       </c>
       <c r="B113" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C113" s="23">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D113" s="24">
         <v>12.5</v>
       </c>
       <c r="E113" s="25">
-        <v>287.5</v>
+        <v>237.5</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4399,16 +4402,16 @@
         <v>129</v>
       </c>
       <c r="B125" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C125" s="23">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D125" s="24">
         <v>15.5</v>
       </c>
       <c r="E125" s="25">
-        <v>124</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4733,16 +4736,16 @@
         <v>149</v>
       </c>
       <c r="B145" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C145" s="23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D145" s="24">
         <v>18.399999999999999</v>
       </c>
       <c r="E145" s="25">
-        <v>183.97</v>
+        <v>147.16999999999999</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4767,16 +4770,16 @@
         <v>151</v>
       </c>
       <c r="B147" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C147" s="23">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="D147" s="24">
-        <v>18.43</v>
+        <v>18.440000000000001</v>
       </c>
       <c r="E147" s="25">
-        <v>64.510000000000005</v>
+        <v>9.2200000000000006</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4835,16 +4838,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C151" s="23">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>188.1</v>
+        <v>184.8</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4869,16 +4872,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C153" s="23">
-        <v>32.5</v>
+        <v>12.5</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>89.38</v>
+        <v>34.380000000000003</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4920,16 +4923,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C156" s="23">
-        <v>153.75</v>
+        <v>151.75</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>522.75</v>
+        <v>515.95000000000005</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4965,16 +4968,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C159" s="23">
-        <v>130.5</v>
+        <v>127.5</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>365.4</v>
+        <v>357</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4982,16 +4985,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C160" s="23">
-        <v>108.5</v>
+        <v>104.5</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>303.8</v>
+        <v>292.60000000000002</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5084,16 +5087,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C166" s="23">
-        <v>248</v>
+        <v>245.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>731.6</v>
+        <v>724.23</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5124,10 +5127,10 @@
         <v>79.5</v>
       </c>
       <c r="D168" s="24">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="E168" s="25">
-        <v>238.5</v>
+        <v>270.68</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5195,16 +5198,16 @@
         <v>177</v>
       </c>
       <c r="B173" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C173" s="23">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D173" s="24">
         <v>3.9</v>
       </c>
       <c r="E173" s="25">
-        <v>183.3</v>
+        <v>175.5</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5349,16 +5352,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C183" s="23">
-        <v>153.5</v>
+        <v>149.5</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>460.5</v>
+        <v>448.5</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5366,16 +5369,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C184" s="23">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5400,16 +5403,16 @@
         <v>190</v>
       </c>
       <c r="B186" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C186" s="23">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D186" s="24">
         <v>3.1</v>
       </c>
       <c r="E186" s="25">
-        <v>93</v>
+        <v>83.7</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5622,16 +5625,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C200" s="23">
-        <v>205.24</v>
+        <v>195.24</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>630.78</v>
+        <v>600.04999999999995</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5665,16 +5668,16 @@
         <v>207</v>
       </c>
       <c r="B203" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C203" s="23">
-        <v>59.5</v>
+        <v>56.5</v>
       </c>
       <c r="D203" s="24">
-        <v>3.29</v>
+        <v>3.38</v>
       </c>
       <c r="E203" s="25">
-        <v>195.89</v>
+        <v>190.96</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5799,16 +5802,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C213" s="23">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>115.26</v>
+        <v>107.02</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5957,16 +5960,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C223" s="23">
-        <v>62</v>
+        <v>59.5</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>279</v>
+        <v>267.75</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -6042,16 +6045,16 @@
         <v>232</v>
       </c>
       <c r="B228" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C228" s="23">
-        <v>38.5</v>
+        <v>38</v>
       </c>
       <c r="D228" s="24">
         <v>4.75</v>
       </c>
       <c r="E228" s="25">
-        <v>182.88</v>
+        <v>180.5</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6288,16 +6291,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C244" s="23">
-        <v>33.409999999999997</v>
+        <v>26.41</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>199.8</v>
+        <v>157.94</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6305,16 +6308,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C245" s="23">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>68.16</v>
+        <v>29.82</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6356,16 +6359,16 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C248" s="23">
-        <v>31.5</v>
+        <v>28</v>
       </c>
       <c r="D248" s="24">
         <v>4.5</v>
       </c>
       <c r="E248" s="25">
-        <v>141.75</v>
+        <v>126</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6435,16 +6438,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C253" s="23">
-        <v>50.5</v>
+        <v>37.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>176.75</v>
+        <v>131.25</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6469,16 +6472,16 @@
         <v>259</v>
       </c>
       <c r="B255" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C255" s="23">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D255" s="24">
         <v>4.25</v>
       </c>
       <c r="E255" s="25">
-        <v>323</v>
+        <v>314.5</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6495,16 +6498,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C257" s="23">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>158.84</v>
+        <v>142.12</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6563,16 +6566,16 @@
         <v>265</v>
       </c>
       <c r="B261" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C261" s="23">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D261" s="24">
         <v>4.5999999999999996</v>
       </c>
       <c r="E261" s="25">
-        <v>124.2</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6734,16 +6737,16 @@
         <v>276</v>
       </c>
       <c r="B272" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C272" s="23">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D272" s="24">
         <v>5.55</v>
       </c>
       <c r="E272" s="25">
-        <v>355.2</v>
+        <v>349.65</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -7027,16 +7030,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C291" s="23">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>537.66</v>
+        <v>525.29999999999995</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7192,16 +7195,16 @@
         <v>306</v>
       </c>
       <c r="B302" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C302" s="23">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D302" s="24">
         <v>7.13</v>
       </c>
       <c r="E302" s="25">
-        <v>613.17999999999995</v>
+        <v>606.04999999999995</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7443,10 +7446,10 @@
         <v>33</v>
       </c>
       <c r="D319" s="24">
-        <v>9.61</v>
+        <v>9.86</v>
       </c>
       <c r="E319" s="25">
-        <v>317.17</v>
+        <v>325.23</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -7505,16 +7508,16 @@
         <v>327</v>
       </c>
       <c r="B323" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C323" s="23">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D323" s="24">
         <v>9</v>
       </c>
       <c r="E323" s="25">
-        <v>49.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7641,16 +7644,16 @@
         <v>335</v>
       </c>
       <c r="B331" s="22">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C331" s="23">
-        <v>83.5</v>
+        <v>70</v>
       </c>
       <c r="D331" s="24">
         <v>5.5</v>
       </c>
       <c r="E331" s="25">
-        <v>459.25</v>
+        <v>385</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7692,16 +7695,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C334" s="23">
-        <v>31.5</v>
+        <v>30.5</v>
       </c>
       <c r="D334" s="24">
         <v>7.13</v>
       </c>
       <c r="E334" s="25">
-        <v>224.6</v>
+        <v>217.47</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7921,16 +7924,16 @@
         <v>353</v>
       </c>
       <c r="B349" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C349" s="23">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="D349" s="24">
         <v>8.67</v>
       </c>
       <c r="E349" s="25">
-        <v>203.83</v>
+        <v>195.16</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -7938,16 +7941,16 @@
         <v>354</v>
       </c>
       <c r="B350" s="22">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C350" s="23">
-        <v>34.5</v>
+        <v>30.5</v>
       </c>
       <c r="D350" s="24">
         <v>6.5</v>
       </c>
       <c r="E350" s="25">
-        <v>224.25</v>
+        <v>198.25</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -8074,16 +8077,16 @@
         <v>362</v>
       </c>
       <c r="B358" s="22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C358" s="23">
-        <v>24.5</v>
+        <v>27.5</v>
       </c>
       <c r="D358" s="24">
         <v>10</v>
       </c>
       <c r="E358" s="25">
-        <v>245</v>
+        <v>275</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
@@ -8213,13 +8216,13 @@
         <v>8</v>
       </c>
       <c r="C366" s="23">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D366" s="24">
         <v>23.5</v>
       </c>
       <c r="E366" s="25">
-        <v>94</v>
+        <v>105.75</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -8865,16 +8868,16 @@
         <v>409</v>
       </c>
       <c r="B405" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C405" s="23">
-        <v>50.5</v>
+        <v>49.5</v>
       </c>
       <c r="D405" s="24">
         <v>2</v>
       </c>
       <c r="E405" s="25">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
@@ -9096,16 +9099,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C420" s="23">
-        <v>22.5</v>
+        <v>21</v>
       </c>
       <c r="D420" s="24">
         <v>2.75</v>
       </c>
       <c r="E420" s="25">
-        <v>61.88</v>
+        <v>57.75</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9173,16 +9176,16 @@
         <v>429</v>
       </c>
       <c r="B425" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C425" s="23">
-        <v>155.34</v>
+        <v>154.84</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>434.95</v>
+        <v>433.55</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9309,16 +9312,16 @@
         <v>437</v>
       </c>
       <c r="B433" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C433" s="23">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D433" s="24">
         <v>3.25</v>
       </c>
       <c r="E433" s="25">
-        <v>71.5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
@@ -9326,16 +9329,16 @@
         <v>438</v>
       </c>
       <c r="B434" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C434" s="23">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D434" s="24">
         <v>3.5</v>
       </c>
       <c r="E434" s="25">
-        <v>52.5</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
@@ -9435,16 +9438,16 @@
         <v>445</v>
       </c>
       <c r="B441" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C441" s="23">
-        <v>26.5</v>
+        <v>26</v>
       </c>
       <c r="D441" s="24">
         <v>3.9</v>
       </c>
       <c r="E441" s="25">
-        <v>103.35</v>
+        <v>101.4</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
@@ -9978,16 +9981,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C476" s="23">
-        <v>19.5</v>
+        <v>16.5</v>
       </c>
       <c r="D476" s="24">
         <v>7.6</v>
       </c>
       <c r="E476" s="25">
-        <v>148.19999999999999</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10100,16 +10103,16 @@
         <v>488</v>
       </c>
       <c r="B484" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C484" s="23">
-        <v>22.5</v>
+        <v>19.5</v>
       </c>
       <c r="D484" s="24">
         <v>9.5</v>
       </c>
       <c r="E484" s="25">
-        <v>213.75</v>
+        <v>185.25</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
@@ -10200,16 +10203,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C490" s="23">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>452.1</v>
+        <v>447.7</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10217,16 +10220,16 @@
         <v>495</v>
       </c>
       <c r="B491" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C491" s="23">
-        <v>248.5</v>
+        <v>194.5</v>
       </c>
       <c r="D491" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E491" s="25">
-        <v>273.35000000000002</v>
+        <v>213.95</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -10251,16 +10254,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C493" s="23">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D493" s="24">
         <v>1.4</v>
       </c>
       <c r="E493" s="25">
-        <v>320.60000000000002</v>
+        <v>317.8</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10347,16 +10350,16 @@
         <v>503</v>
       </c>
       <c r="B499" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C499" s="23">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D499" s="24">
         <v>1.55</v>
       </c>
       <c r="E499" s="25">
-        <v>432.45</v>
+        <v>426.25</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10415,16 +10418,16 @@
         <v>507</v>
       </c>
       <c r="B503" s="22">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C503" s="23">
-        <v>642.5</v>
+        <v>640.25</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>963.75</v>
+        <v>960.38</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10483,16 +10486,16 @@
         <v>511</v>
       </c>
       <c r="B507" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C507" s="23">
-        <v>19</v>
+        <v>17.5</v>
       </c>
       <c r="D507" s="24">
         <v>1.71</v>
       </c>
       <c r="E507" s="25">
-        <v>32.49</v>
+        <v>29.93</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10500,16 +10503,16 @@
         <v>512</v>
       </c>
       <c r="B508" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C508" s="23">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D508" s="24">
         <v>0.92</v>
       </c>
       <c r="E508" s="25">
-        <v>112.74</v>
+        <v>103.5</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10517,16 +10520,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C509" s="23">
-        <v>171.7</v>
+        <v>168.7</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>391.48</v>
+        <v>384.64</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10534,16 +10537,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C510" s="23">
-        <v>192.5</v>
+        <v>188.5</v>
       </c>
       <c r="D510" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E510" s="25">
-        <v>438.9</v>
+        <v>429.78</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10611,16 +10614,16 @@
         <v>519</v>
       </c>
       <c r="B515" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C515" s="23">
-        <v>109.5</v>
+        <v>106.5</v>
       </c>
       <c r="D515" s="24">
         <v>2.8</v>
       </c>
       <c r="E515" s="25">
-        <v>306.60000000000002</v>
+        <v>298.2</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -11176,13 +11179,13 @@
         <v>22</v>
       </c>
       <c r="C551" s="23">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>28.5</v>
+        <v>52.25</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11207,16 +11210,16 @@
         <v>557</v>
       </c>
       <c r="B553" s="22">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C553" s="23">
-        <v>9.1199999999999992</v>
+        <v>7.62</v>
       </c>
       <c r="D553" s="24">
         <v>5</v>
       </c>
       <c r="E553" s="25">
-        <v>45.6</v>
+        <v>38.1</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11295,13 +11298,13 @@
         <v>57</v>
       </c>
       <c r="C558" s="23">
-        <v>40.5</v>
+        <v>42</v>
       </c>
       <c r="D558" s="24">
         <v>5.5</v>
       </c>
       <c r="E558" s="25">
-        <v>222.75</v>
+        <v>231</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11394,16 +11397,16 @@
         <v>568</v>
       </c>
       <c r="B564" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C564" s="23">
-        <v>43</v>
+        <v>40.5</v>
       </c>
       <c r="D564" s="24">
         <v>6</v>
       </c>
       <c r="E564" s="25">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
@@ -11556,16 +11559,16 @@
         <v>578</v>
       </c>
       <c r="B574" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C574" s="23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D574" s="24">
         <v>8.75</v>
       </c>
       <c r="E574" s="25">
-        <v>105</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
@@ -11616,16 +11619,16 @@
         <v>582</v>
       </c>
       <c r="B578" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C578" s="23">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D578" s="24">
         <v>2.76</v>
       </c>
       <c r="E578" s="25">
-        <v>212.51</v>
+        <v>179.39</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
@@ -11633,16 +11636,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C579" s="23">
-        <v>37.24</v>
+        <v>61.24</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>102.78</v>
+        <v>169.02</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11718,16 +11721,16 @@
         <v>588</v>
       </c>
       <c r="B584" s="22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C584" s="23">
-        <v>74.5</v>
+        <v>72.5</v>
       </c>
       <c r="D584" s="24">
         <v>2.76</v>
       </c>
       <c r="E584" s="25">
-        <v>205.62</v>
+        <v>200.1</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11784,16 +11787,16 @@
         <v>592</v>
       </c>
       <c r="B588" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C588" s="23">
-        <v>29.5</v>
+        <v>28.5</v>
       </c>
       <c r="D588" s="24">
         <v>3.1</v>
       </c>
       <c r="E588" s="25">
-        <v>91.45</v>
+        <v>88.35</v>
       </c>
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
@@ -11918,16 +11921,16 @@
         <v>600</v>
       </c>
       <c r="B596" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C596" s="23">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D596" s="24">
         <v>1.92</v>
       </c>
       <c r="E596" s="25">
-        <v>288.07</v>
+        <v>284.23</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
@@ -11969,16 +11972,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C599" s="23">
-        <v>212.5</v>
+        <v>207.5</v>
       </c>
       <c r="D599" s="24">
         <v>2.84</v>
       </c>
       <c r="E599" s="25">
-        <v>603.29999999999995</v>
+        <v>589.11</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -11986,16 +11989,16 @@
         <v>604</v>
       </c>
       <c r="B600" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C600" s="23">
-        <v>35.5</v>
+        <v>33.5</v>
       </c>
       <c r="D600" s="24">
         <v>4.28</v>
       </c>
       <c r="E600" s="25">
-        <v>151.94</v>
+        <v>143.38</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
@@ -12003,16 +12006,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C601" s="23">
-        <v>53.5</v>
+        <v>50.5</v>
       </c>
       <c r="D601" s="24">
         <v>4.28</v>
       </c>
       <c r="E601" s="25">
-        <v>228.98</v>
+        <v>216.14</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12054,16 +12057,16 @@
         <v>608</v>
       </c>
       <c r="B604" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C604" s="23">
-        <v>508.5</v>
+        <v>506.5</v>
       </c>
       <c r="D604" s="24">
         <v>1.4</v>
       </c>
       <c r="E604" s="25">
-        <v>710.77</v>
+        <v>707.98</v>
       </c>
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
@@ -12088,16 +12091,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C606" s="23">
-        <v>-30</v>
+        <v>-31</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>-42</v>
+        <v>-43.4</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12183,33 +12186,29 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="C613" s="23">
-        <v>1018</v>
-      </c>
-      <c r="D613" s="24">
-        <v>0.83</v>
-      </c>
-      <c r="E613" s="25">
-        <v>839.85</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="D613" s="27"/>
+      <c r="E613" s="26"/>
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A614" s="21" t="s">
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C614" s="23">
-        <v>403</v>
+        <v>1018</v>
       </c>
       <c r="D614" s="24">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="E614" s="25">
-        <v>322.39999999999998</v>
+        <v>839.85</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12217,16 +12216,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C615" s="23">
-        <v>764.5</v>
+        <v>396</v>
       </c>
       <c r="D615" s="24">
-        <v>0.81</v>
+        <v>0.8</v>
       </c>
       <c r="E615" s="25">
-        <v>622.84</v>
+        <v>316.8</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12234,16 +12233,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C616" s="23">
-        <v>286</v>
+        <v>745.5</v>
       </c>
       <c r="D616" s="24">
         <v>0.81</v>
       </c>
       <c r="E616" s="25">
-        <v>230.84</v>
+        <v>607.36</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12251,16 +12250,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>5</v>
+        <v>122</v>
       </c>
       <c r="C617" s="23">
-        <v>1012.5</v>
+        <v>271</v>
       </c>
       <c r="D617" s="24">
-        <v>0.5</v>
+        <v>0.81</v>
       </c>
       <c r="E617" s="25">
-        <v>506.25</v>
+        <v>218.73</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12268,16 +12267,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>226</v>
+        <v>5</v>
       </c>
       <c r="C618" s="23">
-        <v>1709</v>
+        <v>1012.5</v>
       </c>
       <c r="D618" s="24">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="E618" s="25">
-        <v>888.68</v>
+        <v>506.25</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12285,16 +12284,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>7</v>
+        <v>227</v>
       </c>
       <c r="C619" s="23">
-        <v>1551</v>
+        <v>1707</v>
       </c>
       <c r="D619" s="24">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="E619" s="25">
-        <v>790.06</v>
+        <v>887.64</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12302,16 +12301,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>251</v>
+        <v>7</v>
       </c>
       <c r="C620" s="23">
-        <v>1150</v>
+        <v>1551</v>
       </c>
       <c r="D620" s="24">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="E620" s="25">
-        <v>598</v>
+        <v>790.06</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12319,16 +12318,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>16</v>
+        <v>254</v>
       </c>
       <c r="C621" s="23">
-        <v>572</v>
+        <v>1141</v>
       </c>
       <c r="D621" s="24">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="E621" s="25">
-        <v>286</v>
+        <v>593.32000000000005</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12336,16 +12335,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>165</v>
+        <v>17</v>
       </c>
       <c r="C622" s="23">
-        <v>151.5</v>
+        <v>562</v>
       </c>
       <c r="D622" s="24">
-        <v>0.52</v>
+        <v>0.5</v>
       </c>
       <c r="E622" s="25">
-        <v>78.78</v>
+        <v>281</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12353,16 +12352,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="C623" s="23">
-        <v>606</v>
+        <v>61</v>
       </c>
       <c r="D623" s="24">
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="E623" s="25">
-        <v>424.2</v>
+        <v>31.72</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12370,16 +12369,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C624" s="23">
-        <v>69.5</v>
+        <v>592</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>48.65</v>
+        <v>414.4</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12387,22 +12386,26 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>126</v>
-      </c>
-      <c r="C625" s="26"/>
-      <c r="D625" s="27"/>
-      <c r="E625" s="26"/>
+        <v>137</v>
+      </c>
+      <c r="C625" s="23">
+        <v>6.5</v>
+      </c>
+      <c r="D625" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="E625" s="25">
+        <v>4.55</v>
+      </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A626" s="21" t="s">
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>1</v>
-      </c>
-      <c r="C626" s="23">
-        <v>227</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C626" s="26"/>
       <c r="D626" s="27"/>
       <c r="E626" s="26"/>
     </row>
@@ -12411,9 +12414,11 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>10</v>
-      </c>
-      <c r="C627" s="26"/>
+        <v>1</v>
+      </c>
+      <c r="C627" s="23">
+        <v>227</v>
+      </c>
       <c r="D627" s="27"/>
       <c r="E627" s="26"/>
     </row>
@@ -12422,33 +12427,27 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>106</v>
-      </c>
-      <c r="C628" s="23">
-        <v>1270</v>
-      </c>
-      <c r="D628" s="24">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E628" s="25">
-        <v>698.86</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C628" s="26"/>
+      <c r="D628" s="27"/>
+      <c r="E628" s="26"/>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A629" s="21" t="s">
         <v>633</v>
       </c>
       <c r="B629" s="22">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="C629" s="23">
-        <v>0.5</v>
+        <v>1198</v>
       </c>
       <c r="D629" s="24">
-        <v>4.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E629" s="25">
-        <v>2.25</v>
+        <v>659.24</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12456,31 +12455,33 @@
         <v>634</v>
       </c>
       <c r="B630" s="22">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C630" s="23">
-        <v>17.5</v>
+        <v>0.5</v>
       </c>
       <c r="D630" s="24">
         <v>4.5</v>
       </c>
       <c r="E630" s="25">
-        <v>78.75</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A631" s="21" t="s">
         <v>635</v>
       </c>
-      <c r="B631" s="22"/>
+      <c r="B631" s="22">
+        <v>12</v>
+      </c>
       <c r="C631" s="23">
-        <v>7</v>
+        <v>17.5</v>
       </c>
       <c r="D631" s="24">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E631" s="25">
-        <v>21</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -12489,26 +12490,41 @@
       </c>
       <c r="B632" s="22"/>
       <c r="C632" s="23">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D632" s="24">
         <v>3</v>
       </c>
       <c r="E632" s="25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="633" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A633" s="21" t="s">
+        <v>637</v>
+      </c>
+      <c r="B633" s="22"/>
+      <c r="C633" s="23">
+        <v>3</v>
+      </c>
+      <c r="D633" s="24">
+        <v>3</v>
+      </c>
+      <c r="E633" s="25">
         <v>9</v>
       </c>
     </row>
-    <row r="633" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A633" s="28" t="s">
-        <v>637</v>
-      </c>
-      <c r="B633" s="29"/>
-      <c r="C633" s="30">
-        <v>65721.77</v>
-      </c>
-      <c r="D633" s="31"/>
-      <c r="E633" s="32">
-        <v>129235.19</v>
+    <row r="634" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A634" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="B634" s="29"/>
+      <c r="C634" s="30">
+        <v>64989.52</v>
+      </c>
+      <c r="D634" s="31"/>
+      <c r="E634" s="32">
+        <v>127685.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:02
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -2719,16 +2719,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18" s="23">
-        <v>61.5</v>
+        <v>60.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C54" s="23">
-        <v>1305.5</v>
+        <v>1299.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>1459.27</v>
+        <v>1452.57</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3352,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C57" s="23">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>758.1</v>
+        <v>748.6</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3518,16 +3518,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C67" s="23">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>58.76</v>
+        <v>53.56</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3552,16 +3552,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C69" s="23">
-        <v>178.5</v>
+        <v>145.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>124.95</v>
+        <v>101.85</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3569,16 +3569,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C70" s="23">
-        <v>-3</v>
+        <v>-8</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>-2.7</v>
+        <v>-7.2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,16 +3586,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C71" s="23">
-        <v>123.5</v>
+        <v>113.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>111.15</v>
+        <v>102.15</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3747,10 +3747,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C82" s="23">
-        <v>100.5</v>
+        <v>97.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3760,16 +3760,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C83" s="23">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>140.30000000000001</v>
+        <v>128.80000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,16 +3794,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C85" s="23">
-        <v>4238</v>
+        <v>4233</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>5933.2</v>
+        <v>5926.2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,16 +3828,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C87" s="23">
-        <v>1024</v>
+        <v>1019</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1433.6</v>
+        <v>1426.6</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4068,10 +4068,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C103" s="23">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4860,16 +4860,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C153" s="23">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>288.75</v>
+        <v>280.5</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4911,16 +4911,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C156" s="23">
-        <v>131.25</v>
+        <v>130.25</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>446.25</v>
+        <v>442.85</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -5510,16 +5510,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C193" s="23">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>150</v>
+        <v>126</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5736,16 +5736,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C209" s="23">
-        <v>49.5</v>
+        <v>48</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>188.1</v>
+        <v>182.4</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5792,16 +5792,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C213" s="23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>24.7</v>
+        <v>16.47</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5933,16 +5933,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C222" s="23">
-        <v>101</v>
+        <v>99.5</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>454.5</v>
+        <v>447.75</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6957,16 +6957,16 @@
         <v>290</v>
       </c>
       <c r="B286" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C286" s="23">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D286" s="24">
         <v>6.8</v>
       </c>
       <c r="E286" s="25">
-        <v>183.57</v>
+        <v>169.97</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -7026,16 +7026,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C291" s="23">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>494.4</v>
+        <v>482.04</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7131,16 +7131,16 @@
         <v>302</v>
       </c>
       <c r="B298" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C298" s="23">
-        <v>66.5</v>
+        <v>63.5</v>
       </c>
       <c r="D298" s="24">
         <v>6.65</v>
       </c>
       <c r="E298" s="25">
-        <v>442.23</v>
+        <v>422.28</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -7999,16 +7999,16 @@
         <v>358</v>
       </c>
       <c r="B354" s="22">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C354" s="23">
-        <v>20</v>
+        <v>21.5</v>
       </c>
       <c r="D354" s="24">
         <v>12.25</v>
       </c>
       <c r="E354" s="25">
-        <v>245</v>
+        <v>263.38</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -8152,16 +8152,16 @@
         <v>367</v>
       </c>
       <c r="B363" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C363" s="23">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="D363" s="24">
         <v>12</v>
       </c>
       <c r="E363" s="25">
-        <v>18</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8186,16 +8186,16 @@
         <v>369</v>
       </c>
       <c r="B365" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C365" s="23">
-        <v>7</v>
+        <v>-3</v>
       </c>
       <c r="D365" s="24">
         <v>11</v>
       </c>
       <c r="E365" s="25">
-        <v>77</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8288,16 +8288,16 @@
         <v>375</v>
       </c>
       <c r="B371" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C371" s="23">
-        <v>31.5</v>
+        <v>29.5</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>315</v>
+        <v>295</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8707,16 +8707,16 @@
         <v>400</v>
       </c>
       <c r="B396" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C396" s="23">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D396" s="24">
         <v>10.93</v>
       </c>
       <c r="E396" s="25">
-        <v>382.55</v>
+        <v>349.76</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
@@ -10189,16 +10189,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C490" s="23">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D490" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E490" s="25">
-        <v>407</v>
+        <v>396</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10240,16 +10240,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C493" s="23">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="D493" s="24">
         <v>1.4</v>
       </c>
       <c r="E493" s="25">
-        <v>264.60000000000002</v>
+        <v>222.6</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10404,16 +10404,16 @@
         <v>507</v>
       </c>
       <c r="B503" s="22">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C503" s="23">
-        <v>624.25</v>
+        <v>621.75</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>936.38</v>
+        <v>932.63</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -11173,16 +11173,16 @@
         <v>556</v>
       </c>
       <c r="B552" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C552" s="23">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D552" s="24">
         <v>4.75</v>
       </c>
       <c r="E552" s="25">
-        <v>35.630000000000003</v>
+        <v>21.38</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11750,16 +11750,16 @@
         <v>591</v>
       </c>
       <c r="B587" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C587" s="23">
-        <v>33.5</v>
+        <v>28.5</v>
       </c>
       <c r="D587" s="24">
         <v>3</v>
       </c>
       <c r="E587" s="25">
-        <v>100.5</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -12179,16 +12179,16 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C614" s="23">
-        <v>978</v>
+        <v>968</v>
       </c>
       <c r="D614" s="24">
         <v>0.83</v>
       </c>
       <c r="E614" s="25">
-        <v>806.85</v>
+        <v>798.6</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12366,16 +12366,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C625" s="23">
-        <v>488.5</v>
+        <v>474.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.7</v>
       </c>
       <c r="E625" s="25">
-        <v>341.95</v>
+        <v>332.15</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12424,16 +12424,16 @@
         <v>633</v>
       </c>
       <c r="B629" s="22">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C629" s="23">
-        <v>1175</v>
+        <v>1165</v>
       </c>
       <c r="D629" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E629" s="25">
-        <v>646.58000000000004</v>
+        <v>641.08000000000004</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12506,11 +12506,11 @@
       </c>
       <c r="B634" s="29"/>
       <c r="C634" s="30">
-        <v>62930.42</v>
+        <v>62702.42</v>
       </c>
       <c r="D634" s="31"/>
       <c r="E634" s="32">
-        <v>120705.32</v>
+        <v>120227.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:47
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -125,7 +125,7 @@
     <t>1866 PATRIKA</t>
   </si>
   <si>
-    <t>1867 PATRIKA (DESIGN CHANGE)</t>
+    <t>1867 PATRIKA</t>
   </si>
   <si>
     <t>1868 PATRIKA</t>
@@ -2566,16 +2566,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="23">
-        <v>634.5</v>
+        <v>624.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>634.5</v>
+        <v>624.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2600,16 +2600,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C11" s="23">
-        <v>563.5</v>
+        <v>546.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>511.6</v>
+        <v>496.17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,16 +2634,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="23">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>103.95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,16 +2685,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" s="23">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>82.8</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2702,16 +2702,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C17" s="23">
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>10</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2719,16 +2719,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="23">
-        <v>60.5</v>
+        <v>58.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2753,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C20" s="23">
-        <v>36</v>
+        <v>31.5</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2770,16 +2770,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="23">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
       </c>
       <c r="E21" s="25">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2787,16 +2787,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="23">
-        <v>20.5</v>
+        <v>6.5</v>
       </c>
       <c r="D22" s="24">
         <v>2</v>
       </c>
       <c r="E22" s="25">
-        <v>41</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2804,16 +2804,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C23" s="23">
-        <v>101.25</v>
+        <v>92.25</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>202.5</v>
+        <v>184.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2821,16 +2821,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C24" s="23">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>155.4</v>
+        <v>138.6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2838,16 +2838,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C25" s="23">
-        <v>41.5</v>
+        <v>40.5</v>
       </c>
       <c r="D25" s="24">
         <v>2.1</v>
       </c>
       <c r="E25" s="25">
-        <v>87.15</v>
+        <v>85.05</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C27" s="23">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>159.80000000000001</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2881,16 +2881,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C28" s="23">
-        <v>94.5</v>
+        <v>81.5</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>222.08</v>
+        <v>191.53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C29" s="23">
-        <v>68.5</v>
+        <v>61.5</v>
       </c>
       <c r="D29" s="24">
         <v>2.57</v>
       </c>
       <c r="E29" s="25">
-        <v>175.82</v>
+        <v>157.85</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2941,16 +2941,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C32" s="23">
-        <v>28.5</v>
+        <v>23.5</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>71.25</v>
+        <v>58.75</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,16 +2969,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C34" s="23">
-        <v>123.5</v>
+        <v>122.5</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>308.75</v>
+        <v>306.25</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,16 +3029,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C38" s="23">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>272.7</v>
+        <v>232.2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3114,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C43" s="23">
-        <v>41.5</v>
+        <v>34.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>93.38</v>
+        <v>77.63</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3131,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C44" s="23">
-        <v>43</v>
+        <v>39.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>96.75</v>
+        <v>88.88</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,16 +3182,16 @@
         <v>51</v>
       </c>
       <c r="B47" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C47" s="23">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D47" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E47" s="25">
-        <v>47.3</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="C49" s="23">
-        <v>1203</v>
+        <v>1147</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>1340.36</v>
+        <v>1277.96</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,16 +3233,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="C50" s="23">
-        <v>1085</v>
+        <v>989.5</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>1212.49</v>
+        <v>1105.77</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,16 +3267,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C52" s="23">
-        <v>750</v>
+        <v>700</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>837.99</v>
+        <v>782.12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C54" s="23">
-        <v>1299.5</v>
+        <v>1253.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>1452.57</v>
+        <v>1401.15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3335,16 +3335,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C56" s="23">
-        <v>243.5</v>
+        <v>210.5</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>267.85000000000002</v>
+        <v>231.55</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3352,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C57" s="23">
-        <v>394</v>
+        <v>359</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>748.6</v>
+        <v>682.1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,16 +3384,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C59" s="23">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>193.8</v>
+        <v>182.4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,16 +3401,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C60" s="23">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>744.8</v>
+        <v>722</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,16 +3418,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C61" s="23">
-        <v>427</v>
+        <v>408.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>896.7</v>
+        <v>857.85</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,16 +3450,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C63" s="23">
-        <v>56</v>
+        <v>51.5</v>
       </c>
       <c r="D63" s="24">
         <v>2.1</v>
       </c>
       <c r="E63" s="25">
-        <v>117.6</v>
+        <v>108.15</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3467,16 +3467,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C64" s="23">
-        <v>206.5</v>
+        <v>195.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>433.65</v>
+        <v>410.55</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3484,16 +3484,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C65" s="23">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>678.3</v>
+        <v>665.7</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3518,16 +3518,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C67" s="23">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>53.56</v>
+        <v>51.48</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3535,16 +3535,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C68" s="23">
-        <v>197</v>
+        <v>188.5</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>137.9</v>
+        <v>131.94999999999999</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3552,16 +3552,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C69" s="23">
-        <v>145.5</v>
+        <v>119.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>101.85</v>
+        <v>83.65</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3569,16 +3569,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C70" s="23">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>-7.2</v>
+        <v>-8.1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,16 +3586,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C71" s="23">
-        <v>113.5</v>
+        <v>90</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>102.15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3603,16 +3603,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C72" s="23">
-        <v>2285</v>
+        <v>2229.5</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3541.75</v>
+        <v>3455.73</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3620,16 +3620,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C73" s="23">
-        <v>1677</v>
+        <v>1618</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2599.35</v>
+        <v>2507.9</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3637,16 +3637,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C74" s="23">
-        <v>1309.5</v>
+        <v>1282.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>2029.73</v>
+        <v>1987.88</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3665,16 +3665,16 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C76" s="23">
-        <v>329</v>
+        <v>318.5</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>105.63</v>
+        <v>102.25</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,10 +3695,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C78" s="23">
-        <v>653.5</v>
+        <v>613.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3721,10 +3721,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C80" s="23">
-        <v>77.5</v>
+        <v>55</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3747,10 +3747,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C82" s="23">
-        <v>97.5</v>
+        <v>92.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3760,16 +3760,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C83" s="23">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>128.80000000000001</v>
+        <v>87.4</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3777,16 +3777,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C84" s="23">
-        <v>573</v>
+        <v>569.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>658.95</v>
+        <v>654.92999999999995</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,16 +3794,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C85" s="23">
-        <v>4233</v>
+        <v>4194</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>5926.2</v>
+        <v>5871.6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,16 +3811,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C86" s="23">
-        <v>2727.5</v>
+        <v>2691.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3818.5</v>
+        <v>3768.1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,16 +3828,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C87" s="23">
-        <v>1019</v>
+        <v>1006.5</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1426.6</v>
+        <v>1409.1</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3854,16 +3854,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C89" s="23">
-        <v>804.5</v>
+        <v>793.5</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1609</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3871,16 +3871,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C90" s="23">
-        <v>1064</v>
+        <v>1060.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2128</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3888,16 +3888,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C91" s="23">
-        <v>298.5</v>
+        <v>287.5</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>376.11</v>
+        <v>362.25</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3905,16 +3905,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C92" s="23">
-        <v>534</v>
+        <v>530.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>672.84</v>
+        <v>668.43</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4000,16 +4000,16 @@
         <v>103</v>
       </c>
       <c r="B99" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C99" s="23">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D99" s="24">
         <v>1.55</v>
       </c>
       <c r="E99" s="25">
-        <v>350.3</v>
+        <v>344.1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4017,16 +4017,16 @@
         <v>104</v>
       </c>
       <c r="B100" s="22">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C100" s="23">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D100" s="24">
         <v>1.55</v>
       </c>
       <c r="E100" s="25">
-        <v>365.8</v>
+        <v>327.05</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4193,16 +4193,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C112" s="23">
-        <v>36.5</v>
+        <v>32.5</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>456.25</v>
+        <v>406.25</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4227,16 +4227,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C114" s="23">
-        <v>30.5</v>
+        <v>29.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>381.25</v>
+        <v>368.75</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4312,16 +4312,16 @@
         <v>123</v>
       </c>
       <c r="B119" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C119" s="23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D119" s="24">
         <v>12.5</v>
       </c>
       <c r="E119" s="25">
-        <v>125</v>
+        <v>100</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4329,11 +4329,17 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>51</v>
-      </c>
-      <c r="C120" s="26"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="26"/>
+        <v>52</v>
+      </c>
+      <c r="C120" s="23">
+        <v>-1.5</v>
+      </c>
+      <c r="D120" s="24">
+        <v>12.5</v>
+      </c>
+      <c r="E120" s="25">
+        <v>-18.75</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="21" t="s">
@@ -4430,16 +4436,16 @@
         <v>131</v>
       </c>
       <c r="B127" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C127" s="23">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="D127" s="24">
         <v>15.5</v>
       </c>
       <c r="E127" s="25">
-        <v>69.75</v>
+        <v>38.75</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4843,16 +4849,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C152" s="23">
-        <v>89</v>
+        <v>60.5</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>249.2</v>
+        <v>169.4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4860,16 +4866,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C153" s="23">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>280.5</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4894,16 +4900,16 @@
         <v>159</v>
       </c>
       <c r="B155" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C155" s="23">
-        <v>25.5</v>
+        <v>22.5</v>
       </c>
       <c r="D155" s="24">
         <v>4.7</v>
       </c>
       <c r="E155" s="25">
-        <v>119.85</v>
+        <v>105.75</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -4956,16 +4962,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C159" s="23">
-        <v>105</v>
+        <v>100.5</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>294</v>
+        <v>281.39999999999998</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4973,16 +4979,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C160" s="23">
-        <v>87.5</v>
+        <v>84.5</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>245</v>
+        <v>236.6</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4990,16 +4996,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C161" s="23">
-        <v>27.5</v>
+        <v>26</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>68.75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5075,16 +5081,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C166" s="23">
-        <v>217.5</v>
+        <v>197.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>641.63</v>
+        <v>582.63</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5092,16 +5098,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C167" s="23">
-        <v>38.5</v>
+        <v>36.5</v>
       </c>
       <c r="D167" s="24">
         <v>3</v>
       </c>
       <c r="E167" s="25">
-        <v>115.5</v>
+        <v>109.5</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5109,16 +5115,16 @@
         <v>172</v>
       </c>
       <c r="B168" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C168" s="23">
-        <v>79.5</v>
+        <v>77</v>
       </c>
       <c r="D168" s="24">
         <v>3.4</v>
       </c>
       <c r="E168" s="25">
-        <v>270.68</v>
+        <v>262.17</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5143,16 +5149,16 @@
         <v>174</v>
       </c>
       <c r="B170" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C170" s="23">
-        <v>86.5</v>
+        <v>83.5</v>
       </c>
       <c r="D170" s="24">
         <v>3.3</v>
       </c>
       <c r="E170" s="25">
-        <v>285.45</v>
+        <v>275.55</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5160,7 +5166,7 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C171" s="23">
         <v>192</v>
@@ -5186,16 +5192,16 @@
         <v>177</v>
       </c>
       <c r="B173" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C173" s="23">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D173" s="24">
         <v>3.9</v>
       </c>
       <c r="E173" s="25">
-        <v>175.5</v>
+        <v>167.7</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5235,16 +5241,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C176" s="23">
-        <v>27.5</v>
+        <v>19.5</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>91.58</v>
+        <v>64.94</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5252,16 +5258,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C177" s="23">
-        <v>39.5</v>
+        <v>30</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>131.54</v>
+        <v>99.9</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5357,16 +5363,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C184" s="23">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>274.5</v>
+        <v>216</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5445,13 +5451,13 @@
         <v>70</v>
       </c>
       <c r="C189" s="23">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5459,16 +5465,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C190" s="23">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D190" s="24">
         <v>3.87</v>
       </c>
       <c r="E190" s="25">
-        <v>154.94999999999999</v>
+        <v>147.21</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5476,16 +5482,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C191" s="23">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="D191" s="24">
         <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>719.14</v>
+        <v>615.84</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5510,16 +5516,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C193" s="23">
-        <v>42</v>
+        <v>32.5</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>126</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5615,16 +5621,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C200" s="23">
-        <v>154.74</v>
+        <v>136.99</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>475.58</v>
+        <v>421.03</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5719,16 +5725,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C208" s="23">
-        <v>32.5</v>
+        <v>22.5</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>123.5</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5736,16 +5742,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C209" s="23">
-        <v>48</v>
+        <v>38.5</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>182.4</v>
+        <v>146.30000000000001</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5753,16 +5759,16 @@
         <v>214</v>
       </c>
       <c r="B210" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C210" s="23">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D210" s="24">
         <v>3.6</v>
       </c>
       <c r="E210" s="25">
-        <v>86.4</v>
+        <v>79.2</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5792,16 +5798,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C213" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>16.47</v>
+        <v>8.23</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5809,16 +5815,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C214" s="23">
-        <v>73</v>
+        <v>68.5</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>300.66000000000003</v>
+        <v>282.12</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5826,16 +5832,16 @@
         <v>219</v>
       </c>
       <c r="B215" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C215" s="23">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D215" s="24">
         <v>4.75</v>
       </c>
       <c r="E215" s="25">
-        <v>185.25</v>
+        <v>175.75</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5843,16 +5849,16 @@
         <v>220</v>
       </c>
       <c r="B216" s="22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C216" s="23">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D216" s="24">
         <v>4.75</v>
       </c>
       <c r="E216" s="25">
-        <v>128.25</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -5860,16 +5866,16 @@
         <v>221</v>
       </c>
       <c r="B217" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C217" s="23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D217" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E217" s="25">
-        <v>88</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -5933,16 +5939,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C222" s="23">
-        <v>99.5</v>
+        <v>93</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>447.75</v>
+        <v>418.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5950,16 +5956,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C223" s="23">
-        <v>145.5</v>
+        <v>143</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>654.75</v>
+        <v>643.5</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5967,16 +5973,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C224" s="23">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>215.25</v>
+        <v>162.75</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6018,16 +6024,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C227" s="23">
-        <v>28.5</v>
+        <v>26</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>128.25</v>
+        <v>117</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6067,16 +6073,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C230" s="23">
-        <v>74.5</v>
+        <v>71.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>391.13</v>
+        <v>375.38</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6174,16 +6180,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C237" s="23">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>510</v>
+        <v>498</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6215,16 +6221,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C240" s="23">
-        <v>84.8</v>
+        <v>79.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>483.36</v>
+        <v>454.86</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6232,16 +6238,16 @@
         <v>245</v>
       </c>
       <c r="B241" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C241" s="23">
-        <v>30.5</v>
+        <v>27</v>
       </c>
       <c r="D241" s="24">
         <v>6.75</v>
       </c>
       <c r="E241" s="25">
-        <v>205.88</v>
+        <v>182.25</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6264,16 +6270,16 @@
         <v>247</v>
       </c>
       <c r="B243" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C243" s="23">
-        <v>25.5</v>
+        <v>24</v>
       </c>
       <c r="D243" s="24">
         <v>6.75</v>
       </c>
       <c r="E243" s="25">
-        <v>172.13</v>
+        <v>162</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6281,16 +6287,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C244" s="23">
-        <v>66.91</v>
+        <v>63.91</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>400.26</v>
+        <v>382.31</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6315,16 +6321,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C246" s="23">
-        <v>73.5</v>
+        <v>47.5</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>294</v>
+        <v>190</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6383,16 +6389,16 @@
         <v>254</v>
       </c>
       <c r="B250" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C250" s="23">
-        <v>21.5</v>
+        <v>8.5</v>
       </c>
       <c r="D250" s="24">
         <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>110.84</v>
+        <v>43.82</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6400,16 +6406,16 @@
         <v>255</v>
       </c>
       <c r="B251" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C251" s="23">
-        <v>24.5</v>
+        <v>16.5</v>
       </c>
       <c r="D251" s="24">
         <v>3.8</v>
       </c>
       <c r="E251" s="25">
-        <v>93.1</v>
+        <v>62.7</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6428,16 +6434,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C253" s="23">
-        <v>106.5</v>
+        <v>103.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>372.75</v>
+        <v>362.25</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6445,16 +6451,16 @@
         <v>258</v>
       </c>
       <c r="B254" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C254" s="23">
-        <v>65.5</v>
+        <v>64.5</v>
       </c>
       <c r="D254" s="24">
         <v>4.25</v>
       </c>
       <c r="E254" s="25">
-        <v>278.38</v>
+        <v>274.13</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6488,16 +6494,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C257" s="23">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>83.6</v>
+        <v>66.88</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6522,16 +6528,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C259" s="23">
-        <v>116.5</v>
+        <v>110.5</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>498.62</v>
+        <v>472.94</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6539,16 +6545,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C260" s="23">
-        <v>38</v>
+        <v>29.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>162.63999999999999</v>
+        <v>126.26</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6676,16 +6682,16 @@
         <v>273</v>
       </c>
       <c r="B269" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C269" s="23">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D269" s="24">
         <v>5.3</v>
       </c>
       <c r="E269" s="25">
-        <v>174.9</v>
+        <v>148.4</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6693,16 +6699,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C270" s="23">
-        <v>30</v>
+        <v>26.5</v>
       </c>
       <c r="D270" s="24">
         <v>5.4</v>
       </c>
       <c r="E270" s="25">
-        <v>162</v>
+        <v>143.1</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6727,16 +6733,16 @@
         <v>276</v>
       </c>
       <c r="B272" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C272" s="23">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D272" s="24">
         <v>5.55</v>
       </c>
       <c r="E272" s="25">
-        <v>271.95</v>
+        <v>266.39999999999998</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -6804,16 +6810,16 @@
         <v>281</v>
       </c>
       <c r="B277" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C277" s="23">
-        <v>49.5</v>
+        <v>43.5</v>
       </c>
       <c r="D277" s="24">
         <v>6.25</v>
       </c>
       <c r="E277" s="25">
-        <v>309.38</v>
+        <v>271.88</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -7000,16 +7006,16 @@
         <v>293</v>
       </c>
       <c r="B289" s="22">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C289" s="23">
-        <v>32</v>
+        <v>20.5</v>
       </c>
       <c r="D289" s="24">
         <v>6.18</v>
       </c>
       <c r="E289" s="25">
-        <v>197.76</v>
+        <v>126.69</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7026,16 +7032,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C291" s="23">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>482.04</v>
+        <v>475.86</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7088,16 +7094,16 @@
         <v>299</v>
       </c>
       <c r="B295" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C295" s="23">
-        <v>16.5</v>
+        <v>10</v>
       </c>
       <c r="D295" s="24">
         <v>6.46</v>
       </c>
       <c r="E295" s="25">
-        <v>106.59</v>
+        <v>64.599999999999994</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -7105,16 +7111,16 @@
         <v>300</v>
       </c>
       <c r="B296" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C296" s="23">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="D296" s="24">
         <v>6.4</v>
       </c>
       <c r="E296" s="25">
-        <v>-6.4</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -7131,16 +7137,16 @@
         <v>302</v>
       </c>
       <c r="B298" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C298" s="23">
-        <v>63.5</v>
+        <v>61</v>
       </c>
       <c r="D298" s="24">
         <v>6.65</v>
       </c>
       <c r="E298" s="25">
-        <v>422.28</v>
+        <v>405.65</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -7148,16 +7154,16 @@
         <v>303</v>
       </c>
       <c r="B299" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C299" s="23">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D299" s="24">
         <v>6.18</v>
       </c>
       <c r="E299" s="25">
-        <v>370.8</v>
+        <v>364.62</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7174,16 +7180,16 @@
         <v>305</v>
       </c>
       <c r="B301" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C301" s="23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D301" s="24">
         <v>7.13</v>
       </c>
       <c r="E301" s="25">
-        <v>42.75</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7191,16 +7197,16 @@
         <v>306</v>
       </c>
       <c r="B302" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C302" s="23">
-        <v>83.5</v>
+        <v>83</v>
       </c>
       <c r="D302" s="24">
         <v>7.13</v>
       </c>
       <c r="E302" s="25">
-        <v>595.36</v>
+        <v>591.79</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -7242,16 +7248,16 @@
         <v>309</v>
       </c>
       <c r="B305" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C305" s="23">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D305" s="24">
         <v>6.65</v>
       </c>
       <c r="E305" s="25">
-        <v>186.2</v>
+        <v>172.9</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -7316,16 +7322,16 @@
         <v>315</v>
       </c>
       <c r="B311" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C311" s="23">
-        <v>16</v>
+        <v>14.5</v>
       </c>
       <c r="D311" s="24">
         <v>7.6</v>
       </c>
       <c r="E311" s="25">
-        <v>121.6</v>
+        <v>110.2</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -7623,16 +7629,16 @@
         <v>334</v>
       </c>
       <c r="B330" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C330" s="23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D330" s="24">
         <v>8.33</v>
       </c>
       <c r="E330" s="25">
-        <v>141.66999999999999</v>
+        <v>116.67</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -7640,16 +7646,16 @@
         <v>335</v>
       </c>
       <c r="B331" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C331" s="23">
-        <v>55</v>
+        <v>52.5</v>
       </c>
       <c r="D331" s="24">
         <v>5.5</v>
       </c>
       <c r="E331" s="25">
-        <v>302.5</v>
+        <v>288.75</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7657,16 +7663,16 @@
         <v>336</v>
       </c>
       <c r="B332" s="22">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C332" s="23">
-        <v>15.5</v>
+        <v>17.5</v>
       </c>
       <c r="D332" s="24">
         <v>6.89</v>
       </c>
       <c r="E332" s="25">
-        <v>106.8</v>
+        <v>120.58</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7674,16 +7680,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C333" s="23">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D333" s="24">
         <v>6.9</v>
       </c>
       <c r="E333" s="25">
-        <v>158.69999999999999</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7691,16 +7697,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C334" s="23">
-        <v>30.5</v>
+        <v>24.5</v>
       </c>
       <c r="D334" s="24">
         <v>7.13</v>
       </c>
       <c r="E334" s="25">
-        <v>217.47</v>
+        <v>174.69</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7852,16 +7858,16 @@
         <v>349</v>
       </c>
       <c r="B345" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C345" s="23">
-        <v>64.5</v>
+        <v>61.5</v>
       </c>
       <c r="D345" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E345" s="25">
-        <v>316.05</v>
+        <v>301.35000000000002</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -7999,16 +8005,16 @@
         <v>358</v>
       </c>
       <c r="B354" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C354" s="23">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="D354" s="24">
         <v>12.25</v>
       </c>
       <c r="E354" s="25">
-        <v>263.38</v>
+        <v>245</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -8118,16 +8124,16 @@
         <v>365</v>
       </c>
       <c r="B361" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C361" s="23">
-        <v>-0.5</v>
+        <v>-2.5</v>
       </c>
       <c r="D361" s="24">
         <v>39</v>
       </c>
       <c r="E361" s="25">
-        <v>-19.5</v>
+        <v>-97.5</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8135,16 +8141,16 @@
         <v>366</v>
       </c>
       <c r="B362" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C362" s="23">
-        <v>20.99</v>
+        <v>15.99</v>
       </c>
       <c r="D362" s="24">
         <v>12</v>
       </c>
       <c r="E362" s="25">
-        <v>251.88</v>
+        <v>191.88</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -8186,16 +8192,16 @@
         <v>369</v>
       </c>
       <c r="B365" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C365" s="23">
-        <v>-3</v>
+        <v>-10</v>
       </c>
       <c r="D365" s="24">
         <v>11</v>
       </c>
       <c r="E365" s="25">
-        <v>-33</v>
+        <v>-110</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8271,16 +8277,16 @@
         <v>374</v>
       </c>
       <c r="B370" s="22">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C370" s="23">
-        <v>30.73</v>
+        <v>28.23</v>
       </c>
       <c r="D370" s="24">
         <v>10</v>
       </c>
       <c r="E370" s="25">
-        <v>307.3</v>
+        <v>282.3</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -8288,16 +8294,16 @@
         <v>375</v>
       </c>
       <c r="B371" s="22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C371" s="23">
-        <v>29.5</v>
+        <v>20.5</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>295</v>
+        <v>205</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8588,16 +8594,16 @@
         <v>393</v>
       </c>
       <c r="B389" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C389" s="23">
-        <v>17.25</v>
+        <v>15.25</v>
       </c>
       <c r="D389" s="24">
         <v>11.5</v>
       </c>
       <c r="E389" s="25">
-        <v>198.38</v>
+        <v>175.38</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
@@ -8622,16 +8628,16 @@
         <v>395</v>
       </c>
       <c r="B391" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C391" s="23">
-        <v>14.5</v>
+        <v>12</v>
       </c>
       <c r="D391" s="24">
         <v>11.4</v>
       </c>
       <c r="E391" s="25">
-        <v>165.3</v>
+        <v>136.80000000000001</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
@@ -8707,16 +8713,16 @@
         <v>400</v>
       </c>
       <c r="B396" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C396" s="23">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D396" s="24">
         <v>10.93</v>
       </c>
       <c r="E396" s="25">
-        <v>349.76</v>
+        <v>316.97000000000003</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
@@ -8724,16 +8730,16 @@
         <v>401</v>
       </c>
       <c r="B397" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C397" s="23">
-        <v>18.5</v>
+        <v>12.5</v>
       </c>
       <c r="D397" s="24">
         <v>10.93</v>
       </c>
       <c r="E397" s="25">
-        <v>202.21</v>
+        <v>136.63</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8809,16 +8815,16 @@
         <v>406</v>
       </c>
       <c r="B402" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C402" s="23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D402" s="24">
         <v>2</v>
       </c>
       <c r="E402" s="25">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
@@ -8938,16 +8944,16 @@
         <v>415</v>
       </c>
       <c r="B411" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C411" s="23">
-        <v>55.5</v>
+        <v>54</v>
       </c>
       <c r="D411" s="24">
         <v>2.25</v>
       </c>
       <c r="E411" s="25">
-        <v>124.88</v>
+        <v>121.5</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -8989,16 +8995,16 @@
         <v>418</v>
       </c>
       <c r="B414" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C414" s="23">
-        <v>13</v>
+        <v>9.5</v>
       </c>
       <c r="D414" s="24">
         <v>2.5</v>
       </c>
       <c r="E414" s="25">
-        <v>32.5</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
@@ -9091,16 +9097,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C420" s="23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D420" s="24">
         <v>2.75</v>
       </c>
       <c r="E420" s="25">
-        <v>2.75</v>
+        <v>11</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9125,16 +9131,16 @@
         <v>426</v>
       </c>
       <c r="B422" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C422" s="23">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D422" s="24">
         <v>2.8</v>
       </c>
       <c r="E422" s="25">
-        <v>50.4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9142,16 +9148,16 @@
         <v>427</v>
       </c>
       <c r="B423" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C423" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D423" s="24">
         <v>2.8</v>
       </c>
       <c r="E423" s="25">
-        <v>28</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -9364,16 +9370,16 @@
         <v>441</v>
       </c>
       <c r="B437" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C437" s="23">
-        <v>9.5</v>
+        <v>6.5</v>
       </c>
       <c r="D437" s="24">
         <v>3.4</v>
       </c>
       <c r="E437" s="25">
-        <v>32.299999999999997</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -9516,16 +9522,16 @@
         <v>451</v>
       </c>
       <c r="B447" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C447" s="23">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D447" s="24">
         <v>4.25</v>
       </c>
       <c r="E447" s="25">
-        <v>136</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9669,16 +9675,16 @@
         <v>460</v>
       </c>
       <c r="B456" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C456" s="23">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D456" s="24">
         <v>4.75</v>
       </c>
       <c r="E456" s="25">
-        <v>161.5</v>
+        <v>156.75</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
@@ -9922,16 +9928,16 @@
         <v>477</v>
       </c>
       <c r="B473" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C473" s="23">
-        <v>43.5</v>
+        <v>39</v>
       </c>
       <c r="D473" s="24">
         <v>7.13</v>
       </c>
       <c r="E473" s="25">
-        <v>310.16000000000003</v>
+        <v>278.07</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
@@ -9956,16 +9962,16 @@
         <v>479</v>
       </c>
       <c r="B475" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C475" s="23">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D475" s="24">
         <v>7</v>
       </c>
       <c r="E475" s="25">
-        <v>112</v>
+        <v>84</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
@@ -9973,16 +9979,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C476" s="23">
-        <v>42.5</v>
+        <v>40</v>
       </c>
       <c r="D476" s="24">
         <v>7.6</v>
       </c>
       <c r="E476" s="25">
-        <v>323</v>
+        <v>304</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10007,16 +10013,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C478" s="23">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D478" s="24">
         <v>7.5</v>
       </c>
       <c r="E478" s="25">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -10240,16 +10246,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C493" s="23">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D493" s="24">
         <v>1.4</v>
       </c>
       <c r="E493" s="25">
-        <v>222.6</v>
+        <v>221.2</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10274,16 +10280,16 @@
         <v>499</v>
       </c>
       <c r="B495" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C495" s="23">
-        <v>340</v>
+        <v>320</v>
       </c>
       <c r="D495" s="24">
         <v>1.4</v>
       </c>
       <c r="E495" s="25">
-        <v>476</v>
+        <v>448</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10336,16 +10342,16 @@
         <v>503</v>
       </c>
       <c r="B499" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C499" s="23">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D499" s="24">
         <v>1.55</v>
       </c>
       <c r="E499" s="25">
-        <v>416.95</v>
+        <v>401.45</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10370,16 +10376,16 @@
         <v>505</v>
       </c>
       <c r="B501" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C501" s="23">
-        <v>92</v>
+        <v>89.5</v>
       </c>
       <c r="D501" s="24">
         <v>1.38</v>
       </c>
       <c r="E501" s="25">
-        <v>126.8</v>
+        <v>123.35</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
@@ -10404,16 +10410,16 @@
         <v>507</v>
       </c>
       <c r="B503" s="22">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C503" s="23">
-        <v>621.75</v>
+        <v>620.75</v>
       </c>
       <c r="D503" s="24">
         <v>1.5</v>
       </c>
       <c r="E503" s="25">
-        <v>932.63</v>
+        <v>931.13</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10472,16 +10478,16 @@
         <v>511</v>
       </c>
       <c r="B507" s="22">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C507" s="23">
-        <v>15.5</v>
+        <v>4</v>
       </c>
       <c r="D507" s="24">
         <v>1.71</v>
       </c>
       <c r="E507" s="25">
-        <v>26.51</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10489,16 +10495,16 @@
         <v>512</v>
       </c>
       <c r="B508" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C508" s="23">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D508" s="24">
         <v>0.92</v>
       </c>
       <c r="E508" s="25">
-        <v>98.88</v>
+        <v>89.64</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10506,16 +10512,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C509" s="23">
-        <v>147.69999999999999</v>
+        <v>141.69999999999999</v>
       </c>
       <c r="D509" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E509" s="25">
-        <v>336.76</v>
+        <v>323.08</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10523,16 +10529,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C510" s="23">
-        <v>169.5</v>
+        <v>166.5</v>
       </c>
       <c r="D510" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E510" s="25">
-        <v>386.46</v>
+        <v>379.62</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10600,16 +10606,16 @@
         <v>519</v>
       </c>
       <c r="B515" s="22">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C515" s="23">
-        <v>84.5</v>
+        <v>78.5</v>
       </c>
       <c r="D515" s="24">
         <v>2.8</v>
       </c>
       <c r="E515" s="25">
-        <v>236.6</v>
+        <v>219.8</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -10806,16 +10812,16 @@
         <v>533</v>
       </c>
       <c r="B529" s="22">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C529" s="23">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D529" s="24">
         <v>3.5</v>
       </c>
       <c r="E529" s="25">
-        <v>31.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -10823,16 +10829,16 @@
         <v>534</v>
       </c>
       <c r="B530" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C530" s="23">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D530" s="24">
         <v>3.33</v>
       </c>
       <c r="E530" s="25">
-        <v>179.82</v>
+        <v>173.16</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -10883,16 +10889,16 @@
         <v>538</v>
       </c>
       <c r="B534" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C534" s="23">
-        <v>24.5</v>
+        <v>23.5</v>
       </c>
       <c r="D534" s="24">
         <v>3.6</v>
       </c>
       <c r="E534" s="25">
-        <v>88.2</v>
+        <v>84.6</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -11020,16 +11026,16 @@
         <v>547</v>
       </c>
       <c r="B543" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C543" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D543" s="24">
         <v>3.8</v>
       </c>
       <c r="E543" s="25">
-        <v>38</v>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -11088,16 +11094,16 @@
         <v>551</v>
       </c>
       <c r="B547" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C547" s="23">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D547" s="24">
         <v>4.91</v>
       </c>
       <c r="E547" s="25">
-        <v>166.8</v>
+        <v>103.02</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
@@ -11156,16 +11162,16 @@
         <v>555</v>
       </c>
       <c r="B551" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C551" s="23">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>40.380000000000003</v>
+        <v>16.63</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11173,16 +11179,16 @@
         <v>556</v>
       </c>
       <c r="B552" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C552" s="23">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="D552" s="24">
         <v>4.75</v>
       </c>
       <c r="E552" s="25">
-        <v>21.38</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11275,16 +11281,16 @@
         <v>562</v>
       </c>
       <c r="B558" s="22">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C558" s="23">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D558" s="24">
         <v>5.5</v>
       </c>
       <c r="E558" s="25">
-        <v>192.5</v>
+        <v>176</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11360,16 +11366,16 @@
         <v>567</v>
       </c>
       <c r="B563" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C563" s="23">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="D563" s="24">
         <v>5.75</v>
       </c>
       <c r="E563" s="25">
-        <v>43.13</v>
+        <v>40.25</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -11411,16 +11417,16 @@
         <v>570</v>
       </c>
       <c r="B566" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C566" s="23">
-        <v>10.5</v>
+        <v>6.5</v>
       </c>
       <c r="D566" s="24">
         <v>6</v>
       </c>
       <c r="E566" s="25">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
@@ -11616,16 +11622,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C579" s="23">
-        <v>50.24</v>
+        <v>46.74</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>138.66</v>
+        <v>129</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11650,16 +11656,16 @@
         <v>585</v>
       </c>
       <c r="B581" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C581" s="23">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D581" s="24">
         <v>2.88</v>
       </c>
       <c r="E581" s="25">
-        <v>121.08</v>
+        <v>112.43</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
@@ -11701,16 +11707,16 @@
         <v>588</v>
       </c>
       <c r="B584" s="22">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C584" s="23">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D584" s="24">
         <v>2.76</v>
       </c>
       <c r="E584" s="25">
-        <v>193.2</v>
+        <v>160.08000000000001</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11818,16 +11824,16 @@
         <v>595</v>
       </c>
       <c r="B591" s="22">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C591" s="23">
-        <v>8.5</v>
+        <v>4.5</v>
       </c>
       <c r="D591" s="24">
         <v>4</v>
       </c>
       <c r="E591" s="25">
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -11884,16 +11890,16 @@
         <v>599</v>
       </c>
       <c r="B595" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C595" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D595" s="24">
         <v>4.95</v>
       </c>
       <c r="E595" s="25">
-        <v>103.86</v>
+        <v>54.4</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -11901,16 +11907,16 @@
         <v>600</v>
       </c>
       <c r="B596" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C596" s="23">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D596" s="24">
         <v>1.92</v>
       </c>
       <c r="E596" s="25">
-        <v>270.79000000000002</v>
+        <v>261.19</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
@@ -11952,16 +11958,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C599" s="23">
-        <v>197</v>
+        <v>191.5</v>
       </c>
       <c r="D599" s="24">
         <v>2.84</v>
       </c>
       <c r="E599" s="25">
-        <v>559.29999999999995</v>
+        <v>543.67999999999995</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -12054,16 +12060,16 @@
         <v>609</v>
       </c>
       <c r="B605" s="22">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C605" s="23">
-        <v>949</v>
+        <v>934</v>
       </c>
       <c r="D605" s="24">
         <v>1.4</v>
       </c>
       <c r="E605" s="25">
-        <v>1328.6</v>
+        <v>1307.5999999999999</v>
       </c>
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
@@ -12071,16 +12077,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C606" s="23">
-        <v>-44</v>
+        <v>-48</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>-61.6</v>
+        <v>-67.2</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12088,10 +12094,10 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C607" s="23">
-        <v>34.5</v>
+        <v>29</v>
       </c>
       <c r="D607" s="27"/>
       <c r="E607" s="26"/>
@@ -12114,10 +12120,10 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C609" s="23">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D609" s="27"/>
       <c r="E609" s="26"/>
@@ -12127,10 +12133,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C610" s="23">
-        <v>39.299999999999997</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12179,16 +12185,16 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C614" s="23">
-        <v>968</v>
+        <v>953</v>
       </c>
       <c r="D614" s="24">
         <v>0.83</v>
       </c>
       <c r="E614" s="25">
-        <v>798.6</v>
+        <v>786.23</v>
       </c>
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
@@ -12196,16 +12202,16 @@
         <v>619</v>
       </c>
       <c r="B615" s="22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C615" s="23">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D615" s="24">
         <v>0.8</v>
       </c>
       <c r="E615" s="25">
-        <v>314.39999999999998</v>
+        <v>305.60000000000002</v>
       </c>
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
@@ -12213,16 +12219,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C616" s="23">
-        <v>745.5</v>
+        <v>735.5</v>
       </c>
       <c r="D616" s="24">
         <v>0.81</v>
       </c>
       <c r="E616" s="25">
-        <v>607.36</v>
+        <v>599.21</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12230,16 +12236,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C617" s="23">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="D617" s="24">
         <v>0.81</v>
       </c>
       <c r="E617" s="25">
-        <v>215.51</v>
+        <v>201.79</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12264,16 +12270,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="C619" s="23">
-        <v>1680</v>
+        <v>1663</v>
       </c>
       <c r="D619" s="24">
         <v>0.52</v>
       </c>
       <c r="E619" s="25">
-        <v>873.6</v>
+        <v>864.76</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12298,16 +12304,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C621" s="23">
-        <v>1065</v>
+        <v>1011</v>
       </c>
       <c r="D621" s="24">
         <v>0.52</v>
       </c>
       <c r="E621" s="25">
-        <v>553.79999999999995</v>
+        <v>525.72</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12318,13 +12324,13 @@
         <v>18</v>
       </c>
       <c r="C622" s="23">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="D622" s="24">
         <v>0.5</v>
       </c>
       <c r="E622" s="25">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12332,16 +12338,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C623" s="23">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D623" s="24">
         <v>0.52</v>
       </c>
       <c r="E623" s="25">
-        <v>223.08</v>
+        <v>221.52</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12349,16 +12355,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C624" s="23">
-        <v>702.5</v>
+        <v>676.5</v>
       </c>
       <c r="D624" s="24">
         <v>0.7</v>
       </c>
       <c r="E624" s="25">
-        <v>491.75</v>
+        <v>473.55</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12366,16 +12372,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C625" s="23">
-        <v>474.5</v>
+        <v>447.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.7</v>
       </c>
       <c r="E625" s="25">
-        <v>332.15</v>
+        <v>313.25</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12424,16 +12430,16 @@
         <v>633</v>
       </c>
       <c r="B629" s="22">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C629" s="23">
-        <v>1165</v>
+        <v>1141.5</v>
       </c>
       <c r="D629" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E629" s="25">
-        <v>641.08000000000004</v>
+        <v>628.14</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12506,11 +12512,11 @@
       </c>
       <c r="B634" s="29"/>
       <c r="C634" s="30">
-        <v>62702.42</v>
+        <v>60844.17</v>
       </c>
       <c r="D634" s="31"/>
       <c r="E634" s="32">
-        <v>120227.62</v>
+        <v>115870.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 2:07
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -248,10 +248,10 @@
     <t>1905 PATRIKA (ARJUN 04)</t>
   </si>
   <si>
-    <t>1906 PATRIKA (KING 01)</t>
-  </si>
-  <si>
-    <t>1907 PATRIKA (KING 02)</t>
+    <t>1906 PATRIKA (KING 01) (MIL JAYEGA)</t>
+  </si>
+  <si>
+    <t>1907 PATRIKA (KING 02) (MIL JAYEGA)</t>
   </si>
   <si>
     <t>1908 PATRIKA (सवाश्री Red)</t>
@@ -1505,7 +1505,7 @@
     <t>7335 PATRIKA (Dc)</t>
   </si>
   <si>
-    <t>7337 PATRIKA</t>
+    <t>7337 PATRIKA AGYA</t>
   </si>
   <si>
     <t>7338 PATRIKA (DC)</t>
@@ -2572,16 +2572,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="23">
-        <v>624.5</v>
+        <v>619.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>624.5</v>
+        <v>619.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2606,16 +2606,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C11" s="23">
-        <v>530</v>
+        <v>479.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>481.19</v>
+        <v>435.34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,16 +2623,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C12" s="23">
-        <v>142</v>
+        <v>138.5</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>234.3</v>
+        <v>228.53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2657,16 +2657,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="23">
-        <v>22.5</v>
+        <v>19.5</v>
       </c>
       <c r="D14" s="24">
         <v>1.8</v>
       </c>
       <c r="E14" s="25">
-        <v>40.5</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2674,16 +2674,16 @@
         <v>19</v>
       </c>
       <c r="B15" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="23">
-        <v>32.5</v>
+        <v>26.5</v>
       </c>
       <c r="D15" s="24">
         <v>1.8</v>
       </c>
       <c r="E15" s="25">
-        <v>58.5</v>
+        <v>47.7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2691,16 +2691,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C16" s="23">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>70.2</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2708,16 +2708,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C17" s="23">
-        <v>68</v>
+        <v>43.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>136</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2725,16 +2725,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="23">
-        <v>49.5</v>
+        <v>47.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,16 +2742,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C19" s="23">
-        <v>93.5</v>
+        <v>76.5</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2759,16 +2759,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C20" s="23">
-        <v>31.5</v>
+        <v>-0.5</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>63</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2793,16 +2793,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C22" s="23">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="D22" s="24">
         <v>2</v>
       </c>
       <c r="E22" s="25">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,16 +2810,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C23" s="23">
-        <v>89.25</v>
+        <v>80.25</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>178.5</v>
+        <v>160.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,16 +2827,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C24" s="23">
-        <v>58.5</v>
+        <v>51.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>122.85</v>
+        <v>108.15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2844,17 +2844,11 @@
         <v>29</v>
       </c>
       <c r="B25" s="22">
-        <v>39</v>
-      </c>
-      <c r="C25" s="23">
-        <v>16.5</v>
-      </c>
-      <c r="D25" s="24">
-        <v>2.1</v>
-      </c>
-      <c r="E25" s="25">
-        <v>34.65</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="26"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
@@ -2870,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C27" s="23">
-        <v>54</v>
+        <v>37.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>126.9</v>
+        <v>88.13</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2887,16 +2881,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C28" s="23">
-        <v>81.5</v>
+        <v>73.5</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>191.53</v>
+        <v>172.73</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C29" s="23">
-        <v>45.5</v>
+        <v>32.5</v>
       </c>
       <c r="D29" s="24">
         <v>2.57</v>
       </c>
       <c r="E29" s="25">
-        <v>116.78</v>
+        <v>83.42</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3001,16 +2995,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="23">
-        <v>59.5</v>
+        <v>58.5</v>
       </c>
       <c r="D36" s="24">
         <v>2.6</v>
       </c>
       <c r="E36" s="25">
-        <v>154.69999999999999</v>
+        <v>152.1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,16 +3012,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C37" s="23">
-        <v>112.5</v>
+        <v>107.5</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>292.5</v>
+        <v>279.5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3035,16 +3029,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C38" s="23">
-        <v>84</v>
+        <v>66.5</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>226.8</v>
+        <v>179.55</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3052,16 +3046,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C39" s="23">
-        <v>127</v>
+        <v>116.5</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>342.9</v>
+        <v>314.55</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,16 +3097,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C42" s="23">
-        <v>63.5</v>
+        <v>61.5</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>180.98</v>
+        <v>175.28</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3120,16 +3114,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C43" s="23">
-        <v>34.5</v>
+        <v>30.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>77.63</v>
+        <v>68.63</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3137,16 +3131,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C44" s="23">
-        <v>45.5</v>
+        <v>41.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>102.38</v>
+        <v>93.38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3171,16 +3165,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C46" s="23">
-        <v>98.5</v>
+        <v>97.5</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>231.48</v>
+        <v>229.13</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3205,16 +3199,16 @@
         <v>52</v>
       </c>
       <c r="B48" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C48" s="23">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="D48" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E48" s="25">
-        <v>211.2</v>
+        <v>200.2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="C49" s="23">
-        <v>1106</v>
+        <v>972.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>1232.28</v>
+        <v>1083.54</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3239,16 +3233,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="C50" s="23">
-        <v>951.5</v>
+        <v>823.5</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>1063.3</v>
+        <v>920.26</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3256,16 +3250,16 @@
         <v>55</v>
       </c>
       <c r="B51" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C51" s="23">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D51" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E51" s="25">
-        <v>72.599999999999994</v>
+        <v>61.6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3273,16 +3267,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="C52" s="23">
-        <v>696</v>
+        <v>534.5</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>777.65</v>
+        <v>597.21</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,16 +3284,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C53" s="23">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="D53" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E53" s="25">
-        <v>231.95</v>
+        <v>209.75</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3307,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="C54" s="23">
-        <v>1193</v>
+        <v>1029.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>1333.52</v>
+        <v>1150.76</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3341,16 +3335,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C56" s="23">
-        <v>202.5</v>
+        <v>154.5</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>222.75</v>
+        <v>169.95</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3358,16 +3352,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C57" s="23">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>655.5</v>
+        <v>630.79999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3390,16 +3384,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C59" s="23">
-        <v>84</v>
+        <v>81.5</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>159.6</v>
+        <v>154.85</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3407,16 +3401,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C60" s="23">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>706.8</v>
+        <v>703</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3424,16 +3418,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C61" s="23">
-        <v>389.5</v>
+        <v>370.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>817.95</v>
+        <v>778.05</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3456,16 +3450,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="22">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C63" s="23">
-        <v>49.5</v>
+        <v>42.5</v>
       </c>
       <c r="D63" s="24">
         <v>2.1</v>
       </c>
       <c r="E63" s="25">
-        <v>103.95</v>
+        <v>89.25</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3473,16 +3467,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C64" s="23">
-        <v>195.5</v>
+        <v>142.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>410.55</v>
+        <v>299.25</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3490,16 +3484,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C65" s="23">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>653.1</v>
+        <v>642.6</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3507,16 +3501,16 @@
         <v>70</v>
       </c>
       <c r="B66" s="22">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C66" s="23">
-        <v>200.5</v>
+        <v>190.5</v>
       </c>
       <c r="D66" s="24">
         <v>0.52</v>
       </c>
       <c r="E66" s="25">
-        <v>104.26</v>
+        <v>99.06</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3541,16 +3535,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C68" s="23">
-        <v>190.5</v>
+        <v>181.5</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>133.35</v>
+        <v>127.05</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3558,16 +3552,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C69" s="23">
-        <v>110.5</v>
+        <v>29.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>77.349999999999994</v>
+        <v>20.65</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3575,16 +3569,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C70" s="23">
-        <v>4</v>
+        <v>369</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>3.6</v>
+        <v>332.1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,16 +3586,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C71" s="23">
-        <v>60</v>
+        <v>217</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>54</v>
+        <v>195.3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3609,16 +3603,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="C72" s="23">
-        <v>2190</v>
+        <v>2044</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3394.5</v>
+        <v>3168.2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3626,16 +3620,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C73" s="23">
-        <v>1588.5</v>
+        <v>1445.5</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2462.1799999999998</v>
+        <v>2240.5300000000002</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3643,16 +3637,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C74" s="23">
-        <v>1232</v>
+        <v>1152</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>1909.6</v>
+        <v>1785.6</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3671,16 +3665,16 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C76" s="23">
-        <v>314.5</v>
+        <v>277.5</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>100.97</v>
+        <v>89.09</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,10 +3695,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C78" s="23">
-        <v>741.5</v>
+        <v>713.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3727,10 +3721,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="C80" s="23">
-        <v>28.5</v>
+        <v>-6.5</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3753,10 +3747,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C82" s="23">
-        <v>284</v>
+        <v>241.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3766,16 +3760,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C83" s="23">
-        <v>52</v>
+        <v>0.5</v>
       </c>
       <c r="D83" s="24">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>59.8</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,16 +3777,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C84" s="23">
-        <v>558.5</v>
+        <v>505.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>642.28</v>
+        <v>581.33000000000004</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3800,16 +3794,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="C85" s="23">
-        <v>4114</v>
+        <v>4021</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>5759.6</v>
+        <v>5629.4</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3817,16 +3811,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C86" s="23">
-        <v>2665.5</v>
+        <v>2604</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3731.7</v>
+        <v>3645.6</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,16 +3828,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C87" s="23">
-        <v>1003.5</v>
+        <v>939.5</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1404.9</v>
+        <v>1315.3</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,16 +3854,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C89" s="23">
-        <v>765</v>
+        <v>688</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1530</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3877,16 +3871,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C90" s="23">
-        <v>1051</v>
+        <v>1036</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2102</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3894,16 +3888,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C91" s="23">
-        <v>261.5</v>
+        <v>227</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>329.49</v>
+        <v>286.02</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,16 +3905,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="C92" s="23">
-        <v>530.5</v>
+        <v>492</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>668.43</v>
+        <v>619.91999999999996</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4006,16 +4000,16 @@
         <v>103</v>
       </c>
       <c r="B99" s="22">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C99" s="23">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="D99" s="24">
         <v>1.55</v>
       </c>
       <c r="E99" s="25">
-        <v>325.5</v>
+        <v>302.25</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4023,16 +4017,16 @@
         <v>104</v>
       </c>
       <c r="B100" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C100" s="23">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="D100" s="24">
         <v>1.55</v>
       </c>
       <c r="E100" s="25">
-        <v>327.05</v>
+        <v>296.05</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,10 +4068,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C103" s="23">
-        <v>379</v>
+        <v>254</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4087,10 +4081,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C104" s="23">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4100,10 +4094,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C105" s="23">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4113,10 +4107,10 @@
         <v>110</v>
       </c>
       <c r="B106" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C106" s="23">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="D106" s="27"/>
       <c r="E106" s="26"/>
@@ -4126,10 +4120,10 @@
         <v>111</v>
       </c>
       <c r="B107" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C107" s="23">
-        <v>-11.5</v>
+        <v>-20.5</v>
       </c>
       <c r="D107" s="27"/>
       <c r="E107" s="26"/>
@@ -4199,16 +4193,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C112" s="23">
-        <v>31.5</v>
+        <v>21</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>393.75</v>
+        <v>262.5</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4216,16 +4210,16 @@
         <v>117</v>
       </c>
       <c r="B113" s="22">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C113" s="23">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D113" s="24">
         <v>12.5</v>
       </c>
       <c r="E113" s="25">
-        <v>237.5</v>
+        <v>137.5</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4233,16 +4227,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C114" s="23">
-        <v>29.5</v>
+        <v>25.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>368.75</v>
+        <v>318.75</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4318,16 +4312,16 @@
         <v>123</v>
       </c>
       <c r="B119" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C119" s="23">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D119" s="24">
         <v>12.5</v>
       </c>
       <c r="E119" s="25">
-        <v>100</v>
+        <v>81.25</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4346,16 +4340,16 @@
         <v>125</v>
       </c>
       <c r="B121" s="22">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C121" s="23">
-        <v>8</v>
+        <v>-1.5</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>100</v>
+        <v>-18.75</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4385,16 +4379,16 @@
         <v>128</v>
       </c>
       <c r="B124" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C124" s="23">
-        <v>16.5</v>
+        <v>15.5</v>
       </c>
       <c r="D124" s="24">
         <v>15.5</v>
       </c>
       <c r="E124" s="25">
-        <v>255.75</v>
+        <v>240.25</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4634,16 +4628,16 @@
         <v>143</v>
       </c>
       <c r="B139" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C139" s="23">
-        <v>6.5</v>
+        <v>1.5</v>
       </c>
       <c r="D139" s="24">
         <v>18.45</v>
       </c>
       <c r="E139" s="25">
-        <v>119.91</v>
+        <v>27.67</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4702,16 +4696,16 @@
         <v>147</v>
       </c>
       <c r="B143" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C143" s="23">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="D143" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E143" s="25">
-        <v>138.30000000000001</v>
+        <v>110.64</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4719,17 +4713,11 @@
         <v>148</v>
       </c>
       <c r="B144" s="22">
-        <v>4</v>
-      </c>
-      <c r="C144" s="23">
-        <v>1</v>
-      </c>
-      <c r="D144" s="24">
-        <v>18.27</v>
-      </c>
-      <c r="E144" s="25">
-        <v>18.27</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C144" s="26"/>
+      <c r="D144" s="27"/>
+      <c r="E144" s="26"/>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="21" t="s">
@@ -4804,11 +4792,17 @@
         <v>153</v>
       </c>
       <c r="B149" s="22">
-        <v>16</v>
-      </c>
-      <c r="C149" s="26"/>
-      <c r="D149" s="27"/>
-      <c r="E149" s="26"/>
+        <v>17</v>
+      </c>
+      <c r="C149" s="23">
+        <v>-2.5</v>
+      </c>
+      <c r="D149" s="24">
+        <v>18.41</v>
+      </c>
+      <c r="E149" s="25">
+        <v>-46.02</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="21" t="s">
@@ -4849,16 +4843,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="C152" s="23">
-        <v>48</v>
+        <v>29.5</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>134.4</v>
+        <v>82.6</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4866,16 +4860,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C153" s="23">
-        <v>82</v>
+        <v>70.5</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>225.5</v>
+        <v>193.88</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4917,16 +4911,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C156" s="23">
-        <v>117.25</v>
+        <v>97.25</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>398.65</v>
+        <v>330.65</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4945,16 +4939,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C158" s="23">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>175.5</v>
+        <v>159.30000000000001</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4962,16 +4956,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C159" s="23">
-        <v>103.5</v>
+        <v>96</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>289.8</v>
+        <v>268.8</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -5030,16 +5024,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C163" s="23">
-        <v>116.5</v>
+        <v>115.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.8</v>
       </c>
       <c r="E163" s="25">
-        <v>326.2</v>
+        <v>323.39999999999998</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5081,16 +5075,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C166" s="23">
-        <v>175.5</v>
+        <v>164.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>517.73</v>
+        <v>485.28</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5098,16 +5092,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C167" s="23">
-        <v>35.5</v>
+        <v>32.5</v>
       </c>
       <c r="D167" s="24">
         <v>3</v>
       </c>
       <c r="E167" s="25">
-        <v>106.5</v>
+        <v>97.5</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5115,16 +5109,16 @@
         <v>172</v>
       </c>
       <c r="B168" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C168" s="23">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D168" s="24">
         <v>3.4</v>
       </c>
       <c r="E168" s="25">
-        <v>262.17</v>
+        <v>258.76</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5132,16 +5126,16 @@
         <v>173</v>
       </c>
       <c r="B169" s="22">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C169" s="23">
-        <v>45</v>
+        <v>37.5</v>
       </c>
       <c r="D169" s="24">
         <v>3.3</v>
       </c>
       <c r="E169" s="25">
-        <v>148.5</v>
+        <v>123.75</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5149,16 +5143,16 @@
         <v>174</v>
       </c>
       <c r="B170" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C170" s="23">
-        <v>83.5</v>
+        <v>81.5</v>
       </c>
       <c r="D170" s="24">
         <v>3.3</v>
       </c>
       <c r="E170" s="25">
-        <v>275.55</v>
+        <v>268.95</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5166,16 +5160,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C171" s="23">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>605.5</v>
+        <v>539</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5241,16 +5235,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C176" s="23">
-        <v>23</v>
+        <v>18.5</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>76.59</v>
+        <v>61.61</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5258,16 +5252,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C177" s="23">
-        <v>26</v>
+        <v>22.5</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>86.58</v>
+        <v>74.930000000000007</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5286,16 +5280,16 @@
         <v>183</v>
       </c>
       <c r="B179" s="22">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C179" s="23">
-        <v>74</v>
+        <v>63.5</v>
       </c>
       <c r="D179" s="24">
         <v>3.6</v>
       </c>
       <c r="E179" s="25">
-        <v>266.39999999999998</v>
+        <v>228.6</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5312,16 +5306,16 @@
         <v>185</v>
       </c>
       <c r="B181" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C181" s="23">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="D181" s="24">
         <v>3.75</v>
       </c>
       <c r="E181" s="25">
-        <v>80.63</v>
+        <v>76.88</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5329,16 +5323,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C182" s="23">
-        <v>41</v>
+        <v>39.5</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>155.80000000000001</v>
+        <v>150.1</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5346,16 +5340,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C183" s="23">
-        <v>139.5</v>
+        <v>136.5</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>418.5</v>
+        <v>409.5</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5363,16 +5357,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C184" s="23">
-        <v>38.5</v>
+        <v>32</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>173.25</v>
+        <v>144</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5448,16 +5442,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C189" s="23">
-        <v>100</v>
+        <v>97.5</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>450</v>
+        <v>438.75</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5465,16 +5459,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C190" s="23">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D190" s="24">
         <v>3.87</v>
       </c>
       <c r="E190" s="25">
-        <v>139.46</v>
+        <v>81.349999999999994</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5482,16 +5476,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C191" s="23">
-        <v>154.5</v>
+        <v>151.5</v>
       </c>
       <c r="D191" s="24">
         <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>613.85</v>
+        <v>601.92999999999995</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5516,16 +5510,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C193" s="23">
-        <v>32</v>
+        <v>29.5</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>96</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5533,16 +5527,16 @@
         <v>198</v>
       </c>
       <c r="B194" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C194" s="23">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D194" s="24">
         <v>2.8</v>
       </c>
       <c r="E194" s="25">
-        <v>124.6</v>
+        <v>119</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5553,13 +5547,13 @@
         <v>11</v>
       </c>
       <c r="C195" s="23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D195" s="24">
         <v>2.8</v>
       </c>
       <c r="E195" s="25">
-        <v>19.600000000000001</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5621,16 +5615,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C200" s="23">
-        <v>152.49</v>
+        <v>126.49</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>468.66</v>
+        <v>388.75</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5664,16 +5658,16 @@
         <v>207</v>
       </c>
       <c r="B203" s="22">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C203" s="23">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D203" s="24">
         <v>3.38</v>
       </c>
       <c r="E203" s="25">
-        <v>175.75</v>
+        <v>168.99</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5725,16 +5719,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C208" s="23">
-        <v>18.5</v>
+        <v>7</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>70.3</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5742,16 +5736,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C209" s="23">
-        <v>18.5</v>
+        <v>5.5</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>70.3</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5798,16 +5792,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C213" s="23">
-        <v>-8</v>
+        <v>0.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.12</v>
       </c>
       <c r="E213" s="25">
-        <v>-32.93</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5815,16 +5809,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C214" s="23">
-        <v>125.5</v>
+        <v>108</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>516.51</v>
+        <v>444.49</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5832,16 +5826,16 @@
         <v>219</v>
       </c>
       <c r="B215" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C215" s="23">
-        <v>35.5</v>
+        <v>30.5</v>
       </c>
       <c r="D215" s="24">
         <v>4.75</v>
       </c>
       <c r="E215" s="25">
-        <v>168.63</v>
+        <v>144.88</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -5883,16 +5877,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C218" s="23">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>325.64</v>
+        <v>312.62</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5939,16 +5933,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="C222" s="23">
-        <v>79.5</v>
+        <v>30</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>357.75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5956,16 +5950,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C223" s="23">
-        <v>143.5</v>
+        <v>136</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>645.75</v>
+        <v>612</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5973,16 +5967,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C224" s="23">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>225.75</v>
+        <v>178.5</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6007,16 +6001,16 @@
         <v>230</v>
       </c>
       <c r="B226" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C226" s="23">
-        <v>32</v>
+        <v>30.5</v>
       </c>
       <c r="D226" s="24">
         <v>4.8</v>
       </c>
       <c r="E226" s="25">
-        <v>153.6</v>
+        <v>146.4</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6090,16 +6084,16 @@
         <v>235</v>
       </c>
       <c r="B231" s="22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C231" s="23">
-        <v>97.5</v>
+        <v>94.5</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>511.88</v>
+        <v>496.13</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6107,16 +6101,16 @@
         <v>236</v>
       </c>
       <c r="B232" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C232" s="23">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D232" s="24">
         <v>4.75</v>
       </c>
       <c r="E232" s="25">
-        <v>85.5</v>
+        <v>80.75</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6180,16 +6174,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C237" s="23">
-        <v>83</v>
+        <v>80.5</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>498</v>
+        <v>483</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6221,16 +6215,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C240" s="23">
-        <v>79.8</v>
+        <v>67.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>454.86</v>
+        <v>386.46</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6270,16 +6264,16 @@
         <v>247</v>
       </c>
       <c r="B243" s="22">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C243" s="23">
-        <v>24</v>
+        <v>17.5</v>
       </c>
       <c r="D243" s="24">
         <v>6.75</v>
       </c>
       <c r="E243" s="25">
-        <v>162</v>
+        <v>118.13</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6287,16 +6281,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C244" s="23">
-        <v>62.41</v>
+        <v>37.909999999999997</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>373.34</v>
+        <v>226.78</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6304,33 +6298,27 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>46</v>
-      </c>
-      <c r="C245" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="D245" s="24">
-        <v>4.26</v>
-      </c>
-      <c r="E245" s="25">
-        <v>2.13</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C245" s="26"/>
+      <c r="D245" s="27"/>
+      <c r="E245" s="26"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" s="21" t="s">
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C246" s="23">
-        <v>42.5</v>
+        <v>32.5</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6355,16 +6343,16 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C248" s="23">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D248" s="24">
         <v>4.5</v>
       </c>
       <c r="E248" s="25">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6406,16 +6394,16 @@
         <v>255</v>
       </c>
       <c r="B251" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C251" s="23">
-        <v>9.5</v>
+        <v>4.5</v>
       </c>
       <c r="D251" s="24">
         <v>3.8</v>
       </c>
       <c r="E251" s="25">
-        <v>36.1</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6434,16 +6422,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C253" s="23">
-        <v>86</v>
+        <v>77.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>301</v>
+        <v>271.25</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6451,16 +6439,16 @@
         <v>258</v>
       </c>
       <c r="B254" s="22">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C254" s="23">
-        <v>68.5</v>
+        <v>58</v>
       </c>
       <c r="D254" s="24">
         <v>4.25</v>
       </c>
       <c r="E254" s="25">
-        <v>291.13</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6494,16 +6482,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C257" s="23">
-        <v>16</v>
+        <v>12.5</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>66.88</v>
+        <v>52.25</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6528,16 +6516,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C259" s="23">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>787.52</v>
+        <v>684.8</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6545,16 +6533,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C260" s="23">
-        <v>89.5</v>
+        <v>85.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>383.06</v>
+        <v>365.94</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6596,16 +6584,16 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C263" s="23">
-        <v>49.8</v>
+        <v>44.8</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>246.51</v>
+        <v>221.76</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6714,16 +6702,16 @@
         <v>275</v>
       </c>
       <c r="B271" s="22">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C271" s="23">
-        <v>27.5</v>
+        <v>14.5</v>
       </c>
       <c r="D271" s="24">
         <v>5.4</v>
       </c>
       <c r="E271" s="25">
-        <v>148.5</v>
+        <v>78.3</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6748,16 +6736,16 @@
         <v>277</v>
       </c>
       <c r="B273" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C273" s="23">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D273" s="24">
         <v>5.55</v>
       </c>
       <c r="E273" s="25">
-        <v>277.5</v>
+        <v>249.75</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6825,16 +6813,16 @@
         <v>282</v>
       </c>
       <c r="B278" s="22">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C278" s="23">
-        <v>47.5</v>
+        <v>37.5</v>
       </c>
       <c r="D278" s="24">
         <v>6.25</v>
       </c>
       <c r="E278" s="25">
-        <v>296.88</v>
+        <v>234.38</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6842,16 +6830,16 @@
         <v>283</v>
       </c>
       <c r="B279" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C279" s="23">
-        <v>33.700000000000003</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="D279" s="24">
         <v>6.38</v>
       </c>
       <c r="E279" s="25">
-        <v>215.04</v>
+        <v>211.85</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -6910,16 +6898,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C283" s="23">
-        <v>46.88</v>
+        <v>40.880000000000003</v>
       </c>
       <c r="D283" s="24">
         <v>5.94</v>
       </c>
       <c r="E283" s="25">
-        <v>278.47000000000003</v>
+        <v>242.83</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6927,16 +6915,16 @@
         <v>288</v>
       </c>
       <c r="B284" s="22">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C284" s="23">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D284" s="24">
         <v>5.7</v>
       </c>
       <c r="E284" s="25">
-        <v>233.7</v>
+        <v>210.9</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -6944,16 +6932,16 @@
         <v>289</v>
       </c>
       <c r="B285" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C285" s="23">
-        <v>46.5</v>
+        <v>44</v>
       </c>
       <c r="D285" s="24">
         <v>5.94</v>
       </c>
       <c r="E285" s="25">
-        <v>276.20999999999998</v>
+        <v>261.36</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -7021,16 +7009,16 @@
         <v>294</v>
       </c>
       <c r="B290" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C290" s="23">
-        <v>22</v>
+        <v>18.5</v>
       </c>
       <c r="D290" s="24">
         <v>6.18</v>
       </c>
       <c r="E290" s="25">
-        <v>135.96</v>
+        <v>114.33</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -7047,16 +7035,16 @@
         <v>296</v>
       </c>
       <c r="B292" s="22">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C292" s="23">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D292" s="24">
         <v>6.18</v>
       </c>
       <c r="E292" s="25">
-        <v>482.04</v>
+        <v>407.88</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -7112,13 +7100,13 @@
         <v>18</v>
       </c>
       <c r="C296" s="23">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D296" s="24">
         <v>6.46</v>
       </c>
       <c r="E296" s="25">
-        <v>64.599999999999994</v>
+        <v>71.06</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -7152,16 +7140,16 @@
         <v>303</v>
       </c>
       <c r="B299" s="22">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C299" s="23">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D299" s="24">
         <v>6.65</v>
       </c>
       <c r="E299" s="25">
-        <v>405.65</v>
+        <v>352.45</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7212,16 +7200,16 @@
         <v>307</v>
       </c>
       <c r="B303" s="22">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C303" s="23">
-        <v>83</v>
+        <v>72.5</v>
       </c>
       <c r="D303" s="24">
         <v>7.13</v>
       </c>
       <c r="E303" s="25">
-        <v>591.79</v>
+        <v>516.92999999999995</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7397,16 +7385,16 @@
         <v>320</v>
       </c>
       <c r="B316" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C316" s="23">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D316" s="24">
         <v>8.08</v>
       </c>
       <c r="E316" s="25">
-        <v>84.84</v>
+        <v>68.680000000000007</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -7474,16 +7462,16 @@
         <v>325</v>
       </c>
       <c r="B321" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C321" s="23">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D321" s="24">
         <v>9.25</v>
       </c>
       <c r="E321" s="25">
-        <v>129.5</v>
+        <v>111</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -7491,16 +7479,16 @@
         <v>326</v>
       </c>
       <c r="B322" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C322" s="23">
-        <v>40.200000000000003</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="D322" s="24">
         <v>8.8000000000000007</v>
       </c>
       <c r="E322" s="25">
-        <v>353.76</v>
+        <v>292.16000000000003</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -7525,16 +7513,16 @@
         <v>328</v>
       </c>
       <c r="B324" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C324" s="23">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="D324" s="24">
         <v>9</v>
       </c>
       <c r="E324" s="25">
-        <v>85.5</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -7593,16 +7581,16 @@
         <v>332</v>
       </c>
       <c r="B328" s="22">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C328" s="23">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D328" s="24">
         <v>9.25</v>
       </c>
       <c r="E328" s="25">
-        <v>157.25</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -7661,16 +7649,16 @@
         <v>336</v>
       </c>
       <c r="B332" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C332" s="23">
-        <v>57.5</v>
+        <v>55</v>
       </c>
       <c r="D332" s="24">
         <v>5.5</v>
       </c>
       <c r="E332" s="25">
-        <v>316.25</v>
+        <v>302.5</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7678,16 +7666,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C333" s="23">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D333" s="24">
         <v>6.89</v>
       </c>
       <c r="E333" s="25">
-        <v>110.24</v>
+        <v>75.790000000000006</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7712,16 +7700,16 @@
         <v>339</v>
       </c>
       <c r="B335" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C335" s="23">
-        <v>27.5</v>
+        <v>26</v>
       </c>
       <c r="D335" s="24">
         <v>7.13</v>
       </c>
       <c r="E335" s="25">
-        <v>196.08</v>
+        <v>185.38</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -7746,16 +7734,16 @@
         <v>341</v>
       </c>
       <c r="B337" s="22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C337" s="23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D337" s="24">
         <v>8.5</v>
       </c>
       <c r="E337" s="25">
-        <v>59.5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -7791,16 +7779,16 @@
         <v>344</v>
       </c>
       <c r="B340" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C340" s="23">
-        <v>26</v>
+        <v>24.5</v>
       </c>
       <c r="D340" s="24">
         <v>7.84</v>
       </c>
       <c r="E340" s="25">
-        <v>203.84</v>
+        <v>192.08</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -7873,16 +7861,16 @@
         <v>350</v>
       </c>
       <c r="B346" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C346" s="23">
-        <v>61.5</v>
+        <v>59.5</v>
       </c>
       <c r="D346" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E346" s="25">
-        <v>301.35000000000002</v>
+        <v>291.55</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -8020,16 +8008,16 @@
         <v>359</v>
       </c>
       <c r="B355" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C355" s="23">
-        <v>21.5</v>
+        <v>20</v>
       </c>
       <c r="D355" s="24">
         <v>12.25</v>
       </c>
       <c r="E355" s="25">
-        <v>263.38</v>
+        <v>245</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -8071,16 +8059,16 @@
         <v>362</v>
       </c>
       <c r="B358" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C358" s="23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D358" s="24">
         <v>18</v>
       </c>
       <c r="E358" s="25">
-        <v>144</v>
+        <v>108</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
@@ -8088,16 +8076,16 @@
         <v>363</v>
       </c>
       <c r="B359" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C359" s="23">
-        <v>27.5</v>
+        <v>26</v>
       </c>
       <c r="D359" s="24">
         <v>10</v>
       </c>
       <c r="E359" s="25">
-        <v>275</v>
+        <v>260</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -8105,16 +8093,16 @@
         <v>364</v>
       </c>
       <c r="B360" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C360" s="23">
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="D360" s="24">
         <v>11</v>
       </c>
       <c r="E360" s="25">
-        <v>104.5</v>
+        <v>82.5</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -8139,16 +8127,16 @@
         <v>366</v>
       </c>
       <c r="B362" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C362" s="23">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D362" s="24">
         <v>39</v>
       </c>
       <c r="E362" s="25">
-        <v>97.5</v>
+        <v>39</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -8190,16 +8178,16 @@
         <v>369</v>
       </c>
       <c r="B365" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C365" s="23">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="D365" s="24">
         <v>7.84</v>
       </c>
       <c r="E365" s="25">
-        <v>54.88</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8292,16 +8280,16 @@
         <v>375</v>
       </c>
       <c r="B371" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C371" s="23">
-        <v>28.23</v>
+        <v>27.73</v>
       </c>
       <c r="D371" s="24">
         <v>10</v>
       </c>
       <c r="E371" s="25">
-        <v>282.3</v>
+        <v>277.3</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -8309,16 +8297,16 @@
         <v>376</v>
       </c>
       <c r="B372" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C372" s="23">
-        <v>16.5</v>
+        <v>14</v>
       </c>
       <c r="D372" s="24">
         <v>10</v>
       </c>
       <c r="E372" s="25">
-        <v>165</v>
+        <v>140</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -8609,16 +8597,16 @@
         <v>394</v>
       </c>
       <c r="B390" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C390" s="23">
-        <v>17.75</v>
+        <v>16.75</v>
       </c>
       <c r="D390" s="24">
         <v>11.5</v>
       </c>
       <c r="E390" s="25">
-        <v>204.13</v>
+        <v>192.63</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
@@ -8643,16 +8631,16 @@
         <v>396</v>
       </c>
       <c r="B392" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C392" s="23">
-        <v>14.5</v>
+        <v>8.5</v>
       </c>
       <c r="D392" s="24">
         <v>11.4</v>
       </c>
       <c r="E392" s="25">
-        <v>165.3</v>
+        <v>96.9</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
@@ -8728,16 +8716,16 @@
         <v>401</v>
       </c>
       <c r="B397" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C397" s="23">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="D397" s="24">
         <v>10.93</v>
       </c>
       <c r="E397" s="25">
-        <v>300.58</v>
+        <v>289.64999999999998</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8745,16 +8733,16 @@
         <v>402</v>
       </c>
       <c r="B398" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C398" s="23">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="D398" s="24">
         <v>10.93</v>
       </c>
       <c r="E398" s="25">
-        <v>202.21</v>
+        <v>180.35</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -8762,16 +8750,16 @@
         <v>403</v>
       </c>
       <c r="B399" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C399" s="23">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D399" s="24">
         <v>14.75</v>
       </c>
       <c r="E399" s="25">
-        <v>51.63</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -8862,17 +8850,11 @@
         <v>409</v>
       </c>
       <c r="B405" s="22">
-        <v>18</v>
-      </c>
-      <c r="C405" s="23">
-        <v>8</v>
-      </c>
-      <c r="D405" s="24">
-        <v>2</v>
-      </c>
-      <c r="E405" s="25">
-        <v>16</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C405" s="26"/>
+      <c r="D405" s="27"/>
+      <c r="E405" s="26"/>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" s="21" t="s">
@@ -8896,16 +8878,16 @@
         <v>411</v>
       </c>
       <c r="B407" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C407" s="23">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D407" s="24">
         <v>2</v>
       </c>
       <c r="E407" s="25">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -9076,16 +9058,16 @@
         <v>423</v>
       </c>
       <c r="B419" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C419" s="23">
-        <v>29.5</v>
+        <v>24.5</v>
       </c>
       <c r="D419" s="24">
         <v>2.7</v>
       </c>
       <c r="E419" s="25">
-        <v>79.650000000000006</v>
+        <v>66.150000000000006</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
@@ -9130,13 +9112,13 @@
         <v>90</v>
       </c>
       <c r="C422" s="23">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D422" s="24">
         <v>2.75</v>
       </c>
       <c r="E422" s="25">
-        <v>4.13</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9161,16 +9143,16 @@
         <v>428</v>
       </c>
       <c r="B424" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C424" s="23">
-        <v>12</v>
+        <v>8.5</v>
       </c>
       <c r="D424" s="24">
         <v>2.8</v>
       </c>
       <c r="E424" s="25">
-        <v>33.6</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -9204,16 +9186,16 @@
         <v>431</v>
       </c>
       <c r="B427" s="22">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C427" s="23">
-        <v>152.84</v>
+        <v>151.84</v>
       </c>
       <c r="D427" s="24">
         <v>2.8</v>
       </c>
       <c r="E427" s="25">
-        <v>427.95</v>
+        <v>425.15</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -9221,16 +9203,16 @@
         <v>432</v>
       </c>
       <c r="B428" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C428" s="23">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D428" s="24">
         <v>2.95</v>
       </c>
       <c r="E428" s="25">
-        <v>53.1</v>
+        <v>50.15</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -9272,16 +9254,16 @@
         <v>435</v>
       </c>
       <c r="B431" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C431" s="23">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D431" s="24">
         <v>3.26</v>
       </c>
       <c r="E431" s="25">
-        <v>58.68</v>
+        <v>52.16</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -9323,16 +9305,16 @@
         <v>438</v>
       </c>
       <c r="B434" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C434" s="23">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D434" s="24">
         <v>3.05</v>
       </c>
       <c r="E434" s="25">
-        <v>97.6</v>
+        <v>94.55</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
@@ -9552,16 +9534,16 @@
         <v>453</v>
       </c>
       <c r="B449" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C449" s="23">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D449" s="24">
         <v>4.25</v>
       </c>
       <c r="E449" s="25">
-        <v>127.5</v>
+        <v>119</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -9586,16 +9568,16 @@
         <v>455</v>
       </c>
       <c r="B451" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C451" s="23">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D451" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E451" s="25">
-        <v>74.709999999999994</v>
+        <v>70.56</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
@@ -9705,16 +9687,16 @@
         <v>462</v>
       </c>
       <c r="B458" s="22">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C458" s="23">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D458" s="24">
         <v>4.75</v>
       </c>
       <c r="E458" s="25">
-        <v>156.75</v>
+        <v>142.5</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -9816,16 +9798,16 @@
         <v>469</v>
       </c>
       <c r="B465" s="22">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C465" s="23">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D465" s="24">
         <v>5.5</v>
       </c>
       <c r="E465" s="25">
-        <v>313.5</v>
+        <v>308</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
@@ -9941,16 +9923,16 @@
         <v>478</v>
       </c>
       <c r="B474" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C474" s="23">
-        <v>18.5</v>
+        <v>16</v>
       </c>
       <c r="D474" s="24">
         <v>7.51</v>
       </c>
       <c r="E474" s="25">
-        <v>138.91</v>
+        <v>120.14</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
@@ -9958,16 +9940,16 @@
         <v>479</v>
       </c>
       <c r="B475" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C475" s="23">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D475" s="24">
         <v>7.13</v>
       </c>
       <c r="E475" s="25">
-        <v>256.68</v>
+        <v>221.03</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
@@ -10009,16 +9991,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C478" s="23">
-        <v>35.5</v>
+        <v>22</v>
       </c>
       <c r="D478" s="24">
         <v>7.6</v>
       </c>
       <c r="E478" s="25">
-        <v>269.8</v>
+        <v>167.2</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -10026,16 +10008,16 @@
         <v>483</v>
       </c>
       <c r="B479" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C479" s="23">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D479" s="24">
         <v>8.5</v>
       </c>
       <c r="E479" s="25">
-        <v>297.5</v>
+        <v>255</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
@@ -10125,16 +10107,16 @@
         <v>490</v>
       </c>
       <c r="B486" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C486" s="23">
-        <v>13.5</v>
+        <v>11</v>
       </c>
       <c r="D486" s="24">
         <v>9.5</v>
       </c>
       <c r="E486" s="25">
-        <v>128.25</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -10225,16 +10207,16 @@
         <v>496</v>
       </c>
       <c r="B492" s="22">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C492" s="23">
-        <v>337</v>
+        <v>226</v>
       </c>
       <c r="D492" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E492" s="25">
-        <v>370.7</v>
+        <v>248.6</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
@@ -10242,16 +10224,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C493" s="23">
-        <v>161.5</v>
+        <v>61.5</v>
       </c>
       <c r="D493" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E493" s="25">
-        <v>177.65</v>
+        <v>67.650000000000006</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10440,16 +10422,16 @@
         <v>509</v>
       </c>
       <c r="B505" s="22">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C505" s="23">
-        <v>620.75</v>
+        <v>615.75</v>
       </c>
       <c r="D505" s="24">
         <v>1.5</v>
       </c>
       <c r="E505" s="25">
-        <v>931.13</v>
+        <v>923.63</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -10508,16 +10490,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C509" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D509" s="24">
         <v>1.71</v>
       </c>
       <c r="E509" s="25">
-        <v>6.84</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10525,16 +10507,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C510" s="23">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D510" s="24">
         <v>0.92</v>
       </c>
       <c r="E510" s="25">
-        <v>89.64</v>
+        <v>79.48</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10542,16 +10524,16 @@
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C511" s="23">
-        <v>139.19999999999999</v>
+        <v>129.19999999999999</v>
       </c>
       <c r="D511" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E511" s="25">
-        <v>317.38</v>
+        <v>294.58</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10559,16 +10541,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C512" s="23">
-        <v>171.5</v>
+        <v>166.5</v>
       </c>
       <c r="D512" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E512" s="25">
-        <v>391.02</v>
+        <v>379.62</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10619,16 +10601,16 @@
         <v>520</v>
       </c>
       <c r="B516" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C516" s="23">
-        <v>32.5</v>
+        <v>27.5</v>
       </c>
       <c r="D516" s="24">
         <v>2.73</v>
       </c>
       <c r="E516" s="25">
-        <v>88.86</v>
+        <v>75.19</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
@@ -10636,16 +10618,16 @@
         <v>521</v>
       </c>
       <c r="B517" s="22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C517" s="23">
-        <v>77.5</v>
+        <v>69.5</v>
       </c>
       <c r="D517" s="24">
         <v>2.8</v>
       </c>
       <c r="E517" s="25">
-        <v>217</v>
+        <v>194.6</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -10762,16 +10744,16 @@
         <v>529</v>
       </c>
       <c r="B525" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C525" s="23">
-        <v>35.5</v>
+        <v>30.5</v>
       </c>
       <c r="D525" s="24">
         <v>2.85</v>
       </c>
       <c r="E525" s="25">
-        <v>101.18</v>
+        <v>86.93</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
@@ -10796,16 +10778,16 @@
         <v>531</v>
       </c>
       <c r="B527" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C527" s="23">
-        <v>36.5</v>
+        <v>31</v>
       </c>
       <c r="D527" s="24">
         <v>3.25</v>
       </c>
       <c r="E527" s="25">
-        <v>118.63</v>
+        <v>100.75</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
@@ -10859,16 +10841,16 @@
         <v>536</v>
       </c>
       <c r="B532" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C532" s="23">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D532" s="24">
         <v>3.33</v>
       </c>
       <c r="E532" s="25">
-        <v>173.16</v>
+        <v>169.83</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -10885,16 +10867,16 @@
         <v>538</v>
       </c>
       <c r="B534" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C534" s="23">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D534" s="24">
         <v>3.8</v>
       </c>
       <c r="E534" s="25">
-        <v>148.19999999999999</v>
+        <v>140.6</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -10922,13 +10904,13 @@
         <v>69</v>
       </c>
       <c r="C536" s="23">
-        <v>19.5</v>
+        <v>21.5</v>
       </c>
       <c r="D536" s="24">
         <v>3.6</v>
       </c>
       <c r="E536" s="25">
-        <v>70.2</v>
+        <v>77.400000000000006</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
@@ -11005,16 +10987,16 @@
         <v>546</v>
       </c>
       <c r="B542" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C542" s="23">
-        <v>49</v>
+        <v>42.5</v>
       </c>
       <c r="D542" s="24">
         <v>3.85</v>
       </c>
       <c r="E542" s="25">
-        <v>188.65</v>
+        <v>163.63</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
@@ -11022,16 +11004,16 @@
         <v>547</v>
       </c>
       <c r="B543" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C543" s="23">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="D543" s="24">
         <v>4</v>
       </c>
       <c r="E543" s="25">
-        <v>144</v>
+        <v>40</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -11090,16 +11072,16 @@
         <v>551</v>
       </c>
       <c r="B547" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C547" s="23">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="D547" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E547" s="25">
-        <v>112.2</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
@@ -11124,16 +11106,16 @@
         <v>553</v>
       </c>
       <c r="B549" s="22">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C549" s="23">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D549" s="24">
         <v>4.91</v>
       </c>
       <c r="E549" s="25">
-        <v>103.02</v>
+        <v>88.31</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -11141,16 +11123,16 @@
         <v>554</v>
       </c>
       <c r="B550" s="22">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C550" s="23">
-        <v>14.5</v>
+        <v>2.5</v>
       </c>
       <c r="D550" s="24">
         <v>4.75</v>
       </c>
       <c r="E550" s="25">
-        <v>68.88</v>
+        <v>11.88</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -11209,16 +11191,16 @@
         <v>558</v>
       </c>
       <c r="B554" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C554" s="23">
-        <v>10.5</v>
+        <v>10</v>
       </c>
       <c r="D554" s="24">
         <v>4.75</v>
       </c>
       <c r="E554" s="25">
-        <v>49.88</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
@@ -11226,16 +11208,16 @@
         <v>559</v>
       </c>
       <c r="B555" s="22">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C555" s="23">
-        <v>17.12</v>
+        <v>13.62</v>
       </c>
       <c r="D555" s="24">
         <v>5</v>
       </c>
       <c r="E555" s="25">
-        <v>85.6</v>
+        <v>68.099999999999994</v>
       </c>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.25">
@@ -11311,16 +11293,16 @@
         <v>564</v>
       </c>
       <c r="B560" s="22">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C560" s="23">
-        <v>32.5</v>
+        <v>27.5</v>
       </c>
       <c r="D560" s="24">
         <v>5.5</v>
       </c>
       <c r="E560" s="25">
-        <v>178.75</v>
+        <v>151.25</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11345,16 +11327,16 @@
         <v>566</v>
       </c>
       <c r="B562" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C562" s="23">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D562" s="24">
         <v>5.75</v>
       </c>
       <c r="E562" s="25">
-        <v>109.25</v>
+        <v>103.5</v>
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
@@ -11618,16 +11600,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C579" s="23">
-        <v>54.5</v>
+        <v>49.5</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>150.36000000000001</v>
+        <v>136.57</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11635,16 +11617,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C580" s="23">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D580" s="24">
         <v>2.76</v>
       </c>
       <c r="E580" s="25">
-        <v>146.28</v>
+        <v>121.44</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11686,16 +11668,16 @@
         <v>587</v>
       </c>
       <c r="B583" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C583" s="23">
-        <v>39</v>
+        <v>37.5</v>
       </c>
       <c r="D583" s="24">
         <v>2.88</v>
       </c>
       <c r="E583" s="25">
-        <v>112.43</v>
+        <v>108.11</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
@@ -11786,16 +11768,16 @@
         <v>593</v>
       </c>
       <c r="B589" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C589" s="23">
-        <v>28.5</v>
+        <v>27</v>
       </c>
       <c r="D589" s="24">
         <v>3</v>
       </c>
       <c r="E589" s="25">
-        <v>85.5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -11803,16 +11785,16 @@
         <v>594</v>
       </c>
       <c r="B590" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C590" s="23">
-        <v>25.5</v>
+        <v>23.5</v>
       </c>
       <c r="D590" s="24">
         <v>3.1</v>
       </c>
       <c r="E590" s="25">
-        <v>79.05</v>
+        <v>72.849999999999994</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
@@ -11854,16 +11836,16 @@
         <v>597</v>
       </c>
       <c r="B593" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C593" s="23">
-        <v>4.5</v>
+        <v>-1.5</v>
       </c>
       <c r="D593" s="24">
         <v>4</v>
       </c>
       <c r="E593" s="25">
-        <v>18</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
@@ -11871,16 +11853,16 @@
         <v>598</v>
       </c>
       <c r="B594" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C594" s="23">
-        <v>19.5</v>
+        <v>14.5</v>
       </c>
       <c r="D594" s="24">
         <v>4</v>
       </c>
       <c r="E594" s="25">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
@@ -11920,16 +11902,16 @@
         <v>601</v>
       </c>
       <c r="B597" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C597" s="23">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D597" s="24">
         <v>4.95</v>
       </c>
       <c r="E597" s="25">
-        <v>71.709999999999994</v>
+        <v>61.82</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -11954,16 +11936,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C599" s="23">
-        <v>446.5</v>
+        <v>430.5</v>
       </c>
       <c r="D599" s="24">
         <v>1.91</v>
       </c>
       <c r="E599" s="25">
-        <v>852.84</v>
+        <v>822.28</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -11971,16 +11953,16 @@
         <v>604</v>
       </c>
       <c r="B600" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C600" s="23">
-        <v>128.19999999999999</v>
+        <v>124.2</v>
       </c>
       <c r="D600" s="24">
         <v>1.93</v>
       </c>
       <c r="E600" s="25">
-        <v>247.38</v>
+        <v>239.66</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
@@ -11988,16 +11970,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C601" s="23">
-        <v>189.5</v>
+        <v>180</v>
       </c>
       <c r="D601" s="24">
         <v>2.84</v>
       </c>
       <c r="E601" s="25">
-        <v>538.01</v>
+        <v>511.03</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -12022,16 +12004,16 @@
         <v>607</v>
       </c>
       <c r="B603" s="22">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C603" s="23">
-        <v>50.5</v>
+        <v>44.5</v>
       </c>
       <c r="D603" s="24">
         <v>4.28</v>
       </c>
       <c r="E603" s="25">
-        <v>216.14</v>
+        <v>190.46</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
@@ -12073,16 +12055,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C606" s="23">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>694.7</v>
+        <v>693.3</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12090,16 +12072,16 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C607" s="23">
-        <v>933</v>
+        <v>923.5</v>
       </c>
       <c r="D607" s="24">
         <v>1.4</v>
       </c>
       <c r="E607" s="25">
-        <v>1306.2</v>
+        <v>1292.9000000000001</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12107,16 +12089,16 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C608" s="23">
-        <v>-54</v>
+        <v>-61</v>
       </c>
       <c r="D608" s="24">
         <v>1.4</v>
       </c>
       <c r="E608" s="25">
-        <v>-75.599999999999994</v>
+        <v>-85.4</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12137,10 +12119,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C610" s="23">
-        <v>78.5</v>
+        <v>72</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12150,10 +12132,10 @@
         <v>615</v>
       </c>
       <c r="B611" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C611" s="23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D611" s="27"/>
       <c r="E611" s="26"/>
@@ -12163,10 +12145,10 @@
         <v>616</v>
       </c>
       <c r="B612" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C612" s="23">
-        <v>37.799999999999997</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="D612" s="27"/>
       <c r="E612" s="26"/>
@@ -12215,16 +12197,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C616" s="23">
-        <v>803</v>
+        <v>713</v>
       </c>
       <c r="D616" s="24">
         <v>0.83</v>
       </c>
       <c r="E616" s="25">
-        <v>662.48</v>
+        <v>588.23</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12232,16 +12214,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C617" s="23">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="D617" s="24">
         <v>0.8</v>
       </c>
       <c r="E617" s="25">
-        <v>296.8</v>
+        <v>284.8</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12249,16 +12231,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C618" s="23">
-        <v>585.5</v>
+        <v>581.5</v>
       </c>
       <c r="D618" s="24">
         <v>0.81</v>
       </c>
       <c r="E618" s="25">
-        <v>477.01</v>
+        <v>473.75</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12266,16 +12248,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C619" s="23">
-        <v>248.5</v>
+        <v>233.5</v>
       </c>
       <c r="D619" s="24">
         <v>0.81</v>
       </c>
       <c r="E619" s="25">
-        <v>200.57</v>
+        <v>188.47</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12300,16 +12282,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="C621" s="23">
-        <v>1654.5</v>
+        <v>1583</v>
       </c>
       <c r="D621" s="24">
         <v>0.52</v>
       </c>
       <c r="E621" s="25">
-        <v>860.34</v>
+        <v>823.16</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12317,16 +12299,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C622" s="23">
-        <v>1551</v>
+        <v>1547</v>
       </c>
       <c r="D622" s="24">
         <v>0.51</v>
       </c>
       <c r="E622" s="25">
-        <v>790.06</v>
+        <v>788.03</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12334,16 +12316,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="C623" s="23">
-        <v>993</v>
+        <v>912.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.52</v>
       </c>
       <c r="E623" s="25">
-        <v>516.36</v>
+        <v>474.5</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12351,16 +12333,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C624" s="23">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D624" s="24">
         <v>0.5</v>
       </c>
       <c r="E624" s="25">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12368,16 +12350,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C625" s="23">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="D625" s="24">
         <v>0.52</v>
       </c>
       <c r="E625" s="25">
-        <v>212.16</v>
+        <v>207.48</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12385,16 +12367,16 @@
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C626" s="23">
-        <v>670.5</v>
+        <v>628.5</v>
       </c>
       <c r="D626" s="24">
         <v>0.7</v>
       </c>
       <c r="E626" s="25">
-        <v>469.35</v>
+        <v>439.95</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12402,16 +12384,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C627" s="23">
-        <v>424.5</v>
+        <v>406.5</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>297.14999999999998</v>
+        <v>284.55</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12419,16 +12401,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C628" s="23">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="D628" s="24">
         <v>0.69</v>
       </c>
       <c r="E628" s="25">
-        <v>160.32</v>
+        <v>139.77000000000001</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12460,16 +12442,16 @@
         <v>635</v>
       </c>
       <c r="B631" s="22">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C631" s="23">
-        <v>1123.5</v>
+        <v>1112.5</v>
       </c>
       <c r="D631" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E631" s="25">
-        <v>618.24</v>
+        <v>612.19000000000005</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -12542,11 +12524,11 @@
       </c>
       <c r="B636" s="29"/>
       <c r="C636" s="30">
-        <v>60112.62</v>
+        <v>56799.12</v>
       </c>
       <c r="D636" s="31"/>
       <c r="E636" s="32">
-        <v>116753.36</v>
+        <v>109456.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 1130
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="642">
   <si>
     <t>StkSummary</t>
   </si>
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 24-Mar-2025</t>
+    <t>1-Jul-2024 to 25-Mar-2025</t>
   </si>
   <si>
     <t/>
@@ -929,7 +929,7 @@
     <t>5892 PATRIKA</t>
   </si>
   <si>
-    <t>5893 PATRIKA {M}</t>
+    <t>5893 PATRIKA {M} 1600</t>
   </si>
   <si>
     <t>5894 PATRIKA (DC)</t>
@@ -1391,7 +1391,7 @@
     <t>7295 PATRIKA</t>
   </si>
   <si>
-    <t>7296 PATRIKA {F}</t>
+    <t>7296 PATRIKA {F} (DC)</t>
   </si>
   <si>
     <t>7297 PATRIKA {F/G}</t>
@@ -1505,7 +1505,7 @@
     <t>7335 PATRIKA (Dc)</t>
   </si>
   <si>
-    <t>7337 PATRIKA AGYA</t>
+    <t>7337 PATRIKA</t>
   </si>
   <si>
     <t>7338 PATRIKA (DC)</t>
@@ -1763,7 +1763,7 @@
     <t>9069 CARD</t>
   </si>
   <si>
-    <t>9070 CARD</t>
+    <t>9070 CARD (Dc)</t>
   </si>
   <si>
     <t>9071 CARD</t>
@@ -1944,6 +1944,9 @@
   </si>
   <si>
     <t>GIFT ENVELOPE 143</t>
+  </si>
+  <si>
+    <t>POSTER</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -2464,7 +2467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E636"/>
+  <dimension ref="A1:E637"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2572,16 +2575,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="23">
-        <v>619.5</v>
+        <v>613.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>619.5</v>
+        <v>613.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2589,16 +2592,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="23">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D10" s="24">
         <v>1</v>
       </c>
       <c r="E10" s="25">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2606,16 +2609,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C11" s="23">
-        <v>479.5</v>
+        <v>472.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>435.34</v>
+        <v>428.98</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,16 +2626,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C12" s="23">
-        <v>138.5</v>
+        <v>126</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>228.53</v>
+        <v>207.9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2657,16 +2660,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="23">
-        <v>19.5</v>
+        <v>18.5</v>
       </c>
       <c r="D14" s="24">
         <v>1.8</v>
       </c>
       <c r="E14" s="25">
-        <v>35.1</v>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2674,16 +2677,16 @@
         <v>19</v>
       </c>
       <c r="B15" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C15" s="23">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="D15" s="24">
         <v>1.8</v>
       </c>
       <c r="E15" s="25">
-        <v>47.7</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2725,16 +2728,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="23">
-        <v>47.5</v>
+        <v>41.5</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2742,16 +2745,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C19" s="23">
-        <v>76.5</v>
+        <v>62.5</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2776,16 +2779,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C21" s="23">
-        <v>60</v>
+        <v>58.5</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
       </c>
       <c r="E21" s="25">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,16 +2813,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C23" s="23">
-        <v>80.25</v>
+        <v>69.25</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>160.5</v>
+        <v>138.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,16 +2830,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C24" s="23">
-        <v>51.5</v>
+        <v>41.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>108.15</v>
+        <v>87.15</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,16 +2867,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C27" s="23">
-        <v>37.5</v>
+        <v>19.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>88.13</v>
+        <v>45.83</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2881,16 +2884,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C28" s="23">
-        <v>73.5</v>
+        <v>69</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>172.73</v>
+        <v>162.15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,16 +2901,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C29" s="23">
-        <v>32.5</v>
+        <v>29.5</v>
       </c>
       <c r="D29" s="24">
         <v>2.57</v>
       </c>
       <c r="E29" s="25">
-        <v>83.42</v>
+        <v>75.72</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2941,16 +2944,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="23">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="D32" s="24">
         <v>2.5</v>
       </c>
       <c r="E32" s="25">
-        <v>58.75</v>
+        <v>56.25</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3015,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" s="23">
-        <v>107.5</v>
+        <v>104.5</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>279.5</v>
+        <v>271.7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,13 +3035,13 @@
         <v>69</v>
       </c>
       <c r="C38" s="23">
-        <v>66.5</v>
+        <v>69</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>179.55</v>
+        <v>186.3</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3100,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" s="23">
-        <v>61.5</v>
+        <v>56.5</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>175.28</v>
+        <v>161.03</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3117,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C43" s="23">
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>68.63</v>
+        <v>64.13</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3134,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C44" s="23">
-        <v>41.5</v>
+        <v>38.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>93.38</v>
+        <v>86.63</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,16 +3168,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C46" s="23">
-        <v>97.5</v>
+        <v>96.5</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>229.13</v>
+        <v>226.78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,16 +3185,16 @@
         <v>51</v>
       </c>
       <c r="B47" s="22">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C47" s="23">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D47" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E47" s="25">
-        <v>25.3</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,16 +3202,16 @@
         <v>52</v>
       </c>
       <c r="B48" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C48" s="23">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D48" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E48" s="25">
-        <v>200.2</v>
+        <v>189.2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,16 +3219,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="C49" s="23">
-        <v>972.5</v>
+        <v>929.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>1083.54</v>
+        <v>1035.6300000000001</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,16 +3236,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C50" s="23">
-        <v>823.5</v>
+        <v>813.5</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>920.26</v>
+        <v>909.09</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3250,16 +3253,16 @@
         <v>55</v>
       </c>
       <c r="B51" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" s="23">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D51" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E51" s="25">
-        <v>61.6</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,16 +3270,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C52" s="23">
-        <v>534.5</v>
+        <v>512.5</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>597.21</v>
+        <v>572.63</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3284,16 +3287,16 @@
         <v>57</v>
       </c>
       <c r="B53" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C53" s="23">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="D53" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E53" s="25">
-        <v>209.75</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3304,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C54" s="23">
-        <v>1029.5</v>
+        <v>1009.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>1150.76</v>
+        <v>1128.4100000000001</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3335,16 +3338,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="22">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C56" s="23">
-        <v>154.5</v>
+        <v>140</v>
       </c>
       <c r="D56" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E56" s="25">
-        <v>169.95</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3355,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C57" s="23">
-        <v>332</v>
+        <v>319.5</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>630.79999999999995</v>
+        <v>607.04999999999995</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,16 +3404,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C60" s="23">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>703</v>
+        <v>685.9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,16 +3421,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C61" s="23">
-        <v>370.5</v>
+        <v>365.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>778.05</v>
+        <v>767.55</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,16 +3453,16 @@
         <v>67</v>
       </c>
       <c r="B63" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C63" s="23">
-        <v>42.5</v>
+        <v>38.5</v>
       </c>
       <c r="D63" s="24">
         <v>2.1</v>
       </c>
       <c r="E63" s="25">
-        <v>89.25</v>
+        <v>80.849999999999994</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3467,16 +3470,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C64" s="23">
-        <v>142.5</v>
+        <v>128.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>299.25</v>
+        <v>269.85000000000002</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3484,16 +3487,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C65" s="23">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>642.6</v>
+        <v>606.9</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3518,16 +3521,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C67" s="23">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>51.48</v>
+        <v>49.92</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3535,16 +3538,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C68" s="23">
-        <v>181.5</v>
+        <v>141.5</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>127.05</v>
+        <v>99.05</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3552,16 +3555,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C69" s="23">
-        <v>29.5</v>
+        <v>10.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>20.65</v>
+        <v>7.35</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3569,16 +3572,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C70" s="23">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>332.1</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3586,16 +3589,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C71" s="23">
-        <v>217</v>
+        <v>213.5</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>195.3</v>
+        <v>192.15</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3603,16 +3606,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C72" s="23">
-        <v>2044</v>
+        <v>1950</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>3168.2</v>
+        <v>3022.5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3620,16 +3623,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C73" s="23">
-        <v>1445.5</v>
+        <v>1419.5</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>2240.5300000000002</v>
+        <v>2200.23</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3637,16 +3640,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C74" s="23">
-        <v>1152</v>
+        <v>1106</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>1785.6</v>
+        <v>1714.3</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,10 +3698,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C78" s="23">
-        <v>713.5</v>
+        <v>529</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3721,10 +3724,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C80" s="23">
-        <v>-6.5</v>
+        <v>141</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3747,10 +3750,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C82" s="23">
-        <v>241.5</v>
+        <v>379.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3780,13 +3783,13 @@
         <v>92</v>
       </c>
       <c r="C84" s="23">
-        <v>505.5</v>
+        <v>509.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>581.33000000000004</v>
+        <v>585.92999999999995</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3794,16 +3797,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C85" s="23">
-        <v>4021</v>
+        <v>3959</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>5629.4</v>
+        <v>5542.6</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3811,16 +3814,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C86" s="23">
-        <v>2604</v>
+        <v>2578</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3645.6</v>
+        <v>3609.2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3828,16 +3831,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C87" s="23">
-        <v>939.5</v>
+        <v>913</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1315.3</v>
+        <v>1278.2</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3854,16 +3857,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C89" s="23">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>1376</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3871,16 +3874,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C90" s="23">
-        <v>1036</v>
+        <v>1020.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>2072</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3888,16 +3891,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C91" s="23">
-        <v>227</v>
+        <v>214.5</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>286.02</v>
+        <v>270.27</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4000,16 +4003,16 @@
         <v>103</v>
       </c>
       <c r="B99" s="22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C99" s="23">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="D99" s="24">
         <v>1.55</v>
       </c>
       <c r="E99" s="25">
-        <v>302.25</v>
+        <v>224.75</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4017,16 +4020,16 @@
         <v>104</v>
       </c>
       <c r="B100" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C100" s="23">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D100" s="24">
         <v>1.55</v>
       </c>
       <c r="E100" s="25">
-        <v>296.05</v>
+        <v>280.55</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4068,10 +4071,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C103" s="23">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4081,10 +4084,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C104" s="23">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4210,16 +4213,16 @@
         <v>117</v>
       </c>
       <c r="B113" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C113" s="23">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D113" s="24">
         <v>12.5</v>
       </c>
       <c r="E113" s="25">
-        <v>137.5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4227,16 +4230,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C114" s="23">
-        <v>25.5</v>
+        <v>24.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>318.75</v>
+        <v>306.25</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4295,16 +4298,16 @@
         <v>122</v>
       </c>
       <c r="B118" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C118" s="23">
-        <v>25.86</v>
+        <v>23.86</v>
       </c>
       <c r="D118" s="24">
         <v>12.5</v>
       </c>
       <c r="E118" s="25">
-        <v>323.25</v>
+        <v>298.25</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4329,11 +4332,17 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>51</v>
-      </c>
-      <c r="C120" s="26"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="26"/>
+        <v>52</v>
+      </c>
+      <c r="C120" s="23">
+        <v>8.5</v>
+      </c>
+      <c r="D120" s="24">
+        <v>12.5</v>
+      </c>
+      <c r="E120" s="25">
+        <v>106.25</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="21" t="s">
@@ -4343,13 +4352,13 @@
         <v>55</v>
       </c>
       <c r="C121" s="23">
-        <v>-1.5</v>
+        <v>8.5</v>
       </c>
       <c r="D121" s="24">
         <v>12.5</v>
       </c>
       <c r="E121" s="25">
-        <v>-18.75</v>
+        <v>106.25</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4396,16 +4405,16 @@
         <v>129</v>
       </c>
       <c r="B125" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C125" s="23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D125" s="24">
         <v>15.5</v>
       </c>
       <c r="E125" s="25">
-        <v>77.5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4628,16 +4637,16 @@
         <v>143</v>
       </c>
       <c r="B139" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C139" s="23">
-        <v>1.5</v>
+        <v>-5.5</v>
       </c>
       <c r="D139" s="24">
         <v>18.45</v>
       </c>
       <c r="E139" s="25">
-        <v>27.67</v>
+        <v>-101.47</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4645,16 +4654,16 @@
         <v>144</v>
       </c>
       <c r="B140" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C140" s="23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D140" s="24">
         <v>18.34</v>
       </c>
       <c r="E140" s="25">
-        <v>128.38999999999999</v>
+        <v>73.37</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4696,16 +4705,16 @@
         <v>147</v>
       </c>
       <c r="B143" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C143" s="23">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="D143" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E143" s="25">
-        <v>110.64</v>
+        <v>101.42</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4724,16 +4733,16 @@
         <v>149</v>
       </c>
       <c r="B145" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C145" s="23">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D145" s="24">
         <v>18.399999999999999</v>
       </c>
       <c r="E145" s="25">
-        <v>147.16999999999999</v>
+        <v>119.58</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4741,16 +4750,16 @@
         <v>150</v>
       </c>
       <c r="B146" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C146" s="23">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D146" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E146" s="25">
-        <v>165.93</v>
+        <v>36.869999999999997</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4758,16 +4767,16 @@
         <v>151</v>
       </c>
       <c r="B147" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C147" s="23">
-        <v>13.5</v>
+        <v>10.5</v>
       </c>
       <c r="D147" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E147" s="25">
-        <v>248.99</v>
+        <v>193.66</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,17 +4801,11 @@
         <v>153</v>
       </c>
       <c r="B149" s="22">
-        <v>17</v>
-      </c>
-      <c r="C149" s="23">
-        <v>-2.5</v>
-      </c>
-      <c r="D149" s="24">
-        <v>18.41</v>
-      </c>
-      <c r="E149" s="25">
-        <v>-46.02</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C149" s="26"/>
+      <c r="D149" s="27"/>
+      <c r="E149" s="26"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="21" t="s">
@@ -4843,16 +4846,16 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="C152" s="23">
-        <v>29.5</v>
+        <v>18</v>
       </c>
       <c r="D152" s="24">
         <v>2.8</v>
       </c>
       <c r="E152" s="25">
-        <v>82.6</v>
+        <v>50.4</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -4860,16 +4863,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C153" s="23">
-        <v>70.5</v>
+        <v>49</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>193.88</v>
+        <v>134.75</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4911,16 +4914,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C156" s="23">
-        <v>97.25</v>
+        <v>78.75</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>330.65</v>
+        <v>267.75</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4939,16 +4942,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C158" s="23">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>159.30000000000001</v>
+        <v>105.3</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4973,16 +4976,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C160" s="23">
-        <v>80.5</v>
+        <v>79</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>225.4</v>
+        <v>221.2</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4990,16 +4993,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C161" s="23">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>47.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5007,16 +5010,16 @@
         <v>166</v>
       </c>
       <c r="B162" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C162" s="23">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D162" s="24">
         <v>2.8</v>
       </c>
       <c r="E162" s="25">
-        <v>254.8</v>
+        <v>226.8</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -5058,16 +5061,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C165" s="23">
-        <v>190.5</v>
+        <v>170.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>561.98</v>
+        <v>502.98</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5075,16 +5078,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C166" s="23">
-        <v>164.5</v>
+        <v>142.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>485.28</v>
+        <v>420.38</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5092,16 +5095,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C167" s="23">
-        <v>32.5</v>
+        <v>12.5</v>
       </c>
       <c r="D167" s="24">
         <v>3</v>
       </c>
       <c r="E167" s="25">
-        <v>97.5</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5126,16 +5129,16 @@
         <v>173</v>
       </c>
       <c r="B169" s="22">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C169" s="23">
-        <v>37.5</v>
+        <v>40.5</v>
       </c>
       <c r="D169" s="24">
         <v>3.3</v>
       </c>
       <c r="E169" s="25">
-        <v>123.75</v>
+        <v>133.65</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5160,16 +5163,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C171" s="23">
-        <v>154</v>
+        <v>152.5</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>539</v>
+        <v>533.75</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5235,16 +5238,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C176" s="23">
-        <v>18.5</v>
+        <v>12.5</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>61.61</v>
+        <v>41.63</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5323,16 +5326,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C182" s="23">
-        <v>39.5</v>
+        <v>30</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>150.1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5340,16 +5343,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C183" s="23">
-        <v>136.5</v>
+        <v>133.5</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>409.5</v>
+        <v>400.5</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5357,16 +5360,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C184" s="23">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5476,16 +5479,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C191" s="23">
-        <v>151.5</v>
+        <v>144.5</v>
       </c>
       <c r="D191" s="24">
         <v>3.97</v>
       </c>
       <c r="E191" s="25">
-        <v>601.92999999999995</v>
+        <v>574.12</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5510,16 +5513,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C193" s="23">
-        <v>29.5</v>
+        <v>23.5</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>88.5</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5544,16 +5547,16 @@
         <v>199</v>
       </c>
       <c r="B195" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C195" s="23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D195" s="24">
         <v>2.8</v>
       </c>
       <c r="E195" s="25">
-        <v>16.8</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5615,16 +5618,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C200" s="23">
-        <v>126.49</v>
+        <v>114.99</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>388.75</v>
+        <v>353.41</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5658,16 +5661,16 @@
         <v>207</v>
       </c>
       <c r="B203" s="22">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C203" s="23">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D203" s="24">
         <v>3.38</v>
       </c>
       <c r="E203" s="25">
-        <v>168.99</v>
+        <v>172.37</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5719,16 +5722,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C208" s="23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>26.6</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5739,13 +5742,13 @@
         <v>94</v>
       </c>
       <c r="C209" s="23">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>20.9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5792,16 +5795,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C213" s="23">
-        <v>0.5</v>
+        <v>76</v>
       </c>
       <c r="D213" s="24">
-        <v>4.12</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="E213" s="25">
-        <v>2.06</v>
+        <v>312.45</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5809,16 +5812,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C214" s="23">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>444.49</v>
+        <v>358.06</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5877,16 +5880,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C218" s="23">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>312.62</v>
+        <v>303.93</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5916,16 +5919,16 @@
         <v>225</v>
       </c>
       <c r="B221" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C221" s="23">
-        <v>52</v>
+        <v>49.5</v>
       </c>
       <c r="D221" s="24">
         <v>4.5</v>
       </c>
       <c r="E221" s="25">
-        <v>234</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -5933,16 +5936,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C222" s="23">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>135</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5950,16 +5953,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C223" s="23">
-        <v>136</v>
+        <v>134.5</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>612</v>
+        <v>605.25</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5967,16 +5970,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C224" s="23">
-        <v>34</v>
+        <v>28.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>178.5</v>
+        <v>149.63</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6001,16 +6004,16 @@
         <v>230</v>
       </c>
       <c r="B226" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C226" s="23">
-        <v>30.5</v>
+        <v>27.5</v>
       </c>
       <c r="D226" s="24">
         <v>4.8</v>
       </c>
       <c r="E226" s="25">
-        <v>146.4</v>
+        <v>132</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6018,16 +6021,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C227" s="23">
-        <v>25</v>
+        <v>23.5</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>112.5</v>
+        <v>105.75</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6067,16 +6070,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C230" s="23">
-        <v>66.5</v>
+        <v>63.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>349.13</v>
+        <v>333.38</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6087,13 +6090,13 @@
         <v>21</v>
       </c>
       <c r="C231" s="23">
-        <v>94.5</v>
+        <v>85.5</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>496.13</v>
+        <v>448.88</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6157,16 +6160,16 @@
         <v>240</v>
       </c>
       <c r="B236" s="22">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C236" s="23">
-        <v>18</v>
+        <v>4.5</v>
       </c>
       <c r="D236" s="24">
         <v>6</v>
       </c>
       <c r="E236" s="25">
-        <v>108</v>
+        <v>27</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -6218,13 +6221,13 @@
         <v>91</v>
       </c>
       <c r="C240" s="23">
-        <v>67.8</v>
+        <v>70.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>386.46</v>
+        <v>403.56</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6264,16 +6267,16 @@
         <v>247</v>
       </c>
       <c r="B243" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C243" s="23">
-        <v>17.5</v>
+        <v>15.5</v>
       </c>
       <c r="D243" s="24">
         <v>6.75</v>
       </c>
       <c r="E243" s="25">
-        <v>118.13</v>
+        <v>104.63</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6281,16 +6284,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C244" s="23">
-        <v>37.909999999999997</v>
+        <v>40.409999999999997</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>226.78</v>
+        <v>241.73</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6309,16 +6312,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C246" s="23">
-        <v>32.5</v>
+        <v>32</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6394,16 +6397,16 @@
         <v>255</v>
       </c>
       <c r="B251" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C251" s="23">
-        <v>4.5</v>
+        <v>0.5</v>
       </c>
       <c r="D251" s="24">
         <v>3.8</v>
       </c>
       <c r="E251" s="25">
-        <v>17.100000000000001</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6422,16 +6425,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C253" s="23">
-        <v>77.5</v>
+        <v>74.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>271.25</v>
+        <v>260.75</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6439,16 +6442,16 @@
         <v>258</v>
       </c>
       <c r="B254" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C254" s="23">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D254" s="24">
         <v>4.25</v>
       </c>
       <c r="E254" s="25">
-        <v>246.5</v>
+        <v>242.25</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6516,16 +6519,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C259" s="23">
-        <v>160</v>
+        <v>209.5</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>684.8</v>
+        <v>896.66</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6533,16 +6536,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C260" s="23">
-        <v>85.5</v>
+        <v>80.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>365.94</v>
+        <v>344.54</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6584,16 +6587,16 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C263" s="23">
-        <v>44.8</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>221.76</v>
+        <v>164.84</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6702,16 +6705,16 @@
         <v>275</v>
       </c>
       <c r="B271" s="22">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C271" s="23">
-        <v>14.5</v>
+        <v>55.5</v>
       </c>
       <c r="D271" s="24">
         <v>5.4</v>
       </c>
       <c r="E271" s="25">
-        <v>78.3</v>
+        <v>299.7</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6898,16 +6901,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C283" s="23">
-        <v>40.880000000000003</v>
+        <v>33.880000000000003</v>
       </c>
       <c r="D283" s="24">
         <v>5.94</v>
       </c>
       <c r="E283" s="25">
-        <v>242.83</v>
+        <v>201.25</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6932,16 +6935,16 @@
         <v>289</v>
       </c>
       <c r="B285" s="22">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C285" s="23">
-        <v>44</v>
+        <v>40.5</v>
       </c>
       <c r="D285" s="24">
         <v>5.94</v>
       </c>
       <c r="E285" s="25">
-        <v>261.36</v>
+        <v>240.57</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6966,16 +6969,16 @@
         <v>291</v>
       </c>
       <c r="B287" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C287" s="23">
-        <v>26.5</v>
+        <v>21</v>
       </c>
       <c r="D287" s="24">
         <v>6.8</v>
       </c>
       <c r="E287" s="25">
-        <v>180.17</v>
+        <v>142.77000000000001</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -7035,16 +7038,16 @@
         <v>296</v>
       </c>
       <c r="B292" s="22">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C292" s="23">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D292" s="24">
         <v>6.18</v>
       </c>
       <c r="E292" s="25">
-        <v>407.88</v>
+        <v>426.42</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -7117,13 +7120,13 @@
         <v>26</v>
       </c>
       <c r="C297" s="23">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="D297" s="24">
         <v>6.4</v>
       </c>
       <c r="E297" s="25">
-        <v>-32</v>
+        <v>-64</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -7143,13 +7146,13 @@
         <v>44</v>
       </c>
       <c r="C299" s="23">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="D299" s="24">
         <v>6.65</v>
       </c>
       <c r="E299" s="25">
-        <v>352.45</v>
+        <v>525.35</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -7200,16 +7203,16 @@
         <v>307</v>
       </c>
       <c r="B303" s="22">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C303" s="23">
-        <v>72.5</v>
+        <v>67.5</v>
       </c>
       <c r="D303" s="24">
         <v>7.13</v>
       </c>
       <c r="E303" s="25">
-        <v>516.92999999999995</v>
+        <v>481.28</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -7217,16 +7220,16 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C304" s="23">
-        <v>57.4</v>
+        <v>48.9</v>
       </c>
       <c r="D304" s="24">
         <v>7.13</v>
       </c>
       <c r="E304" s="25">
-        <v>409.26</v>
+        <v>348.66</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7277,16 +7280,16 @@
         <v>312</v>
       </c>
       <c r="B308" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C308" s="23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D308" s="24">
         <v>7.6</v>
       </c>
       <c r="E308" s="25">
-        <v>121.6</v>
+        <v>106.4</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -7482,13 +7485,13 @@
         <v>53</v>
       </c>
       <c r="C322" s="23">
-        <v>33.200000000000003</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="D322" s="24">
         <v>8.8000000000000007</v>
       </c>
       <c r="E322" s="25">
-        <v>292.16000000000003</v>
+        <v>300.95999999999998</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -7581,16 +7584,16 @@
         <v>332</v>
       </c>
       <c r="B328" s="22">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C328" s="23">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="D328" s="24">
         <v>9.25</v>
       </c>
       <c r="E328" s="25">
-        <v>55.5</v>
+        <v>-9.25</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -7649,16 +7652,16 @@
         <v>336</v>
       </c>
       <c r="B332" s="22">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C332" s="23">
-        <v>55</v>
+        <v>51.5</v>
       </c>
       <c r="D332" s="24">
         <v>5.5</v>
       </c>
       <c r="E332" s="25">
-        <v>302.5</v>
+        <v>283.25</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7666,16 +7669,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C333" s="23">
-        <v>11</v>
+        <v>8.5</v>
       </c>
       <c r="D333" s="24">
         <v>6.89</v>
       </c>
       <c r="E333" s="25">
-        <v>75.790000000000006</v>
+        <v>58.57</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7683,16 +7686,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C334" s="23">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D334" s="24">
         <v>6.9</v>
       </c>
       <c r="E334" s="25">
-        <v>124.2</v>
+        <v>117.3</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7734,16 +7737,16 @@
         <v>341</v>
       </c>
       <c r="B337" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C337" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D337" s="24">
         <v>8.5</v>
       </c>
       <c r="E337" s="25">
-        <v>34</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -7833,16 +7836,16 @@
         <v>348</v>
       </c>
       <c r="B344" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C344" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D344" s="24">
         <v>6.51</v>
       </c>
       <c r="E344" s="25">
-        <v>65.099999999999994</v>
+        <v>58.59</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
@@ -7895,16 +7898,16 @@
         <v>352</v>
       </c>
       <c r="B348" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C348" s="23">
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="D348" s="24">
         <v>7.36</v>
       </c>
       <c r="E348" s="25">
-        <v>158.24</v>
+        <v>143.52000000000001</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -7980,16 +7983,16 @@
         <v>357</v>
       </c>
       <c r="B353" s="22">
+        <v>7</v>
+      </c>
+      <c r="C353" s="23">
         <v>6</v>
-      </c>
-      <c r="C353" s="23">
-        <v>8</v>
       </c>
       <c r="D353" s="24">
         <v>16</v>
       </c>
       <c r="E353" s="25">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -8025,16 +8028,16 @@
         <v>360</v>
       </c>
       <c r="B356" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C356" s="23">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D356" s="24">
         <v>16.25</v>
       </c>
       <c r="E356" s="25">
-        <v>73.13</v>
+        <v>56.88</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -8144,16 +8147,16 @@
         <v>367</v>
       </c>
       <c r="B363" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C363" s="23">
-        <v>15.99</v>
+        <v>13.99</v>
       </c>
       <c r="D363" s="24">
         <v>12</v>
       </c>
       <c r="E363" s="25">
-        <v>191.88</v>
+        <v>167.88</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -8181,13 +8184,13 @@
         <v>46</v>
       </c>
       <c r="C365" s="23">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D365" s="24">
         <v>7.84</v>
       </c>
       <c r="E365" s="25">
-        <v>3.92</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -8198,13 +8201,13 @@
         <v>16</v>
       </c>
       <c r="C366" s="23">
-        <v>-4</v>
+        <v>6</v>
       </c>
       <c r="D366" s="24">
         <v>11</v>
       </c>
       <c r="E366" s="25">
-        <v>-44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -8365,17 +8368,11 @@
         <v>380</v>
       </c>
       <c r="B376" s="22">
-        <v>10</v>
-      </c>
-      <c r="C376" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D376" s="24">
-        <v>10.5</v>
-      </c>
-      <c r="E376" s="25">
-        <v>15.75</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C376" s="26"/>
+      <c r="D376" s="27"/>
+      <c r="E376" s="26"/>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" s="21" t="s">
@@ -8399,16 +8396,16 @@
         <v>382</v>
       </c>
       <c r="B378" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C378" s="23">
-        <v>3.8</v>
+        <v>1.8</v>
       </c>
       <c r="D378" s="24">
         <v>15</v>
       </c>
       <c r="E378" s="25">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
@@ -8631,16 +8628,16 @@
         <v>396</v>
       </c>
       <c r="B392" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C392" s="23">
-        <v>8.5</v>
+        <v>3.5</v>
       </c>
       <c r="D392" s="24">
         <v>11.4</v>
       </c>
       <c r="E392" s="25">
-        <v>96.9</v>
+        <v>39.9</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
@@ -8939,16 +8936,16 @@
         <v>416</v>
       </c>
       <c r="B412" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C412" s="23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D412" s="24">
         <v>2.5</v>
       </c>
       <c r="E412" s="25">
-        <v>27.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -8990,16 +8987,16 @@
         <v>419</v>
       </c>
       <c r="B415" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C415" s="23">
-        <v>21.5</v>
+        <v>19.5</v>
       </c>
       <c r="D415" s="24">
         <v>2.25</v>
       </c>
       <c r="E415" s="25">
-        <v>48.38</v>
+        <v>43.88</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
@@ -9075,16 +9072,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C420" s="23">
-        <v>52.5</v>
+        <v>51.5</v>
       </c>
       <c r="D420" s="24">
         <v>2.6</v>
       </c>
       <c r="E420" s="25">
-        <v>136.5</v>
+        <v>133.9</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9092,16 +9089,16 @@
         <v>425</v>
       </c>
       <c r="B421" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C421" s="23">
-        <v>64</v>
+        <v>61.5</v>
       </c>
       <c r="D421" s="24">
         <v>2.75</v>
       </c>
       <c r="E421" s="25">
-        <v>176</v>
+        <v>169.13</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
@@ -9109,16 +9106,16 @@
         <v>426</v>
       </c>
       <c r="B422" s="22">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C422" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D422" s="24">
         <v>2.75</v>
       </c>
       <c r="E422" s="25">
-        <v>8.25</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -9163,13 +9160,13 @@
         <v>42</v>
       </c>
       <c r="C425" s="23">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>9.8000000000000007</v>
+        <v>7</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9186,16 +9183,16 @@
         <v>431</v>
       </c>
       <c r="B427" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C427" s="23">
-        <v>151.84</v>
+        <v>150.34</v>
       </c>
       <c r="D427" s="24">
         <v>2.8</v>
       </c>
       <c r="E427" s="25">
-        <v>425.15</v>
+        <v>420.95</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -9322,16 +9319,16 @@
         <v>439</v>
       </c>
       <c r="B435" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C435" s="23">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D435" s="24">
         <v>3.25</v>
       </c>
       <c r="E435" s="25">
-        <v>65</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
@@ -9365,16 +9362,16 @@
         <v>442</v>
       </c>
       <c r="B438" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C438" s="23">
-        <v>42</v>
+        <v>39.5</v>
       </c>
       <c r="D438" s="24">
         <v>3.25</v>
       </c>
       <c r="E438" s="25">
-        <v>136.5</v>
+        <v>128.38</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -9482,16 +9479,16 @@
         <v>449</v>
       </c>
       <c r="B445" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C445" s="23">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D445" s="24">
         <v>3.33</v>
       </c>
       <c r="E445" s="25">
-        <v>183.15</v>
+        <v>179.82</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -9568,16 +9565,16 @@
         <v>455</v>
       </c>
       <c r="B451" s="22">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C451" s="23">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D451" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E451" s="25">
-        <v>70.56</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
@@ -9687,16 +9684,16 @@
         <v>462</v>
       </c>
       <c r="B458" s="22">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C458" s="23">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D458" s="24">
         <v>4.75</v>
       </c>
       <c r="E458" s="25">
-        <v>142.5</v>
+        <v>152</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -9926,13 +9923,13 @@
         <v>25</v>
       </c>
       <c r="C474" s="23">
-        <v>16</v>
+        <v>36.5</v>
       </c>
       <c r="D474" s="24">
         <v>7.51</v>
       </c>
       <c r="E474" s="25">
-        <v>120.14</v>
+        <v>274</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
@@ -9974,16 +9971,16 @@
         <v>481</v>
       </c>
       <c r="B477" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C477" s="23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D477" s="24">
         <v>7</v>
       </c>
       <c r="E477" s="25">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
@@ -9991,16 +9988,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C478" s="23">
-        <v>22</v>
+        <v>25.5</v>
       </c>
       <c r="D478" s="24">
         <v>7.6</v>
       </c>
       <c r="E478" s="25">
-        <v>167.2</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -10090,16 +10087,16 @@
         <v>489</v>
       </c>
       <c r="B485" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C485" s="23">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="D485" s="24">
         <v>4.28</v>
       </c>
       <c r="E485" s="25">
-        <v>53.5</v>
+        <v>49.22</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
@@ -10107,16 +10104,16 @@
         <v>490</v>
       </c>
       <c r="B486" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C486" s="23">
-        <v>11</v>
+        <v>25.5</v>
       </c>
       <c r="D486" s="24">
         <v>9.5</v>
       </c>
       <c r="E486" s="25">
-        <v>104.5</v>
+        <v>242.25</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -10159,13 +10156,13 @@
         <v>43</v>
       </c>
       <c r="C489" s="23">
-        <v>0.5</v>
+        <v>30.5</v>
       </c>
       <c r="D489" s="24">
         <v>5.7</v>
       </c>
       <c r="E489" s="25">
-        <v>2.85</v>
+        <v>173.85</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.25">
@@ -10207,16 +10204,16 @@
         <v>496</v>
       </c>
       <c r="B492" s="22">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C492" s="23">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D492" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E492" s="25">
-        <v>248.6</v>
+        <v>240.9</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
@@ -10224,16 +10221,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C493" s="23">
-        <v>61.5</v>
+        <v>51.5</v>
       </c>
       <c r="D493" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E493" s="25">
-        <v>67.650000000000006</v>
+        <v>56.65</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10258,16 +10255,16 @@
         <v>499</v>
       </c>
       <c r="B495" s="22">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C495" s="23">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D495" s="24">
         <v>1.4</v>
       </c>
       <c r="E495" s="25">
-        <v>207.2</v>
+        <v>186.2</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10275,16 +10272,16 @@
         <v>500</v>
       </c>
       <c r="B496" s="22">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C496" s="23">
-        <v>320.5</v>
+        <v>310.5</v>
       </c>
       <c r="D496" s="24">
         <v>1.4</v>
       </c>
       <c r="E496" s="25">
-        <v>448.7</v>
+        <v>434.7</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -10292,16 +10289,16 @@
         <v>501</v>
       </c>
       <c r="B497" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C497" s="23">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="D497" s="24">
         <v>1.4</v>
       </c>
       <c r="E497" s="25">
-        <v>445.2</v>
+        <v>431.2</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
@@ -10354,16 +10351,16 @@
         <v>505</v>
       </c>
       <c r="B501" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C501" s="23">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D501" s="24">
         <v>1.55</v>
       </c>
       <c r="E501" s="25">
-        <v>401.45</v>
+        <v>385.95</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
@@ -10422,16 +10419,16 @@
         <v>509</v>
       </c>
       <c r="B505" s="22">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C505" s="23">
-        <v>615.75</v>
+        <v>610.75</v>
       </c>
       <c r="D505" s="24">
         <v>1.5</v>
       </c>
       <c r="E505" s="25">
-        <v>923.63</v>
+        <v>916.13</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -10507,16 +10504,16 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C510" s="23">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D510" s="24">
         <v>0.92</v>
       </c>
       <c r="E510" s="25">
-        <v>79.48</v>
+        <v>83.17</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10524,16 +10521,16 @@
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C511" s="23">
-        <v>129.19999999999999</v>
+        <v>126.7</v>
       </c>
       <c r="D511" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E511" s="25">
-        <v>294.58</v>
+        <v>288.88</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10541,16 +10538,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C512" s="23">
-        <v>166.5</v>
+        <v>161.5</v>
       </c>
       <c r="D512" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E512" s="25">
-        <v>379.62</v>
+        <v>368.22</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10618,16 +10615,16 @@
         <v>521</v>
       </c>
       <c r="B517" s="22">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C517" s="23">
-        <v>69.5</v>
+        <v>66.5</v>
       </c>
       <c r="D517" s="24">
         <v>2.8</v>
       </c>
       <c r="E517" s="25">
-        <v>194.6</v>
+        <v>186.2</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -10744,16 +10741,16 @@
         <v>529</v>
       </c>
       <c r="B525" s="22">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C525" s="23">
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="D525" s="24">
         <v>2.85</v>
       </c>
       <c r="E525" s="25">
-        <v>86.93</v>
+        <v>89.78</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
@@ -10761,16 +10758,16 @@
         <v>530</v>
       </c>
       <c r="B526" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C526" s="23">
-        <v>41</v>
+        <v>39.5</v>
       </c>
       <c r="D526" s="24">
         <v>3.25</v>
       </c>
       <c r="E526" s="25">
-        <v>133.25</v>
+        <v>128.38</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10824,16 +10821,16 @@
         <v>535</v>
       </c>
       <c r="B531" s="22">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C531" s="23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D531" s="24">
         <v>3.5</v>
       </c>
       <c r="E531" s="25">
-        <v>24.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.25">
@@ -11004,16 +11001,16 @@
         <v>547</v>
       </c>
       <c r="B543" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C543" s="23">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D543" s="24">
         <v>4</v>
       </c>
       <c r="E543" s="25">
-        <v>40</v>
+        <v>4</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -11072,16 +11069,16 @@
         <v>551</v>
       </c>
       <c r="B547" s="22">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C547" s="23">
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="D547" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E547" s="25">
-        <v>107.8</v>
+        <v>112.2</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
@@ -11106,16 +11103,16 @@
         <v>553</v>
       </c>
       <c r="B549" s="22">
+        <v>18</v>
+      </c>
+      <c r="C549" s="23">
         <v>19</v>
-      </c>
-      <c r="C549" s="23">
-        <v>18</v>
       </c>
       <c r="D549" s="24">
         <v>4.91</v>
       </c>
       <c r="E549" s="25">
-        <v>88.31</v>
+        <v>93.21</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -11123,16 +11120,16 @@
         <v>554</v>
       </c>
       <c r="B550" s="22">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C550" s="23">
-        <v>2.5</v>
+        <v>10.5</v>
       </c>
       <c r="D550" s="24">
         <v>4.75</v>
       </c>
       <c r="E550" s="25">
-        <v>11.88</v>
+        <v>49.88</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -11157,16 +11154,16 @@
         <v>556</v>
       </c>
       <c r="B552" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C552" s="23">
-        <v>31.5</v>
+        <v>30</v>
       </c>
       <c r="D552" s="24">
         <v>4.75</v>
       </c>
       <c r="E552" s="25">
-        <v>149.63</v>
+        <v>142.5</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11211,13 +11208,13 @@
         <v>67</v>
       </c>
       <c r="C555" s="23">
-        <v>13.62</v>
+        <v>39.619999999999997</v>
       </c>
       <c r="D555" s="24">
         <v>5</v>
       </c>
       <c r="E555" s="25">
-        <v>68.099999999999994</v>
+        <v>198.1</v>
       </c>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.25">
@@ -11296,13 +11293,13 @@
         <v>65</v>
       </c>
       <c r="C560" s="23">
-        <v>27.5</v>
+        <v>28</v>
       </c>
       <c r="D560" s="24">
         <v>5.5</v>
       </c>
       <c r="E560" s="25">
-        <v>151.25</v>
+        <v>154</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11327,16 +11324,16 @@
         <v>566</v>
       </c>
       <c r="B562" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C562" s="23">
-        <v>18</v>
+        <v>14.5</v>
       </c>
       <c r="D562" s="24">
         <v>5.75</v>
       </c>
       <c r="E562" s="25">
-        <v>103.5</v>
+        <v>83.38</v>
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
@@ -11378,16 +11375,16 @@
         <v>569</v>
       </c>
       <c r="B565" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C565" s="23">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D565" s="24">
         <v>5.75</v>
       </c>
       <c r="E565" s="25">
-        <v>40.25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
@@ -11540,17 +11537,11 @@
         <v>579</v>
       </c>
       <c r="B575" s="22">
-        <v>24</v>
-      </c>
-      <c r="C575" s="23">
-        <v>3</v>
-      </c>
-      <c r="D575" s="24">
-        <v>10</v>
-      </c>
-      <c r="E575" s="25">
-        <v>30</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C575" s="26"/>
+      <c r="D575" s="27"/>
+      <c r="E575" s="26"/>
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A576" s="21" t="s">
@@ -11600,16 +11591,16 @@
         <v>583</v>
       </c>
       <c r="B579" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C579" s="23">
-        <v>49.5</v>
+        <v>48</v>
       </c>
       <c r="D579" s="24">
         <v>2.76</v>
       </c>
       <c r="E579" s="25">
-        <v>136.57</v>
+        <v>132.43</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -11634,16 +11625,16 @@
         <v>585</v>
       </c>
       <c r="B581" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C581" s="23">
-        <v>46.74</v>
+        <v>44.24</v>
       </c>
       <c r="D581" s="24">
         <v>2.76</v>
       </c>
       <c r="E581" s="25">
-        <v>129</v>
+        <v>122.1</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
@@ -11685,16 +11676,16 @@
         <v>588</v>
       </c>
       <c r="B584" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C584" s="23">
-        <v>40.5</v>
+        <v>30.5</v>
       </c>
       <c r="D584" s="24">
         <v>2.76</v>
       </c>
       <c r="E584" s="25">
-        <v>111.78</v>
+        <v>84.18</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11702,16 +11693,16 @@
         <v>589</v>
       </c>
       <c r="B585" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C585" s="23">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D585" s="24">
         <v>2.76</v>
       </c>
       <c r="E585" s="25">
-        <v>57.96</v>
+        <v>30.36</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
@@ -11719,16 +11710,16 @@
         <v>590</v>
       </c>
       <c r="B586" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C586" s="23">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D586" s="24">
         <v>2.76</v>
       </c>
       <c r="E586" s="25">
-        <v>173.88</v>
+        <v>168.36</v>
       </c>
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
@@ -11836,16 +11827,16 @@
         <v>597</v>
       </c>
       <c r="B593" s="22">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C593" s="23">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="D593" s="24">
         <v>4</v>
       </c>
       <c r="E593" s="25">
-        <v>-6</v>
+        <v>6</v>
       </c>
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
@@ -11953,16 +11944,16 @@
         <v>604</v>
       </c>
       <c r="B600" s="22">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C600" s="23">
-        <v>124.2</v>
+        <v>117.7</v>
       </c>
       <c r="D600" s="24">
         <v>1.93</v>
       </c>
       <c r="E600" s="25">
-        <v>239.66</v>
+        <v>227.12</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
@@ -11970,16 +11961,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C601" s="23">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D601" s="24">
         <v>2.84</v>
       </c>
       <c r="E601" s="25">
-        <v>511.03</v>
+        <v>451.41</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -11987,16 +11978,16 @@
         <v>606</v>
       </c>
       <c r="B602" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C602" s="23">
-        <v>33.5</v>
+        <v>31.5</v>
       </c>
       <c r="D602" s="24">
         <v>4.28</v>
       </c>
       <c r="E602" s="25">
-        <v>143.38</v>
+        <v>134.82</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12004,16 +11995,16 @@
         <v>607</v>
       </c>
       <c r="B603" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C603" s="23">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D603" s="24">
         <v>4.28</v>
       </c>
       <c r="E603" s="25">
-        <v>190.46</v>
+        <v>181.9</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
@@ -12055,16 +12046,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C606" s="23">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>693.3</v>
+        <v>687.71</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12072,16 +12063,16 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C607" s="23">
-        <v>923.5</v>
+        <v>924.5</v>
       </c>
       <c r="D607" s="24">
         <v>1.4</v>
       </c>
       <c r="E607" s="25">
-        <v>1292.9000000000001</v>
+        <v>1294.3</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12089,16 +12080,16 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C608" s="23">
-        <v>-61</v>
+        <v>-62</v>
       </c>
       <c r="D608" s="24">
         <v>1.4</v>
       </c>
       <c r="E608" s="25">
-        <v>-85.4</v>
+        <v>-86.8</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12106,10 +12097,10 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C609" s="23">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D609" s="27"/>
       <c r="E609" s="26"/>
@@ -12119,10 +12110,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C610" s="23">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12132,10 +12123,10 @@
         <v>615</v>
       </c>
       <c r="B611" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C611" s="23">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="D611" s="27"/>
       <c r="E611" s="26"/>
@@ -12145,10 +12136,10 @@
         <v>616</v>
       </c>
       <c r="B612" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C612" s="23">
-        <v>36.799999999999997</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="D612" s="27"/>
       <c r="E612" s="26"/>
@@ -12158,10 +12149,10 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C613" s="23">
-        <v>735</v>
+        <v>720</v>
       </c>
       <c r="D613" s="27"/>
       <c r="E613" s="26"/>
@@ -12171,10 +12162,10 @@
         <v>618</v>
       </c>
       <c r="B614" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C614" s="23">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D614" s="27"/>
       <c r="E614" s="26"/>
@@ -12197,16 +12188,16 @@
         <v>620</v>
       </c>
       <c r="B616" s="22">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C616" s="23">
-        <v>713</v>
+        <v>700</v>
       </c>
       <c r="D616" s="24">
         <v>0.83</v>
       </c>
       <c r="E616" s="25">
-        <v>588.23</v>
+        <v>577.5</v>
       </c>
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
@@ -12214,16 +12205,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C617" s="23">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="D617" s="24">
         <v>0.8</v>
       </c>
       <c r="E617" s="25">
-        <v>284.8</v>
+        <v>272.8</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12231,16 +12222,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C618" s="23">
-        <v>581.5</v>
+        <v>580.5</v>
       </c>
       <c r="D618" s="24">
         <v>0.81</v>
       </c>
       <c r="E618" s="25">
-        <v>473.75</v>
+        <v>472.93</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12316,16 +12307,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="C623" s="23">
-        <v>912.5</v>
+        <v>877.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.52</v>
       </c>
       <c r="E623" s="25">
-        <v>474.5</v>
+        <v>456.3</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12333,16 +12324,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C624" s="23">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="D624" s="24">
         <v>0.5</v>
       </c>
       <c r="E624" s="25">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12350,16 +12341,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C625" s="23">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="D625" s="24">
         <v>0.52</v>
       </c>
       <c r="E625" s="25">
-        <v>207.48</v>
+        <v>197.08</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12367,16 +12358,16 @@
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C626" s="23">
-        <v>628.5</v>
+        <v>622.5</v>
       </c>
       <c r="D626" s="24">
         <v>0.7</v>
       </c>
       <c r="E626" s="25">
-        <v>439.95</v>
+        <v>435.75</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12384,16 +12375,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C627" s="23">
-        <v>406.5</v>
+        <v>392.5</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>284.55</v>
+        <v>274.75</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12442,16 +12433,16 @@
         <v>635</v>
       </c>
       <c r="B631" s="22">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C631" s="23">
-        <v>1112.5</v>
+        <v>1102.5</v>
       </c>
       <c r="D631" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E631" s="25">
-        <v>612.19000000000005</v>
+        <v>606.67999999999995</v>
       </c>
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
@@ -12519,16 +12510,29 @@
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A636" s="28" t="s">
+      <c r="A636" s="21" t="s">
         <v>640</v>
       </c>
-      <c r="B636" s="29"/>
-      <c r="C636" s="30">
-        <v>56799.12</v>
-      </c>
-      <c r="D636" s="31"/>
-      <c r="E636" s="32">
-        <v>109456.07</v>
+      <c r="B636" s="22">
+        <v>1</v>
+      </c>
+      <c r="C636" s="23">
+        <v>-10</v>
+      </c>
+      <c r="D636" s="27"/>
+      <c r="E636" s="26"/>
+    </row>
+    <row r="637" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A637" s="28" t="s">
+        <v>641</v>
+      </c>
+      <c r="B637" s="29"/>
+      <c r="C637" s="30">
+        <v>55634.62</v>
+      </c>
+      <c r="D637" s="31"/>
+      <c r="E637" s="32">
+        <v>107494.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:48
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -89,7 +89,7 @@
     <t>1854 PATRIKA</t>
   </si>
   <si>
-    <t>1855 PATRIKA (8000)</t>
+    <t>1855 PATRIKA</t>
   </si>
   <si>
     <t>1856 PATRIKA</t>
@@ -110,10 +110,10 @@
     <t>1861 PATRIKA</t>
   </si>
   <si>
-    <t>1862 PATRIKA (8k)</t>
-  </si>
-  <si>
-    <t>1863 PATRIKA (AGYA)</t>
+    <t>1862 PATRIKA</t>
+  </si>
+  <si>
+    <t>1863 PATRIKA</t>
   </si>
   <si>
     <t>1864 PATRIKA (DC)</t>
@@ -128,7 +128,7 @@
     <t>1867 PATRIKA</t>
   </si>
   <si>
-    <t>1868 PATRIKA (3k AGYA)</t>
+    <t>1868 PATRIKA</t>
   </si>
   <si>
     <t>1869 PATRIKA (DC)</t>
@@ -512,7 +512,7 @@
     <t>4207 PATRIKA (DC)  {{10}}</t>
   </si>
   <si>
-    <t>4208 PATRIKA (AGYA)</t>
+    <t>4208 PATRIKA</t>
   </si>
   <si>
     <t>4209 PATRIKA (STK LT N.)</t>
@@ -521,7 +521,7 @@
     <t>4210 PATRIKA</t>
   </si>
   <si>
-    <t>4211 PATRIKA (AGYA)</t>
+    <t>4211 PATRIKA</t>
   </si>
   <si>
     <t>4212 PATRIKA</t>
@@ -569,7 +569,7 @@
     <t>4225 PATRIKA (Design Change)</t>
   </si>
   <si>
-    <t>4226 PATRIKA (3k  AGYA)</t>
+    <t>4226 PATRIKA</t>
   </si>
   <si>
     <t>4227 PATRIKA</t>
@@ -608,7 +608,7 @@
     <t>4238 PATRIKA (R)</t>
   </si>
   <si>
-    <t>4239 PATRIKA (AGYA)</t>
+    <t>4239 PATRIKA (5600)</t>
   </si>
   <si>
     <t>4240 PATRIKA</t>
@@ -665,7 +665,7 @@
     <t>5008 PATRIKA</t>
   </si>
   <si>
-    <t>5009 PATRIKA (10k)</t>
+    <t>5009 PATRIKA</t>
   </si>
   <si>
     <t>5010 PATRIKA</t>
@@ -680,7 +680,7 @@
     <t>5012 PATRIKA</t>
   </si>
   <si>
-    <t>5013 PATRIKA</t>
+    <t>5013 PATRIKA (13.1k)</t>
   </si>
   <si>
     <t>5014 PATRIKA</t>
@@ -719,7 +719,7 @@
     <t>5024 PATRIKA</t>
   </si>
   <si>
-    <t>5025 PATRIKA (DORI) {M} (AGYA)</t>
+    <t>5025 PATRIKA (DORI) {M}</t>
   </si>
   <si>
     <t>5026 PATRIKA</t>
@@ -773,7 +773,7 @@
     <t>5040 PATRIKA (GRAPH AAYEGA)</t>
   </si>
   <si>
-    <t>5041 PATRIKA ( AGYA)</t>
+    <t>5041 PATRIKA</t>
   </si>
   <si>
     <t>5042 PATRIKA (AGYA)</t>
@@ -791,7 +791,7 @@
     <t>5045 Patrika (DC)</t>
   </si>
   <si>
-    <t>5046 PATRIKA (2400)</t>
+    <t>5046 PATRIKA</t>
   </si>
   <si>
     <t>5047 PATRIKA (5022-B)</t>
@@ -809,7 +809,7 @@
     <t>5853 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5854 PATRIKA (AGYA)</t>
+    <t>5854 PATRIKA</t>
   </si>
   <si>
     <t>5855 PATRIKA</t>
@@ -887,7 +887,7 @@
     <t>5878 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5879 PATRIKA (AA GYA)</t>
+    <t>5879 PATRIKA</t>
   </si>
   <si>
     <t>5880 PATRIKA</t>
@@ -911,7 +911,7 @@
     <t>5885 PATRIKA</t>
   </si>
   <si>
-    <t>5886 PATRIKA (2600)</t>
+    <t>5886 PATRIKA</t>
   </si>
   <si>
     <t>5887 PATRIKA (DC)</t>
@@ -1007,7 +1007,7 @@
     <t>5917 PATRIKA</t>
   </si>
   <si>
-    <t>5918 PATRIKA {M} (AGYA)</t>
+    <t>5918 PATRIKA {M}</t>
   </si>
   <si>
     <t>5919 PATRIKA {M}</t>
@@ -1025,7 +1025,7 @@
     <t>5923 PATRIKA (DC) {{10}}</t>
   </si>
   <si>
-    <t>5924 PATRIKA {M} (AGYA)</t>
+    <t>5924 PATRIKA {M}</t>
   </si>
   <si>
     <t>5925 PATRIKA {M}</t>
@@ -1103,7 +1103,7 @@
     <t>6501 PATRIKA</t>
   </si>
   <si>
-    <t>6502 PATRIKA (525)</t>
+    <t>6502 PATRIKA</t>
   </si>
   <si>
     <t>6503 PATRIKA</t>
@@ -1169,7 +1169,7 @@
     <t>6523 PATRIKA</t>
   </si>
   <si>
-    <t>6524 PATRIKA</t>
+    <t>6524 PATRIKA (500)</t>
   </si>
   <si>
     <t>6525 PATRIKA {M}</t>
@@ -1703,7 +1703,7 @@
     <t>9048 CARD</t>
   </si>
   <si>
-    <t>9049 CARD (700)</t>
+    <t>9049 CARD</t>
   </si>
   <si>
     <t>9050 CARD (Stk Nt)</t>
@@ -1844,7 +1844,7 @@
     <t>9095 CARD</t>
   </si>
   <si>
-    <t>9096 CARD</t>
+    <t>9096 CARD (3k)</t>
   </si>
   <si>
     <t>9097 CARD</t>
@@ -2578,16 +2578,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="23">
-        <v>549.5</v>
+        <v>539.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>549.5</v>
+        <v>539.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,16 +2612,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C11" s="23">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>332.29</v>
+        <v>325.02999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,16 +2629,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C12" s="23">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>155.1</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,17 +2663,11 @@
         <v>18</v>
       </c>
       <c r="B14" s="22">
-        <v>25</v>
-      </c>
-      <c r="C14" s="23">
-        <v>7</v>
-      </c>
-      <c r="D14" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="E14" s="25">
-        <v>12.6</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
@@ -2697,16 +2691,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C16" s="23">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>34.200000000000003</v>
+        <v>28.8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,16 +2708,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C17" s="23">
-        <v>-6.5</v>
+        <v>57</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>-13</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,33 +2725,27 @@
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>66</v>
-      </c>
-      <c r="C18" s="23">
-        <v>1</v>
-      </c>
-      <c r="D18" s="24">
-        <v>2</v>
-      </c>
-      <c r="E18" s="25">
-        <v>2</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C19" s="23">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C20" s="23">
-        <v>25.5</v>
+        <v>15.5</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,16 +2770,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="23">
-        <v>46.5</v>
+        <v>43.5</v>
       </c>
       <c r="D21" s="24">
         <v>2</v>
       </c>
       <c r="E21" s="25">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2801,25 +2789,31 @@
       <c r="B22" s="22">
         <v>42</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="26"/>
+      <c r="C22" s="23">
+        <v>40</v>
+      </c>
+      <c r="D22" s="24">
+        <v>2</v>
+      </c>
+      <c r="E22" s="25">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C23" s="23">
-        <v>84.75</v>
+        <v>16.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>169.5</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2827,16 +2821,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C24" s="23">
-        <v>-8</v>
+        <v>64.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>-16.8</v>
+        <v>135.44999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2844,16 +2838,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="22">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C25" s="23">
-        <v>-7.5</v>
+        <v>52.5</v>
       </c>
       <c r="D25" s="24">
         <v>2.1</v>
       </c>
       <c r="E25" s="25">
-        <v>-15.75</v>
+        <v>110.25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2870,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C27" s="23">
-        <v>70</v>
+        <v>60.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>164.5</v>
+        <v>142.18</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2887,16 +2881,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="22">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C28" s="23">
-        <v>30.5</v>
+        <v>6.5</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>71.680000000000007</v>
+        <v>15.28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,13 +2912,13 @@
         <v>32</v>
       </c>
       <c r="C30" s="23">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="D30" s="24">
-        <v>2.57</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E30" s="25">
-        <v>17.97</v>
+        <v>104.55</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2969,16 +2963,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C34" s="23">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3006,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C37" s="23">
-        <v>72.5</v>
+        <v>69.5</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>188.5</v>
+        <v>180.7</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3029,16 +3023,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C38" s="23">
-        <v>-0.5</v>
+        <v>-3</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>-1.35</v>
+        <v>-8.1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3040,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C39" s="23">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>280.8</v>
+        <v>278.10000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3091,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C42" s="23">
-        <v>16</v>
+        <v>10.5</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>45.6</v>
+        <v>29.93</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,16 +3108,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="23">
-        <v>2</v>
+        <v>8.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>4.5</v>
+        <v>19.13</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3125,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C44" s="23">
-        <v>108.5</v>
+        <v>97.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>244.13</v>
+        <v>219.38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,16 +3142,16 @@
         <v>49</v>
       </c>
       <c r="B45" s="22">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C45" s="23">
-        <v>25.5</v>
+        <v>18</v>
       </c>
       <c r="D45" s="24">
         <v>2.35</v>
       </c>
       <c r="E45" s="25">
-        <v>59.93</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,16 +3159,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C46" s="23">
-        <v>77</v>
+        <v>64.5</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>180.95</v>
+        <v>151.58000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,16 +3210,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C49" s="23">
-        <v>485.5</v>
+        <v>457.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>540.92999999999995</v>
+        <v>509.74</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,16 +3227,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C50" s="23">
-        <v>512</v>
+        <v>453.5</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>572.16</v>
+        <v>506.79</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3267,16 +3261,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C52" s="23">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>200</v>
+        <v>141.9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3295,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="C54" s="23">
-        <v>722.5</v>
+        <v>660</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>807.6</v>
+        <v>737.74</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3346,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C57" s="23">
-        <v>199.5</v>
+        <v>159.5</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>379.05</v>
+        <v>303.05</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3386,16 +3380,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C59" s="23">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>2.85</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3403,16 +3397,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C60" s="23">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>628.9</v>
+        <v>617.5</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,16 +3414,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C61" s="23">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>661.5</v>
+        <v>630</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3465,16 +3459,16 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C64" s="23">
-        <v>14.5</v>
+        <v>2.5</v>
       </c>
       <c r="D64" s="24">
         <v>2.1</v>
       </c>
       <c r="E64" s="25">
-        <v>30.45</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,16 +3476,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C65" s="23">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>573.29999999999995</v>
+        <v>571.20000000000005</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3516,16 +3510,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C67" s="23">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>37.44</v>
+        <v>35.36</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3567,16 +3561,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C70" s="23">
-        <v>195.5</v>
+        <v>178.5</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>175.95</v>
+        <v>160.65</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,16 +3578,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C71" s="23">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>104.4</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3601,16 +3595,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C72" s="23">
-        <v>1710</v>
+        <v>1674</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>2650.5</v>
+        <v>2594.6999999999998</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3618,16 +3612,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C73" s="23">
-        <v>1182.5</v>
+        <v>1173</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>1832.88</v>
+        <v>1818.15</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3635,16 +3629,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C74" s="23">
-        <v>1010</v>
+        <v>994</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>1565.5</v>
+        <v>1540.7</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3663,16 +3657,16 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C76" s="23">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>63.25</v>
+        <v>58.43</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3693,10 +3687,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C78" s="23">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3719,10 +3713,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C80" s="23">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3745,10 +3739,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C82" s="23">
-        <v>294.5</v>
+        <v>288.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3758,16 +3752,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C83" s="23">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>169.05</v>
+        <v>154.1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3775,16 +3769,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C84" s="23">
-        <v>405.5</v>
+        <v>404.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>466.33</v>
+        <v>465.18</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3792,16 +3786,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="C85" s="23">
-        <v>3456</v>
+        <v>3371.5</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>4838.3999999999996</v>
+        <v>4720.1000000000004</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3809,16 +3803,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C86" s="23">
-        <v>2384.5</v>
+        <v>2371.5</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3338.3</v>
+        <v>3320.1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3826,16 +3820,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C87" s="23">
-        <v>812.5</v>
+        <v>769.5</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1137.5</v>
+        <v>1077.3</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3852,16 +3846,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C89" s="23">
-        <v>477</v>
+        <v>456.5</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>954</v>
+        <v>913</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3869,16 +3863,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C90" s="23">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1836</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3886,16 +3880,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C91" s="23">
-        <v>-25.5</v>
+        <v>-30.5</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>-32.130000000000003</v>
+        <v>-38.43</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3903,16 +3897,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C92" s="23">
-        <v>372</v>
+        <v>319</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>468.72</v>
+        <v>401.94</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3998,16 +3992,16 @@
         <v>103</v>
       </c>
       <c r="B99" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C99" s="23">
-        <v>111.5</v>
+        <v>91.5</v>
       </c>
       <c r="D99" s="24">
         <v>1.55</v>
       </c>
       <c r="E99" s="25">
-        <v>172.83</v>
+        <v>141.83000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4015,16 +4009,16 @@
         <v>104</v>
       </c>
       <c r="B100" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C100" s="23">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D100" s="24">
         <v>1.55</v>
       </c>
       <c r="E100" s="25">
-        <v>271.25</v>
+        <v>263.5</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4066,10 +4060,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C103" s="23">
-        <v>7.5</v>
+        <v>-22.5</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4079,10 +4073,10 @@
         <v>108</v>
       </c>
       <c r="B104" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C104" s="23">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="26"/>
@@ -4225,16 +4219,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C114" s="23">
-        <v>9.5</v>
+        <v>3.5</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>118.75</v>
+        <v>43.75</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4276,16 +4270,16 @@
         <v>121</v>
       </c>
       <c r="B117" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C117" s="23">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
       <c r="D117" s="24">
         <v>12.5</v>
       </c>
       <c r="E117" s="25">
-        <v>68.75</v>
+        <v>31.25</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4327,16 +4321,16 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C120" s="23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D120" s="24">
         <v>12.5</v>
       </c>
       <c r="E120" s="25">
-        <v>150</v>
+        <v>125</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4445,16 +4439,16 @@
         <v>132</v>
       </c>
       <c r="B128" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C128" s="23">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D128" s="24">
         <v>15.5</v>
       </c>
       <c r="E128" s="25">
-        <v>178.25</v>
+        <v>147.25</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4524,16 +4518,16 @@
         <v>137</v>
       </c>
       <c r="B133" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C133" s="23">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="D133" s="24">
         <v>15.5</v>
       </c>
       <c r="E133" s="25">
-        <v>77.5</v>
+        <v>38.75</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4806,16 +4800,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C151" s="23">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>171.6</v>
+        <v>168.3</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4823,17 +4817,11 @@
         <v>156</v>
       </c>
       <c r="B152" s="22">
-        <v>244</v>
-      </c>
-      <c r="C152" s="23">
-        <v>2</v>
-      </c>
-      <c r="D152" s="24">
-        <v>2.8</v>
-      </c>
-      <c r="E152" s="25">
-        <v>5.6</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="C152" s="26"/>
+      <c r="D152" s="27"/>
+      <c r="E152" s="26"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="21" t="s">
@@ -4857,16 +4845,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C154" s="23">
-        <v>78.349999999999994</v>
+        <v>59.35</v>
       </c>
       <c r="D154" s="24">
         <v>2.75</v>
       </c>
       <c r="E154" s="25">
-        <v>215.46</v>
+        <v>163.21</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4885,16 +4873,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C156" s="23">
-        <v>107.85</v>
+        <v>95.85</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>366.69</v>
+        <v>325.89</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4913,27 +4901,33 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>90</v>
-      </c>
-      <c r="C158" s="26"/>
-      <c r="D158" s="27"/>
-      <c r="E158" s="26"/>
+        <v>98</v>
+      </c>
+      <c r="C158" s="23">
+        <v>20</v>
+      </c>
+      <c r="D158" s="24">
+        <v>2.7</v>
+      </c>
+      <c r="E158" s="25">
+        <v>54</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="21" t="s">
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C159" s="23">
-        <v>27.5</v>
+        <v>10</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>77</v>
+        <v>28</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4941,16 +4935,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C160" s="23">
-        <v>19.5</v>
+        <v>1</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>54.6</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4961,13 +4955,13 @@
         <v>40</v>
       </c>
       <c r="C161" s="23">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>2.5</v>
+        <v>272.5</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4992,16 +4986,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C163" s="23">
-        <v>73.5</v>
+        <v>64.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.8</v>
       </c>
       <c r="E163" s="25">
-        <v>205.8</v>
+        <v>180.6</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5009,16 +5003,16 @@
         <v>168</v>
       </c>
       <c r="B164" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C164" s="23">
-        <v>83.5</v>
+        <v>80.5</v>
       </c>
       <c r="D164" s="24">
         <v>2.8</v>
       </c>
       <c r="E164" s="25">
-        <v>233.8</v>
+        <v>225.4</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5026,16 +5020,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C165" s="23">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>469.05</v>
+        <v>454.3</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5043,16 +5037,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C166" s="23">
-        <v>74.5</v>
+        <v>54.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>219.78</v>
+        <v>160.78</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5060,33 +5054,27 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>49</v>
-      </c>
-      <c r="C167" s="23">
-        <v>2</v>
-      </c>
-      <c r="D167" s="24">
-        <v>3</v>
-      </c>
-      <c r="E167" s="25">
-        <v>6</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C167" s="26"/>
+      <c r="D167" s="27"/>
+      <c r="E167" s="26"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="21" t="s">
         <v>172</v>
       </c>
       <c r="B168" s="22">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C168" s="23">
-        <v>49.5</v>
+        <v>42.5</v>
       </c>
       <c r="D168" s="24">
         <v>3.4</v>
       </c>
       <c r="E168" s="25">
-        <v>168.54</v>
+        <v>144.69999999999999</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5094,16 +5082,16 @@
         <v>173</v>
       </c>
       <c r="B169" s="22">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C169" s="23">
-        <v>17.5</v>
+        <v>7.5</v>
       </c>
       <c r="D169" s="24">
         <v>3.3</v>
       </c>
       <c r="E169" s="25">
-        <v>57.75</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5128,16 +5116,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C171" s="23">
-        <v>101.5</v>
+        <v>97</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>355.25</v>
+        <v>339.5</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5154,16 +5142,16 @@
         <v>177</v>
       </c>
       <c r="B173" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C173" s="23">
-        <v>34.5</v>
+        <v>24.5</v>
       </c>
       <c r="D173" s="24">
         <v>3.9</v>
       </c>
       <c r="E173" s="25">
-        <v>134.55000000000001</v>
+        <v>95.55</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5203,16 +5191,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C176" s="23">
-        <v>15.5</v>
+        <v>21.5</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>51.62</v>
+        <v>71.599999999999994</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5220,16 +5208,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C177" s="23">
-        <v>-15</v>
+        <v>13</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>-49.95</v>
+        <v>43.29</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5248,16 +5236,16 @@
         <v>183</v>
       </c>
       <c r="B179" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C179" s="23">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D179" s="24">
         <v>3.6</v>
       </c>
       <c r="E179" s="25">
-        <v>183.6</v>
+        <v>147.6</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5291,16 +5279,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C182" s="23">
-        <v>19.5</v>
+        <v>10.1</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>74.099999999999994</v>
+        <v>38.380000000000003</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5308,16 +5296,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C183" s="23">
-        <v>124.5</v>
+        <v>119</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>373.5</v>
+        <v>357</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5325,16 +5313,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C184" s="23">
-        <v>17.5</v>
+        <v>7.5</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>78.75</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5393,16 +5381,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C188" s="23">
-        <v>58.5</v>
+        <v>55.5</v>
       </c>
       <c r="D188" s="24">
         <v>4.5</v>
       </c>
       <c r="E188" s="25">
-        <v>263.25</v>
+        <v>249.75</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5410,16 +5398,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C189" s="23">
-        <v>60.5</v>
+        <v>59</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>272.25</v>
+        <v>265.5</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5427,16 +5415,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C190" s="23">
-        <v>-7</v>
+        <v>64.5</v>
       </c>
       <c r="D190" s="24">
-        <v>3.94</v>
+        <v>3.83</v>
       </c>
       <c r="E190" s="25">
-        <v>-27.57</v>
+        <v>246.73</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5444,16 +5432,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C191" s="23">
-        <v>42.5</v>
+        <v>39.5</v>
       </c>
       <c r="D191" s="24">
-        <v>3.97</v>
+        <v>3.96</v>
       </c>
       <c r="E191" s="25">
-        <v>168.86</v>
+        <v>156.6</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5495,16 +5483,16 @@
         <v>198</v>
       </c>
       <c r="B194" s="22">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C194" s="23">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D194" s="24">
         <v>2.8</v>
       </c>
       <c r="E194" s="25">
-        <v>86.8</v>
+        <v>64.400000000000006</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5583,16 +5571,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C200" s="23">
-        <v>17.489999999999998</v>
+        <v>4.49</v>
       </c>
       <c r="D200" s="24">
         <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>53.75</v>
+        <v>13.8</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5626,16 +5614,16 @@
         <v>207</v>
       </c>
       <c r="B203" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C203" s="23">
-        <v>47</v>
+        <v>41.5</v>
       </c>
       <c r="D203" s="24">
         <v>3.38</v>
       </c>
       <c r="E203" s="25">
-        <v>158.85</v>
+        <v>140.26</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5681,16 +5669,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C208" s="23">
-        <v>13.5</v>
+        <v>11</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>51.3</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5698,16 +5686,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C209" s="23">
-        <v>-12.5</v>
+        <v>41</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>-47.5</v>
+        <v>155.80000000000001</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5715,16 +5703,16 @@
         <v>214</v>
       </c>
       <c r="B210" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C210" s="23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D210" s="24">
         <v>3.6</v>
       </c>
       <c r="E210" s="25">
-        <v>32.4</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5754,33 +5742,27 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>101</v>
-      </c>
-      <c r="C213" s="23">
-        <v>-5</v>
-      </c>
-      <c r="D213" s="24">
-        <v>4.12</v>
-      </c>
-      <c r="E213" s="25">
-        <v>-20.58</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="C213" s="26"/>
+      <c r="D213" s="27"/>
+      <c r="E213" s="26"/>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="21" t="s">
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="C214" s="23">
-        <v>-15.5</v>
+        <v>-65</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>-63.84</v>
+        <v>-267.72000000000003</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5839,16 +5821,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C218" s="23">
-        <v>9</v>
+        <v>6.5</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>39.049999999999997</v>
+        <v>28.2</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5889,16 +5871,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C222" s="23">
-        <v>-6.5</v>
+        <v>-10</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>-29.25</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5906,16 +5888,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C223" s="23">
-        <v>91.5</v>
+        <v>70.5</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>411.75</v>
+        <v>317.25</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5923,16 +5905,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C224" s="23">
-        <v>15.5</v>
+        <v>11.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>81.38</v>
+        <v>60.38</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5974,16 +5956,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C227" s="23">
-        <v>-15</v>
+        <v>1.5</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>-67.5</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5991,16 +5973,16 @@
         <v>232</v>
       </c>
       <c r="B228" s="22">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C228" s="23">
-        <v>26</v>
+        <v>22.5</v>
       </c>
       <c r="D228" s="24">
         <v>4.75</v>
       </c>
       <c r="E228" s="25">
-        <v>123.5</v>
+        <v>106.88</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6023,16 +6005,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C230" s="23">
-        <v>35.5</v>
+        <v>29</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>186.38</v>
+        <v>152.25</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6057,16 +6039,16 @@
         <v>236</v>
       </c>
       <c r="B232" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C232" s="23">
-        <v>9.3000000000000007</v>
+        <v>5.3</v>
       </c>
       <c r="D232" s="24">
         <v>4.75</v>
       </c>
       <c r="E232" s="25">
-        <v>44.18</v>
+        <v>25.18</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6074,16 +6056,16 @@
         <v>237</v>
       </c>
       <c r="B233" s="22">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C233" s="23">
-        <v>37.5</v>
+        <v>25</v>
       </c>
       <c r="D233" s="24">
         <v>4.75</v>
       </c>
       <c r="E233" s="25">
-        <v>178.13</v>
+        <v>118.75</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -6124,16 +6106,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C237" s="23">
-        <v>47</v>
+        <v>41.5</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>282</v>
+        <v>249</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6165,16 +6147,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C240" s="23">
-        <v>51.8</v>
+        <v>49.8</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>295.26</v>
+        <v>283.86</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6185,13 +6167,13 @@
         <v>18</v>
       </c>
       <c r="C241" s="23">
-        <v>23.5</v>
+        <v>25</v>
       </c>
       <c r="D241" s="24">
         <v>6.75</v>
       </c>
       <c r="E241" s="25">
-        <v>158.63</v>
+        <v>168.75</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6231,16 +6213,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C244" s="23">
-        <v>53.41</v>
+        <v>50.41</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>319.64999999999998</v>
+        <v>301.7</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6248,16 +6230,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C245" s="23">
-        <v>-21.5</v>
+        <v>-10</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>-91.59</v>
+        <v>-42.59</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6265,16 +6247,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C246" s="23">
-        <v>-4</v>
+        <v>24</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>-16</v>
+        <v>96</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6299,16 +6281,16 @@
         <v>252</v>
       </c>
       <c r="B248" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C248" s="23">
-        <v>9.5</v>
+        <v>7</v>
       </c>
       <c r="D248" s="24">
         <v>4.5</v>
       </c>
       <c r="E248" s="25">
-        <v>42.75</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6333,16 +6315,16 @@
         <v>254</v>
       </c>
       <c r="B250" s="22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C250" s="23">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="D250" s="24">
         <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>36.090000000000003</v>
+        <v>-5.16</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6350,11 +6332,17 @@
         <v>255</v>
       </c>
       <c r="B251" s="22">
-        <v>32</v>
-      </c>
-      <c r="C251" s="26"/>
-      <c r="D251" s="27"/>
-      <c r="E251" s="26"/>
+        <v>36</v>
+      </c>
+      <c r="C251" s="23">
+        <v>7</v>
+      </c>
+      <c r="D251" s="24">
+        <v>3.8</v>
+      </c>
+      <c r="E251" s="25">
+        <v>26.6</v>
+      </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" s="21" t="s">
@@ -6372,16 +6360,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="C253" s="23">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>217</v>
+        <v>185.5</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6389,16 +6377,16 @@
         <v>258</v>
       </c>
       <c r="B254" s="22">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C254" s="23">
-        <v>23.5</v>
+        <v>7.5</v>
       </c>
       <c r="D254" s="24">
         <v>4.25</v>
       </c>
       <c r="E254" s="25">
-        <v>99.88</v>
+        <v>31.88</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6406,16 +6394,16 @@
         <v>259</v>
       </c>
       <c r="B255" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C255" s="23">
-        <v>63.5</v>
+        <v>58.5</v>
       </c>
       <c r="D255" s="24">
         <v>4.25</v>
       </c>
       <c r="E255" s="25">
-        <v>269.88</v>
+        <v>248.63</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6432,16 +6420,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C257" s="23">
-        <v>-1.5</v>
+        <v>13.5</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>-6.27</v>
+        <v>56.43</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6466,16 +6454,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
+        <v>160</v>
+      </c>
+      <c r="C259" s="23">
         <v>154</v>
-      </c>
-      <c r="C259" s="23">
-        <v>145.5</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>622.74</v>
+        <v>659.12</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6483,16 +6471,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C260" s="23">
-        <v>63.5</v>
+        <v>60.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>271.77999999999997</v>
+        <v>258.94</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6534,16 +6522,16 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C263" s="23">
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>13.86</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6618,16 +6606,16 @@
         <v>273</v>
       </c>
       <c r="B269" s="22">
+        <v>30</v>
+      </c>
+      <c r="C269" s="23">
         <v>29</v>
-      </c>
-      <c r="C269" s="23">
-        <v>30.5</v>
       </c>
       <c r="D269" s="24">
         <v>5.0999999999999996</v>
       </c>
       <c r="E269" s="25">
-        <v>155.55000000000001</v>
+        <v>147.9</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6635,16 +6623,16 @@
         <v>274</v>
       </c>
       <c r="B270" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C270" s="23">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D270" s="24">
         <v>5.3</v>
       </c>
       <c r="E270" s="25">
-        <v>90.1</v>
+        <v>74.2</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6652,16 +6640,16 @@
         <v>275</v>
       </c>
       <c r="B271" s="22">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C271" s="23">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D271" s="24">
         <v>5.4</v>
       </c>
       <c r="E271" s="25">
-        <v>91.8</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6686,16 +6674,16 @@
         <v>277</v>
       </c>
       <c r="B273" s="22">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C273" s="23">
-        <v>36.5</v>
+        <v>33</v>
       </c>
       <c r="D273" s="24">
         <v>5.55</v>
       </c>
       <c r="E273" s="25">
-        <v>202.58</v>
+        <v>183.15</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6763,16 +6751,16 @@
         <v>282</v>
       </c>
       <c r="B278" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C278" s="23">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D278" s="24">
         <v>6.25</v>
       </c>
       <c r="E278" s="25">
-        <v>37.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6814,16 +6802,16 @@
         <v>285</v>
       </c>
       <c r="B281" s="22">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C281" s="23">
-        <v>6.5</v>
+        <v>-8.5</v>
       </c>
       <c r="D281" s="24">
         <v>6</v>
       </c>
       <c r="E281" s="25">
-        <v>39</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6848,16 +6836,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C283" s="23">
-        <v>-1.62</v>
+        <v>16.38</v>
       </c>
       <c r="D283" s="24">
         <v>5.94</v>
       </c>
       <c r="E283" s="25">
-        <v>-9.6199999999999992</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6865,16 +6853,16 @@
         <v>288</v>
       </c>
       <c r="B284" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C284" s="23">
-        <v>13.5</v>
+        <v>3.5</v>
       </c>
       <c r="D284" s="24">
         <v>5.7</v>
       </c>
       <c r="E284" s="25">
-        <v>76.95</v>
+        <v>19.95</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -6882,16 +6870,16 @@
         <v>289</v>
       </c>
       <c r="B285" s="22">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C285" s="23">
-        <v>19.5</v>
+        <v>11.5</v>
       </c>
       <c r="D285" s="24">
         <v>5.94</v>
       </c>
       <c r="E285" s="25">
-        <v>115.83</v>
+        <v>68.31</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6959,16 +6947,16 @@
         <v>294</v>
       </c>
       <c r="B290" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C290" s="23">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D290" s="24">
         <v>6.18</v>
       </c>
       <c r="E290" s="25">
-        <v>275.01</v>
+        <v>262.64999999999998</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6976,16 +6964,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C291" s="23">
-        <v>-2</v>
+        <v>17</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>-12.36</v>
+        <v>105.06</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7002,16 +6990,16 @@
         <v>297</v>
       </c>
       <c r="B293" s="22">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C293" s="23">
-        <v>7.5</v>
+        <v>-3</v>
       </c>
       <c r="D293" s="24">
         <v>6.18</v>
       </c>
       <c r="E293" s="25">
-        <v>46.35</v>
+        <v>-18.54</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -7107,16 +7095,16 @@
         <v>304</v>
       </c>
       <c r="B300" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C300" s="23">
-        <v>47.5</v>
+        <v>42</v>
       </c>
       <c r="D300" s="24">
         <v>6.65</v>
       </c>
       <c r="E300" s="25">
-        <v>315.88</v>
+        <v>279.3</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7161,16 +7149,16 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C304" s="23">
-        <v>12.5</v>
+        <v>6</v>
       </c>
       <c r="D304" s="24">
         <v>7.13</v>
       </c>
       <c r="E304" s="25">
-        <v>89.13</v>
+        <v>42.78</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7195,16 +7183,16 @@
         <v>310</v>
       </c>
       <c r="B306" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C306" s="23">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D306" s="24">
         <v>7.13</v>
       </c>
       <c r="E306" s="25">
-        <v>53.48</v>
+        <v>46.35</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -7212,16 +7200,16 @@
         <v>311</v>
       </c>
       <c r="B307" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C307" s="23">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D307" s="24">
         <v>6.65</v>
       </c>
       <c r="E307" s="25">
-        <v>119.7</v>
+        <v>86.45</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7346,16 +7334,16 @@
         <v>321</v>
       </c>
       <c r="B317" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C317" s="23">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="D317" s="24">
         <v>8.08</v>
       </c>
       <c r="E317" s="25">
-        <v>8.08</v>
+        <v>-4.04</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -7406,7 +7394,7 @@
         <v>325</v>
       </c>
       <c r="B321" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C321" s="23">
         <v>24.5</v>
@@ -7440,16 +7428,16 @@
         <v>327</v>
       </c>
       <c r="B323" s="22">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C323" s="23">
-        <v>4.7</v>
+        <v>16.2</v>
       </c>
       <c r="D323" s="24">
         <v>8.8000000000000007</v>
       </c>
       <c r="E323" s="25">
-        <v>41.36</v>
+        <v>142.56</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7542,16 +7530,16 @@
         <v>333</v>
       </c>
       <c r="B329" s="22">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C329" s="23">
-        <v>-13</v>
+        <v>12.5</v>
       </c>
       <c r="D329" s="24">
         <v>9.25</v>
       </c>
       <c r="E329" s="25">
-        <v>-120.25</v>
+        <v>115.63</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
@@ -7593,16 +7581,16 @@
         <v>336</v>
       </c>
       <c r="B332" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C332" s="23">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="D332" s="24">
         <v>8.33</v>
       </c>
       <c r="E332" s="25">
-        <v>50</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7610,16 +7598,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C333" s="23">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D333" s="24">
         <v>5.5</v>
       </c>
       <c r="E333" s="25">
-        <v>121</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7644,16 +7632,16 @@
         <v>339</v>
       </c>
       <c r="B335" s="22">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C335" s="23">
-        <v>11</v>
+        <v>4.5</v>
       </c>
       <c r="D335" s="24">
         <v>6.9</v>
       </c>
       <c r="E335" s="25">
-        <v>75.900000000000006</v>
+        <v>31.05</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -7695,16 +7683,16 @@
         <v>342</v>
       </c>
       <c r="B338" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C338" s="23">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D338" s="24">
         <v>8.5</v>
       </c>
       <c r="E338" s="25">
-        <v>93.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -7822,16 +7810,16 @@
         <v>351</v>
       </c>
       <c r="B347" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C347" s="23">
-        <v>41.5</v>
+        <v>35</v>
       </c>
       <c r="D347" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E347" s="25">
-        <v>203.35</v>
+        <v>171.5</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -7907,16 +7895,16 @@
         <v>356</v>
       </c>
       <c r="B352" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C352" s="23">
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="D352" s="24">
         <v>6.5</v>
       </c>
       <c r="E352" s="25">
-        <v>198.25</v>
+        <v>185.25</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
@@ -7924,16 +7912,16 @@
         <v>357</v>
       </c>
       <c r="B353" s="22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C353" s="23">
-        <v>7.5</v>
+        <v>4.5</v>
       </c>
       <c r="D353" s="24">
         <v>17</v>
       </c>
       <c r="E353" s="25">
-        <v>127.5</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -7941,16 +7929,16 @@
         <v>358</v>
       </c>
       <c r="B354" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C354" s="23">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="D354" s="24">
         <v>16</v>
       </c>
       <c r="E354" s="25">
-        <v>72</v>
+        <v>40</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -7958,16 +7946,16 @@
         <v>359</v>
       </c>
       <c r="B355" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C355" s="23">
-        <v>-2.5</v>
+        <v>-0.25</v>
       </c>
       <c r="D355" s="24">
-        <v>12.5</v>
+        <v>12.52</v>
       </c>
       <c r="E355" s="25">
-        <v>-31.25</v>
+        <v>-3.13</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -8026,16 +8014,16 @@
         <v>363</v>
       </c>
       <c r="B359" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C359" s="23">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="D359" s="24">
         <v>18</v>
       </c>
       <c r="E359" s="25">
-        <v>144</v>
+        <v>99</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -8060,16 +8048,16 @@
         <v>365</v>
       </c>
       <c r="B361" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C361" s="23">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D361" s="24">
         <v>11</v>
       </c>
       <c r="E361" s="25">
-        <v>77</v>
+        <v>33</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8139,16 +8127,16 @@
         <v>370</v>
       </c>
       <c r="B366" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C366" s="23">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D366" s="24">
         <v>7.84</v>
       </c>
       <c r="E366" s="25">
-        <v>11.76</v>
+        <v>7.84</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -8156,16 +8144,16 @@
         <v>371</v>
       </c>
       <c r="B367" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C367" s="23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D367" s="24">
         <v>11</v>
       </c>
       <c r="E367" s="25">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -8190,16 +8178,16 @@
         <v>373</v>
       </c>
       <c r="B369" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C369" s="23">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D369" s="24">
         <v>14.79</v>
       </c>
       <c r="E369" s="25">
-        <v>96.12</v>
+        <v>66.540000000000006</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -8382,16 +8370,16 @@
         <v>385</v>
       </c>
       <c r="B381" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C381" s="23">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="D381" s="24">
         <v>10</v>
       </c>
       <c r="E381" s="25">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -8416,16 +8404,16 @@
         <v>387</v>
       </c>
       <c r="B383" s="22">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C383" s="23">
-        <v>13.5</v>
+        <v>5.5</v>
       </c>
       <c r="D383" s="24">
         <v>7.84</v>
       </c>
       <c r="E383" s="25">
-        <v>105.84</v>
+        <v>43.12</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
@@ -8461,16 +8449,16 @@
         <v>390</v>
       </c>
       <c r="B386" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C386" s="23">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D386" s="24">
         <v>10.93</v>
       </c>
       <c r="E386" s="25">
-        <v>76.510000000000005</v>
+        <v>32.79</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8546,16 +8534,16 @@
         <v>395</v>
       </c>
       <c r="B391" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C391" s="23">
-        <v>13.75</v>
+        <v>10.75</v>
       </c>
       <c r="D391" s="24">
         <v>11.5</v>
       </c>
       <c r="E391" s="25">
-        <v>158.13</v>
+        <v>123.63</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
@@ -8648,16 +8636,16 @@
         <v>401</v>
       </c>
       <c r="B397" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C397" s="23">
-        <v>12</v>
+        <v>10.5</v>
       </c>
       <c r="D397" s="24">
         <v>9.5</v>
       </c>
       <c r="E397" s="25">
-        <v>114</v>
+        <v>99.75</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8710,16 +8698,16 @@
         <v>405</v>
       </c>
       <c r="B401" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C401" s="23">
-        <v>1.45</v>
+        <v>0.45</v>
       </c>
       <c r="D401" s="24">
         <v>10</v>
       </c>
       <c r="E401" s="25">
-        <v>14.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
@@ -8804,16 +8792,16 @@
         <v>411</v>
       </c>
       <c r="B407" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C407" s="23">
-        <v>34.5</v>
+        <v>32</v>
       </c>
       <c r="D407" s="24">
         <v>2.1</v>
       </c>
       <c r="E407" s="25">
-        <v>72.45</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -8821,16 +8809,16 @@
         <v>412</v>
       </c>
       <c r="B408" s="22">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C408" s="23">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D408" s="24">
         <v>2</v>
       </c>
       <c r="E408" s="25">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -8967,16 +8955,16 @@
         <v>422</v>
       </c>
       <c r="B418" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C418" s="23">
-        <v>29.5</v>
+        <v>27.5</v>
       </c>
       <c r="D418" s="24">
         <v>2.5</v>
       </c>
       <c r="E418" s="25">
-        <v>73.75</v>
+        <v>68.75</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
@@ -8984,16 +8972,16 @@
         <v>423</v>
       </c>
       <c r="B419" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C419" s="23">
-        <v>11.5</v>
+        <v>9</v>
       </c>
       <c r="D419" s="24">
         <v>2.7</v>
       </c>
       <c r="E419" s="25">
-        <v>31.05</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
@@ -9001,16 +8989,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C420" s="23">
-        <v>11.5</v>
+        <v>6</v>
       </c>
       <c r="D420" s="24">
         <v>2.7</v>
       </c>
       <c r="E420" s="25">
-        <v>31.05</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9052,16 +9040,16 @@
         <v>427</v>
       </c>
       <c r="B423" s="22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C423" s="23">
-        <v>26.5</v>
+        <v>23.5</v>
       </c>
       <c r="D423" s="24">
         <v>2.75</v>
       </c>
       <c r="E423" s="25">
-        <v>72.88</v>
+        <v>64.63</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -9129,16 +9117,16 @@
         <v>432</v>
       </c>
       <c r="B428" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C428" s="23">
-        <v>144.34</v>
+        <v>139.84</v>
       </c>
       <c r="D428" s="24">
         <v>2.8</v>
       </c>
       <c r="E428" s="25">
-        <v>404.15</v>
+        <v>391.55</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -9146,16 +9134,16 @@
         <v>433</v>
       </c>
       <c r="B429" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C429" s="23">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="D429" s="24">
         <v>2.95</v>
       </c>
       <c r="E429" s="25">
-        <v>33.93</v>
+        <v>30.98</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9265,17 +9253,11 @@
         <v>440</v>
       </c>
       <c r="B436" s="22">
-        <v>22</v>
-      </c>
-      <c r="C436" s="23">
-        <v>15</v>
-      </c>
-      <c r="D436" s="24">
-        <v>3.25</v>
-      </c>
-      <c r="E436" s="25">
-        <v>48.75</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C436" s="26"/>
+      <c r="D436" s="27"/>
+      <c r="E436" s="26"/>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" s="21" t="s">
@@ -9374,16 +9356,16 @@
         <v>447</v>
       </c>
       <c r="B443" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C443" s="23">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D443" s="24">
         <v>3.8</v>
       </c>
       <c r="E443" s="25">
-        <v>228</v>
+        <v>209</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
@@ -9408,16 +9390,16 @@
         <v>449</v>
       </c>
       <c r="B445" s="22">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C445" s="23">
-        <v>23.5</v>
+        <v>12.5</v>
       </c>
       <c r="D445" s="24">
         <v>3.33</v>
       </c>
       <c r="E445" s="25">
-        <v>78.260000000000005</v>
+        <v>41.63</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -9511,16 +9493,16 @@
         <v>456</v>
       </c>
       <c r="B452" s="22">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C452" s="23">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D452" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E452" s="25">
-        <v>62.26</v>
+        <v>45.66</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
@@ -9613,16 +9595,16 @@
         <v>462</v>
       </c>
       <c r="B458" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C458" s="23">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D458" s="24">
         <v>4.28</v>
       </c>
       <c r="E458" s="25">
-        <v>415.16</v>
+        <v>402.32</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -9741,16 +9723,16 @@
         <v>470</v>
       </c>
       <c r="B466" s="22">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C466" s="23">
-        <v>44.5</v>
+        <v>42.5</v>
       </c>
       <c r="D466" s="24">
         <v>5.5</v>
       </c>
       <c r="E466" s="25">
-        <v>244.75</v>
+        <v>233.75</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
@@ -9866,16 +9848,16 @@
         <v>479</v>
       </c>
       <c r="B475" s="22">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C475" s="23">
-        <v>19</v>
+        <v>8.5</v>
       </c>
       <c r="D475" s="24">
         <v>7.51</v>
       </c>
       <c r="E475" s="25">
-        <v>142.71</v>
+        <v>63.85</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
@@ -9883,16 +9865,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C476" s="23">
-        <v>14.5</v>
+        <v>10</v>
       </c>
       <c r="D476" s="24">
         <v>7.13</v>
       </c>
       <c r="E476" s="25">
-        <v>103.39</v>
+        <v>71.3</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -9917,16 +9899,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C478" s="23">
-        <v>11</v>
+        <v>2.5</v>
       </c>
       <c r="D478" s="24">
         <v>7</v>
       </c>
       <c r="E478" s="25">
-        <v>77</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -9934,16 +9916,16 @@
         <v>483</v>
       </c>
       <c r="B479" s="22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C479" s="23">
-        <v>8</v>
+        <v>5.5</v>
       </c>
       <c r="D479" s="24">
         <v>7.6</v>
       </c>
       <c r="E479" s="25">
-        <v>60.8</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
@@ -10050,16 +10032,16 @@
         <v>491</v>
       </c>
       <c r="B487" s="22">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C487" s="23">
-        <v>5.5</v>
+        <v>-3</v>
       </c>
       <c r="D487" s="24">
         <v>9.5</v>
       </c>
       <c r="E487" s="25">
-        <v>52.25</v>
+        <v>-28.5</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
@@ -10099,16 +10081,16 @@
         <v>494</v>
       </c>
       <c r="B490" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C490" s="23">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D490" s="24">
         <v>5.7</v>
       </c>
       <c r="E490" s="25">
-        <v>165.3</v>
+        <v>125.4</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10116,33 +10098,27 @@
         <v>495</v>
       </c>
       <c r="B491" s="22">
-        <v>3</v>
-      </c>
-      <c r="C491" s="23">
-        <v>24</v>
-      </c>
-      <c r="D491" s="24">
-        <v>1.92</v>
-      </c>
-      <c r="E491" s="25">
-        <v>46.04</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C491" s="26"/>
+      <c r="D491" s="27"/>
+      <c r="E491" s="26"/>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A492" s="21" t="s">
         <v>496</v>
       </c>
       <c r="B492" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C492" s="23">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D492" s="24">
         <v>1.9</v>
       </c>
       <c r="E492" s="25">
-        <v>153.9</v>
+        <v>115.9</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
@@ -10150,16 +10126,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C493" s="23">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D493" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E493" s="25">
-        <v>116.6</v>
+        <v>101.2</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10167,16 +10143,16 @@
         <v>498</v>
       </c>
       <c r="B494" s="22">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C494" s="23">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="D494" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E494" s="25">
-        <v>-7.7</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
@@ -10184,16 +10160,16 @@
         <v>499</v>
       </c>
       <c r="B495" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C495" s="23">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D495" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E495" s="25">
-        <v>232.4</v>
+        <v>219.95</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -10201,16 +10177,16 @@
         <v>500</v>
       </c>
       <c r="B496" s="22">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C496" s="23">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D496" s="24">
         <v>1.4</v>
       </c>
       <c r="E496" s="25">
-        <v>91</v>
+        <v>75.599999999999994</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -10365,16 +10341,16 @@
         <v>510</v>
       </c>
       <c r="B506" s="22">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C506" s="23">
-        <v>566.75</v>
+        <v>562.75</v>
       </c>
       <c r="D506" s="24">
         <v>1.5</v>
       </c>
       <c r="E506" s="25">
-        <v>850.13</v>
+        <v>844.13</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
@@ -10433,33 +10409,27 @@
         <v>514</v>
       </c>
       <c r="B510" s="22">
-        <v>59</v>
-      </c>
-      <c r="C510" s="23">
-        <v>1</v>
-      </c>
-      <c r="D510" s="24">
-        <v>1.71</v>
-      </c>
-      <c r="E510" s="25">
-        <v>1.71</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C510" s="26"/>
+      <c r="D510" s="27"/>
+      <c r="E510" s="26"/>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A511" s="21" t="s">
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C511" s="23">
-        <v>41.5</v>
+        <v>31.5</v>
       </c>
       <c r="D511" s="24">
         <v>0.92</v>
       </c>
       <c r="E511" s="25">
-        <v>38.35</v>
+        <v>29.11</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10467,16 +10437,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C512" s="23">
-        <v>56.7</v>
+        <v>29.2</v>
       </c>
       <c r="D512" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E512" s="25">
-        <v>129.28</v>
+        <v>66.58</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10484,16 +10454,16 @@
         <v>517</v>
       </c>
       <c r="B513" s="22">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C513" s="23">
-        <v>97.5</v>
+        <v>94.5</v>
       </c>
       <c r="D513" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E513" s="25">
-        <v>222.3</v>
+        <v>215.46</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10561,16 +10531,16 @@
         <v>522</v>
       </c>
       <c r="B518" s="22">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C518" s="23">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D518" s="24">
         <v>2.8</v>
       </c>
       <c r="E518" s="25">
-        <v>103.6</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
@@ -10661,16 +10631,16 @@
         <v>528</v>
       </c>
       <c r="B524" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C524" s="23">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D524" s="24">
         <v>3.2</v>
       </c>
       <c r="E524" s="25">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
@@ -10687,16 +10657,16 @@
         <v>530</v>
       </c>
       <c r="B526" s="22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C526" s="23">
-        <v>18</v>
+        <v>14.5</v>
       </c>
       <c r="D526" s="24">
         <v>2.85</v>
       </c>
       <c r="E526" s="25">
-        <v>51.3</v>
+        <v>41.33</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10756,16 +10726,16 @@
         <v>535</v>
       </c>
       <c r="B531" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C531" s="23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D531" s="24">
         <v>3.5</v>
       </c>
       <c r="E531" s="25">
-        <v>38.5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.25">
@@ -10773,7 +10743,7 @@
         <v>536</v>
       </c>
       <c r="B532" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C532" s="23">
         <v>1</v>
@@ -10790,16 +10760,16 @@
         <v>537</v>
       </c>
       <c r="B533" s="22">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C533" s="23">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D533" s="24">
         <v>3.33</v>
       </c>
       <c r="E533" s="25">
-        <v>169.83</v>
+        <v>153.18</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -10850,16 +10820,16 @@
         <v>541</v>
       </c>
       <c r="B537" s="22">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C537" s="23">
-        <v>14.5</v>
+        <v>8.5</v>
       </c>
       <c r="D537" s="24">
         <v>3.6</v>
       </c>
       <c r="E537" s="25">
-        <v>52.2</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -10987,16 +10957,16 @@
         <v>550</v>
       </c>
       <c r="B546" s="22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C546" s="23">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D546" s="24">
         <v>3.8</v>
       </c>
       <c r="E546" s="25">
-        <v>22.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -11072,16 +11042,16 @@
         <v>555</v>
       </c>
       <c r="B551" s="22">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C551" s="23">
-        <v>10.5</v>
+        <v>8.5</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>49.88</v>
+        <v>40.380000000000003</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11106,16 +11076,16 @@
         <v>557</v>
       </c>
       <c r="B553" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C553" s="23">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D553" s="24">
         <v>4.75</v>
       </c>
       <c r="E553" s="25">
-        <v>142.5</v>
+        <v>137.75</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -11143,13 +11113,13 @@
         <v>27</v>
       </c>
       <c r="C555" s="23">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D555" s="24">
         <v>4.75</v>
       </c>
       <c r="E555" s="25">
-        <v>33.25</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.25">
@@ -11157,16 +11127,16 @@
         <v>560</v>
       </c>
       <c r="B556" s="22">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C556" s="23">
-        <v>5.62</v>
+        <v>3.62</v>
       </c>
       <c r="D556" s="24">
         <v>5</v>
       </c>
       <c r="E556" s="25">
-        <v>28.1</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
@@ -11174,16 +11144,16 @@
         <v>561</v>
       </c>
       <c r="B557" s="22">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C557" s="23">
-        <v>18.5</v>
+        <v>17</v>
       </c>
       <c r="D557" s="24">
         <v>5</v>
       </c>
       <c r="E557" s="25">
-        <v>92.5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11276,16 +11246,16 @@
         <v>567</v>
       </c>
       <c r="B563" s="22">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C563" s="23">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D563" s="24">
         <v>5.75</v>
       </c>
       <c r="E563" s="25">
-        <v>138</v>
+        <v>97.75</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -11489,28 +11459,28 @@
         <v>580</v>
       </c>
       <c r="B576" s="22">
-        <v>26</v>
-      </c>
-      <c r="C576" s="26"/>
-      <c r="D576" s="27"/>
-      <c r="E576" s="26"/>
+        <v>27</v>
+      </c>
+      <c r="C576" s="23">
+        <v>1</v>
+      </c>
+      <c r="D576" s="24">
+        <v>10</v>
+      </c>
+      <c r="E576" s="25">
+        <v>10</v>
+      </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A577" s="21" t="s">
         <v>581</v>
       </c>
       <c r="B577" s="22">
-        <v>37</v>
-      </c>
-      <c r="C577" s="23">
-        <v>1</v>
-      </c>
-      <c r="D577" s="24">
-        <v>8.75</v>
-      </c>
-      <c r="E577" s="25">
-        <v>8.75</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C577" s="26"/>
+      <c r="D577" s="27"/>
+      <c r="E577" s="26"/>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A578" s="21" t="s">
@@ -11543,16 +11513,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C580" s="23">
-        <v>20.5</v>
+        <v>18.5</v>
       </c>
       <c r="D580" s="24">
         <v>2.76</v>
       </c>
       <c r="E580" s="25">
-        <v>56.59</v>
+        <v>51.08</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11594,16 +11564,16 @@
         <v>587</v>
       </c>
       <c r="B583" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C583" s="23">
-        <v>18.5</v>
+        <v>17.5</v>
       </c>
       <c r="D583" s="24">
         <v>2.8</v>
       </c>
       <c r="E583" s="25">
-        <v>51.8</v>
+        <v>49</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
@@ -11662,16 +11632,16 @@
         <v>591</v>
       </c>
       <c r="B587" s="22">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C587" s="23">
-        <v>43.5</v>
+        <v>41</v>
       </c>
       <c r="D587" s="24">
         <v>2.76</v>
       </c>
       <c r="E587" s="25">
-        <v>120.06</v>
+        <v>113.16</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -11711,16 +11681,16 @@
         <v>594</v>
       </c>
       <c r="B590" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C590" s="23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D590" s="24">
         <v>3</v>
       </c>
       <c r="E590" s="25">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
@@ -11728,16 +11698,16 @@
         <v>595</v>
       </c>
       <c r="B591" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C591" s="23">
-        <v>18.5</v>
+        <v>17.5</v>
       </c>
       <c r="D591" s="24">
         <v>3.1</v>
       </c>
       <c r="E591" s="25">
-        <v>57.35</v>
+        <v>54.25</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -11845,16 +11815,16 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C598" s="23">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D598" s="24">
         <v>4.92</v>
       </c>
       <c r="E598" s="25">
-        <v>132.94</v>
+        <v>39.39</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11862,16 +11832,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C599" s="23">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D599" s="24">
         <v>1.92</v>
       </c>
       <c r="E599" s="25">
-        <v>205.49</v>
+        <v>203.57</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -11913,16 +11883,16 @@
         <v>606</v>
       </c>
       <c r="B602" s="22">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C602" s="23">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D602" s="24">
         <v>2.84</v>
       </c>
       <c r="E602" s="25">
-        <v>193.06</v>
+        <v>187.38</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12015,16 +11985,16 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C608" s="23">
-        <v>887.5</v>
+        <v>879.5</v>
       </c>
       <c r="D608" s="24">
         <v>1.4</v>
       </c>
       <c r="E608" s="25">
-        <v>1242.5</v>
+        <v>1231.3</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12032,16 +12002,16 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C609" s="23">
-        <v>-105.5</v>
+        <v>-106.5</v>
       </c>
       <c r="D609" s="24">
         <v>1.4</v>
       </c>
       <c r="E609" s="25">
-        <v>-147.69999999999999</v>
+        <v>-149.1</v>
       </c>
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
@@ -12049,10 +12019,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C610" s="23">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12062,10 +12032,10 @@
         <v>615</v>
       </c>
       <c r="B611" s="22">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C611" s="23">
-        <v>43.5</v>
+        <v>40.5</v>
       </c>
       <c r="D611" s="27"/>
       <c r="E611" s="26"/>
@@ -12075,10 +12045,10 @@
         <v>616</v>
       </c>
       <c r="B612" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C612" s="23">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="D612" s="27"/>
       <c r="E612" s="26"/>
@@ -12174,16 +12144,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C619" s="23">
-        <v>537.5</v>
+        <v>535.5</v>
       </c>
       <c r="D619" s="24">
         <v>0.81</v>
       </c>
       <c r="E619" s="25">
-        <v>437.9</v>
+        <v>436.27</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12191,16 +12161,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C620" s="23">
-        <v>104.5</v>
+        <v>97.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.81</v>
       </c>
       <c r="E620" s="25">
-        <v>84.35</v>
+        <v>78.7</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12208,16 +12178,16 @@
         <v>625</v>
       </c>
       <c r="B621" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C621" s="23">
-        <v>1010.5</v>
+        <v>1000.5</v>
       </c>
       <c r="D621" s="24">
         <v>0.5</v>
       </c>
       <c r="E621" s="25">
-        <v>505.25</v>
+        <v>500.25</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
@@ -12225,16 +12195,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C622" s="23">
-        <v>1419</v>
+        <v>1399</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>737.88</v>
+        <v>727.48</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12242,16 +12212,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C623" s="23">
-        <v>1537</v>
+        <v>1527</v>
       </c>
       <c r="D623" s="24">
         <v>0.51</v>
       </c>
       <c r="E623" s="25">
-        <v>782.93</v>
+        <v>777.84</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12259,16 +12229,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C624" s="23">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="D624" s="24">
         <v>0.52</v>
       </c>
       <c r="E624" s="25">
-        <v>359.32</v>
+        <v>354.12</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12293,16 +12263,16 @@
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C626" s="23">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D626" s="24">
         <v>0.52</v>
       </c>
       <c r="E626" s="25">
-        <v>167.44</v>
+        <v>165.36</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12310,16 +12280,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C627" s="23">
-        <v>550</v>
+        <v>540.5</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>385</v>
+        <v>378.35</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12327,16 +12297,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C628" s="23">
-        <v>279.5</v>
+        <v>275.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.7</v>
       </c>
       <c r="E628" s="25">
-        <v>195.65</v>
+        <v>192.85</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12344,16 +12314,16 @@
         <v>633</v>
       </c>
       <c r="B629" s="22">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C629" s="23">
-        <v>159.5</v>
+        <v>149.5</v>
       </c>
       <c r="D629" s="24">
         <v>0.69</v>
       </c>
       <c r="E629" s="25">
-        <v>109.28</v>
+        <v>102.43</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12385,16 +12355,16 @@
         <v>636</v>
       </c>
       <c r="B632" s="22">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C632" s="23">
-        <v>962.5</v>
+        <v>955.5</v>
       </c>
       <c r="D632" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E632" s="25">
-        <v>529.64</v>
+        <v>525.79</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
@@ -12480,11 +12450,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>44896.17</v>
+        <v>43679.02</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>82635.520000000004</v>
+        <v>79931.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:08
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -125,7 +125,7 @@
     <t>1866 PATRIKA</t>
   </si>
   <si>
-    <t>1867 PATRIKA</t>
+    <t>1867 PATRIKA (STCK LOT NO )</t>
   </si>
   <si>
     <t>1868 PATRIKA</t>
@@ -503,10 +503,10 @@
     <t>4203 PATRIKA</t>
   </si>
   <si>
-    <t>4204 PATRIKA (GGN) {M}</t>
-  </si>
-  <si>
-    <t>4205 PATRIKA (AGYA)</t>
+    <t>4204 PATRIKA (GGN) {M} (DC)</t>
+  </si>
+  <si>
+    <t>4205 PATRIKA</t>
   </si>
   <si>
     <t>4207 PATRIKA (DC)  {{10}}</t>
@@ -608,7 +608,7 @@
     <t>4238 PATRIKA (R)</t>
   </si>
   <si>
-    <t>4239 PATRIKA (5600)</t>
+    <t>4239 PATRIKA</t>
   </si>
   <si>
     <t>4240 PATRIKA</t>
@@ -617,7 +617,7 @@
     <t>4241 PATRIKA</t>
   </si>
   <si>
-    <t>4242 PATRIKA</t>
+    <t>4242 PATRIKA (DESIGN CHNG)</t>
   </si>
   <si>
     <t>4244 PATRIKA (4202-B)</t>
@@ -662,7 +662,7 @@
     <t>5007 PATRIKA (Dc) {{10}}</t>
   </si>
   <si>
-    <t>5008 PATRIKA</t>
+    <t>5008 PATRIKA (08.04)</t>
   </si>
   <si>
     <t>5009 PATRIKA</t>
@@ -680,7 +680,7 @@
     <t>5012 PATRIKA</t>
   </si>
   <si>
-    <t>5013 PATRIKA (13.1k)</t>
+    <t>5013 PATRIKA</t>
   </si>
   <si>
     <t>5014 PATRIKA</t>
@@ -704,7 +704,7 @@
     <t>5020 PATRIKA - B</t>
   </si>
   <si>
-    <t>5020 PATRIKA (DIRECT) {M}</t>
+    <t>5020 PATRIKA (DIRECT) {M} (4.4k)</t>
   </si>
   <si>
     <t>5021 PATRIKA</t>
@@ -776,7 +776,7 @@
     <t>5041 PATRIKA</t>
   </si>
   <si>
-    <t>5042 PATRIKA (AGYA)</t>
+    <t>5042 PATRIKA</t>
   </si>
   <si>
     <t>5042 PATRIKA - B (DC)</t>
@@ -917,7 +917,7 @@
     <t>5887 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5888 PATRIKA {M}</t>
+    <t>5888 PATRIKA {M} (08.04 - 2k)</t>
   </si>
   <si>
     <t>5889 PATRIKA (DC) {{10}}</t>
@@ -1121,7 +1121,7 @@
     <t>6507 PATRIKA (GGN)</t>
   </si>
   <si>
-    <t>6508 PATRIKA {M}</t>
+    <t>6508 PATRIKA {M} (800 10.02)</t>
   </si>
   <si>
     <t>6509 PATRIKA</t>
@@ -1169,7 +1169,7 @@
     <t>6523 PATRIKA</t>
   </si>
   <si>
-    <t>6524 PATRIKA (500)</t>
+    <t>6524 PATRIKA</t>
   </si>
   <si>
     <t>6525 PATRIKA {M}</t>
@@ -1844,7 +1844,7 @@
     <t>9095 CARD</t>
   </si>
   <si>
-    <t>9096 CARD (3k)</t>
+    <t>9096 CARD</t>
   </si>
   <si>
     <t>9097 CARD</t>
@@ -2612,16 +2612,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C11" s="23">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>325.02999999999997</v>
+        <v>322.3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,16 +2629,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="22">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C12" s="23">
-        <v>76</v>
+        <v>64.5</v>
       </c>
       <c r="D12" s="24">
         <v>1.65</v>
       </c>
       <c r="E12" s="25">
-        <v>125.4</v>
+        <v>106.43</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,16 +2646,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C13" s="23">
-        <v>20.5</v>
+        <v>8.5</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>33.83</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2708,16 +2708,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C17" s="23">
-        <v>57</v>
+        <v>47.5</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2736,16 +2736,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" s="23">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2753,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" s="23">
-        <v>15.5</v>
+        <v>25.5</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2804,16 +2804,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C23" s="23">
-        <v>16.75</v>
+        <v>14.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>33.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2821,16 +2821,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="22">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C24" s="23">
-        <v>64.5</v>
+        <v>139.5</v>
       </c>
       <c r="D24" s="24">
         <v>2.1</v>
       </c>
       <c r="E24" s="25">
-        <v>135.44999999999999</v>
+        <v>292.95</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,13 +2841,13 @@
         <v>53</v>
       </c>
       <c r="C25" s="23">
-        <v>52.5</v>
+        <v>55.5</v>
       </c>
       <c r="D25" s="24">
         <v>2.1</v>
       </c>
       <c r="E25" s="25">
-        <v>110.25</v>
+        <v>116.55</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C27" s="23">
-        <v>60.5</v>
+        <v>44</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>142.18</v>
+        <v>103.4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,13 +2884,13 @@
         <v>118</v>
       </c>
       <c r="C28" s="23">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="D28" s="24">
         <v>2.35</v>
       </c>
       <c r="E28" s="25">
-        <v>15.28</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2900,25 +2900,31 @@
       <c r="B29" s="22">
         <v>88</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="26"/>
+      <c r="C29" s="23">
+        <v>31</v>
+      </c>
+      <c r="D29" s="24">
+        <v>2.58</v>
+      </c>
+      <c r="E29" s="25">
+        <v>80</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" s="23">
-        <v>41</v>
+        <v>40.5</v>
       </c>
       <c r="D30" s="24">
         <v>2.5499999999999998</v>
       </c>
       <c r="E30" s="25">
-        <v>104.55</v>
+        <v>103.28</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,13 +2972,13 @@
         <v>73</v>
       </c>
       <c r="C34" s="23">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D34" s="24">
         <v>2.5</v>
       </c>
       <c r="E34" s="25">
-        <v>210</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3006,16 +3012,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C37" s="23">
-        <v>69.5</v>
+        <v>69</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>180.7</v>
+        <v>179.4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3023,16 +3029,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="22">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" s="23">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="D38" s="24">
         <v>2.7</v>
       </c>
       <c r="E38" s="25">
-        <v>-8.1</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3040,16 +3046,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C39" s="23">
-        <v>103</v>
+        <v>89.5</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>278.10000000000002</v>
+        <v>241.65</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3091,16 +3097,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C42" s="23">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>29.93</v>
+        <v>25.65</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3108,16 +3114,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C43" s="23">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="D43" s="24">
         <v>2.25</v>
       </c>
       <c r="E43" s="25">
-        <v>19.13</v>
+        <v>16.88</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3128,13 +3134,13 @@
         <v>71</v>
       </c>
       <c r="C44" s="23">
-        <v>97.5</v>
+        <v>131.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>219.38</v>
+        <v>295.88</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3210,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="C49" s="23">
-        <v>457.5</v>
+        <v>384</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>509.74</v>
+        <v>427.85</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3227,16 +3233,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="C50" s="23">
-        <v>453.5</v>
+        <v>406.5</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>506.79</v>
+        <v>454.26</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3261,16 +3267,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C52" s="23">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>141.9</v>
+        <v>131.84</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3295,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C54" s="23">
-        <v>660</v>
+        <v>608</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>737.74</v>
+        <v>679.62</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3346,16 +3352,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C57" s="23">
-        <v>159.5</v>
+        <v>161.5</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>303.05</v>
+        <v>306.85000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3397,16 +3403,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C60" s="23">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>617.5</v>
+        <v>609.9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3414,16 +3420,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C61" s="23">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>630</v>
+        <v>623.70000000000005</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3431,16 +3437,16 @@
         <v>66</v>
       </c>
       <c r="B62" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62" s="23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="24">
         <v>2.1</v>
       </c>
       <c r="E62" s="25">
-        <v>73.5</v>
+        <v>71.400000000000006</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3459,33 +3465,27 @@
         <v>68</v>
       </c>
       <c r="B64" s="22">
-        <v>97</v>
-      </c>
-      <c r="C64" s="23">
-        <v>2.5</v>
-      </c>
-      <c r="D64" s="24">
-        <v>2.1</v>
-      </c>
-      <c r="E64" s="25">
-        <v>5.25</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C64" s="26"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C65" s="23">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>571.20000000000005</v>
+        <v>554.4</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3493,16 +3493,16 @@
         <v>70</v>
       </c>
       <c r="B66" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C66" s="23">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D66" s="24">
         <v>0.52</v>
       </c>
       <c r="E66" s="25">
-        <v>79.040000000000006</v>
+        <v>77.48</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3510,16 +3510,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C67" s="23">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>35.36</v>
+        <v>33.799999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3527,16 +3527,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C68" s="23">
-        <v>57.5</v>
+        <v>32.5</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>40.25</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,16 +3544,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C69" s="23">
-        <v>293.5</v>
+        <v>269.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>205.45</v>
+        <v>188.65</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,16 +3561,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C70" s="23">
-        <v>178.5</v>
+        <v>169.5</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>160.65</v>
+        <v>152.55000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,16 +3578,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C71" s="23">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>99</v>
+        <v>96.3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,16 +3595,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C72" s="23">
-        <v>1674</v>
+        <v>1642.5</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>2594.6999999999998</v>
+        <v>2545.88</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,16 +3612,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C73" s="23">
-        <v>1173</v>
+        <v>1157</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>1818.15</v>
+        <v>1793.35</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,16 +3629,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C74" s="23">
-        <v>994</v>
+        <v>984</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>1540.7</v>
+        <v>1525.2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3657,16 +3657,16 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C76" s="23">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>58.43</v>
+        <v>55.54</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,10 +3687,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C78" s="23">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3700,10 +3700,10 @@
         <v>83</v>
       </c>
       <c r="B79" s="22">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C79" s="23">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D79" s="27"/>
       <c r="E79" s="26"/>
@@ -3713,10 +3713,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C80" s="23">
-        <v>3</v>
+        <v>-13</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3739,10 +3739,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="C82" s="23">
-        <v>288.5</v>
+        <v>251.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3752,16 +3752,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C83" s="23">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>154.1</v>
+        <v>110.4</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3769,16 +3769,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C84" s="23">
-        <v>404.5</v>
+        <v>399.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>465.18</v>
+        <v>459.43</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3786,16 +3786,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C85" s="23">
-        <v>3371.5</v>
+        <v>3339.5</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>4720.1000000000004</v>
+        <v>4675.3</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3803,16 +3803,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C86" s="23">
-        <v>2371.5</v>
+        <v>2345</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3320.1</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3846,16 +3846,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C89" s="23">
-        <v>456.5</v>
+        <v>450.5</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>913</v>
+        <v>901</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,16 +3863,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C90" s="23">
-        <v>910</v>
+        <v>901.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1820</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3880,16 +3880,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C91" s="23">
-        <v>-30.5</v>
+        <v>-33.5</v>
       </c>
       <c r="D91" s="24">
         <v>1.26</v>
       </c>
       <c r="E91" s="25">
-        <v>-38.43</v>
+        <v>-42.21</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,16 +3897,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C92" s="23">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>401.94</v>
+        <v>383.04</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4026,16 +4026,16 @@
         <v>105</v>
       </c>
       <c r="B101" s="22">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C101" s="23">
-        <v>295</v>
+        <v>215</v>
       </c>
       <c r="D101" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E101" s="25">
-        <v>339.25</v>
+        <v>247.25</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4043,16 +4043,16 @@
         <v>106</v>
       </c>
       <c r="B102" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C102" s="23">
-        <v>362</v>
+        <v>322</v>
       </c>
       <c r="D102" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E102" s="25">
-        <v>416.3</v>
+        <v>370.3</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4060,10 +4060,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C103" s="23">
-        <v>-22.5</v>
+        <v>-32.5</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4185,16 +4185,16 @@
         <v>116</v>
       </c>
       <c r="B112" s="22">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C112" s="23">
-        <v>32.5</v>
+        <v>30.5</v>
       </c>
       <c r="D112" s="24">
         <v>12.5</v>
       </c>
       <c r="E112" s="25">
-        <v>406.25</v>
+        <v>381.25</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4222,13 +4222,13 @@
         <v>82</v>
       </c>
       <c r="C114" s="23">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>43.75</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4270,16 +4270,16 @@
         <v>121</v>
       </c>
       <c r="B117" s="22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C117" s="23">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="D117" s="24">
         <v>12.5</v>
       </c>
       <c r="E117" s="25">
-        <v>31.25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4321,16 +4321,16 @@
         <v>124</v>
       </c>
       <c r="B120" s="22">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C120" s="23">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="D120" s="24">
         <v>12.5</v>
       </c>
       <c r="E120" s="25">
-        <v>125</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4439,16 +4439,16 @@
         <v>132</v>
       </c>
       <c r="B128" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C128" s="23">
-        <v>9.5</v>
+        <v>1.5</v>
       </c>
       <c r="D128" s="24">
         <v>15.5</v>
       </c>
       <c r="E128" s="25">
-        <v>147.25</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4755,16 +4755,16 @@
         <v>152</v>
       </c>
       <c r="B148" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C148" s="23">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D148" s="24">
         <v>18.440000000000001</v>
       </c>
       <c r="E148" s="25">
-        <v>55.31</v>
+        <v>46.09</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4772,27 +4772,33 @@
         <v>153</v>
       </c>
       <c r="B149" s="22">
-        <v>16</v>
-      </c>
-      <c r="C149" s="26"/>
-      <c r="D149" s="27"/>
-      <c r="E149" s="26"/>
+        <v>15</v>
+      </c>
+      <c r="C149" s="23">
+        <v>6</v>
+      </c>
+      <c r="D149" s="24">
+        <v>18.41</v>
+      </c>
+      <c r="E149" s="25">
+        <v>110.45</v>
+      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="21" t="s">
         <v>154</v>
       </c>
       <c r="B150" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C150" s="23">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="D150" s="24">
         <v>14.5</v>
       </c>
       <c r="E150" s="25">
-        <v>50.75</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4800,16 +4806,16 @@
         <v>155</v>
       </c>
       <c r="B151" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C151" s="23">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D151" s="24">
         <v>3.3</v>
       </c>
       <c r="E151" s="25">
-        <v>168.3</v>
+        <v>161.69999999999999</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -4845,16 +4851,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C154" s="23">
-        <v>59.35</v>
+        <v>51.35</v>
       </c>
       <c r="D154" s="24">
         <v>2.75</v>
       </c>
       <c r="E154" s="25">
-        <v>163.21</v>
+        <v>141.21</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4873,16 +4879,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C156" s="23">
-        <v>95.85</v>
+        <v>99.35</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>325.89</v>
+        <v>337.79</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4901,16 +4907,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C158" s="23">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>54</v>
+        <v>270</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4918,16 +4924,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C159" s="23">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>28</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4935,16 +4941,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C160" s="23">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>2.8</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4952,16 +4958,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="22">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C161" s="23">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D161" s="24">
         <v>2.5</v>
       </c>
       <c r="E161" s="25">
-        <v>272.5</v>
+        <v>247.5</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -4986,16 +4992,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C163" s="23">
-        <v>64.5</v>
+        <v>57.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.8</v>
       </c>
       <c r="E163" s="25">
-        <v>180.6</v>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5020,16 +5026,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C165" s="23">
-        <v>154</v>
+        <v>147.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>454.3</v>
+        <v>435.13</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5037,16 +5043,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C166" s="23">
-        <v>54.5</v>
+        <v>59.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>160.78</v>
+        <v>175.53</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5056,9 +5062,15 @@
       <c r="B167" s="22">
         <v>50</v>
       </c>
-      <c r="C167" s="26"/>
-      <c r="D167" s="27"/>
-      <c r="E167" s="26"/>
+      <c r="C167" s="23">
+        <v>17</v>
+      </c>
+      <c r="D167" s="24">
+        <v>3</v>
+      </c>
+      <c r="E167" s="25">
+        <v>51</v>
+      </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="21" t="s">
@@ -5099,16 +5111,16 @@
         <v>174</v>
       </c>
       <c r="B170" s="22">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C170" s="23">
-        <v>65</v>
+        <v>63.5</v>
       </c>
       <c r="D170" s="24">
         <v>3.3</v>
       </c>
       <c r="E170" s="25">
-        <v>214.5</v>
+        <v>209.55</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5116,16 +5128,16 @@
         <v>175</v>
       </c>
       <c r="B171" s="22">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C171" s="23">
-        <v>97</v>
+        <v>91.5</v>
       </c>
       <c r="D171" s="24">
         <v>3.5</v>
       </c>
       <c r="E171" s="25">
-        <v>339.5</v>
+        <v>320.25</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5191,16 +5203,16 @@
         <v>180</v>
       </c>
       <c r="B176" s="22">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C176" s="23">
-        <v>21.5</v>
+        <v>29.5</v>
       </c>
       <c r="D176" s="24">
         <v>3.33</v>
       </c>
       <c r="E176" s="25">
-        <v>71.599999999999994</v>
+        <v>98.24</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5208,16 +5220,16 @@
         <v>181</v>
       </c>
       <c r="B177" s="22">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C177" s="23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D177" s="24">
         <v>3.33</v>
       </c>
       <c r="E177" s="25">
-        <v>43.29</v>
+        <v>39.96</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5236,16 +5248,16 @@
         <v>183</v>
       </c>
       <c r="B179" s="22">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C179" s="23">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D179" s="24">
         <v>3.6</v>
       </c>
       <c r="E179" s="25">
-        <v>147.6</v>
+        <v>165.6</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5279,16 +5291,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C182" s="23">
-        <v>10.1</v>
+        <v>9.1</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>38.380000000000003</v>
+        <v>34.58</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5296,16 +5308,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C183" s="23">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5313,16 +5325,16 @@
         <v>188</v>
       </c>
       <c r="B184" s="22">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C184" s="23">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="D184" s="24">
         <v>4.5</v>
       </c>
       <c r="E184" s="25">
-        <v>33.75</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5381,16 +5393,16 @@
         <v>192</v>
       </c>
       <c r="B188" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C188" s="23">
-        <v>55.5</v>
+        <v>53.5</v>
       </c>
       <c r="D188" s="24">
         <v>4.5</v>
       </c>
       <c r="E188" s="25">
-        <v>249.75</v>
+        <v>240.75</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5398,16 +5410,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C189" s="23">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>265.5</v>
+        <v>252</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5415,16 +5427,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C190" s="23">
-        <v>64.5</v>
+        <v>124</v>
       </c>
       <c r="D190" s="24">
-        <v>3.83</v>
+        <v>3.77</v>
       </c>
       <c r="E190" s="25">
-        <v>246.73</v>
+        <v>467.79</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5432,16 +5444,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C191" s="23">
-        <v>39.5</v>
+        <v>38</v>
       </c>
       <c r="D191" s="24">
         <v>3.96</v>
       </c>
       <c r="E191" s="25">
-        <v>156.6</v>
+        <v>150.65</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5466,16 +5478,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C193" s="23">
-        <v>-6</v>
+        <v>34</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>-18</v>
+        <v>102</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5571,16 +5583,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C200" s="23">
-        <v>4.49</v>
+        <v>-0.51</v>
       </c>
       <c r="D200" s="24">
-        <v>3.07</v>
+        <v>3.08</v>
       </c>
       <c r="E200" s="25">
-        <v>13.8</v>
+        <v>-1.57</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5669,16 +5681,16 @@
         <v>212</v>
       </c>
       <c r="B208" s="22">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C208" s="23">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D208" s="24">
         <v>3.8</v>
       </c>
       <c r="E208" s="25">
-        <v>41.8</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5689,13 +5701,13 @@
         <v>117</v>
       </c>
       <c r="C209" s="23">
-        <v>41</v>
+        <v>38.5</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>155.80000000000001</v>
+        <v>146.30000000000001</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5703,16 +5715,16 @@
         <v>214</v>
       </c>
       <c r="B210" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C210" s="23">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="D210" s="24">
         <v>3.6</v>
       </c>
       <c r="E210" s="25">
-        <v>25.2</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -5753,16 +5765,16 @@
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C214" s="23">
-        <v>-65</v>
+        <v>29.5</v>
       </c>
       <c r="D214" s="24">
         <v>4.12</v>
       </c>
       <c r="E214" s="25">
-        <v>-267.72000000000003</v>
+        <v>121.42</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -5787,16 +5799,16 @@
         <v>220</v>
       </c>
       <c r="B216" s="22">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C216" s="23">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D216" s="24">
         <v>4.75</v>
       </c>
       <c r="E216" s="25">
-        <v>61.75</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -5821,16 +5833,16 @@
         <v>222</v>
       </c>
       <c r="B218" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C218" s="23">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="D218" s="24">
         <v>4.34</v>
       </c>
       <c r="E218" s="25">
-        <v>28.2</v>
+        <v>15.19</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -5871,16 +5883,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C222" s="23">
-        <v>-10</v>
+        <v>-27</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>-45</v>
+        <v>-121.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5888,16 +5900,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C223" s="23">
-        <v>70.5</v>
+        <v>49</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>317.25</v>
+        <v>220.5</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5908,13 +5920,13 @@
         <v>124</v>
       </c>
       <c r="C224" s="23">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>60.38</v>
+        <v>55.13</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5956,16 +5968,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C227" s="23">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>6.75</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -5976,13 +5988,13 @@
         <v>27</v>
       </c>
       <c r="C228" s="23">
-        <v>22.5</v>
+        <v>21.5</v>
       </c>
       <c r="D228" s="24">
         <v>4.75</v>
       </c>
       <c r="E228" s="25">
-        <v>106.88</v>
+        <v>102.13</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6005,16 +6017,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C230" s="23">
-        <v>29</v>
+        <v>24.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>152.25</v>
+        <v>128.63</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6022,16 +6034,16 @@
         <v>235</v>
       </c>
       <c r="B231" s="22">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C231" s="23">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>383.25</v>
+        <v>393.75</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6039,16 +6051,16 @@
         <v>236</v>
       </c>
       <c r="B232" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C232" s="23">
-        <v>5.3</v>
+        <v>1.3</v>
       </c>
       <c r="D232" s="24">
         <v>4.75</v>
       </c>
       <c r="E232" s="25">
-        <v>25.18</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6106,16 +6118,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C237" s="23">
-        <v>41.5</v>
+        <v>37</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>249</v>
+        <v>222</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6147,16 +6159,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C240" s="23">
-        <v>49.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="D240" s="24">
         <v>5.7</v>
       </c>
       <c r="E240" s="25">
-        <v>283.86</v>
+        <v>232.56</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6213,16 +6225,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C244" s="23">
-        <v>50.41</v>
+        <v>43.41</v>
       </c>
       <c r="D244" s="24">
         <v>5.98</v>
       </c>
       <c r="E244" s="25">
-        <v>301.7</v>
+        <v>259.8</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6233,13 +6245,13 @@
         <v>56</v>
       </c>
       <c r="C245" s="23">
-        <v>-10</v>
+        <v>5.5</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>-42.59</v>
+        <v>23.42</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6247,16 +6259,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C246" s="23">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6315,16 +6327,16 @@
         <v>254</v>
       </c>
       <c r="B250" s="22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C250" s="23">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D250" s="24">
         <v>5.16</v>
       </c>
       <c r="E250" s="25">
-        <v>-5.16</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6332,16 +6344,16 @@
         <v>255</v>
       </c>
       <c r="B251" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C251" s="23">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D251" s="24">
         <v>3.8</v>
       </c>
       <c r="E251" s="25">
-        <v>26.6</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6360,16 +6372,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C253" s="23">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>185.5</v>
+        <v>168</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6377,33 +6389,27 @@
         <v>258</v>
       </c>
       <c r="B254" s="22">
-        <v>82</v>
-      </c>
-      <c r="C254" s="23">
-        <v>7.5</v>
-      </c>
-      <c r="D254" s="24">
-        <v>4.25</v>
-      </c>
-      <c r="E254" s="25">
-        <v>31.88</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C254" s="26"/>
+      <c r="D254" s="27"/>
+      <c r="E254" s="26"/>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="21" t="s">
         <v>259</v>
       </c>
       <c r="B255" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C255" s="23">
-        <v>58.5</v>
+        <v>50</v>
       </c>
       <c r="D255" s="24">
         <v>4.25</v>
       </c>
       <c r="E255" s="25">
-        <v>248.63</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6420,16 +6426,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C257" s="23">
-        <v>13.5</v>
+        <v>8.5</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>56.43</v>
+        <v>35.53</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6437,16 +6443,16 @@
         <v>262</v>
       </c>
       <c r="B258" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C258" s="23">
-        <v>27.5</v>
+        <v>25.5</v>
       </c>
       <c r="D258" s="24">
         <v>4.18</v>
       </c>
       <c r="E258" s="25">
-        <v>114.95</v>
+        <v>106.59</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6454,16 +6460,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C259" s="23">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>659.12</v>
+        <v>624.88</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6471,16 +6477,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C260" s="23">
-        <v>60.5</v>
+        <v>59.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>258.94</v>
+        <v>254.66</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6522,16 +6528,16 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C263" s="23">
-        <v>0.8</v>
+        <v>22.8</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>3.96</v>
+        <v>112.86</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6571,16 +6577,16 @@
         <v>270</v>
       </c>
       <c r="B266" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C266" s="23">
-        <v>5.0999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D266" s="24">
         <v>5</v>
       </c>
       <c r="E266" s="25">
-        <v>25.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6606,16 +6612,16 @@
         <v>273</v>
       </c>
       <c r="B269" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C269" s="23">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D269" s="24">
         <v>5.0999999999999996</v>
       </c>
       <c r="E269" s="25">
-        <v>147.9</v>
+        <v>137.69999999999999</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6640,16 +6646,16 @@
         <v>275</v>
       </c>
       <c r="B271" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C271" s="23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D271" s="24">
         <v>5.4</v>
       </c>
       <c r="E271" s="25">
-        <v>32.4</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6674,16 +6680,16 @@
         <v>277</v>
       </c>
       <c r="B273" s="22">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C273" s="23">
-        <v>33</v>
+        <v>21.5</v>
       </c>
       <c r="D273" s="24">
         <v>5.55</v>
       </c>
       <c r="E273" s="25">
-        <v>183.15</v>
+        <v>119.33</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -6725,16 +6731,16 @@
         <v>280</v>
       </c>
       <c r="B276" s="22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C276" s="23">
-        <v>27.5</v>
+        <v>25.5</v>
       </c>
       <c r="D276" s="24">
         <v>5.46</v>
       </c>
       <c r="E276" s="25">
-        <v>150.15</v>
+        <v>139.22999999999999</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -6751,17 +6757,11 @@
         <v>282</v>
       </c>
       <c r="B278" s="22">
-        <v>67</v>
-      </c>
-      <c r="C278" s="23">
-        <v>4</v>
-      </c>
-      <c r="D278" s="24">
-        <v>6.25</v>
-      </c>
-      <c r="E278" s="25">
-        <v>25</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C278" s="26"/>
+      <c r="D278" s="27"/>
+      <c r="E278" s="26"/>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="21" t="s">
@@ -6802,16 +6802,16 @@
         <v>285</v>
       </c>
       <c r="B281" s="22">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C281" s="23">
-        <v>-8.5</v>
+        <v>3</v>
       </c>
       <c r="D281" s="24">
         <v>6</v>
       </c>
       <c r="E281" s="25">
-        <v>-51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -6836,16 +6836,16 @@
         <v>287</v>
       </c>
       <c r="B283" s="22">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C283" s="23">
-        <v>16.38</v>
+        <v>17.88</v>
       </c>
       <c r="D283" s="24">
         <v>5.94</v>
       </c>
       <c r="E283" s="25">
-        <v>97.3</v>
+        <v>106.21</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -6853,16 +6853,16 @@
         <v>288</v>
       </c>
       <c r="B284" s="22">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C284" s="23">
-        <v>3.5</v>
+        <v>13.5</v>
       </c>
       <c r="D284" s="24">
         <v>5.7</v>
       </c>
       <c r="E284" s="25">
-        <v>19.95</v>
+        <v>76.95</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -6870,16 +6870,16 @@
         <v>289</v>
       </c>
       <c r="B285" s="22">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C285" s="23">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D285" s="24">
         <v>5.94</v>
       </c>
       <c r="E285" s="25">
-        <v>68.31</v>
+        <v>56.43</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -6967,13 +6967,13 @@
         <v>66</v>
       </c>
       <c r="C291" s="23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>105.06</v>
+        <v>98.88</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6990,16 +6990,16 @@
         <v>297</v>
       </c>
       <c r="B293" s="22">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C293" s="23">
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="D293" s="24">
         <v>6.18</v>
       </c>
       <c r="E293" s="25">
-        <v>-18.54</v>
+        <v>18.54</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -7035,16 +7035,16 @@
         <v>300</v>
       </c>
       <c r="B296" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C296" s="23">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D296" s="24">
         <v>6.4</v>
       </c>
       <c r="E296" s="25">
-        <v>60.8</v>
+        <v>54.4</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -7095,16 +7095,16 @@
         <v>304</v>
       </c>
       <c r="B300" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C300" s="23">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D300" s="24">
         <v>6.65</v>
       </c>
       <c r="E300" s="25">
-        <v>279.3</v>
+        <v>252.7</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7112,16 +7112,16 @@
         <v>305</v>
       </c>
       <c r="B301" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C301" s="23">
-        <v>39.5</v>
+        <v>37.5</v>
       </c>
       <c r="D301" s="24">
         <v>6.18</v>
       </c>
       <c r="E301" s="25">
-        <v>244.11</v>
+        <v>231.75</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -7149,7 +7149,7 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C304" s="23">
         <v>6</v>
@@ -7274,16 +7274,16 @@
         <v>317</v>
       </c>
       <c r="B313" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C313" s="23">
-        <v>3.5</v>
+        <v>1.5</v>
       </c>
       <c r="D313" s="24">
         <v>7.6</v>
       </c>
       <c r="E313" s="25">
-        <v>26.6</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -7334,16 +7334,16 @@
         <v>321</v>
       </c>
       <c r="B317" s="22">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C317" s="23">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="D317" s="24">
         <v>8.08</v>
       </c>
       <c r="E317" s="25">
-        <v>-4.04</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -7428,16 +7428,16 @@
         <v>327</v>
       </c>
       <c r="B323" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C323" s="23">
-        <v>16.2</v>
+        <v>14.2</v>
       </c>
       <c r="D323" s="24">
         <v>8.8000000000000007</v>
       </c>
       <c r="E323" s="25">
-        <v>142.56</v>
+        <v>124.96</v>
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
@@ -7445,16 +7445,16 @@
         <v>328</v>
       </c>
       <c r="B324" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C324" s="23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D324" s="24">
         <v>9.31</v>
       </c>
       <c r="E324" s="25">
-        <v>149</v>
+        <v>130.38</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -7496,16 +7496,16 @@
         <v>331</v>
       </c>
       <c r="B327" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C327" s="23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D327" s="24">
         <v>10</v>
       </c>
       <c r="E327" s="25">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -7530,16 +7530,16 @@
         <v>333</v>
       </c>
       <c r="B329" s="22">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C329" s="23">
-        <v>12.5</v>
+        <v>15.5</v>
       </c>
       <c r="D329" s="24">
         <v>9.25</v>
       </c>
       <c r="E329" s="25">
-        <v>115.63</v>
+        <v>143.38</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
@@ -7547,16 +7547,16 @@
         <v>334</v>
       </c>
       <c r="B330" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C330" s="23">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D330" s="24">
         <v>11.75</v>
       </c>
       <c r="E330" s="25">
-        <v>170.38</v>
+        <v>146.88</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -7598,16 +7598,16 @@
         <v>337</v>
       </c>
       <c r="B333" s="22">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C333" s="23">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="D333" s="24">
         <v>5.5</v>
       </c>
       <c r="E333" s="25">
-        <v>104.5</v>
+        <v>269.5</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7649,16 +7649,16 @@
         <v>340</v>
       </c>
       <c r="B336" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C336" s="23">
-        <v>20.5</v>
+        <v>18.05</v>
       </c>
       <c r="D336" s="24">
         <v>7.13</v>
       </c>
       <c r="E336" s="25">
-        <v>146.16999999999999</v>
+        <v>128.69999999999999</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -7666,16 +7666,16 @@
         <v>341</v>
       </c>
       <c r="B337" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C337" s="23">
-        <v>26.5</v>
+        <v>25</v>
       </c>
       <c r="D337" s="24">
         <v>8.5</v>
       </c>
       <c r="E337" s="25">
-        <v>225.25</v>
+        <v>212.5</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -7810,16 +7810,16 @@
         <v>351</v>
       </c>
       <c r="B347" s="22">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C347" s="23">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D347" s="24">
         <v>4.9000000000000004</v>
       </c>
       <c r="E347" s="25">
-        <v>171.5</v>
+        <v>127.4</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -7878,16 +7878,16 @@
         <v>355</v>
       </c>
       <c r="B351" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C351" s="23">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="D351" s="24">
         <v>8.67</v>
       </c>
       <c r="E351" s="25">
-        <v>125.77</v>
+        <v>117.09</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
@@ -7912,16 +7912,16 @@
         <v>357</v>
       </c>
       <c r="B353" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C353" s="23">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="D353" s="24">
         <v>17</v>
       </c>
       <c r="E353" s="25">
-        <v>76.5</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -7946,16 +7946,16 @@
         <v>359</v>
       </c>
       <c r="B355" s="22">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C355" s="23">
-        <v>-0.25</v>
+        <v>1.25</v>
       </c>
       <c r="D355" s="24">
-        <v>12.52</v>
+        <v>12.5</v>
       </c>
       <c r="E355" s="25">
-        <v>-3.13</v>
+        <v>15.63</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -7980,16 +7980,16 @@
         <v>361</v>
       </c>
       <c r="B357" s="22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C357" s="23">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="D357" s="24">
         <v>16.25</v>
       </c>
       <c r="E357" s="25">
-        <v>56.88</v>
+        <v>73.13</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -8014,16 +8014,16 @@
         <v>363</v>
       </c>
       <c r="B359" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C359" s="23">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="D359" s="24">
         <v>18</v>
       </c>
       <c r="E359" s="25">
-        <v>99</v>
+        <v>54</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -8048,16 +8048,16 @@
         <v>365</v>
       </c>
       <c r="B361" s="22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C361" s="23">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="D361" s="24">
         <v>11</v>
       </c>
       <c r="E361" s="25">
-        <v>33</v>
+        <v>-44</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -8099,16 +8099,16 @@
         <v>368</v>
       </c>
       <c r="B364" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C364" s="23">
-        <v>11.99</v>
+        <v>8.99</v>
       </c>
       <c r="D364" s="24">
         <v>12</v>
       </c>
       <c r="E364" s="25">
-        <v>143.88</v>
+        <v>107.88</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -8116,11 +8116,17 @@
         <v>369</v>
       </c>
       <c r="B365" s="22">
-        <v>15</v>
-      </c>
-      <c r="C365" s="26"/>
-      <c r="D365" s="27"/>
-      <c r="E365" s="26"/>
+        <v>14</v>
+      </c>
+      <c r="C365" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D365" s="24">
+        <v>12</v>
+      </c>
+      <c r="E365" s="25">
+        <v>18</v>
+      </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" s="21" t="s">
@@ -8144,16 +8150,16 @@
         <v>371</v>
       </c>
       <c r="B367" s="22">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C367" s="23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D367" s="24">
         <v>11</v>
       </c>
       <c r="E367" s="25">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -8305,13 +8311,13 @@
         <v>14</v>
       </c>
       <c r="C377" s="23">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="D377" s="24">
         <v>10.5</v>
       </c>
       <c r="E377" s="25">
-        <v>-42</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -8370,16 +8376,16 @@
         <v>385</v>
       </c>
       <c r="B381" s="22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C381" s="23">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D381" s="24">
         <v>10</v>
       </c>
       <c r="E381" s="25">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -8517,16 +8523,16 @@
         <v>394</v>
       </c>
       <c r="B390" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C390" s="23">
-        <v>12.5</v>
+        <v>10.5</v>
       </c>
       <c r="D390" s="24">
         <v>12.75</v>
       </c>
       <c r="E390" s="25">
-        <v>159.38</v>
+        <v>133.88</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
@@ -8585,16 +8591,16 @@
         <v>398</v>
       </c>
       <c r="B394" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C394" s="23">
-        <v>12.5</v>
+        <v>13.5</v>
       </c>
       <c r="D394" s="24">
         <v>14.5</v>
       </c>
       <c r="E394" s="25">
-        <v>181.25</v>
+        <v>195.75</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -8639,13 +8645,13 @@
         <v>19</v>
       </c>
       <c r="C397" s="23">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D397" s="24">
         <v>9.5</v>
       </c>
       <c r="E397" s="25">
-        <v>99.75</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8653,16 +8659,16 @@
         <v>402</v>
       </c>
       <c r="B398" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C398" s="23">
-        <v>17</v>
+        <v>13.5</v>
       </c>
       <c r="D398" s="24">
         <v>10.93</v>
       </c>
       <c r="E398" s="25">
-        <v>185.81</v>
+        <v>147.56</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -8670,16 +8676,16 @@
         <v>403</v>
       </c>
       <c r="B399" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C399" s="23">
-        <v>12.5</v>
+        <v>8.5</v>
       </c>
       <c r="D399" s="24">
         <v>10.93</v>
       </c>
       <c r="E399" s="25">
-        <v>136.63</v>
+        <v>92.91</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -8698,16 +8704,16 @@
         <v>405</v>
       </c>
       <c r="B401" s="22">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C401" s="23">
-        <v>0.45</v>
+        <v>1.45</v>
       </c>
       <c r="D401" s="24">
         <v>10</v>
       </c>
       <c r="E401" s="25">
-        <v>4.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
@@ -8748,15 +8754,17 @@
       <c r="A404" s="21" t="s">
         <v>408</v>
       </c>
-      <c r="B404" s="22"/>
+      <c r="B404" s="22">
+        <v>1</v>
+      </c>
       <c r="C404" s="23">
-        <v>19.5</v>
+        <v>17.5</v>
       </c>
       <c r="D404" s="24">
         <v>27</v>
       </c>
       <c r="E404" s="25">
-        <v>526.5</v>
+        <v>472.5</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
@@ -8809,16 +8817,16 @@
         <v>412</v>
       </c>
       <c r="B408" s="22">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C408" s="23">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D408" s="24">
         <v>2</v>
       </c>
       <c r="E408" s="25">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -8955,16 +8963,16 @@
         <v>422</v>
       </c>
       <c r="B418" s="22">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C418" s="23">
-        <v>27.5</v>
+        <v>26.5</v>
       </c>
       <c r="D418" s="24">
         <v>2.5</v>
       </c>
       <c r="E418" s="25">
-        <v>68.75</v>
+        <v>66.25</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
@@ -8972,16 +8980,16 @@
         <v>423</v>
       </c>
       <c r="B419" s="22">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C419" s="23">
-        <v>9</v>
+        <v>11.5</v>
       </c>
       <c r="D419" s="24">
         <v>2.7</v>
       </c>
       <c r="E419" s="25">
-        <v>24.3</v>
+        <v>31.05</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
@@ -8989,16 +8997,16 @@
         <v>424</v>
       </c>
       <c r="B420" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C420" s="23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D420" s="24">
         <v>2.7</v>
       </c>
       <c r="E420" s="25">
-        <v>16.2</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -9040,16 +9048,16 @@
         <v>427</v>
       </c>
       <c r="B423" s="22">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C423" s="23">
-        <v>23.5</v>
+        <v>21.5</v>
       </c>
       <c r="D423" s="24">
         <v>2.75</v>
       </c>
       <c r="E423" s="25">
-        <v>64.63</v>
+        <v>59.13</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
@@ -9074,16 +9082,16 @@
         <v>429</v>
       </c>
       <c r="B425" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C425" s="23">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D425" s="24">
         <v>2.8</v>
       </c>
       <c r="E425" s="25">
-        <v>86.8</v>
+        <v>84</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -9091,17 +9099,11 @@
         <v>430</v>
       </c>
       <c r="B426" s="22">
-        <v>42</v>
-      </c>
-      <c r="C426" s="23">
-        <v>2.5</v>
-      </c>
-      <c r="D426" s="24">
-        <v>2.8</v>
-      </c>
-      <c r="E426" s="25">
-        <v>7</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C426" s="26"/>
+      <c r="D426" s="27"/>
+      <c r="E426" s="26"/>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" s="21" t="s">
@@ -9117,16 +9119,16 @@
         <v>432</v>
       </c>
       <c r="B428" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C428" s="23">
-        <v>139.84</v>
+        <v>137.84</v>
       </c>
       <c r="D428" s="24">
         <v>2.8</v>
       </c>
       <c r="E428" s="25">
-        <v>391.55</v>
+        <v>385.95</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -9134,16 +9136,16 @@
         <v>433</v>
       </c>
       <c r="B429" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C429" s="23">
-        <v>10.5</v>
+        <v>9.5</v>
       </c>
       <c r="D429" s="24">
         <v>2.95</v>
       </c>
       <c r="E429" s="25">
-        <v>30.98</v>
+        <v>28.03</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -9236,16 +9238,16 @@
         <v>439</v>
       </c>
       <c r="B435" s="22">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C435" s="23">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D435" s="24">
         <v>3.05</v>
       </c>
       <c r="E435" s="25">
-        <v>85.4</v>
+        <v>76.25</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
@@ -9253,27 +9255,33 @@
         <v>440</v>
       </c>
       <c r="B436" s="22">
-        <v>24</v>
-      </c>
-      <c r="C436" s="26"/>
-      <c r="D436" s="27"/>
-      <c r="E436" s="26"/>
+        <v>23</v>
+      </c>
+      <c r="C436" s="23">
+        <v>7.5</v>
+      </c>
+      <c r="D436" s="24">
+        <v>3.25</v>
+      </c>
+      <c r="E436" s="25">
+        <v>24.38</v>
+      </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" s="21" t="s">
         <v>441</v>
       </c>
       <c r="B437" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C437" s="23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D437" s="24">
         <v>3.5</v>
       </c>
       <c r="E437" s="25">
-        <v>45.5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -9307,16 +9315,16 @@
         <v>444</v>
       </c>
       <c r="B440" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C440" s="23">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="D440" s="24">
         <v>3.4</v>
       </c>
       <c r="E440" s="25">
-        <v>18.7</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
@@ -9393,13 +9401,13 @@
         <v>37</v>
       </c>
       <c r="C445" s="23">
-        <v>12.5</v>
+        <v>11.5</v>
       </c>
       <c r="D445" s="24">
         <v>3.33</v>
       </c>
       <c r="E445" s="25">
-        <v>41.63</v>
+        <v>38.299999999999997</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -9459,16 +9467,16 @@
         <v>454</v>
       </c>
       <c r="B450" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C450" s="23">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="D450" s="24">
         <v>4.25</v>
       </c>
       <c r="E450" s="25">
-        <v>78.63</v>
+        <v>70.13</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
@@ -9493,16 +9501,16 @@
         <v>456</v>
       </c>
       <c r="B452" s="22">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C452" s="23">
-        <v>11</v>
+        <v>7.5</v>
       </c>
       <c r="D452" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E452" s="25">
-        <v>45.66</v>
+        <v>31.13</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
@@ -9510,16 +9518,16 @@
         <v>457</v>
       </c>
       <c r="B453" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C453" s="23">
-        <v>11.5</v>
+        <v>9.5</v>
       </c>
       <c r="D453" s="24">
         <v>4.25</v>
       </c>
       <c r="E453" s="25">
-        <v>48.88</v>
+        <v>40.380000000000003</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
@@ -9691,16 +9699,16 @@
         <v>468</v>
       </c>
       <c r="B464" s="22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C464" s="23">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D464" s="24">
         <v>5.25</v>
       </c>
       <c r="E464" s="25">
-        <v>34.130000000000003</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.25">
@@ -9723,16 +9731,16 @@
         <v>470</v>
       </c>
       <c r="B466" s="22">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C466" s="23">
-        <v>42.5</v>
+        <v>37.5</v>
       </c>
       <c r="D466" s="24">
         <v>5.5</v>
       </c>
       <c r="E466" s="25">
-        <v>233.75</v>
+        <v>206.25</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
@@ -9851,13 +9859,13 @@
         <v>35</v>
       </c>
       <c r="C475" s="23">
-        <v>8.5</v>
+        <v>11</v>
       </c>
       <c r="D475" s="24">
         <v>7.51</v>
       </c>
       <c r="E475" s="25">
-        <v>63.85</v>
+        <v>82.62</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
@@ -9865,16 +9873,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C476" s="23">
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="D476" s="24">
         <v>7.13</v>
       </c>
       <c r="E476" s="25">
-        <v>71.3</v>
+        <v>24.96</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -9899,16 +9907,16 @@
         <v>482</v>
       </c>
       <c r="B478" s="22">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C478" s="23">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="D478" s="24">
         <v>7</v>
       </c>
       <c r="E478" s="25">
-        <v>17.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -9916,16 +9924,16 @@
         <v>483</v>
       </c>
       <c r="B479" s="22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C479" s="23">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D479" s="24">
         <v>7.6</v>
       </c>
       <c r="E479" s="25">
-        <v>41.8</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
@@ -10015,16 +10023,16 @@
         <v>490</v>
       </c>
       <c r="B486" s="22">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C486" s="23">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="D486" s="24">
         <v>4.28</v>
       </c>
       <c r="E486" s="25">
-        <v>14.98</v>
+        <v>4.28</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -10084,13 +10092,13 @@
         <v>46</v>
       </c>
       <c r="C490" s="23">
-        <v>22</v>
+        <v>23.5</v>
       </c>
       <c r="D490" s="24">
         <v>5.7</v>
       </c>
       <c r="E490" s="25">
-        <v>125.4</v>
+        <v>133.94999999999999</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -10126,16 +10134,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C493" s="23">
-        <v>92</v>
+        <v>78.5</v>
       </c>
       <c r="D493" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E493" s="25">
-        <v>101.2</v>
+        <v>86.35</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10143,17 +10151,11 @@
         <v>498</v>
       </c>
       <c r="B494" s="22">
-        <v>109</v>
-      </c>
-      <c r="C494" s="23">
-        <v>3</v>
-      </c>
-      <c r="D494" s="24">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E494" s="25">
-        <v>3.3</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C494" s="26"/>
+      <c r="D494" s="27"/>
+      <c r="E494" s="26"/>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A495" s="21" t="s">
@@ -10177,16 +10179,16 @@
         <v>500</v>
       </c>
       <c r="B496" s="22">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C496" s="23">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D496" s="24">
         <v>1.4</v>
       </c>
       <c r="E496" s="25">
-        <v>75.599999999999994</v>
+        <v>70</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -10307,16 +10309,16 @@
         <v>508</v>
       </c>
       <c r="B504" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C504" s="23">
-        <v>53.5</v>
+        <v>52.5</v>
       </c>
       <c r="D504" s="24">
         <v>1.38</v>
       </c>
       <c r="E504" s="25">
-        <v>73.739999999999995</v>
+        <v>72.36</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
@@ -10341,16 +10343,16 @@
         <v>510</v>
       </c>
       <c r="B506" s="22">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C506" s="23">
-        <v>562.75</v>
+        <v>556.75</v>
       </c>
       <c r="D506" s="24">
         <v>1.5</v>
       </c>
       <c r="E506" s="25">
-        <v>844.13</v>
+        <v>835.13</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
@@ -10375,16 +10377,16 @@
         <v>512</v>
       </c>
       <c r="B508" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C508" s="23">
-        <v>311.5</v>
+        <v>310</v>
       </c>
       <c r="D508" s="24">
         <v>1.5</v>
       </c>
       <c r="E508" s="25">
-        <v>467.25</v>
+        <v>465</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10420,16 +10422,16 @@
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C511" s="23">
-        <v>31.5</v>
+        <v>25.5</v>
       </c>
       <c r="D511" s="24">
         <v>0.92</v>
       </c>
       <c r="E511" s="25">
-        <v>29.11</v>
+        <v>23.57</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10437,16 +10439,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C512" s="23">
-        <v>29.2</v>
+        <v>26.2</v>
       </c>
       <c r="D512" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E512" s="25">
-        <v>66.58</v>
+        <v>59.74</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10454,16 +10456,16 @@
         <v>517</v>
       </c>
       <c r="B513" s="22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C513" s="23">
-        <v>94.5</v>
+        <v>90.5</v>
       </c>
       <c r="D513" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E513" s="25">
-        <v>215.46</v>
+        <v>206.34</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10514,16 +10516,16 @@
         <v>521</v>
       </c>
       <c r="B517" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C517" s="23">
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="D517" s="24">
         <v>2.73</v>
       </c>
       <c r="E517" s="25">
-        <v>47.85</v>
+        <v>45.11</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -10531,16 +10533,16 @@
         <v>522</v>
       </c>
       <c r="B518" s="22">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C518" s="23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D518" s="24">
         <v>2.8</v>
       </c>
       <c r="E518" s="25">
-        <v>19.600000000000001</v>
+        <v>14</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
@@ -10614,16 +10616,16 @@
         <v>527</v>
       </c>
       <c r="B523" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C523" s="23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D523" s="24">
         <v>3.2</v>
       </c>
       <c r="E523" s="25">
-        <v>60.8</v>
+        <v>54.4</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
@@ -10631,16 +10633,16 @@
         <v>528</v>
       </c>
       <c r="B524" s="22">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C524" s="23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D524" s="24">
         <v>3.2</v>
       </c>
       <c r="E524" s="25">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
@@ -10657,16 +10659,16 @@
         <v>530</v>
       </c>
       <c r="B526" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C526" s="23">
-        <v>14.5</v>
+        <v>13.5</v>
       </c>
       <c r="D526" s="24">
         <v>2.85</v>
       </c>
       <c r="E526" s="25">
-        <v>41.33</v>
+        <v>38.479999999999997</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10760,16 +10762,16 @@
         <v>537</v>
       </c>
       <c r="B533" s="22">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C533" s="23">
-        <v>46</v>
+        <v>48.5</v>
       </c>
       <c r="D533" s="24">
         <v>3.33</v>
       </c>
       <c r="E533" s="25">
-        <v>153.18</v>
+        <v>161.51</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -10786,16 +10788,16 @@
         <v>539</v>
       </c>
       <c r="B535" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C535" s="23">
-        <v>25.5</v>
+        <v>23</v>
       </c>
       <c r="D535" s="24">
         <v>3.8</v>
       </c>
       <c r="E535" s="25">
-        <v>96.9</v>
+        <v>87.4</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">
@@ -10823,13 +10825,13 @@
         <v>82</v>
       </c>
       <c r="C537" s="23">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="D537" s="24">
         <v>3.6</v>
       </c>
       <c r="E537" s="25">
-        <v>30.6</v>
+        <v>32.4</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -10923,16 +10925,16 @@
         <v>548</v>
       </c>
       <c r="B544" s="22">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C544" s="23">
-        <v>33</v>
+        <v>19.5</v>
       </c>
       <c r="D544" s="24">
         <v>4</v>
       </c>
       <c r="E544" s="25">
-        <v>132</v>
+        <v>78</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.25">
@@ -10957,16 +10959,16 @@
         <v>550</v>
       </c>
       <c r="B546" s="22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C546" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D546" s="24">
         <v>3.8</v>
       </c>
       <c r="E546" s="25">
-        <v>3.8</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -11008,16 +11010,16 @@
         <v>553</v>
       </c>
       <c r="B549" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C549" s="23">
-        <v>13.5</v>
+        <v>11.5</v>
       </c>
       <c r="D549" s="24">
         <v>4.4000000000000004</v>
       </c>
       <c r="E549" s="25">
-        <v>59.4</v>
+        <v>50.6</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -11042,16 +11044,16 @@
         <v>555</v>
       </c>
       <c r="B551" s="22">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C551" s="23">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="D551" s="24">
         <v>4.75</v>
       </c>
       <c r="E551" s="25">
-        <v>40.380000000000003</v>
+        <v>45.13</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -11059,16 +11061,16 @@
         <v>556</v>
       </c>
       <c r="B552" s="22">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C552" s="23">
-        <v>24</v>
+        <v>15.5</v>
       </c>
       <c r="D552" s="24">
         <v>4.75</v>
       </c>
       <c r="E552" s="25">
-        <v>114</v>
+        <v>73.63</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -11110,16 +11112,16 @@
         <v>559</v>
       </c>
       <c r="B555" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C555" s="23">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D555" s="24">
         <v>4.75</v>
       </c>
       <c r="E555" s="25">
-        <v>66.5</v>
+        <v>52.25</v>
       </c>
     </row>
     <row r="556" spans="1:5" x14ac:dyDescent="0.25">
@@ -11127,16 +11129,16 @@
         <v>560</v>
       </c>
       <c r="B556" s="22">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C556" s="23">
-        <v>3.62</v>
+        <v>5.62</v>
       </c>
       <c r="D556" s="24">
         <v>5</v>
       </c>
       <c r="E556" s="25">
-        <v>18.100000000000001</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
@@ -11246,16 +11248,16 @@
         <v>567</v>
       </c>
       <c r="B563" s="22">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C563" s="23">
-        <v>17</v>
+        <v>20.5</v>
       </c>
       <c r="D563" s="24">
         <v>5.75</v>
       </c>
       <c r="E563" s="25">
-        <v>97.75</v>
+        <v>117.88</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -11263,16 +11265,16 @@
         <v>568</v>
       </c>
       <c r="B564" s="22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C564" s="23">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D564" s="24">
         <v>5.5</v>
       </c>
       <c r="E564" s="25">
-        <v>258.5</v>
+        <v>247.5</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
@@ -11314,16 +11316,16 @@
         <v>571</v>
       </c>
       <c r="B567" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C567" s="23">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D567" s="24">
         <v>6</v>
       </c>
       <c r="E567" s="25">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
@@ -11331,16 +11333,16 @@
         <v>572</v>
       </c>
       <c r="B568" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C568" s="23">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D568" s="24">
         <v>6</v>
       </c>
       <c r="E568" s="25">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
@@ -11391,17 +11393,11 @@
         <v>576</v>
       </c>
       <c r="B572" s="22">
-        <v>13</v>
-      </c>
-      <c r="C572" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="D572" s="24">
-        <v>7</v>
-      </c>
-      <c r="E572" s="25">
-        <v>3.5</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C572" s="26"/>
+      <c r="D572" s="27"/>
+      <c r="E572" s="26"/>
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A573" s="21" t="s">
@@ -11459,7 +11455,7 @@
         <v>580</v>
       </c>
       <c r="B576" s="22">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C576" s="23">
         <v>1</v>
@@ -11513,16 +11509,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C580" s="23">
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="D580" s="24">
         <v>2.76</v>
       </c>
       <c r="E580" s="25">
-        <v>51.08</v>
+        <v>45.56</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11530,16 +11526,16 @@
         <v>585</v>
       </c>
       <c r="B581" s="22">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C581" s="23">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D581" s="24">
         <v>2.76</v>
       </c>
       <c r="E581" s="25">
-        <v>110.4</v>
+        <v>99.36</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
@@ -11547,16 +11543,16 @@
         <v>586</v>
       </c>
       <c r="B582" s="22">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C582" s="23">
-        <v>51.74</v>
+        <v>49.74</v>
       </c>
       <c r="D582" s="24">
         <v>2.76</v>
       </c>
       <c r="E582" s="25">
-        <v>142.80000000000001</v>
+        <v>137.28</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
@@ -11581,16 +11577,16 @@
         <v>588</v>
       </c>
       <c r="B584" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C584" s="23">
-        <v>23.5</v>
+        <v>15.5</v>
       </c>
       <c r="D584" s="24">
         <v>2.88</v>
       </c>
       <c r="E584" s="25">
-        <v>67.75</v>
+        <v>44.69</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
@@ -11632,16 +11628,16 @@
         <v>591</v>
       </c>
       <c r="B587" s="22">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C587" s="23">
-        <v>41</v>
+        <v>38.5</v>
       </c>
       <c r="D587" s="24">
         <v>2.76</v>
       </c>
       <c r="E587" s="25">
-        <v>113.16</v>
+        <v>106.26</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
@@ -11681,16 +11677,16 @@
         <v>594</v>
       </c>
       <c r="B590" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C590" s="23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D590" s="24">
         <v>3</v>
       </c>
       <c r="E590" s="25">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
@@ -11698,16 +11694,16 @@
         <v>595</v>
       </c>
       <c r="B591" s="22">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C591" s="23">
-        <v>17.5</v>
+        <v>13.5</v>
       </c>
       <c r="D591" s="24">
         <v>3.1</v>
       </c>
       <c r="E591" s="25">
-        <v>54.25</v>
+        <v>41.85</v>
       </c>
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
@@ -11766,16 +11762,16 @@
         <v>599</v>
       </c>
       <c r="B595" s="22">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C595" s="23">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D595" s="24">
         <v>4</v>
       </c>
       <c r="E595" s="25">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
@@ -11815,16 +11811,16 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C598" s="23">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D598" s="24">
         <v>4.92</v>
       </c>
       <c r="E598" s="25">
-        <v>39.39</v>
+        <v>64.010000000000005</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11832,16 +11828,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C599" s="23">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D599" s="24">
         <v>1.92</v>
       </c>
       <c r="E599" s="25">
-        <v>203.57</v>
+        <v>197.81</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -11849,16 +11845,16 @@
         <v>604</v>
       </c>
       <c r="B600" s="22">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C600" s="23">
-        <v>383.5</v>
+        <v>379.5</v>
       </c>
       <c r="D600" s="24">
         <v>1.91</v>
       </c>
       <c r="E600" s="25">
-        <v>732.51</v>
+        <v>724.87</v>
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
@@ -11866,16 +11862,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C601" s="23">
-        <v>92.7</v>
+        <v>89.2</v>
       </c>
       <c r="D601" s="24">
         <v>1.93</v>
       </c>
       <c r="E601" s="25">
-        <v>178.88</v>
+        <v>172.12</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -11883,16 +11879,16 @@
         <v>606</v>
       </c>
       <c r="B602" s="22">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C602" s="23">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D602" s="24">
-        <v>2.84</v>
+        <v>2.83</v>
       </c>
       <c r="E602" s="25">
-        <v>187.38</v>
+        <v>226.62</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -11968,16 +11964,16 @@
         <v>611</v>
       </c>
       <c r="B607" s="22">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C607" s="23">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="D607" s="24">
         <v>1.4</v>
       </c>
       <c r="E607" s="25">
-        <v>626.21</v>
+        <v>610.83000000000004</v>
       </c>
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
@@ -12002,16 +11998,16 @@
         <v>613</v>
       </c>
       <c r="B609" s="22">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C609" s="23">
-        <v>-106.5</v>
+        <v>-107.5</v>
       </c>
       <c r="D609" s="24">
         <v>1.4</v>
       </c>
       <c r="E609" s="25">
-        <v>-149.1</v>
+        <v>-150.5</v>
       </c>
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
@@ -12019,10 +12015,10 @@
         <v>614</v>
       </c>
       <c r="B610" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C610" s="23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D610" s="27"/>
       <c r="E610" s="26"/>
@@ -12032,10 +12028,10 @@
         <v>615</v>
       </c>
       <c r="B611" s="22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C611" s="23">
-        <v>40.5</v>
+        <v>38.5</v>
       </c>
       <c r="D611" s="27"/>
       <c r="E611" s="26"/>
@@ -12045,11 +12041,9 @@
         <v>616</v>
       </c>
       <c r="B612" s="22">
-        <v>46</v>
-      </c>
-      <c r="C612" s="23">
-        <v>-1.5</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C612" s="26"/>
       <c r="D612" s="27"/>
       <c r="E612" s="26"/>
     </row>
@@ -12058,10 +12052,10 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C613" s="23">
-        <v>25.8</v>
+        <v>24.8</v>
       </c>
       <c r="D613" s="27"/>
       <c r="E613" s="26"/>
@@ -12110,16 +12104,16 @@
         <v>621</v>
       </c>
       <c r="B617" s="22">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C617" s="23">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="D617" s="24">
         <v>0.83</v>
       </c>
       <c r="E617" s="25">
-        <v>565.95000000000005</v>
+        <v>562.65</v>
       </c>
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
@@ -12127,16 +12121,16 @@
         <v>622</v>
       </c>
       <c r="B618" s="22">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C618" s="23">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="D618" s="24">
         <v>0.8</v>
       </c>
       <c r="E618" s="25">
-        <v>245.6</v>
+        <v>234.4</v>
       </c>
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
@@ -12144,16 +12138,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C619" s="23">
-        <v>535.5</v>
+        <v>529.5</v>
       </c>
       <c r="D619" s="24">
         <v>0.81</v>
       </c>
       <c r="E619" s="25">
-        <v>436.27</v>
+        <v>431.38</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12164,13 +12158,13 @@
         <v>151</v>
       </c>
       <c r="C620" s="23">
-        <v>97.5</v>
+        <v>99.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.81</v>
       </c>
       <c r="E620" s="25">
-        <v>78.7</v>
+        <v>80.31</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12195,16 +12189,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C622" s="23">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>727.48</v>
+        <v>724.88</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12212,16 +12206,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C623" s="23">
-        <v>1527</v>
+        <v>1521</v>
       </c>
       <c r="D623" s="24">
         <v>0.51</v>
       </c>
       <c r="E623" s="25">
-        <v>777.84</v>
+        <v>774.78</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -12229,16 +12223,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C624" s="23">
-        <v>681</v>
+        <v>642</v>
       </c>
       <c r="D624" s="24">
         <v>0.52</v>
       </c>
       <c r="E624" s="25">
-        <v>354.12</v>
+        <v>333.84</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12263,16 +12257,16 @@
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C626" s="23">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="D626" s="24">
         <v>0.52</v>
       </c>
       <c r="E626" s="25">
-        <v>165.36</v>
+        <v>155.47999999999999</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12280,16 +12274,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C627" s="23">
-        <v>540.5</v>
+        <v>543</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>378.35</v>
+        <v>380.1</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12297,16 +12291,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C628" s="23">
-        <v>275.5</v>
+        <v>253.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.7</v>
       </c>
       <c r="E628" s="25">
-        <v>192.85</v>
+        <v>177.45</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12314,16 +12308,16 @@
         <v>633</v>
       </c>
       <c r="B629" s="22">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C629" s="23">
-        <v>149.5</v>
+        <v>131.5</v>
       </c>
       <c r="D629" s="24">
         <v>0.69</v>
       </c>
       <c r="E629" s="25">
-        <v>102.43</v>
+        <v>90.09</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
@@ -12355,16 +12349,16 @@
         <v>636</v>
       </c>
       <c r="B632" s="22">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C632" s="23">
-        <v>955.5</v>
+        <v>918.5</v>
       </c>
       <c r="D632" s="24">
         <v>0.55000000000000004</v>
       </c>
       <c r="E632" s="25">
-        <v>525.79</v>
+        <v>505.43</v>
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
@@ -12450,11 +12444,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>43679.02</v>
+        <v>42938.07</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>79931.38</v>
+        <v>79223.259999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 1:15
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -2753,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="23">
-        <v>15.5</v>
+        <v>13</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C29" s="23">
-        <v>30</v>
+        <v>26.5</v>
       </c>
       <c r="D29" s="24">
         <v>2.58</v>
       </c>
       <c r="E29" s="25">
-        <v>77.42</v>
+        <v>68.39</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3046,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C39" s="23">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>237.6</v>
+        <v>224.1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3131,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C44" s="23">
-        <v>111.5</v>
+        <v>108.5</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>250.88</v>
+        <v>244.13</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3403,16 +3403,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C60" s="23">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>602.29999999999995</v>
+        <v>596.6</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,16 +3420,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C61" s="23">
-        <v>292.5</v>
+        <v>283.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>614.25</v>
+        <v>595.35</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,16 +3544,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C69" s="23">
-        <v>259.5</v>
+        <v>255.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>181.65</v>
+        <v>178.85</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,16 +3561,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C70" s="23">
-        <v>146.5</v>
+        <v>144.5</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>131.85</v>
+        <v>130.05000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,16 +3578,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C71" s="23">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>90.9</v>
+        <v>87.3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,16 +3612,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C73" s="23">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>1756.15</v>
+        <v>1753.05</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,10 +3687,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C78" s="23">
-        <v>396.5</v>
+        <v>393</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3713,10 +3713,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C80" s="23">
-        <v>-66</v>
+        <v>-69</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3739,10 +3739,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C82" s="23">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3786,16 +3786,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C85" s="23">
-        <v>3291</v>
+        <v>3288</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>4607.3999999999996</v>
+        <v>4603.2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3820,16 +3820,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C87" s="23">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1069.5999999999999</v>
+        <v>1061.2</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3846,16 +3846,16 @@
         <v>93</v>
       </c>
       <c r="B89" s="22">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C89" s="23">
-        <v>447.5</v>
+        <v>444.5</v>
       </c>
       <c r="D89" s="24">
         <v>2</v>
       </c>
       <c r="E89" s="25">
-        <v>895</v>
+        <v>889</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,16 +3863,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C90" s="23">
-        <v>892.5</v>
+        <v>889.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1785</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,16 +3897,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C92" s="23">
-        <v>273.5</v>
+        <v>269.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>344.61</v>
+        <v>339.57</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4060,10 +4060,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C103" s="23">
-        <v>-66.5</v>
+        <v>-70.5</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -5026,16 +5026,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C165" s="23">
-        <v>147.5</v>
+        <v>143.5</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>435.13</v>
+        <v>423.33</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5043,16 +5043,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C166" s="23">
-        <v>51.5</v>
+        <v>50.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>151.93</v>
+        <v>148.97999999999999</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5060,17 +5060,11 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>53</v>
-      </c>
-      <c r="C167" s="23">
-        <v>3</v>
-      </c>
-      <c r="D167" s="24">
-        <v>3</v>
-      </c>
-      <c r="E167" s="25">
-        <v>9</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C167" s="26"/>
+      <c r="D167" s="27"/>
+      <c r="E167" s="26"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="21" t="s">
@@ -5277,13 +5271,13 @@
         <v>18</v>
       </c>
       <c r="C181" s="23">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="D181" s="24">
-        <v>3.76</v>
+        <v>3.75</v>
       </c>
       <c r="E181" s="25">
-        <v>1.88</v>
+        <v>-3.75</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5291,16 +5285,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C182" s="23">
-        <v>0.6</v>
+        <v>2.6</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>2.2799999999999998</v>
+        <v>9.8800000000000008</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5308,16 +5302,16 @@
         <v>187</v>
       </c>
       <c r="B183" s="22">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C183" s="23">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D183" s="24">
         <v>3</v>
       </c>
       <c r="E183" s="25">
-        <v>288</v>
+        <v>303</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5421,16 +5415,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C190" s="23">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D190" s="24">
         <v>3.77</v>
       </c>
       <c r="E190" s="25">
-        <v>350.84</v>
+        <v>343.29</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5761,15 +5755,9 @@
       <c r="B214" s="22">
         <v>210</v>
       </c>
-      <c r="C214" s="23">
-        <v>4</v>
-      </c>
-      <c r="D214" s="24">
-        <v>4.12</v>
-      </c>
-      <c r="E214" s="25">
-        <v>16.46</v>
-      </c>
+      <c r="C214" s="26"/>
+      <c r="D214" s="27"/>
+      <c r="E214" s="26"/>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="21" t="s">
@@ -5877,16 +5865,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C222" s="23">
-        <v>-43</v>
+        <v>-45</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>-193.5</v>
+        <v>-202.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5911,16 +5899,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C224" s="23">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>55.13</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6045,16 +6033,16 @@
         <v>236</v>
       </c>
       <c r="B232" s="22">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C232" s="23">
-        <v>-0.7</v>
+        <v>1.3</v>
       </c>
       <c r="D232" s="24">
-        <v>4.76</v>
+        <v>4.75</v>
       </c>
       <c r="E232" s="25">
-        <v>-3.33</v>
+        <v>6.18</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6236,16 +6224,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C245" s="23">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>21.29</v>
+        <v>14.9</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6448,16 +6436,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C259" s="23">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>522.16</v>
+        <v>483.64</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6952,16 +6940,16 @@
         <v>295</v>
       </c>
       <c r="B291" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C291" s="23">
-        <v>11</v>
+        <v>8.5</v>
       </c>
       <c r="D291" s="24">
         <v>6.18</v>
       </c>
       <c r="E291" s="25">
-        <v>67.98</v>
+        <v>52.53</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -9095,16 +9083,16 @@
         <v>432</v>
       </c>
       <c r="B428" s="22">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C428" s="23">
-        <v>137.84</v>
+        <v>136.84</v>
       </c>
       <c r="D428" s="24">
         <v>2.8</v>
       </c>
       <c r="E428" s="25">
-        <v>385.95</v>
+        <v>383.15</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -9849,16 +9837,16 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C476" s="23">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="D476" s="24">
         <v>7.13</v>
       </c>
       <c r="E476" s="25">
-        <v>-21.39</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -10609,11 +10597,17 @@
         <v>528</v>
       </c>
       <c r="B524" s="22">
-        <v>38</v>
-      </c>
-      <c r="C524" s="26"/>
-      <c r="D524" s="27"/>
-      <c r="E524" s="26"/>
+        <v>37</v>
+      </c>
+      <c r="C524" s="23">
+        <v>5</v>
+      </c>
+      <c r="D524" s="24">
+        <v>3.2</v>
+      </c>
+      <c r="E524" s="25">
+        <v>16</v>
+      </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="21" t="s">
@@ -11473,16 +11467,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C580" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D580" s="24">
         <v>2.76</v>
       </c>
       <c r="E580" s="25">
-        <v>27.63</v>
+        <v>24.87</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11826,16 +11820,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C601" s="23">
-        <v>89.2</v>
+        <v>88.2</v>
       </c>
       <c r="D601" s="24">
         <v>1.93</v>
       </c>
       <c r="E601" s="25">
-        <v>172.12</v>
+        <v>170.19</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -11843,16 +11837,16 @@
         <v>606</v>
       </c>
       <c r="B602" s="22">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C602" s="23">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D602" s="24">
         <v>2.83</v>
       </c>
       <c r="E602" s="25">
-        <v>127.48</v>
+        <v>118.98</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
@@ -12238,16 +12232,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C627" s="23">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>380.1</v>
+        <v>377.3</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12408,11 +12402,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>41006.57</v>
+        <v>40905.57</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>73862.22</v>
+        <v>73655.490000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:21
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -77,13 +77,13 @@
     <t>1850 PATRIKA</t>
   </si>
   <si>
-    <t>1851 PATRIKA</t>
+    <t>1851 PATRIKA (AD)</t>
   </si>
   <si>
     <t>1852 PATRIKA</t>
   </si>
   <si>
-    <t>1853 PATRIKA</t>
+    <t>1853 PATRIKA (7.4.25)</t>
   </si>
   <si>
     <t>1854 PATRIKA</t>
@@ -122,7 +122,7 @@
     <t>1865 PATRIKA</t>
   </si>
   <si>
-    <t>1866 PATRIKA</t>
+    <t>1866 PATRIKA (DC)</t>
   </si>
   <si>
     <t>1867 PATRIKA (STCK LOT NO )</t>
@@ -134,7 +134,7 @@
     <t>1869 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>1870 PATRIKA</t>
+    <t>1870 PATRIKA (DC)</t>
   </si>
   <si>
     <t>1871 PATRIKA (DC)</t>
@@ -152,7 +152,7 @@
     <t>1875 PATRIKA</t>
   </si>
   <si>
-    <t>1876 PATRIKA</t>
+    <t>1876 PATRIKA (DC)</t>
   </si>
   <si>
     <t>1877 PATRIKA</t>
@@ -167,7 +167,7 @@
     <t>1880 PATRIKA</t>
   </si>
   <si>
-    <t>1881 PATRIKA</t>
+    <t>1881 PATRIKA (DC)</t>
   </si>
   <si>
     <t>1882 PATRIKA</t>
@@ -227,10 +227,10 @@
     <t>1899 PATRIKA- B</t>
   </si>
   <si>
-    <t>1899  PATRIKA (PEARL 52)</t>
-  </si>
-  <si>
-    <t>1900 PATRIKA</t>
+    <t>1899  PATRIKA (PEARL 52) DC</t>
+  </si>
+  <si>
+    <t>1900 PATRIKA (DC)</t>
   </si>
   <si>
     <t>1901 PATRIKA</t>
@@ -395,7 +395,7 @@
     <t>2027 PATRIKA {L}</t>
   </si>
   <si>
-    <t>2028 PATRIKA {M}</t>
+    <t>2028 PATRIKA {M} (AD)</t>
   </si>
   <si>
     <t>2029 PATRIKA {M}</t>
@@ -545,7 +545,7 @@
     <t>4218 PATRIKA</t>
   </si>
   <si>
-    <t>4219 PATRIKA</t>
+    <t>4219 PATRIKA (AD)</t>
   </si>
   <si>
     <t>4220 PATRIKA</t>
@@ -581,16 +581,16 @@
     <t>4229 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>4230 PATRIKA</t>
-  </si>
-  <si>
-    <t>4231 PATRIKA</t>
+    <t>4230 PATRIKA (AD)</t>
+  </si>
+  <si>
+    <t>4231 PATRIKA (DC)</t>
   </si>
   <si>
     <t>4232 PATRIKA (4170)</t>
   </si>
   <si>
-    <t>4233 PATRIKA (Alter Avlbl Only)</t>
+    <t>4233 PATRIKA (Alter Avlbl Only) DC</t>
   </si>
   <si>
     <t>4234 PATRIKA</t>
@@ -611,7 +611,7 @@
     <t>4239 PATRIKA</t>
   </si>
   <si>
-    <t>4240 PATRIKA</t>
+    <t>4240 PATRIKA (AD)</t>
   </si>
   <si>
     <t>4241 PATRIKA</t>
@@ -632,13 +632,13 @@
     <t>4247 PATRIKA (4232-B)</t>
   </si>
   <si>
-    <t>5000 PATRIKA</t>
-  </si>
-  <si>
     <t>5000 PATRIKA- B (DC)</t>
   </si>
   <si>
-    <t>5001 PATRIKA</t>
+    <t>5000 PATRIKA (DC)</t>
+  </si>
+  <si>
+    <t>5001 PATRIKA (Ane Wala Hai )</t>
   </si>
   <si>
     <t>5002 PATRIKA (Dc)</t>
@@ -677,7 +677,7 @@
     <t>5011 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5012 PATRIKA</t>
+    <t>5012 PATRIKA 7.4.2025</t>
   </si>
   <si>
     <t>5013 PATRIKA</t>
@@ -695,7 +695,7 @@
     <t>5017 PATRIKA</t>
   </si>
   <si>
-    <t>5018 PATRIKA</t>
+    <t>5018 PATRIKA (AD)</t>
   </si>
   <si>
     <t>5019 PATRIKA (DC) {{10}}</t>
@@ -710,7 +710,7 @@
     <t>5021 PATRIKA</t>
   </si>
   <si>
-    <t>5022 PATRIKA</t>
+    <t>5022 PATRIKA(6.4.25)</t>
   </si>
   <si>
     <t>5023 PATRIKA</t>
@@ -734,7 +734,7 @@
     <t>5029 PATRIKA</t>
   </si>
   <si>
-    <t>5030 PATRIKA</t>
+    <t>5030 PATRIKA (AD)</t>
   </si>
   <si>
     <t>5031 PATRIKA</t>
@@ -746,7 +746,7 @@
     <t>5033 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5034 PATRIKA (Direct)</t>
+    <t>5034 PATRIKA (Direct) (Ane Wala)</t>
   </si>
   <si>
     <t>5035 PATRIKA</t>
@@ -767,7 +767,7 @@
     <t>5038 PATRIKA - B</t>
   </si>
   <si>
-    <t>5039 PATRIKA</t>
+    <t>5039 PATRIKA (Ane Wala Hai)</t>
   </si>
   <si>
     <t>5040 PATRIKA (GRAPH AAYEGA)</t>
@@ -782,7 +782,7 @@
     <t>5042 PATRIKA - B (DC)</t>
   </si>
   <si>
-    <t>5043 PATRIKA</t>
+    <t>5043 PATRIKA (DC)</t>
   </si>
   <si>
     <t>5044 PATRIKA (Dc)</t>
@@ -794,7 +794,7 @@
     <t>5046 PATRIKA</t>
   </si>
   <si>
-    <t>5047 PATRIKA (5022-B)</t>
+    <t>5047 PATRIKA (5022-B) (DC)</t>
   </si>
   <si>
     <t>5850 PATRIKA (माल छापने से पहले चेक करे )</t>
@@ -830,12 +830,12 @@
     <t>5860 PATRIKA</t>
   </si>
   <si>
-    <t>5861 PATRIKA</t>
-  </si>
-  <si>
     <t>5861 PATRIKA - B</t>
   </si>
   <si>
+    <t>5861 PATRIKA (DC)</t>
+  </si>
+  <si>
     <t>5862 PATRIKA (GGN)</t>
   </si>
   <si>
@@ -872,7 +872,7 @@
     <t>5873 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5874 PATRIKA</t>
+    <t>5874 PATRIKA (7.4.25) Design Change</t>
   </si>
   <si>
     <t>5875 PATRIKA {M}</t>
@@ -902,7 +902,7 @@
     <t>5883 PATRIKA - B (DESIGN CHNG)</t>
   </si>
   <si>
-    <t>5883 PATRIKA {M}</t>
+    <t>5883 PATRIKA {M} (Ad)</t>
   </si>
   <si>
     <t>5884 PATRIKA (DC)</t>
@@ -947,7 +947,7 @@
     <t>5897 PATRIKA (DC)</t>
   </si>
   <si>
-    <t>5898 PATRIKA {M}</t>
+    <t>5898 PATRIKA {M} (AD)</t>
   </si>
   <si>
     <t>5899 PATRIKA</t>
@@ -974,10 +974,10 @@
     <t>5906 PATRIKA (Dc)</t>
   </si>
   <si>
-    <t>5907 PATRIKA {M}</t>
-  </si>
-  <si>
-    <t>5908 PATRIKA</t>
+    <t>5907 PATRIKA {M} (DC)</t>
+  </si>
+  <si>
+    <t>5908 PATRIKA (AD)</t>
   </si>
   <si>
     <t>5909 PATRIKA {M}</t>
@@ -989,7 +989,7 @@
     <t>5911 PATRIKA (Dc)</t>
   </si>
   <si>
-    <t>5912 PATRIKA</t>
+    <t>5912 PATRIKA (AD)</t>
   </si>
   <si>
     <t>5913 PATRIKA</t>
@@ -1013,7 +1013,7 @@
     <t>5919 PATRIKA {M}</t>
   </si>
   <si>
-    <t>5920 PATRIKA {M}</t>
+    <t>5920 PATRIKA {M} AD</t>
   </si>
   <si>
     <t>5921 PATRIKA (GGN) {M}</t>
@@ -1052,7 +1052,7 @@
     <t>5932 PATRIKA (GGN) {M}</t>
   </si>
   <si>
-    <t>5933 PATRIKA (GGN) {M} (DC)</t>
+    <t>5933 PATRIKA (GGN) {M} (AD)</t>
   </si>
   <si>
     <t>5934 PATRIKA (DC) {{10}}</t>
@@ -1151,16 +1151,16 @@
     <t>6517 PATRIKA {M} (Dc)</t>
   </si>
   <si>
-    <t>6518 PATRIKA {M}</t>
+    <t>6518 PATRIKA {M} (AD)</t>
   </si>
   <si>
     <t>6519 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6520 PATRIKA {M}</t>
-  </si>
-  <si>
-    <t>6521 PATRIKA (GGN) {M}</t>
+    <t>6520 PATRIKA {M} (DC)</t>
+  </si>
+  <si>
+    <t>6521 PATRIKA (GGN) {M} (AD)</t>
   </si>
   <si>
     <t>6522 PATRIKA</t>
@@ -1187,7 +1187,7 @@
     <t>6529 PATRIKA</t>
   </si>
   <si>
-    <t>6530 PATRIKA {M}</t>
+    <t>6530 PATRIKA {M} (DC)</t>
   </si>
   <si>
     <t>6531 PATRIKA {M}</t>
@@ -1238,7 +1238,7 @@
     <t>6546 PATRIKA {M}</t>
   </si>
   <si>
-    <t>6547 PATRIKA {M}</t>
+    <t>6547 PATRIKA {M} (AD)</t>
   </si>
   <si>
     <t>6548 PATRIKA {M} (Dc)</t>
@@ -1253,10 +1253,10 @@
     <t>6551 PATRIKA</t>
   </si>
   <si>
-    <t>7250 PATRIKA</t>
-  </si>
-  <si>
-    <t>7251 PATRIKA</t>
+    <t>7250 PATRIKA(AD)</t>
+  </si>
+  <si>
+    <t>7251 PATRIKA (AD)</t>
   </si>
   <si>
     <t>7252 PATRIKA</t>
@@ -1298,7 +1298,7 @@
     <t>7263 PATRIKA</t>
   </si>
   <si>
-    <t>7264 PATRIKA</t>
+    <t>7264 PATRIKA (AD)</t>
   </si>
   <si>
     <t>7265 PATRIKA</t>
@@ -1316,7 +1316,7 @@
     <t>7269 PATRIKA</t>
   </si>
   <si>
-    <t>7270 PATRIKA</t>
+    <t>7270 PATRIKA (AD)</t>
   </si>
   <si>
     <t>7271 PATRIKA (DC)</t>
@@ -1466,7 +1466,7 @@
     <t>7320 PATRIKA (F/G}</t>
   </si>
   <si>
-    <t>7321 PATRIKA {F/G}</t>
+    <t>7321 PATRIKA {F/G} (AD)</t>
   </si>
   <si>
     <t>7322 PATRIKA (GGN) {M}</t>
@@ -1490,7 +1490,7 @@
     <t>7328 PATRIKA - B (DC)</t>
   </si>
   <si>
-    <t>7328 PATRIKA {M}</t>
+    <t>7328 PATRIKA {M} (AD)</t>
   </si>
   <si>
     <t>7329 PATRIKA</t>
@@ -1499,7 +1499,7 @@
     <t>7330 PATRIKA</t>
   </si>
   <si>
-    <t>7331 PATRIKA {F/G}</t>
+    <t>7331 PATRIKA {F/G} (6.4.25)</t>
   </si>
   <si>
     <t>7332 PATRIKA</t>
@@ -1535,13 +1535,13 @@
     <t>7345 PATRIKA</t>
   </si>
   <si>
-    <t>7346 PATRIKA</t>
+    <t>7346 PATRIKA (AD)</t>
   </si>
   <si>
     <t>7348 PATRIKA (7279-B)</t>
   </si>
   <si>
-    <t>7349 PATRIKA (S.S.60)</t>
+    <t>7349 PATRIKA (S.S.60) (AD)</t>
   </si>
   <si>
     <t>7350 PATRIKA (S.S.61)</t>
@@ -1580,7 +1580,7 @@
     <t>9006 CARD</t>
   </si>
   <si>
-    <t>9008 CARD</t>
+    <t>9008 CARD (DC)</t>
   </si>
   <si>
     <t>9009 CARD</t>
@@ -1610,7 +1610,7 @@
     <t>9017 CARD</t>
   </si>
   <si>
-    <t>9018 CARD</t>
+    <t>9018 CARD (DC)</t>
   </si>
   <si>
     <t>9019 CARD (Dc)</t>
@@ -1676,7 +1676,7 @@
     <t>9039 CARD</t>
   </si>
   <si>
-    <t>9040 CARD</t>
+    <t>9040 CARD (AD)</t>
   </si>
   <si>
     <t>9041 CARD</t>
@@ -1754,7 +1754,7 @@
     <t>9065 CARD</t>
   </si>
   <si>
-    <t>9066 CARD</t>
+    <t>9066 CARD (AD)</t>
   </si>
   <si>
     <t>9067 CARD</t>
@@ -1769,7 +1769,7 @@
     <t>9070 CARD (Dc)</t>
   </si>
   <si>
-    <t>9071 CARD</t>
+    <t>9071 CARD (AD)</t>
   </si>
   <si>
     <t>9072 CARD</t>
@@ -1853,7 +1853,7 @@
     <t>9098 CARD {M}</t>
   </si>
   <si>
-    <t>9099 CARD</t>
+    <t>9099 CARD (AD)</t>
   </si>
   <si>
     <t>9100 CARD</t>
@@ -1874,7 +1874,7 @@
     <t>9105 CARD</t>
   </si>
   <si>
-    <t>9106 CARD</t>
+    <t>9106 CARD (DC)</t>
   </si>
   <si>
     <t>9107 CARD</t>
@@ -1931,7 +1931,7 @@
     <t>9211 CARD (NEW)</t>
   </si>
   <si>
-    <t>9212 CARDS (NEW)</t>
+    <t>9212 CARDS (NEW) (Dc)</t>
   </si>
   <si>
     <t>9*5 OFFSET CARD (9204)</t>
@@ -2612,16 +2612,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C11" s="23">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>311.41000000000003</v>
+        <v>305.95999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,16 +2646,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="23">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="24">
         <v>1.65</v>
       </c>
       <c r="E13" s="25">
-        <v>7.43</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2691,16 +2691,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="23">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" s="24">
         <v>1.8</v>
       </c>
       <c r="E16" s="25">
-        <v>21.6</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2708,16 +2708,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C17" s="23">
-        <v>41.5</v>
+        <v>39</v>
       </c>
       <c r="D17" s="24">
         <v>2</v>
       </c>
       <c r="E17" s="25">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2736,16 +2736,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="22">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="23">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="24">
         <v>2</v>
       </c>
       <c r="E19" s="25">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2753,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C20" s="23">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2838,16 +2838,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="23">
-        <v>54</v>
+        <v>52.5</v>
       </c>
       <c r="D25" s="24">
         <v>2.1</v>
       </c>
       <c r="E25" s="25">
-        <v>113.4</v>
+        <v>110.25</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,16 +2864,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="22">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C27" s="23">
-        <v>25.5</v>
+        <v>20.5</v>
       </c>
       <c r="D27" s="24">
         <v>2.35</v>
       </c>
       <c r="E27" s="25">
-        <v>59.93</v>
+        <v>48.18</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="22">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C29" s="23">
-        <v>26.5</v>
+        <v>20.5</v>
       </c>
       <c r="D29" s="24">
         <v>2.58</v>
       </c>
       <c r="E29" s="25">
-        <v>68.39</v>
+        <v>52.9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2995,16 +2995,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36" s="23">
-        <v>45.5</v>
+        <v>44</v>
       </c>
       <c r="D36" s="24">
         <v>2.6</v>
       </c>
       <c r="E36" s="25">
-        <v>118.3</v>
+        <v>114.4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3012,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C37" s="23">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>169</v>
+        <v>161.19999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,16 +3097,16 @@
         <v>46</v>
       </c>
       <c r="B42" s="22">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C42" s="23">
-        <v>-2</v>
+        <v>-3.5</v>
       </c>
       <c r="D42" s="24">
         <v>2.85</v>
       </c>
       <c r="E42" s="25">
-        <v>-5.7</v>
+        <v>-9.98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,16 +3131,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="22">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" s="23">
-        <v>108.5</v>
+        <v>105</v>
       </c>
       <c r="D44" s="24">
         <v>2.25</v>
       </c>
       <c r="E44" s="25">
-        <v>244.13</v>
+        <v>236.25</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C49" s="23">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="D49" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>377.71</v>
+        <v>367.68</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,16 +3233,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C50" s="23">
-        <v>381</v>
+        <v>362</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>425.77</v>
+        <v>404.54</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3270,13 +3270,13 @@
         <v>255</v>
       </c>
       <c r="C52" s="23">
-        <v>91.5</v>
+        <v>97.5</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>102.23</v>
+        <v>108.94</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3301,16 +3301,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="C54" s="23">
-        <v>589</v>
+        <v>578.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>658.38</v>
+        <v>646.64</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3318,16 +3318,16 @@
         <v>59</v>
       </c>
       <c r="B55" s="22">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C55" s="23">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D55" s="24">
         <v>1.1100000000000001</v>
       </c>
       <c r="E55" s="25">
-        <v>113.21</v>
+        <v>110.99</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,16 +3352,16 @@
         <v>61</v>
       </c>
       <c r="B57" s="22">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C57" s="23">
-        <v>149.5</v>
+        <v>149</v>
       </c>
       <c r="D57" s="24">
         <v>1.9</v>
       </c>
       <c r="E57" s="25">
-        <v>284.05</v>
+        <v>283.10000000000002</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3403,16 +3403,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C60" s="23">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>596.6</v>
+        <v>592.79999999999995</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3420,16 +3420,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C61" s="23">
-        <v>283.5</v>
+        <v>279.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>595.35</v>
+        <v>586.95000000000005</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3476,16 +3476,16 @@
         <v>69</v>
       </c>
       <c r="B65" s="22">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C65" s="23">
-        <v>252.5</v>
+        <v>237.5</v>
       </c>
       <c r="D65" s="24">
         <v>2.1</v>
       </c>
       <c r="E65" s="25">
-        <v>530.25</v>
+        <v>498.75</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3510,16 +3510,16 @@
         <v>71</v>
       </c>
       <c r="B67" s="22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C67" s="23">
-        <v>50</v>
+        <v>48.5</v>
       </c>
       <c r="D67" s="24">
         <v>0.52</v>
       </c>
       <c r="E67" s="25">
-        <v>26</v>
+        <v>25.22</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3527,16 +3527,16 @@
         <v>72</v>
       </c>
       <c r="B68" s="22">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C68" s="23">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D68" s="24">
         <v>0.7</v>
       </c>
       <c r="E68" s="25">
-        <v>18.899999999999999</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,16 +3544,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C69" s="23">
-        <v>255.5</v>
+        <v>252.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>178.85</v>
+        <v>176.75</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3561,16 +3561,16 @@
         <v>74</v>
       </c>
       <c r="B70" s="22">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C70" s="23">
-        <v>144.5</v>
+        <v>132.5</v>
       </c>
       <c r="D70" s="24">
         <v>0.9</v>
       </c>
       <c r="E70" s="25">
-        <v>130.05000000000001</v>
+        <v>119.25</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,16 +3578,16 @@
         <v>75</v>
       </c>
       <c r="B71" s="22">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C71" s="23">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="D71" s="24">
         <v>0.9</v>
       </c>
       <c r="E71" s="25">
-        <v>87.3</v>
+        <v>66.599999999999994</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,16 +3595,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C72" s="23">
-        <v>1608.5</v>
+        <v>1598.5</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>2493.1799999999998</v>
+        <v>2477.6799999999998</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3612,16 +3612,16 @@
         <v>77</v>
       </c>
       <c r="B73" s="22">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C73" s="23">
-        <v>1131</v>
+        <v>1119</v>
       </c>
       <c r="D73" s="24">
         <v>1.55</v>
       </c>
       <c r="E73" s="25">
-        <v>1753.05</v>
+        <v>1734.45</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3629,16 +3629,16 @@
         <v>78</v>
       </c>
       <c r="B74" s="22">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C74" s="23">
-        <v>964</v>
+        <v>962.5</v>
       </c>
       <c r="D74" s="24">
         <v>1.55</v>
       </c>
       <c r="E74" s="25">
-        <v>1494.2</v>
+        <v>1491.88</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3657,16 +3657,16 @@
         <v>80</v>
       </c>
       <c r="B76" s="22">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C76" s="23">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D76" s="24">
         <v>0.32</v>
       </c>
       <c r="E76" s="25">
-        <v>51.37</v>
+        <v>49.44</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,10 +3687,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C78" s="23">
-        <v>393</v>
+        <v>378</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3713,10 +3713,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C80" s="23">
-        <v>-69</v>
+        <v>-74.5</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3739,10 +3739,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C82" s="23">
-        <v>238</v>
+        <v>221.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3752,16 +3752,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="C83" s="23">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>96.6</v>
+        <v>43.7</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3769,16 +3769,16 @@
         <v>88</v>
       </c>
       <c r="B84" s="22">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C84" s="23">
-        <v>371.5</v>
+        <v>361.5</v>
       </c>
       <c r="D84" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E84" s="25">
-        <v>427.23</v>
+        <v>415.73</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3786,16 +3786,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C85" s="23">
-        <v>3288</v>
+        <v>3263</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>4603.2</v>
+        <v>4568.2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3803,16 +3803,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C86" s="23">
-        <v>2335.5</v>
+        <v>2316</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>3269.7</v>
+        <v>3242.4</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3820,16 +3820,16 @@
         <v>91</v>
       </c>
       <c r="B87" s="22">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C87" s="23">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D87" s="24">
         <v>1.4</v>
       </c>
       <c r="E87" s="25">
-        <v>1061.2</v>
+        <v>1059.8</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,16 +3863,16 @@
         <v>94</v>
       </c>
       <c r="B90" s="22">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C90" s="23">
-        <v>889.5</v>
+        <v>884.5</v>
       </c>
       <c r="D90" s="24">
         <v>2</v>
       </c>
       <c r="E90" s="25">
-        <v>1779</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,16 +3897,16 @@
         <v>96</v>
       </c>
       <c r="B92" s="22">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C92" s="23">
-        <v>269.5</v>
+        <v>265.5</v>
       </c>
       <c r="D92" s="24">
         <v>1.26</v>
       </c>
       <c r="E92" s="25">
-        <v>339.57</v>
+        <v>334.53</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4060,10 +4060,10 @@
         <v>107</v>
       </c>
       <c r="B103" s="22">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C103" s="23">
-        <v>-70.5</v>
+        <v>-85.5</v>
       </c>
       <c r="D103" s="27"/>
       <c r="E103" s="26"/>
@@ -4086,10 +4086,10 @@
         <v>109</v>
       </c>
       <c r="B105" s="22">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C105" s="23">
-        <v>129.5</v>
+        <v>126.5</v>
       </c>
       <c r="D105" s="27"/>
       <c r="E105" s="26"/>
@@ -4202,16 +4202,16 @@
         <v>117</v>
       </c>
       <c r="B113" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C113" s="23">
-        <v>16</v>
+        <v>12.5</v>
       </c>
       <c r="D113" s="24">
         <v>12.5</v>
       </c>
       <c r="E113" s="25">
-        <v>200</v>
+        <v>156.25</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,16 +4219,16 @@
         <v>118</v>
       </c>
       <c r="B114" s="22">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C114" s="23">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="D114" s="24">
         <v>12.5</v>
       </c>
       <c r="E114" s="25">
-        <v>-25</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4851,16 +4851,16 @@
         <v>158</v>
       </c>
       <c r="B154" s="22">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C154" s="23">
-        <v>35.85</v>
+        <v>20.85</v>
       </c>
       <c r="D154" s="24">
         <v>2.75</v>
       </c>
       <c r="E154" s="25">
-        <v>98.59</v>
+        <v>57.34</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4879,16 +4879,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C156" s="23">
-        <v>83.85</v>
+        <v>75.849999999999994</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>285.08999999999997</v>
+        <v>257.89</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -4907,16 +4907,16 @@
         <v>162</v>
       </c>
       <c r="B158" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C158" s="23">
-        <v>92.5</v>
+        <v>82.5</v>
       </c>
       <c r="D158" s="24">
         <v>2.7</v>
       </c>
       <c r="E158" s="25">
-        <v>249.75</v>
+        <v>222.75</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -4924,16 +4924,16 @@
         <v>163</v>
       </c>
       <c r="B159" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C159" s="23">
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="D159" s="24">
         <v>2.8</v>
       </c>
       <c r="E159" s="25">
-        <v>29.4</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -4992,16 +4992,16 @@
         <v>167</v>
       </c>
       <c r="B163" s="22">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C163" s="23">
-        <v>46.5</v>
+        <v>34.5</v>
       </c>
       <c r="D163" s="24">
         <v>2.8</v>
       </c>
       <c r="E163" s="25">
-        <v>130.19999999999999</v>
+        <v>96.6</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5026,16 +5026,16 @@
         <v>169</v>
       </c>
       <c r="B165" s="22">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C165" s="23">
-        <v>143.5</v>
+        <v>137</v>
       </c>
       <c r="D165" s="24">
         <v>2.95</v>
       </c>
       <c r="E165" s="25">
-        <v>423.33</v>
+        <v>404.15</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5043,16 +5043,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C166" s="23">
-        <v>50.5</v>
+        <v>49</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>148.97999999999999</v>
+        <v>144.55000000000001</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5071,16 +5071,16 @@
         <v>172</v>
       </c>
       <c r="B168" s="22">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C168" s="23">
-        <v>35.5</v>
+        <v>31.5</v>
       </c>
       <c r="D168" s="24">
         <v>3.4</v>
       </c>
       <c r="E168" s="25">
-        <v>120.87</v>
+        <v>107.25</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5105,16 +5105,16 @@
         <v>174</v>
       </c>
       <c r="B170" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C170" s="23">
-        <v>58.5</v>
+        <v>56.5</v>
       </c>
       <c r="D170" s="24">
         <v>3.3</v>
       </c>
       <c r="E170" s="25">
-        <v>193.05</v>
+        <v>186.45</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5285,16 +5285,16 @@
         <v>186</v>
       </c>
       <c r="B182" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C182" s="23">
-        <v>2.6</v>
+        <v>0.1</v>
       </c>
       <c r="D182" s="24">
         <v>3.8</v>
       </c>
       <c r="E182" s="25">
-        <v>9.8800000000000008</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5432,16 +5432,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C191" s="23">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="D191" s="24">
-        <v>3.97</v>
+        <v>3.96</v>
       </c>
       <c r="E191" s="25">
-        <v>31.72</v>
+        <v>25.77</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5449,16 +5449,16 @@
         <v>196</v>
       </c>
       <c r="B192" s="22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C192" s="23">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D192" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E192" s="25">
-        <v>269.75</v>
+        <v>232.4</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5466,16 +5466,16 @@
         <v>197</v>
       </c>
       <c r="B193" s="22">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C193" s="23">
-        <v>15.5</v>
+        <v>10</v>
       </c>
       <c r="D193" s="24">
         <v>3</v>
       </c>
       <c r="E193" s="25">
-        <v>46.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5550,9 +5550,7 @@
       <c r="A198" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="B198" s="22">
-        <v>2</v>
-      </c>
+      <c r="B198" s="22"/>
       <c r="C198" s="26"/>
       <c r="D198" s="27"/>
       <c r="E198" s="26"/>
@@ -5561,7 +5559,9 @@
       <c r="A199" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="B199" s="22"/>
+      <c r="B199" s="22">
+        <v>2</v>
+      </c>
       <c r="C199" s="26"/>
       <c r="D199" s="27"/>
       <c r="E199" s="26"/>
@@ -5571,16 +5571,16 @@
         <v>204</v>
       </c>
       <c r="B200" s="22">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C200" s="23">
-        <v>-0.51</v>
+        <v>-5.51</v>
       </c>
       <c r="D200" s="24">
-        <v>3.08</v>
+        <v>3.07</v>
       </c>
       <c r="E200" s="25">
-        <v>-1.57</v>
+        <v>-16.93</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5686,16 +5686,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C209" s="23">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>72.2</v>
+        <v>60.8</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5742,22 +5742,34 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>100</v>
-      </c>
-      <c r="C213" s="26"/>
-      <c r="D213" s="27"/>
-      <c r="E213" s="26"/>
+        <v>101</v>
+      </c>
+      <c r="C213" s="23">
+        <v>-5</v>
+      </c>
+      <c r="D213" s="24">
+        <v>4.12</v>
+      </c>
+      <c r="E213" s="25">
+        <v>-20.58</v>
+      </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" s="21" t="s">
         <v>218</v>
       </c>
       <c r="B214" s="22">
-        <v>210</v>
-      </c>
-      <c r="C214" s="26"/>
-      <c r="D214" s="27"/>
-      <c r="E214" s="26"/>
+        <v>211</v>
+      </c>
+      <c r="C214" s="23">
+        <v>-5</v>
+      </c>
+      <c r="D214" s="24">
+        <v>4.12</v>
+      </c>
+      <c r="E214" s="25">
+        <v>-20.58</v>
+      </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" s="21" t="s">
@@ -5865,16 +5877,16 @@
         <v>226</v>
       </c>
       <c r="B222" s="22">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C222" s="23">
-        <v>-45</v>
+        <v>-47</v>
       </c>
       <c r="D222" s="24">
         <v>4.5</v>
       </c>
       <c r="E222" s="25">
-        <v>-202.5</v>
+        <v>-211.5</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -5882,16 +5894,16 @@
         <v>227</v>
       </c>
       <c r="B223" s="22">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C223" s="23">
-        <v>24</v>
+        <v>16.5</v>
       </c>
       <c r="D223" s="24">
         <v>4.5</v>
       </c>
       <c r="E223" s="25">
-        <v>108</v>
+        <v>74.25</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -5899,16 +5911,16 @@
         <v>228</v>
       </c>
       <c r="B224" s="22">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C224" s="23">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D224" s="24">
         <v>5.25</v>
       </c>
       <c r="E224" s="25">
-        <v>13.13</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -5933,16 +5945,16 @@
         <v>230</v>
       </c>
       <c r="B226" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C226" s="23">
-        <v>10.5</v>
+        <v>0.5</v>
       </c>
       <c r="D226" s="24">
         <v>4.8</v>
       </c>
       <c r="E226" s="25">
-        <v>50.4</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -5999,16 +6011,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C230" s="23">
-        <v>23.5</v>
+        <v>10.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>123.38</v>
+        <v>55.13</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6016,16 +6028,16 @@
         <v>235</v>
       </c>
       <c r="B231" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C231" s="23">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D231" s="24">
         <v>5.25</v>
       </c>
       <c r="E231" s="25">
-        <v>336</v>
+        <v>330.75</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6207,16 +6219,16 @@
         <v>248</v>
       </c>
       <c r="B244" s="22">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C244" s="23">
-        <v>27.41</v>
+        <v>21.41</v>
       </c>
       <c r="D244" s="24">
         <v>5.99</v>
       </c>
       <c r="E244" s="25">
-        <v>164.05</v>
+        <v>128.13999999999999</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6224,16 +6236,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C245" s="23">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="D245" s="24">
         <v>4.26</v>
       </c>
       <c r="E245" s="25">
-        <v>14.9</v>
+        <v>21.29</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6241,16 +6253,16 @@
         <v>250</v>
       </c>
       <c r="B246" s="22">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C246" s="23">
-        <v>-2</v>
+        <v>0.5</v>
       </c>
       <c r="D246" s="24">
         <v>4</v>
       </c>
       <c r="E246" s="25">
-        <v>-8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6258,16 +6270,16 @@
         <v>251</v>
       </c>
       <c r="B247" s="22">
+        <v>2</v>
+      </c>
+      <c r="C247" s="23">
         <v>1</v>
-      </c>
-      <c r="C247" s="23">
-        <v>2.5</v>
       </c>
       <c r="D247" s="24">
         <v>4</v>
       </c>
       <c r="E247" s="25">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6348,16 +6360,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C253" s="23">
-        <v>37</v>
+        <v>34.5</v>
       </c>
       <c r="D253" s="24">
         <v>3.5</v>
       </c>
       <c r="E253" s="25">
-        <v>129.5</v>
+        <v>120.75</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6376,16 +6388,16 @@
         <v>259</v>
       </c>
       <c r="B255" s="22">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C255" s="23">
-        <v>46.5</v>
+        <v>45.5</v>
       </c>
       <c r="D255" s="24">
         <v>4.25</v>
       </c>
       <c r="E255" s="25">
-        <v>197.63</v>
+        <v>193.38</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6402,16 +6414,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C257" s="23">
-        <v>8.5</v>
+        <v>1</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>35.53</v>
+        <v>4.18</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6419,16 +6431,16 @@
         <v>262</v>
       </c>
       <c r="B258" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C258" s="23">
-        <v>25.5</v>
+        <v>23.5</v>
       </c>
       <c r="D258" s="24">
         <v>4.18</v>
       </c>
       <c r="E258" s="25">
-        <v>106.59</v>
+        <v>98.23</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6436,16 +6448,16 @@
         <v>263</v>
       </c>
       <c r="B259" s="22">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C259" s="23">
-        <v>113</v>
+        <v>110.5</v>
       </c>
       <c r="D259" s="24">
         <v>4.28</v>
       </c>
       <c r="E259" s="25">
-        <v>483.64</v>
+        <v>472.94</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6453,16 +6465,16 @@
         <v>264</v>
       </c>
       <c r="B260" s="22">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C260" s="23">
-        <v>55.5</v>
+        <v>51.5</v>
       </c>
       <c r="D260" s="24">
         <v>4.28</v>
       </c>
       <c r="E260" s="25">
-        <v>237.54</v>
+        <v>220.42</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6504,48 +6516,48 @@
         <v>267</v>
       </c>
       <c r="B263" s="22">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C263" s="23">
-        <v>16.8</v>
+        <v>12.3</v>
       </c>
       <c r="D263" s="24">
         <v>4.95</v>
       </c>
       <c r="E263" s="25">
-        <v>83.16</v>
+        <v>60.89</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="B264" s="22">
-        <v>15</v>
-      </c>
+      <c r="B264" s="22"/>
       <c r="C264" s="23">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D264" s="24">
-        <v>4.76</v>
+        <v>4.75</v>
       </c>
       <c r="E264" s="25">
-        <v>2.38</v>
+        <v>47.5</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="B265" s="22"/>
+      <c r="B265" s="22">
+        <v>15</v>
+      </c>
       <c r="C265" s="23">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="D265" s="24">
-        <v>4.75</v>
+        <v>4.76</v>
       </c>
       <c r="E265" s="25">
-        <v>47.5</v>
+        <v>2.38</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6553,16 +6565,16 @@
         <v>270</v>
       </c>
       <c r="B266" s="22">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C266" s="23">
-        <v>4.0999999999999996</v>
+        <v>-0.9</v>
       </c>
       <c r="D266" s="24">
         <v>5</v>
       </c>
       <c r="E266" s="25">
-        <v>20.5</v>
+        <v>-4.5</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6588,16 +6600,16 @@
         <v>273</v>
       </c>
       <c r="B269" s="22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C269" s="23">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D269" s="24">
         <v>5.0999999999999996</v>
       </c>
       <c r="E269" s="25">
-        <v>107.1</v>
+        <v>81.599999999999994</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6863,16 +6875,16 @@
         <v>290</v>
       </c>
       <c r="B286" s="22">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C286" s="23">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
       <c r="D286" s="24">
         <v>5.94</v>
       </c>
       <c r="E286" s="25">
-        <v>204.93</v>
+        <v>193.05</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -7071,16 +7083,16 @@
         <v>304</v>
       </c>
       <c r="B300" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C300" s="23">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D300" s="24">
         <v>6.65</v>
       </c>
       <c r="E300" s="25">
-        <v>239.4</v>
+        <v>226.1</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -7125,16 +7137,16 @@
         <v>308</v>
       </c>
       <c r="B304" s="22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C304" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D304" s="24">
         <v>7.13</v>
       </c>
       <c r="E304" s="25">
-        <v>21.39</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -7176,16 +7188,16 @@
         <v>311</v>
       </c>
       <c r="B307" s="22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C307" s="23">
-        <v>13</v>
+        <v>11.5</v>
       </c>
       <c r="D307" s="24">
         <v>6.65</v>
       </c>
       <c r="E307" s="25">
-        <v>86.45</v>
+        <v>76.48</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -7326,15 +7338,17 @@
       <c r="A318" s="21" t="s">
         <v>322</v>
       </c>
-      <c r="B318" s="22"/>
+      <c r="B318" s="22">
+        <v>1</v>
+      </c>
       <c r="C318" s="23">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="D318" s="24">
         <v>9</v>
       </c>
       <c r="E318" s="25">
-        <v>90</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
@@ -8352,11 +8366,17 @@
         <v>385</v>
       </c>
       <c r="B381" s="22">
-        <v>21</v>
-      </c>
-      <c r="C381" s="26"/>
-      <c r="D381" s="27"/>
-      <c r="E381" s="26"/>
+        <v>20</v>
+      </c>
+      <c r="C381" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D381" s="24">
+        <v>10</v>
+      </c>
+      <c r="E381" s="25">
+        <v>15</v>
+      </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" s="21" t="s">
@@ -8383,13 +8403,13 @@
         <v>36</v>
       </c>
       <c r="C383" s="23">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="D383" s="24">
         <v>7.84</v>
       </c>
       <c r="E383" s="25">
-        <v>11.76</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
@@ -9168,16 +9188,16 @@
         <v>437</v>
       </c>
       <c r="B433" s="22">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C433" s="23">
-        <v>9.5</v>
+        <v>4.5</v>
       </c>
       <c r="D433" s="24">
         <v>3.3</v>
       </c>
       <c r="E433" s="25">
-        <v>31.35</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
@@ -9465,16 +9485,16 @@
         <v>456</v>
       </c>
       <c r="B452" s="22">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C452" s="23">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="D452" s="24">
         <v>4.1500000000000004</v>
       </c>
       <c r="E452" s="25">
-        <v>18.68</v>
+        <v>6.23</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
@@ -9567,16 +9587,16 @@
         <v>462</v>
       </c>
       <c r="B458" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C458" s="23">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D458" s="24">
         <v>4.28</v>
       </c>
       <c r="E458" s="25">
-        <v>393.76</v>
+        <v>380.92</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -9646,17 +9666,11 @@
         <v>467</v>
       </c>
       <c r="B463" s="22">
-        <v>13</v>
-      </c>
-      <c r="C463" s="23">
-        <v>2.5</v>
-      </c>
-      <c r="D463" s="24">
-        <v>4.5</v>
-      </c>
-      <c r="E463" s="25">
-        <v>11.25</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C463" s="26"/>
+      <c r="D463" s="27"/>
+      <c r="E463" s="26"/>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" s="21" t="s">
@@ -9837,17 +9851,11 @@
         <v>480</v>
       </c>
       <c r="B476" s="22">
-        <v>72</v>
-      </c>
-      <c r="C476" s="23">
-        <v>1</v>
-      </c>
-      <c r="D476" s="24">
-        <v>7.13</v>
-      </c>
-      <c r="E476" s="25">
-        <v>7.13</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C476" s="26"/>
+      <c r="D476" s="27"/>
+      <c r="E476" s="26"/>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" s="21" t="s">
@@ -9888,16 +9896,16 @@
         <v>483</v>
       </c>
       <c r="B479" s="22">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C479" s="23">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="D479" s="24">
         <v>7.6</v>
       </c>
       <c r="E479" s="25">
-        <v>34.200000000000003</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
@@ -10004,16 +10012,16 @@
         <v>491</v>
       </c>
       <c r="B487" s="22">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C487" s="23">
-        <v>-3</v>
+        <v>-3.5</v>
       </c>
       <c r="D487" s="24">
         <v>9.5</v>
       </c>
       <c r="E487" s="25">
-        <v>-28.5</v>
+        <v>-33.25</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
@@ -10273,16 +10281,16 @@
         <v>508</v>
       </c>
       <c r="B504" s="22">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C504" s="23">
-        <v>52.5</v>
+        <v>51</v>
       </c>
       <c r="D504" s="24">
         <v>1.38</v>
       </c>
       <c r="E504" s="25">
-        <v>72.36</v>
+        <v>70.290000000000006</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
@@ -10403,16 +10411,16 @@
         <v>516</v>
       </c>
       <c r="B512" s="22">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C512" s="23">
-        <v>16.7</v>
+        <v>13.7</v>
       </c>
       <c r="D512" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E512" s="25">
-        <v>38.08</v>
+        <v>31.24</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10420,16 +10428,16 @@
         <v>517</v>
       </c>
       <c r="B513" s="22">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C513" s="23">
-        <v>87.5</v>
+        <v>85.5</v>
       </c>
       <c r="D513" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E513" s="25">
-        <v>199.5</v>
+        <v>194.94</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10623,16 +10631,16 @@
         <v>530</v>
       </c>
       <c r="B526" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C526" s="23">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D526" s="24">
         <v>2.85</v>
       </c>
       <c r="E526" s="25">
-        <v>37.049999999999997</v>
+        <v>31.35</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10769,16 +10777,16 @@
         <v>540</v>
       </c>
       <c r="B536" s="22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C536" s="23">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D536" s="24">
         <v>3.71</v>
       </c>
       <c r="E536" s="25">
-        <v>245.1</v>
+        <v>241.38</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
@@ -11467,16 +11475,16 @@
         <v>584</v>
       </c>
       <c r="B580" s="22">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C580" s="23">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D580" s="24">
-        <v>2.76</v>
+        <v>2.77</v>
       </c>
       <c r="E580" s="25">
-        <v>24.87</v>
+        <v>16.59</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
@@ -11501,16 +11509,16 @@
         <v>586</v>
       </c>
       <c r="B582" s="22">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C582" s="23">
-        <v>49.74</v>
+        <v>43.74</v>
       </c>
       <c r="D582" s="24">
         <v>2.76</v>
       </c>
       <c r="E582" s="25">
-        <v>137.28</v>
+        <v>120.72</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
@@ -11820,16 +11828,16 @@
         <v>605</v>
       </c>
       <c r="B601" s="22">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C601" s="23">
-        <v>88.2</v>
+        <v>87.2</v>
       </c>
       <c r="D601" s="24">
         <v>1.93</v>
       </c>
       <c r="E601" s="25">
-        <v>170.19</v>
+        <v>168.26</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
@@ -11854,16 +11862,16 @@
         <v>607</v>
       </c>
       <c r="B603" s="22">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C603" s="23">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D603" s="24">
         <v>4.28</v>
       </c>
       <c r="E603" s="25">
-        <v>107</v>
+        <v>55.64</v>
       </c>
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
@@ -11939,16 +11947,16 @@
         <v>612</v>
       </c>
       <c r="B608" s="22">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C608" s="23">
-        <v>879.5</v>
+        <v>878.5</v>
       </c>
       <c r="D608" s="24">
         <v>1.4</v>
       </c>
       <c r="E608" s="25">
-        <v>1231.3</v>
+        <v>1229.9000000000001</v>
       </c>
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
@@ -12096,16 +12104,16 @@
         <v>623</v>
       </c>
       <c r="B619" s="22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C619" s="23">
-        <v>529.5</v>
+        <v>525.5</v>
       </c>
       <c r="D619" s="24">
         <v>0.81</v>
       </c>
       <c r="E619" s="25">
-        <v>431.38</v>
+        <v>428.12</v>
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
@@ -12113,16 +12121,16 @@
         <v>624</v>
       </c>
       <c r="B620" s="22">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C620" s="23">
-        <v>98.5</v>
+        <v>78.5</v>
       </c>
       <c r="D620" s="24">
         <v>0.81</v>
       </c>
       <c r="E620" s="25">
-        <v>79.5</v>
+        <v>63.36</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
@@ -12147,16 +12155,16 @@
         <v>626</v>
       </c>
       <c r="B622" s="22">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C622" s="23">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="D622" s="24">
         <v>0.52</v>
       </c>
       <c r="E622" s="25">
-        <v>721.76</v>
+        <v>718.64</v>
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
@@ -12181,16 +12189,16 @@
         <v>628</v>
       </c>
       <c r="B624" s="22">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C624" s="23">
-        <v>604.5</v>
+        <v>591.5</v>
       </c>
       <c r="D624" s="24">
         <v>0.52</v>
       </c>
       <c r="E624" s="25">
-        <v>314.33999999999997</v>
+        <v>307.58</v>
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
@@ -12215,16 +12223,16 @@
         <v>630</v>
       </c>
       <c r="B626" s="22">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C626" s="23">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D626" s="24">
         <v>0.52</v>
       </c>
       <c r="E626" s="25">
-        <v>146.12</v>
+        <v>143.52000000000001</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
@@ -12232,16 +12240,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C627" s="23">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>377.3</v>
+        <v>374.5</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12402,11 +12410,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>40905.57</v>
+        <v>40288.07</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>73655.490000000005</v>
+        <v>72293.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:13
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -3538,16 +3538,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C69" s="23">
-        <v>207.5</v>
+        <v>197.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>145.25</v>
+        <v>138.25</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3681,10 +3681,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C78" s="23">
-        <v>269</v>
+        <v>267.5</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -4249,16 +4249,16 @@
         <v>120</v>
       </c>
       <c r="B116" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C116" s="23">
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="D116" s="24">
         <v>12.5</v>
       </c>
       <c r="E116" s="25">
-        <v>12.5</v>
+        <v>-18.75</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4941,16 +4941,16 @@
         <v>166</v>
       </c>
       <c r="B162" s="22">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C162" s="23">
-        <v>55.5</v>
+        <v>54.5</v>
       </c>
       <c r="D162" s="24">
         <v>2.8</v>
       </c>
       <c r="E162" s="25">
-        <v>155.4</v>
+        <v>152.6</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -5026,16 +5026,16 @@
         <v>171</v>
       </c>
       <c r="B167" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C167" s="23">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D167" s="24">
         <v>3</v>
       </c>
       <c r="E167" s="25">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5364,16 +5364,16 @@
         <v>193</v>
       </c>
       <c r="B189" s="22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C189" s="23">
-        <v>23.5</v>
+        <v>18.5</v>
       </c>
       <c r="D189" s="24">
         <v>4.5</v>
       </c>
       <c r="E189" s="25">
-        <v>105.75</v>
+        <v>83.25</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5381,16 +5381,16 @@
         <v>194</v>
       </c>
       <c r="B190" s="22">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C190" s="23">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D190" s="24">
         <v>3.77</v>
       </c>
       <c r="E190" s="25">
-        <v>109.4</v>
+        <v>101.86</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5690,16 +5690,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C213" s="23">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.1100000000000003</v>
       </c>
       <c r="E213" s="25">
-        <v>12.34</v>
+        <v>6.17</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5898,16 +5898,16 @@
         <v>231</v>
       </c>
       <c r="B227" s="22">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C227" s="23">
-        <v>-4.5</v>
+        <v>-6</v>
       </c>
       <c r="D227" s="24">
         <v>4.5</v>
       </c>
       <c r="E227" s="25">
-        <v>-20.25</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6054,16 +6054,16 @@
         <v>241</v>
       </c>
       <c r="B237" s="22">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C237" s="23">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D237" s="24">
         <v>6</v>
       </c>
       <c r="E237" s="25">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6902,16 +6902,16 @@
         <v>297</v>
       </c>
       <c r="B293" s="22">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C293" s="23">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="D293" s="24">
         <v>6.18</v>
       </c>
       <c r="E293" s="25">
-        <v>46.35</v>
+        <v>40.17</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -7517,16 +7517,16 @@
         <v>338</v>
       </c>
       <c r="B334" s="22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C334" s="23">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D334" s="24">
         <v>6.91</v>
       </c>
       <c r="E334" s="25">
-        <v>124.39</v>
+        <v>117.48</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -8210,16 +8210,16 @@
         <v>381</v>
       </c>
       <c r="B377" s="22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C377" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D377" s="24">
         <v>10.5</v>
       </c>
       <c r="E377" s="25">
-        <v>21</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -8955,16 +8955,16 @@
         <v>428</v>
       </c>
       <c r="B424" s="22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C424" s="23">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D424" s="24">
         <v>3.8</v>
       </c>
       <c r="E424" s="25">
-        <v>110.2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -9926,16 +9926,16 @@
         <v>491</v>
       </c>
       <c r="B487" s="22">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C487" s="23">
-        <v>-5.5</v>
+        <v>-9.5</v>
       </c>
       <c r="D487" s="24">
         <v>9.5</v>
       </c>
       <c r="E487" s="25">
-        <v>-52.25</v>
+        <v>-90.25</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
@@ -10348,16 +10348,16 @@
         <v>517</v>
       </c>
       <c r="B513" s="22">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C513" s="23">
-        <v>47.5</v>
+        <v>47</v>
       </c>
       <c r="D513" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E513" s="25">
-        <v>108.3</v>
+        <v>107.16</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10702,16 +10702,16 @@
         <v>541</v>
       </c>
       <c r="B537" s="22">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C537" s="23">
-        <v>18.5</v>
+        <v>17.5</v>
       </c>
       <c r="D537" s="24">
         <v>3.6</v>
       </c>
       <c r="E537" s="25">
-        <v>66.599999999999994</v>
+        <v>63</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -11088,11 +11088,17 @@
         <v>565</v>
       </c>
       <c r="B561" s="22">
-        <v>75</v>
-      </c>
-      <c r="C561" s="26"/>
-      <c r="D561" s="27"/>
-      <c r="E561" s="26"/>
+        <v>76</v>
+      </c>
+      <c r="C561" s="23">
+        <v>-7</v>
+      </c>
+      <c r="D561" s="24">
+        <v>5.5</v>
+      </c>
+      <c r="E561" s="25">
+        <v>-38.5</v>
+      </c>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A562" s="21" t="s">
@@ -11524,16 +11530,16 @@
         <v>593</v>
       </c>
       <c r="B589" s="22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C589" s="23">
-        <v>16.5</v>
+        <v>13.5</v>
       </c>
       <c r="D589" s="24">
         <v>3</v>
       </c>
       <c r="E589" s="25">
-        <v>49.5</v>
+        <v>40.5</v>
       </c>
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
@@ -11908,10 +11914,10 @@
         <v>617</v>
       </c>
       <c r="B613" s="22">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C613" s="23">
-        <v>13.3</v>
+        <v>12.3</v>
       </c>
       <c r="D613" s="27"/>
       <c r="E613" s="26"/>
@@ -12300,11 +12306,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>37609.01</v>
+        <v>37557.51</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>67792.740000000005</v>
+        <v>67564.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 11:43
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -3227,16 +3227,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C50" s="23">
-        <v>-97</v>
+        <v>-105</v>
       </c>
       <c r="D50" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>-108.4</v>
+        <v>-117.34</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3295,16 +3295,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C54" s="23">
-        <v>51.5</v>
+        <v>39.5</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>57.57</v>
+        <v>44.15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3577,16 +3577,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C72" s="23">
-        <v>1187</v>
+        <v>1154</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>1839.85</v>
+        <v>1788.7</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,16 +3783,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C86" s="23">
-        <v>2113</v>
+        <v>2108</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>2958.2</v>
+        <v>2951.2</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4668,16 +4668,16 @@
         <v>149</v>
       </c>
       <c r="B145" s="22">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C145" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D145" s="24">
         <v>18.420000000000002</v>
       </c>
       <c r="E145" s="25">
-        <v>55.27</v>
+        <v>36.840000000000003</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,16 +4792,16 @@
         <v>157</v>
       </c>
       <c r="B153" s="22">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C153" s="23">
-        <v>14.5</v>
+        <v>12.5</v>
       </c>
       <c r="D153" s="24">
         <v>2.75</v>
       </c>
       <c r="E153" s="25">
-        <v>39.880000000000003</v>
+        <v>34.380000000000003</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -4887,16 +4887,16 @@
         <v>164</v>
       </c>
       <c r="B160" s="22">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C160" s="23">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="D160" s="24">
         <v>2.8</v>
       </c>
       <c r="E160" s="25">
-        <v>12.6</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -4921,16 +4921,16 @@
         <v>166</v>
       </c>
       <c r="B162" s="22">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C162" s="23">
-        <v>46</v>
+        <v>43.5</v>
       </c>
       <c r="D162" s="24">
         <v>2.8</v>
       </c>
       <c r="E162" s="25">
-        <v>128.80000000000001</v>
+        <v>121.8</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -4989,16 +4989,16 @@
         <v>170</v>
       </c>
       <c r="B166" s="22">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C166" s="23">
-        <v>73.5</v>
+        <v>72.5</v>
       </c>
       <c r="D166" s="24">
         <v>2.95</v>
       </c>
       <c r="E166" s="25">
-        <v>216.83</v>
+        <v>213.88</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5658,16 +5658,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C213" s="23">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D213" s="24">
         <v>4.1100000000000003</v>
       </c>
       <c r="E213" s="25">
-        <v>168.57</v>
+        <v>143.9</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5770,16 +5770,16 @@
         <v>225</v>
       </c>
       <c r="B221" s="22">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C221" s="23">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D221" s="24">
         <v>4.5</v>
       </c>
       <c r="E221" s="25">
-        <v>220.5</v>
+        <v>216</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -6146,16 +6146,16 @@
         <v>249</v>
       </c>
       <c r="B245" s="22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C245" s="23">
-        <v>9.3000000000000007</v>
+        <v>7.3</v>
       </c>
       <c r="D245" s="24">
         <v>4</v>
       </c>
       <c r="E245" s="25">
-        <v>37.200000000000003</v>
+        <v>29.2</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6258,16 +6258,16 @@
         <v>257</v>
       </c>
       <c r="B253" s="22">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C253" s="23">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D253" s="24">
         <v>4.25</v>
       </c>
       <c r="E253" s="25">
-        <v>72.25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -11964,16 +11964,16 @@
         <v>627</v>
       </c>
       <c r="B623" s="22">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C623" s="23">
-        <v>290.5</v>
+        <v>285.5</v>
       </c>
       <c r="D623" s="24">
         <v>0.52</v>
       </c>
       <c r="E623" s="25">
-        <v>151.06</v>
+        <v>148.46</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
@@ -11998,16 +11998,16 @@
         <v>629</v>
       </c>
       <c r="B625" s="22">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C625" s="23">
-        <v>204.5</v>
+        <v>199.5</v>
       </c>
       <c r="D625" s="24">
         <v>0.52</v>
       </c>
       <c r="E625" s="25">
-        <v>106.34</v>
+        <v>103.74</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
@@ -12032,16 +12032,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C627" s="23">
-        <v>143.5</v>
+        <v>138.5</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>100.45</v>
+        <v>96.95</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12049,16 +12049,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C628" s="23">
-        <v>71.5</v>
+        <v>66.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.69</v>
       </c>
       <c r="E628" s="25">
-        <v>49.01</v>
+        <v>45.58</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12196,11 +12196,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>31159.93</v>
+        <v>31058.43</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>56437.23</v>
+        <v>56243.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock updated by raj time 12:20
</commit_message>
<xml_diff>
--- a/StkSum_new.xlsx
+++ b/StkSum_new.xlsx
@@ -32,7 +32,7 @@
     <t>Stock Summary</t>
   </si>
   <si>
-    <t>1-Jul-2024 to 15-Apr-2025</t>
+    <t>1-Jul-2024 to 16-Apr-2025</t>
   </si>
   <si>
     <t/>
@@ -2578,16 +2578,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="22">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="23">
-        <v>482.5</v>
+        <v>480.5</v>
       </c>
       <c r="D9" s="24">
         <v>1</v>
       </c>
       <c r="E9" s="25">
-        <v>482.5</v>
+        <v>480.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,16 +2612,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="22">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C11" s="23">
-        <v>195</v>
+        <v>193.5</v>
       </c>
       <c r="D11" s="24">
         <v>0.91</v>
       </c>
       <c r="E11" s="25">
-        <v>177.04</v>
+        <v>175.68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,33 +2714,27 @@
         <v>21</v>
       </c>
       <c r="B17" s="22">
-        <v>193</v>
-      </c>
-      <c r="C17" s="23">
-        <v>5</v>
-      </c>
-      <c r="D17" s="24">
-        <v>2</v>
-      </c>
-      <c r="E17" s="25">
-        <v>10</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="22">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C18" s="23">
-        <v>12.5</v>
+        <v>9</v>
       </c>
       <c r="D18" s="24">
         <v>2</v>
       </c>
       <c r="E18" s="25">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2759,16 +2753,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="22">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="23">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D20" s="24">
         <v>2</v>
       </c>
       <c r="E20" s="25">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,16 +2804,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="22">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C23" s="23">
-        <v>110.75</v>
+        <v>109.75</v>
       </c>
       <c r="D23" s="24">
         <v>2</v>
       </c>
       <c r="E23" s="25">
-        <v>221.5</v>
+        <v>219.5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2995,16 +2989,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="22">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C36" s="23">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D36" s="24">
         <v>2.6</v>
       </c>
       <c r="E36" s="25">
-        <v>98.8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,16 +3006,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="22">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" s="23">
-        <v>25.5</v>
+        <v>23.5</v>
       </c>
       <c r="D37" s="24">
         <v>2.6</v>
       </c>
       <c r="E37" s="25">
-        <v>66.3</v>
+        <v>61.1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3046,16 +3040,16 @@
         <v>43</v>
       </c>
       <c r="B39" s="22">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C39" s="23">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="D39" s="24">
         <v>2.7</v>
       </c>
       <c r="E39" s="25">
-        <v>29.7</v>
+        <v>28.35</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3159,16 +3153,16 @@
         <v>50</v>
       </c>
       <c r="B46" s="22">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" s="23">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D46" s="24">
         <v>2.35</v>
       </c>
       <c r="E46" s="25">
-        <v>44.65</v>
+        <v>39.950000000000003</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3210,16 +3204,16 @@
         <v>53</v>
       </c>
       <c r="B49" s="22">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C49" s="23">
-        <v>345.5</v>
+        <v>333.5</v>
       </c>
       <c r="D49" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E49" s="25">
-        <v>387.41</v>
+        <v>373.95</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3227,16 +3221,16 @@
         <v>54</v>
       </c>
       <c r="B50" s="22">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="C50" s="23">
-        <v>491.5</v>
+        <v>478.5</v>
       </c>
       <c r="D50" s="24">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E50" s="25">
-        <v>552.94000000000005</v>
+        <v>538.30999999999995</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3261,16 +3255,16 @@
         <v>56</v>
       </c>
       <c r="B52" s="22">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C52" s="23">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D52" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E52" s="25">
-        <v>597.30999999999995</v>
+        <v>595.05999999999995</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3295,16 +3289,16 @@
         <v>58</v>
       </c>
       <c r="B54" s="22">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C54" s="23">
-        <v>748.5</v>
+        <v>744</v>
       </c>
       <c r="D54" s="24">
         <v>1.1200000000000001</v>
       </c>
       <c r="E54" s="25">
-        <v>841.46</v>
+        <v>836.4</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3374,16 +3368,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="22">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C59" s="23">
-        <v>93.5</v>
+        <v>92.5</v>
       </c>
       <c r="D59" s="24">
         <v>1.9</v>
       </c>
       <c r="E59" s="25">
-        <v>177.65</v>
+        <v>175.75</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3391,16 +3385,16 @@
         <v>64</v>
       </c>
       <c r="B60" s="22">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C60" s="23">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D60" s="24">
         <v>1.9</v>
       </c>
       <c r="E60" s="25">
-        <v>471.2</v>
+        <v>467.4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3408,16 +3402,16 @@
         <v>65</v>
       </c>
       <c r="B61" s="22">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C61" s="23">
-        <v>196.5</v>
+        <v>193.5</v>
       </c>
       <c r="D61" s="24">
         <v>2.1</v>
       </c>
       <c r="E61" s="25">
-        <v>412.65</v>
+        <v>406.35</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3532,16 +3526,16 @@
         <v>73</v>
       </c>
       <c r="B69" s="22">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C69" s="23">
-        <v>78.5</v>
+        <v>76.5</v>
       </c>
       <c r="D69" s="24">
         <v>0.7</v>
       </c>
       <c r="E69" s="25">
-        <v>54.95</v>
+        <v>53.55</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3577,16 +3571,16 @@
         <v>76</v>
       </c>
       <c r="B72" s="22">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="C72" s="23">
-        <v>1125.5</v>
+        <v>1116</v>
       </c>
       <c r="D72" s="24">
         <v>1.55</v>
       </c>
       <c r="E72" s="25">
-        <v>1744.53</v>
+        <v>1729.8</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3669,10 +3663,10 @@
         <v>82</v>
       </c>
       <c r="B78" s="22">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C78" s="23">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="26"/>
@@ -3695,10 +3689,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="22">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C80" s="23">
-        <v>-77</v>
+        <v>-89</v>
       </c>
       <c r="D80" s="27"/>
       <c r="E80" s="26"/>
@@ -3719,10 +3713,10 @@
         <v>86</v>
       </c>
       <c r="B82" s="22">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C82" s="23">
-        <v>114.5</v>
+        <v>104.5</v>
       </c>
       <c r="D82" s="27"/>
       <c r="E82" s="26"/>
@@ -3732,16 +3726,16 @@
         <v>87</v>
       </c>
       <c r="B83" s="22">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C83" s="23">
-        <v>35.5</v>
+        <v>33.5</v>
       </c>
       <c r="D83" s="24">
         <v>1.1499999999999999</v>
       </c>
       <c r="E83" s="25">
-        <v>40.83</v>
+        <v>38.53</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3766,16 +3760,16 @@
         <v>89</v>
       </c>
       <c r="B85" s="22">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C85" s="23">
-        <v>2720</v>
+        <v>2675</v>
       </c>
       <c r="D85" s="24">
         <v>1.4</v>
       </c>
       <c r="E85" s="25">
-        <v>3808</v>
+        <v>3745</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,16 +3777,16 @@
         <v>90</v>
       </c>
       <c r="B86" s="22">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C86" s="23">
-        <v>2085</v>
+        <v>2075</v>
       </c>
       <c r="D86" s="24">
         <v>1.4</v>
       </c>
       <c r="E86" s="25">
-        <v>2919</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3860,16 +3854,16 @@
         <v>95</v>
       </c>
       <c r="B91" s="22">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C91" s="23">
-        <v>173.5</v>
+        <v>156</v>
       </c>
       <c r="D91" s="24">
         <v>1.24</v>
       </c>
       <c r="E91" s="25">
-        <v>214.47</v>
+        <v>192.84</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4437,16 +4431,16 @@
         <v>134</v>
       </c>
       <c r="B130" s="22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C130" s="23">
-        <v>14.5</v>
+        <v>16</v>
       </c>
       <c r="D130" s="24">
         <v>15.5</v>
       </c>
       <c r="E130" s="25">
-        <v>224.75</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4709,9 +4703,15 @@
       <c r="B148" s="22">
         <v>21</v>
       </c>
-      <c r="C148" s="26"/>
-      <c r="D148" s="27"/>
-      <c r="E148" s="26"/>
+      <c r="C148" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="D148" s="24">
+        <v>18.440000000000001</v>
+      </c>
+      <c r="E148" s="25">
+        <v>9.2200000000000006</v>
+      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="21" t="s">
@@ -4825,16 +4825,16 @@
         <v>160</v>
       </c>
       <c r="B156" s="22">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C156" s="23">
-        <v>39.35</v>
+        <v>38.35</v>
       </c>
       <c r="D156" s="24">
         <v>3.4</v>
       </c>
       <c r="E156" s="25">
-        <v>133.79</v>
+        <v>130.38999999999999</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -5366,16 +5366,16 @@
         <v>195</v>
       </c>
       <c r="B191" s="22">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C191" s="23">
-        <v>37</v>
+        <v>34.5</v>
       </c>
       <c r="D191" s="24">
         <v>3.92</v>
       </c>
       <c r="E191" s="25">
-        <v>144.93</v>
+        <v>135.13999999999999</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5530,16 +5530,16 @@
         <v>207</v>
       </c>
       <c r="B203" s="22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C203" s="23">
-        <v>36</v>
+        <v>35.5</v>
       </c>
       <c r="D203" s="24">
         <v>3.37</v>
       </c>
       <c r="E203" s="25">
-        <v>121.34</v>
+        <v>119.66</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5602,16 +5602,16 @@
         <v>213</v>
       </c>
       <c r="B209" s="22">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C209" s="23">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D209" s="24">
         <v>3.8</v>
       </c>
       <c r="E209" s="25">
-        <v>60.8</v>
+        <v>49.4</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5658,16 +5658,16 @@
         <v>217</v>
       </c>
       <c r="B213" s="22">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C213" s="23">
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="D213" s="24">
         <v>4.1100000000000003</v>
       </c>
       <c r="E213" s="25">
-        <v>108.95</v>
+        <v>100.73</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -5921,16 +5921,16 @@
         <v>234</v>
       </c>
       <c r="B230" s="22">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C230" s="23">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="D230" s="24">
         <v>5.25</v>
       </c>
       <c r="E230" s="25">
-        <v>44.63</v>
+        <v>28.88</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6069,16 +6069,16 @@
         <v>244</v>
       </c>
       <c r="B240" s="22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C240" s="23">
-        <v>19.5</v>
+        <v>16.5</v>
       </c>
       <c r="D240" s="24">
         <v>6.75</v>
       </c>
       <c r="E240" s="25">
-        <v>131.63</v>
+        <v>111.38</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6318,16 +6318,16 @@
         <v>261</v>
       </c>
       <c r="B257" s="22">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C257" s="23">
-        <v>14.5</v>
+        <v>14</v>
       </c>
       <c r="D257" s="24">
         <v>4.18</v>
       </c>
       <c r="E257" s="25">
-        <v>60.61</v>
+        <v>58.52</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -7379,17 +7379,11 @@
         <v>332</v>
       </c>
       <c r="B328" s="22">
-        <v>78</v>
-      </c>
-      <c r="C328" s="23">
-        <v>1</v>
-      </c>
-      <c r="D328" s="24">
-        <v>9.25</v>
-      </c>
-      <c r="E328" s="25">
-        <v>9.25</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C328" s="26"/>
+      <c r="D328" s="27"/>
+      <c r="E328" s="26"/>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" s="21" t="s">
@@ -7554,16 +7548,16 @@
         <v>343</v>
       </c>
       <c r="B339" s="22">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C339" s="23">
-        <v>11.5</v>
+        <v>10.5</v>
       </c>
       <c r="D339" s="24">
         <v>10.77</v>
       </c>
       <c r="E339" s="25">
-        <v>123.82</v>
+        <v>113.06</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -9033,16 +9027,16 @@
         <v>438</v>
       </c>
       <c r="B434" s="22">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C434" s="23">
-        <v>4.4000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="D434" s="24">
         <v>3.05</v>
       </c>
       <c r="E434" s="25">
-        <v>13.42</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
@@ -9819,16 +9813,16 @@
         <v>490</v>
       </c>
       <c r="B486" s="22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C486" s="23">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="D486" s="24">
         <v>9.5</v>
       </c>
       <c r="E486" s="25">
-        <v>61.75</v>
+        <v>42.75</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -9930,16 +9924,16 @@
         <v>497</v>
       </c>
       <c r="B493" s="22">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C493" s="23">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D493" s="24">
         <v>1.1000000000000001</v>
       </c>
       <c r="E493" s="25">
-        <v>189.2</v>
+        <v>187</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -10032,16 +10026,16 @@
         <v>503</v>
       </c>
       <c r="B499" s="22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C499" s="23">
-        <v>20.5</v>
+        <v>20</v>
       </c>
       <c r="D499" s="24">
         <v>3.05</v>
       </c>
       <c r="E499" s="25">
-        <v>62.53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10196,16 +10190,16 @@
         <v>513</v>
       </c>
       <c r="B509" s="22">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C509" s="23">
-        <v>49.5</v>
+        <v>38.5</v>
       </c>
       <c r="D509" s="24">
         <v>1.71</v>
       </c>
       <c r="E509" s="25">
-        <v>84.65</v>
+        <v>65.84</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10230,16 +10224,16 @@
         <v>515</v>
       </c>
       <c r="B511" s="22">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C511" s="23">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D511" s="24">
         <v>2.2799999999999998</v>
       </c>
       <c r="E511" s="25">
-        <v>70.680000000000007</v>
+        <v>59.28</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -11585,16 +11579,16 @@
         <v>602</v>
       </c>
       <c r="B598" s="22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C598" s="23">
-        <v>66.5</v>
+        <v>62.5</v>
       </c>
       <c r="D598" s="24">
         <v>1.92</v>
       </c>
       <c r="E598" s="25">
-        <v>127.71</v>
+        <v>120.03</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
@@ -11602,16 +11596,16 @@
         <v>603</v>
       </c>
       <c r="B599" s="22">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C599" s="23">
-        <v>363.5</v>
+        <v>360.5</v>
       </c>
       <c r="D599" s="24">
         <v>1.91</v>
       </c>
       <c r="E599" s="25">
-        <v>694.06</v>
+        <v>688.34</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
@@ -11715,16 +11709,16 @@
         <v>610</v>
       </c>
       <c r="B606" s="22">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C606" s="23">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D606" s="24">
         <v>1.4</v>
       </c>
       <c r="E606" s="25">
-        <v>493.42</v>
+        <v>492.02</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -12036,16 +12030,16 @@
         <v>631</v>
       </c>
       <c r="B627" s="22">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C627" s="23">
-        <v>136.5</v>
+        <v>126.5</v>
       </c>
       <c r="D627" s="24">
         <v>0.7</v>
       </c>
       <c r="E627" s="25">
-        <v>95.55</v>
+        <v>88.55</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
@@ -12053,16 +12047,16 @@
         <v>632</v>
       </c>
       <c r="B628" s="22">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C628" s="23">
-        <v>66.5</v>
+        <v>65.5</v>
       </c>
       <c r="D628" s="24">
         <v>0.69</v>
       </c>
       <c r="E628" s="25">
-        <v>45.58</v>
+        <v>44.9</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
@@ -12200,11 +12194,11 @@
       </c>
       <c r="B638" s="29"/>
       <c r="C638" s="30">
-        <v>34301.43</v>
+        <v>34072.43</v>
       </c>
       <c r="D638" s="31"/>
       <c r="E638" s="32">
-        <v>60610.77</v>
+        <v>60253.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>